<commit_message>
'Se agrega el 7 Alumno al archivo
</commit_message>
<xml_diff>
--- a/Lista de Alumnos.xlsx
+++ b/Lista de Alumnos.xlsx
@@ -1,17 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Documents\ISPC\ELECTRONICA MICROCONTROLADA\GitHub\Alumnos\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23970" windowHeight="9600"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Electronica Microcontrolada" sheetId="1" r:id="rId4"/>
+    <sheet name="Electronica Microcontrolada" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>#</t>
   </si>
@@ -78,56 +86,72 @@
   <si>
     <t>sharonmulka</t>
   </si>
+  <si>
+    <t>Ezequiel Mansilla</t>
+  </si>
+  <si>
+    <t>advanceezequiel@gmail.com</t>
+  </si>
+  <si>
+    <t>Ezequiel0681</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="8">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="18.0"/>
+      <sz val="18"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
       <u/>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
       <u/>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
       <u/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="10"/>
       <name val="Calibri"/>
     </font>
     <font>
       <u/>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -135,31 +159,43 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="5">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
+      <right/>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
+      <left/>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
@@ -169,6 +205,7 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -183,71 +220,80 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+  <cellStyleXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="3" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+  <cellXfs count="16">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="2" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="2" fillId="0" fontId="1" numFmtId="3" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="3" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="4" fillId="0" fontId="2" numFmtId="3" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="4" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="4" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="4" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="4" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="4" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="4" fillId="0" fontId="2" numFmtId="3" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="4" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="7" numFmtId="3" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+  <cellStyles count="2">
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -437,28 +483,30 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="6.86"/>
-    <col customWidth="1" min="2" max="2" width="37.14"/>
-    <col customWidth="1" min="3" max="3" width="10.57"/>
-    <col customWidth="1" min="4" max="4" width="31.0"/>
-    <col customWidth="1" min="5" max="5" width="29.0"/>
-    <col customWidth="1" min="6" max="6" width="8.71"/>
+    <col min="1" max="1" width="6.85546875" customWidth="1"/>
+    <col min="2" max="2" width="37.140625" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" customWidth="1"/>
+    <col min="4" max="4" width="31" customWidth="1"/>
+    <col min="5" max="5" width="29" customWidth="1"/>
+    <col min="6" max="6" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="27.0" customHeight="1">
+    <row r="1" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -475,15 +523,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" ht="19.5" customHeight="1">
+    <row r="2" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>5</v>
       </c>
       <c r="C2" s="5">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="D2" s="7" t="s">
         <v>6</v>
@@ -492,30 +540,30 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" ht="19.5" customHeight="1">
+    <row r="3" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>8</v>
       </c>
       <c r="C3" s="5">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>9</v>
       </c>
       <c r="E3" s="6"/>
     </row>
-    <row r="4" ht="19.5" customHeight="1">
+    <row r="4" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>10</v>
       </c>
       <c r="C4" s="5">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="D4" s="7" t="s">
         <v>11</v>
@@ -524,15 +572,15 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" ht="19.5" customHeight="1">
+    <row r="5" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>13</v>
       </c>
       <c r="C5" s="5">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="D5" s="9" t="s">
         <v>14</v>
@@ -541,15 +589,15 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" ht="19.5" customHeight="1">
+    <row r="6" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>16</v>
       </c>
       <c r="C6" s="5">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="D6" s="7" t="s">
         <v>17</v>
@@ -558,15 +606,15 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" ht="19.5" customHeight="1">
+    <row r="7" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="B7" s="10" t="s">
         <v>19</v>
       </c>
       <c r="C7" s="11">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="D7" s="12" t="s">
         <v>20</v>
@@ -575,2631 +623,2638 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" ht="19.5" customHeight="1">
+    <row r="8" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
-        <v>7.0</v>
-      </c>
-      <c r="B8" s="6"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="6"/>
-    </row>
-    <row r="9" ht="19.5" customHeight="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="5">
+        <v>1</v>
+      </c>
+      <c r="D8" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="B9" s="6"/>
       <c r="C9" s="5"/>
       <c r="D9" s="7"/>
       <c r="E9" s="6"/>
     </row>
-    <row r="10" ht="19.5" customHeight="1">
+    <row r="10" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
-        <v>9.0</v>
+        <v>9</v>
       </c>
       <c r="B10" s="6"/>
       <c r="C10" s="5"/>
       <c r="D10" s="7"/>
       <c r="E10" s="6"/>
     </row>
-    <row r="11" ht="19.5" customHeight="1">
+    <row r="11" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="B11" s="6"/>
       <c r="C11" s="5"/>
       <c r="D11" s="6"/>
       <c r="E11" s="6"/>
     </row>
-    <row r="12" ht="19.5" customHeight="1">
+    <row r="12" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
-        <v>11.0</v>
+        <v>11</v>
       </c>
       <c r="B12" s="6"/>
       <c r="C12" s="5"/>
       <c r="D12" s="6"/>
       <c r="E12" s="6"/>
     </row>
-    <row r="13" ht="19.5" customHeight="1">
+    <row r="13" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
-        <v>12.0</v>
+        <v>12</v>
       </c>
       <c r="B13" s="6"/>
       <c r="C13" s="5"/>
       <c r="D13" s="6"/>
       <c r="E13" s="6"/>
     </row>
-    <row r="14" ht="19.5" customHeight="1">
+    <row r="14" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
-        <v>13.0</v>
+        <v>13</v>
       </c>
       <c r="B14" s="6"/>
       <c r="C14" s="5"/>
       <c r="D14" s="6"/>
       <c r="E14" s="6"/>
     </row>
-    <row r="15" ht="19.5" customHeight="1">
+    <row r="15" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
-        <v>14.0</v>
+        <v>14</v>
       </c>
       <c r="B15" s="6"/>
       <c r="C15" s="5"/>
       <c r="D15" s="6"/>
       <c r="E15" s="6"/>
     </row>
-    <row r="16" ht="19.5" customHeight="1">
+    <row r="16" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
-        <v>15.0</v>
+        <v>15</v>
       </c>
       <c r="B16" s="6"/>
       <c r="C16" s="5"/>
       <c r="D16" s="6"/>
       <c r="E16" s="6"/>
     </row>
-    <row r="17" ht="19.5" customHeight="1">
+    <row r="17" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
-        <v>16.0</v>
+        <v>16</v>
       </c>
       <c r="B17" s="6"/>
       <c r="C17" s="5"/>
       <c r="D17" s="6"/>
       <c r="E17" s="6"/>
     </row>
-    <row r="18" ht="25.5" customHeight="1">
+    <row r="18" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
-        <v>17.0</v>
+        <v>17</v>
       </c>
       <c r="B18" s="6"/>
       <c r="C18" s="5"/>
       <c r="D18" s="6"/>
       <c r="E18" s="6"/>
     </row>
-    <row r="19" ht="25.5" customHeight="1">
+    <row r="19" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
-        <v>18.0</v>
+        <v>18</v>
       </c>
       <c r="B19" s="6"/>
       <c r="C19" s="5"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
     </row>
-    <row r="20" ht="25.5" customHeight="1">
+    <row r="20" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
-        <v>19.0</v>
+        <v>19</v>
       </c>
       <c r="B20" s="6"/>
       <c r="C20" s="5"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
     </row>
-    <row r="21" ht="25.5" customHeight="1">
+    <row r="21" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="5">
-        <v>20.0</v>
+        <v>20</v>
       </c>
       <c r="B21" s="6"/>
       <c r="C21" s="5"/>
       <c r="D21" s="6"/>
       <c r="E21" s="6"/>
     </row>
-    <row r="22" ht="25.5" customHeight="1">
+    <row r="22" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="5">
-        <v>21.0</v>
+        <v>21</v>
       </c>
       <c r="B22" s="6"/>
       <c r="C22" s="5"/>
       <c r="D22" s="6"/>
       <c r="E22" s="6"/>
     </row>
-    <row r="23" ht="25.5" customHeight="1">
+    <row r="23" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="5">
-        <v>22.0</v>
+        <v>22</v>
       </c>
       <c r="B23" s="6"/>
       <c r="C23" s="5"/>
       <c r="D23" s="6"/>
       <c r="E23" s="6"/>
     </row>
-    <row r="24" ht="25.5" customHeight="1">
+    <row r="24" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="5">
-        <v>23.0</v>
+        <v>23</v>
       </c>
       <c r="B24" s="6"/>
       <c r="C24" s="5"/>
       <c r="D24" s="6"/>
       <c r="E24" s="6"/>
     </row>
-    <row r="25" ht="25.5" customHeight="1">
+    <row r="25" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="5">
-        <v>24.0</v>
+        <v>24</v>
       </c>
       <c r="B25" s="6"/>
       <c r="C25" s="5"/>
       <c r="D25" s="6"/>
       <c r="E25" s="6"/>
     </row>
-    <row r="26" ht="25.5" customHeight="1">
+    <row r="26" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="5">
-        <v>25.0</v>
+        <v>25</v>
       </c>
       <c r="B26" s="6"/>
       <c r="C26" s="5"/>
       <c r="D26" s="6"/>
       <c r="E26" s="6"/>
     </row>
-    <row r="27" ht="25.5" customHeight="1">
+    <row r="27" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="5">
-        <v>26.0</v>
+        <v>26</v>
       </c>
       <c r="B27" s="6"/>
       <c r="C27" s="5"/>
       <c r="D27" s="6"/>
       <c r="E27" s="6"/>
     </row>
-    <row r="28" ht="25.5" customHeight="1">
+    <row r="28" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="5">
-        <v>27.0</v>
+        <v>27</v>
       </c>
       <c r="B28" s="6"/>
       <c r="C28" s="5"/>
       <c r="D28" s="6"/>
       <c r="E28" s="6"/>
     </row>
-    <row r="29" ht="25.5" customHeight="1">
+    <row r="29" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="5">
-        <v>28.0</v>
+        <v>28</v>
       </c>
       <c r="B29" s="6"/>
       <c r="C29" s="5"/>
       <c r="D29" s="6"/>
       <c r="E29" s="6"/>
     </row>
-    <row r="30" ht="25.5" customHeight="1">
+    <row r="30" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="5">
-        <v>29.0</v>
+        <v>29</v>
       </c>
       <c r="B30" s="6"/>
       <c r="C30" s="5"/>
       <c r="D30" s="6"/>
       <c r="E30" s="6"/>
     </row>
-    <row r="31" ht="25.5" customHeight="1">
+    <row r="31" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="5">
-        <v>30.0</v>
+        <v>30</v>
       </c>
       <c r="B31" s="6"/>
       <c r="C31" s="5"/>
       <c r="D31" s="6"/>
       <c r="E31" s="6"/>
     </row>
-    <row r="32" ht="25.5" customHeight="1">
+    <row r="32" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="5">
-        <v>31.0</v>
+        <v>31</v>
       </c>
       <c r="B32" s="6"/>
       <c r="C32" s="5"/>
       <c r="D32" s="6"/>
       <c r="E32" s="6"/>
     </row>
-    <row r="33" ht="25.5" customHeight="1">
+    <row r="33" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="5">
-        <v>32.0</v>
+        <v>32</v>
       </c>
       <c r="B33" s="6"/>
       <c r="C33" s="5"/>
       <c r="D33" s="6"/>
       <c r="E33" s="6"/>
     </row>
-    <row r="34" ht="25.5" customHeight="1">
+    <row r="34" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="5">
-        <v>33.0</v>
+        <v>33</v>
       </c>
       <c r="B34" s="6"/>
       <c r="C34" s="5"/>
       <c r="D34" s="6"/>
       <c r="E34" s="6"/>
     </row>
-    <row r="35" ht="25.5" customHeight="1">
+    <row r="35" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="5">
-        <v>34.0</v>
+        <v>34</v>
       </c>
       <c r="B35" s="6"/>
       <c r="C35" s="5"/>
       <c r="D35" s="6"/>
       <c r="E35" s="6"/>
     </row>
-    <row r="36" ht="25.5" customHeight="1">
+    <row r="36" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="5">
-        <v>35.0</v>
+        <v>35</v>
       </c>
       <c r="B36" s="6"/>
       <c r="C36" s="5"/>
       <c r="D36" s="6"/>
       <c r="E36" s="6"/>
     </row>
-    <row r="37" ht="25.5" customHeight="1">
+    <row r="37" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="5">
-        <v>36.0</v>
+        <v>36</v>
       </c>
       <c r="B37" s="6"/>
       <c r="C37" s="5"/>
       <c r="D37" s="6"/>
       <c r="E37" s="6"/>
     </row>
-    <row r="38" ht="25.5" customHeight="1">
+    <row r="38" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="5">
-        <v>37.0</v>
+        <v>37</v>
       </c>
       <c r="B38" s="6"/>
       <c r="C38" s="5"/>
       <c r="D38" s="6"/>
       <c r="E38" s="6"/>
     </row>
-    <row r="39" ht="25.5" customHeight="1">
+    <row r="39" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="5">
-        <v>38.0</v>
+        <v>38</v>
       </c>
       <c r="B39" s="6"/>
       <c r="C39" s="5"/>
       <c r="D39" s="6"/>
       <c r="E39" s="6"/>
     </row>
-    <row r="40" ht="25.5" customHeight="1">
+    <row r="40" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="5">
-        <v>39.0</v>
+        <v>39</v>
       </c>
       <c r="B40" s="6"/>
       <c r="C40" s="5"/>
       <c r="D40" s="6"/>
       <c r="E40" s="6"/>
     </row>
-    <row r="41" ht="25.5" customHeight="1">
+    <row r="41" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="5">
-        <v>40.0</v>
+        <v>40</v>
       </c>
       <c r="B41" s="6"/>
       <c r="C41" s="5"/>
       <c r="D41" s="6"/>
       <c r="E41" s="6"/>
     </row>
-    <row r="42" ht="25.5" customHeight="1">
+    <row r="42" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="5">
-        <v>41.0</v>
+        <v>41</v>
       </c>
       <c r="B42" s="6"/>
       <c r="C42" s="5"/>
       <c r="D42" s="6"/>
       <c r="E42" s="6"/>
     </row>
-    <row r="43" ht="25.5" customHeight="1">
+    <row r="43" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="5">
-        <v>42.0</v>
+        <v>42</v>
       </c>
       <c r="B43" s="6"/>
       <c r="C43" s="5"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
     </row>
-    <row r="44" ht="25.5" customHeight="1">
+    <row r="44" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="5">
-        <v>43.0</v>
+        <v>43</v>
       </c>
       <c r="B44" s="6"/>
       <c r="C44" s="5"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
     </row>
-    <row r="45" ht="25.5" customHeight="1">
+    <row r="45" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="5">
-        <v>44.0</v>
+        <v>44</v>
       </c>
       <c r="B45" s="6"/>
       <c r="C45" s="5"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
     </row>
-    <row r="46" ht="25.5" customHeight="1">
+    <row r="46" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="5">
-        <v>45.0</v>
+        <v>45</v>
       </c>
       <c r="B46" s="6"/>
       <c r="C46" s="5"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
     </row>
-    <row r="47" ht="25.5" customHeight="1">
+    <row r="47" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="5">
-        <v>46.0</v>
+        <v>46</v>
       </c>
       <c r="B47" s="6"/>
       <c r="C47" s="5"/>
       <c r="D47" s="6"/>
       <c r="E47" s="6"/>
     </row>
-    <row r="48" ht="25.5" customHeight="1">
+    <row r="48" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="5">
-        <v>47.0</v>
+        <v>47</v>
       </c>
       <c r="B48" s="6"/>
       <c r="C48" s="5"/>
       <c r="D48" s="6"/>
       <c r="E48" s="6"/>
     </row>
-    <row r="49" ht="25.5" customHeight="1">
+    <row r="49" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="5">
-        <v>48.0</v>
+        <v>48</v>
       </c>
       <c r="B49" s="6"/>
       <c r="C49" s="5"/>
       <c r="D49" s="6"/>
       <c r="E49" s="6"/>
     </row>
-    <row r="50" ht="25.5" customHeight="1">
+    <row r="50" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="5">
-        <v>49.0</v>
+        <v>49</v>
       </c>
       <c r="B50" s="6"/>
       <c r="C50" s="5"/>
       <c r="D50" s="6"/>
       <c r="E50" s="6"/>
     </row>
-    <row r="51" ht="25.5" customHeight="1">
+    <row r="51" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="5">
-        <v>50.0</v>
+        <v>50</v>
       </c>
       <c r="B51" s="6"/>
       <c r="C51" s="5"/>
       <c r="D51" s="6"/>
       <c r="E51" s="6"/>
     </row>
-    <row r="52" ht="25.5" customHeight="1">
+    <row r="52" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="5">
-        <v>51.0</v>
+        <v>51</v>
       </c>
       <c r="B52" s="6"/>
       <c r="C52" s="5"/>
       <c r="D52" s="6"/>
       <c r="E52" s="6"/>
     </row>
-    <row r="53" ht="25.5" customHeight="1">
+    <row r="53" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="5">
-        <v>52.0</v>
+        <v>52</v>
       </c>
       <c r="B53" s="6"/>
       <c r="C53" s="5"/>
       <c r="D53" s="6"/>
       <c r="E53" s="6"/>
     </row>
-    <row r="54" ht="25.5" customHeight="1">
+    <row r="54" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="5">
-        <v>53.0</v>
+        <v>53</v>
       </c>
       <c r="B54" s="6"/>
       <c r="C54" s="5"/>
       <c r="D54" s="6"/>
       <c r="E54" s="6"/>
     </row>
-    <row r="55" ht="25.5" customHeight="1">
+    <row r="55" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="5">
-        <v>54.0</v>
+        <v>54</v>
       </c>
       <c r="B55" s="6"/>
       <c r="C55" s="5"/>
       <c r="D55" s="6"/>
       <c r="E55" s="6"/>
     </row>
-    <row r="56" ht="25.5" customHeight="1">
+    <row r="56" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="5">
-        <v>55.0</v>
+        <v>55</v>
       </c>
       <c r="B56" s="6"/>
       <c r="C56" s="5"/>
       <c r="D56" s="6"/>
       <c r="E56" s="6"/>
     </row>
-    <row r="57" ht="25.5" customHeight="1">
+    <row r="57" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="5">
-        <v>56.0</v>
+        <v>56</v>
       </c>
       <c r="B57" s="6"/>
       <c r="C57" s="5"/>
       <c r="D57" s="6"/>
       <c r="E57" s="6"/>
     </row>
-    <row r="58" ht="25.5" customHeight="1">
+    <row r="58" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="5">
-        <v>57.0</v>
+        <v>57</v>
       </c>
       <c r="B58" s="6"/>
       <c r="C58" s="5"/>
       <c r="D58" s="6"/>
       <c r="E58" s="6"/>
     </row>
-    <row r="59" ht="25.5" customHeight="1">
+    <row r="59" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="5">
-        <v>58.0</v>
+        <v>58</v>
       </c>
       <c r="B59" s="6"/>
       <c r="C59" s="5"/>
       <c r="D59" s="6"/>
       <c r="E59" s="6"/>
     </row>
-    <row r="60" ht="25.5" customHeight="1">
+    <row r="60" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="5">
-        <v>59.0</v>
+        <v>59</v>
       </c>
       <c r="B60" s="6"/>
       <c r="C60" s="5"/>
       <c r="D60" s="6"/>
       <c r="E60" s="6"/>
     </row>
-    <row r="61" ht="15.75" customHeight="1">
+    <row r="61" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="13"/>
       <c r="B61" s="14"/>
       <c r="C61" s="13"/>
       <c r="D61" s="14"/>
       <c r="E61" s="14"/>
     </row>
-    <row r="62" ht="15.75" customHeight="1">
+    <row r="62" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="13"/>
       <c r="B62" s="14"/>
       <c r="C62" s="13"/>
       <c r="D62" s="14"/>
       <c r="E62" s="14"/>
     </row>
-    <row r="63" ht="15.75" customHeight="1">
+    <row r="63" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="13"/>
       <c r="B63" s="14"/>
       <c r="C63" s="13"/>
       <c r="D63" s="14"/>
       <c r="E63" s="14"/>
     </row>
-    <row r="64" ht="15.75" customHeight="1">
+    <row r="64" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="13"/>
       <c r="B64" s="14"/>
       <c r="C64" s="13"/>
       <c r="D64" s="14"/>
       <c r="E64" s="14"/>
     </row>
-    <row r="65" ht="15.75" customHeight="1">
+    <row r="65" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="13"/>
       <c r="B65" s="14"/>
       <c r="C65" s="13"/>
       <c r="D65" s="14"/>
       <c r="E65" s="14"/>
     </row>
-    <row r="66" ht="15.75" customHeight="1">
+    <row r="66" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="13"/>
       <c r="B66" s="14"/>
       <c r="C66" s="13"/>
       <c r="D66" s="14"/>
       <c r="E66" s="14"/>
     </row>
-    <row r="67" ht="15.75" customHeight="1">
+    <row r="67" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="13"/>
       <c r="B67" s="14"/>
       <c r="C67" s="13"/>
       <c r="D67" s="14"/>
       <c r="E67" s="14"/>
     </row>
-    <row r="68" ht="15.75" customHeight="1">
+    <row r="68" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="13"/>
       <c r="B68" s="14"/>
       <c r="C68" s="13"/>
       <c r="D68" s="14"/>
       <c r="E68" s="14"/>
     </row>
-    <row r="69" ht="15.75" customHeight="1">
+    <row r="69" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="13"/>
       <c r="B69" s="14"/>
       <c r="C69" s="13"/>
       <c r="D69" s="14"/>
       <c r="E69" s="14"/>
     </row>
-    <row r="70" ht="15.75" customHeight="1">
+    <row r="70" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="13"/>
       <c r="B70" s="14"/>
       <c r="C70" s="13"/>
       <c r="D70" s="14"/>
       <c r="E70" s="14"/>
     </row>
-    <row r="71" ht="15.75" customHeight="1">
+    <row r="71" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="13"/>
       <c r="B71" s="14"/>
       <c r="C71" s="13"/>
       <c r="D71" s="14"/>
       <c r="E71" s="14"/>
     </row>
-    <row r="72" ht="15.75" customHeight="1">
+    <row r="72" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="13"/>
       <c r="B72" s="14"/>
       <c r="C72" s="13"/>
       <c r="D72" s="14"/>
       <c r="E72" s="14"/>
     </row>
-    <row r="73" ht="15.75" customHeight="1">
+    <row r="73" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="13"/>
       <c r="B73" s="14"/>
       <c r="C73" s="13"/>
       <c r="D73" s="14"/>
       <c r="E73" s="14"/>
     </row>
-    <row r="74" ht="15.75" customHeight="1">
+    <row r="74" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="13"/>
       <c r="B74" s="14"/>
       <c r="C74" s="13"/>
       <c r="D74" s="14"/>
       <c r="E74" s="14"/>
     </row>
-    <row r="75" ht="15.75" customHeight="1">
+    <row r="75" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="13"/>
       <c r="B75" s="14"/>
       <c r="C75" s="13"/>
       <c r="D75" s="14"/>
       <c r="E75" s="14"/>
     </row>
-    <row r="76" ht="15.75" customHeight="1">
+    <row r="76" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="13"/>
       <c r="B76" s="14"/>
       <c r="C76" s="13"/>
       <c r="D76" s="14"/>
       <c r="E76" s="14"/>
     </row>
-    <row r="77" ht="15.75" customHeight="1">
+    <row r="77" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="13"/>
       <c r="B77" s="14"/>
       <c r="C77" s="13"/>
       <c r="D77" s="14"/>
       <c r="E77" s="14"/>
     </row>
-    <row r="78" ht="15.75" customHeight="1">
+    <row r="78" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="13"/>
       <c r="B78" s="14"/>
       <c r="C78" s="13"/>
       <c r="D78" s="14"/>
       <c r="E78" s="14"/>
     </row>
-    <row r="79" ht="15.75" customHeight="1">
+    <row r="79" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="13"/>
       <c r="B79" s="14"/>
       <c r="C79" s="13"/>
       <c r="D79" s="14"/>
       <c r="E79" s="14"/>
     </row>
-    <row r="80" ht="15.75" customHeight="1">
+    <row r="80" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="13"/>
       <c r="B80" s="14"/>
       <c r="C80" s="13"/>
       <c r="D80" s="14"/>
       <c r="E80" s="14"/>
     </row>
-    <row r="81" ht="15.75" customHeight="1">
+    <row r="81" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="13"/>
       <c r="B81" s="14"/>
       <c r="C81" s="13"/>
       <c r="D81" s="14"/>
       <c r="E81" s="14"/>
     </row>
-    <row r="82" ht="15.75" customHeight="1">
+    <row r="82" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="13"/>
       <c r="B82" s="14"/>
       <c r="C82" s="13"/>
       <c r="D82" s="14"/>
       <c r="E82" s="14"/>
     </row>
-    <row r="83" ht="15.75" customHeight="1">
+    <row r="83" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="13"/>
       <c r="B83" s="14"/>
       <c r="C83" s="13"/>
       <c r="D83" s="14"/>
       <c r="E83" s="14"/>
     </row>
-    <row r="84" ht="15.75" customHeight="1">
+    <row r="84" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="13"/>
       <c r="B84" s="14"/>
       <c r="C84" s="13"/>
       <c r="D84" s="14"/>
       <c r="E84" s="14"/>
     </row>
-    <row r="85" ht="15.75" customHeight="1">
+    <row r="85" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="13"/>
       <c r="B85" s="14"/>
       <c r="C85" s="13"/>
       <c r="D85" s="14"/>
       <c r="E85" s="14"/>
     </row>
-    <row r="86" ht="15.75" customHeight="1">
+    <row r="86" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="13"/>
       <c r="B86" s="14"/>
       <c r="C86" s="13"/>
       <c r="D86" s="14"/>
       <c r="E86" s="14"/>
     </row>
-    <row r="87" ht="15.75" customHeight="1">
+    <row r="87" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="13"/>
       <c r="B87" s="14"/>
       <c r="C87" s="13"/>
       <c r="D87" s="14"/>
       <c r="E87" s="14"/>
     </row>
-    <row r="88" ht="15.75" customHeight="1">
+    <row r="88" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="13"/>
       <c r="B88" s="14"/>
       <c r="C88" s="13"/>
       <c r="D88" s="14"/>
       <c r="E88" s="14"/>
     </row>
-    <row r="89" ht="15.75" customHeight="1">
+    <row r="89" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="13"/>
       <c r="B89" s="14"/>
       <c r="C89" s="13"/>
       <c r="D89" s="14"/>
       <c r="E89" s="14"/>
     </row>
-    <row r="90" ht="15.75" customHeight="1">
+    <row r="90" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="13"/>
       <c r="B90" s="14"/>
       <c r="C90" s="13"/>
       <c r="D90" s="14"/>
       <c r="E90" s="14"/>
     </row>
-    <row r="91" ht="15.75" customHeight="1">
+    <row r="91" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="13"/>
       <c r="B91" s="14"/>
       <c r="C91" s="13"/>
       <c r="D91" s="14"/>
       <c r="E91" s="14"/>
     </row>
-    <row r="92" ht="15.75" customHeight="1">
+    <row r="92" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="13"/>
       <c r="B92" s="14"/>
       <c r="C92" s="13"/>
       <c r="D92" s="14"/>
       <c r="E92" s="14"/>
     </row>
-    <row r="93" ht="15.75" customHeight="1">
+    <row r="93" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="13"/>
       <c r="B93" s="14"/>
       <c r="C93" s="13"/>
       <c r="D93" s="14"/>
       <c r="E93" s="14"/>
     </row>
-    <row r="94" ht="15.75" customHeight="1">
+    <row r="94" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="13"/>
       <c r="B94" s="14"/>
       <c r="C94" s="13"/>
       <c r="D94" s="14"/>
       <c r="E94" s="14"/>
     </row>
-    <row r="95" ht="15.75" customHeight="1">
+    <row r="95" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="13"/>
       <c r="B95" s="14"/>
       <c r="C95" s="13"/>
       <c r="D95" s="14"/>
       <c r="E95" s="14"/>
     </row>
-    <row r="96" ht="15.75" customHeight="1">
+    <row r="96" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="13"/>
       <c r="B96" s="14"/>
       <c r="C96" s="13"/>
       <c r="D96" s="14"/>
       <c r="E96" s="14"/>
     </row>
-    <row r="97" ht="15.75" customHeight="1">
+    <row r="97" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="13"/>
       <c r="B97" s="14"/>
       <c r="C97" s="13"/>
       <c r="D97" s="14"/>
       <c r="E97" s="14"/>
     </row>
-    <row r="98" ht="15.75" customHeight="1">
+    <row r="98" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="13"/>
       <c r="B98" s="14"/>
       <c r="C98" s="13"/>
       <c r="D98" s="14"/>
       <c r="E98" s="14"/>
     </row>
-    <row r="99" ht="15.75" customHeight="1">
+    <row r="99" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="13"/>
       <c r="B99" s="14"/>
       <c r="C99" s="13"/>
       <c r="D99" s="14"/>
       <c r="E99" s="14"/>
     </row>
-    <row r="100" ht="15.75" customHeight="1">
+    <row r="100" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="13"/>
       <c r="B100" s="14"/>
       <c r="C100" s="13"/>
       <c r="D100" s="14"/>
       <c r="E100" s="14"/>
     </row>
-    <row r="101" ht="15.75" customHeight="1">
+    <row r="101" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="13"/>
       <c r="B101" s="14"/>
       <c r="C101" s="13"/>
       <c r="D101" s="14"/>
       <c r="E101" s="14"/>
     </row>
-    <row r="102" ht="15.75" customHeight="1">
+    <row r="102" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="13"/>
       <c r="B102" s="14"/>
       <c r="C102" s="13"/>
       <c r="D102" s="14"/>
       <c r="E102" s="14"/>
     </row>
-    <row r="103" ht="15.75" customHeight="1">
+    <row r="103" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" s="13"/>
       <c r="B103" s="14"/>
       <c r="C103" s="13"/>
       <c r="D103" s="14"/>
       <c r="E103" s="14"/>
     </row>
-    <row r="104" ht="15.75" customHeight="1">
+    <row r="104" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="13"/>
       <c r="B104" s="14"/>
       <c r="C104" s="13"/>
       <c r="D104" s="14"/>
       <c r="E104" s="14"/>
     </row>
-    <row r="105" ht="15.75" customHeight="1">
+    <row r="105" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" s="13"/>
       <c r="B105" s="14"/>
       <c r="C105" s="13"/>
       <c r="D105" s="14"/>
       <c r="E105" s="14"/>
     </row>
-    <row r="106" ht="15.75" customHeight="1">
+    <row r="106" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="13"/>
       <c r="B106" s="14"/>
       <c r="C106" s="13"/>
       <c r="D106" s="14"/>
       <c r="E106" s="14"/>
     </row>
-    <row r="107" ht="15.75" customHeight="1">
+    <row r="107" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" s="13"/>
       <c r="B107" s="14"/>
       <c r="C107" s="13"/>
       <c r="D107" s="14"/>
       <c r="E107" s="14"/>
     </row>
-    <row r="108" ht="15.75" customHeight="1">
+    <row r="108" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" s="13"/>
       <c r="B108" s="14"/>
       <c r="C108" s="13"/>
       <c r="D108" s="14"/>
       <c r="E108" s="14"/>
     </row>
-    <row r="109" ht="15.75" customHeight="1">
+    <row r="109" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" s="13"/>
       <c r="B109" s="14"/>
       <c r="C109" s="13"/>
       <c r="D109" s="14"/>
       <c r="E109" s="14"/>
     </row>
-    <row r="110" ht="15.75" customHeight="1">
+    <row r="110" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" s="13"/>
       <c r="B110" s="14"/>
       <c r="C110" s="13"/>
       <c r="D110" s="14"/>
       <c r="E110" s="14"/>
     </row>
-    <row r="111" ht="15.75" customHeight="1">
+    <row r="111" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" s="13"/>
       <c r="B111" s="14"/>
       <c r="C111" s="13"/>
       <c r="D111" s="14"/>
       <c r="E111" s="14"/>
     </row>
-    <row r="112" ht="15.75" customHeight="1">
+    <row r="112" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" s="13"/>
       <c r="B112" s="14"/>
       <c r="C112" s="13"/>
       <c r="D112" s="14"/>
       <c r="E112" s="14"/>
     </row>
-    <row r="113" ht="15.75" customHeight="1">
+    <row r="113" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" s="13"/>
       <c r="B113" s="14"/>
       <c r="C113" s="13"/>
       <c r="D113" s="14"/>
       <c r="E113" s="14"/>
     </row>
-    <row r="114" ht="15.75" customHeight="1">
+    <row r="114" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A114" s="13"/>
       <c r="B114" s="14"/>
       <c r="C114" s="13"/>
       <c r="D114" s="14"/>
       <c r="E114" s="14"/>
     </row>
-    <row r="115" ht="15.75" customHeight="1">
+    <row r="115" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A115" s="13"/>
       <c r="B115" s="14"/>
       <c r="C115" s="13"/>
       <c r="D115" s="14"/>
       <c r="E115" s="14"/>
     </row>
-    <row r="116" ht="15.75" customHeight="1">
+    <row r="116" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A116" s="13"/>
       <c r="B116" s="14"/>
       <c r="C116" s="13"/>
       <c r="D116" s="14"/>
       <c r="E116" s="14"/>
     </row>
-    <row r="117" ht="15.75" customHeight="1">
+    <row r="117" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A117" s="13"/>
       <c r="B117" s="14"/>
       <c r="C117" s="13"/>
       <c r="D117" s="14"/>
       <c r="E117" s="14"/>
     </row>
-    <row r="118" ht="15.75" customHeight="1">
+    <row r="118" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A118" s="13"/>
       <c r="B118" s="14"/>
       <c r="C118" s="13"/>
       <c r="D118" s="14"/>
       <c r="E118" s="14"/>
     </row>
-    <row r="119" ht="15.75" customHeight="1">
+    <row r="119" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A119" s="13"/>
       <c r="B119" s="14"/>
       <c r="C119" s="13"/>
       <c r="D119" s="14"/>
       <c r="E119" s="14"/>
     </row>
-    <row r="120" ht="15.75" customHeight="1">
+    <row r="120" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A120" s="13"/>
       <c r="B120" s="14"/>
       <c r="C120" s="13"/>
       <c r="D120" s="14"/>
       <c r="E120" s="14"/>
     </row>
-    <row r="121" ht="15.75" customHeight="1">
+    <row r="121" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A121" s="13"/>
       <c r="B121" s="14"/>
       <c r="C121" s="13"/>
       <c r="D121" s="14"/>
       <c r="E121" s="14"/>
     </row>
-    <row r="122" ht="15.75" customHeight="1">
+    <row r="122" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A122" s="13"/>
       <c r="B122" s="14"/>
       <c r="C122" s="13"/>
       <c r="D122" s="14"/>
       <c r="E122" s="14"/>
     </row>
-    <row r="123" ht="15.75" customHeight="1">
+    <row r="123" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A123" s="13"/>
       <c r="B123" s="14"/>
       <c r="C123" s="13"/>
       <c r="D123" s="14"/>
       <c r="E123" s="14"/>
     </row>
-    <row r="124" ht="15.75" customHeight="1">
+    <row r="124" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A124" s="13"/>
       <c r="B124" s="14"/>
       <c r="C124" s="13"/>
       <c r="D124" s="14"/>
       <c r="E124" s="14"/>
     </row>
-    <row r="125" ht="15.75" customHeight="1">
+    <row r="125" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A125" s="13"/>
       <c r="B125" s="14"/>
       <c r="C125" s="13"/>
       <c r="D125" s="14"/>
       <c r="E125" s="14"/>
     </row>
-    <row r="126" ht="15.75" customHeight="1">
+    <row r="126" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A126" s="13"/>
       <c r="B126" s="14"/>
       <c r="C126" s="13"/>
       <c r="D126" s="14"/>
       <c r="E126" s="14"/>
     </row>
-    <row r="127" ht="15.75" customHeight="1">
+    <row r="127" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A127" s="13"/>
       <c r="B127" s="14"/>
       <c r="C127" s="13"/>
       <c r="D127" s="14"/>
       <c r="E127" s="14"/>
     </row>
-    <row r="128" ht="15.75" customHeight="1">
+    <row r="128" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A128" s="13"/>
       <c r="B128" s="14"/>
       <c r="C128" s="13"/>
       <c r="D128" s="14"/>
       <c r="E128" s="14"/>
     </row>
-    <row r="129" ht="15.75" customHeight="1">
+    <row r="129" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A129" s="13"/>
       <c r="B129" s="14"/>
       <c r="C129" s="13"/>
       <c r="D129" s="14"/>
       <c r="E129" s="14"/>
     </row>
-    <row r="130" ht="15.75" customHeight="1">
+    <row r="130" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A130" s="13"/>
       <c r="B130" s="14"/>
       <c r="C130" s="13"/>
       <c r="D130" s="14"/>
       <c r="E130" s="14"/>
     </row>
-    <row r="131" ht="15.75" customHeight="1">
+    <row r="131" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A131" s="13"/>
       <c r="B131" s="14"/>
       <c r="C131" s="13"/>
       <c r="D131" s="14"/>
       <c r="E131" s="14"/>
     </row>
-    <row r="132" ht="15.75" customHeight="1">
+    <row r="132" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A132" s="13"/>
       <c r="B132" s="14"/>
       <c r="C132" s="13"/>
       <c r="D132" s="14"/>
       <c r="E132" s="14"/>
     </row>
-    <row r="133" ht="15.75" customHeight="1">
+    <row r="133" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A133" s="13"/>
       <c r="B133" s="14"/>
       <c r="C133" s="13"/>
       <c r="D133" s="14"/>
       <c r="E133" s="14"/>
     </row>
-    <row r="134" ht="15.75" customHeight="1">
+    <row r="134" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A134" s="13"/>
       <c r="B134" s="14"/>
       <c r="C134" s="13"/>
       <c r="D134" s="14"/>
       <c r="E134" s="14"/>
     </row>
-    <row r="135" ht="15.75" customHeight="1">
+    <row r="135" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A135" s="13"/>
       <c r="B135" s="14"/>
       <c r="C135" s="13"/>
       <c r="D135" s="14"/>
       <c r="E135" s="14"/>
     </row>
-    <row r="136" ht="15.75" customHeight="1">
+    <row r="136" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A136" s="13"/>
       <c r="B136" s="14"/>
       <c r="C136" s="13"/>
       <c r="D136" s="14"/>
       <c r="E136" s="14"/>
     </row>
-    <row r="137" ht="15.75" customHeight="1">
+    <row r="137" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A137" s="13"/>
       <c r="B137" s="14"/>
       <c r="C137" s="13"/>
       <c r="D137" s="14"/>
       <c r="E137" s="14"/>
     </row>
-    <row r="138" ht="15.75" customHeight="1">
+    <row r="138" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A138" s="13"/>
       <c r="B138" s="14"/>
       <c r="C138" s="13"/>
       <c r="D138" s="14"/>
       <c r="E138" s="14"/>
     </row>
-    <row r="139" ht="15.75" customHeight="1">
+    <row r="139" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A139" s="13"/>
       <c r="B139" s="14"/>
       <c r="C139" s="13"/>
       <c r="D139" s="14"/>
       <c r="E139" s="14"/>
     </row>
-    <row r="140" ht="15.75" customHeight="1">
+    <row r="140" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A140" s="13"/>
       <c r="B140" s="14"/>
       <c r="C140" s="13"/>
       <c r="D140" s="14"/>
       <c r="E140" s="14"/>
     </row>
-    <row r="141" ht="15.75" customHeight="1">
+    <row r="141" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A141" s="13"/>
       <c r="B141" s="14"/>
       <c r="C141" s="13"/>
       <c r="D141" s="14"/>
       <c r="E141" s="14"/>
     </row>
-    <row r="142" ht="15.75" customHeight="1">
+    <row r="142" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A142" s="13"/>
       <c r="B142" s="14"/>
       <c r="C142" s="13"/>
       <c r="D142" s="14"/>
       <c r="E142" s="14"/>
     </row>
-    <row r="143" ht="15.75" customHeight="1">
+    <row r="143" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A143" s="13"/>
       <c r="B143" s="14"/>
       <c r="C143" s="13"/>
       <c r="D143" s="14"/>
       <c r="E143" s="14"/>
     </row>
-    <row r="144" ht="15.75" customHeight="1">
+    <row r="144" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A144" s="13"/>
       <c r="B144" s="14"/>
       <c r="C144" s="13"/>
       <c r="D144" s="14"/>
       <c r="E144" s="14"/>
     </row>
-    <row r="145" ht="15.75" customHeight="1">
+    <row r="145" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A145" s="13"/>
       <c r="B145" s="14"/>
       <c r="C145" s="13"/>
       <c r="D145" s="14"/>
       <c r="E145" s="14"/>
     </row>
-    <row r="146" ht="15.75" customHeight="1">
+    <row r="146" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A146" s="13"/>
       <c r="B146" s="14"/>
       <c r="C146" s="13"/>
       <c r="D146" s="14"/>
       <c r="E146" s="14"/>
     </row>
-    <row r="147" ht="15.75" customHeight="1">
+    <row r="147" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A147" s="13"/>
       <c r="B147" s="14"/>
       <c r="C147" s="13"/>
       <c r="D147" s="14"/>
       <c r="E147" s="14"/>
     </row>
-    <row r="148" ht="15.75" customHeight="1">
+    <row r="148" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A148" s="13"/>
       <c r="B148" s="14"/>
       <c r="C148" s="13"/>
       <c r="D148" s="14"/>
       <c r="E148" s="14"/>
     </row>
-    <row r="149" ht="15.75" customHeight="1">
+    <row r="149" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A149" s="13"/>
       <c r="B149" s="14"/>
       <c r="C149" s="13"/>
       <c r="D149" s="14"/>
       <c r="E149" s="14"/>
     </row>
-    <row r="150" ht="15.75" customHeight="1">
+    <row r="150" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A150" s="13"/>
       <c r="B150" s="14"/>
       <c r="C150" s="13"/>
       <c r="D150" s="14"/>
       <c r="E150" s="14"/>
     </row>
-    <row r="151" ht="15.75" customHeight="1">
+    <row r="151" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A151" s="13"/>
       <c r="B151" s="14"/>
       <c r="C151" s="13"/>
       <c r="D151" s="14"/>
       <c r="E151" s="14"/>
     </row>
-    <row r="152" ht="15.75" customHeight="1">
+    <row r="152" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A152" s="13"/>
       <c r="B152" s="14"/>
       <c r="C152" s="13"/>
       <c r="D152" s="14"/>
       <c r="E152" s="14"/>
     </row>
-    <row r="153" ht="15.75" customHeight="1">
+    <row r="153" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A153" s="13"/>
       <c r="B153" s="14"/>
       <c r="C153" s="13"/>
       <c r="D153" s="14"/>
       <c r="E153" s="14"/>
     </row>
-    <row r="154" ht="15.75" customHeight="1">
+    <row r="154" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A154" s="13"/>
       <c r="B154" s="14"/>
       <c r="C154" s="13"/>
       <c r="D154" s="14"/>
       <c r="E154" s="14"/>
     </row>
-    <row r="155" ht="15.75" customHeight="1">
+    <row r="155" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A155" s="13"/>
       <c r="B155" s="14"/>
       <c r="C155" s="13"/>
       <c r="D155" s="14"/>
       <c r="E155" s="14"/>
     </row>
-    <row r="156" ht="15.75" customHeight="1">
+    <row r="156" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A156" s="13"/>
       <c r="B156" s="14"/>
       <c r="C156" s="13"/>
       <c r="D156" s="14"/>
       <c r="E156" s="14"/>
     </row>
-    <row r="157" ht="15.75" customHeight="1">
+    <row r="157" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A157" s="13"/>
       <c r="B157" s="14"/>
       <c r="C157" s="13"/>
       <c r="D157" s="14"/>
       <c r="E157" s="14"/>
     </row>
-    <row r="158" ht="15.75" customHeight="1">
+    <row r="158" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A158" s="13"/>
       <c r="B158" s="14"/>
       <c r="C158" s="13"/>
       <c r="D158" s="14"/>
       <c r="E158" s="14"/>
     </row>
-    <row r="159" ht="15.75" customHeight="1">
+    <row r="159" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A159" s="13"/>
       <c r="B159" s="14"/>
       <c r="C159" s="13"/>
       <c r="D159" s="14"/>
       <c r="E159" s="14"/>
     </row>
-    <row r="160" ht="15.75" customHeight="1">
+    <row r="160" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A160" s="13"/>
       <c r="B160" s="14"/>
       <c r="C160" s="13"/>
       <c r="D160" s="14"/>
       <c r="E160" s="14"/>
     </row>
-    <row r="161" ht="15.75" customHeight="1">
+    <row r="161" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A161" s="13"/>
       <c r="B161" s="14"/>
       <c r="C161" s="13"/>
       <c r="D161" s="14"/>
       <c r="E161" s="14"/>
     </row>
-    <row r="162" ht="15.75" customHeight="1">
+    <row r="162" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A162" s="13"/>
       <c r="B162" s="14"/>
       <c r="C162" s="13"/>
       <c r="D162" s="14"/>
       <c r="E162" s="14"/>
     </row>
-    <row r="163" ht="15.75" customHeight="1">
+    <row r="163" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A163" s="13"/>
       <c r="B163" s="14"/>
       <c r="C163" s="13"/>
       <c r="D163" s="14"/>
       <c r="E163" s="14"/>
     </row>
-    <row r="164" ht="15.75" customHeight="1">
+    <row r="164" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A164" s="13"/>
       <c r="B164" s="14"/>
       <c r="C164" s="13"/>
       <c r="D164" s="14"/>
       <c r="E164" s="14"/>
     </row>
-    <row r="165" ht="15.75" customHeight="1">
+    <row r="165" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A165" s="13"/>
       <c r="B165" s="14"/>
       <c r="C165" s="13"/>
       <c r="D165" s="14"/>
       <c r="E165" s="14"/>
     </row>
-    <row r="166" ht="15.75" customHeight="1">
+    <row r="166" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A166" s="13"/>
       <c r="B166" s="14"/>
       <c r="C166" s="13"/>
       <c r="D166" s="14"/>
       <c r="E166" s="14"/>
     </row>
-    <row r="167" ht="15.75" customHeight="1">
+    <row r="167" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A167" s="13"/>
       <c r="B167" s="14"/>
       <c r="C167" s="13"/>
       <c r="D167" s="14"/>
       <c r="E167" s="14"/>
     </row>
-    <row r="168" ht="15.75" customHeight="1">
+    <row r="168" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A168" s="13"/>
       <c r="B168" s="14"/>
       <c r="C168" s="13"/>
       <c r="D168" s="14"/>
       <c r="E168" s="14"/>
     </row>
-    <row r="169" ht="15.75" customHeight="1">
+    <row r="169" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A169" s="13"/>
       <c r="B169" s="14"/>
       <c r="C169" s="13"/>
       <c r="D169" s="14"/>
       <c r="E169" s="14"/>
     </row>
-    <row r="170" ht="15.75" customHeight="1">
+    <row r="170" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A170" s="13"/>
       <c r="B170" s="14"/>
       <c r="C170" s="13"/>
       <c r="D170" s="14"/>
       <c r="E170" s="14"/>
     </row>
-    <row r="171" ht="15.75" customHeight="1">
+    <row r="171" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A171" s="13"/>
       <c r="B171" s="14"/>
       <c r="C171" s="13"/>
       <c r="D171" s="14"/>
       <c r="E171" s="14"/>
     </row>
-    <row r="172" ht="15.75" customHeight="1">
+    <row r="172" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A172" s="13"/>
       <c r="B172" s="14"/>
       <c r="C172" s="13"/>
       <c r="D172" s="14"/>
       <c r="E172" s="14"/>
     </row>
-    <row r="173" ht="15.75" customHeight="1">
+    <row r="173" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A173" s="13"/>
       <c r="B173" s="14"/>
       <c r="C173" s="13"/>
       <c r="D173" s="14"/>
       <c r="E173" s="14"/>
     </row>
-    <row r="174" ht="15.75" customHeight="1">
+    <row r="174" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A174" s="13"/>
       <c r="B174" s="14"/>
       <c r="C174" s="13"/>
       <c r="D174" s="14"/>
       <c r="E174" s="14"/>
     </row>
-    <row r="175" ht="15.75" customHeight="1">
+    <row r="175" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A175" s="13"/>
       <c r="B175" s="14"/>
       <c r="C175" s="13"/>
       <c r="D175" s="14"/>
       <c r="E175" s="14"/>
     </row>
-    <row r="176" ht="15.75" customHeight="1">
+    <row r="176" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A176" s="13"/>
       <c r="B176" s="14"/>
       <c r="C176" s="13"/>
       <c r="D176" s="14"/>
       <c r="E176" s="14"/>
     </row>
-    <row r="177" ht="15.75" customHeight="1">
+    <row r="177" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A177" s="13"/>
       <c r="B177" s="14"/>
       <c r="C177" s="13"/>
       <c r="D177" s="14"/>
       <c r="E177" s="14"/>
     </row>
-    <row r="178" ht="15.75" customHeight="1">
+    <row r="178" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A178" s="13"/>
       <c r="B178" s="14"/>
       <c r="C178" s="13"/>
       <c r="D178" s="14"/>
       <c r="E178" s="14"/>
     </row>
-    <row r="179" ht="15.75" customHeight="1">
+    <row r="179" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A179" s="13"/>
       <c r="B179" s="14"/>
       <c r="C179" s="13"/>
       <c r="D179" s="14"/>
       <c r="E179" s="14"/>
     </row>
-    <row r="180" ht="15.75" customHeight="1">
+    <row r="180" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A180" s="13"/>
       <c r="B180" s="14"/>
       <c r="C180" s="13"/>
       <c r="D180" s="14"/>
       <c r="E180" s="14"/>
     </row>
-    <row r="181" ht="15.75" customHeight="1">
+    <row r="181" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A181" s="13"/>
       <c r="B181" s="14"/>
       <c r="C181" s="13"/>
       <c r="D181" s="14"/>
       <c r="E181" s="14"/>
     </row>
-    <row r="182" ht="15.75" customHeight="1">
+    <row r="182" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A182" s="13"/>
       <c r="B182" s="14"/>
       <c r="C182" s="13"/>
       <c r="D182" s="14"/>
       <c r="E182" s="14"/>
     </row>
-    <row r="183" ht="15.75" customHeight="1">
+    <row r="183" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A183" s="13"/>
       <c r="B183" s="14"/>
       <c r="C183" s="13"/>
       <c r="D183" s="14"/>
       <c r="E183" s="14"/>
     </row>
-    <row r="184" ht="15.75" customHeight="1">
+    <row r="184" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A184" s="13"/>
       <c r="B184" s="14"/>
       <c r="C184" s="13"/>
       <c r="D184" s="14"/>
       <c r="E184" s="14"/>
     </row>
-    <row r="185" ht="15.75" customHeight="1">
+    <row r="185" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A185" s="13"/>
       <c r="B185" s="14"/>
       <c r="C185" s="13"/>
       <c r="D185" s="14"/>
       <c r="E185" s="14"/>
     </row>
-    <row r="186" ht="15.75" customHeight="1">
+    <row r="186" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A186" s="13"/>
       <c r="B186" s="14"/>
       <c r="C186" s="13"/>
       <c r="D186" s="14"/>
       <c r="E186" s="14"/>
     </row>
-    <row r="187" ht="15.75" customHeight="1">
+    <row r="187" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A187" s="13"/>
       <c r="B187" s="14"/>
       <c r="C187" s="13"/>
       <c r="D187" s="14"/>
       <c r="E187" s="14"/>
     </row>
-    <row r="188" ht="15.75" customHeight="1">
+    <row r="188" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A188" s="13"/>
       <c r="B188" s="14"/>
       <c r="C188" s="13"/>
       <c r="D188" s="14"/>
       <c r="E188" s="14"/>
     </row>
-    <row r="189" ht="15.75" customHeight="1">
+    <row r="189" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A189" s="13"/>
       <c r="B189" s="14"/>
       <c r="C189" s="13"/>
       <c r="D189" s="14"/>
       <c r="E189" s="14"/>
     </row>
-    <row r="190" ht="15.75" customHeight="1">
+    <row r="190" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A190" s="13"/>
       <c r="B190" s="14"/>
       <c r="C190" s="13"/>
       <c r="D190" s="14"/>
       <c r="E190" s="14"/>
     </row>
-    <row r="191" ht="15.75" customHeight="1">
+    <row r="191" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A191" s="13"/>
       <c r="B191" s="14"/>
       <c r="C191" s="13"/>
       <c r="D191" s="14"/>
       <c r="E191" s="14"/>
     </row>
-    <row r="192" ht="15.75" customHeight="1">
+    <row r="192" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A192" s="13"/>
       <c r="B192" s="14"/>
       <c r="C192" s="13"/>
       <c r="D192" s="14"/>
       <c r="E192" s="14"/>
     </row>
-    <row r="193" ht="15.75" customHeight="1">
+    <row r="193" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A193" s="13"/>
       <c r="B193" s="14"/>
       <c r="C193" s="13"/>
       <c r="D193" s="14"/>
       <c r="E193" s="14"/>
     </row>
-    <row r="194" ht="15.75" customHeight="1">
+    <row r="194" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A194" s="13"/>
       <c r="B194" s="14"/>
       <c r="C194" s="13"/>
       <c r="D194" s="14"/>
       <c r="E194" s="14"/>
     </row>
-    <row r="195" ht="15.75" customHeight="1">
+    <row r="195" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A195" s="13"/>
       <c r="B195" s="14"/>
       <c r="C195" s="13"/>
       <c r="D195" s="14"/>
       <c r="E195" s="14"/>
     </row>
-    <row r="196" ht="15.75" customHeight="1">
+    <row r="196" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A196" s="13"/>
       <c r="B196" s="14"/>
       <c r="C196" s="13"/>
       <c r="D196" s="14"/>
       <c r="E196" s="14"/>
     </row>
-    <row r="197" ht="15.75" customHeight="1">
+    <row r="197" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A197" s="13"/>
       <c r="B197" s="14"/>
       <c r="C197" s="13"/>
       <c r="D197" s="14"/>
       <c r="E197" s="14"/>
     </row>
-    <row r="198" ht="15.75" customHeight="1">
+    <row r="198" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A198" s="13"/>
       <c r="B198" s="14"/>
       <c r="C198" s="13"/>
       <c r="D198" s="14"/>
       <c r="E198" s="14"/>
     </row>
-    <row r="199" ht="15.75" customHeight="1">
+    <row r="199" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A199" s="13"/>
       <c r="B199" s="14"/>
       <c r="C199" s="13"/>
       <c r="D199" s="14"/>
       <c r="E199" s="14"/>
     </row>
-    <row r="200" ht="15.75" customHeight="1">
+    <row r="200" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A200" s="13"/>
       <c r="B200" s="14"/>
       <c r="C200" s="13"/>
       <c r="D200" s="14"/>
       <c r="E200" s="14"/>
     </row>
-    <row r="201" ht="15.75" customHeight="1">
+    <row r="201" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A201" s="13"/>
       <c r="B201" s="14"/>
       <c r="C201" s="13"/>
       <c r="D201" s="14"/>
       <c r="E201" s="14"/>
     </row>
-    <row r="202" ht="15.75" customHeight="1">
+    <row r="202" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A202" s="13"/>
       <c r="B202" s="14"/>
       <c r="C202" s="13"/>
       <c r="D202" s="14"/>
       <c r="E202" s="14"/>
     </row>
-    <row r="203" ht="15.75" customHeight="1">
+    <row r="203" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A203" s="13"/>
       <c r="B203" s="14"/>
       <c r="C203" s="13"/>
       <c r="D203" s="14"/>
       <c r="E203" s="14"/>
     </row>
-    <row r="204" ht="15.75" customHeight="1">
+    <row r="204" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A204" s="13"/>
       <c r="B204" s="14"/>
       <c r="C204" s="13"/>
       <c r="D204" s="14"/>
       <c r="E204" s="14"/>
     </row>
-    <row r="205" ht="15.75" customHeight="1">
+    <row r="205" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A205" s="13"/>
       <c r="B205" s="14"/>
       <c r="C205" s="13"/>
       <c r="D205" s="14"/>
       <c r="E205" s="14"/>
     </row>
-    <row r="206" ht="15.75" customHeight="1">
+    <row r="206" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A206" s="13"/>
       <c r="B206" s="14"/>
       <c r="C206" s="13"/>
       <c r="D206" s="14"/>
       <c r="E206" s="14"/>
     </row>
-    <row r="207" ht="15.75" customHeight="1">
+    <row r="207" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A207" s="13"/>
       <c r="B207" s="14"/>
       <c r="C207" s="13"/>
       <c r="D207" s="14"/>
       <c r="E207" s="14"/>
     </row>
-    <row r="208" ht="15.75" customHeight="1">
+    <row r="208" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A208" s="13"/>
       <c r="B208" s="14"/>
       <c r="C208" s="13"/>
       <c r="D208" s="14"/>
       <c r="E208" s="14"/>
     </row>
-    <row r="209" ht="15.75" customHeight="1">
+    <row r="209" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A209" s="13"/>
       <c r="B209" s="14"/>
       <c r="C209" s="13"/>
       <c r="D209" s="14"/>
       <c r="E209" s="14"/>
     </row>
-    <row r="210" ht="15.75" customHeight="1">
+    <row r="210" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A210" s="13"/>
       <c r="B210" s="14"/>
       <c r="C210" s="13"/>
       <c r="D210" s="14"/>
       <c r="E210" s="14"/>
     </row>
-    <row r="211" ht="15.75" customHeight="1">
+    <row r="211" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A211" s="13"/>
       <c r="B211" s="14"/>
       <c r="C211" s="13"/>
       <c r="D211" s="14"/>
       <c r="E211" s="14"/>
     </row>
-    <row r="212" ht="15.75" customHeight="1">
+    <row r="212" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A212" s="13"/>
       <c r="B212" s="14"/>
       <c r="C212" s="13"/>
       <c r="D212" s="14"/>
       <c r="E212" s="14"/>
     </row>
-    <row r="213" ht="15.75" customHeight="1">
+    <row r="213" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A213" s="13"/>
       <c r="B213" s="14"/>
       <c r="C213" s="13"/>
       <c r="D213" s="14"/>
       <c r="E213" s="14"/>
     </row>
-    <row r="214" ht="15.75" customHeight="1">
+    <row r="214" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A214" s="13"/>
       <c r="B214" s="14"/>
       <c r="C214" s="13"/>
       <c r="D214" s="14"/>
       <c r="E214" s="14"/>
     </row>
-    <row r="215" ht="15.75" customHeight="1">
+    <row r="215" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A215" s="13"/>
       <c r="B215" s="14"/>
       <c r="C215" s="13"/>
       <c r="D215" s="14"/>
       <c r="E215" s="14"/>
     </row>
-    <row r="216" ht="15.75" customHeight="1">
+    <row r="216" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A216" s="13"/>
       <c r="B216" s="14"/>
       <c r="C216" s="13"/>
       <c r="D216" s="14"/>
       <c r="E216" s="14"/>
     </row>
-    <row r="217" ht="15.75" customHeight="1">
+    <row r="217" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A217" s="13"/>
       <c r="B217" s="14"/>
       <c r="C217" s="13"/>
       <c r="D217" s="14"/>
       <c r="E217" s="14"/>
     </row>
-    <row r="218" ht="15.75" customHeight="1">
+    <row r="218" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A218" s="13"/>
       <c r="B218" s="14"/>
       <c r="C218" s="13"/>
       <c r="D218" s="14"/>
       <c r="E218" s="14"/>
     </row>
-    <row r="219" ht="15.75" customHeight="1">
+    <row r="219" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A219" s="13"/>
       <c r="B219" s="14"/>
       <c r="C219" s="13"/>
       <c r="D219" s="14"/>
       <c r="E219" s="14"/>
     </row>
-    <row r="220" ht="15.75" customHeight="1">
+    <row r="220" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A220" s="13"/>
       <c r="B220" s="14"/>
       <c r="C220" s="13"/>
       <c r="D220" s="14"/>
       <c r="E220" s="14"/>
     </row>
-    <row r="221" ht="15.75" customHeight="1">
+    <row r="221" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A221" s="13"/>
       <c r="B221" s="14"/>
       <c r="C221" s="13"/>
       <c r="D221" s="14"/>
       <c r="E221" s="14"/>
     </row>
-    <row r="222" ht="15.75" customHeight="1">
+    <row r="222" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A222" s="13"/>
       <c r="B222" s="14"/>
       <c r="C222" s="13"/>
       <c r="D222" s="14"/>
       <c r="E222" s="14"/>
     </row>
-    <row r="223" ht="15.75" customHeight="1">
+    <row r="223" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A223" s="13"/>
       <c r="B223" s="14"/>
       <c r="C223" s="13"/>
       <c r="D223" s="14"/>
       <c r="E223" s="14"/>
     </row>
-    <row r="224" ht="15.75" customHeight="1">
+    <row r="224" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A224" s="13"/>
       <c r="B224" s="14"/>
       <c r="C224" s="13"/>
       <c r="D224" s="14"/>
       <c r="E224" s="14"/>
     </row>
-    <row r="225" ht="15.75" customHeight="1">
+    <row r="225" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A225" s="13"/>
       <c r="B225" s="14"/>
       <c r="C225" s="13"/>
       <c r="D225" s="14"/>
       <c r="E225" s="14"/>
     </row>
-    <row r="226" ht="15.75" customHeight="1">
+    <row r="226" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A226" s="13"/>
       <c r="B226" s="14"/>
       <c r="C226" s="13"/>
       <c r="D226" s="14"/>
       <c r="E226" s="14"/>
     </row>
-    <row r="227" ht="15.75" customHeight="1">
+    <row r="227" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A227" s="13"/>
       <c r="B227" s="14"/>
       <c r="C227" s="13"/>
       <c r="D227" s="14"/>
       <c r="E227" s="14"/>
     </row>
-    <row r="228" ht="15.75" customHeight="1">
+    <row r="228" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A228" s="13"/>
       <c r="B228" s="14"/>
       <c r="C228" s="13"/>
       <c r="D228" s="14"/>
       <c r="E228" s="14"/>
     </row>
-    <row r="229" ht="15.75" customHeight="1">
+    <row r="229" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A229" s="13"/>
       <c r="B229" s="14"/>
       <c r="C229" s="13"/>
       <c r="D229" s="14"/>
       <c r="E229" s="14"/>
     </row>
-    <row r="230" ht="15.75" customHeight="1">
+    <row r="230" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A230" s="13"/>
       <c r="B230" s="14"/>
       <c r="C230" s="13"/>
       <c r="D230" s="14"/>
       <c r="E230" s="14"/>
     </row>
-    <row r="231" ht="15.75" customHeight="1">
+    <row r="231" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A231" s="13"/>
       <c r="B231" s="14"/>
       <c r="C231" s="13"/>
       <c r="D231" s="14"/>
       <c r="E231" s="14"/>
     </row>
-    <row r="232" ht="15.75" customHeight="1">
+    <row r="232" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A232" s="13"/>
       <c r="B232" s="14"/>
       <c r="C232" s="13"/>
       <c r="D232" s="14"/>
       <c r="E232" s="14"/>
     </row>
-    <row r="233" ht="15.75" customHeight="1">
+    <row r="233" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A233" s="13"/>
       <c r="B233" s="14"/>
       <c r="C233" s="13"/>
       <c r="D233" s="14"/>
       <c r="E233" s="14"/>
     </row>
-    <row r="234" ht="15.75" customHeight="1">
+    <row r="234" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A234" s="13"/>
       <c r="B234" s="14"/>
       <c r="C234" s="13"/>
       <c r="D234" s="14"/>
       <c r="E234" s="14"/>
     </row>
-    <row r="235" ht="15.75" customHeight="1">
+    <row r="235" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A235" s="13"/>
       <c r="B235" s="14"/>
       <c r="C235" s="13"/>
       <c r="D235" s="14"/>
       <c r="E235" s="14"/>
     </row>
-    <row r="236" ht="15.75" customHeight="1">
+    <row r="236" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A236" s="13"/>
       <c r="B236" s="14"/>
       <c r="C236" s="13"/>
       <c r="D236" s="14"/>
       <c r="E236" s="14"/>
     </row>
-    <row r="237" ht="15.75" customHeight="1">
+    <row r="237" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A237" s="13"/>
       <c r="B237" s="14"/>
       <c r="C237" s="13"/>
       <c r="D237" s="14"/>
       <c r="E237" s="14"/>
     </row>
-    <row r="238" ht="15.75" customHeight="1">
+    <row r="238" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A238" s="13"/>
       <c r="B238" s="14"/>
       <c r="C238" s="13"/>
       <c r="D238" s="14"/>
       <c r="E238" s="14"/>
     </row>
-    <row r="239" ht="15.75" customHeight="1">
+    <row r="239" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A239" s="13"/>
       <c r="B239" s="14"/>
       <c r="C239" s="13"/>
       <c r="D239" s="14"/>
       <c r="E239" s="14"/>
     </row>
-    <row r="240" ht="15.75" customHeight="1">
+    <row r="240" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A240" s="13"/>
       <c r="B240" s="14"/>
       <c r="C240" s="13"/>
       <c r="D240" s="14"/>
       <c r="E240" s="14"/>
     </row>
-    <row r="241" ht="15.75" customHeight="1">
+    <row r="241" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A241" s="13"/>
       <c r="B241" s="14"/>
       <c r="C241" s="13"/>
       <c r="D241" s="14"/>
       <c r="E241" s="14"/>
     </row>
-    <row r="242" ht="15.75" customHeight="1">
+    <row r="242" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A242" s="13"/>
       <c r="B242" s="14"/>
       <c r="C242" s="13"/>
       <c r="D242" s="14"/>
       <c r="E242" s="14"/>
     </row>
-    <row r="243" ht="15.75" customHeight="1">
+    <row r="243" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A243" s="13"/>
       <c r="B243" s="14"/>
       <c r="C243" s="13"/>
       <c r="D243" s="14"/>
       <c r="E243" s="14"/>
     </row>
-    <row r="244" ht="15.75" customHeight="1">
+    <row r="244" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A244" s="13"/>
       <c r="B244" s="14"/>
       <c r="C244" s="13"/>
       <c r="D244" s="14"/>
       <c r="E244" s="14"/>
     </row>
-    <row r="245" ht="15.75" customHeight="1">
+    <row r="245" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A245" s="13"/>
       <c r="B245" s="14"/>
       <c r="C245" s="13"/>
       <c r="D245" s="14"/>
       <c r="E245" s="14"/>
     </row>
-    <row r="246" ht="15.75" customHeight="1">
+    <row r="246" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A246" s="13"/>
       <c r="B246" s="14"/>
       <c r="C246" s="13"/>
       <c r="D246" s="14"/>
       <c r="E246" s="14"/>
     </row>
-    <row r="247" ht="15.75" customHeight="1">
+    <row r="247" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A247" s="13"/>
       <c r="B247" s="14"/>
       <c r="C247" s="13"/>
       <c r="D247" s="14"/>
       <c r="E247" s="14"/>
     </row>
-    <row r="248" ht="15.75" customHeight="1">
+    <row r="248" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A248" s="13"/>
       <c r="B248" s="14"/>
       <c r="C248" s="13"/>
       <c r="D248" s="14"/>
       <c r="E248" s="14"/>
     </row>
-    <row r="249" ht="15.75" customHeight="1">
+    <row r="249" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A249" s="13"/>
       <c r="B249" s="14"/>
       <c r="C249" s="13"/>
       <c r="D249" s="14"/>
       <c r="E249" s="14"/>
     </row>
-    <row r="250" ht="15.75" customHeight="1">
+    <row r="250" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A250" s="13"/>
       <c r="B250" s="14"/>
       <c r="C250" s="13"/>
       <c r="D250" s="14"/>
       <c r="E250" s="14"/>
     </row>
-    <row r="251" ht="15.75" customHeight="1">
+    <row r="251" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A251" s="13"/>
       <c r="B251" s="14"/>
       <c r="C251" s="13"/>
       <c r="D251" s="14"/>
       <c r="E251" s="14"/>
     </row>
-    <row r="252" ht="15.75" customHeight="1">
+    <row r="252" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A252" s="13"/>
       <c r="B252" s="14"/>
       <c r="C252" s="13"/>
       <c r="D252" s="14"/>
       <c r="E252" s="14"/>
     </row>
-    <row r="253" ht="15.75" customHeight="1">
+    <row r="253" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A253" s="13"/>
       <c r="B253" s="14"/>
       <c r="C253" s="13"/>
       <c r="D253" s="14"/>
       <c r="E253" s="14"/>
     </row>
-    <row r="254" ht="15.75" customHeight="1">
+    <row r="254" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A254" s="13"/>
       <c r="B254" s="14"/>
       <c r="C254" s="13"/>
       <c r="D254" s="14"/>
       <c r="E254" s="14"/>
     </row>
-    <row r="255" ht="15.75" customHeight="1">
+    <row r="255" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A255" s="13"/>
       <c r="B255" s="14"/>
       <c r="C255" s="13"/>
       <c r="D255" s="14"/>
       <c r="E255" s="14"/>
     </row>
-    <row r="256" ht="15.75" customHeight="1">
+    <row r="256" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A256" s="13"/>
       <c r="B256" s="14"/>
       <c r="C256" s="13"/>
       <c r="D256" s="14"/>
       <c r="E256" s="14"/>
     </row>
-    <row r="257" ht="15.75" customHeight="1">
+    <row r="257" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A257" s="13"/>
       <c r="B257" s="14"/>
       <c r="C257" s="13"/>
       <c r="D257" s="14"/>
       <c r="E257" s="14"/>
     </row>
-    <row r="258" ht="15.75" customHeight="1">
+    <row r="258" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A258" s="13"/>
       <c r="B258" s="14"/>
       <c r="C258" s="13"/>
       <c r="D258" s="14"/>
       <c r="E258" s="14"/>
     </row>
-    <row r="259" ht="15.75" customHeight="1">
+    <row r="259" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A259" s="13"/>
       <c r="B259" s="14"/>
       <c r="C259" s="13"/>
       <c r="D259" s="14"/>
       <c r="E259" s="14"/>
     </row>
-    <row r="260" ht="15.75" customHeight="1">
+    <row r="260" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A260" s="13"/>
       <c r="B260" s="14"/>
       <c r="C260" s="13"/>
       <c r="D260" s="14"/>
       <c r="E260" s="14"/>
     </row>
-    <row r="261" ht="15.75" customHeight="1"/>
-    <row r="262" ht="15.75" customHeight="1"/>
-    <row r="263" ht="15.75" customHeight="1"/>
-    <row r="264" ht="15.75" customHeight="1"/>
-    <row r="265" ht="15.75" customHeight="1"/>
-    <row r="266" ht="15.75" customHeight="1"/>
-    <row r="267" ht="15.75" customHeight="1"/>
-    <row r="268" ht="15.75" customHeight="1"/>
-    <row r="269" ht="15.75" customHeight="1"/>
-    <row r="270" ht="15.75" customHeight="1"/>
-    <row r="271" ht="15.75" customHeight="1"/>
-    <row r="272" ht="15.75" customHeight="1"/>
-    <row r="273" ht="15.75" customHeight="1"/>
-    <row r="274" ht="15.75" customHeight="1"/>
-    <row r="275" ht="15.75" customHeight="1"/>
-    <row r="276" ht="15.75" customHeight="1"/>
-    <row r="277" ht="15.75" customHeight="1"/>
-    <row r="278" ht="15.75" customHeight="1"/>
-    <row r="279" ht="15.75" customHeight="1"/>
-    <row r="280" ht="15.75" customHeight="1"/>
-    <row r="281" ht="15.75" customHeight="1"/>
-    <row r="282" ht="15.75" customHeight="1"/>
-    <row r="283" ht="15.75" customHeight="1"/>
-    <row r="284" ht="15.75" customHeight="1"/>
-    <row r="285" ht="15.75" customHeight="1"/>
-    <row r="286" ht="15.75" customHeight="1"/>
-    <row r="287" ht="15.75" customHeight="1"/>
-    <row r="288" ht="15.75" customHeight="1"/>
-    <row r="289" ht="15.75" customHeight="1"/>
-    <row r="290" ht="15.75" customHeight="1"/>
-    <row r="291" ht="15.75" customHeight="1"/>
-    <row r="292" ht="15.75" customHeight="1"/>
-    <row r="293" ht="15.75" customHeight="1"/>
-    <row r="294" ht="15.75" customHeight="1"/>
-    <row r="295" ht="15.75" customHeight="1"/>
-    <row r="296" ht="15.75" customHeight="1"/>
-    <row r="297" ht="15.75" customHeight="1"/>
-    <row r="298" ht="15.75" customHeight="1"/>
-    <row r="299" ht="15.75" customHeight="1"/>
-    <row r="300" ht="15.75" customHeight="1"/>
-    <row r="301" ht="15.75" customHeight="1"/>
-    <row r="302" ht="15.75" customHeight="1"/>
-    <row r="303" ht="15.75" customHeight="1"/>
-    <row r="304" ht="15.75" customHeight="1"/>
-    <row r="305" ht="15.75" customHeight="1"/>
-    <row r="306" ht="15.75" customHeight="1"/>
-    <row r="307" ht="15.75" customHeight="1"/>
-    <row r="308" ht="15.75" customHeight="1"/>
-    <row r="309" ht="15.75" customHeight="1"/>
-    <row r="310" ht="15.75" customHeight="1"/>
-    <row r="311" ht="15.75" customHeight="1"/>
-    <row r="312" ht="15.75" customHeight="1"/>
-    <row r="313" ht="15.75" customHeight="1"/>
-    <row r="314" ht="15.75" customHeight="1"/>
-    <row r="315" ht="15.75" customHeight="1"/>
-    <row r="316" ht="15.75" customHeight="1"/>
-    <row r="317" ht="15.75" customHeight="1"/>
-    <row r="318" ht="15.75" customHeight="1"/>
-    <row r="319" ht="15.75" customHeight="1"/>
-    <row r="320" ht="15.75" customHeight="1"/>
-    <row r="321" ht="15.75" customHeight="1"/>
-    <row r="322" ht="15.75" customHeight="1"/>
-    <row r="323" ht="15.75" customHeight="1"/>
-    <row r="324" ht="15.75" customHeight="1"/>
-    <row r="325" ht="15.75" customHeight="1"/>
-    <row r="326" ht="15.75" customHeight="1"/>
-    <row r="327" ht="15.75" customHeight="1"/>
-    <row r="328" ht="15.75" customHeight="1"/>
-    <row r="329" ht="15.75" customHeight="1"/>
-    <row r="330" ht="15.75" customHeight="1"/>
-    <row r="331" ht="15.75" customHeight="1"/>
-    <row r="332" ht="15.75" customHeight="1"/>
-    <row r="333" ht="15.75" customHeight="1"/>
-    <row r="334" ht="15.75" customHeight="1"/>
-    <row r="335" ht="15.75" customHeight="1"/>
-    <row r="336" ht="15.75" customHeight="1"/>
-    <row r="337" ht="15.75" customHeight="1"/>
-    <row r="338" ht="15.75" customHeight="1"/>
-    <row r="339" ht="15.75" customHeight="1"/>
-    <row r="340" ht="15.75" customHeight="1"/>
-    <row r="341" ht="15.75" customHeight="1"/>
-    <row r="342" ht="15.75" customHeight="1"/>
-    <row r="343" ht="15.75" customHeight="1"/>
-    <row r="344" ht="15.75" customHeight="1"/>
-    <row r="345" ht="15.75" customHeight="1"/>
-    <row r="346" ht="15.75" customHeight="1"/>
-    <row r="347" ht="15.75" customHeight="1"/>
-    <row r="348" ht="15.75" customHeight="1"/>
-    <row r="349" ht="15.75" customHeight="1"/>
-    <row r="350" ht="15.75" customHeight="1"/>
-    <row r="351" ht="15.75" customHeight="1"/>
-    <row r="352" ht="15.75" customHeight="1"/>
-    <row r="353" ht="15.75" customHeight="1"/>
-    <row r="354" ht="15.75" customHeight="1"/>
-    <row r="355" ht="15.75" customHeight="1"/>
-    <row r="356" ht="15.75" customHeight="1"/>
-    <row r="357" ht="15.75" customHeight="1"/>
-    <row r="358" ht="15.75" customHeight="1"/>
-    <row r="359" ht="15.75" customHeight="1"/>
-    <row r="360" ht="15.75" customHeight="1"/>
-    <row r="361" ht="15.75" customHeight="1"/>
-    <row r="362" ht="15.75" customHeight="1"/>
-    <row r="363" ht="15.75" customHeight="1"/>
-    <row r="364" ht="15.75" customHeight="1"/>
-    <row r="365" ht="15.75" customHeight="1"/>
-    <row r="366" ht="15.75" customHeight="1"/>
-    <row r="367" ht="15.75" customHeight="1"/>
-    <row r="368" ht="15.75" customHeight="1"/>
-    <row r="369" ht="15.75" customHeight="1"/>
-    <row r="370" ht="15.75" customHeight="1"/>
-    <row r="371" ht="15.75" customHeight="1"/>
-    <row r="372" ht="15.75" customHeight="1"/>
-    <row r="373" ht="15.75" customHeight="1"/>
-    <row r="374" ht="15.75" customHeight="1"/>
-    <row r="375" ht="15.75" customHeight="1"/>
-    <row r="376" ht="15.75" customHeight="1"/>
-    <row r="377" ht="15.75" customHeight="1"/>
-    <row r="378" ht="15.75" customHeight="1"/>
-    <row r="379" ht="15.75" customHeight="1"/>
-    <row r="380" ht="15.75" customHeight="1"/>
-    <row r="381" ht="15.75" customHeight="1"/>
-    <row r="382" ht="15.75" customHeight="1"/>
-    <row r="383" ht="15.75" customHeight="1"/>
-    <row r="384" ht="15.75" customHeight="1"/>
-    <row r="385" ht="15.75" customHeight="1"/>
-    <row r="386" ht="15.75" customHeight="1"/>
-    <row r="387" ht="15.75" customHeight="1"/>
-    <row r="388" ht="15.75" customHeight="1"/>
-    <row r="389" ht="15.75" customHeight="1"/>
-    <row r="390" ht="15.75" customHeight="1"/>
-    <row r="391" ht="15.75" customHeight="1"/>
-    <row r="392" ht="15.75" customHeight="1"/>
-    <row r="393" ht="15.75" customHeight="1"/>
-    <row r="394" ht="15.75" customHeight="1"/>
-    <row r="395" ht="15.75" customHeight="1"/>
-    <row r="396" ht="15.75" customHeight="1"/>
-    <row r="397" ht="15.75" customHeight="1"/>
-    <row r="398" ht="15.75" customHeight="1"/>
-    <row r="399" ht="15.75" customHeight="1"/>
-    <row r="400" ht="15.75" customHeight="1"/>
-    <row r="401" ht="15.75" customHeight="1"/>
-    <row r="402" ht="15.75" customHeight="1"/>
-    <row r="403" ht="15.75" customHeight="1"/>
-    <row r="404" ht="15.75" customHeight="1"/>
-    <row r="405" ht="15.75" customHeight="1"/>
-    <row r="406" ht="15.75" customHeight="1"/>
-    <row r="407" ht="15.75" customHeight="1"/>
-    <row r="408" ht="15.75" customHeight="1"/>
-    <row r="409" ht="15.75" customHeight="1"/>
-    <row r="410" ht="15.75" customHeight="1"/>
-    <row r="411" ht="15.75" customHeight="1"/>
-    <row r="412" ht="15.75" customHeight="1"/>
-    <row r="413" ht="15.75" customHeight="1"/>
-    <row r="414" ht="15.75" customHeight="1"/>
-    <row r="415" ht="15.75" customHeight="1"/>
-    <row r="416" ht="15.75" customHeight="1"/>
-    <row r="417" ht="15.75" customHeight="1"/>
-    <row r="418" ht="15.75" customHeight="1"/>
-    <row r="419" ht="15.75" customHeight="1"/>
-    <row r="420" ht="15.75" customHeight="1"/>
-    <row r="421" ht="15.75" customHeight="1"/>
-    <row r="422" ht="15.75" customHeight="1"/>
-    <row r="423" ht="15.75" customHeight="1"/>
-    <row r="424" ht="15.75" customHeight="1"/>
-    <row r="425" ht="15.75" customHeight="1"/>
-    <row r="426" ht="15.75" customHeight="1"/>
-    <row r="427" ht="15.75" customHeight="1"/>
-    <row r="428" ht="15.75" customHeight="1"/>
-    <row r="429" ht="15.75" customHeight="1"/>
-    <row r="430" ht="15.75" customHeight="1"/>
-    <row r="431" ht="15.75" customHeight="1"/>
-    <row r="432" ht="15.75" customHeight="1"/>
-    <row r="433" ht="15.75" customHeight="1"/>
-    <row r="434" ht="15.75" customHeight="1"/>
-    <row r="435" ht="15.75" customHeight="1"/>
-    <row r="436" ht="15.75" customHeight="1"/>
-    <row r="437" ht="15.75" customHeight="1"/>
-    <row r="438" ht="15.75" customHeight="1"/>
-    <row r="439" ht="15.75" customHeight="1"/>
-    <row r="440" ht="15.75" customHeight="1"/>
-    <row r="441" ht="15.75" customHeight="1"/>
-    <row r="442" ht="15.75" customHeight="1"/>
-    <row r="443" ht="15.75" customHeight="1"/>
-    <row r="444" ht="15.75" customHeight="1"/>
-    <row r="445" ht="15.75" customHeight="1"/>
-    <row r="446" ht="15.75" customHeight="1"/>
-    <row r="447" ht="15.75" customHeight="1"/>
-    <row r="448" ht="15.75" customHeight="1"/>
-    <row r="449" ht="15.75" customHeight="1"/>
-    <row r="450" ht="15.75" customHeight="1"/>
-    <row r="451" ht="15.75" customHeight="1"/>
-    <row r="452" ht="15.75" customHeight="1"/>
-    <row r="453" ht="15.75" customHeight="1"/>
-    <row r="454" ht="15.75" customHeight="1"/>
-    <row r="455" ht="15.75" customHeight="1"/>
-    <row r="456" ht="15.75" customHeight="1"/>
-    <row r="457" ht="15.75" customHeight="1"/>
-    <row r="458" ht="15.75" customHeight="1"/>
-    <row r="459" ht="15.75" customHeight="1"/>
-    <row r="460" ht="15.75" customHeight="1"/>
-    <row r="461" ht="15.75" customHeight="1"/>
-    <row r="462" ht="15.75" customHeight="1"/>
-    <row r="463" ht="15.75" customHeight="1"/>
-    <row r="464" ht="15.75" customHeight="1"/>
-    <row r="465" ht="15.75" customHeight="1"/>
-    <row r="466" ht="15.75" customHeight="1"/>
-    <row r="467" ht="15.75" customHeight="1"/>
-    <row r="468" ht="15.75" customHeight="1"/>
-    <row r="469" ht="15.75" customHeight="1"/>
-    <row r="470" ht="15.75" customHeight="1"/>
-    <row r="471" ht="15.75" customHeight="1"/>
-    <row r="472" ht="15.75" customHeight="1"/>
-    <row r="473" ht="15.75" customHeight="1"/>
-    <row r="474" ht="15.75" customHeight="1"/>
-    <row r="475" ht="15.75" customHeight="1"/>
-    <row r="476" ht="15.75" customHeight="1"/>
-    <row r="477" ht="15.75" customHeight="1"/>
-    <row r="478" ht="15.75" customHeight="1"/>
-    <row r="479" ht="15.75" customHeight="1"/>
-    <row r="480" ht="15.75" customHeight="1"/>
-    <row r="481" ht="15.75" customHeight="1"/>
-    <row r="482" ht="15.75" customHeight="1"/>
-    <row r="483" ht="15.75" customHeight="1"/>
-    <row r="484" ht="15.75" customHeight="1"/>
-    <row r="485" ht="15.75" customHeight="1"/>
-    <row r="486" ht="15.75" customHeight="1"/>
-    <row r="487" ht="15.75" customHeight="1"/>
-    <row r="488" ht="15.75" customHeight="1"/>
-    <row r="489" ht="15.75" customHeight="1"/>
-    <row r="490" ht="15.75" customHeight="1"/>
-    <row r="491" ht="15.75" customHeight="1"/>
-    <row r="492" ht="15.75" customHeight="1"/>
-    <row r="493" ht="15.75" customHeight="1"/>
-    <row r="494" ht="15.75" customHeight="1"/>
-    <row r="495" ht="15.75" customHeight="1"/>
-    <row r="496" ht="15.75" customHeight="1"/>
-    <row r="497" ht="15.75" customHeight="1"/>
-    <row r="498" ht="15.75" customHeight="1"/>
-    <row r="499" ht="15.75" customHeight="1"/>
-    <row r="500" ht="15.75" customHeight="1"/>
-    <row r="501" ht="15.75" customHeight="1"/>
-    <row r="502" ht="15.75" customHeight="1"/>
-    <row r="503" ht="15.75" customHeight="1"/>
-    <row r="504" ht="15.75" customHeight="1"/>
-    <row r="505" ht="15.75" customHeight="1"/>
-    <row r="506" ht="15.75" customHeight="1"/>
-    <row r="507" ht="15.75" customHeight="1"/>
-    <row r="508" ht="15.75" customHeight="1"/>
-    <row r="509" ht="15.75" customHeight="1"/>
-    <row r="510" ht="15.75" customHeight="1"/>
-    <row r="511" ht="15.75" customHeight="1"/>
-    <row r="512" ht="15.75" customHeight="1"/>
-    <row r="513" ht="15.75" customHeight="1"/>
-    <row r="514" ht="15.75" customHeight="1"/>
-    <row r="515" ht="15.75" customHeight="1"/>
-    <row r="516" ht="15.75" customHeight="1"/>
-    <row r="517" ht="15.75" customHeight="1"/>
-    <row r="518" ht="15.75" customHeight="1"/>
-    <row r="519" ht="15.75" customHeight="1"/>
-    <row r="520" ht="15.75" customHeight="1"/>
-    <row r="521" ht="15.75" customHeight="1"/>
-    <row r="522" ht="15.75" customHeight="1"/>
-    <row r="523" ht="15.75" customHeight="1"/>
-    <row r="524" ht="15.75" customHeight="1"/>
-    <row r="525" ht="15.75" customHeight="1"/>
-    <row r="526" ht="15.75" customHeight="1"/>
-    <row r="527" ht="15.75" customHeight="1"/>
-    <row r="528" ht="15.75" customHeight="1"/>
-    <row r="529" ht="15.75" customHeight="1"/>
-    <row r="530" ht="15.75" customHeight="1"/>
-    <row r="531" ht="15.75" customHeight="1"/>
-    <row r="532" ht="15.75" customHeight="1"/>
-    <row r="533" ht="15.75" customHeight="1"/>
-    <row r="534" ht="15.75" customHeight="1"/>
-    <row r="535" ht="15.75" customHeight="1"/>
-    <row r="536" ht="15.75" customHeight="1"/>
-    <row r="537" ht="15.75" customHeight="1"/>
-    <row r="538" ht="15.75" customHeight="1"/>
-    <row r="539" ht="15.75" customHeight="1"/>
-    <row r="540" ht="15.75" customHeight="1"/>
-    <row r="541" ht="15.75" customHeight="1"/>
-    <row r="542" ht="15.75" customHeight="1"/>
-    <row r="543" ht="15.75" customHeight="1"/>
-    <row r="544" ht="15.75" customHeight="1"/>
-    <row r="545" ht="15.75" customHeight="1"/>
-    <row r="546" ht="15.75" customHeight="1"/>
-    <row r="547" ht="15.75" customHeight="1"/>
-    <row r="548" ht="15.75" customHeight="1"/>
-    <row r="549" ht="15.75" customHeight="1"/>
-    <row r="550" ht="15.75" customHeight="1"/>
-    <row r="551" ht="15.75" customHeight="1"/>
-    <row r="552" ht="15.75" customHeight="1"/>
-    <row r="553" ht="15.75" customHeight="1"/>
-    <row r="554" ht="15.75" customHeight="1"/>
-    <row r="555" ht="15.75" customHeight="1"/>
-    <row r="556" ht="15.75" customHeight="1"/>
-    <row r="557" ht="15.75" customHeight="1"/>
-    <row r="558" ht="15.75" customHeight="1"/>
-    <row r="559" ht="15.75" customHeight="1"/>
-    <row r="560" ht="15.75" customHeight="1"/>
-    <row r="561" ht="15.75" customHeight="1"/>
-    <row r="562" ht="15.75" customHeight="1"/>
-    <row r="563" ht="15.75" customHeight="1"/>
-    <row r="564" ht="15.75" customHeight="1"/>
-    <row r="565" ht="15.75" customHeight="1"/>
-    <row r="566" ht="15.75" customHeight="1"/>
-    <row r="567" ht="15.75" customHeight="1"/>
-    <row r="568" ht="15.75" customHeight="1"/>
-    <row r="569" ht="15.75" customHeight="1"/>
-    <row r="570" ht="15.75" customHeight="1"/>
-    <row r="571" ht="15.75" customHeight="1"/>
-    <row r="572" ht="15.75" customHeight="1"/>
-    <row r="573" ht="15.75" customHeight="1"/>
-    <row r="574" ht="15.75" customHeight="1"/>
-    <row r="575" ht="15.75" customHeight="1"/>
-    <row r="576" ht="15.75" customHeight="1"/>
-    <row r="577" ht="15.75" customHeight="1"/>
-    <row r="578" ht="15.75" customHeight="1"/>
-    <row r="579" ht="15.75" customHeight="1"/>
-    <row r="580" ht="15.75" customHeight="1"/>
-    <row r="581" ht="15.75" customHeight="1"/>
-    <row r="582" ht="15.75" customHeight="1"/>
-    <row r="583" ht="15.75" customHeight="1"/>
-    <row r="584" ht="15.75" customHeight="1"/>
-    <row r="585" ht="15.75" customHeight="1"/>
-    <row r="586" ht="15.75" customHeight="1"/>
-    <row r="587" ht="15.75" customHeight="1"/>
-    <row r="588" ht="15.75" customHeight="1"/>
-    <row r="589" ht="15.75" customHeight="1"/>
-    <row r="590" ht="15.75" customHeight="1"/>
-    <row r="591" ht="15.75" customHeight="1"/>
-    <row r="592" ht="15.75" customHeight="1"/>
-    <row r="593" ht="15.75" customHeight="1"/>
-    <row r="594" ht="15.75" customHeight="1"/>
-    <row r="595" ht="15.75" customHeight="1"/>
-    <row r="596" ht="15.75" customHeight="1"/>
-    <row r="597" ht="15.75" customHeight="1"/>
-    <row r="598" ht="15.75" customHeight="1"/>
-    <row r="599" ht="15.75" customHeight="1"/>
-    <row r="600" ht="15.75" customHeight="1"/>
-    <row r="601" ht="15.75" customHeight="1"/>
-    <row r="602" ht="15.75" customHeight="1"/>
-    <row r="603" ht="15.75" customHeight="1"/>
-    <row r="604" ht="15.75" customHeight="1"/>
-    <row r="605" ht="15.75" customHeight="1"/>
-    <row r="606" ht="15.75" customHeight="1"/>
-    <row r="607" ht="15.75" customHeight="1"/>
-    <row r="608" ht="15.75" customHeight="1"/>
-    <row r="609" ht="15.75" customHeight="1"/>
-    <row r="610" ht="15.75" customHeight="1"/>
-    <row r="611" ht="15.75" customHeight="1"/>
-    <row r="612" ht="15.75" customHeight="1"/>
-    <row r="613" ht="15.75" customHeight="1"/>
-    <row r="614" ht="15.75" customHeight="1"/>
-    <row r="615" ht="15.75" customHeight="1"/>
-    <row r="616" ht="15.75" customHeight="1"/>
-    <row r="617" ht="15.75" customHeight="1"/>
-    <row r="618" ht="15.75" customHeight="1"/>
-    <row r="619" ht="15.75" customHeight="1"/>
-    <row r="620" ht="15.75" customHeight="1"/>
-    <row r="621" ht="15.75" customHeight="1"/>
-    <row r="622" ht="15.75" customHeight="1"/>
-    <row r="623" ht="15.75" customHeight="1"/>
-    <row r="624" ht="15.75" customHeight="1"/>
-    <row r="625" ht="15.75" customHeight="1"/>
-    <row r="626" ht="15.75" customHeight="1"/>
-    <row r="627" ht="15.75" customHeight="1"/>
-    <row r="628" ht="15.75" customHeight="1"/>
-    <row r="629" ht="15.75" customHeight="1"/>
-    <row r="630" ht="15.75" customHeight="1"/>
-    <row r="631" ht="15.75" customHeight="1"/>
-    <row r="632" ht="15.75" customHeight="1"/>
-    <row r="633" ht="15.75" customHeight="1"/>
-    <row r="634" ht="15.75" customHeight="1"/>
-    <row r="635" ht="15.75" customHeight="1"/>
-    <row r="636" ht="15.75" customHeight="1"/>
-    <row r="637" ht="15.75" customHeight="1"/>
-    <row r="638" ht="15.75" customHeight="1"/>
-    <row r="639" ht="15.75" customHeight="1"/>
-    <row r="640" ht="15.75" customHeight="1"/>
-    <row r="641" ht="15.75" customHeight="1"/>
-    <row r="642" ht="15.75" customHeight="1"/>
-    <row r="643" ht="15.75" customHeight="1"/>
-    <row r="644" ht="15.75" customHeight="1"/>
-    <row r="645" ht="15.75" customHeight="1"/>
-    <row r="646" ht="15.75" customHeight="1"/>
-    <row r="647" ht="15.75" customHeight="1"/>
-    <row r="648" ht="15.75" customHeight="1"/>
-    <row r="649" ht="15.75" customHeight="1"/>
-    <row r="650" ht="15.75" customHeight="1"/>
-    <row r="651" ht="15.75" customHeight="1"/>
-    <row r="652" ht="15.75" customHeight="1"/>
-    <row r="653" ht="15.75" customHeight="1"/>
-    <row r="654" ht="15.75" customHeight="1"/>
-    <row r="655" ht="15.75" customHeight="1"/>
-    <row r="656" ht="15.75" customHeight="1"/>
-    <row r="657" ht="15.75" customHeight="1"/>
-    <row r="658" ht="15.75" customHeight="1"/>
-    <row r="659" ht="15.75" customHeight="1"/>
-    <row r="660" ht="15.75" customHeight="1"/>
-    <row r="661" ht="15.75" customHeight="1"/>
-    <row r="662" ht="15.75" customHeight="1"/>
-    <row r="663" ht="15.75" customHeight="1"/>
-    <row r="664" ht="15.75" customHeight="1"/>
-    <row r="665" ht="15.75" customHeight="1"/>
-    <row r="666" ht="15.75" customHeight="1"/>
-    <row r="667" ht="15.75" customHeight="1"/>
-    <row r="668" ht="15.75" customHeight="1"/>
-    <row r="669" ht="15.75" customHeight="1"/>
-    <row r="670" ht="15.75" customHeight="1"/>
-    <row r="671" ht="15.75" customHeight="1"/>
-    <row r="672" ht="15.75" customHeight="1"/>
-    <row r="673" ht="15.75" customHeight="1"/>
-    <row r="674" ht="15.75" customHeight="1"/>
-    <row r="675" ht="15.75" customHeight="1"/>
-    <row r="676" ht="15.75" customHeight="1"/>
-    <row r="677" ht="15.75" customHeight="1"/>
-    <row r="678" ht="15.75" customHeight="1"/>
-    <row r="679" ht="15.75" customHeight="1"/>
-    <row r="680" ht="15.75" customHeight="1"/>
-    <row r="681" ht="15.75" customHeight="1"/>
-    <row r="682" ht="15.75" customHeight="1"/>
-    <row r="683" ht="15.75" customHeight="1"/>
-    <row r="684" ht="15.75" customHeight="1"/>
-    <row r="685" ht="15.75" customHeight="1"/>
-    <row r="686" ht="15.75" customHeight="1"/>
-    <row r="687" ht="15.75" customHeight="1"/>
-    <row r="688" ht="15.75" customHeight="1"/>
-    <row r="689" ht="15.75" customHeight="1"/>
-    <row r="690" ht="15.75" customHeight="1"/>
-    <row r="691" ht="15.75" customHeight="1"/>
-    <row r="692" ht="15.75" customHeight="1"/>
-    <row r="693" ht="15.75" customHeight="1"/>
-    <row r="694" ht="15.75" customHeight="1"/>
-    <row r="695" ht="15.75" customHeight="1"/>
-    <row r="696" ht="15.75" customHeight="1"/>
-    <row r="697" ht="15.75" customHeight="1"/>
-    <row r="698" ht="15.75" customHeight="1"/>
-    <row r="699" ht="15.75" customHeight="1"/>
-    <row r="700" ht="15.75" customHeight="1"/>
-    <row r="701" ht="15.75" customHeight="1"/>
-    <row r="702" ht="15.75" customHeight="1"/>
-    <row r="703" ht="15.75" customHeight="1"/>
-    <row r="704" ht="15.75" customHeight="1"/>
-    <row r="705" ht="15.75" customHeight="1"/>
-    <row r="706" ht="15.75" customHeight="1"/>
-    <row r="707" ht="15.75" customHeight="1"/>
-    <row r="708" ht="15.75" customHeight="1"/>
-    <row r="709" ht="15.75" customHeight="1"/>
-    <row r="710" ht="15.75" customHeight="1"/>
-    <row r="711" ht="15.75" customHeight="1"/>
-    <row r="712" ht="15.75" customHeight="1"/>
-    <row r="713" ht="15.75" customHeight="1"/>
-    <row r="714" ht="15.75" customHeight="1"/>
-    <row r="715" ht="15.75" customHeight="1"/>
-    <row r="716" ht="15.75" customHeight="1"/>
-    <row r="717" ht="15.75" customHeight="1"/>
-    <row r="718" ht="15.75" customHeight="1"/>
-    <row r="719" ht="15.75" customHeight="1"/>
-    <row r="720" ht="15.75" customHeight="1"/>
-    <row r="721" ht="15.75" customHeight="1"/>
-    <row r="722" ht="15.75" customHeight="1"/>
-    <row r="723" ht="15.75" customHeight="1"/>
-    <row r="724" ht="15.75" customHeight="1"/>
-    <row r="725" ht="15.75" customHeight="1"/>
-    <row r="726" ht="15.75" customHeight="1"/>
-    <row r="727" ht="15.75" customHeight="1"/>
-    <row r="728" ht="15.75" customHeight="1"/>
-    <row r="729" ht="15.75" customHeight="1"/>
-    <row r="730" ht="15.75" customHeight="1"/>
-    <row r="731" ht="15.75" customHeight="1"/>
-    <row r="732" ht="15.75" customHeight="1"/>
-    <row r="733" ht="15.75" customHeight="1"/>
-    <row r="734" ht="15.75" customHeight="1"/>
-    <row r="735" ht="15.75" customHeight="1"/>
-    <row r="736" ht="15.75" customHeight="1"/>
-    <row r="737" ht="15.75" customHeight="1"/>
-    <row r="738" ht="15.75" customHeight="1"/>
-    <row r="739" ht="15.75" customHeight="1"/>
-    <row r="740" ht="15.75" customHeight="1"/>
-    <row r="741" ht="15.75" customHeight="1"/>
-    <row r="742" ht="15.75" customHeight="1"/>
-    <row r="743" ht="15.75" customHeight="1"/>
-    <row r="744" ht="15.75" customHeight="1"/>
-    <row r="745" ht="15.75" customHeight="1"/>
-    <row r="746" ht="15.75" customHeight="1"/>
-    <row r="747" ht="15.75" customHeight="1"/>
-    <row r="748" ht="15.75" customHeight="1"/>
-    <row r="749" ht="15.75" customHeight="1"/>
-    <row r="750" ht="15.75" customHeight="1"/>
-    <row r="751" ht="15.75" customHeight="1"/>
-    <row r="752" ht="15.75" customHeight="1"/>
-    <row r="753" ht="15.75" customHeight="1"/>
-    <row r="754" ht="15.75" customHeight="1"/>
-    <row r="755" ht="15.75" customHeight="1"/>
-    <row r="756" ht="15.75" customHeight="1"/>
-    <row r="757" ht="15.75" customHeight="1"/>
-    <row r="758" ht="15.75" customHeight="1"/>
-    <row r="759" ht="15.75" customHeight="1"/>
-    <row r="760" ht="15.75" customHeight="1"/>
-    <row r="761" ht="15.75" customHeight="1"/>
-    <row r="762" ht="15.75" customHeight="1"/>
-    <row r="763" ht="15.75" customHeight="1"/>
-    <row r="764" ht="15.75" customHeight="1"/>
-    <row r="765" ht="15.75" customHeight="1"/>
-    <row r="766" ht="15.75" customHeight="1"/>
-    <row r="767" ht="15.75" customHeight="1"/>
-    <row r="768" ht="15.75" customHeight="1"/>
-    <row r="769" ht="15.75" customHeight="1"/>
-    <row r="770" ht="15.75" customHeight="1"/>
-    <row r="771" ht="15.75" customHeight="1"/>
-    <row r="772" ht="15.75" customHeight="1"/>
-    <row r="773" ht="15.75" customHeight="1"/>
-    <row r="774" ht="15.75" customHeight="1"/>
-    <row r="775" ht="15.75" customHeight="1"/>
-    <row r="776" ht="15.75" customHeight="1"/>
-    <row r="777" ht="15.75" customHeight="1"/>
-    <row r="778" ht="15.75" customHeight="1"/>
-    <row r="779" ht="15.75" customHeight="1"/>
-    <row r="780" ht="15.75" customHeight="1"/>
-    <row r="781" ht="15.75" customHeight="1"/>
-    <row r="782" ht="15.75" customHeight="1"/>
-    <row r="783" ht="15.75" customHeight="1"/>
-    <row r="784" ht="15.75" customHeight="1"/>
-    <row r="785" ht="15.75" customHeight="1"/>
-    <row r="786" ht="15.75" customHeight="1"/>
-    <row r="787" ht="15.75" customHeight="1"/>
-    <row r="788" ht="15.75" customHeight="1"/>
-    <row r="789" ht="15.75" customHeight="1"/>
-    <row r="790" ht="15.75" customHeight="1"/>
-    <row r="791" ht="15.75" customHeight="1"/>
-    <row r="792" ht="15.75" customHeight="1"/>
-    <row r="793" ht="15.75" customHeight="1"/>
-    <row r="794" ht="15.75" customHeight="1"/>
-    <row r="795" ht="15.75" customHeight="1"/>
-    <row r="796" ht="15.75" customHeight="1"/>
-    <row r="797" ht="15.75" customHeight="1"/>
-    <row r="798" ht="15.75" customHeight="1"/>
-    <row r="799" ht="15.75" customHeight="1"/>
-    <row r="800" ht="15.75" customHeight="1"/>
-    <row r="801" ht="15.75" customHeight="1"/>
-    <row r="802" ht="15.75" customHeight="1"/>
-    <row r="803" ht="15.75" customHeight="1"/>
-    <row r="804" ht="15.75" customHeight="1"/>
-    <row r="805" ht="15.75" customHeight="1"/>
-    <row r="806" ht="15.75" customHeight="1"/>
-    <row r="807" ht="15.75" customHeight="1"/>
-    <row r="808" ht="15.75" customHeight="1"/>
-    <row r="809" ht="15.75" customHeight="1"/>
-    <row r="810" ht="15.75" customHeight="1"/>
-    <row r="811" ht="15.75" customHeight="1"/>
-    <row r="812" ht="15.75" customHeight="1"/>
-    <row r="813" ht="15.75" customHeight="1"/>
-    <row r="814" ht="15.75" customHeight="1"/>
-    <row r="815" ht="15.75" customHeight="1"/>
-    <row r="816" ht="15.75" customHeight="1"/>
-    <row r="817" ht="15.75" customHeight="1"/>
-    <row r="818" ht="15.75" customHeight="1"/>
-    <row r="819" ht="15.75" customHeight="1"/>
-    <row r="820" ht="15.75" customHeight="1"/>
-    <row r="821" ht="15.75" customHeight="1"/>
-    <row r="822" ht="15.75" customHeight="1"/>
-    <row r="823" ht="15.75" customHeight="1"/>
-    <row r="824" ht="15.75" customHeight="1"/>
-    <row r="825" ht="15.75" customHeight="1"/>
-    <row r="826" ht="15.75" customHeight="1"/>
-    <row r="827" ht="15.75" customHeight="1"/>
-    <row r="828" ht="15.75" customHeight="1"/>
-    <row r="829" ht="15.75" customHeight="1"/>
-    <row r="830" ht="15.75" customHeight="1"/>
-    <row r="831" ht="15.75" customHeight="1"/>
-    <row r="832" ht="15.75" customHeight="1"/>
-    <row r="833" ht="15.75" customHeight="1"/>
-    <row r="834" ht="15.75" customHeight="1"/>
-    <row r="835" ht="15.75" customHeight="1"/>
-    <row r="836" ht="15.75" customHeight="1"/>
-    <row r="837" ht="15.75" customHeight="1"/>
-    <row r="838" ht="15.75" customHeight="1"/>
-    <row r="839" ht="15.75" customHeight="1"/>
-    <row r="840" ht="15.75" customHeight="1"/>
-    <row r="841" ht="15.75" customHeight="1"/>
-    <row r="842" ht="15.75" customHeight="1"/>
-    <row r="843" ht="15.75" customHeight="1"/>
-    <row r="844" ht="15.75" customHeight="1"/>
-    <row r="845" ht="15.75" customHeight="1"/>
-    <row r="846" ht="15.75" customHeight="1"/>
-    <row r="847" ht="15.75" customHeight="1"/>
-    <row r="848" ht="15.75" customHeight="1"/>
-    <row r="849" ht="15.75" customHeight="1"/>
-    <row r="850" ht="15.75" customHeight="1"/>
-    <row r="851" ht="15.75" customHeight="1"/>
-    <row r="852" ht="15.75" customHeight="1"/>
-    <row r="853" ht="15.75" customHeight="1"/>
-    <row r="854" ht="15.75" customHeight="1"/>
-    <row r="855" ht="15.75" customHeight="1"/>
-    <row r="856" ht="15.75" customHeight="1"/>
-    <row r="857" ht="15.75" customHeight="1"/>
-    <row r="858" ht="15.75" customHeight="1"/>
-    <row r="859" ht="15.75" customHeight="1"/>
-    <row r="860" ht="15.75" customHeight="1"/>
-    <row r="861" ht="15.75" customHeight="1"/>
-    <row r="862" ht="15.75" customHeight="1"/>
-    <row r="863" ht="15.75" customHeight="1"/>
-    <row r="864" ht="15.75" customHeight="1"/>
-    <row r="865" ht="15.75" customHeight="1"/>
-    <row r="866" ht="15.75" customHeight="1"/>
-    <row r="867" ht="15.75" customHeight="1"/>
-    <row r="868" ht="15.75" customHeight="1"/>
-    <row r="869" ht="15.75" customHeight="1"/>
-    <row r="870" ht="15.75" customHeight="1"/>
-    <row r="871" ht="15.75" customHeight="1"/>
-    <row r="872" ht="15.75" customHeight="1"/>
-    <row r="873" ht="15.75" customHeight="1"/>
-    <row r="874" ht="15.75" customHeight="1"/>
-    <row r="875" ht="15.75" customHeight="1"/>
-    <row r="876" ht="15.75" customHeight="1"/>
-    <row r="877" ht="15.75" customHeight="1"/>
-    <row r="878" ht="15.75" customHeight="1"/>
-    <row r="879" ht="15.75" customHeight="1"/>
-    <row r="880" ht="15.75" customHeight="1"/>
-    <row r="881" ht="15.75" customHeight="1"/>
-    <row r="882" ht="15.75" customHeight="1"/>
-    <row r="883" ht="15.75" customHeight="1"/>
-    <row r="884" ht="15.75" customHeight="1"/>
-    <row r="885" ht="15.75" customHeight="1"/>
-    <row r="886" ht="15.75" customHeight="1"/>
-    <row r="887" ht="15.75" customHeight="1"/>
-    <row r="888" ht="15.75" customHeight="1"/>
-    <row r="889" ht="15.75" customHeight="1"/>
-    <row r="890" ht="15.75" customHeight="1"/>
-    <row r="891" ht="15.75" customHeight="1"/>
-    <row r="892" ht="15.75" customHeight="1"/>
-    <row r="893" ht="15.75" customHeight="1"/>
-    <row r="894" ht="15.75" customHeight="1"/>
-    <row r="895" ht="15.75" customHeight="1"/>
-    <row r="896" ht="15.75" customHeight="1"/>
-    <row r="897" ht="15.75" customHeight="1"/>
-    <row r="898" ht="15.75" customHeight="1"/>
-    <row r="899" ht="15.75" customHeight="1"/>
-    <row r="900" ht="15.75" customHeight="1"/>
-    <row r="901" ht="15.75" customHeight="1"/>
-    <row r="902" ht="15.75" customHeight="1"/>
-    <row r="903" ht="15.75" customHeight="1"/>
-    <row r="904" ht="15.75" customHeight="1"/>
-    <row r="905" ht="15.75" customHeight="1"/>
-    <row r="906" ht="15.75" customHeight="1"/>
-    <row r="907" ht="15.75" customHeight="1"/>
-    <row r="908" ht="15.75" customHeight="1"/>
-    <row r="909" ht="15.75" customHeight="1"/>
-    <row r="910" ht="15.75" customHeight="1"/>
-    <row r="911" ht="15.75" customHeight="1"/>
-    <row r="912" ht="15.75" customHeight="1"/>
-    <row r="913" ht="15.75" customHeight="1"/>
-    <row r="914" ht="15.75" customHeight="1"/>
-    <row r="915" ht="15.75" customHeight="1"/>
-    <row r="916" ht="15.75" customHeight="1"/>
-    <row r="917" ht="15.75" customHeight="1"/>
-    <row r="918" ht="15.75" customHeight="1"/>
-    <row r="919" ht="15.75" customHeight="1"/>
-    <row r="920" ht="15.75" customHeight="1"/>
-    <row r="921" ht="15.75" customHeight="1"/>
-    <row r="922" ht="15.75" customHeight="1"/>
-    <row r="923" ht="15.75" customHeight="1"/>
-    <row r="924" ht="15.75" customHeight="1"/>
-    <row r="925" ht="15.75" customHeight="1"/>
-    <row r="926" ht="15.75" customHeight="1"/>
-    <row r="927" ht="15.75" customHeight="1"/>
-    <row r="928" ht="15.75" customHeight="1"/>
-    <row r="929" ht="15.75" customHeight="1"/>
-    <row r="930" ht="15.75" customHeight="1"/>
-    <row r="931" ht="15.75" customHeight="1"/>
-    <row r="932" ht="15.75" customHeight="1"/>
-    <row r="933" ht="15.75" customHeight="1"/>
-    <row r="934" ht="15.75" customHeight="1"/>
-    <row r="935" ht="15.75" customHeight="1"/>
-    <row r="936" ht="15.75" customHeight="1"/>
-    <row r="937" ht="15.75" customHeight="1"/>
-    <row r="938" ht="15.75" customHeight="1"/>
-    <row r="939" ht="15.75" customHeight="1"/>
-    <row r="940" ht="15.75" customHeight="1"/>
-    <row r="941" ht="15.75" customHeight="1"/>
-    <row r="942" ht="15.75" customHeight="1"/>
-    <row r="943" ht="15.75" customHeight="1"/>
-    <row r="944" ht="15.75" customHeight="1"/>
-    <row r="945" ht="15.75" customHeight="1"/>
-    <row r="946" ht="15.75" customHeight="1"/>
-    <row r="947" ht="15.75" customHeight="1"/>
-    <row r="948" ht="15.75" customHeight="1"/>
-    <row r="949" ht="15.75" customHeight="1"/>
-    <row r="950" ht="15.75" customHeight="1"/>
-    <row r="951" ht="15.75" customHeight="1"/>
-    <row r="952" ht="15.75" customHeight="1"/>
-    <row r="953" ht="15.75" customHeight="1"/>
-    <row r="954" ht="15.75" customHeight="1"/>
-    <row r="955" ht="15.75" customHeight="1"/>
-    <row r="956" ht="15.75" customHeight="1"/>
-    <row r="957" ht="15.75" customHeight="1"/>
-    <row r="958" ht="15.75" customHeight="1"/>
-    <row r="959" ht="15.75" customHeight="1"/>
-    <row r="960" ht="15.75" customHeight="1"/>
-    <row r="961" ht="15.75" customHeight="1"/>
-    <row r="962" ht="15.75" customHeight="1"/>
-    <row r="963" ht="15.75" customHeight="1"/>
-    <row r="964" ht="15.75" customHeight="1"/>
-    <row r="965" ht="15.75" customHeight="1"/>
-    <row r="966" ht="15.75" customHeight="1"/>
-    <row r="967" ht="15.75" customHeight="1"/>
-    <row r="968" ht="15.75" customHeight="1"/>
-    <row r="969" ht="15.75" customHeight="1"/>
-    <row r="970" ht="15.75" customHeight="1"/>
-    <row r="971" ht="15.75" customHeight="1"/>
-    <row r="972" ht="15.75" customHeight="1"/>
-    <row r="973" ht="15.75" customHeight="1"/>
-    <row r="974" ht="15.75" customHeight="1"/>
-    <row r="975" ht="15.75" customHeight="1"/>
-    <row r="976" ht="15.75" customHeight="1"/>
-    <row r="977" ht="15.75" customHeight="1"/>
-    <row r="978" ht="15.75" customHeight="1"/>
-    <row r="979" ht="15.75" customHeight="1"/>
-    <row r="980" ht="15.75" customHeight="1"/>
-    <row r="981" ht="15.75" customHeight="1"/>
-    <row r="982" ht="15.75" customHeight="1"/>
-    <row r="983" ht="15.75" customHeight="1"/>
-    <row r="984" ht="15.75" customHeight="1"/>
-    <row r="985" ht="15.75" customHeight="1"/>
-    <row r="986" ht="15.75" customHeight="1"/>
-    <row r="987" ht="15.75" customHeight="1"/>
-    <row r="988" ht="15.75" customHeight="1"/>
-    <row r="989" ht="15.75" customHeight="1"/>
-    <row r="990" ht="15.75" customHeight="1"/>
-    <row r="991" ht="15.75" customHeight="1"/>
-    <row r="992" ht="15.75" customHeight="1"/>
-    <row r="993" ht="15.75" customHeight="1"/>
-    <row r="994" ht="15.75" customHeight="1"/>
-    <row r="995" ht="15.75" customHeight="1"/>
-    <row r="996" ht="15.75" customHeight="1"/>
-    <row r="997" ht="15.75" customHeight="1"/>
-    <row r="998" ht="15.75" customHeight="1"/>
-    <row r="999" ht="15.75" customHeight="1"/>
-    <row r="1000" ht="15.75" customHeight="1"/>
+    <row r="261" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="262" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="263" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="264" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="265" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="266" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="267" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="268" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="269" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="270" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="271" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="272" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="273" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="274" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="275" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="276" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="277" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="278" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="279" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="280" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="281" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="282" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="283" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="284" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="285" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="286" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="287" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="288" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="289" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="290" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="291" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="292" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="293" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="294" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="295" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="296" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="297" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="298" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="299" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="300" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="301" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="302" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="303" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="304" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="305" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="306" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="307" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="308" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="309" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="310" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="311" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="312" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="313" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="314" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="315" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="316" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="317" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="318" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="319" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="320" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="321" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="322" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="323" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="324" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="325" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="326" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="327" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="328" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="329" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="330" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="331" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="332" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="333" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="334" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="335" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="336" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="337" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="338" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="339" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="340" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="341" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="342" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="343" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="344" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="345" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="346" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="347" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="348" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="349" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="350" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="351" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="352" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="353" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="354" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="355" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="356" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="357" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="358" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="359" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="360" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="361" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="362" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="363" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="364" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="365" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="366" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="367" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="368" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="369" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="370" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="371" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="372" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="373" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="374" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="375" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="376" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="377" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="378" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="379" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="380" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="381" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="382" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="383" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="384" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="385" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="386" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="387" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="388" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="389" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="390" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="391" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="392" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="393" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="394" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="395" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="396" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="397" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="398" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="399" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="400" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="401" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="402" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="403" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="404" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="405" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="406" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="407" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="408" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="409" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="410" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="411" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="412" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="413" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="414" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="415" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="416" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="417" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="418" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="419" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="420" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="421" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="422" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="423" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="424" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="425" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="426" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="427" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="428" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="429" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="430" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="431" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="432" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="433" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="434" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="435" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="436" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="437" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="438" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="439" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="440" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="441" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="442" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="443" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="444" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="445" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="446" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="447" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="448" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="449" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="450" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="451" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="452" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="453" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="454" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="455" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="456" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="457" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="458" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="459" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="460" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="461" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="462" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="463" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="464" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="465" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="466" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="467" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="468" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="469" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="470" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="471" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="472" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="473" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="474" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="475" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="476" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="477" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="478" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="479" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="480" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="481" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="482" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="483" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="484" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="485" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="486" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="487" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="488" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="489" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="490" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="491" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="492" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="493" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="494" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="495" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="496" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="497" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="498" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="499" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="500" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="501" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="502" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="503" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="504" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="505" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="506" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="507" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="508" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="509" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="510" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="511" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="512" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="513" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="514" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="515" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="516" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="517" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="518" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="519" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="520" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="521" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="522" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="523" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="524" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="525" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="526" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="527" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="528" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="529" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="530" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="531" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="532" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="533" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="534" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="535" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="536" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="537" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="538" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="539" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="540" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="541" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="542" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="543" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="544" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="545" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="546" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="547" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="548" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="549" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="550" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="551" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="552" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="553" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="554" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="555" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="556" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="557" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="558" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="559" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="560" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="561" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="562" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="563" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="564" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="565" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="566" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="567" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="568" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="569" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="570" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="571" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="572" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="573" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="574" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="575" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="576" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="577" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="578" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="579" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="580" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="581" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="582" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="583" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="584" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="585" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="586" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="587" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="588" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="589" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="590" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="591" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="592" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="593" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="594" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="595" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="596" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="597" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="598" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="599" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="600" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="601" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="602" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="603" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="604" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="605" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="606" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="607" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="608" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="609" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="610" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="611" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="612" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="613" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="614" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="615" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="616" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="617" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="618" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="619" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="620" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="621" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="622" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="623" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="624" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="625" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="626" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="627" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="628" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="629" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="630" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="631" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="632" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="633" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="634" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="635" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="636" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="637" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="638" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="639" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="640" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="641" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="642" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="643" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="644" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="645" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="646" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="647" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="648" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="649" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="650" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="651" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="652" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="653" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="654" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="655" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="656" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="657" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="658" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="659" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="660" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="661" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="662" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="663" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="664" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="665" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="666" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="667" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="668" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="669" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="670" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="671" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="672" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="673" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="674" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="675" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="676" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="677" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="678" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="679" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="680" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="681" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="682" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="683" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="684" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="685" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="686" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="687" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="688" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="689" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="690" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="691" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="692" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="693" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="694" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="695" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="696" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="697" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="698" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="699" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="700" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="701" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="702" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="703" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="704" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="705" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="706" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="707" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="708" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="709" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="710" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="711" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="712" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="713" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="714" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="715" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="716" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="717" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="718" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="719" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="720" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="721" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="722" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="723" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="724" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="725" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="726" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="727" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="728" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="729" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="730" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="731" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="732" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="733" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="734" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="735" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="736" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="737" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="738" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="739" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="740" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="741" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="742" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="743" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="744" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="745" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="746" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="747" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="748" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="749" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="750" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="751" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="752" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="753" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="754" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="755" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="756" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="757" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="758" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="759" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="760" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="761" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="762" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="763" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="764" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="765" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="766" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="767" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="768" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="769" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="770" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="771" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="772" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="773" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="774" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="775" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="776" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="777" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="778" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="779" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="780" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="781" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="782" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="783" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="784" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="785" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="786" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="787" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="788" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="789" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="790" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="791" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="792" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="793" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="794" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="795" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="796" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="797" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="798" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="799" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="800" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="801" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="802" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="803" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="804" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="805" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="806" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="807" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="808" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="809" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="810" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="811" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="812" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="813" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="814" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="815" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="816" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="817" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="818" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="819" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="820" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="821" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="822" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="823" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="824" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="825" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="826" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="827" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="828" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="829" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="830" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="831" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="832" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="833" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="834" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="835" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="836" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="837" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="838" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="839" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="840" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="841" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="842" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="843" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="844" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="845" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="846" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="847" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="848" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="849" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="850" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="851" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="852" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="853" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="854" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="855" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="856" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="857" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="858" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="859" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="860" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="861" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="862" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="863" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="864" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="865" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="866" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="867" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="868" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="869" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="870" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="871" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="872" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="873" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="874" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="875" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="876" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="877" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="878" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="879" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="880" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="881" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="882" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="883" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="884" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="885" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="886" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="887" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="888" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="889" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="890" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="891" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="892" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="893" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="894" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="895" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="896" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="897" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="898" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="899" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="900" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="901" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="902" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="903" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="904" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="905" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="906" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="907" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="908" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="909" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="910" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="911" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="912" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="913" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="914" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="915" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="916" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="917" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="918" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="919" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="920" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="921" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="922" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="923" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="924" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="925" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="926" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="927" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="928" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="929" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="930" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="931" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="932" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="933" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="934" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="935" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="936" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="937" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="938" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="939" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="940" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="941" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="942" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="943" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="944" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="945" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="946" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="947" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="948" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="949" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="950" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="951" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="952" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="953" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="954" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="955" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="956" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="957" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="958" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="959" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="960" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="961" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="962" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="963" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="964" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="965" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="966" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="967" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="968" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="969" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="970" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="971" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="972" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="973" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="974" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="975" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="976" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="977" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="978" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="979" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="980" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="981" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="982" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="983" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="984" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="985" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="986" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="987" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="988" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="989" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="990" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="991" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="992" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="993" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="994" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="995" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="996" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="997" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="998" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="999" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="D4"/>
-    <hyperlink r:id="rId2" ref="D5"/>
+    <hyperlink ref="D4" r:id="rId1"/>
+    <hyperlink ref="D5" r:id="rId2"/>
+    <hyperlink ref="D8" r:id="rId3"/>
   </hyperlinks>
-  <printOptions/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <drawing r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Se agrega el 10 Alumno al archivo
</commit_message>
<xml_diff>
--- a/Lista de Alumnos.xlsx
+++ b/Lista de Alumnos.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21601"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nano\Documents\Programacion\ISPC\Electronica microcontrolada\git proteus\Alumnos\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1813A112-83C4-4B0C-A759-2731FD4CBD4F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15600" windowHeight="8190" tabRatio="500"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Electronica Microcontrolada" sheetId="1" r:id="rId1"/>
@@ -19,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>#</t>
   </si>
@@ -113,12 +119,21 @@
   <si>
     <t>Cabro645</t>
   </si>
+  <si>
+    <t>William Bernardo Leyton Segovia</t>
+  </si>
+  <si>
+    <t>williamleyton89@gmail.com</t>
+  </si>
+  <si>
+    <t>Wleyton89</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -346,6 +361,14 @@
       <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -392,7 +415,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -424,9 +447,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -458,6 +499,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -633,14 +692,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E1000"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.85546875" customWidth="1"/>
     <col min="2" max="2" width="37.140625" customWidth="1"/>
@@ -650,7 +709,7 @@
     <col min="6" max="6" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="27" customHeight="1">
+    <row r="1" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -667,7 +726,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="19.5" customHeight="1">
+    <row r="2" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -684,7 +743,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="19.5" customHeight="1">
+    <row r="3" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>2</v>
       </c>
@@ -699,7 +758,7 @@
       </c>
       <c r="E3" s="6"/>
     </row>
-    <row r="4" spans="1:5" ht="19.5" customHeight="1">
+    <row r="4" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>3</v>
       </c>
@@ -716,7 +775,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="19.5" customHeight="1">
+    <row r="5" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>4</v>
       </c>
@@ -733,7 +792,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="19.5" customHeight="1">
+    <row r="6" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>5</v>
       </c>
@@ -750,7 +809,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="19.5" customHeight="1">
+    <row r="7" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>6</v>
       </c>
@@ -767,7 +826,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="19.5" customHeight="1">
+    <row r="8" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>7</v>
       </c>
@@ -784,7 +843,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="19.5" customHeight="1">
+    <row r="9" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>8</v>
       </c>
@@ -801,7 +860,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="19.5" customHeight="1">
+    <row r="10" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>9</v>
       </c>
@@ -816,16 +875,24 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="19.5" customHeight="1">
+    <row r="11" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <v>10</v>
       </c>
-      <c r="B11" s="6"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-    </row>
-    <row r="12" spans="1:5" ht="19.5" customHeight="1">
+      <c r="B11" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" s="5">
+        <v>3</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>11</v>
       </c>
@@ -834,7 +901,7 @@
       <c r="D12" s="6"/>
       <c r="E12" s="6"/>
     </row>
-    <row r="13" spans="1:5" ht="19.5" customHeight="1">
+    <row r="13" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
         <v>12</v>
       </c>
@@ -843,7 +910,7 @@
       <c r="D13" s="6"/>
       <c r="E13" s="6"/>
     </row>
-    <row r="14" spans="1:5" ht="19.5" customHeight="1">
+    <row r="14" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
         <v>13</v>
       </c>
@@ -852,7 +919,7 @@
       <c r="D14" s="6"/>
       <c r="E14" s="6"/>
     </row>
-    <row r="15" spans="1:5" ht="19.5" customHeight="1">
+    <row r="15" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
         <v>14</v>
       </c>
@@ -861,7 +928,7 @@
       <c r="D15" s="6"/>
       <c r="E15" s="6"/>
     </row>
-    <row r="16" spans="1:5" ht="19.5" customHeight="1">
+    <row r="16" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
         <v>15</v>
       </c>
@@ -870,7 +937,7 @@
       <c r="D16" s="6"/>
       <c r="E16" s="6"/>
     </row>
-    <row r="17" spans="1:5" ht="19.5" customHeight="1">
+    <row r="17" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
         <v>16</v>
       </c>
@@ -879,7 +946,7 @@
       <c r="D17" s="6"/>
       <c r="E17" s="6"/>
     </row>
-    <row r="18" spans="1:5" ht="25.5" customHeight="1">
+    <row r="18" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <v>17</v>
       </c>
@@ -888,7 +955,7 @@
       <c r="D18" s="6"/>
       <c r="E18" s="6"/>
     </row>
-    <row r="19" spans="1:5" ht="25.5" customHeight="1">
+    <row r="19" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
         <v>18</v>
       </c>
@@ -897,7 +964,7 @@
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
     </row>
-    <row r="20" spans="1:5" ht="25.5" customHeight="1">
+    <row r="20" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
         <v>19</v>
       </c>
@@ -906,7 +973,7 @@
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
     </row>
-    <row r="21" spans="1:5" ht="25.5" customHeight="1">
+    <row r="21" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="5">
         <v>20</v>
       </c>
@@ -915,7 +982,7 @@
       <c r="D21" s="6"/>
       <c r="E21" s="6"/>
     </row>
-    <row r="22" spans="1:5" ht="25.5" customHeight="1">
+    <row r="22" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="5">
         <v>21</v>
       </c>
@@ -924,7 +991,7 @@
       <c r="D22" s="6"/>
       <c r="E22" s="6"/>
     </row>
-    <row r="23" spans="1:5" ht="25.5" customHeight="1">
+    <row r="23" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="5">
         <v>22</v>
       </c>
@@ -933,7 +1000,7 @@
       <c r="D23" s="6"/>
       <c r="E23" s="6"/>
     </row>
-    <row r="24" spans="1:5" ht="25.5" customHeight="1">
+    <row r="24" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="5">
         <v>23</v>
       </c>
@@ -942,7 +1009,7 @@
       <c r="D24" s="6"/>
       <c r="E24" s="6"/>
     </row>
-    <row r="25" spans="1:5" ht="25.5" customHeight="1">
+    <row r="25" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="5">
         <v>24</v>
       </c>
@@ -951,7 +1018,7 @@
       <c r="D25" s="6"/>
       <c r="E25" s="6"/>
     </row>
-    <row r="26" spans="1:5" ht="25.5" customHeight="1">
+    <row r="26" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="5">
         <v>25</v>
       </c>
@@ -960,7 +1027,7 @@
       <c r="D26" s="6"/>
       <c r="E26" s="6"/>
     </row>
-    <row r="27" spans="1:5" ht="25.5" customHeight="1">
+    <row r="27" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="5">
         <v>26</v>
       </c>
@@ -969,7 +1036,7 @@
       <c r="D27" s="6"/>
       <c r="E27" s="6"/>
     </row>
-    <row r="28" spans="1:5" ht="25.5" customHeight="1">
+    <row r="28" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="5">
         <v>27</v>
       </c>
@@ -978,7 +1045,7 @@
       <c r="D28" s="6"/>
       <c r="E28" s="6"/>
     </row>
-    <row r="29" spans="1:5" ht="25.5" customHeight="1">
+    <row r="29" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="5">
         <v>28</v>
       </c>
@@ -987,7 +1054,7 @@
       <c r="D29" s="6"/>
       <c r="E29" s="6"/>
     </row>
-    <row r="30" spans="1:5" ht="25.5" customHeight="1">
+    <row r="30" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="5">
         <v>29</v>
       </c>
@@ -996,7 +1063,7 @@
       <c r="D30" s="6"/>
       <c r="E30" s="6"/>
     </row>
-    <row r="31" spans="1:5" ht="25.5" customHeight="1">
+    <row r="31" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="5">
         <v>30</v>
       </c>
@@ -1005,7 +1072,7 @@
       <c r="D31" s="6"/>
       <c r="E31" s="6"/>
     </row>
-    <row r="32" spans="1:5" ht="25.5" customHeight="1">
+    <row r="32" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="5">
         <v>31</v>
       </c>
@@ -1014,7 +1081,7 @@
       <c r="D32" s="6"/>
       <c r="E32" s="6"/>
     </row>
-    <row r="33" spans="1:5" ht="25.5" customHeight="1">
+    <row r="33" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="5">
         <v>32</v>
       </c>
@@ -1023,7 +1090,7 @@
       <c r="D33" s="6"/>
       <c r="E33" s="6"/>
     </row>
-    <row r="34" spans="1:5" ht="25.5" customHeight="1">
+    <row r="34" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="5">
         <v>33</v>
       </c>
@@ -1032,7 +1099,7 @@
       <c r="D34" s="6"/>
       <c r="E34" s="6"/>
     </row>
-    <row r="35" spans="1:5" ht="25.5" customHeight="1">
+    <row r="35" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="5">
         <v>34</v>
       </c>
@@ -1041,7 +1108,7 @@
       <c r="D35" s="6"/>
       <c r="E35" s="6"/>
     </row>
-    <row r="36" spans="1:5" ht="25.5" customHeight="1">
+    <row r="36" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="5">
         <v>35</v>
       </c>
@@ -1050,7 +1117,7 @@
       <c r="D36" s="6"/>
       <c r="E36" s="6"/>
     </row>
-    <row r="37" spans="1:5" ht="25.5" customHeight="1">
+    <row r="37" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="5">
         <v>36</v>
       </c>
@@ -1059,7 +1126,7 @@
       <c r="D37" s="6"/>
       <c r="E37" s="6"/>
     </row>
-    <row r="38" spans="1:5" ht="25.5" customHeight="1">
+    <row r="38" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="5">
         <v>37</v>
       </c>
@@ -1068,7 +1135,7 @@
       <c r="D38" s="6"/>
       <c r="E38" s="6"/>
     </row>
-    <row r="39" spans="1:5" ht="25.5" customHeight="1">
+    <row r="39" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="5">
         <v>38</v>
       </c>
@@ -1077,7 +1144,7 @@
       <c r="D39" s="6"/>
       <c r="E39" s="6"/>
     </row>
-    <row r="40" spans="1:5" ht="25.5" customHeight="1">
+    <row r="40" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="5">
         <v>39</v>
       </c>
@@ -1086,7 +1153,7 @@
       <c r="D40" s="6"/>
       <c r="E40" s="6"/>
     </row>
-    <row r="41" spans="1:5" ht="25.5" customHeight="1">
+    <row r="41" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="5">
         <v>40</v>
       </c>
@@ -1095,7 +1162,7 @@
       <c r="D41" s="6"/>
       <c r="E41" s="6"/>
     </row>
-    <row r="42" spans="1:5" ht="25.5" customHeight="1">
+    <row r="42" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="5">
         <v>41</v>
       </c>
@@ -1104,7 +1171,7 @@
       <c r="D42" s="6"/>
       <c r="E42" s="6"/>
     </row>
-    <row r="43" spans="1:5" ht="25.5" customHeight="1">
+    <row r="43" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="5">
         <v>42</v>
       </c>
@@ -1113,7 +1180,7 @@
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
     </row>
-    <row r="44" spans="1:5" ht="25.5" customHeight="1">
+    <row r="44" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="5">
         <v>43</v>
       </c>
@@ -1122,7 +1189,7 @@
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
     </row>
-    <row r="45" spans="1:5" ht="25.5" customHeight="1">
+    <row r="45" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="5">
         <v>44</v>
       </c>
@@ -1131,7 +1198,7 @@
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
     </row>
-    <row r="46" spans="1:5" ht="25.5" customHeight="1">
+    <row r="46" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="5">
         <v>45</v>
       </c>
@@ -1140,7 +1207,7 @@
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
     </row>
-    <row r="47" spans="1:5" ht="25.5" customHeight="1">
+    <row r="47" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="5">
         <v>46</v>
       </c>
@@ -1149,7 +1216,7 @@
       <c r="D47" s="6"/>
       <c r="E47" s="6"/>
     </row>
-    <row r="48" spans="1:5" ht="25.5" customHeight="1">
+    <row r="48" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="5">
         <v>47</v>
       </c>
@@ -1158,7 +1225,7 @@
       <c r="D48" s="6"/>
       <c r="E48" s="6"/>
     </row>
-    <row r="49" spans="1:5" ht="25.5" customHeight="1">
+    <row r="49" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="5">
         <v>48</v>
       </c>
@@ -1167,7 +1234,7 @@
       <c r="D49" s="6"/>
       <c r="E49" s="6"/>
     </row>
-    <row r="50" spans="1:5" ht="25.5" customHeight="1">
+    <row r="50" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="5">
         <v>49</v>
       </c>
@@ -1176,7 +1243,7 @@
       <c r="D50" s="6"/>
       <c r="E50" s="6"/>
     </row>
-    <row r="51" spans="1:5" ht="25.5" customHeight="1">
+    <row r="51" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="5">
         <v>50</v>
       </c>
@@ -1185,7 +1252,7 @@
       <c r="D51" s="6"/>
       <c r="E51" s="6"/>
     </row>
-    <row r="52" spans="1:5" ht="25.5" customHeight="1">
+    <row r="52" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="5">
         <v>51</v>
       </c>
@@ -1194,7 +1261,7 @@
       <c r="D52" s="6"/>
       <c r="E52" s="6"/>
     </row>
-    <row r="53" spans="1:5" ht="25.5" customHeight="1">
+    <row r="53" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="5">
         <v>52</v>
       </c>
@@ -1203,7 +1270,7 @@
       <c r="D53" s="6"/>
       <c r="E53" s="6"/>
     </row>
-    <row r="54" spans="1:5" ht="25.5" customHeight="1">
+    <row r="54" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="5">
         <v>53</v>
       </c>
@@ -1212,7 +1279,7 @@
       <c r="D54" s="6"/>
       <c r="E54" s="6"/>
     </row>
-    <row r="55" spans="1:5" ht="25.5" customHeight="1">
+    <row r="55" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="5">
         <v>54</v>
       </c>
@@ -1221,7 +1288,7 @@
       <c r="D55" s="6"/>
       <c r="E55" s="6"/>
     </row>
-    <row r="56" spans="1:5" ht="25.5" customHeight="1">
+    <row r="56" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="5">
         <v>55</v>
       </c>
@@ -1230,7 +1297,7 @@
       <c r="D56" s="6"/>
       <c r="E56" s="6"/>
     </row>
-    <row r="57" spans="1:5" ht="25.5" customHeight="1">
+    <row r="57" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="5">
         <v>56</v>
       </c>
@@ -1239,7 +1306,7 @@
       <c r="D57" s="6"/>
       <c r="E57" s="6"/>
     </row>
-    <row r="58" spans="1:5" ht="25.5" customHeight="1">
+    <row r="58" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="5">
         <v>57</v>
       </c>
@@ -1248,7 +1315,7 @@
       <c r="D58" s="6"/>
       <c r="E58" s="6"/>
     </row>
-    <row r="59" spans="1:5" ht="25.5" customHeight="1">
+    <row r="59" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="5">
         <v>58</v>
       </c>
@@ -1257,7 +1324,7 @@
       <c r="D59" s="6"/>
       <c r="E59" s="6"/>
     </row>
-    <row r="60" spans="1:5" ht="25.5" customHeight="1">
+    <row r="60" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="5">
         <v>59</v>
       </c>
@@ -1266,2153 +1333,2154 @@
       <c r="D60" s="6"/>
       <c r="E60" s="6"/>
     </row>
-    <row r="61" spans="1:5" ht="15.75" customHeight="1">
+    <row r="61" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="11"/>
       <c r="B61" s="12"/>
       <c r="C61" s="11"/>
       <c r="D61" s="12"/>
       <c r="E61" s="12"/>
     </row>
-    <row r="62" spans="1:5" ht="15.75" customHeight="1">
+    <row r="62" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="11"/>
       <c r="B62" s="12"/>
       <c r="C62" s="11"/>
       <c r="D62" s="12"/>
       <c r="E62" s="12"/>
     </row>
-    <row r="63" spans="1:5" ht="15.75" customHeight="1">
+    <row r="63" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="11"/>
       <c r="B63" s="12"/>
       <c r="C63" s="11"/>
       <c r="D63" s="12"/>
       <c r="E63" s="12"/>
     </row>
-    <row r="64" spans="1:5" ht="15.75" customHeight="1">
+    <row r="64" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="11"/>
       <c r="B64" s="12"/>
       <c r="C64" s="11"/>
       <c r="D64" s="12"/>
       <c r="E64" s="12"/>
     </row>
-    <row r="65" spans="1:5" ht="15.75" customHeight="1">
+    <row r="65" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="11"/>
       <c r="B65" s="12"/>
       <c r="C65" s="11"/>
       <c r="D65" s="12"/>
       <c r="E65" s="12"/>
     </row>
-    <row r="66" spans="1:5" ht="15.75" customHeight="1">
+    <row r="66" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="11"/>
       <c r="B66" s="12"/>
       <c r="C66" s="11"/>
       <c r="D66" s="12"/>
       <c r="E66" s="12"/>
     </row>
-    <row r="67" spans="1:5" ht="15.75" customHeight="1">
+    <row r="67" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="11"/>
       <c r="B67" s="12"/>
       <c r="C67" s="11"/>
       <c r="D67" s="12"/>
       <c r="E67" s="12"/>
     </row>
-    <row r="68" spans="1:5" ht="15.75" customHeight="1">
+    <row r="68" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="11"/>
       <c r="B68" s="12"/>
       <c r="C68" s="11"/>
       <c r="D68" s="12"/>
       <c r="E68" s="12"/>
     </row>
-    <row r="69" spans="1:5" ht="15.75" customHeight="1">
+    <row r="69" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="11"/>
       <c r="B69" s="12"/>
       <c r="C69" s="11"/>
       <c r="D69" s="12"/>
       <c r="E69" s="12"/>
     </row>
-    <row r="70" spans="1:5" ht="15.75" customHeight="1">
+    <row r="70" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="11"/>
       <c r="B70" s="12"/>
       <c r="C70" s="11"/>
       <c r="D70" s="12"/>
       <c r="E70" s="12"/>
     </row>
-    <row r="71" spans="1:5" ht="15.75" customHeight="1">
+    <row r="71" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="11"/>
       <c r="B71" s="12"/>
       <c r="C71" s="11"/>
       <c r="D71" s="12"/>
       <c r="E71" s="12"/>
     </row>
-    <row r="72" spans="1:5" ht="15.75" customHeight="1">
+    <row r="72" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="11"/>
       <c r="B72" s="12"/>
       <c r="C72" s="11"/>
       <c r="D72" s="12"/>
       <c r="E72" s="12"/>
     </row>
-    <row r="73" spans="1:5" ht="15.75" customHeight="1">
+    <row r="73" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="11"/>
       <c r="B73" s="12"/>
       <c r="C73" s="11"/>
       <c r="D73" s="12"/>
       <c r="E73" s="12"/>
     </row>
-    <row r="74" spans="1:5" ht="15.75" customHeight="1">
+    <row r="74" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="11"/>
       <c r="B74" s="12"/>
       <c r="C74" s="11"/>
       <c r="D74" s="12"/>
       <c r="E74" s="12"/>
     </row>
-    <row r="75" spans="1:5" ht="15.75" customHeight="1">
+    <row r="75" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="11"/>
       <c r="B75" s="12"/>
       <c r="C75" s="11"/>
       <c r="D75" s="12"/>
       <c r="E75" s="12"/>
     </row>
-    <row r="76" spans="1:5" ht="15.75" customHeight="1">
+    <row r="76" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="11"/>
       <c r="B76" s="12"/>
       <c r="C76" s="11"/>
       <c r="D76" s="12"/>
       <c r="E76" s="12"/>
     </row>
-    <row r="77" spans="1:5" ht="15.75" customHeight="1">
+    <row r="77" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="11"/>
       <c r="B77" s="12"/>
       <c r="C77" s="11"/>
       <c r="D77" s="12"/>
       <c r="E77" s="12"/>
     </row>
-    <row r="78" spans="1:5" ht="15.75" customHeight="1">
+    <row r="78" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="11"/>
       <c r="B78" s="12"/>
       <c r="C78" s="11"/>
       <c r="D78" s="12"/>
       <c r="E78" s="12"/>
     </row>
-    <row r="79" spans="1:5" ht="15.75" customHeight="1">
+    <row r="79" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="11"/>
       <c r="B79" s="12"/>
       <c r="C79" s="11"/>
       <c r="D79" s="12"/>
       <c r="E79" s="12"/>
     </row>
-    <row r="80" spans="1:5" ht="15.75" customHeight="1">
+    <row r="80" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="11"/>
       <c r="B80" s="12"/>
       <c r="C80" s="11"/>
       <c r="D80" s="12"/>
       <c r="E80" s="12"/>
     </row>
-    <row r="81" spans="1:5" ht="15.75" customHeight="1">
+    <row r="81" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="11"/>
       <c r="B81" s="12"/>
       <c r="C81" s="11"/>
       <c r="D81" s="12"/>
       <c r="E81" s="12"/>
     </row>
-    <row r="82" spans="1:5" ht="15.75" customHeight="1">
+    <row r="82" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="11"/>
       <c r="B82" s="12"/>
       <c r="C82" s="11"/>
       <c r="D82" s="12"/>
       <c r="E82" s="12"/>
     </row>
-    <row r="83" spans="1:5" ht="15.75" customHeight="1">
+    <row r="83" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="11"/>
       <c r="B83" s="12"/>
       <c r="C83" s="11"/>
       <c r="D83" s="12"/>
       <c r="E83" s="12"/>
     </row>
-    <row r="84" spans="1:5" ht="15.75" customHeight="1">
+    <row r="84" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="11"/>
       <c r="B84" s="12"/>
       <c r="C84" s="11"/>
       <c r="D84" s="12"/>
       <c r="E84" s="12"/>
     </row>
-    <row r="85" spans="1:5" ht="15.75" customHeight="1">
+    <row r="85" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="11"/>
       <c r="B85" s="12"/>
       <c r="C85" s="11"/>
       <c r="D85" s="12"/>
       <c r="E85" s="12"/>
     </row>
-    <row r="86" spans="1:5" ht="15.75" customHeight="1">
+    <row r="86" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="11"/>
       <c r="B86" s="12"/>
       <c r="C86" s="11"/>
       <c r="D86" s="12"/>
       <c r="E86" s="12"/>
     </row>
-    <row r="87" spans="1:5" ht="15.75" customHeight="1">
+    <row r="87" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="11"/>
       <c r="B87" s="12"/>
       <c r="C87" s="11"/>
       <c r="D87" s="12"/>
       <c r="E87" s="12"/>
     </row>
-    <row r="88" spans="1:5" ht="15.75" customHeight="1">
+    <row r="88" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="11"/>
       <c r="B88" s="12"/>
       <c r="C88" s="11"/>
       <c r="D88" s="12"/>
       <c r="E88" s="12"/>
     </row>
-    <row r="89" spans="1:5" ht="15.75" customHeight="1">
+    <row r="89" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="11"/>
       <c r="B89" s="12"/>
       <c r="C89" s="11"/>
       <c r="D89" s="12"/>
       <c r="E89" s="12"/>
     </row>
-    <row r="90" spans="1:5" ht="15.75" customHeight="1">
+    <row r="90" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="11"/>
       <c r="B90" s="12"/>
       <c r="C90" s="11"/>
       <c r="D90" s="12"/>
       <c r="E90" s="12"/>
     </row>
-    <row r="91" spans="1:5" ht="15.75" customHeight="1">
+    <row r="91" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="11"/>
       <c r="B91" s="12"/>
       <c r="C91" s="11"/>
       <c r="D91" s="12"/>
       <c r="E91" s="12"/>
     </row>
-    <row r="92" spans="1:5" ht="15.75" customHeight="1">
+    <row r="92" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="11"/>
       <c r="B92" s="12"/>
       <c r="C92" s="11"/>
       <c r="D92" s="12"/>
       <c r="E92" s="12"/>
     </row>
-    <row r="93" spans="1:5" ht="15.75" customHeight="1">
+    <row r="93" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="11"/>
       <c r="B93" s="12"/>
       <c r="C93" s="11"/>
       <c r="D93" s="12"/>
       <c r="E93" s="12"/>
     </row>
-    <row r="94" spans="1:5" ht="15.75" customHeight="1">
+    <row r="94" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="11"/>
       <c r="B94" s="12"/>
       <c r="C94" s="11"/>
       <c r="D94" s="12"/>
       <c r="E94" s="12"/>
     </row>
-    <row r="95" spans="1:5" ht="15.75" customHeight="1">
+    <row r="95" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="11"/>
       <c r="B95" s="12"/>
       <c r="C95" s="11"/>
       <c r="D95" s="12"/>
       <c r="E95" s="12"/>
     </row>
-    <row r="96" spans="1:5" ht="15.75" customHeight="1">
+    <row r="96" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="11"/>
       <c r="B96" s="12"/>
       <c r="C96" s="11"/>
       <c r="D96" s="12"/>
       <c r="E96" s="12"/>
     </row>
-    <row r="97" spans="1:5" ht="15.75" customHeight="1">
+    <row r="97" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="11"/>
       <c r="B97" s="12"/>
       <c r="C97" s="11"/>
       <c r="D97" s="12"/>
       <c r="E97" s="12"/>
     </row>
-    <row r="98" spans="1:5" ht="15.75" customHeight="1">
+    <row r="98" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="11"/>
       <c r="B98" s="12"/>
       <c r="C98" s="11"/>
       <c r="D98" s="12"/>
       <c r="E98" s="12"/>
     </row>
-    <row r="99" spans="1:5" ht="15.75" customHeight="1">
+    <row r="99" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="11"/>
       <c r="B99" s="12"/>
       <c r="C99" s="11"/>
       <c r="D99" s="12"/>
       <c r="E99" s="12"/>
     </row>
-    <row r="100" spans="1:5" ht="15.75" customHeight="1">
+    <row r="100" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="11"/>
       <c r="B100" s="12"/>
       <c r="C100" s="11"/>
       <c r="D100" s="12"/>
       <c r="E100" s="12"/>
     </row>
-    <row r="101" spans="1:5" ht="15.75" customHeight="1">
+    <row r="101" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="11"/>
       <c r="B101" s="12"/>
       <c r="C101" s="11"/>
       <c r="D101" s="12"/>
       <c r="E101" s="12"/>
     </row>
-    <row r="102" spans="1:5" ht="15.75" customHeight="1">
+    <row r="102" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="11"/>
       <c r="B102" s="12"/>
       <c r="C102" s="11"/>
       <c r="D102" s="12"/>
       <c r="E102" s="12"/>
     </row>
-    <row r="103" spans="1:5" ht="15.75" customHeight="1">
+    <row r="103" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" s="11"/>
       <c r="B103" s="12"/>
       <c r="C103" s="11"/>
       <c r="D103" s="12"/>
       <c r="E103" s="12"/>
     </row>
-    <row r="104" spans="1:5" ht="15.75" customHeight="1">
+    <row r="104" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="11"/>
       <c r="B104" s="12"/>
       <c r="C104" s="11"/>
       <c r="D104" s="12"/>
       <c r="E104" s="12"/>
     </row>
-    <row r="105" spans="1:5" ht="15.75" customHeight="1">
+    <row r="105" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" s="11"/>
       <c r="B105" s="12"/>
       <c r="C105" s="11"/>
       <c r="D105" s="12"/>
       <c r="E105" s="12"/>
     </row>
-    <row r="106" spans="1:5" ht="15.75" customHeight="1">
+    <row r="106" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="11"/>
       <c r="B106" s="12"/>
       <c r="C106" s="11"/>
       <c r="D106" s="12"/>
       <c r="E106" s="12"/>
     </row>
-    <row r="107" spans="1:5" ht="15.75" customHeight="1">
+    <row r="107" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" s="11"/>
       <c r="B107" s="12"/>
       <c r="C107" s="11"/>
       <c r="D107" s="12"/>
       <c r="E107" s="12"/>
     </row>
-    <row r="108" spans="1:5" ht="15.75" customHeight="1">
+    <row r="108" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" s="11"/>
       <c r="B108" s="12"/>
       <c r="C108" s="11"/>
       <c r="D108" s="12"/>
       <c r="E108" s="12"/>
     </row>
-    <row r="109" spans="1:5" ht="15.75" customHeight="1">
+    <row r="109" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" s="11"/>
       <c r="B109" s="12"/>
       <c r="C109" s="11"/>
       <c r="D109" s="12"/>
       <c r="E109" s="12"/>
     </row>
-    <row r="110" spans="1:5" ht="15.75" customHeight="1">
+    <row r="110" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" s="11"/>
       <c r="B110" s="12"/>
       <c r="C110" s="11"/>
       <c r="D110" s="12"/>
       <c r="E110" s="12"/>
     </row>
-    <row r="111" spans="1:5" ht="15.75" customHeight="1">
+    <row r="111" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" s="11"/>
       <c r="B111" s="12"/>
       <c r="C111" s="11"/>
       <c r="D111" s="12"/>
       <c r="E111" s="12"/>
     </row>
-    <row r="112" spans="1:5" ht="15.75" customHeight="1">
+    <row r="112" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" s="11"/>
       <c r="B112" s="12"/>
       <c r="C112" s="11"/>
       <c r="D112" s="12"/>
       <c r="E112" s="12"/>
     </row>
-    <row r="113" spans="1:5" ht="15.75" customHeight="1">
+    <row r="113" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" s="11"/>
       <c r="B113" s="12"/>
       <c r="C113" s="11"/>
       <c r="D113" s="12"/>
       <c r="E113" s="12"/>
     </row>
-    <row r="114" spans="1:5" ht="15.75" customHeight="1">
+    <row r="114" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A114" s="11"/>
       <c r="B114" s="12"/>
       <c r="C114" s="11"/>
       <c r="D114" s="12"/>
       <c r="E114" s="12"/>
     </row>
-    <row r="115" spans="1:5" ht="15.75" customHeight="1">
+    <row r="115" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A115" s="11"/>
       <c r="B115" s="12"/>
       <c r="C115" s="11"/>
       <c r="D115" s="12"/>
       <c r="E115" s="12"/>
     </row>
-    <row r="116" spans="1:5" ht="15.75" customHeight="1">
+    <row r="116" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A116" s="11"/>
       <c r="B116" s="12"/>
       <c r="C116" s="11"/>
       <c r="D116" s="12"/>
       <c r="E116" s="12"/>
     </row>
-    <row r="117" spans="1:5" ht="15.75" customHeight="1">
+    <row r="117" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A117" s="11"/>
       <c r="B117" s="12"/>
       <c r="C117" s="11"/>
       <c r="D117" s="12"/>
       <c r="E117" s="12"/>
     </row>
-    <row r="118" spans="1:5" ht="15.75" customHeight="1">
+    <row r="118" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A118" s="11"/>
       <c r="B118" s="12"/>
       <c r="C118" s="11"/>
       <c r="D118" s="12"/>
       <c r="E118" s="12"/>
     </row>
-    <row r="119" spans="1:5" ht="15.75" customHeight="1">
+    <row r="119" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A119" s="11"/>
       <c r="B119" s="12"/>
       <c r="C119" s="11"/>
       <c r="D119" s="12"/>
       <c r="E119" s="12"/>
     </row>
-    <row r="120" spans="1:5" ht="15.75" customHeight="1">
+    <row r="120" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A120" s="11"/>
       <c r="B120" s="12"/>
       <c r="C120" s="11"/>
       <c r="D120" s="12"/>
       <c r="E120" s="12"/>
     </row>
-    <row r="121" spans="1:5" ht="15.75" customHeight="1">
+    <row r="121" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A121" s="11"/>
       <c r="B121" s="12"/>
       <c r="C121" s="11"/>
       <c r="D121" s="12"/>
       <c r="E121" s="12"/>
     </row>
-    <row r="122" spans="1:5" ht="15.75" customHeight="1">
+    <row r="122" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A122" s="11"/>
       <c r="B122" s="12"/>
       <c r="C122" s="11"/>
       <c r="D122" s="12"/>
       <c r="E122" s="12"/>
     </row>
-    <row r="123" spans="1:5" ht="15.75" customHeight="1">
+    <row r="123" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A123" s="11"/>
       <c r="B123" s="12"/>
       <c r="C123" s="11"/>
       <c r="D123" s="12"/>
       <c r="E123" s="12"/>
     </row>
-    <row r="124" spans="1:5" ht="15.75" customHeight="1">
+    <row r="124" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A124" s="11"/>
       <c r="B124" s="12"/>
       <c r="C124" s="11"/>
       <c r="D124" s="12"/>
       <c r="E124" s="12"/>
     </row>
-    <row r="125" spans="1:5" ht="15.75" customHeight="1">
+    <row r="125" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A125" s="11"/>
       <c r="B125" s="12"/>
       <c r="C125" s="11"/>
       <c r="D125" s="12"/>
       <c r="E125" s="12"/>
     </row>
-    <row r="126" spans="1:5" ht="15.75" customHeight="1">
+    <row r="126" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A126" s="11"/>
       <c r="B126" s="12"/>
       <c r="C126" s="11"/>
       <c r="D126" s="12"/>
       <c r="E126" s="12"/>
     </row>
-    <row r="127" spans="1:5" ht="15.75" customHeight="1">
+    <row r="127" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A127" s="11"/>
       <c r="B127" s="12"/>
       <c r="C127" s="11"/>
       <c r="D127" s="12"/>
       <c r="E127" s="12"/>
     </row>
-    <row r="128" spans="1:5" ht="15.75" customHeight="1">
+    <row r="128" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A128" s="11"/>
       <c r="B128" s="12"/>
       <c r="C128" s="11"/>
       <c r="D128" s="12"/>
       <c r="E128" s="12"/>
     </row>
-    <row r="129" spans="1:5" ht="15.75" customHeight="1">
+    <row r="129" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A129" s="11"/>
       <c r="B129" s="12"/>
       <c r="C129" s="11"/>
       <c r="D129" s="12"/>
       <c r="E129" s="12"/>
     </row>
-    <row r="130" spans="1:5" ht="15.75" customHeight="1">
+    <row r="130" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A130" s="11"/>
       <c r="B130" s="12"/>
       <c r="C130" s="11"/>
       <c r="D130" s="12"/>
       <c r="E130" s="12"/>
     </row>
-    <row r="131" spans="1:5" ht="15.75" customHeight="1">
+    <row r="131" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A131" s="11"/>
       <c r="B131" s="12"/>
       <c r="C131" s="11"/>
       <c r="D131" s="12"/>
       <c r="E131" s="12"/>
     </row>
-    <row r="132" spans="1:5" ht="15.75" customHeight="1">
+    <row r="132" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A132" s="11"/>
       <c r="B132" s="12"/>
       <c r="C132" s="11"/>
       <c r="D132" s="12"/>
       <c r="E132" s="12"/>
     </row>
-    <row r="133" spans="1:5" ht="15.75" customHeight="1">
+    <row r="133" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A133" s="11"/>
       <c r="B133" s="12"/>
       <c r="C133" s="11"/>
       <c r="D133" s="12"/>
       <c r="E133" s="12"/>
     </row>
-    <row r="134" spans="1:5" ht="15.75" customHeight="1">
+    <row r="134" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A134" s="11"/>
       <c r="B134" s="12"/>
       <c r="C134" s="11"/>
       <c r="D134" s="12"/>
       <c r="E134" s="12"/>
     </row>
-    <row r="135" spans="1:5" ht="15.75" customHeight="1">
+    <row r="135" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A135" s="11"/>
       <c r="B135" s="12"/>
       <c r="C135" s="11"/>
       <c r="D135" s="12"/>
       <c r="E135" s="12"/>
     </row>
-    <row r="136" spans="1:5" ht="15.75" customHeight="1">
+    <row r="136" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A136" s="11"/>
       <c r="B136" s="12"/>
       <c r="C136" s="11"/>
       <c r="D136" s="12"/>
       <c r="E136" s="12"/>
     </row>
-    <row r="137" spans="1:5" ht="15.75" customHeight="1">
+    <row r="137" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A137" s="11"/>
       <c r="B137" s="12"/>
       <c r="C137" s="11"/>
       <c r="D137" s="12"/>
       <c r="E137" s="12"/>
     </row>
-    <row r="138" spans="1:5" ht="15.75" customHeight="1">
+    <row r="138" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A138" s="11"/>
       <c r="B138" s="12"/>
       <c r="C138" s="11"/>
       <c r="D138" s="12"/>
       <c r="E138" s="12"/>
     </row>
-    <row r="139" spans="1:5" ht="15.75" customHeight="1">
+    <row r="139" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A139" s="11"/>
       <c r="B139" s="12"/>
       <c r="C139" s="11"/>
       <c r="D139" s="12"/>
       <c r="E139" s="12"/>
     </row>
-    <row r="140" spans="1:5" ht="15.75" customHeight="1">
+    <row r="140" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A140" s="11"/>
       <c r="B140" s="12"/>
       <c r="C140" s="11"/>
       <c r="D140" s="12"/>
       <c r="E140" s="12"/>
     </row>
-    <row r="141" spans="1:5" ht="15.75" customHeight="1">
+    <row r="141" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A141" s="11"/>
       <c r="B141" s="12"/>
       <c r="C141" s="11"/>
       <c r="D141" s="12"/>
       <c r="E141" s="12"/>
     </row>
-    <row r="142" spans="1:5" ht="15.75" customHeight="1">
+    <row r="142" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A142" s="11"/>
       <c r="B142" s="12"/>
       <c r="C142" s="11"/>
       <c r="D142" s="12"/>
       <c r="E142" s="12"/>
     </row>
-    <row r="143" spans="1:5" ht="15.75" customHeight="1">
+    <row r="143" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A143" s="11"/>
       <c r="B143" s="12"/>
       <c r="C143" s="11"/>
       <c r="D143" s="12"/>
       <c r="E143" s="12"/>
     </row>
-    <row r="144" spans="1:5" ht="15.75" customHeight="1">
+    <row r="144" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A144" s="11"/>
       <c r="B144" s="12"/>
       <c r="C144" s="11"/>
       <c r="D144" s="12"/>
       <c r="E144" s="12"/>
     </row>
-    <row r="145" spans="1:5" ht="15.75" customHeight="1">
+    <row r="145" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A145" s="11"/>
       <c r="B145" s="12"/>
       <c r="C145" s="11"/>
       <c r="D145" s="12"/>
       <c r="E145" s="12"/>
     </row>
-    <row r="146" spans="1:5" ht="15.75" customHeight="1">
+    <row r="146" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A146" s="11"/>
       <c r="B146" s="12"/>
       <c r="C146" s="11"/>
       <c r="D146" s="12"/>
       <c r="E146" s="12"/>
     </row>
-    <row r="147" spans="1:5" ht="15.75" customHeight="1">
+    <row r="147" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A147" s="11"/>
       <c r="B147" s="12"/>
       <c r="C147" s="11"/>
       <c r="D147" s="12"/>
       <c r="E147" s="12"/>
     </row>
-    <row r="148" spans="1:5" ht="15.75" customHeight="1">
+    <row r="148" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A148" s="11"/>
       <c r="B148" s="12"/>
       <c r="C148" s="11"/>
       <c r="D148" s="12"/>
       <c r="E148" s="12"/>
     </row>
-    <row r="149" spans="1:5" ht="15.75" customHeight="1">
+    <row r="149" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A149" s="11"/>
       <c r="B149" s="12"/>
       <c r="C149" s="11"/>
       <c r="D149" s="12"/>
       <c r="E149" s="12"/>
     </row>
-    <row r="150" spans="1:5" ht="15.75" customHeight="1">
+    <row r="150" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A150" s="11"/>
       <c r="B150" s="12"/>
       <c r="C150" s="11"/>
       <c r="D150" s="12"/>
       <c r="E150" s="12"/>
     </row>
-    <row r="151" spans="1:5" ht="15.75" customHeight="1">
+    <row r="151" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A151" s="11"/>
       <c r="B151" s="12"/>
       <c r="C151" s="11"/>
       <c r="D151" s="12"/>
       <c r="E151" s="12"/>
     </row>
-    <row r="152" spans="1:5" ht="15.75" customHeight="1">
+    <row r="152" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A152" s="11"/>
       <c r="B152" s="12"/>
       <c r="C152" s="11"/>
       <c r="D152" s="12"/>
       <c r="E152" s="12"/>
     </row>
-    <row r="153" spans="1:5" ht="15.75" customHeight="1">
+    <row r="153" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A153" s="11"/>
       <c r="B153" s="12"/>
       <c r="C153" s="11"/>
       <c r="D153" s="12"/>
       <c r="E153" s="12"/>
     </row>
-    <row r="154" spans="1:5" ht="15.75" customHeight="1">
+    <row r="154" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A154" s="11"/>
       <c r="B154" s="12"/>
       <c r="C154" s="11"/>
       <c r="D154" s="12"/>
       <c r="E154" s="12"/>
     </row>
-    <row r="155" spans="1:5" ht="15.75" customHeight="1">
+    <row r="155" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A155" s="11"/>
       <c r="B155" s="12"/>
       <c r="C155" s="11"/>
       <c r="D155" s="12"/>
       <c r="E155" s="12"/>
     </row>
-    <row r="156" spans="1:5" ht="15.75" customHeight="1">
+    <row r="156" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A156" s="11"/>
       <c r="B156" s="12"/>
       <c r="C156" s="11"/>
       <c r="D156" s="12"/>
       <c r="E156" s="12"/>
     </row>
-    <row r="157" spans="1:5" ht="15.75" customHeight="1">
+    <row r="157" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A157" s="11"/>
       <c r="B157" s="12"/>
       <c r="C157" s="11"/>
       <c r="D157" s="12"/>
       <c r="E157" s="12"/>
     </row>
-    <row r="158" spans="1:5" ht="15.75" customHeight="1">
+    <row r="158" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A158" s="11"/>
       <c r="B158" s="12"/>
       <c r="C158" s="11"/>
       <c r="D158" s="12"/>
       <c r="E158" s="12"/>
     </row>
-    <row r="159" spans="1:5" ht="15.75" customHeight="1">
+    <row r="159" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A159" s="11"/>
       <c r="B159" s="12"/>
       <c r="C159" s="11"/>
       <c r="D159" s="12"/>
       <c r="E159" s="12"/>
     </row>
-    <row r="160" spans="1:5" ht="15.75" customHeight="1">
+    <row r="160" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A160" s="11"/>
       <c r="B160" s="12"/>
       <c r="C160" s="11"/>
       <c r="D160" s="12"/>
       <c r="E160" s="12"/>
     </row>
-    <row r="161" spans="1:5" ht="15.75" customHeight="1">
+    <row r="161" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A161" s="11"/>
       <c r="B161" s="12"/>
       <c r="C161" s="11"/>
       <c r="D161" s="12"/>
       <c r="E161" s="12"/>
     </row>
-    <row r="162" spans="1:5" ht="15.75" customHeight="1">
+    <row r="162" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A162" s="11"/>
       <c r="B162" s="12"/>
       <c r="C162" s="11"/>
       <c r="D162" s="12"/>
       <c r="E162" s="12"/>
     </row>
-    <row r="163" spans="1:5" ht="15.75" customHeight="1">
+    <row r="163" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A163" s="11"/>
       <c r="B163" s="12"/>
       <c r="C163" s="11"/>
       <c r="D163" s="12"/>
       <c r="E163" s="12"/>
     </row>
-    <row r="164" spans="1:5" ht="15.75" customHeight="1">
+    <row r="164" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A164" s="11"/>
       <c r="B164" s="12"/>
       <c r="C164" s="11"/>
       <c r="D164" s="12"/>
       <c r="E164" s="12"/>
     </row>
-    <row r="165" spans="1:5" ht="15.75" customHeight="1">
+    <row r="165" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A165" s="11"/>
       <c r="B165" s="12"/>
       <c r="C165" s="11"/>
       <c r="D165" s="12"/>
       <c r="E165" s="12"/>
     </row>
-    <row r="166" spans="1:5" ht="15.75" customHeight="1">
+    <row r="166" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A166" s="11"/>
       <c r="B166" s="12"/>
       <c r="C166" s="11"/>
       <c r="D166" s="12"/>
       <c r="E166" s="12"/>
     </row>
-    <row r="167" spans="1:5" ht="15.75" customHeight="1">
+    <row r="167" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A167" s="11"/>
       <c r="B167" s="12"/>
       <c r="C167" s="11"/>
       <c r="D167" s="12"/>
       <c r="E167" s="12"/>
     </row>
-    <row r="168" spans="1:5" ht="15.75" customHeight="1">
+    <row r="168" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A168" s="11"/>
       <c r="B168" s="12"/>
       <c r="C168" s="11"/>
       <c r="D168" s="12"/>
       <c r="E168" s="12"/>
     </row>
-    <row r="169" spans="1:5" ht="15.75" customHeight="1">
+    <row r="169" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A169" s="11"/>
       <c r="B169" s="12"/>
       <c r="C169" s="11"/>
       <c r="D169" s="12"/>
       <c r="E169" s="12"/>
     </row>
-    <row r="170" spans="1:5" ht="15.75" customHeight="1">
+    <row r="170" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A170" s="11"/>
       <c r="B170" s="12"/>
       <c r="C170" s="11"/>
       <c r="D170" s="12"/>
       <c r="E170" s="12"/>
     </row>
-    <row r="171" spans="1:5" ht="15.75" customHeight="1">
+    <row r="171" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A171" s="11"/>
       <c r="B171" s="12"/>
       <c r="C171" s="11"/>
       <c r="D171" s="12"/>
       <c r="E171" s="12"/>
     </row>
-    <row r="172" spans="1:5" ht="15.75" customHeight="1">
+    <row r="172" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A172" s="11"/>
       <c r="B172" s="12"/>
       <c r="C172" s="11"/>
       <c r="D172" s="12"/>
       <c r="E172" s="12"/>
     </row>
-    <row r="173" spans="1:5" ht="15.75" customHeight="1">
+    <row r="173" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A173" s="11"/>
       <c r="B173" s="12"/>
       <c r="C173" s="11"/>
       <c r="D173" s="12"/>
       <c r="E173" s="12"/>
     </row>
-    <row r="174" spans="1:5" ht="15.75" customHeight="1">
+    <row r="174" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A174" s="11"/>
       <c r="B174" s="12"/>
       <c r="C174" s="11"/>
       <c r="D174" s="12"/>
       <c r="E174" s="12"/>
     </row>
-    <row r="175" spans="1:5" ht="15.75" customHeight="1">
+    <row r="175" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A175" s="11"/>
       <c r="B175" s="12"/>
       <c r="C175" s="11"/>
       <c r="D175" s="12"/>
       <c r="E175" s="12"/>
     </row>
-    <row r="176" spans="1:5" ht="15.75" customHeight="1">
+    <row r="176" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A176" s="11"/>
       <c r="B176" s="12"/>
       <c r="C176" s="11"/>
       <c r="D176" s="12"/>
       <c r="E176" s="12"/>
     </row>
-    <row r="177" spans="1:5" ht="15.75" customHeight="1">
+    <row r="177" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A177" s="11"/>
       <c r="B177" s="12"/>
       <c r="C177" s="11"/>
       <c r="D177" s="12"/>
       <c r="E177" s="12"/>
     </row>
-    <row r="178" spans="1:5" ht="15.75" customHeight="1">
+    <row r="178" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A178" s="11"/>
       <c r="B178" s="12"/>
       <c r="C178" s="11"/>
       <c r="D178" s="12"/>
       <c r="E178" s="12"/>
     </row>
-    <row r="179" spans="1:5" ht="15.75" customHeight="1">
+    <row r="179" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A179" s="11"/>
       <c r="B179" s="12"/>
       <c r="C179" s="11"/>
       <c r="D179" s="12"/>
       <c r="E179" s="12"/>
     </row>
-    <row r="180" spans="1:5" ht="15.75" customHeight="1">
+    <row r="180" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A180" s="11"/>
       <c r="B180" s="12"/>
       <c r="C180" s="11"/>
       <c r="D180" s="12"/>
       <c r="E180" s="12"/>
     </row>
-    <row r="181" spans="1:5" ht="15.75" customHeight="1">
+    <row r="181" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A181" s="11"/>
       <c r="B181" s="12"/>
       <c r="C181" s="11"/>
       <c r="D181" s="12"/>
       <c r="E181" s="12"/>
     </row>
-    <row r="182" spans="1:5" ht="15.75" customHeight="1">
+    <row r="182" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A182" s="11"/>
       <c r="B182" s="12"/>
       <c r="C182" s="11"/>
       <c r="D182" s="12"/>
       <c r="E182" s="12"/>
     </row>
-    <row r="183" spans="1:5" ht="15.75" customHeight="1">
+    <row r="183" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A183" s="11"/>
       <c r="B183" s="12"/>
       <c r="C183" s="11"/>
       <c r="D183" s="12"/>
       <c r="E183" s="12"/>
     </row>
-    <row r="184" spans="1:5" ht="15.75" customHeight="1">
+    <row r="184" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A184" s="11"/>
       <c r="B184" s="12"/>
       <c r="C184" s="11"/>
       <c r="D184" s="12"/>
       <c r="E184" s="12"/>
     </row>
-    <row r="185" spans="1:5" ht="15.75" customHeight="1">
+    <row r="185" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A185" s="11"/>
       <c r="B185" s="12"/>
       <c r="C185" s="11"/>
       <c r="D185" s="12"/>
       <c r="E185" s="12"/>
     </row>
-    <row r="186" spans="1:5" ht="15.75" customHeight="1">
+    <row r="186" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A186" s="11"/>
       <c r="B186" s="12"/>
       <c r="C186" s="11"/>
       <c r="D186" s="12"/>
       <c r="E186" s="12"/>
     </row>
-    <row r="187" spans="1:5" ht="15.75" customHeight="1">
+    <row r="187" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A187" s="11"/>
       <c r="B187" s="12"/>
       <c r="C187" s="11"/>
       <c r="D187" s="12"/>
       <c r="E187" s="12"/>
     </row>
-    <row r="188" spans="1:5" ht="15.75" customHeight="1">
+    <row r="188" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A188" s="11"/>
       <c r="B188" s="12"/>
       <c r="C188" s="11"/>
       <c r="D188" s="12"/>
       <c r="E188" s="12"/>
     </row>
-    <row r="189" spans="1:5" ht="15.75" customHeight="1">
+    <row r="189" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A189" s="11"/>
       <c r="B189" s="12"/>
       <c r="C189" s="11"/>
       <c r="D189" s="12"/>
       <c r="E189" s="12"/>
     </row>
-    <row r="190" spans="1:5" ht="15.75" customHeight="1">
+    <row r="190" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A190" s="11"/>
       <c r="B190" s="12"/>
       <c r="C190" s="11"/>
       <c r="D190" s="12"/>
       <c r="E190" s="12"/>
     </row>
-    <row r="191" spans="1:5" ht="15.75" customHeight="1">
+    <row r="191" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A191" s="11"/>
       <c r="B191" s="12"/>
       <c r="C191" s="11"/>
       <c r="D191" s="12"/>
       <c r="E191" s="12"/>
     </row>
-    <row r="192" spans="1:5" ht="15.75" customHeight="1">
+    <row r="192" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A192" s="11"/>
       <c r="B192" s="12"/>
       <c r="C192" s="11"/>
       <c r="D192" s="12"/>
       <c r="E192" s="12"/>
     </row>
-    <row r="193" spans="1:5" ht="15.75" customHeight="1">
+    <row r="193" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A193" s="11"/>
       <c r="B193" s="12"/>
       <c r="C193" s="11"/>
       <c r="D193" s="12"/>
       <c r="E193" s="12"/>
     </row>
-    <row r="194" spans="1:5" ht="15.75" customHeight="1">
+    <row r="194" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A194" s="11"/>
       <c r="B194" s="12"/>
       <c r="C194" s="11"/>
       <c r="D194" s="12"/>
       <c r="E194" s="12"/>
     </row>
-    <row r="195" spans="1:5" ht="15.75" customHeight="1">
+    <row r="195" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A195" s="11"/>
       <c r="B195" s="12"/>
       <c r="C195" s="11"/>
       <c r="D195" s="12"/>
       <c r="E195" s="12"/>
     </row>
-    <row r="196" spans="1:5" ht="15.75" customHeight="1">
+    <row r="196" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A196" s="11"/>
       <c r="B196" s="12"/>
       <c r="C196" s="11"/>
       <c r="D196" s="12"/>
       <c r="E196" s="12"/>
     </row>
-    <row r="197" spans="1:5" ht="15.75" customHeight="1">
+    <row r="197" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A197" s="11"/>
       <c r="B197" s="12"/>
       <c r="C197" s="11"/>
       <c r="D197" s="12"/>
       <c r="E197" s="12"/>
     </row>
-    <row r="198" spans="1:5" ht="15.75" customHeight="1">
+    <row r="198" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A198" s="11"/>
       <c r="B198" s="12"/>
       <c r="C198" s="11"/>
       <c r="D198" s="12"/>
       <c r="E198" s="12"/>
     </row>
-    <row r="199" spans="1:5" ht="15.75" customHeight="1">
+    <row r="199" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A199" s="11"/>
       <c r="B199" s="12"/>
       <c r="C199" s="11"/>
       <c r="D199" s="12"/>
       <c r="E199" s="12"/>
     </row>
-    <row r="200" spans="1:5" ht="15.75" customHeight="1">
+    <row r="200" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A200" s="11"/>
       <c r="B200" s="12"/>
       <c r="C200" s="11"/>
       <c r="D200" s="12"/>
       <c r="E200" s="12"/>
     </row>
-    <row r="201" spans="1:5" ht="15.75" customHeight="1">
+    <row r="201" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A201" s="11"/>
       <c r="B201" s="12"/>
       <c r="C201" s="11"/>
       <c r="D201" s="12"/>
       <c r="E201" s="12"/>
     </row>
-    <row r="202" spans="1:5" ht="15.75" customHeight="1">
+    <row r="202" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A202" s="11"/>
       <c r="B202" s="12"/>
       <c r="C202" s="11"/>
       <c r="D202" s="12"/>
       <c r="E202" s="12"/>
     </row>
-    <row r="203" spans="1:5" ht="15.75" customHeight="1">
+    <row r="203" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A203" s="11"/>
       <c r="B203" s="12"/>
       <c r="C203" s="11"/>
       <c r="D203" s="12"/>
       <c r="E203" s="12"/>
     </row>
-    <row r="204" spans="1:5" ht="15.75" customHeight="1">
+    <row r="204" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A204" s="11"/>
       <c r="B204" s="12"/>
       <c r="C204" s="11"/>
       <c r="D204" s="12"/>
       <c r="E204" s="12"/>
     </row>
-    <row r="205" spans="1:5" ht="15.75" customHeight="1">
+    <row r="205" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A205" s="11"/>
       <c r="B205" s="12"/>
       <c r="C205" s="11"/>
       <c r="D205" s="12"/>
       <c r="E205" s="12"/>
     </row>
-    <row r="206" spans="1:5" ht="15.75" customHeight="1">
+    <row r="206" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A206" s="11"/>
       <c r="B206" s="12"/>
       <c r="C206" s="11"/>
       <c r="D206" s="12"/>
       <c r="E206" s="12"/>
     </row>
-    <row r="207" spans="1:5" ht="15.75" customHeight="1">
+    <row r="207" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A207" s="11"/>
       <c r="B207" s="12"/>
       <c r="C207" s="11"/>
       <c r="D207" s="12"/>
       <c r="E207" s="12"/>
     </row>
-    <row r="208" spans="1:5" ht="15.75" customHeight="1">
+    <row r="208" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A208" s="11"/>
       <c r="B208" s="12"/>
       <c r="C208" s="11"/>
       <c r="D208" s="12"/>
       <c r="E208" s="12"/>
     </row>
-    <row r="209" spans="1:5" ht="15.75" customHeight="1">
+    <row r="209" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A209" s="11"/>
       <c r="B209" s="12"/>
       <c r="C209" s="11"/>
       <c r="D209" s="12"/>
       <c r="E209" s="12"/>
     </row>
-    <row r="210" spans="1:5" ht="15.75" customHeight="1">
+    <row r="210" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A210" s="11"/>
       <c r="B210" s="12"/>
       <c r="C210" s="11"/>
       <c r="D210" s="12"/>
       <c r="E210" s="12"/>
     </row>
-    <row r="211" spans="1:5" ht="15.75" customHeight="1">
+    <row r="211" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A211" s="11"/>
       <c r="B211" s="12"/>
       <c r="C211" s="11"/>
       <c r="D211" s="12"/>
       <c r="E211" s="12"/>
     </row>
-    <row r="212" spans="1:5" ht="15.75" customHeight="1">
+    <row r="212" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A212" s="11"/>
       <c r="B212" s="12"/>
       <c r="C212" s="11"/>
       <c r="D212" s="12"/>
       <c r="E212" s="12"/>
     </row>
-    <row r="213" spans="1:5" ht="15.75" customHeight="1">
+    <row r="213" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A213" s="11"/>
       <c r="B213" s="12"/>
       <c r="C213" s="11"/>
       <c r="D213" s="12"/>
       <c r="E213" s="12"/>
     </row>
-    <row r="214" spans="1:5" ht="15.75" customHeight="1">
+    <row r="214" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A214" s="11"/>
       <c r="B214" s="12"/>
       <c r="C214" s="11"/>
       <c r="D214" s="12"/>
       <c r="E214" s="12"/>
     </row>
-    <row r="215" spans="1:5" ht="15.75" customHeight="1">
+    <row r="215" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A215" s="11"/>
       <c r="B215" s="12"/>
       <c r="C215" s="11"/>
       <c r="D215" s="12"/>
       <c r="E215" s="12"/>
     </row>
-    <row r="216" spans="1:5" ht="15.75" customHeight="1">
+    <row r="216" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A216" s="11"/>
       <c r="B216" s="12"/>
       <c r="C216" s="11"/>
       <c r="D216" s="12"/>
       <c r="E216" s="12"/>
     </row>
-    <row r="217" spans="1:5" ht="15.75" customHeight="1">
+    <row r="217" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A217" s="11"/>
       <c r="B217" s="12"/>
       <c r="C217" s="11"/>
       <c r="D217" s="12"/>
       <c r="E217" s="12"/>
     </row>
-    <row r="218" spans="1:5" ht="15.75" customHeight="1">
+    <row r="218" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A218" s="11"/>
       <c r="B218" s="12"/>
       <c r="C218" s="11"/>
       <c r="D218" s="12"/>
       <c r="E218" s="12"/>
     </row>
-    <row r="219" spans="1:5" ht="15.75" customHeight="1">
+    <row r="219" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A219" s="11"/>
       <c r="B219" s="12"/>
       <c r="C219" s="11"/>
       <c r="D219" s="12"/>
       <c r="E219" s="12"/>
     </row>
-    <row r="220" spans="1:5" ht="15.75" customHeight="1">
+    <row r="220" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A220" s="11"/>
       <c r="B220" s="12"/>
       <c r="C220" s="11"/>
       <c r="D220" s="12"/>
       <c r="E220" s="12"/>
     </row>
-    <row r="221" spans="1:5" ht="15.75" customHeight="1">
+    <row r="221" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A221" s="11"/>
       <c r="B221" s="12"/>
       <c r="C221" s="11"/>
       <c r="D221" s="12"/>
       <c r="E221" s="12"/>
     </row>
-    <row r="222" spans="1:5" ht="15.75" customHeight="1">
+    <row r="222" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A222" s="11"/>
       <c r="B222" s="12"/>
       <c r="C222" s="11"/>
       <c r="D222" s="12"/>
       <c r="E222" s="12"/>
     </row>
-    <row r="223" spans="1:5" ht="15.75" customHeight="1">
+    <row r="223" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A223" s="11"/>
       <c r="B223" s="12"/>
       <c r="C223" s="11"/>
       <c r="D223" s="12"/>
       <c r="E223" s="12"/>
     </row>
-    <row r="224" spans="1:5" ht="15.75" customHeight="1">
+    <row r="224" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A224" s="11"/>
       <c r="B224" s="12"/>
       <c r="C224" s="11"/>
       <c r="D224" s="12"/>
       <c r="E224" s="12"/>
     </row>
-    <row r="225" spans="1:5" ht="15.75" customHeight="1">
+    <row r="225" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A225" s="11"/>
       <c r="B225" s="12"/>
       <c r="C225" s="11"/>
       <c r="D225" s="12"/>
       <c r="E225" s="12"/>
     </row>
-    <row r="226" spans="1:5" ht="15.75" customHeight="1">
+    <row r="226" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A226" s="11"/>
       <c r="B226" s="12"/>
       <c r="C226" s="11"/>
       <c r="D226" s="12"/>
       <c r="E226" s="12"/>
     </row>
-    <row r="227" spans="1:5" ht="15.75" customHeight="1">
+    <row r="227" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A227" s="11"/>
       <c r="B227" s="12"/>
       <c r="C227" s="11"/>
       <c r="D227" s="12"/>
       <c r="E227" s="12"/>
     </row>
-    <row r="228" spans="1:5" ht="15.75" customHeight="1">
+    <row r="228" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A228" s="11"/>
       <c r="B228" s="12"/>
       <c r="C228" s="11"/>
       <c r="D228" s="12"/>
       <c r="E228" s="12"/>
     </row>
-    <row r="229" spans="1:5" ht="15.75" customHeight="1">
+    <row r="229" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A229" s="11"/>
       <c r="B229" s="12"/>
       <c r="C229" s="11"/>
       <c r="D229" s="12"/>
       <c r="E229" s="12"/>
     </row>
-    <row r="230" spans="1:5" ht="15.75" customHeight="1">
+    <row r="230" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A230" s="11"/>
       <c r="B230" s="12"/>
       <c r="C230" s="11"/>
       <c r="D230" s="12"/>
       <c r="E230" s="12"/>
     </row>
-    <row r="231" spans="1:5" ht="15.75" customHeight="1">
+    <row r="231" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A231" s="11"/>
       <c r="B231" s="12"/>
       <c r="C231" s="11"/>
       <c r="D231" s="12"/>
       <c r="E231" s="12"/>
     </row>
-    <row r="232" spans="1:5" ht="15.75" customHeight="1">
+    <row r="232" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A232" s="11"/>
       <c r="B232" s="12"/>
       <c r="C232" s="11"/>
       <c r="D232" s="12"/>
       <c r="E232" s="12"/>
     </row>
-    <row r="233" spans="1:5" ht="15.75" customHeight="1">
+    <row r="233" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A233" s="11"/>
       <c r="B233" s="12"/>
       <c r="C233" s="11"/>
       <c r="D233" s="12"/>
       <c r="E233" s="12"/>
     </row>
-    <row r="234" spans="1:5" ht="15.75" customHeight="1">
+    <row r="234" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A234" s="11"/>
       <c r="B234" s="12"/>
       <c r="C234" s="11"/>
       <c r="D234" s="12"/>
       <c r="E234" s="12"/>
     </row>
-    <row r="235" spans="1:5" ht="15.75" customHeight="1">
+    <row r="235" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A235" s="11"/>
       <c r="B235" s="12"/>
       <c r="C235" s="11"/>
       <c r="D235" s="12"/>
       <c r="E235" s="12"/>
     </row>
-    <row r="236" spans="1:5" ht="15.75" customHeight="1">
+    <row r="236" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A236" s="11"/>
       <c r="B236" s="12"/>
       <c r="C236" s="11"/>
       <c r="D236" s="12"/>
       <c r="E236" s="12"/>
     </row>
-    <row r="237" spans="1:5" ht="15.75" customHeight="1">
+    <row r="237" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A237" s="11"/>
       <c r="B237" s="12"/>
       <c r="C237" s="11"/>
       <c r="D237" s="12"/>
       <c r="E237" s="12"/>
     </row>
-    <row r="238" spans="1:5" ht="15.75" customHeight="1">
+    <row r="238" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A238" s="11"/>
       <c r="B238" s="12"/>
       <c r="C238" s="11"/>
       <c r="D238" s="12"/>
       <c r="E238" s="12"/>
     </row>
-    <row r="239" spans="1:5" ht="15.75" customHeight="1">
+    <row r="239" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A239" s="11"/>
       <c r="B239" s="12"/>
       <c r="C239" s="11"/>
       <c r="D239" s="12"/>
       <c r="E239" s="12"/>
     </row>
-    <row r="240" spans="1:5" ht="15.75" customHeight="1">
+    <row r="240" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A240" s="11"/>
       <c r="B240" s="12"/>
       <c r="C240" s="11"/>
       <c r="D240" s="12"/>
       <c r="E240" s="12"/>
     </row>
-    <row r="241" spans="1:5" ht="15.75" customHeight="1">
+    <row r="241" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A241" s="11"/>
       <c r="B241" s="12"/>
       <c r="C241" s="11"/>
       <c r="D241" s="12"/>
       <c r="E241" s="12"/>
     </row>
-    <row r="242" spans="1:5" ht="15.75" customHeight="1">
+    <row r="242" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A242" s="11"/>
       <c r="B242" s="12"/>
       <c r="C242" s="11"/>
       <c r="D242" s="12"/>
       <c r="E242" s="12"/>
     </row>
-    <row r="243" spans="1:5" ht="15.75" customHeight="1">
+    <row r="243" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A243" s="11"/>
       <c r="B243" s="12"/>
       <c r="C243" s="11"/>
       <c r="D243" s="12"/>
       <c r="E243" s="12"/>
     </row>
-    <row r="244" spans="1:5" ht="15.75" customHeight="1">
+    <row r="244" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A244" s="11"/>
       <c r="B244" s="12"/>
       <c r="C244" s="11"/>
       <c r="D244" s="12"/>
       <c r="E244" s="12"/>
     </row>
-    <row r="245" spans="1:5" ht="15.75" customHeight="1">
+    <row r="245" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A245" s="11"/>
       <c r="B245" s="12"/>
       <c r="C245" s="11"/>
       <c r="D245" s="12"/>
       <c r="E245" s="12"/>
     </row>
-    <row r="246" spans="1:5" ht="15.75" customHeight="1">
+    <row r="246" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A246" s="11"/>
       <c r="B246" s="12"/>
       <c r="C246" s="11"/>
       <c r="D246" s="12"/>
       <c r="E246" s="12"/>
     </row>
-    <row r="247" spans="1:5" ht="15.75" customHeight="1">
+    <row r="247" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A247" s="11"/>
       <c r="B247" s="12"/>
       <c r="C247" s="11"/>
       <c r="D247" s="12"/>
       <c r="E247" s="12"/>
     </row>
-    <row r="248" spans="1:5" ht="15.75" customHeight="1">
+    <row r="248" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A248" s="11"/>
       <c r="B248" s="12"/>
       <c r="C248" s="11"/>
       <c r="D248" s="12"/>
       <c r="E248" s="12"/>
     </row>
-    <row r="249" spans="1:5" ht="15.75" customHeight="1">
+    <row r="249" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A249" s="11"/>
       <c r="B249" s="12"/>
       <c r="C249" s="11"/>
       <c r="D249" s="12"/>
       <c r="E249" s="12"/>
     </row>
-    <row r="250" spans="1:5" ht="15.75" customHeight="1">
+    <row r="250" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A250" s="11"/>
       <c r="B250" s="12"/>
       <c r="C250" s="11"/>
       <c r="D250" s="12"/>
       <c r="E250" s="12"/>
     </row>
-    <row r="251" spans="1:5" ht="15.75" customHeight="1">
+    <row r="251" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A251" s="11"/>
       <c r="B251" s="12"/>
       <c r="C251" s="11"/>
       <c r="D251" s="12"/>
       <c r="E251" s="12"/>
     </row>
-    <row r="252" spans="1:5" ht="15.75" customHeight="1">
+    <row r="252" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A252" s="11"/>
       <c r="B252" s="12"/>
       <c r="C252" s="11"/>
       <c r="D252" s="12"/>
       <c r="E252" s="12"/>
     </row>
-    <row r="253" spans="1:5" ht="15.75" customHeight="1">
+    <row r="253" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A253" s="11"/>
       <c r="B253" s="12"/>
       <c r="C253" s="11"/>
       <c r="D253" s="12"/>
       <c r="E253" s="12"/>
     </row>
-    <row r="254" spans="1:5" ht="15.75" customHeight="1">
+    <row r="254" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A254" s="11"/>
       <c r="B254" s="12"/>
       <c r="C254" s="11"/>
       <c r="D254" s="12"/>
       <c r="E254" s="12"/>
     </row>
-    <row r="255" spans="1:5" ht="15.75" customHeight="1">
+    <row r="255" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A255" s="11"/>
       <c r="B255" s="12"/>
       <c r="C255" s="11"/>
       <c r="D255" s="12"/>
       <c r="E255" s="12"/>
     </row>
-    <row r="256" spans="1:5" ht="15.75" customHeight="1">
+    <row r="256" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A256" s="11"/>
       <c r="B256" s="12"/>
       <c r="C256" s="11"/>
       <c r="D256" s="12"/>
       <c r="E256" s="12"/>
     </row>
-    <row r="257" spans="1:5" ht="15.75" customHeight="1">
+    <row r="257" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A257" s="11"/>
       <c r="B257" s="12"/>
       <c r="C257" s="11"/>
       <c r="D257" s="12"/>
       <c r="E257" s="12"/>
     </row>
-    <row r="258" spans="1:5" ht="15.75" customHeight="1">
+    <row r="258" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A258" s="11"/>
       <c r="B258" s="12"/>
       <c r="C258" s="11"/>
       <c r="D258" s="12"/>
       <c r="E258" s="12"/>
     </row>
-    <row r="259" spans="1:5" ht="15.75" customHeight="1">
+    <row r="259" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A259" s="11"/>
       <c r="B259" s="12"/>
       <c r="C259" s="11"/>
       <c r="D259" s="12"/>
       <c r="E259" s="12"/>
     </row>
-    <row r="260" spans="1:5" ht="15.75" customHeight="1">
+    <row r="260" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A260" s="11"/>
       <c r="B260" s="12"/>
       <c r="C260" s="11"/>
       <c r="D260" s="12"/>
       <c r="E260" s="12"/>
     </row>
-    <row r="261" spans="1:5" ht="15.75" customHeight="1"/>
-    <row r="262" spans="1:5" ht="15.75" customHeight="1"/>
-    <row r="263" spans="1:5" ht="15.75" customHeight="1"/>
-    <row r="264" spans="1:5" ht="15.75" customHeight="1"/>
-    <row r="265" spans="1:5" ht="15.75" customHeight="1"/>
-    <row r="266" spans="1:5" ht="15.75" customHeight="1"/>
-    <row r="267" spans="1:5" ht="15.75" customHeight="1"/>
-    <row r="268" spans="1:5" ht="15.75" customHeight="1"/>
-    <row r="269" spans="1:5" ht="15.75" customHeight="1"/>
-    <row r="270" spans="1:5" ht="15.75" customHeight="1"/>
-    <row r="271" spans="1:5" ht="15.75" customHeight="1"/>
-    <row r="272" spans="1:5" ht="15.75" customHeight="1"/>
-    <row r="273" ht="15.75" customHeight="1"/>
-    <row r="274" ht="15.75" customHeight="1"/>
-    <row r="275" ht="15.75" customHeight="1"/>
-    <row r="276" ht="15.75" customHeight="1"/>
-    <row r="277" ht="15.75" customHeight="1"/>
-    <row r="278" ht="15.75" customHeight="1"/>
-    <row r="279" ht="15.75" customHeight="1"/>
-    <row r="280" ht="15.75" customHeight="1"/>
-    <row r="281" ht="15.75" customHeight="1"/>
-    <row r="282" ht="15.75" customHeight="1"/>
-    <row r="283" ht="15.75" customHeight="1"/>
-    <row r="284" ht="15.75" customHeight="1"/>
-    <row r="285" ht="15.75" customHeight="1"/>
-    <row r="286" ht="15.75" customHeight="1"/>
-    <row r="287" ht="15.75" customHeight="1"/>
-    <row r="288" ht="15.75" customHeight="1"/>
-    <row r="289" ht="15.75" customHeight="1"/>
-    <row r="290" ht="15.75" customHeight="1"/>
-    <row r="291" ht="15.75" customHeight="1"/>
-    <row r="292" ht="15.75" customHeight="1"/>
-    <row r="293" ht="15.75" customHeight="1"/>
-    <row r="294" ht="15.75" customHeight="1"/>
-    <row r="295" ht="15.75" customHeight="1"/>
-    <row r="296" ht="15.75" customHeight="1"/>
-    <row r="297" ht="15.75" customHeight="1"/>
-    <row r="298" ht="15.75" customHeight="1"/>
-    <row r="299" ht="15.75" customHeight="1"/>
-    <row r="300" ht="15.75" customHeight="1"/>
-    <row r="301" ht="15.75" customHeight="1"/>
-    <row r="302" ht="15.75" customHeight="1"/>
-    <row r="303" ht="15.75" customHeight="1"/>
-    <row r="304" ht="15.75" customHeight="1"/>
-    <row r="305" ht="15.75" customHeight="1"/>
-    <row r="306" ht="15.75" customHeight="1"/>
-    <row r="307" ht="15.75" customHeight="1"/>
-    <row r="308" ht="15.75" customHeight="1"/>
-    <row r="309" ht="15.75" customHeight="1"/>
-    <row r="310" ht="15.75" customHeight="1"/>
-    <row r="311" ht="15.75" customHeight="1"/>
-    <row r="312" ht="15.75" customHeight="1"/>
-    <row r="313" ht="15.75" customHeight="1"/>
-    <row r="314" ht="15.75" customHeight="1"/>
-    <row r="315" ht="15.75" customHeight="1"/>
-    <row r="316" ht="15.75" customHeight="1"/>
-    <row r="317" ht="15.75" customHeight="1"/>
-    <row r="318" ht="15.75" customHeight="1"/>
-    <row r="319" ht="15.75" customHeight="1"/>
-    <row r="320" ht="15.75" customHeight="1"/>
-    <row r="321" ht="15.75" customHeight="1"/>
-    <row r="322" ht="15.75" customHeight="1"/>
-    <row r="323" ht="15.75" customHeight="1"/>
-    <row r="324" ht="15.75" customHeight="1"/>
-    <row r="325" ht="15.75" customHeight="1"/>
-    <row r="326" ht="15.75" customHeight="1"/>
-    <row r="327" ht="15.75" customHeight="1"/>
-    <row r="328" ht="15.75" customHeight="1"/>
-    <row r="329" ht="15.75" customHeight="1"/>
-    <row r="330" ht="15.75" customHeight="1"/>
-    <row r="331" ht="15.75" customHeight="1"/>
-    <row r="332" ht="15.75" customHeight="1"/>
-    <row r="333" ht="15.75" customHeight="1"/>
-    <row r="334" ht="15.75" customHeight="1"/>
-    <row r="335" ht="15.75" customHeight="1"/>
-    <row r="336" ht="15.75" customHeight="1"/>
-    <row r="337" ht="15.75" customHeight="1"/>
-    <row r="338" ht="15.75" customHeight="1"/>
-    <row r="339" ht="15.75" customHeight="1"/>
-    <row r="340" ht="15.75" customHeight="1"/>
-    <row r="341" ht="15.75" customHeight="1"/>
-    <row r="342" ht="15.75" customHeight="1"/>
-    <row r="343" ht="15.75" customHeight="1"/>
-    <row r="344" ht="15.75" customHeight="1"/>
-    <row r="345" ht="15.75" customHeight="1"/>
-    <row r="346" ht="15.75" customHeight="1"/>
-    <row r="347" ht="15.75" customHeight="1"/>
-    <row r="348" ht="15.75" customHeight="1"/>
-    <row r="349" ht="15.75" customHeight="1"/>
-    <row r="350" ht="15.75" customHeight="1"/>
-    <row r="351" ht="15.75" customHeight="1"/>
-    <row r="352" ht="15.75" customHeight="1"/>
-    <row r="353" ht="15.75" customHeight="1"/>
-    <row r="354" ht="15.75" customHeight="1"/>
-    <row r="355" ht="15.75" customHeight="1"/>
-    <row r="356" ht="15.75" customHeight="1"/>
-    <row r="357" ht="15.75" customHeight="1"/>
-    <row r="358" ht="15.75" customHeight="1"/>
-    <row r="359" ht="15.75" customHeight="1"/>
-    <row r="360" ht="15.75" customHeight="1"/>
-    <row r="361" ht="15.75" customHeight="1"/>
-    <row r="362" ht="15.75" customHeight="1"/>
-    <row r="363" ht="15.75" customHeight="1"/>
-    <row r="364" ht="15.75" customHeight="1"/>
-    <row r="365" ht="15.75" customHeight="1"/>
-    <row r="366" ht="15.75" customHeight="1"/>
-    <row r="367" ht="15.75" customHeight="1"/>
-    <row r="368" ht="15.75" customHeight="1"/>
-    <row r="369" ht="15.75" customHeight="1"/>
-    <row r="370" ht="15.75" customHeight="1"/>
-    <row r="371" ht="15.75" customHeight="1"/>
-    <row r="372" ht="15.75" customHeight="1"/>
-    <row r="373" ht="15.75" customHeight="1"/>
-    <row r="374" ht="15.75" customHeight="1"/>
-    <row r="375" ht="15.75" customHeight="1"/>
-    <row r="376" ht="15.75" customHeight="1"/>
-    <row r="377" ht="15.75" customHeight="1"/>
-    <row r="378" ht="15.75" customHeight="1"/>
-    <row r="379" ht="15.75" customHeight="1"/>
-    <row r="380" ht="15.75" customHeight="1"/>
-    <row r="381" ht="15.75" customHeight="1"/>
-    <row r="382" ht="15.75" customHeight="1"/>
-    <row r="383" ht="15.75" customHeight="1"/>
-    <row r="384" ht="15.75" customHeight="1"/>
-    <row r="385" ht="15.75" customHeight="1"/>
-    <row r="386" ht="15.75" customHeight="1"/>
-    <row r="387" ht="15.75" customHeight="1"/>
-    <row r="388" ht="15.75" customHeight="1"/>
-    <row r="389" ht="15.75" customHeight="1"/>
-    <row r="390" ht="15.75" customHeight="1"/>
-    <row r="391" ht="15.75" customHeight="1"/>
-    <row r="392" ht="15.75" customHeight="1"/>
-    <row r="393" ht="15.75" customHeight="1"/>
-    <row r="394" ht="15.75" customHeight="1"/>
-    <row r="395" ht="15.75" customHeight="1"/>
-    <row r="396" ht="15.75" customHeight="1"/>
-    <row r="397" ht="15.75" customHeight="1"/>
-    <row r="398" ht="15.75" customHeight="1"/>
-    <row r="399" ht="15.75" customHeight="1"/>
-    <row r="400" ht="15.75" customHeight="1"/>
-    <row r="401" ht="15.75" customHeight="1"/>
-    <row r="402" ht="15.75" customHeight="1"/>
-    <row r="403" ht="15.75" customHeight="1"/>
-    <row r="404" ht="15.75" customHeight="1"/>
-    <row r="405" ht="15.75" customHeight="1"/>
-    <row r="406" ht="15.75" customHeight="1"/>
-    <row r="407" ht="15.75" customHeight="1"/>
-    <row r="408" ht="15.75" customHeight="1"/>
-    <row r="409" ht="15.75" customHeight="1"/>
-    <row r="410" ht="15.75" customHeight="1"/>
-    <row r="411" ht="15.75" customHeight="1"/>
-    <row r="412" ht="15.75" customHeight="1"/>
-    <row r="413" ht="15.75" customHeight="1"/>
-    <row r="414" ht="15.75" customHeight="1"/>
-    <row r="415" ht="15.75" customHeight="1"/>
-    <row r="416" ht="15.75" customHeight="1"/>
-    <row r="417" ht="15.75" customHeight="1"/>
-    <row r="418" ht="15.75" customHeight="1"/>
-    <row r="419" ht="15.75" customHeight="1"/>
-    <row r="420" ht="15.75" customHeight="1"/>
-    <row r="421" ht="15.75" customHeight="1"/>
-    <row r="422" ht="15.75" customHeight="1"/>
-    <row r="423" ht="15.75" customHeight="1"/>
-    <row r="424" ht="15.75" customHeight="1"/>
-    <row r="425" ht="15.75" customHeight="1"/>
-    <row r="426" ht="15.75" customHeight="1"/>
-    <row r="427" ht="15.75" customHeight="1"/>
-    <row r="428" ht="15.75" customHeight="1"/>
-    <row r="429" ht="15.75" customHeight="1"/>
-    <row r="430" ht="15.75" customHeight="1"/>
-    <row r="431" ht="15.75" customHeight="1"/>
-    <row r="432" ht="15.75" customHeight="1"/>
-    <row r="433" ht="15.75" customHeight="1"/>
-    <row r="434" ht="15.75" customHeight="1"/>
-    <row r="435" ht="15.75" customHeight="1"/>
-    <row r="436" ht="15.75" customHeight="1"/>
-    <row r="437" ht="15.75" customHeight="1"/>
-    <row r="438" ht="15.75" customHeight="1"/>
-    <row r="439" ht="15.75" customHeight="1"/>
-    <row r="440" ht="15.75" customHeight="1"/>
-    <row r="441" ht="15.75" customHeight="1"/>
-    <row r="442" ht="15.75" customHeight="1"/>
-    <row r="443" ht="15.75" customHeight="1"/>
-    <row r="444" ht="15.75" customHeight="1"/>
-    <row r="445" ht="15.75" customHeight="1"/>
-    <row r="446" ht="15.75" customHeight="1"/>
-    <row r="447" ht="15.75" customHeight="1"/>
-    <row r="448" ht="15.75" customHeight="1"/>
-    <row r="449" ht="15.75" customHeight="1"/>
-    <row r="450" ht="15.75" customHeight="1"/>
-    <row r="451" ht="15.75" customHeight="1"/>
-    <row r="452" ht="15.75" customHeight="1"/>
-    <row r="453" ht="15.75" customHeight="1"/>
-    <row r="454" ht="15.75" customHeight="1"/>
-    <row r="455" ht="15.75" customHeight="1"/>
-    <row r="456" ht="15.75" customHeight="1"/>
-    <row r="457" ht="15.75" customHeight="1"/>
-    <row r="458" ht="15.75" customHeight="1"/>
-    <row r="459" ht="15.75" customHeight="1"/>
-    <row r="460" ht="15.75" customHeight="1"/>
-    <row r="461" ht="15.75" customHeight="1"/>
-    <row r="462" ht="15.75" customHeight="1"/>
-    <row r="463" ht="15.75" customHeight="1"/>
-    <row r="464" ht="15.75" customHeight="1"/>
-    <row r="465" ht="15.75" customHeight="1"/>
-    <row r="466" ht="15.75" customHeight="1"/>
-    <row r="467" ht="15.75" customHeight="1"/>
-    <row r="468" ht="15.75" customHeight="1"/>
-    <row r="469" ht="15.75" customHeight="1"/>
-    <row r="470" ht="15.75" customHeight="1"/>
-    <row r="471" ht="15.75" customHeight="1"/>
-    <row r="472" ht="15.75" customHeight="1"/>
-    <row r="473" ht="15.75" customHeight="1"/>
-    <row r="474" ht="15.75" customHeight="1"/>
-    <row r="475" ht="15.75" customHeight="1"/>
-    <row r="476" ht="15.75" customHeight="1"/>
-    <row r="477" ht="15.75" customHeight="1"/>
-    <row r="478" ht="15.75" customHeight="1"/>
-    <row r="479" ht="15.75" customHeight="1"/>
-    <row r="480" ht="15.75" customHeight="1"/>
-    <row r="481" ht="15.75" customHeight="1"/>
-    <row r="482" ht="15.75" customHeight="1"/>
-    <row r="483" ht="15.75" customHeight="1"/>
-    <row r="484" ht="15.75" customHeight="1"/>
-    <row r="485" ht="15.75" customHeight="1"/>
-    <row r="486" ht="15.75" customHeight="1"/>
-    <row r="487" ht="15.75" customHeight="1"/>
-    <row r="488" ht="15.75" customHeight="1"/>
-    <row r="489" ht="15.75" customHeight="1"/>
-    <row r="490" ht="15.75" customHeight="1"/>
-    <row r="491" ht="15.75" customHeight="1"/>
-    <row r="492" ht="15.75" customHeight="1"/>
-    <row r="493" ht="15.75" customHeight="1"/>
-    <row r="494" ht="15.75" customHeight="1"/>
-    <row r="495" ht="15.75" customHeight="1"/>
-    <row r="496" ht="15.75" customHeight="1"/>
-    <row r="497" ht="15.75" customHeight="1"/>
-    <row r="498" ht="15.75" customHeight="1"/>
-    <row r="499" ht="15.75" customHeight="1"/>
-    <row r="500" ht="15.75" customHeight="1"/>
-    <row r="501" ht="15.75" customHeight="1"/>
-    <row r="502" ht="15.75" customHeight="1"/>
-    <row r="503" ht="15.75" customHeight="1"/>
-    <row r="504" ht="15.75" customHeight="1"/>
-    <row r="505" ht="15.75" customHeight="1"/>
-    <row r="506" ht="15.75" customHeight="1"/>
-    <row r="507" ht="15.75" customHeight="1"/>
-    <row r="508" ht="15.75" customHeight="1"/>
-    <row r="509" ht="15.75" customHeight="1"/>
-    <row r="510" ht="15.75" customHeight="1"/>
-    <row r="511" ht="15.75" customHeight="1"/>
-    <row r="512" ht="15.75" customHeight="1"/>
-    <row r="513" ht="15.75" customHeight="1"/>
-    <row r="514" ht="15.75" customHeight="1"/>
-    <row r="515" ht="15.75" customHeight="1"/>
-    <row r="516" ht="15.75" customHeight="1"/>
-    <row r="517" ht="15.75" customHeight="1"/>
-    <row r="518" ht="15.75" customHeight="1"/>
-    <row r="519" ht="15.75" customHeight="1"/>
-    <row r="520" ht="15.75" customHeight="1"/>
-    <row r="521" ht="15.75" customHeight="1"/>
-    <row r="522" ht="15.75" customHeight="1"/>
-    <row r="523" ht="15.75" customHeight="1"/>
-    <row r="524" ht="15.75" customHeight="1"/>
-    <row r="525" ht="15.75" customHeight="1"/>
-    <row r="526" ht="15.75" customHeight="1"/>
-    <row r="527" ht="15.75" customHeight="1"/>
-    <row r="528" ht="15.75" customHeight="1"/>
-    <row r="529" ht="15.75" customHeight="1"/>
-    <row r="530" ht="15.75" customHeight="1"/>
-    <row r="531" ht="15.75" customHeight="1"/>
-    <row r="532" ht="15.75" customHeight="1"/>
-    <row r="533" ht="15.75" customHeight="1"/>
-    <row r="534" ht="15.75" customHeight="1"/>
-    <row r="535" ht="15.75" customHeight="1"/>
-    <row r="536" ht="15.75" customHeight="1"/>
-    <row r="537" ht="15.75" customHeight="1"/>
-    <row r="538" ht="15.75" customHeight="1"/>
-    <row r="539" ht="15.75" customHeight="1"/>
-    <row r="540" ht="15.75" customHeight="1"/>
-    <row r="541" ht="15.75" customHeight="1"/>
-    <row r="542" ht="15.75" customHeight="1"/>
-    <row r="543" ht="15.75" customHeight="1"/>
-    <row r="544" ht="15.75" customHeight="1"/>
-    <row r="545" ht="15.75" customHeight="1"/>
-    <row r="546" ht="15.75" customHeight="1"/>
-    <row r="547" ht="15.75" customHeight="1"/>
-    <row r="548" ht="15.75" customHeight="1"/>
-    <row r="549" ht="15.75" customHeight="1"/>
-    <row r="550" ht="15.75" customHeight="1"/>
-    <row r="551" ht="15.75" customHeight="1"/>
-    <row r="552" ht="15.75" customHeight="1"/>
-    <row r="553" ht="15.75" customHeight="1"/>
-    <row r="554" ht="15.75" customHeight="1"/>
-    <row r="555" ht="15.75" customHeight="1"/>
-    <row r="556" ht="15.75" customHeight="1"/>
-    <row r="557" ht="15.75" customHeight="1"/>
-    <row r="558" ht="15.75" customHeight="1"/>
-    <row r="559" ht="15.75" customHeight="1"/>
-    <row r="560" ht="15.75" customHeight="1"/>
-    <row r="561" ht="15.75" customHeight="1"/>
-    <row r="562" ht="15.75" customHeight="1"/>
-    <row r="563" ht="15.75" customHeight="1"/>
-    <row r="564" ht="15.75" customHeight="1"/>
-    <row r="565" ht="15.75" customHeight="1"/>
-    <row r="566" ht="15.75" customHeight="1"/>
-    <row r="567" ht="15.75" customHeight="1"/>
-    <row r="568" ht="15.75" customHeight="1"/>
-    <row r="569" ht="15.75" customHeight="1"/>
-    <row r="570" ht="15.75" customHeight="1"/>
-    <row r="571" ht="15.75" customHeight="1"/>
-    <row r="572" ht="15.75" customHeight="1"/>
-    <row r="573" ht="15.75" customHeight="1"/>
-    <row r="574" ht="15.75" customHeight="1"/>
-    <row r="575" ht="15.75" customHeight="1"/>
-    <row r="576" ht="15.75" customHeight="1"/>
-    <row r="577" ht="15.75" customHeight="1"/>
-    <row r="578" ht="15.75" customHeight="1"/>
-    <row r="579" ht="15.75" customHeight="1"/>
-    <row r="580" ht="15.75" customHeight="1"/>
-    <row r="581" ht="15.75" customHeight="1"/>
-    <row r="582" ht="15.75" customHeight="1"/>
-    <row r="583" ht="15.75" customHeight="1"/>
-    <row r="584" ht="15.75" customHeight="1"/>
-    <row r="585" ht="15.75" customHeight="1"/>
-    <row r="586" ht="15.75" customHeight="1"/>
-    <row r="587" ht="15.75" customHeight="1"/>
-    <row r="588" ht="15.75" customHeight="1"/>
-    <row r="589" ht="15.75" customHeight="1"/>
-    <row r="590" ht="15.75" customHeight="1"/>
-    <row r="591" ht="15.75" customHeight="1"/>
-    <row r="592" ht="15.75" customHeight="1"/>
-    <row r="593" ht="15.75" customHeight="1"/>
-    <row r="594" ht="15.75" customHeight="1"/>
-    <row r="595" ht="15.75" customHeight="1"/>
-    <row r="596" ht="15.75" customHeight="1"/>
-    <row r="597" ht="15.75" customHeight="1"/>
-    <row r="598" ht="15.75" customHeight="1"/>
-    <row r="599" ht="15.75" customHeight="1"/>
-    <row r="600" ht="15.75" customHeight="1"/>
-    <row r="601" ht="15.75" customHeight="1"/>
-    <row r="602" ht="15.75" customHeight="1"/>
-    <row r="603" ht="15.75" customHeight="1"/>
-    <row r="604" ht="15.75" customHeight="1"/>
-    <row r="605" ht="15.75" customHeight="1"/>
-    <row r="606" ht="15.75" customHeight="1"/>
-    <row r="607" ht="15.75" customHeight="1"/>
-    <row r="608" ht="15.75" customHeight="1"/>
-    <row r="609" ht="15.75" customHeight="1"/>
-    <row r="610" ht="15.75" customHeight="1"/>
-    <row r="611" ht="15.75" customHeight="1"/>
-    <row r="612" ht="15.75" customHeight="1"/>
-    <row r="613" ht="15.75" customHeight="1"/>
-    <row r="614" ht="15.75" customHeight="1"/>
-    <row r="615" ht="15.75" customHeight="1"/>
-    <row r="616" ht="15.75" customHeight="1"/>
-    <row r="617" ht="15.75" customHeight="1"/>
-    <row r="618" ht="15.75" customHeight="1"/>
-    <row r="619" ht="15.75" customHeight="1"/>
-    <row r="620" ht="15.75" customHeight="1"/>
-    <row r="621" ht="15.75" customHeight="1"/>
-    <row r="622" ht="15.75" customHeight="1"/>
-    <row r="623" ht="15.75" customHeight="1"/>
-    <row r="624" ht="15.75" customHeight="1"/>
-    <row r="625" ht="15.75" customHeight="1"/>
-    <row r="626" ht="15.75" customHeight="1"/>
-    <row r="627" ht="15.75" customHeight="1"/>
-    <row r="628" ht="15.75" customHeight="1"/>
-    <row r="629" ht="15.75" customHeight="1"/>
-    <row r="630" ht="15.75" customHeight="1"/>
-    <row r="631" ht="15.75" customHeight="1"/>
-    <row r="632" ht="15.75" customHeight="1"/>
-    <row r="633" ht="15.75" customHeight="1"/>
-    <row r="634" ht="15.75" customHeight="1"/>
-    <row r="635" ht="15.75" customHeight="1"/>
-    <row r="636" ht="15.75" customHeight="1"/>
-    <row r="637" ht="15.75" customHeight="1"/>
-    <row r="638" ht="15.75" customHeight="1"/>
-    <row r="639" ht="15.75" customHeight="1"/>
-    <row r="640" ht="15.75" customHeight="1"/>
-    <row r="641" ht="15.75" customHeight="1"/>
-    <row r="642" ht="15.75" customHeight="1"/>
-    <row r="643" ht="15.75" customHeight="1"/>
-    <row r="644" ht="15.75" customHeight="1"/>
-    <row r="645" ht="15.75" customHeight="1"/>
-    <row r="646" ht="15.75" customHeight="1"/>
-    <row r="647" ht="15.75" customHeight="1"/>
-    <row r="648" ht="15.75" customHeight="1"/>
-    <row r="649" ht="15.75" customHeight="1"/>
-    <row r="650" ht="15.75" customHeight="1"/>
-    <row r="651" ht="15.75" customHeight="1"/>
-    <row r="652" ht="15.75" customHeight="1"/>
-    <row r="653" ht="15.75" customHeight="1"/>
-    <row r="654" ht="15.75" customHeight="1"/>
-    <row r="655" ht="15.75" customHeight="1"/>
-    <row r="656" ht="15.75" customHeight="1"/>
-    <row r="657" ht="15.75" customHeight="1"/>
-    <row r="658" ht="15.75" customHeight="1"/>
-    <row r="659" ht="15.75" customHeight="1"/>
-    <row r="660" ht="15.75" customHeight="1"/>
-    <row r="661" ht="15.75" customHeight="1"/>
-    <row r="662" ht="15.75" customHeight="1"/>
-    <row r="663" ht="15.75" customHeight="1"/>
-    <row r="664" ht="15.75" customHeight="1"/>
-    <row r="665" ht="15.75" customHeight="1"/>
-    <row r="666" ht="15.75" customHeight="1"/>
-    <row r="667" ht="15.75" customHeight="1"/>
-    <row r="668" ht="15.75" customHeight="1"/>
-    <row r="669" ht="15.75" customHeight="1"/>
-    <row r="670" ht="15.75" customHeight="1"/>
-    <row r="671" ht="15.75" customHeight="1"/>
-    <row r="672" ht="15.75" customHeight="1"/>
-    <row r="673" ht="15.75" customHeight="1"/>
-    <row r="674" ht="15.75" customHeight="1"/>
-    <row r="675" ht="15.75" customHeight="1"/>
-    <row r="676" ht="15.75" customHeight="1"/>
-    <row r="677" ht="15.75" customHeight="1"/>
-    <row r="678" ht="15.75" customHeight="1"/>
-    <row r="679" ht="15.75" customHeight="1"/>
-    <row r="680" ht="15.75" customHeight="1"/>
-    <row r="681" ht="15.75" customHeight="1"/>
-    <row r="682" ht="15.75" customHeight="1"/>
-    <row r="683" ht="15.75" customHeight="1"/>
-    <row r="684" ht="15.75" customHeight="1"/>
-    <row r="685" ht="15.75" customHeight="1"/>
-    <row r="686" ht="15.75" customHeight="1"/>
-    <row r="687" ht="15.75" customHeight="1"/>
-    <row r="688" ht="15.75" customHeight="1"/>
-    <row r="689" ht="15.75" customHeight="1"/>
-    <row r="690" ht="15.75" customHeight="1"/>
-    <row r="691" ht="15.75" customHeight="1"/>
-    <row r="692" ht="15.75" customHeight="1"/>
-    <row r="693" ht="15.75" customHeight="1"/>
-    <row r="694" ht="15.75" customHeight="1"/>
-    <row r="695" ht="15.75" customHeight="1"/>
-    <row r="696" ht="15.75" customHeight="1"/>
-    <row r="697" ht="15.75" customHeight="1"/>
-    <row r="698" ht="15.75" customHeight="1"/>
-    <row r="699" ht="15.75" customHeight="1"/>
-    <row r="700" ht="15.75" customHeight="1"/>
-    <row r="701" ht="15.75" customHeight="1"/>
-    <row r="702" ht="15.75" customHeight="1"/>
-    <row r="703" ht="15.75" customHeight="1"/>
-    <row r="704" ht="15.75" customHeight="1"/>
-    <row r="705" ht="15.75" customHeight="1"/>
-    <row r="706" ht="15.75" customHeight="1"/>
-    <row r="707" ht="15.75" customHeight="1"/>
-    <row r="708" ht="15.75" customHeight="1"/>
-    <row r="709" ht="15.75" customHeight="1"/>
-    <row r="710" ht="15.75" customHeight="1"/>
-    <row r="711" ht="15.75" customHeight="1"/>
-    <row r="712" ht="15.75" customHeight="1"/>
-    <row r="713" ht="15.75" customHeight="1"/>
-    <row r="714" ht="15.75" customHeight="1"/>
-    <row r="715" ht="15.75" customHeight="1"/>
-    <row r="716" ht="15.75" customHeight="1"/>
-    <row r="717" ht="15.75" customHeight="1"/>
-    <row r="718" ht="15.75" customHeight="1"/>
-    <row r="719" ht="15.75" customHeight="1"/>
-    <row r="720" ht="15.75" customHeight="1"/>
-    <row r="721" ht="15.75" customHeight="1"/>
-    <row r="722" ht="15.75" customHeight="1"/>
-    <row r="723" ht="15.75" customHeight="1"/>
-    <row r="724" ht="15.75" customHeight="1"/>
-    <row r="725" ht="15.75" customHeight="1"/>
-    <row r="726" ht="15.75" customHeight="1"/>
-    <row r="727" ht="15.75" customHeight="1"/>
-    <row r="728" ht="15.75" customHeight="1"/>
-    <row r="729" ht="15.75" customHeight="1"/>
-    <row r="730" ht="15.75" customHeight="1"/>
-    <row r="731" ht="15.75" customHeight="1"/>
-    <row r="732" ht="15.75" customHeight="1"/>
-    <row r="733" ht="15.75" customHeight="1"/>
-    <row r="734" ht="15.75" customHeight="1"/>
-    <row r="735" ht="15.75" customHeight="1"/>
-    <row r="736" ht="15.75" customHeight="1"/>
-    <row r="737" ht="15.75" customHeight="1"/>
-    <row r="738" ht="15.75" customHeight="1"/>
-    <row r="739" ht="15.75" customHeight="1"/>
-    <row r="740" ht="15.75" customHeight="1"/>
-    <row r="741" ht="15.75" customHeight="1"/>
-    <row r="742" ht="15.75" customHeight="1"/>
-    <row r="743" ht="15.75" customHeight="1"/>
-    <row r="744" ht="15.75" customHeight="1"/>
-    <row r="745" ht="15.75" customHeight="1"/>
-    <row r="746" ht="15.75" customHeight="1"/>
-    <row r="747" ht="15.75" customHeight="1"/>
-    <row r="748" ht="15.75" customHeight="1"/>
-    <row r="749" ht="15.75" customHeight="1"/>
-    <row r="750" ht="15.75" customHeight="1"/>
-    <row r="751" ht="15.75" customHeight="1"/>
-    <row r="752" ht="15.75" customHeight="1"/>
-    <row r="753" ht="15.75" customHeight="1"/>
-    <row r="754" ht="15.75" customHeight="1"/>
-    <row r="755" ht="15.75" customHeight="1"/>
-    <row r="756" ht="15.75" customHeight="1"/>
-    <row r="757" ht="15.75" customHeight="1"/>
-    <row r="758" ht="15.75" customHeight="1"/>
-    <row r="759" ht="15.75" customHeight="1"/>
-    <row r="760" ht="15.75" customHeight="1"/>
-    <row r="761" ht="15.75" customHeight="1"/>
-    <row r="762" ht="15.75" customHeight="1"/>
-    <row r="763" ht="15.75" customHeight="1"/>
-    <row r="764" ht="15.75" customHeight="1"/>
-    <row r="765" ht="15.75" customHeight="1"/>
-    <row r="766" ht="15.75" customHeight="1"/>
-    <row r="767" ht="15.75" customHeight="1"/>
-    <row r="768" ht="15.75" customHeight="1"/>
-    <row r="769" ht="15.75" customHeight="1"/>
-    <row r="770" ht="15.75" customHeight="1"/>
-    <row r="771" ht="15.75" customHeight="1"/>
-    <row r="772" ht="15.75" customHeight="1"/>
-    <row r="773" ht="15.75" customHeight="1"/>
-    <row r="774" ht="15.75" customHeight="1"/>
-    <row r="775" ht="15.75" customHeight="1"/>
-    <row r="776" ht="15.75" customHeight="1"/>
-    <row r="777" ht="15.75" customHeight="1"/>
-    <row r="778" ht="15.75" customHeight="1"/>
-    <row r="779" ht="15.75" customHeight="1"/>
-    <row r="780" ht="15.75" customHeight="1"/>
-    <row r="781" ht="15.75" customHeight="1"/>
-    <row r="782" ht="15.75" customHeight="1"/>
-    <row r="783" ht="15.75" customHeight="1"/>
-    <row r="784" ht="15.75" customHeight="1"/>
-    <row r="785" ht="15.75" customHeight="1"/>
-    <row r="786" ht="15.75" customHeight="1"/>
-    <row r="787" ht="15.75" customHeight="1"/>
-    <row r="788" ht="15.75" customHeight="1"/>
-    <row r="789" ht="15.75" customHeight="1"/>
-    <row r="790" ht="15.75" customHeight="1"/>
-    <row r="791" ht="15.75" customHeight="1"/>
-    <row r="792" ht="15.75" customHeight="1"/>
-    <row r="793" ht="15.75" customHeight="1"/>
-    <row r="794" ht="15.75" customHeight="1"/>
-    <row r="795" ht="15.75" customHeight="1"/>
-    <row r="796" ht="15.75" customHeight="1"/>
-    <row r="797" ht="15.75" customHeight="1"/>
-    <row r="798" ht="15.75" customHeight="1"/>
-    <row r="799" ht="15.75" customHeight="1"/>
-    <row r="800" ht="15.75" customHeight="1"/>
-    <row r="801" ht="15.75" customHeight="1"/>
-    <row r="802" ht="15.75" customHeight="1"/>
-    <row r="803" ht="15.75" customHeight="1"/>
-    <row r="804" ht="15.75" customHeight="1"/>
-    <row r="805" ht="15.75" customHeight="1"/>
-    <row r="806" ht="15.75" customHeight="1"/>
-    <row r="807" ht="15.75" customHeight="1"/>
-    <row r="808" ht="15.75" customHeight="1"/>
-    <row r="809" ht="15.75" customHeight="1"/>
-    <row r="810" ht="15.75" customHeight="1"/>
-    <row r="811" ht="15.75" customHeight="1"/>
-    <row r="812" ht="15.75" customHeight="1"/>
-    <row r="813" ht="15.75" customHeight="1"/>
-    <row r="814" ht="15.75" customHeight="1"/>
-    <row r="815" ht="15.75" customHeight="1"/>
-    <row r="816" ht="15.75" customHeight="1"/>
-    <row r="817" ht="15.75" customHeight="1"/>
-    <row r="818" ht="15.75" customHeight="1"/>
-    <row r="819" ht="15.75" customHeight="1"/>
-    <row r="820" ht="15.75" customHeight="1"/>
-    <row r="821" ht="15.75" customHeight="1"/>
-    <row r="822" ht="15.75" customHeight="1"/>
-    <row r="823" ht="15.75" customHeight="1"/>
-    <row r="824" ht="15.75" customHeight="1"/>
-    <row r="825" ht="15.75" customHeight="1"/>
-    <row r="826" ht="15.75" customHeight="1"/>
-    <row r="827" ht="15.75" customHeight="1"/>
-    <row r="828" ht="15.75" customHeight="1"/>
-    <row r="829" ht="15.75" customHeight="1"/>
-    <row r="830" ht="15.75" customHeight="1"/>
-    <row r="831" ht="15.75" customHeight="1"/>
-    <row r="832" ht="15.75" customHeight="1"/>
-    <row r="833" ht="15.75" customHeight="1"/>
-    <row r="834" ht="15.75" customHeight="1"/>
-    <row r="835" ht="15.75" customHeight="1"/>
-    <row r="836" ht="15.75" customHeight="1"/>
-    <row r="837" ht="15.75" customHeight="1"/>
-    <row r="838" ht="15.75" customHeight="1"/>
-    <row r="839" ht="15.75" customHeight="1"/>
-    <row r="840" ht="15.75" customHeight="1"/>
-    <row r="841" ht="15.75" customHeight="1"/>
-    <row r="842" ht="15.75" customHeight="1"/>
-    <row r="843" ht="15.75" customHeight="1"/>
-    <row r="844" ht="15.75" customHeight="1"/>
-    <row r="845" ht="15.75" customHeight="1"/>
-    <row r="846" ht="15.75" customHeight="1"/>
-    <row r="847" ht="15.75" customHeight="1"/>
-    <row r="848" ht="15.75" customHeight="1"/>
-    <row r="849" ht="15.75" customHeight="1"/>
-    <row r="850" ht="15.75" customHeight="1"/>
-    <row r="851" ht="15.75" customHeight="1"/>
-    <row r="852" ht="15.75" customHeight="1"/>
-    <row r="853" ht="15.75" customHeight="1"/>
-    <row r="854" ht="15.75" customHeight="1"/>
-    <row r="855" ht="15.75" customHeight="1"/>
-    <row r="856" ht="15.75" customHeight="1"/>
-    <row r="857" ht="15.75" customHeight="1"/>
-    <row r="858" ht="15.75" customHeight="1"/>
-    <row r="859" ht="15.75" customHeight="1"/>
-    <row r="860" ht="15.75" customHeight="1"/>
-    <row r="861" ht="15.75" customHeight="1"/>
-    <row r="862" ht="15.75" customHeight="1"/>
-    <row r="863" ht="15.75" customHeight="1"/>
-    <row r="864" ht="15.75" customHeight="1"/>
-    <row r="865" ht="15.75" customHeight="1"/>
-    <row r="866" ht="15.75" customHeight="1"/>
-    <row r="867" ht="15.75" customHeight="1"/>
-    <row r="868" ht="15.75" customHeight="1"/>
-    <row r="869" ht="15.75" customHeight="1"/>
-    <row r="870" ht="15.75" customHeight="1"/>
-    <row r="871" ht="15.75" customHeight="1"/>
-    <row r="872" ht="15.75" customHeight="1"/>
-    <row r="873" ht="15.75" customHeight="1"/>
-    <row r="874" ht="15.75" customHeight="1"/>
-    <row r="875" ht="15.75" customHeight="1"/>
-    <row r="876" ht="15.75" customHeight="1"/>
-    <row r="877" ht="15.75" customHeight="1"/>
-    <row r="878" ht="15.75" customHeight="1"/>
-    <row r="879" ht="15.75" customHeight="1"/>
-    <row r="880" ht="15.75" customHeight="1"/>
-    <row r="881" ht="15.75" customHeight="1"/>
-    <row r="882" ht="15.75" customHeight="1"/>
-    <row r="883" ht="15.75" customHeight="1"/>
-    <row r="884" ht="15.75" customHeight="1"/>
-    <row r="885" ht="15.75" customHeight="1"/>
-    <row r="886" ht="15.75" customHeight="1"/>
-    <row r="887" ht="15.75" customHeight="1"/>
-    <row r="888" ht="15.75" customHeight="1"/>
-    <row r="889" ht="15.75" customHeight="1"/>
-    <row r="890" ht="15.75" customHeight="1"/>
-    <row r="891" ht="15.75" customHeight="1"/>
-    <row r="892" ht="15.75" customHeight="1"/>
-    <row r="893" ht="15.75" customHeight="1"/>
-    <row r="894" ht="15.75" customHeight="1"/>
-    <row r="895" ht="15.75" customHeight="1"/>
-    <row r="896" ht="15.75" customHeight="1"/>
-    <row r="897" ht="15.75" customHeight="1"/>
-    <row r="898" ht="15.75" customHeight="1"/>
-    <row r="899" ht="15.75" customHeight="1"/>
-    <row r="900" ht="15.75" customHeight="1"/>
-    <row r="901" ht="15.75" customHeight="1"/>
-    <row r="902" ht="15.75" customHeight="1"/>
-    <row r="903" ht="15.75" customHeight="1"/>
-    <row r="904" ht="15.75" customHeight="1"/>
-    <row r="905" ht="15.75" customHeight="1"/>
-    <row r="906" ht="15.75" customHeight="1"/>
-    <row r="907" ht="15.75" customHeight="1"/>
-    <row r="908" ht="15.75" customHeight="1"/>
-    <row r="909" ht="15.75" customHeight="1"/>
-    <row r="910" ht="15.75" customHeight="1"/>
-    <row r="911" ht="15.75" customHeight="1"/>
-    <row r="912" ht="15.75" customHeight="1"/>
-    <row r="913" ht="15.75" customHeight="1"/>
-    <row r="914" ht="15.75" customHeight="1"/>
-    <row r="915" ht="15.75" customHeight="1"/>
-    <row r="916" ht="15.75" customHeight="1"/>
-    <row r="917" ht="15.75" customHeight="1"/>
-    <row r="918" ht="15.75" customHeight="1"/>
-    <row r="919" ht="15.75" customHeight="1"/>
-    <row r="920" ht="15.75" customHeight="1"/>
-    <row r="921" ht="15.75" customHeight="1"/>
-    <row r="922" ht="15.75" customHeight="1"/>
-    <row r="923" ht="15.75" customHeight="1"/>
-    <row r="924" ht="15.75" customHeight="1"/>
-    <row r="925" ht="15.75" customHeight="1"/>
-    <row r="926" ht="15.75" customHeight="1"/>
-    <row r="927" ht="15.75" customHeight="1"/>
-    <row r="928" ht="15.75" customHeight="1"/>
-    <row r="929" ht="15.75" customHeight="1"/>
-    <row r="930" ht="15.75" customHeight="1"/>
-    <row r="931" ht="15.75" customHeight="1"/>
-    <row r="932" ht="15.75" customHeight="1"/>
-    <row r="933" ht="15.75" customHeight="1"/>
-    <row r="934" ht="15.75" customHeight="1"/>
-    <row r="935" ht="15.75" customHeight="1"/>
-    <row r="936" ht="15.75" customHeight="1"/>
-    <row r="937" ht="15.75" customHeight="1"/>
-    <row r="938" ht="15.75" customHeight="1"/>
-    <row r="939" ht="15.75" customHeight="1"/>
-    <row r="940" ht="15.75" customHeight="1"/>
-    <row r="941" ht="15.75" customHeight="1"/>
-    <row r="942" ht="15.75" customHeight="1"/>
-    <row r="943" ht="15.75" customHeight="1"/>
-    <row r="944" ht="15.75" customHeight="1"/>
-    <row r="945" ht="15.75" customHeight="1"/>
-    <row r="946" ht="15.75" customHeight="1"/>
-    <row r="947" ht="15.75" customHeight="1"/>
-    <row r="948" ht="15.75" customHeight="1"/>
-    <row r="949" ht="15.75" customHeight="1"/>
-    <row r="950" ht="15.75" customHeight="1"/>
-    <row r="951" ht="15.75" customHeight="1"/>
-    <row r="952" ht="15.75" customHeight="1"/>
-    <row r="953" ht="15.75" customHeight="1"/>
-    <row r="954" ht="15.75" customHeight="1"/>
-    <row r="955" ht="15.75" customHeight="1"/>
-    <row r="956" ht="15.75" customHeight="1"/>
-    <row r="957" ht="15.75" customHeight="1"/>
-    <row r="958" ht="15.75" customHeight="1"/>
-    <row r="959" ht="15.75" customHeight="1"/>
-    <row r="960" ht="15.75" customHeight="1"/>
-    <row r="961" ht="15.75" customHeight="1"/>
-    <row r="962" ht="15.75" customHeight="1"/>
-    <row r="963" ht="15.75" customHeight="1"/>
-    <row r="964" ht="15.75" customHeight="1"/>
-    <row r="965" ht="15.75" customHeight="1"/>
-    <row r="966" ht="15.75" customHeight="1"/>
-    <row r="967" ht="15.75" customHeight="1"/>
-    <row r="968" ht="15.75" customHeight="1"/>
-    <row r="969" ht="15.75" customHeight="1"/>
-    <row r="970" ht="15.75" customHeight="1"/>
-    <row r="971" ht="15.75" customHeight="1"/>
-    <row r="972" ht="15.75" customHeight="1"/>
-    <row r="973" ht="15.75" customHeight="1"/>
-    <row r="974" ht="15.75" customHeight="1"/>
-    <row r="975" ht="15.75" customHeight="1"/>
-    <row r="976" ht="15.75" customHeight="1"/>
-    <row r="977" ht="15.75" customHeight="1"/>
-    <row r="978" ht="15.75" customHeight="1"/>
-    <row r="979" ht="15.75" customHeight="1"/>
-    <row r="980" ht="15.75" customHeight="1"/>
-    <row r="981" ht="15.75" customHeight="1"/>
-    <row r="982" ht="15.75" customHeight="1"/>
-    <row r="983" ht="15.75" customHeight="1"/>
-    <row r="984" ht="15.75" customHeight="1"/>
-    <row r="985" ht="15.75" customHeight="1"/>
-    <row r="986" ht="15.75" customHeight="1"/>
-    <row r="987" ht="15.75" customHeight="1"/>
-    <row r="988" ht="15.75" customHeight="1"/>
-    <row r="989" ht="15.75" customHeight="1"/>
-    <row r="990" ht="15.75" customHeight="1"/>
-    <row r="991" ht="15.75" customHeight="1"/>
-    <row r="992" ht="15.75" customHeight="1"/>
-    <row r="993" ht="15.75" customHeight="1"/>
-    <row r="994" ht="15.75" customHeight="1"/>
-    <row r="995" ht="15.75" customHeight="1"/>
-    <row r="996" ht="15.75" customHeight="1"/>
-    <row r="997" ht="15.75" customHeight="1"/>
-    <row r="998" ht="15.75" customHeight="1"/>
-    <row r="999" ht="15.75" customHeight="1"/>
-    <row r="1000" ht="15.75" customHeight="1"/>
+    <row r="261" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="262" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="263" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="264" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="265" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="266" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="267" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="268" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="269" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="270" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="271" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="272" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="273" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="274" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="275" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="276" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="277" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="278" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="279" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="280" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="281" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="282" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="283" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="284" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="285" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="286" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="287" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="288" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="289" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="290" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="291" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="292" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="293" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="294" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="295" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="296" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="297" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="298" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="299" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="300" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="301" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="302" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="303" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="304" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="305" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="306" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="307" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="308" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="309" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="310" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="311" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="312" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="313" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="314" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="315" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="316" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="317" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="318" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="319" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="320" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="321" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="322" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="323" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="324" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="325" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="326" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="327" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="328" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="329" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="330" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="331" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="332" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="333" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="334" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="335" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="336" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="337" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="338" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="339" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="340" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="341" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="342" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="343" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="344" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="345" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="346" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="347" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="348" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="349" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="350" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="351" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="352" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="353" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="354" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="355" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="356" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="357" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="358" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="359" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="360" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="361" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="362" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="363" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="364" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="365" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="366" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="367" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="368" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="369" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="370" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="371" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="372" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="373" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="374" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="375" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="376" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="377" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="378" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="379" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="380" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="381" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="382" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="383" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="384" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="385" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="386" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="387" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="388" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="389" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="390" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="391" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="392" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="393" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="394" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="395" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="396" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="397" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="398" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="399" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="400" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="401" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="402" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="403" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="404" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="405" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="406" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="407" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="408" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="409" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="410" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="411" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="412" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="413" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="414" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="415" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="416" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="417" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="418" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="419" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="420" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="421" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="422" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="423" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="424" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="425" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="426" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="427" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="428" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="429" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="430" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="431" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="432" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="433" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="434" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="435" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="436" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="437" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="438" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="439" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="440" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="441" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="442" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="443" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="444" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="445" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="446" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="447" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="448" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="449" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="450" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="451" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="452" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="453" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="454" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="455" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="456" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="457" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="458" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="459" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="460" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="461" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="462" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="463" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="464" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="465" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="466" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="467" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="468" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="469" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="470" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="471" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="472" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="473" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="474" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="475" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="476" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="477" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="478" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="479" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="480" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="481" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="482" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="483" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="484" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="485" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="486" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="487" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="488" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="489" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="490" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="491" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="492" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="493" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="494" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="495" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="496" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="497" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="498" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="499" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="500" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="501" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="502" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="503" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="504" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="505" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="506" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="507" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="508" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="509" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="510" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="511" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="512" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="513" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="514" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="515" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="516" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="517" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="518" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="519" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="520" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="521" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="522" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="523" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="524" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="525" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="526" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="527" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="528" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="529" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="530" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="531" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="532" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="533" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="534" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="535" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="536" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="537" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="538" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="539" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="540" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="541" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="542" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="543" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="544" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="545" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="546" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="547" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="548" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="549" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="550" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="551" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="552" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="553" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="554" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="555" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="556" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="557" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="558" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="559" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="560" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="561" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="562" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="563" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="564" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="565" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="566" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="567" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="568" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="569" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="570" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="571" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="572" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="573" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="574" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="575" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="576" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="577" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="578" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="579" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="580" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="581" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="582" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="583" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="584" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="585" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="586" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="587" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="588" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="589" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="590" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="591" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="592" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="593" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="594" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="595" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="596" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="597" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="598" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="599" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="600" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="601" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="602" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="603" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="604" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="605" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="606" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="607" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="608" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="609" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="610" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="611" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="612" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="613" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="614" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="615" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="616" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="617" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="618" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="619" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="620" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="621" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="622" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="623" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="624" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="625" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="626" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="627" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="628" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="629" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="630" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="631" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="632" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="633" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="634" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="635" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="636" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="637" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="638" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="639" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="640" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="641" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="642" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="643" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="644" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="645" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="646" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="647" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="648" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="649" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="650" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="651" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="652" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="653" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="654" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="655" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="656" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="657" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="658" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="659" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="660" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="661" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="662" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="663" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="664" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="665" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="666" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="667" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="668" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="669" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="670" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="671" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="672" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="673" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="674" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="675" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="676" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="677" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="678" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="679" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="680" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="681" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="682" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="683" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="684" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="685" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="686" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="687" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="688" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="689" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="690" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="691" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="692" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="693" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="694" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="695" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="696" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="697" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="698" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="699" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="700" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="701" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="702" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="703" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="704" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="705" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="706" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="707" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="708" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="709" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="710" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="711" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="712" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="713" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="714" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="715" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="716" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="717" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="718" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="719" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="720" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="721" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="722" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="723" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="724" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="725" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="726" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="727" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="728" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="729" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="730" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="731" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="732" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="733" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="734" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="735" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="736" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="737" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="738" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="739" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="740" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="741" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="742" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="743" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="744" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="745" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="746" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="747" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="748" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="749" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="750" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="751" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="752" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="753" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="754" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="755" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="756" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="757" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="758" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="759" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="760" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="761" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="762" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="763" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="764" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="765" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="766" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="767" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="768" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="769" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="770" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="771" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="772" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="773" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="774" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="775" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="776" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="777" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="778" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="779" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="780" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="781" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="782" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="783" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="784" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="785" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="786" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="787" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="788" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="789" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="790" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="791" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="792" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="793" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="794" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="795" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="796" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="797" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="798" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="799" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="800" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="801" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="802" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="803" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="804" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="805" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="806" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="807" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="808" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="809" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="810" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="811" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="812" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="813" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="814" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="815" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="816" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="817" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="818" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="819" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="820" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="821" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="822" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="823" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="824" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="825" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="826" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="827" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="828" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="829" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="830" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="831" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="832" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="833" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="834" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="835" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="836" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="837" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="838" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="839" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="840" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="841" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="842" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="843" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="844" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="845" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="846" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="847" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="848" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="849" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="850" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="851" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="852" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="853" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="854" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="855" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="856" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="857" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="858" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="859" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="860" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="861" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="862" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="863" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="864" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="865" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="866" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="867" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="868" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="869" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="870" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="871" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="872" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="873" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="874" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="875" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="876" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="877" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="878" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="879" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="880" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="881" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="882" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="883" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="884" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="885" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="886" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="887" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="888" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="889" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="890" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="891" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="892" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="893" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="894" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="895" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="896" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="897" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="898" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="899" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="900" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="901" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="902" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="903" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="904" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="905" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="906" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="907" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="908" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="909" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="910" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="911" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="912" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="913" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="914" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="915" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="916" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="917" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="918" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="919" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="920" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="921" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="922" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="923" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="924" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="925" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="926" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="927" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="928" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="929" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="930" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="931" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="932" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="933" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="934" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="935" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="936" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="937" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="938" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="939" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="940" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="941" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="942" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="943" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="944" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="945" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="946" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="947" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="948" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="949" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="950" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="951" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="952" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="953" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="954" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="955" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="956" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="957" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="958" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="959" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="960" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="961" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="962" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="963" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="964" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="965" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="966" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="967" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="968" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="969" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="970" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="971" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="972" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="973" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="974" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="975" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="976" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="977" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="978" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="979" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="980" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="981" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="982" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="983" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="984" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="985" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="986" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="987" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="988" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="989" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="990" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="991" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="992" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="993" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="994" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="995" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="996" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="997" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="998" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="999" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D4" r:id="rId1"/>
-    <hyperlink ref="D5" r:id="rId2"/>
-    <hyperlink ref="D8" r:id="rId3"/>
-    <hyperlink ref="D9" r:id="rId4"/>
-    <hyperlink ref="D10" r:id="rId5"/>
+    <hyperlink ref="D4" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="D5" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="D8" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="D9" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="D10" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="D11" r:id="rId6" xr:uid="{D5E07517-70A2-400E-81E3-BC651813A3D1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
se agrega un alumna Carla
</commit_message>
<xml_diff>
--- a/Lista de Alumnos.xlsx
+++ b/Lista de Alumnos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nano\Documents\Programacion\ISPC\Electronica microcontrolada\git proteus\Alumnos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/529c39ee85bc7ffb/Escritorio/repositorio/electronica/Alumnos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1813A112-83C4-4B0C-A759-2731FD4CBD4F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="14_{CC8F6900-3272-4D67-86DA-2AFE2C612C7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Electronica Microcontrolada" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>#</t>
   </si>
@@ -127,6 +127,15 @@
   </si>
   <si>
     <t>Wleyton89</t>
+  </si>
+  <si>
+    <t>Carla Wayar</t>
+  </si>
+  <si>
+    <t>carlaargentinawayar@gmail.com</t>
+  </si>
+  <si>
+    <t>WayarCarla</t>
   </si>
 </sst>
 </file>
@@ -696,20 +705,20 @@
   <dimension ref="A1:E1000"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.85546875" customWidth="1"/>
-    <col min="2" max="2" width="37.140625" customWidth="1"/>
-    <col min="3" max="3" width="10.5703125" customWidth="1"/>
+    <col min="1" max="1" width="6.88671875" customWidth="1"/>
+    <col min="2" max="2" width="37.109375" customWidth="1"/>
+    <col min="3" max="3" width="10.5546875" customWidth="1"/>
     <col min="4" max="4" width="31" customWidth="1"/>
     <col min="5" max="5" width="29" customWidth="1"/>
-    <col min="6" max="6" width="8.7109375" customWidth="1"/>
+    <col min="6" max="6" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -726,7 +735,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -743,7 +752,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5">
         <v>2</v>
       </c>
@@ -758,7 +767,7 @@
       </c>
       <c r="E3" s="6"/>
     </row>
-    <row r="4" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5">
         <v>3</v>
       </c>
@@ -775,7 +784,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="5">
         <v>4</v>
       </c>
@@ -792,7 +801,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="5">
         <v>5</v>
       </c>
@@ -809,7 +818,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="5">
         <v>6</v>
       </c>
@@ -826,7 +835,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5">
         <v>7</v>
       </c>
@@ -843,7 +852,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="5">
         <v>8</v>
       </c>
@@ -860,7 +869,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="5">
         <v>9</v>
       </c>
@@ -875,7 +884,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="5">
         <v>10</v>
       </c>
@@ -892,16 +901,24 @@
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="5">
         <v>11</v>
       </c>
-      <c r="B12" s="6"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-    </row>
-    <row r="13" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" s="5">
+        <v>1</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="5">
         <v>12</v>
       </c>
@@ -910,7 +927,7 @@
       <c r="D13" s="6"/>
       <c r="E13" s="6"/>
     </row>
-    <row r="14" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="5">
         <v>13</v>
       </c>
@@ -919,7 +936,7 @@
       <c r="D14" s="6"/>
       <c r="E14" s="6"/>
     </row>
-    <row r="15" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="5">
         <v>14</v>
       </c>
@@ -928,7 +945,7 @@
       <c r="D15" s="6"/>
       <c r="E15" s="6"/>
     </row>
-    <row r="16" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="5">
         <v>15</v>
       </c>
@@ -937,7 +954,7 @@
       <c r="D16" s="6"/>
       <c r="E16" s="6"/>
     </row>
-    <row r="17" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="5">
         <v>16</v>
       </c>
@@ -946,7 +963,7 @@
       <c r="D17" s="6"/>
       <c r="E17" s="6"/>
     </row>
-    <row r="18" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="5">
         <v>17</v>
       </c>
@@ -955,7 +972,7 @@
       <c r="D18" s="6"/>
       <c r="E18" s="6"/>
     </row>
-    <row r="19" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="5">
         <v>18</v>
       </c>
@@ -964,7 +981,7 @@
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
     </row>
-    <row r="20" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="5">
         <v>19</v>
       </c>
@@ -973,7 +990,7 @@
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
     </row>
-    <row r="21" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="5">
         <v>20</v>
       </c>
@@ -982,7 +999,7 @@
       <c r="D21" s="6"/>
       <c r="E21" s="6"/>
     </row>
-    <row r="22" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="5">
         <v>21</v>
       </c>
@@ -991,7 +1008,7 @@
       <c r="D22" s="6"/>
       <c r="E22" s="6"/>
     </row>
-    <row r="23" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="5">
         <v>22</v>
       </c>
@@ -1000,7 +1017,7 @@
       <c r="D23" s="6"/>
       <c r="E23" s="6"/>
     </row>
-    <row r="24" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="5">
         <v>23</v>
       </c>
@@ -1009,7 +1026,7 @@
       <c r="D24" s="6"/>
       <c r="E24" s="6"/>
     </row>
-    <row r="25" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="5">
         <v>24</v>
       </c>
@@ -1018,7 +1035,7 @@
       <c r="D25" s="6"/>
       <c r="E25" s="6"/>
     </row>
-    <row r="26" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="5">
         <v>25</v>
       </c>
@@ -1027,7 +1044,7 @@
       <c r="D26" s="6"/>
       <c r="E26" s="6"/>
     </row>
-    <row r="27" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="5">
         <v>26</v>
       </c>
@@ -1036,7 +1053,7 @@
       <c r="D27" s="6"/>
       <c r="E27" s="6"/>
     </row>
-    <row r="28" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="5">
         <v>27</v>
       </c>
@@ -1045,7 +1062,7 @@
       <c r="D28" s="6"/>
       <c r="E28" s="6"/>
     </row>
-    <row r="29" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="5">
         <v>28</v>
       </c>
@@ -1054,7 +1071,7 @@
       <c r="D29" s="6"/>
       <c r="E29" s="6"/>
     </row>
-    <row r="30" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="5">
         <v>29</v>
       </c>
@@ -1063,7 +1080,7 @@
       <c r="D30" s="6"/>
       <c r="E30" s="6"/>
     </row>
-    <row r="31" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="5">
         <v>30</v>
       </c>
@@ -1072,7 +1089,7 @@
       <c r="D31" s="6"/>
       <c r="E31" s="6"/>
     </row>
-    <row r="32" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="5">
         <v>31</v>
       </c>
@@ -1081,7 +1098,7 @@
       <c r="D32" s="6"/>
       <c r="E32" s="6"/>
     </row>
-    <row r="33" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="5">
         <v>32</v>
       </c>
@@ -1090,7 +1107,7 @@
       <c r="D33" s="6"/>
       <c r="E33" s="6"/>
     </row>
-    <row r="34" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="5">
         <v>33</v>
       </c>
@@ -1099,7 +1116,7 @@
       <c r="D34" s="6"/>
       <c r="E34" s="6"/>
     </row>
-    <row r="35" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="5">
         <v>34</v>
       </c>
@@ -1108,7 +1125,7 @@
       <c r="D35" s="6"/>
       <c r="E35" s="6"/>
     </row>
-    <row r="36" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="5">
         <v>35</v>
       </c>
@@ -1117,7 +1134,7 @@
       <c r="D36" s="6"/>
       <c r="E36" s="6"/>
     </row>
-    <row r="37" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="5">
         <v>36</v>
       </c>
@@ -1126,7 +1143,7 @@
       <c r="D37" s="6"/>
       <c r="E37" s="6"/>
     </row>
-    <row r="38" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="5">
         <v>37</v>
       </c>
@@ -1135,7 +1152,7 @@
       <c r="D38" s="6"/>
       <c r="E38" s="6"/>
     </row>
-    <row r="39" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="5">
         <v>38</v>
       </c>
@@ -1144,7 +1161,7 @@
       <c r="D39" s="6"/>
       <c r="E39" s="6"/>
     </row>
-    <row r="40" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="5">
         <v>39</v>
       </c>
@@ -1153,7 +1170,7 @@
       <c r="D40" s="6"/>
       <c r="E40" s="6"/>
     </row>
-    <row r="41" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="5">
         <v>40</v>
       </c>
@@ -1162,7 +1179,7 @@
       <c r="D41" s="6"/>
       <c r="E41" s="6"/>
     </row>
-    <row r="42" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="5">
         <v>41</v>
       </c>
@@ -1171,7 +1188,7 @@
       <c r="D42" s="6"/>
       <c r="E42" s="6"/>
     </row>
-    <row r="43" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="5">
         <v>42</v>
       </c>
@@ -1180,7 +1197,7 @@
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
     </row>
-    <row r="44" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="5">
         <v>43</v>
       </c>
@@ -1189,7 +1206,7 @@
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
     </row>
-    <row r="45" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="5">
         <v>44</v>
       </c>
@@ -1198,7 +1215,7 @@
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
     </row>
-    <row r="46" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="5">
         <v>45</v>
       </c>
@@ -1207,7 +1224,7 @@
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
     </row>
-    <row r="47" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="5">
         <v>46</v>
       </c>
@@ -1216,7 +1233,7 @@
       <c r="D47" s="6"/>
       <c r="E47" s="6"/>
     </row>
-    <row r="48" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="5">
         <v>47</v>
       </c>
@@ -1225,7 +1242,7 @@
       <c r="D48" s="6"/>
       <c r="E48" s="6"/>
     </row>
-    <row r="49" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="5">
         <v>48</v>
       </c>
@@ -1234,7 +1251,7 @@
       <c r="D49" s="6"/>
       <c r="E49" s="6"/>
     </row>
-    <row r="50" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="5">
         <v>49</v>
       </c>
@@ -1243,7 +1260,7 @@
       <c r="D50" s="6"/>
       <c r="E50" s="6"/>
     </row>
-    <row r="51" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="5">
         <v>50</v>
       </c>
@@ -1252,7 +1269,7 @@
       <c r="D51" s="6"/>
       <c r="E51" s="6"/>
     </row>
-    <row r="52" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="5">
         <v>51</v>
       </c>
@@ -1261,7 +1278,7 @@
       <c r="D52" s="6"/>
       <c r="E52" s="6"/>
     </row>
-    <row r="53" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="5">
         <v>52</v>
       </c>
@@ -1270,7 +1287,7 @@
       <c r="D53" s="6"/>
       <c r="E53" s="6"/>
     </row>
-    <row r="54" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="5">
         <v>53</v>
       </c>
@@ -1279,7 +1296,7 @@
       <c r="D54" s="6"/>
       <c r="E54" s="6"/>
     </row>
-    <row r="55" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="5">
         <v>54</v>
       </c>
@@ -1288,7 +1305,7 @@
       <c r="D55" s="6"/>
       <c r="E55" s="6"/>
     </row>
-    <row r="56" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="5">
         <v>55</v>
       </c>
@@ -1297,7 +1314,7 @@
       <c r="D56" s="6"/>
       <c r="E56" s="6"/>
     </row>
-    <row r="57" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="5">
         <v>56</v>
       </c>
@@ -1306,7 +1323,7 @@
       <c r="D57" s="6"/>
       <c r="E57" s="6"/>
     </row>
-    <row r="58" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="5">
         <v>57</v>
       </c>
@@ -1315,7 +1332,7 @@
       <c r="D58" s="6"/>
       <c r="E58" s="6"/>
     </row>
-    <row r="59" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="5">
         <v>58</v>
       </c>
@@ -1324,7 +1341,7 @@
       <c r="D59" s="6"/>
       <c r="E59" s="6"/>
     </row>
-    <row r="60" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" s="5">
         <v>59</v>
       </c>
@@ -1333,2146 +1350,2146 @@
       <c r="D60" s="6"/>
       <c r="E60" s="6"/>
     </row>
-    <row r="61" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" s="11"/>
       <c r="B61" s="12"/>
       <c r="C61" s="11"/>
       <c r="D61" s="12"/>
       <c r="E61" s="12"/>
     </row>
-    <row r="62" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" s="11"/>
       <c r="B62" s="12"/>
       <c r="C62" s="11"/>
       <c r="D62" s="12"/>
       <c r="E62" s="12"/>
     </row>
-    <row r="63" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" s="11"/>
       <c r="B63" s="12"/>
       <c r="C63" s="11"/>
       <c r="D63" s="12"/>
       <c r="E63" s="12"/>
     </row>
-    <row r="64" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" s="11"/>
       <c r="B64" s="12"/>
       <c r="C64" s="11"/>
       <c r="D64" s="12"/>
       <c r="E64" s="12"/>
     </row>
-    <row r="65" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A65" s="11"/>
       <c r="B65" s="12"/>
       <c r="C65" s="11"/>
       <c r="D65" s="12"/>
       <c r="E65" s="12"/>
     </row>
-    <row r="66" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A66" s="11"/>
       <c r="B66" s="12"/>
       <c r="C66" s="11"/>
       <c r="D66" s="12"/>
       <c r="E66" s="12"/>
     </row>
-    <row r="67" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67" s="11"/>
       <c r="B67" s="12"/>
       <c r="C67" s="11"/>
       <c r="D67" s="12"/>
       <c r="E67" s="12"/>
     </row>
-    <row r="68" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" s="11"/>
       <c r="B68" s="12"/>
       <c r="C68" s="11"/>
       <c r="D68" s="12"/>
       <c r="E68" s="12"/>
     </row>
-    <row r="69" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69" s="11"/>
       <c r="B69" s="12"/>
       <c r="C69" s="11"/>
       <c r="D69" s="12"/>
       <c r="E69" s="12"/>
     </row>
-    <row r="70" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A70" s="11"/>
       <c r="B70" s="12"/>
       <c r="C70" s="11"/>
       <c r="D70" s="12"/>
       <c r="E70" s="12"/>
     </row>
-    <row r="71" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A71" s="11"/>
       <c r="B71" s="12"/>
       <c r="C71" s="11"/>
       <c r="D71" s="12"/>
       <c r="E71" s="12"/>
     </row>
-    <row r="72" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72" s="11"/>
       <c r="B72" s="12"/>
       <c r="C72" s="11"/>
       <c r="D72" s="12"/>
       <c r="E72" s="12"/>
     </row>
-    <row r="73" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A73" s="11"/>
       <c r="B73" s="12"/>
       <c r="C73" s="11"/>
       <c r="D73" s="12"/>
       <c r="E73" s="12"/>
     </row>
-    <row r="74" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A74" s="11"/>
       <c r="B74" s="12"/>
       <c r="C74" s="11"/>
       <c r="D74" s="12"/>
       <c r="E74" s="12"/>
     </row>
-    <row r="75" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A75" s="11"/>
       <c r="B75" s="12"/>
       <c r="C75" s="11"/>
       <c r="D75" s="12"/>
       <c r="E75" s="12"/>
     </row>
-    <row r="76" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A76" s="11"/>
       <c r="B76" s="12"/>
       <c r="C76" s="11"/>
       <c r="D76" s="12"/>
       <c r="E76" s="12"/>
     </row>
-    <row r="77" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A77" s="11"/>
       <c r="B77" s="12"/>
       <c r="C77" s="11"/>
       <c r="D77" s="12"/>
       <c r="E77" s="12"/>
     </row>
-    <row r="78" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A78" s="11"/>
       <c r="B78" s="12"/>
       <c r="C78" s="11"/>
       <c r="D78" s="12"/>
       <c r="E78" s="12"/>
     </row>
-    <row r="79" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A79" s="11"/>
       <c r="B79" s="12"/>
       <c r="C79" s="11"/>
       <c r="D79" s="12"/>
       <c r="E79" s="12"/>
     </row>
-    <row r="80" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A80" s="11"/>
       <c r="B80" s="12"/>
       <c r="C80" s="11"/>
       <c r="D80" s="12"/>
       <c r="E80" s="12"/>
     </row>
-    <row r="81" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A81" s="11"/>
       <c r="B81" s="12"/>
       <c r="C81" s="11"/>
       <c r="D81" s="12"/>
       <c r="E81" s="12"/>
     </row>
-    <row r="82" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A82" s="11"/>
       <c r="B82" s="12"/>
       <c r="C82" s="11"/>
       <c r="D82" s="12"/>
       <c r="E82" s="12"/>
     </row>
-    <row r="83" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A83" s="11"/>
       <c r="B83" s="12"/>
       <c r="C83" s="11"/>
       <c r="D83" s="12"/>
       <c r="E83" s="12"/>
     </row>
-    <row r="84" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A84" s="11"/>
       <c r="B84" s="12"/>
       <c r="C84" s="11"/>
       <c r="D84" s="12"/>
       <c r="E84" s="12"/>
     </row>
-    <row r="85" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A85" s="11"/>
       <c r="B85" s="12"/>
       <c r="C85" s="11"/>
       <c r="D85" s="12"/>
       <c r="E85" s="12"/>
     </row>
-    <row r="86" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A86" s="11"/>
       <c r="B86" s="12"/>
       <c r="C86" s="11"/>
       <c r="D86" s="12"/>
       <c r="E86" s="12"/>
     </row>
-    <row r="87" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A87" s="11"/>
       <c r="B87" s="12"/>
       <c r="C87" s="11"/>
       <c r="D87" s="12"/>
       <c r="E87" s="12"/>
     </row>
-    <row r="88" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A88" s="11"/>
       <c r="B88" s="12"/>
       <c r="C88" s="11"/>
       <c r="D88" s="12"/>
       <c r="E88" s="12"/>
     </row>
-    <row r="89" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A89" s="11"/>
       <c r="B89" s="12"/>
       <c r="C89" s="11"/>
       <c r="D89" s="12"/>
       <c r="E89" s="12"/>
     </row>
-    <row r="90" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A90" s="11"/>
       <c r="B90" s="12"/>
       <c r="C90" s="11"/>
       <c r="D90" s="12"/>
       <c r="E90" s="12"/>
     </row>
-    <row r="91" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A91" s="11"/>
       <c r="B91" s="12"/>
       <c r="C91" s="11"/>
       <c r="D91" s="12"/>
       <c r="E91" s="12"/>
     </row>
-    <row r="92" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A92" s="11"/>
       <c r="B92" s="12"/>
       <c r="C92" s="11"/>
       <c r="D92" s="12"/>
       <c r="E92" s="12"/>
     </row>
-    <row r="93" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A93" s="11"/>
       <c r="B93" s="12"/>
       <c r="C93" s="11"/>
       <c r="D93" s="12"/>
       <c r="E93" s="12"/>
     </row>
-    <row r="94" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A94" s="11"/>
       <c r="B94" s="12"/>
       <c r="C94" s="11"/>
       <c r="D94" s="12"/>
       <c r="E94" s="12"/>
     </row>
-    <row r="95" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A95" s="11"/>
       <c r="B95" s="12"/>
       <c r="C95" s="11"/>
       <c r="D95" s="12"/>
       <c r="E95" s="12"/>
     </row>
-    <row r="96" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A96" s="11"/>
       <c r="B96" s="12"/>
       <c r="C96" s="11"/>
       <c r="D96" s="12"/>
       <c r="E96" s="12"/>
     </row>
-    <row r="97" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A97" s="11"/>
       <c r="B97" s="12"/>
       <c r="C97" s="11"/>
       <c r="D97" s="12"/>
       <c r="E97" s="12"/>
     </row>
-    <row r="98" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A98" s="11"/>
       <c r="B98" s="12"/>
       <c r="C98" s="11"/>
       <c r="D98" s="12"/>
       <c r="E98" s="12"/>
     </row>
-    <row r="99" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A99" s="11"/>
       <c r="B99" s="12"/>
       <c r="C99" s="11"/>
       <c r="D99" s="12"/>
       <c r="E99" s="12"/>
     </row>
-    <row r="100" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A100" s="11"/>
       <c r="B100" s="12"/>
       <c r="C100" s="11"/>
       <c r="D100" s="12"/>
       <c r="E100" s="12"/>
     </row>
-    <row r="101" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A101" s="11"/>
       <c r="B101" s="12"/>
       <c r="C101" s="11"/>
       <c r="D101" s="12"/>
       <c r="E101" s="12"/>
     </row>
-    <row r="102" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A102" s="11"/>
       <c r="B102" s="12"/>
       <c r="C102" s="11"/>
       <c r="D102" s="12"/>
       <c r="E102" s="12"/>
     </row>
-    <row r="103" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A103" s="11"/>
       <c r="B103" s="12"/>
       <c r="C103" s="11"/>
       <c r="D103" s="12"/>
       <c r="E103" s="12"/>
     </row>
-    <row r="104" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A104" s="11"/>
       <c r="B104" s="12"/>
       <c r="C104" s="11"/>
       <c r="D104" s="12"/>
       <c r="E104" s="12"/>
     </row>
-    <row r="105" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A105" s="11"/>
       <c r="B105" s="12"/>
       <c r="C105" s="11"/>
       <c r="D105" s="12"/>
       <c r="E105" s="12"/>
     </row>
-    <row r="106" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A106" s="11"/>
       <c r="B106" s="12"/>
       <c r="C106" s="11"/>
       <c r="D106" s="12"/>
       <c r="E106" s="12"/>
     </row>
-    <row r="107" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A107" s="11"/>
       <c r="B107" s="12"/>
       <c r="C107" s="11"/>
       <c r="D107" s="12"/>
       <c r="E107" s="12"/>
     </row>
-    <row r="108" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A108" s="11"/>
       <c r="B108" s="12"/>
       <c r="C108" s="11"/>
       <c r="D108" s="12"/>
       <c r="E108" s="12"/>
     </row>
-    <row r="109" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A109" s="11"/>
       <c r="B109" s="12"/>
       <c r="C109" s="11"/>
       <c r="D109" s="12"/>
       <c r="E109" s="12"/>
     </row>
-    <row r="110" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A110" s="11"/>
       <c r="B110" s="12"/>
       <c r="C110" s="11"/>
       <c r="D110" s="12"/>
       <c r="E110" s="12"/>
     </row>
-    <row r="111" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A111" s="11"/>
       <c r="B111" s="12"/>
       <c r="C111" s="11"/>
       <c r="D111" s="12"/>
       <c r="E111" s="12"/>
     </row>
-    <row r="112" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A112" s="11"/>
       <c r="B112" s="12"/>
       <c r="C112" s="11"/>
       <c r="D112" s="12"/>
       <c r="E112" s="12"/>
     </row>
-    <row r="113" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A113" s="11"/>
       <c r="B113" s="12"/>
       <c r="C113" s="11"/>
       <c r="D113" s="12"/>
       <c r="E113" s="12"/>
     </row>
-    <row r="114" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A114" s="11"/>
       <c r="B114" s="12"/>
       <c r="C114" s="11"/>
       <c r="D114" s="12"/>
       <c r="E114" s="12"/>
     </row>
-    <row r="115" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A115" s="11"/>
       <c r="B115" s="12"/>
       <c r="C115" s="11"/>
       <c r="D115" s="12"/>
       <c r="E115" s="12"/>
     </row>
-    <row r="116" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A116" s="11"/>
       <c r="B116" s="12"/>
       <c r="C116" s="11"/>
       <c r="D116" s="12"/>
       <c r="E116" s="12"/>
     </row>
-    <row r="117" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A117" s="11"/>
       <c r="B117" s="12"/>
       <c r="C117" s="11"/>
       <c r="D117" s="12"/>
       <c r="E117" s="12"/>
     </row>
-    <row r="118" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A118" s="11"/>
       <c r="B118" s="12"/>
       <c r="C118" s="11"/>
       <c r="D118" s="12"/>
       <c r="E118" s="12"/>
     </row>
-    <row r="119" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A119" s="11"/>
       <c r="B119" s="12"/>
       <c r="C119" s="11"/>
       <c r="D119" s="12"/>
       <c r="E119" s="12"/>
     </row>
-    <row r="120" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A120" s="11"/>
       <c r="B120" s="12"/>
       <c r="C120" s="11"/>
       <c r="D120" s="12"/>
       <c r="E120" s="12"/>
     </row>
-    <row r="121" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A121" s="11"/>
       <c r="B121" s="12"/>
       <c r="C121" s="11"/>
       <c r="D121" s="12"/>
       <c r="E121" s="12"/>
     </row>
-    <row r="122" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A122" s="11"/>
       <c r="B122" s="12"/>
       <c r="C122" s="11"/>
       <c r="D122" s="12"/>
       <c r="E122" s="12"/>
     </row>
-    <row r="123" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A123" s="11"/>
       <c r="B123" s="12"/>
       <c r="C123" s="11"/>
       <c r="D123" s="12"/>
       <c r="E123" s="12"/>
     </row>
-    <row r="124" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A124" s="11"/>
       <c r="B124" s="12"/>
       <c r="C124" s="11"/>
       <c r="D124" s="12"/>
       <c r="E124" s="12"/>
     </row>
-    <row r="125" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A125" s="11"/>
       <c r="B125" s="12"/>
       <c r="C125" s="11"/>
       <c r="D125" s="12"/>
       <c r="E125" s="12"/>
     </row>
-    <row r="126" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A126" s="11"/>
       <c r="B126" s="12"/>
       <c r="C126" s="11"/>
       <c r="D126" s="12"/>
       <c r="E126" s="12"/>
     </row>
-    <row r="127" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A127" s="11"/>
       <c r="B127" s="12"/>
       <c r="C127" s="11"/>
       <c r="D127" s="12"/>
       <c r="E127" s="12"/>
     </row>
-    <row r="128" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A128" s="11"/>
       <c r="B128" s="12"/>
       <c r="C128" s="11"/>
       <c r="D128" s="12"/>
       <c r="E128" s="12"/>
     </row>
-    <row r="129" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A129" s="11"/>
       <c r="B129" s="12"/>
       <c r="C129" s="11"/>
       <c r="D129" s="12"/>
       <c r="E129" s="12"/>
     </row>
-    <row r="130" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A130" s="11"/>
       <c r="B130" s="12"/>
       <c r="C130" s="11"/>
       <c r="D130" s="12"/>
       <c r="E130" s="12"/>
     </row>
-    <row r="131" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A131" s="11"/>
       <c r="B131" s="12"/>
       <c r="C131" s="11"/>
       <c r="D131" s="12"/>
       <c r="E131" s="12"/>
     </row>
-    <row r="132" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A132" s="11"/>
       <c r="B132" s="12"/>
       <c r="C132" s="11"/>
       <c r="D132" s="12"/>
       <c r="E132" s="12"/>
     </row>
-    <row r="133" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A133" s="11"/>
       <c r="B133" s="12"/>
       <c r="C133" s="11"/>
       <c r="D133" s="12"/>
       <c r="E133" s="12"/>
     </row>
-    <row r="134" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A134" s="11"/>
       <c r="B134" s="12"/>
       <c r="C134" s="11"/>
       <c r="D134" s="12"/>
       <c r="E134" s="12"/>
     </row>
-    <row r="135" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A135" s="11"/>
       <c r="B135" s="12"/>
       <c r="C135" s="11"/>
       <c r="D135" s="12"/>
       <c r="E135" s="12"/>
     </row>
-    <row r="136" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A136" s="11"/>
       <c r="B136" s="12"/>
       <c r="C136" s="11"/>
       <c r="D136" s="12"/>
       <c r="E136" s="12"/>
     </row>
-    <row r="137" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A137" s="11"/>
       <c r="B137" s="12"/>
       <c r="C137" s="11"/>
       <c r="D137" s="12"/>
       <c r="E137" s="12"/>
     </row>
-    <row r="138" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A138" s="11"/>
       <c r="B138" s="12"/>
       <c r="C138" s="11"/>
       <c r="D138" s="12"/>
       <c r="E138" s="12"/>
     </row>
-    <row r="139" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A139" s="11"/>
       <c r="B139" s="12"/>
       <c r="C139" s="11"/>
       <c r="D139" s="12"/>
       <c r="E139" s="12"/>
     </row>
-    <row r="140" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A140" s="11"/>
       <c r="B140" s="12"/>
       <c r="C140" s="11"/>
       <c r="D140" s="12"/>
       <c r="E140" s="12"/>
     </row>
-    <row r="141" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A141" s="11"/>
       <c r="B141" s="12"/>
       <c r="C141" s="11"/>
       <c r="D141" s="12"/>
       <c r="E141" s="12"/>
     </row>
-    <row r="142" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A142" s="11"/>
       <c r="B142" s="12"/>
       <c r="C142" s="11"/>
       <c r="D142" s="12"/>
       <c r="E142" s="12"/>
     </row>
-    <row r="143" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A143" s="11"/>
       <c r="B143" s="12"/>
       <c r="C143" s="11"/>
       <c r="D143" s="12"/>
       <c r="E143" s="12"/>
     </row>
-    <row r="144" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A144" s="11"/>
       <c r="B144" s="12"/>
       <c r="C144" s="11"/>
       <c r="D144" s="12"/>
       <c r="E144" s="12"/>
     </row>
-    <row r="145" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A145" s="11"/>
       <c r="B145" s="12"/>
       <c r="C145" s="11"/>
       <c r="D145" s="12"/>
       <c r="E145" s="12"/>
     </row>
-    <row r="146" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A146" s="11"/>
       <c r="B146" s="12"/>
       <c r="C146" s="11"/>
       <c r="D146" s="12"/>
       <c r="E146" s="12"/>
     </row>
-    <row r="147" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A147" s="11"/>
       <c r="B147" s="12"/>
       <c r="C147" s="11"/>
       <c r="D147" s="12"/>
       <c r="E147" s="12"/>
     </row>
-    <row r="148" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A148" s="11"/>
       <c r="B148" s="12"/>
       <c r="C148" s="11"/>
       <c r="D148" s="12"/>
       <c r="E148" s="12"/>
     </row>
-    <row r="149" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A149" s="11"/>
       <c r="B149" s="12"/>
       <c r="C149" s="11"/>
       <c r="D149" s="12"/>
       <c r="E149" s="12"/>
     </row>
-    <row r="150" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A150" s="11"/>
       <c r="B150" s="12"/>
       <c r="C150" s="11"/>
       <c r="D150" s="12"/>
       <c r="E150" s="12"/>
     </row>
-    <row r="151" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A151" s="11"/>
       <c r="B151" s="12"/>
       <c r="C151" s="11"/>
       <c r="D151" s="12"/>
       <c r="E151" s="12"/>
     </row>
-    <row r="152" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A152" s="11"/>
       <c r="B152" s="12"/>
       <c r="C152" s="11"/>
       <c r="D152" s="12"/>
       <c r="E152" s="12"/>
     </row>
-    <row r="153" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A153" s="11"/>
       <c r="B153" s="12"/>
       <c r="C153" s="11"/>
       <c r="D153" s="12"/>
       <c r="E153" s="12"/>
     </row>
-    <row r="154" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A154" s="11"/>
       <c r="B154" s="12"/>
       <c r="C154" s="11"/>
       <c r="D154" s="12"/>
       <c r="E154" s="12"/>
     </row>
-    <row r="155" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A155" s="11"/>
       <c r="B155" s="12"/>
       <c r="C155" s="11"/>
       <c r="D155" s="12"/>
       <c r="E155" s="12"/>
     </row>
-    <row r="156" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A156" s="11"/>
       <c r="B156" s="12"/>
       <c r="C156" s="11"/>
       <c r="D156" s="12"/>
       <c r="E156" s="12"/>
     </row>
-    <row r="157" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A157" s="11"/>
       <c r="B157" s="12"/>
       <c r="C157" s="11"/>
       <c r="D157" s="12"/>
       <c r="E157" s="12"/>
     </row>
-    <row r="158" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A158" s="11"/>
       <c r="B158" s="12"/>
       <c r="C158" s="11"/>
       <c r="D158" s="12"/>
       <c r="E158" s="12"/>
     </row>
-    <row r="159" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A159" s="11"/>
       <c r="B159" s="12"/>
       <c r="C159" s="11"/>
       <c r="D159" s="12"/>
       <c r="E159" s="12"/>
     </row>
-    <row r="160" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A160" s="11"/>
       <c r="B160" s="12"/>
       <c r="C160" s="11"/>
       <c r="D160" s="12"/>
       <c r="E160" s="12"/>
     </row>
-    <row r="161" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A161" s="11"/>
       <c r="B161" s="12"/>
       <c r="C161" s="11"/>
       <c r="D161" s="12"/>
       <c r="E161" s="12"/>
     </row>
-    <row r="162" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A162" s="11"/>
       <c r="B162" s="12"/>
       <c r="C162" s="11"/>
       <c r="D162" s="12"/>
       <c r="E162" s="12"/>
     </row>
-    <row r="163" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A163" s="11"/>
       <c r="B163" s="12"/>
       <c r="C163" s="11"/>
       <c r="D163" s="12"/>
       <c r="E163" s="12"/>
     </row>
-    <row r="164" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A164" s="11"/>
       <c r="B164" s="12"/>
       <c r="C164" s="11"/>
       <c r="D164" s="12"/>
       <c r="E164" s="12"/>
     </row>
-    <row r="165" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A165" s="11"/>
       <c r="B165" s="12"/>
       <c r="C165" s="11"/>
       <c r="D165" s="12"/>
       <c r="E165" s="12"/>
     </row>
-    <row r="166" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A166" s="11"/>
       <c r="B166" s="12"/>
       <c r="C166" s="11"/>
       <c r="D166" s="12"/>
       <c r="E166" s="12"/>
     </row>
-    <row r="167" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A167" s="11"/>
       <c r="B167" s="12"/>
       <c r="C167" s="11"/>
       <c r="D167" s="12"/>
       <c r="E167" s="12"/>
     </row>
-    <row r="168" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A168" s="11"/>
       <c r="B168" s="12"/>
       <c r="C168" s="11"/>
       <c r="D168" s="12"/>
       <c r="E168" s="12"/>
     </row>
-    <row r="169" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A169" s="11"/>
       <c r="B169" s="12"/>
       <c r="C169" s="11"/>
       <c r="D169" s="12"/>
       <c r="E169" s="12"/>
     </row>
-    <row r="170" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A170" s="11"/>
       <c r="B170" s="12"/>
       <c r="C170" s="11"/>
       <c r="D170" s="12"/>
       <c r="E170" s="12"/>
     </row>
-    <row r="171" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A171" s="11"/>
       <c r="B171" s="12"/>
       <c r="C171" s="11"/>
       <c r="D171" s="12"/>
       <c r="E171" s="12"/>
     </row>
-    <row r="172" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A172" s="11"/>
       <c r="B172" s="12"/>
       <c r="C172" s="11"/>
       <c r="D172" s="12"/>
       <c r="E172" s="12"/>
     </row>
-    <row r="173" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A173" s="11"/>
       <c r="B173" s="12"/>
       <c r="C173" s="11"/>
       <c r="D173" s="12"/>
       <c r="E173" s="12"/>
     </row>
-    <row r="174" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A174" s="11"/>
       <c r="B174" s="12"/>
       <c r="C174" s="11"/>
       <c r="D174" s="12"/>
       <c r="E174" s="12"/>
     </row>
-    <row r="175" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A175" s="11"/>
       <c r="B175" s="12"/>
       <c r="C175" s="11"/>
       <c r="D175" s="12"/>
       <c r="E175" s="12"/>
     </row>
-    <row r="176" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A176" s="11"/>
       <c r="B176" s="12"/>
       <c r="C176" s="11"/>
       <c r="D176" s="12"/>
       <c r="E176" s="12"/>
     </row>
-    <row r="177" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A177" s="11"/>
       <c r="B177" s="12"/>
       <c r="C177" s="11"/>
       <c r="D177" s="12"/>
       <c r="E177" s="12"/>
     </row>
-    <row r="178" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A178" s="11"/>
       <c r="B178" s="12"/>
       <c r="C178" s="11"/>
       <c r="D178" s="12"/>
       <c r="E178" s="12"/>
     </row>
-    <row r="179" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A179" s="11"/>
       <c r="B179" s="12"/>
       <c r="C179" s="11"/>
       <c r="D179" s="12"/>
       <c r="E179" s="12"/>
     </row>
-    <row r="180" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A180" s="11"/>
       <c r="B180" s="12"/>
       <c r="C180" s="11"/>
       <c r="D180" s="12"/>
       <c r="E180" s="12"/>
     </row>
-    <row r="181" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A181" s="11"/>
       <c r="B181" s="12"/>
       <c r="C181" s="11"/>
       <c r="D181" s="12"/>
       <c r="E181" s="12"/>
     </row>
-    <row r="182" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A182" s="11"/>
       <c r="B182" s="12"/>
       <c r="C182" s="11"/>
       <c r="D182" s="12"/>
       <c r="E182" s="12"/>
     </row>
-    <row r="183" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A183" s="11"/>
       <c r="B183" s="12"/>
       <c r="C183" s="11"/>
       <c r="D183" s="12"/>
       <c r="E183" s="12"/>
     </row>
-    <row r="184" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A184" s="11"/>
       <c r="B184" s="12"/>
       <c r="C184" s="11"/>
       <c r="D184" s="12"/>
       <c r="E184" s="12"/>
     </row>
-    <row r="185" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A185" s="11"/>
       <c r="B185" s="12"/>
       <c r="C185" s="11"/>
       <c r="D185" s="12"/>
       <c r="E185" s="12"/>
     </row>
-    <row r="186" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A186" s="11"/>
       <c r="B186" s="12"/>
       <c r="C186" s="11"/>
       <c r="D186" s="12"/>
       <c r="E186" s="12"/>
     </row>
-    <row r="187" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A187" s="11"/>
       <c r="B187" s="12"/>
       <c r="C187" s="11"/>
       <c r="D187" s="12"/>
       <c r="E187" s="12"/>
     </row>
-    <row r="188" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A188" s="11"/>
       <c r="B188" s="12"/>
       <c r="C188" s="11"/>
       <c r="D188" s="12"/>
       <c r="E188" s="12"/>
     </row>
-    <row r="189" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A189" s="11"/>
       <c r="B189" s="12"/>
       <c r="C189" s="11"/>
       <c r="D189" s="12"/>
       <c r="E189" s="12"/>
     </row>
-    <row r="190" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A190" s="11"/>
       <c r="B190" s="12"/>
       <c r="C190" s="11"/>
       <c r="D190" s="12"/>
       <c r="E190" s="12"/>
     </row>
-    <row r="191" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A191" s="11"/>
       <c r="B191" s="12"/>
       <c r="C191" s="11"/>
       <c r="D191" s="12"/>
       <c r="E191" s="12"/>
     </row>
-    <row r="192" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A192" s="11"/>
       <c r="B192" s="12"/>
       <c r="C192" s="11"/>
       <c r="D192" s="12"/>
       <c r="E192" s="12"/>
     </row>
-    <row r="193" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A193" s="11"/>
       <c r="B193" s="12"/>
       <c r="C193" s="11"/>
       <c r="D193" s="12"/>
       <c r="E193" s="12"/>
     </row>
-    <row r="194" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A194" s="11"/>
       <c r="B194" s="12"/>
       <c r="C194" s="11"/>
       <c r="D194" s="12"/>
       <c r="E194" s="12"/>
     </row>
-    <row r="195" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A195" s="11"/>
       <c r="B195" s="12"/>
       <c r="C195" s="11"/>
       <c r="D195" s="12"/>
       <c r="E195" s="12"/>
     </row>
-    <row r="196" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A196" s="11"/>
       <c r="B196" s="12"/>
       <c r="C196" s="11"/>
       <c r="D196" s="12"/>
       <c r="E196" s="12"/>
     </row>
-    <row r="197" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A197" s="11"/>
       <c r="B197" s="12"/>
       <c r="C197" s="11"/>
       <c r="D197" s="12"/>
       <c r="E197" s="12"/>
     </row>
-    <row r="198" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A198" s="11"/>
       <c r="B198" s="12"/>
       <c r="C198" s="11"/>
       <c r="D198" s="12"/>
       <c r="E198" s="12"/>
     </row>
-    <row r="199" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A199" s="11"/>
       <c r="B199" s="12"/>
       <c r="C199" s="11"/>
       <c r="D199" s="12"/>
       <c r="E199" s="12"/>
     </row>
-    <row r="200" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A200" s="11"/>
       <c r="B200" s="12"/>
       <c r="C200" s="11"/>
       <c r="D200" s="12"/>
       <c r="E200" s="12"/>
     </row>
-    <row r="201" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A201" s="11"/>
       <c r="B201" s="12"/>
       <c r="C201" s="11"/>
       <c r="D201" s="12"/>
       <c r="E201" s="12"/>
     </row>
-    <row r="202" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A202" s="11"/>
       <c r="B202" s="12"/>
       <c r="C202" s="11"/>
       <c r="D202" s="12"/>
       <c r="E202" s="12"/>
     </row>
-    <row r="203" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A203" s="11"/>
       <c r="B203" s="12"/>
       <c r="C203" s="11"/>
       <c r="D203" s="12"/>
       <c r="E203" s="12"/>
     </row>
-    <row r="204" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A204" s="11"/>
       <c r="B204" s="12"/>
       <c r="C204" s="11"/>
       <c r="D204" s="12"/>
       <c r="E204" s="12"/>
     </row>
-    <row r="205" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A205" s="11"/>
       <c r="B205" s="12"/>
       <c r="C205" s="11"/>
       <c r="D205" s="12"/>
       <c r="E205" s="12"/>
     </row>
-    <row r="206" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A206" s="11"/>
       <c r="B206" s="12"/>
       <c r="C206" s="11"/>
       <c r="D206" s="12"/>
       <c r="E206" s="12"/>
     </row>
-    <row r="207" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A207" s="11"/>
       <c r="B207" s="12"/>
       <c r="C207" s="11"/>
       <c r="D207" s="12"/>
       <c r="E207" s="12"/>
     </row>
-    <row r="208" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A208" s="11"/>
       <c r="B208" s="12"/>
       <c r="C208" s="11"/>
       <c r="D208" s="12"/>
       <c r="E208" s="12"/>
     </row>
-    <row r="209" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A209" s="11"/>
       <c r="B209" s="12"/>
       <c r="C209" s="11"/>
       <c r="D209" s="12"/>
       <c r="E209" s="12"/>
     </row>
-    <row r="210" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A210" s="11"/>
       <c r="B210" s="12"/>
       <c r="C210" s="11"/>
       <c r="D210" s="12"/>
       <c r="E210" s="12"/>
     </row>
-    <row r="211" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A211" s="11"/>
       <c r="B211" s="12"/>
       <c r="C211" s="11"/>
       <c r="D211" s="12"/>
       <c r="E211" s="12"/>
     </row>
-    <row r="212" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A212" s="11"/>
       <c r="B212" s="12"/>
       <c r="C212" s="11"/>
       <c r="D212" s="12"/>
       <c r="E212" s="12"/>
     </row>
-    <row r="213" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A213" s="11"/>
       <c r="B213" s="12"/>
       <c r="C213" s="11"/>
       <c r="D213" s="12"/>
       <c r="E213" s="12"/>
     </row>
-    <row r="214" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A214" s="11"/>
       <c r="B214" s="12"/>
       <c r="C214" s="11"/>
       <c r="D214" s="12"/>
       <c r="E214" s="12"/>
     </row>
-    <row r="215" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A215" s="11"/>
       <c r="B215" s="12"/>
       <c r="C215" s="11"/>
       <c r="D215" s="12"/>
       <c r="E215" s="12"/>
     </row>
-    <row r="216" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A216" s="11"/>
       <c r="B216" s="12"/>
       <c r="C216" s="11"/>
       <c r="D216" s="12"/>
       <c r="E216" s="12"/>
     </row>
-    <row r="217" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A217" s="11"/>
       <c r="B217" s="12"/>
       <c r="C217" s="11"/>
       <c r="D217" s="12"/>
       <c r="E217" s="12"/>
     </row>
-    <row r="218" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A218" s="11"/>
       <c r="B218" s="12"/>
       <c r="C218" s="11"/>
       <c r="D218" s="12"/>
       <c r="E218" s="12"/>
     </row>
-    <row r="219" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A219" s="11"/>
       <c r="B219" s="12"/>
       <c r="C219" s="11"/>
       <c r="D219" s="12"/>
       <c r="E219" s="12"/>
     </row>
-    <row r="220" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A220" s="11"/>
       <c r="B220" s="12"/>
       <c r="C220" s="11"/>
       <c r="D220" s="12"/>
       <c r="E220" s="12"/>
     </row>
-    <row r="221" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A221" s="11"/>
       <c r="B221" s="12"/>
       <c r="C221" s="11"/>
       <c r="D221" s="12"/>
       <c r="E221" s="12"/>
     </row>
-    <row r="222" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A222" s="11"/>
       <c r="B222" s="12"/>
       <c r="C222" s="11"/>
       <c r="D222" s="12"/>
       <c r="E222" s="12"/>
     </row>
-    <row r="223" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A223" s="11"/>
       <c r="B223" s="12"/>
       <c r="C223" s="11"/>
       <c r="D223" s="12"/>
       <c r="E223" s="12"/>
     </row>
-    <row r="224" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A224" s="11"/>
       <c r="B224" s="12"/>
       <c r="C224" s="11"/>
       <c r="D224" s="12"/>
       <c r="E224" s="12"/>
     </row>
-    <row r="225" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A225" s="11"/>
       <c r="B225" s="12"/>
       <c r="C225" s="11"/>
       <c r="D225" s="12"/>
       <c r="E225" s="12"/>
     </row>
-    <row r="226" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A226" s="11"/>
       <c r="B226" s="12"/>
       <c r="C226" s="11"/>
       <c r="D226" s="12"/>
       <c r="E226" s="12"/>
     </row>
-    <row r="227" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A227" s="11"/>
       <c r="B227" s="12"/>
       <c r="C227" s="11"/>
       <c r="D227" s="12"/>
       <c r="E227" s="12"/>
     </row>
-    <row r="228" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A228" s="11"/>
       <c r="B228" s="12"/>
       <c r="C228" s="11"/>
       <c r="D228" s="12"/>
       <c r="E228" s="12"/>
     </row>
-    <row r="229" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A229" s="11"/>
       <c r="B229" s="12"/>
       <c r="C229" s="11"/>
       <c r="D229" s="12"/>
       <c r="E229" s="12"/>
     </row>
-    <row r="230" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A230" s="11"/>
       <c r="B230" s="12"/>
       <c r="C230" s="11"/>
       <c r="D230" s="12"/>
       <c r="E230" s="12"/>
     </row>
-    <row r="231" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A231" s="11"/>
       <c r="B231" s="12"/>
       <c r="C231" s="11"/>
       <c r="D231" s="12"/>
       <c r="E231" s="12"/>
     </row>
-    <row r="232" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A232" s="11"/>
       <c r="B232" s="12"/>
       <c r="C232" s="11"/>
       <c r="D232" s="12"/>
       <c r="E232" s="12"/>
     </row>
-    <row r="233" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A233" s="11"/>
       <c r="B233" s="12"/>
       <c r="C233" s="11"/>
       <c r="D233" s="12"/>
       <c r="E233" s="12"/>
     </row>
-    <row r="234" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A234" s="11"/>
       <c r="B234" s="12"/>
       <c r="C234" s="11"/>
       <c r="D234" s="12"/>
       <c r="E234" s="12"/>
     </row>
-    <row r="235" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A235" s="11"/>
       <c r="B235" s="12"/>
       <c r="C235" s="11"/>
       <c r="D235" s="12"/>
       <c r="E235" s="12"/>
     </row>
-    <row r="236" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A236" s="11"/>
       <c r="B236" s="12"/>
       <c r="C236" s="11"/>
       <c r="D236" s="12"/>
       <c r="E236" s="12"/>
     </row>
-    <row r="237" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A237" s="11"/>
       <c r="B237" s="12"/>
       <c r="C237" s="11"/>
       <c r="D237" s="12"/>
       <c r="E237" s="12"/>
     </row>
-    <row r="238" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A238" s="11"/>
       <c r="B238" s="12"/>
       <c r="C238" s="11"/>
       <c r="D238" s="12"/>
       <c r="E238" s="12"/>
     </row>
-    <row r="239" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A239" s="11"/>
       <c r="B239" s="12"/>
       <c r="C239" s="11"/>
       <c r="D239" s="12"/>
       <c r="E239" s="12"/>
     </row>
-    <row r="240" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A240" s="11"/>
       <c r="B240" s="12"/>
       <c r="C240" s="11"/>
       <c r="D240" s="12"/>
       <c r="E240" s="12"/>
     </row>
-    <row r="241" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A241" s="11"/>
       <c r="B241" s="12"/>
       <c r="C241" s="11"/>
       <c r="D241" s="12"/>
       <c r="E241" s="12"/>
     </row>
-    <row r="242" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A242" s="11"/>
       <c r="B242" s="12"/>
       <c r="C242" s="11"/>
       <c r="D242" s="12"/>
       <c r="E242" s="12"/>
     </row>
-    <row r="243" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A243" s="11"/>
       <c r="B243" s="12"/>
       <c r="C243" s="11"/>
       <c r="D243" s="12"/>
       <c r="E243" s="12"/>
     </row>
-    <row r="244" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A244" s="11"/>
       <c r="B244" s="12"/>
       <c r="C244" s="11"/>
       <c r="D244" s="12"/>
       <c r="E244" s="12"/>
     </row>
-    <row r="245" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A245" s="11"/>
       <c r="B245" s="12"/>
       <c r="C245" s="11"/>
       <c r="D245" s="12"/>
       <c r="E245" s="12"/>
     </row>
-    <row r="246" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A246" s="11"/>
       <c r="B246" s="12"/>
       <c r="C246" s="11"/>
       <c r="D246" s="12"/>
       <c r="E246" s="12"/>
     </row>
-    <row r="247" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A247" s="11"/>
       <c r="B247" s="12"/>
       <c r="C247" s="11"/>
       <c r="D247" s="12"/>
       <c r="E247" s="12"/>
     </row>
-    <row r="248" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A248" s="11"/>
       <c r="B248" s="12"/>
       <c r="C248" s="11"/>
       <c r="D248" s="12"/>
       <c r="E248" s="12"/>
     </row>
-    <row r="249" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A249" s="11"/>
       <c r="B249" s="12"/>
       <c r="C249" s="11"/>
       <c r="D249" s="12"/>
       <c r="E249" s="12"/>
     </row>
-    <row r="250" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A250" s="11"/>
       <c r="B250" s="12"/>
       <c r="C250" s="11"/>
       <c r="D250" s="12"/>
       <c r="E250" s="12"/>
     </row>
-    <row r="251" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A251" s="11"/>
       <c r="B251" s="12"/>
       <c r="C251" s="11"/>
       <c r="D251" s="12"/>
       <c r="E251" s="12"/>
     </row>
-    <row r="252" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A252" s="11"/>
       <c r="B252" s="12"/>
       <c r="C252" s="11"/>
       <c r="D252" s="12"/>
       <c r="E252" s="12"/>
     </row>
-    <row r="253" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A253" s="11"/>
       <c r="B253" s="12"/>
       <c r="C253" s="11"/>
       <c r="D253" s="12"/>
       <c r="E253" s="12"/>
     </row>
-    <row r="254" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A254" s="11"/>
       <c r="B254" s="12"/>
       <c r="C254" s="11"/>
       <c r="D254" s="12"/>
       <c r="E254" s="12"/>
     </row>
-    <row r="255" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A255" s="11"/>
       <c r="B255" s="12"/>
       <c r="C255" s="11"/>
       <c r="D255" s="12"/>
       <c r="E255" s="12"/>
     </row>
-    <row r="256" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A256" s="11"/>
       <c r="B256" s="12"/>
       <c r="C256" s="11"/>
       <c r="D256" s="12"/>
       <c r="E256" s="12"/>
     </row>
-    <row r="257" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A257" s="11"/>
       <c r="B257" s="12"/>
       <c r="C257" s="11"/>
       <c r="D257" s="12"/>
       <c r="E257" s="12"/>
     </row>
-    <row r="258" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A258" s="11"/>
       <c r="B258" s="12"/>
       <c r="C258" s="11"/>
       <c r="D258" s="12"/>
       <c r="E258" s="12"/>
     </row>
-    <row r="259" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A259" s="11"/>
       <c r="B259" s="12"/>
       <c r="C259" s="11"/>
       <c r="D259" s="12"/>
       <c r="E259" s="12"/>
     </row>
-    <row r="260" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A260" s="11"/>
       <c r="B260" s="12"/>
       <c r="C260" s="11"/>
       <c r="D260" s="12"/>
       <c r="E260" s="12"/>
     </row>
-    <row r="261" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="262" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="263" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="264" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="265" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="266" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="267" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="268" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="269" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="270" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="271" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="272" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="273" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="274" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="275" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="276" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="277" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="278" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="279" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="280" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="281" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="282" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="283" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="284" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="285" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="286" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="287" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="288" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="289" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="290" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="291" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="292" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="293" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="294" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="295" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="296" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="297" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="298" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="299" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="300" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="301" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="302" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="303" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="304" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="305" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="306" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="307" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="308" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="309" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="310" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="311" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="312" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="313" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="314" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="315" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="316" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="317" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="318" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="319" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="320" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="321" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="322" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="323" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="324" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="325" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="326" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="327" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="328" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="329" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="330" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="331" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="332" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="333" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="334" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="335" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="336" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="337" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="338" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="339" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="340" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="341" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="342" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="343" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="344" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="345" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="346" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="347" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="348" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="349" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="350" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="351" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="352" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="353" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="354" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="355" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="356" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="357" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="358" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="359" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="360" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="361" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="362" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="363" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="364" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="365" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="366" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="367" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="368" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="369" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="370" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="371" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="372" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="373" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="374" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="375" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="376" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="377" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="378" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="379" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="380" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="381" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="382" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="383" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="384" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="385" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="386" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="387" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="388" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="389" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="390" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="391" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="392" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="393" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="394" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="395" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="396" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="397" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="398" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="399" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="400" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="401" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="402" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="403" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="404" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="405" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="406" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="407" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="408" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="409" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="410" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="411" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="412" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="413" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="414" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="415" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="416" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="417" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="418" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="419" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="420" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="421" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="422" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="423" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="424" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="425" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="426" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="427" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="428" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="429" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="430" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="431" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="432" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="433" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="434" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="435" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="436" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="437" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="438" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="439" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="440" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="441" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="442" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="443" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="444" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="445" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="446" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="447" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="448" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="449" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="450" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="451" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="452" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="453" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="454" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="455" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="456" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="457" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="458" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="459" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="460" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="461" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="462" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="463" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="464" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="465" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="466" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="467" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="468" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="469" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="470" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="471" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="472" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="473" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="474" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="475" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="476" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="477" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="478" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="479" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="480" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="481" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="482" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="483" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="484" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="485" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="486" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="487" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="488" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="489" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="490" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="491" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="492" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="493" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="494" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="495" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="496" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="497" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="498" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="499" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="500" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="501" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="502" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="503" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="504" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="505" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="506" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="507" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="508" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="509" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="510" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="511" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="512" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="513" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="514" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="515" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="516" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="517" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="518" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="519" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="520" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="521" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="522" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="523" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="524" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="525" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="526" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="527" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="528" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="529" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="530" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="531" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="532" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="533" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="534" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="535" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="536" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="537" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="538" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="539" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="540" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="541" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="542" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="543" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="544" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="545" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="546" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="547" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="548" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="549" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="550" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="551" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="552" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="553" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="554" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="555" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="556" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="557" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="558" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="559" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="560" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="561" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="562" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="563" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="564" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="565" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="566" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="567" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="568" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="569" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="570" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="571" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="572" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="573" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="574" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="575" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="576" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="577" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="578" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="579" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="580" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="581" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="582" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="583" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="584" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="585" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="586" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="587" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="588" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="589" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="590" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="591" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="592" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="593" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="594" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="595" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="596" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="597" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="598" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="599" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="600" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="601" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="602" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="603" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="604" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="605" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="606" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="607" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="608" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="609" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="610" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="611" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="612" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="613" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="614" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="615" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="616" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="617" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="618" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="619" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="620" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="621" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="622" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="623" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="624" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="625" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="626" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="627" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="628" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="629" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="630" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="631" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="632" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="633" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="634" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="635" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="636" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="637" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="638" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="639" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="640" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="641" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="642" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="643" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="644" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="645" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="646" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="647" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="648" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="649" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="650" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="651" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="652" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="653" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="654" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="655" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="656" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="657" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="658" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="659" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="660" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="661" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="662" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="663" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="664" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="665" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="666" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="667" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="668" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="669" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="670" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="671" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="672" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="673" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="674" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="675" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="676" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="677" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="678" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="679" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="680" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="681" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="682" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="683" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="684" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="685" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="686" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="687" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="688" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="689" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="690" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="691" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="692" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="693" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="694" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="695" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="696" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="697" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="698" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="699" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="700" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="701" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="702" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="703" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="704" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="705" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="706" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="707" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="708" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="709" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="710" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="711" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="712" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="713" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="714" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="715" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="716" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="717" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="718" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="719" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="720" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="721" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="722" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="723" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="724" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="725" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="726" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="727" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="728" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="729" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="730" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="731" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="732" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="733" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="734" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="735" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="736" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="737" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="738" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="739" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="740" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="741" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="742" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="743" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="744" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="745" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="746" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="747" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="748" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="749" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="750" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="751" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="752" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="753" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="754" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="755" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="756" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="757" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="758" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="759" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="760" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="761" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="762" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="763" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="764" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="765" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="766" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="767" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="768" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="769" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="770" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="771" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="772" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="773" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="774" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="775" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="776" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="777" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="778" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="779" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="780" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="781" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="782" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="783" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="784" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="785" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="786" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="787" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="788" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="789" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="790" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="791" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="792" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="793" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="794" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="795" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="796" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="797" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="798" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="799" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="800" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="801" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="802" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="803" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="804" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="805" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="806" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="807" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="808" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="809" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="810" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="811" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="812" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="813" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="814" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="815" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="816" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="817" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="818" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="819" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="820" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="821" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="822" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="823" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="824" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="825" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="826" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="827" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="828" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="829" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="830" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="831" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="832" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="833" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="834" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="835" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="836" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="837" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="838" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="839" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="840" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="841" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="842" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="843" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="844" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="845" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="846" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="847" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="848" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="849" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="850" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="851" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="852" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="853" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="854" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="855" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="856" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="857" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="858" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="859" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="860" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="861" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="862" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="863" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="864" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="865" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="866" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="867" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="868" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="869" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="870" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="871" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="872" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="873" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="874" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="875" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="876" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="877" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="878" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="879" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="880" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="881" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="882" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="883" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="884" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="885" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="886" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="887" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="888" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="889" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="890" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="891" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="892" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="893" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="894" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="895" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="896" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="897" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="898" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="899" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="900" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="901" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="902" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="903" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="904" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="905" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="906" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="907" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="908" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="909" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="910" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="911" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="912" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="913" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="914" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="915" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="916" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="917" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="918" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="919" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="920" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="921" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="922" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="923" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="924" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="925" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="926" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="927" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="928" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="929" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="930" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="931" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="932" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="933" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="934" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="935" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="936" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="937" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="938" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="939" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="940" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="941" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="942" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="943" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="944" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="945" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="946" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="947" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="948" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="949" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="950" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="951" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="952" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="953" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="954" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="955" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="956" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="957" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="958" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="959" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="960" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="961" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="962" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="963" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="964" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="965" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="966" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="967" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="968" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="969" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="970" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="971" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="972" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="973" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="974" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="975" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="976" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="977" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="978" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="979" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="980" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="981" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="982" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="983" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="984" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="985" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="986" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="987" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="988" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="989" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="990" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="991" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="992" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="993" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="994" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="995" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="996" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="997" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="998" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="999" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="261" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="262" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="263" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="264" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="265" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="266" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="267" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="268" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="269" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="270" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="271" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="272" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="273" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="274" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="275" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="276" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="277" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="278" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="279" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="280" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="281" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="282" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="283" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="284" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="285" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="286" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="287" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="288" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="289" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="290" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="291" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="292" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="293" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="294" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="295" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="296" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="297" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="298" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="299" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="300" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="301" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="302" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="303" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="304" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="305" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="306" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="307" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="308" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="309" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="310" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="311" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="312" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="313" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="314" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="315" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="316" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="317" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="318" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="319" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="320" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="321" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="322" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="323" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="324" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="325" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="326" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="327" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="328" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="329" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="330" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="331" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="332" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="333" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="334" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="335" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="336" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="337" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="338" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="339" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="340" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="341" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="342" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="343" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="344" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="345" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="346" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="347" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="348" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="349" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="350" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="351" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="352" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="353" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="354" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="355" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="356" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="357" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="358" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="359" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="360" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="361" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="362" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="363" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="364" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="365" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="366" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="367" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="368" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="369" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="370" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="371" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="372" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="373" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="374" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="375" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="376" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="377" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="378" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="379" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="380" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="381" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="382" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="383" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="384" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="385" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="386" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="387" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="388" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="389" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="390" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="391" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="392" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="393" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="394" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="395" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="396" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="397" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="398" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="399" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="400" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="401" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="402" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="403" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="404" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="405" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="406" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="407" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="408" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="409" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="410" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="411" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="412" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="413" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="414" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="415" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="416" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="417" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="418" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="419" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="420" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="421" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="422" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="423" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="424" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="425" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="426" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="427" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="428" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="429" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="430" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="431" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="432" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="433" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="434" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="435" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="436" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="437" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="438" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="439" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="440" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="441" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="442" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="443" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="444" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="445" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="446" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="447" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="448" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="449" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="450" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="451" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="452" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="453" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="454" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="455" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="456" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="457" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="458" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="459" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="460" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="461" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="462" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="463" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="464" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="465" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="466" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="467" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="468" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="469" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="470" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="471" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="472" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="473" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="474" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="475" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="476" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="477" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="478" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="479" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="480" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="481" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="482" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="483" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="484" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="485" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="486" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="487" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="488" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="489" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="490" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="491" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="492" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="493" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="494" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="495" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="496" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="497" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="498" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="499" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="500" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="501" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="502" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="503" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="504" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="505" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="506" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="507" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="508" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="509" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="510" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="511" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="512" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="513" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="514" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="515" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="516" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="517" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="518" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="519" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="520" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="521" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="522" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="523" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="524" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="525" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="526" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="527" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="528" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="529" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="530" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="531" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="532" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="533" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="534" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="535" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="536" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="537" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="538" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="539" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="540" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="541" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="542" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="543" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="544" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="545" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="546" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="547" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="548" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="549" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="550" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="551" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="552" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="553" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="554" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="555" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="556" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="557" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="558" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="559" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="560" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="561" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="562" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="563" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="564" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="565" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="566" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="567" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="568" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="569" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="570" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="571" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="572" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="573" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="574" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="575" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="576" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="577" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="578" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="579" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="580" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="581" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="582" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="583" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="584" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="585" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="586" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="587" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="588" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="589" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="590" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="591" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="592" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="593" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="594" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="595" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="596" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="597" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="598" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="599" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="600" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="601" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="602" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="603" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="604" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="605" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="606" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="607" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="608" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="609" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="610" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="611" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="612" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="613" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="614" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="615" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="616" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="617" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="618" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="619" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="620" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="621" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="622" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="623" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="624" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="625" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="626" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="627" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="628" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="629" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="630" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="631" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="632" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="633" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="634" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="635" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="636" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="637" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="638" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="639" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="640" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="641" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="642" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="643" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="644" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="645" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="646" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="647" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="648" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="649" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="650" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="651" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="652" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="653" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="654" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="655" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="656" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="657" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="658" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="659" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="660" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="661" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="662" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="663" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="664" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="665" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="666" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="667" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="668" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="669" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="670" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="671" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="672" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="673" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="674" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="675" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="676" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="677" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="678" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="679" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="680" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="681" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="682" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="683" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="684" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="685" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="686" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="687" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="688" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="689" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="690" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="691" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="692" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="693" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="694" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="695" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="696" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="697" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="698" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="699" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="700" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="701" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="702" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="703" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="704" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="705" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="706" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="707" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="708" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="709" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="710" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="711" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="712" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="713" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="714" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="715" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="716" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="717" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="718" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="719" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="720" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="721" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="722" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="723" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="724" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="725" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="726" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="727" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="728" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="729" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="730" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="731" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="732" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="733" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="734" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="735" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="736" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="737" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="738" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="739" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="740" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="741" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="742" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="743" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="744" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="745" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="746" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="747" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="748" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="749" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="750" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="751" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="752" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="753" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="754" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="755" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="756" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="757" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="758" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="759" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="760" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="761" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="762" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="763" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="764" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="765" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="766" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="767" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="768" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="769" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="770" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="771" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="772" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="773" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="774" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="775" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="776" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="777" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="778" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="779" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="780" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="781" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="782" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="783" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="784" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="785" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="786" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="787" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="788" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="789" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="790" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="791" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="792" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="793" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="794" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="795" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="796" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="797" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="798" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="799" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="800" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="801" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="802" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="803" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="804" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="805" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="806" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="807" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="808" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="809" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="810" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="811" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="812" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="813" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="814" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="815" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="816" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="817" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="818" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="819" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="820" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="821" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="822" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="823" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="824" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="825" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="826" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="827" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="828" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="829" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="830" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="831" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="832" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="833" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="834" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="835" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="836" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="837" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="838" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="839" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="840" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="841" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="842" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="843" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="844" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="845" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="846" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="847" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="848" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="849" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="850" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="851" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="852" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="853" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="854" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="855" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="856" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="857" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="858" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="859" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="860" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="861" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="862" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="863" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="864" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="865" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="866" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="867" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="868" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="869" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="870" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="871" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="872" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="873" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="874" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="875" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="876" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="877" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="878" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="879" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="880" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="881" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="882" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="883" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="884" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="885" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="886" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="887" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="888" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="889" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="890" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="891" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="892" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="893" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="894" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="895" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="896" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="897" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="898" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="899" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="900" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="901" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="902" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="903" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="904" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="905" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="906" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="907" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="908" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="909" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="910" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="911" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="912" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="913" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="914" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="915" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="916" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="917" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="918" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="919" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="920" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="921" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="922" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="923" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="924" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="925" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="926" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="927" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="928" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="929" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="930" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="931" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="932" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="933" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="934" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="935" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="936" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="937" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="938" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="939" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="940" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="941" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="942" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="943" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="944" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="945" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="946" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="947" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="948" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="949" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="950" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="951" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="952" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="953" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="954" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="955" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="956" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="957" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="958" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="959" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="960" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="961" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="962" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="963" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="964" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="965" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="966" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="967" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="968" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="969" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="970" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="971" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="972" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="973" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="974" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="975" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="976" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="977" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="978" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="979" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="980" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="981" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="982" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="983" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="984" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="985" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="986" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="987" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="988" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="989" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="990" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="991" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="992" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="993" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="994" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="995" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="996" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="997" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="998" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="999" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D4" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
@@ -3481,6 +3498,7 @@
     <hyperlink ref="D9" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
     <hyperlink ref="D10" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
     <hyperlink ref="D11" r:id="rId6" xr:uid="{D5E07517-70A2-400E-81E3-BC651813A3D1}"/>
+    <hyperlink ref="D12" r:id="rId7" xr:uid="{3E69F7D3-612D-4AF4-9DCF-D06E3569F3F5}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
se agrego el 12 alumno  al archivo
</commit_message>
<xml_diff>
--- a/Lista de Alumnos.xlsx
+++ b/Lista de Alumnos.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t>#</t>
   </si>
@@ -104,6 +104,24 @@
   </si>
   <si>
     <t>Cabro645</t>
+  </si>
+  <si>
+    <t>William Bernardo Leyton Segovia</t>
+  </si>
+  <si>
+    <t>williamleyton89@gmail.com</t>
+  </si>
+  <si>
+    <t>Wleyton89</t>
+  </si>
+  <si>
+    <t>Carla Wayar</t>
+  </si>
+  <si>
+    <t>carlaargentinawayar@gmail.com</t>
+  </si>
+  <si>
+    <t>WayarCarla</t>
   </si>
   <si>
     <t xml:space="preserve">Iván Exequiel Gomez </t>
@@ -323,7 +341,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -355,9 +373,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -389,6 +425,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -751,16 +805,16 @@
       <c r="A11" s="5">
         <v>10.0</v>
       </c>
-      <c r="B11" s="11" t="s">
+      <c r="B11" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="C11" s="12">
-        <v>1.0</v>
-      </c>
-      <c r="D11" s="11" t="s">
+      <c r="C11" s="5">
+        <v>3.0</v>
+      </c>
+      <c r="D11" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="E11" s="11" t="s">
+      <c r="E11" s="6" t="s">
         <v>33</v>
       </c>
     </row>
@@ -768,19 +822,35 @@
       <c r="A12" s="5">
         <v>11.0</v>
       </c>
-      <c r="B12" s="6"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
+      <c r="B12" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="13" ht="19.5" customHeight="1">
       <c r="A13" s="5">
         <v>12.0</v>
       </c>
-      <c r="B13" s="6"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
+      <c r="B13" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="E13" s="11" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="14" ht="19.5" customHeight="1">
       <c r="A14" s="5">
@@ -2612,10 +2682,12 @@
     <hyperlink r:id="rId3" ref="D8"/>
     <hyperlink r:id="rId4" ref="D9"/>
     <hyperlink r:id="rId5" ref="D10"/>
+    <hyperlink r:id="rId6" ref="D11"/>
+    <hyperlink r:id="rId7" ref="D12"/>
   </hyperlinks>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <drawing r:id="rId6"/>
+  <drawing r:id="rId8"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Se agrega el 13 alumno al archivo
</commit_message>
<xml_diff>
--- a/Lista de Alumnos.xlsx
+++ b/Lista de Alumnos.xlsx
@@ -1,17 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Temp\nuevo\Alumnos\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55072BD9-E547-429B-A066-FB6D82893E87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Electronica Microcontrolada" sheetId="1" r:id="rId4"/>
+    <sheet name="Electronica Microcontrolada" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
   <si>
     <t>#</t>
   </si>
@@ -131,57 +140,73 @@
   </si>
   <si>
     <t xml:space="preserve">ivanexegomez </t>
+  </si>
+  <si>
+    <t>Alfredo Sebastian Palacios</t>
+  </si>
+  <si>
+    <t>alfredo.pc@gmail.com</t>
+  </si>
+  <si>
+    <t>alfredop</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="8">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="18.0"/>
+      <sz val="18"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
       <u/>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
       <u/>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
       <u/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF0563C1"/>
       <name val="Calibri"/>
     </font>
     <font>
       <u/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF0563C1"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -189,31 +214,43 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="5">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
+      <right/>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
+      <left/>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
@@ -223,6 +260,7 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -237,76 +275,85 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+  <cellStyleXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="3" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+  <cellXfs count="16">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="2" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="2" fillId="0" fontId="1" numFmtId="3" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="3" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="4" fillId="0" fontId="2" numFmtId="3" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="4" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="4" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="4" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="4" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="4" fillId="0" fontId="6" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="4" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="4" fillId="0" fontId="2" numFmtId="3" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="7" numFmtId="3" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+  <cellStyles count="2">
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -498,7 +545,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln cap="flat" cmpd="sng" w="9525" algn="ctr">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -507,13 +554,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln cap="flat" cmpd="sng" w="25400" algn="ctr">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln cap="flat" cmpd="sng" w="38100" algn="ctr">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -523,7 +570,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" rotWithShape="0" dir="5400000" dist="20000">
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -532,7 +579,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" rotWithShape="0" dir="5400000" dist="23000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -541,7 +588,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" rotWithShape="0" dir="5400000" dist="23000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -551,12 +598,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
+            <a:lightRig rig="threePt" dir="t">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT h="25400" w="63500"/>
+            <a:bevelT w="63500" h="25400"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -587,7 +634,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -606,7 +653,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -618,24 +665,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E260"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="6.86"/>
-    <col customWidth="1" min="2" max="2" width="37.14"/>
-    <col customWidth="1" min="3" max="3" width="10.57"/>
-    <col customWidth="1" min="4" max="4" width="31.0"/>
-    <col customWidth="1" min="5" max="5" width="29.0"/>
-    <col customWidth="1" min="6" max="6" width="8.71"/>
+    <col min="1" max="1" width="6.85546875" customWidth="1"/>
+    <col min="2" max="2" width="37.140625" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" customWidth="1"/>
+    <col min="4" max="4" width="31" customWidth="1"/>
+    <col min="5" max="5" width="29" customWidth="1"/>
+    <col min="6" max="6" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="27.0" customHeight="1">
+    <row r="1" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -652,15 +699,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" ht="19.5" customHeight="1">
+    <row r="2" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>5</v>
       </c>
       <c r="C2" s="5">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="D2" s="7" t="s">
         <v>6</v>
@@ -669,30 +716,30 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" ht="19.5" customHeight="1">
+    <row r="3" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>8</v>
       </c>
       <c r="C3" s="5">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>9</v>
       </c>
       <c r="E3" s="6"/>
     </row>
-    <row r="4" ht="19.5" customHeight="1">
+    <row r="4" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>10</v>
       </c>
       <c r="C4" s="5">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="D4" s="7" t="s">
         <v>11</v>
@@ -701,15 +748,15 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" ht="19.5" customHeight="1">
+    <row r="5" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>13</v>
       </c>
       <c r="C5" s="5">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="D5" s="9" t="s">
         <v>14</v>
@@ -718,15 +765,15 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" ht="19.5" customHeight="1">
+    <row r="6" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>16</v>
       </c>
       <c r="C6" s="5">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="D6" s="7" t="s">
         <v>17</v>
@@ -735,15 +782,15 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" ht="19.5" customHeight="1">
+    <row r="7" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>19</v>
       </c>
       <c r="C7" s="5">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="D7" s="7" t="s">
         <v>20</v>
@@ -752,15 +799,15 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" ht="19.5" customHeight="1">
+    <row r="8" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="B8" s="6" t="s">
         <v>22</v>
       </c>
       <c r="C8" s="5">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="D8" s="9" t="s">
         <v>23</v>
@@ -769,15 +816,15 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" ht="19.5" customHeight="1">
+    <row r="9" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="B9" s="6" t="s">
         <v>25</v>
       </c>
       <c r="C9" s="5">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="D9" s="7" t="s">
         <v>26</v>
@@ -786,9 +833,9 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" ht="19.5" customHeight="1">
+    <row r="10" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
-        <v>9.0</v>
+        <v>9</v>
       </c>
       <c r="B10" s="6" t="s">
         <v>28</v>
@@ -801,15 +848,15 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" ht="19.5" customHeight="1">
+    <row r="11" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>31</v>
       </c>
       <c r="C11" s="5">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="D11" s="10" t="s">
         <v>32</v>
@@ -818,15 +865,15 @@
         <v>33</v>
       </c>
     </row>
-    <row r="12" ht="19.5" customHeight="1">
+    <row r="12" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
-        <v>11.0</v>
+        <v>11</v>
       </c>
       <c r="B12" s="6" t="s">
         <v>34</v>
       </c>
       <c r="C12" s="5">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="D12" s="10" t="s">
         <v>35</v>
@@ -835,15 +882,15 @@
         <v>36</v>
       </c>
     </row>
-    <row r="13" ht="19.5" customHeight="1">
+    <row r="13" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
-        <v>12.0</v>
+        <v>12</v>
       </c>
       <c r="B13" s="11" t="s">
         <v>37</v>
       </c>
       <c r="C13" s="12">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="D13" s="11" t="s">
         <v>38</v>
@@ -852,1823 +899,1831 @@
         <v>39</v>
       </c>
     </row>
-    <row r="14" ht="19.5" customHeight="1">
+    <row r="14" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
-        <v>13.0</v>
-      </c>
-      <c r="B14" s="6"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-    </row>
-    <row r="15" ht="19.5" customHeight="1">
+        <v>13</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C14" s="5">
+        <v>2</v>
+      </c>
+      <c r="D14" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
-        <v>14.0</v>
+        <v>14</v>
       </c>
       <c r="B15" s="6"/>
       <c r="C15" s="5"/>
       <c r="D15" s="6"/>
       <c r="E15" s="6"/>
     </row>
-    <row r="16" ht="19.5" customHeight="1">
+    <row r="16" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
-        <v>15.0</v>
+        <v>15</v>
       </c>
       <c r="B16" s="6"/>
       <c r="C16" s="5"/>
       <c r="D16" s="6"/>
       <c r="E16" s="6"/>
     </row>
-    <row r="17" ht="19.5" customHeight="1">
+    <row r="17" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
-        <v>16.0</v>
+        <v>16</v>
       </c>
       <c r="B17" s="6"/>
       <c r="C17" s="5"/>
       <c r="D17" s="6"/>
       <c r="E17" s="6"/>
     </row>
-    <row r="18" ht="25.5" customHeight="1">
+    <row r="18" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
-        <v>17.0</v>
+        <v>17</v>
       </c>
       <c r="B18" s="6"/>
       <c r="C18" s="5"/>
       <c r="D18" s="6"/>
       <c r="E18" s="6"/>
     </row>
-    <row r="19" ht="25.5" customHeight="1">
+    <row r="19" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
-        <v>18.0</v>
+        <v>18</v>
       </c>
       <c r="B19" s="6"/>
       <c r="C19" s="5"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
     </row>
-    <row r="20" ht="25.5" customHeight="1">
+    <row r="20" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
-        <v>19.0</v>
+        <v>19</v>
       </c>
       <c r="B20" s="6"/>
       <c r="C20" s="5"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
     </row>
-    <row r="21" ht="25.5" customHeight="1">
+    <row r="21" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="5">
-        <v>20.0</v>
+        <v>20</v>
       </c>
       <c r="B21" s="6"/>
       <c r="C21" s="5"/>
       <c r="D21" s="6"/>
       <c r="E21" s="6"/>
     </row>
-    <row r="22" ht="25.5" customHeight="1">
+    <row r="22" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="5">
-        <v>21.0</v>
+        <v>21</v>
       </c>
       <c r="B22" s="6"/>
       <c r="C22" s="5"/>
       <c r="D22" s="6"/>
       <c r="E22" s="6"/>
     </row>
-    <row r="23" ht="25.5" customHeight="1">
+    <row r="23" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="5">
-        <v>22.0</v>
+        <v>22</v>
       </c>
       <c r="B23" s="6"/>
       <c r="C23" s="5"/>
       <c r="D23" s="6"/>
       <c r="E23" s="6"/>
     </row>
-    <row r="24" ht="25.5" customHeight="1">
+    <row r="24" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="5">
-        <v>23.0</v>
+        <v>23</v>
       </c>
       <c r="B24" s="6"/>
       <c r="C24" s="5"/>
       <c r="D24" s="6"/>
       <c r="E24" s="6"/>
     </row>
-    <row r="25" ht="25.5" customHeight="1">
+    <row r="25" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="5">
-        <v>24.0</v>
+        <v>24</v>
       </c>
       <c r="B25" s="6"/>
       <c r="C25" s="5"/>
       <c r="D25" s="6"/>
       <c r="E25" s="6"/>
     </row>
-    <row r="26" ht="25.5" customHeight="1">
+    <row r="26" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="5">
-        <v>25.0</v>
+        <v>25</v>
       </c>
       <c r="B26" s="6"/>
       <c r="C26" s="5"/>
       <c r="D26" s="6"/>
       <c r="E26" s="6"/>
     </row>
-    <row r="27" ht="25.5" customHeight="1">
+    <row r="27" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="5">
-        <v>26.0</v>
+        <v>26</v>
       </c>
       <c r="B27" s="6"/>
       <c r="C27" s="5"/>
       <c r="D27" s="6"/>
       <c r="E27" s="6"/>
     </row>
-    <row r="28" ht="25.5" customHeight="1">
+    <row r="28" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="5">
-        <v>27.0</v>
+        <v>27</v>
       </c>
       <c r="B28" s="6"/>
       <c r="C28" s="5"/>
       <c r="D28" s="6"/>
       <c r="E28" s="6"/>
     </row>
-    <row r="29" ht="25.5" customHeight="1">
+    <row r="29" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="5">
-        <v>28.0</v>
+        <v>28</v>
       </c>
       <c r="B29" s="6"/>
       <c r="C29" s="5"/>
       <c r="D29" s="6"/>
       <c r="E29" s="6"/>
     </row>
-    <row r="30" ht="25.5" customHeight="1">
+    <row r="30" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="5">
-        <v>29.0</v>
+        <v>29</v>
       </c>
       <c r="B30" s="6"/>
       <c r="C30" s="5"/>
       <c r="D30" s="6"/>
       <c r="E30" s="6"/>
     </row>
-    <row r="31" ht="25.5" customHeight="1">
+    <row r="31" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="5">
-        <v>30.0</v>
+        <v>30</v>
       </c>
       <c r="B31" s="6"/>
       <c r="C31" s="5"/>
       <c r="D31" s="6"/>
       <c r="E31" s="6"/>
     </row>
-    <row r="32" ht="25.5" customHeight="1">
+    <row r="32" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="5">
-        <v>31.0</v>
+        <v>31</v>
       </c>
       <c r="B32" s="6"/>
       <c r="C32" s="5"/>
       <c r="D32" s="6"/>
       <c r="E32" s="6"/>
     </row>
-    <row r="33" ht="25.5" customHeight="1">
+    <row r="33" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="5">
-        <v>32.0</v>
+        <v>32</v>
       </c>
       <c r="B33" s="6"/>
       <c r="C33" s="5"/>
       <c r="D33" s="6"/>
       <c r="E33" s="6"/>
     </row>
-    <row r="34" ht="25.5" customHeight="1">
+    <row r="34" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="5">
-        <v>33.0</v>
+        <v>33</v>
       </c>
       <c r="B34" s="6"/>
       <c r="C34" s="5"/>
       <c r="D34" s="6"/>
       <c r="E34" s="6"/>
     </row>
-    <row r="35" ht="25.5" customHeight="1">
+    <row r="35" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="5">
-        <v>34.0</v>
+        <v>34</v>
       </c>
       <c r="B35" s="6"/>
       <c r="C35" s="5"/>
       <c r="D35" s="6"/>
       <c r="E35" s="6"/>
     </row>
-    <row r="36" ht="25.5" customHeight="1">
+    <row r="36" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="5">
-        <v>35.0</v>
+        <v>35</v>
       </c>
       <c r="B36" s="6"/>
       <c r="C36" s="5"/>
       <c r="D36" s="6"/>
       <c r="E36" s="6"/>
     </row>
-    <row r="37" ht="25.5" customHeight="1">
+    <row r="37" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="5">
-        <v>36.0</v>
+        <v>36</v>
       </c>
       <c r="B37" s="6"/>
       <c r="C37" s="5"/>
       <c r="D37" s="6"/>
       <c r="E37" s="6"/>
     </row>
-    <row r="38" ht="25.5" customHeight="1">
+    <row r="38" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="5">
-        <v>37.0</v>
+        <v>37</v>
       </c>
       <c r="B38" s="6"/>
       <c r="C38" s="5"/>
       <c r="D38" s="6"/>
       <c r="E38" s="6"/>
     </row>
-    <row r="39" ht="25.5" customHeight="1">
+    <row r="39" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="5">
-        <v>38.0</v>
+        <v>38</v>
       </c>
       <c r="B39" s="6"/>
       <c r="C39" s="5"/>
       <c r="D39" s="6"/>
       <c r="E39" s="6"/>
     </row>
-    <row r="40" ht="25.5" customHeight="1">
+    <row r="40" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="5">
-        <v>39.0</v>
+        <v>39</v>
       </c>
       <c r="B40" s="6"/>
       <c r="C40" s="5"/>
       <c r="D40" s="6"/>
       <c r="E40" s="6"/>
     </row>
-    <row r="41" ht="25.5" customHeight="1">
+    <row r="41" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="5">
-        <v>40.0</v>
+        <v>40</v>
       </c>
       <c r="B41" s="6"/>
       <c r="C41" s="5"/>
       <c r="D41" s="6"/>
       <c r="E41" s="6"/>
     </row>
-    <row r="42" ht="25.5" customHeight="1">
+    <row r="42" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="5">
-        <v>41.0</v>
+        <v>41</v>
       </c>
       <c r="B42" s="6"/>
       <c r="C42" s="5"/>
       <c r="D42" s="6"/>
       <c r="E42" s="6"/>
     </row>
-    <row r="43" ht="25.5" customHeight="1">
+    <row r="43" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="5">
-        <v>42.0</v>
+        <v>42</v>
       </c>
       <c r="B43" s="6"/>
       <c r="C43" s="5"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
     </row>
-    <row r="44" ht="25.5" customHeight="1">
+    <row r="44" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="5">
-        <v>43.0</v>
+        <v>43</v>
       </c>
       <c r="B44" s="6"/>
       <c r="C44" s="5"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
     </row>
-    <row r="45" ht="25.5" customHeight="1">
+    <row r="45" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="5">
-        <v>44.0</v>
+        <v>44</v>
       </c>
       <c r="B45" s="6"/>
       <c r="C45" s="5"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
     </row>
-    <row r="46" ht="25.5" customHeight="1">
+    <row r="46" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="5">
-        <v>45.0</v>
+        <v>45</v>
       </c>
       <c r="B46" s="6"/>
       <c r="C46" s="5"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
     </row>
-    <row r="47" ht="25.5" customHeight="1">
+    <row r="47" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="5">
-        <v>46.0</v>
+        <v>46</v>
       </c>
       <c r="B47" s="6"/>
       <c r="C47" s="5"/>
       <c r="D47" s="6"/>
       <c r="E47" s="6"/>
     </row>
-    <row r="48" ht="25.5" customHeight="1">
+    <row r="48" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="5">
-        <v>47.0</v>
+        <v>47</v>
       </c>
       <c r="B48" s="6"/>
       <c r="C48" s="5"/>
       <c r="D48" s="6"/>
       <c r="E48" s="6"/>
     </row>
-    <row r="49" ht="25.5" customHeight="1">
+    <row r="49" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="5">
-        <v>48.0</v>
+        <v>48</v>
       </c>
       <c r="B49" s="6"/>
       <c r="C49" s="5"/>
       <c r="D49" s="6"/>
       <c r="E49" s="6"/>
     </row>
-    <row r="50" ht="25.5" customHeight="1">
+    <row r="50" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="5">
-        <v>49.0</v>
+        <v>49</v>
       </c>
       <c r="B50" s="6"/>
       <c r="C50" s="5"/>
       <c r="D50" s="6"/>
       <c r="E50" s="6"/>
     </row>
-    <row r="51" ht="25.5" customHeight="1">
+    <row r="51" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="5">
-        <v>50.0</v>
+        <v>50</v>
       </c>
       <c r="B51" s="6"/>
       <c r="C51" s="5"/>
       <c r="D51" s="6"/>
       <c r="E51" s="6"/>
     </row>
-    <row r="52" ht="25.5" customHeight="1">
+    <row r="52" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="5">
-        <v>51.0</v>
+        <v>51</v>
       </c>
       <c r="B52" s="6"/>
       <c r="C52" s="5"/>
       <c r="D52" s="6"/>
       <c r="E52" s="6"/>
     </row>
-    <row r="53" ht="25.5" customHeight="1">
+    <row r="53" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="5">
-        <v>52.0</v>
+        <v>52</v>
       </c>
       <c r="B53" s="6"/>
       <c r="C53" s="5"/>
       <c r="D53" s="6"/>
       <c r="E53" s="6"/>
     </row>
-    <row r="54" ht="25.5" customHeight="1">
+    <row r="54" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="5">
-        <v>53.0</v>
+        <v>53</v>
       </c>
       <c r="B54" s="6"/>
       <c r="C54" s="5"/>
       <c r="D54" s="6"/>
       <c r="E54" s="6"/>
     </row>
-    <row r="55" ht="25.5" customHeight="1">
+    <row r="55" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="5">
-        <v>54.0</v>
+        <v>54</v>
       </c>
       <c r="B55" s="6"/>
       <c r="C55" s="5"/>
       <c r="D55" s="6"/>
       <c r="E55" s="6"/>
     </row>
-    <row r="56" ht="25.5" customHeight="1">
+    <row r="56" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="5">
-        <v>55.0</v>
+        <v>55</v>
       </c>
       <c r="B56" s="6"/>
       <c r="C56" s="5"/>
       <c r="D56" s="6"/>
       <c r="E56" s="6"/>
     </row>
-    <row r="57" ht="25.5" customHeight="1">
+    <row r="57" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="5">
-        <v>56.0</v>
+        <v>56</v>
       </c>
       <c r="B57" s="6"/>
       <c r="C57" s="5"/>
       <c r="D57" s="6"/>
       <c r="E57" s="6"/>
     </row>
-    <row r="58" ht="25.5" customHeight="1">
+    <row r="58" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="5">
-        <v>57.0</v>
+        <v>57</v>
       </c>
       <c r="B58" s="6"/>
       <c r="C58" s="5"/>
       <c r="D58" s="6"/>
       <c r="E58" s="6"/>
     </row>
-    <row r="59" ht="25.5" customHeight="1">
+    <row r="59" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="5">
-        <v>58.0</v>
+        <v>58</v>
       </c>
       <c r="B59" s="6"/>
       <c r="C59" s="5"/>
       <c r="D59" s="6"/>
       <c r="E59" s="6"/>
     </row>
-    <row r="60" ht="25.5" customHeight="1">
+    <row r="60" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="5">
-        <v>59.0</v>
+        <v>59</v>
       </c>
       <c r="B60" s="6"/>
       <c r="C60" s="5"/>
       <c r="D60" s="6"/>
       <c r="E60" s="6"/>
     </row>
-    <row r="61" ht="15.75" customHeight="1">
+    <row r="61" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="13"/>
       <c r="B61" s="14"/>
       <c r="C61" s="13"/>
       <c r="D61" s="14"/>
       <c r="E61" s="14"/>
     </row>
-    <row r="62" ht="15.75" customHeight="1">
+    <row r="62" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="13"/>
       <c r="B62" s="14"/>
       <c r="C62" s="13"/>
       <c r="D62" s="14"/>
       <c r="E62" s="14"/>
     </row>
-    <row r="63" ht="15.75" customHeight="1">
+    <row r="63" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="13"/>
       <c r="B63" s="14"/>
       <c r="C63" s="13"/>
       <c r="D63" s="14"/>
       <c r="E63" s="14"/>
     </row>
-    <row r="64" ht="15.75" customHeight="1">
+    <row r="64" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="13"/>
       <c r="B64" s="14"/>
       <c r="C64" s="13"/>
       <c r="D64" s="14"/>
       <c r="E64" s="14"/>
     </row>
-    <row r="65" ht="15.75" customHeight="1">
+    <row r="65" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="13"/>
       <c r="B65" s="14"/>
       <c r="C65" s="13"/>
       <c r="D65" s="14"/>
       <c r="E65" s="14"/>
     </row>
-    <row r="66" ht="15.75" customHeight="1">
+    <row r="66" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="13"/>
       <c r="B66" s="14"/>
       <c r="C66" s="13"/>
       <c r="D66" s="14"/>
       <c r="E66" s="14"/>
     </row>
-    <row r="67" ht="15.75" customHeight="1">
+    <row r="67" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="13"/>
       <c r="B67" s="14"/>
       <c r="C67" s="13"/>
       <c r="D67" s="14"/>
       <c r="E67" s="14"/>
     </row>
-    <row r="68" ht="15.75" customHeight="1">
+    <row r="68" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="13"/>
       <c r="B68" s="14"/>
       <c r="C68" s="13"/>
       <c r="D68" s="14"/>
       <c r="E68" s="14"/>
     </row>
-    <row r="69" ht="15.75" customHeight="1">
+    <row r="69" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="13"/>
       <c r="B69" s="14"/>
       <c r="C69" s="13"/>
       <c r="D69" s="14"/>
       <c r="E69" s="14"/>
     </row>
-    <row r="70" ht="15.75" customHeight="1">
+    <row r="70" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="13"/>
       <c r="B70" s="14"/>
       <c r="C70" s="13"/>
       <c r="D70" s="14"/>
       <c r="E70" s="14"/>
     </row>
-    <row r="71" ht="15.75" customHeight="1">
+    <row r="71" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="13"/>
       <c r="B71" s="14"/>
       <c r="C71" s="13"/>
       <c r="D71" s="14"/>
       <c r="E71" s="14"/>
     </row>
-    <row r="72" ht="15.75" customHeight="1">
+    <row r="72" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="13"/>
       <c r="B72" s="14"/>
       <c r="C72" s="13"/>
       <c r="D72" s="14"/>
       <c r="E72" s="14"/>
     </row>
-    <row r="73" ht="15.75" customHeight="1">
+    <row r="73" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="13"/>
       <c r="B73" s="14"/>
       <c r="C73" s="13"/>
       <c r="D73" s="14"/>
       <c r="E73" s="14"/>
     </row>
-    <row r="74" ht="15.75" customHeight="1">
+    <row r="74" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="13"/>
       <c r="B74" s="14"/>
       <c r="C74" s="13"/>
       <c r="D74" s="14"/>
       <c r="E74" s="14"/>
     </row>
-    <row r="75" ht="15.75" customHeight="1">
+    <row r="75" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="13"/>
       <c r="B75" s="14"/>
       <c r="C75" s="13"/>
       <c r="D75" s="14"/>
       <c r="E75" s="14"/>
     </row>
-    <row r="76" ht="15.75" customHeight="1">
+    <row r="76" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="13"/>
       <c r="B76" s="14"/>
       <c r="C76" s="13"/>
       <c r="D76" s="14"/>
       <c r="E76" s="14"/>
     </row>
-    <row r="77" ht="15.75" customHeight="1">
+    <row r="77" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="13"/>
       <c r="B77" s="14"/>
       <c r="C77" s="13"/>
       <c r="D77" s="14"/>
       <c r="E77" s="14"/>
     </row>
-    <row r="78" ht="15.75" customHeight="1">
+    <row r="78" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="13"/>
       <c r="B78" s="14"/>
       <c r="C78" s="13"/>
       <c r="D78" s="14"/>
       <c r="E78" s="14"/>
     </row>
-    <row r="79" ht="15.75" customHeight="1">
+    <row r="79" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="13"/>
       <c r="B79" s="14"/>
       <c r="C79" s="13"/>
       <c r="D79" s="14"/>
       <c r="E79" s="14"/>
     </row>
-    <row r="80" ht="15.75" customHeight="1">
+    <row r="80" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="13"/>
       <c r="B80" s="14"/>
       <c r="C80" s="13"/>
       <c r="D80" s="14"/>
       <c r="E80" s="14"/>
     </row>
-    <row r="81" ht="15.75" customHeight="1">
+    <row r="81" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="13"/>
       <c r="B81" s="14"/>
       <c r="C81" s="13"/>
       <c r="D81" s="14"/>
       <c r="E81" s="14"/>
     </row>
-    <row r="82" ht="15.75" customHeight="1">
+    <row r="82" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="13"/>
       <c r="B82" s="14"/>
       <c r="C82" s="13"/>
       <c r="D82" s="14"/>
       <c r="E82" s="14"/>
     </row>
-    <row r="83" ht="15.75" customHeight="1">
+    <row r="83" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="13"/>
       <c r="B83" s="14"/>
       <c r="C83" s="13"/>
       <c r="D83" s="14"/>
       <c r="E83" s="14"/>
     </row>
-    <row r="84" ht="15.75" customHeight="1">
+    <row r="84" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="13"/>
       <c r="B84" s="14"/>
       <c r="C84" s="13"/>
       <c r="D84" s="14"/>
       <c r="E84" s="14"/>
     </row>
-    <row r="85" ht="15.75" customHeight="1">
+    <row r="85" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="13"/>
       <c r="B85" s="14"/>
       <c r="C85" s="13"/>
       <c r="D85" s="14"/>
       <c r="E85" s="14"/>
     </row>
-    <row r="86" ht="15.75" customHeight="1">
+    <row r="86" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="13"/>
       <c r="B86" s="14"/>
       <c r="C86" s="13"/>
       <c r="D86" s="14"/>
       <c r="E86" s="14"/>
     </row>
-    <row r="87" ht="15.75" customHeight="1">
+    <row r="87" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="13"/>
       <c r="B87" s="14"/>
       <c r="C87" s="13"/>
       <c r="D87" s="14"/>
       <c r="E87" s="14"/>
     </row>
-    <row r="88" ht="15.75" customHeight="1">
+    <row r="88" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="13"/>
       <c r="B88" s="14"/>
       <c r="C88" s="13"/>
       <c r="D88" s="14"/>
       <c r="E88" s="14"/>
     </row>
-    <row r="89" ht="15.75" customHeight="1">
+    <row r="89" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="13"/>
       <c r="B89" s="14"/>
       <c r="C89" s="13"/>
       <c r="D89" s="14"/>
       <c r="E89" s="14"/>
     </row>
-    <row r="90" ht="15.75" customHeight="1">
+    <row r="90" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="13"/>
       <c r="B90" s="14"/>
       <c r="C90" s="13"/>
       <c r="D90" s="14"/>
       <c r="E90" s="14"/>
     </row>
-    <row r="91" ht="15.75" customHeight="1">
+    <row r="91" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="13"/>
       <c r="B91" s="14"/>
       <c r="C91" s="13"/>
       <c r="D91" s="14"/>
       <c r="E91" s="14"/>
     </row>
-    <row r="92" ht="15.75" customHeight="1">
+    <row r="92" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="13"/>
       <c r="B92" s="14"/>
       <c r="C92" s="13"/>
       <c r="D92" s="14"/>
       <c r="E92" s="14"/>
     </row>
-    <row r="93" ht="15.75" customHeight="1">
+    <row r="93" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="13"/>
       <c r="B93" s="14"/>
       <c r="C93" s="13"/>
       <c r="D93" s="14"/>
       <c r="E93" s="14"/>
     </row>
-    <row r="94" ht="15.75" customHeight="1">
+    <row r="94" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="13"/>
       <c r="B94" s="14"/>
       <c r="C94" s="13"/>
       <c r="D94" s="14"/>
       <c r="E94" s="14"/>
     </row>
-    <row r="95" ht="15.75" customHeight="1">
+    <row r="95" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="13"/>
       <c r="B95" s="14"/>
       <c r="C95" s="13"/>
       <c r="D95" s="14"/>
       <c r="E95" s="14"/>
     </row>
-    <row r="96" ht="15.75" customHeight="1">
+    <row r="96" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="13"/>
       <c r="B96" s="14"/>
       <c r="C96" s="13"/>
       <c r="D96" s="14"/>
       <c r="E96" s="14"/>
     </row>
-    <row r="97" ht="15.75" customHeight="1">
+    <row r="97" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="13"/>
       <c r="B97" s="14"/>
       <c r="C97" s="13"/>
       <c r="D97" s="14"/>
       <c r="E97" s="14"/>
     </row>
-    <row r="98" ht="15.75" customHeight="1">
+    <row r="98" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="13"/>
       <c r="B98" s="14"/>
       <c r="C98" s="13"/>
       <c r="D98" s="14"/>
       <c r="E98" s="14"/>
     </row>
-    <row r="99" ht="15.75" customHeight="1">
+    <row r="99" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="13"/>
       <c r="B99" s="14"/>
       <c r="C99" s="13"/>
       <c r="D99" s="14"/>
       <c r="E99" s="14"/>
     </row>
-    <row r="100" ht="15.75" customHeight="1">
+    <row r="100" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="13"/>
       <c r="B100" s="14"/>
       <c r="C100" s="13"/>
       <c r="D100" s="14"/>
       <c r="E100" s="14"/>
     </row>
-    <row r="101" ht="15.75" customHeight="1">
+    <row r="101" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="13"/>
       <c r="B101" s="14"/>
       <c r="C101" s="13"/>
       <c r="D101" s="14"/>
       <c r="E101" s="14"/>
     </row>
-    <row r="102" ht="15.75" customHeight="1">
+    <row r="102" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="13"/>
       <c r="B102" s="14"/>
       <c r="C102" s="13"/>
       <c r="D102" s="14"/>
       <c r="E102" s="14"/>
     </row>
-    <row r="103" ht="15.75" customHeight="1">
+    <row r="103" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" s="13"/>
       <c r="B103" s="14"/>
       <c r="C103" s="13"/>
       <c r="D103" s="14"/>
       <c r="E103" s="14"/>
     </row>
-    <row r="104" ht="15.75" customHeight="1">
+    <row r="104" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="13"/>
       <c r="B104" s="14"/>
       <c r="C104" s="13"/>
       <c r="D104" s="14"/>
       <c r="E104" s="14"/>
     </row>
-    <row r="105" ht="15.75" customHeight="1">
+    <row r="105" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" s="13"/>
       <c r="B105" s="14"/>
       <c r="C105" s="13"/>
       <c r="D105" s="14"/>
       <c r="E105" s="14"/>
     </row>
-    <row r="106" ht="15.75" customHeight="1">
+    <row r="106" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="13"/>
       <c r="B106" s="14"/>
       <c r="C106" s="13"/>
       <c r="D106" s="14"/>
       <c r="E106" s="14"/>
     </row>
-    <row r="107" ht="15.75" customHeight="1">
+    <row r="107" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" s="13"/>
       <c r="B107" s="14"/>
       <c r="C107" s="13"/>
       <c r="D107" s="14"/>
       <c r="E107" s="14"/>
     </row>
-    <row r="108" ht="15.75" customHeight="1">
+    <row r="108" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" s="13"/>
       <c r="B108" s="14"/>
       <c r="C108" s="13"/>
       <c r="D108" s="14"/>
       <c r="E108" s="14"/>
     </row>
-    <row r="109" ht="15.75" customHeight="1">
+    <row r="109" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" s="13"/>
       <c r="B109" s="14"/>
       <c r="C109" s="13"/>
       <c r="D109" s="14"/>
       <c r="E109" s="14"/>
     </row>
-    <row r="110" ht="15.75" customHeight="1">
+    <row r="110" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" s="13"/>
       <c r="B110" s="14"/>
       <c r="C110" s="13"/>
       <c r="D110" s="14"/>
       <c r="E110" s="14"/>
     </row>
-    <row r="111" ht="15.75" customHeight="1">
+    <row r="111" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" s="13"/>
       <c r="B111" s="14"/>
       <c r="C111" s="13"/>
       <c r="D111" s="14"/>
       <c r="E111" s="14"/>
     </row>
-    <row r="112" ht="15.75" customHeight="1">
+    <row r="112" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" s="13"/>
       <c r="B112" s="14"/>
       <c r="C112" s="13"/>
       <c r="D112" s="14"/>
       <c r="E112" s="14"/>
     </row>
-    <row r="113" ht="15.75" customHeight="1">
+    <row r="113" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" s="13"/>
       <c r="B113" s="14"/>
       <c r="C113" s="13"/>
       <c r="D113" s="14"/>
       <c r="E113" s="14"/>
     </row>
-    <row r="114" ht="15.75" customHeight="1">
+    <row r="114" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A114" s="13"/>
       <c r="B114" s="14"/>
       <c r="C114" s="13"/>
       <c r="D114" s="14"/>
       <c r="E114" s="14"/>
     </row>
-    <row r="115" ht="15.75" customHeight="1">
+    <row r="115" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A115" s="13"/>
       <c r="B115" s="14"/>
       <c r="C115" s="13"/>
       <c r="D115" s="14"/>
       <c r="E115" s="14"/>
     </row>
-    <row r="116" ht="15.75" customHeight="1">
+    <row r="116" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A116" s="13"/>
       <c r="B116" s="14"/>
       <c r="C116" s="13"/>
       <c r="D116" s="14"/>
       <c r="E116" s="14"/>
     </row>
-    <row r="117" ht="15.75" customHeight="1">
+    <row r="117" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A117" s="13"/>
       <c r="B117" s="14"/>
       <c r="C117" s="13"/>
       <c r="D117" s="14"/>
       <c r="E117" s="14"/>
     </row>
-    <row r="118" ht="15.75" customHeight="1">
+    <row r="118" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A118" s="13"/>
       <c r="B118" s="14"/>
       <c r="C118" s="13"/>
       <c r="D118" s="14"/>
       <c r="E118" s="14"/>
     </row>
-    <row r="119" ht="15.75" customHeight="1">
+    <row r="119" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A119" s="13"/>
       <c r="B119" s="14"/>
       <c r="C119" s="13"/>
       <c r="D119" s="14"/>
       <c r="E119" s="14"/>
     </row>
-    <row r="120" ht="15.75" customHeight="1">
+    <row r="120" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A120" s="13"/>
       <c r="B120" s="14"/>
       <c r="C120" s="13"/>
       <c r="D120" s="14"/>
       <c r="E120" s="14"/>
     </row>
-    <row r="121" ht="15.75" customHeight="1">
+    <row r="121" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A121" s="13"/>
       <c r="B121" s="14"/>
       <c r="C121" s="13"/>
       <c r="D121" s="14"/>
       <c r="E121" s="14"/>
     </row>
-    <row r="122" ht="15.75" customHeight="1">
+    <row r="122" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A122" s="13"/>
       <c r="B122" s="14"/>
       <c r="C122" s="13"/>
       <c r="D122" s="14"/>
       <c r="E122" s="14"/>
     </row>
-    <row r="123" ht="15.75" customHeight="1">
+    <row r="123" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A123" s="13"/>
       <c r="B123" s="14"/>
       <c r="C123" s="13"/>
       <c r="D123" s="14"/>
       <c r="E123" s="14"/>
     </row>
-    <row r="124" ht="15.75" customHeight="1">
+    <row r="124" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A124" s="13"/>
       <c r="B124" s="14"/>
       <c r="C124" s="13"/>
       <c r="D124" s="14"/>
       <c r="E124" s="14"/>
     </row>
-    <row r="125" ht="15.75" customHeight="1">
+    <row r="125" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A125" s="13"/>
       <c r="B125" s="14"/>
       <c r="C125" s="13"/>
       <c r="D125" s="14"/>
       <c r="E125" s="14"/>
     </row>
-    <row r="126" ht="15.75" customHeight="1">
+    <row r="126" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A126" s="13"/>
       <c r="B126" s="14"/>
       <c r="C126" s="13"/>
       <c r="D126" s="14"/>
       <c r="E126" s="14"/>
     </row>
-    <row r="127" ht="15.75" customHeight="1">
+    <row r="127" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A127" s="13"/>
       <c r="B127" s="14"/>
       <c r="C127" s="13"/>
       <c r="D127" s="14"/>
       <c r="E127" s="14"/>
     </row>
-    <row r="128" ht="15.75" customHeight="1">
+    <row r="128" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A128" s="13"/>
       <c r="B128" s="14"/>
       <c r="C128" s="13"/>
       <c r="D128" s="14"/>
       <c r="E128" s="14"/>
     </row>
-    <row r="129" ht="15.75" customHeight="1">
+    <row r="129" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A129" s="13"/>
       <c r="B129" s="14"/>
       <c r="C129" s="13"/>
       <c r="D129" s="14"/>
       <c r="E129" s="14"/>
     </row>
-    <row r="130" ht="15.75" customHeight="1">
+    <row r="130" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A130" s="13"/>
       <c r="B130" s="14"/>
       <c r="C130" s="13"/>
       <c r="D130" s="14"/>
       <c r="E130" s="14"/>
     </row>
-    <row r="131" ht="15.75" customHeight="1">
+    <row r="131" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A131" s="13"/>
       <c r="B131" s="14"/>
       <c r="C131" s="13"/>
       <c r="D131" s="14"/>
       <c r="E131" s="14"/>
     </row>
-    <row r="132" ht="15.75" customHeight="1">
+    <row r="132" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A132" s="13"/>
       <c r="B132" s="14"/>
       <c r="C132" s="13"/>
       <c r="D132" s="14"/>
       <c r="E132" s="14"/>
     </row>
-    <row r="133" ht="15.75" customHeight="1">
+    <row r="133" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A133" s="13"/>
       <c r="B133" s="14"/>
       <c r="C133" s="13"/>
       <c r="D133" s="14"/>
       <c r="E133" s="14"/>
     </row>
-    <row r="134" ht="15.75" customHeight="1">
+    <row r="134" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A134" s="13"/>
       <c r="B134" s="14"/>
       <c r="C134" s="13"/>
       <c r="D134" s="14"/>
       <c r="E134" s="14"/>
     </row>
-    <row r="135" ht="15.75" customHeight="1">
+    <row r="135" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A135" s="13"/>
       <c r="B135" s="14"/>
       <c r="C135" s="13"/>
       <c r="D135" s="14"/>
       <c r="E135" s="14"/>
     </row>
-    <row r="136" ht="15.75" customHeight="1">
+    <row r="136" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A136" s="13"/>
       <c r="B136" s="14"/>
       <c r="C136" s="13"/>
       <c r="D136" s="14"/>
       <c r="E136" s="14"/>
     </row>
-    <row r="137" ht="15.75" customHeight="1">
+    <row r="137" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A137" s="13"/>
       <c r="B137" s="14"/>
       <c r="C137" s="13"/>
       <c r="D137" s="14"/>
       <c r="E137" s="14"/>
     </row>
-    <row r="138" ht="15.75" customHeight="1">
+    <row r="138" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A138" s="13"/>
       <c r="B138" s="14"/>
       <c r="C138" s="13"/>
       <c r="D138" s="14"/>
       <c r="E138" s="14"/>
     </row>
-    <row r="139" ht="15.75" customHeight="1">
+    <row r="139" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A139" s="13"/>
       <c r="B139" s="14"/>
       <c r="C139" s="13"/>
       <c r="D139" s="14"/>
       <c r="E139" s="14"/>
     </row>
-    <row r="140" ht="15.75" customHeight="1">
+    <row r="140" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A140" s="13"/>
       <c r="B140" s="14"/>
       <c r="C140" s="13"/>
       <c r="D140" s="14"/>
       <c r="E140" s="14"/>
     </row>
-    <row r="141" ht="15.75" customHeight="1">
+    <row r="141" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A141" s="13"/>
       <c r="B141" s="14"/>
       <c r="C141" s="13"/>
       <c r="D141" s="14"/>
       <c r="E141" s="14"/>
     </row>
-    <row r="142" ht="15.75" customHeight="1">
+    <row r="142" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A142" s="13"/>
       <c r="B142" s="14"/>
       <c r="C142" s="13"/>
       <c r="D142" s="14"/>
       <c r="E142" s="14"/>
     </row>
-    <row r="143" ht="15.75" customHeight="1">
+    <row r="143" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A143" s="13"/>
       <c r="B143" s="14"/>
       <c r="C143" s="13"/>
       <c r="D143" s="14"/>
       <c r="E143" s="14"/>
     </row>
-    <row r="144" ht="15.75" customHeight="1">
+    <row r="144" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A144" s="13"/>
       <c r="B144" s="14"/>
       <c r="C144" s="13"/>
       <c r="D144" s="14"/>
       <c r="E144" s="14"/>
     </row>
-    <row r="145" ht="15.75" customHeight="1">
+    <row r="145" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A145" s="13"/>
       <c r="B145" s="14"/>
       <c r="C145" s="13"/>
       <c r="D145" s="14"/>
       <c r="E145" s="14"/>
     </row>
-    <row r="146" ht="15.75" customHeight="1">
+    <row r="146" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A146" s="13"/>
       <c r="B146" s="14"/>
       <c r="C146" s="13"/>
       <c r="D146" s="14"/>
       <c r="E146" s="14"/>
     </row>
-    <row r="147" ht="15.75" customHeight="1">
+    <row r="147" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A147" s="13"/>
       <c r="B147" s="14"/>
       <c r="C147" s="13"/>
       <c r="D147" s="14"/>
       <c r="E147" s="14"/>
     </row>
-    <row r="148" ht="15.75" customHeight="1">
+    <row r="148" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A148" s="13"/>
       <c r="B148" s="14"/>
       <c r="C148" s="13"/>
       <c r="D148" s="14"/>
       <c r="E148" s="14"/>
     </row>
-    <row r="149" ht="15.75" customHeight="1">
+    <row r="149" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A149" s="13"/>
       <c r="B149" s="14"/>
       <c r="C149" s="13"/>
       <c r="D149" s="14"/>
       <c r="E149" s="14"/>
     </row>
-    <row r="150" ht="15.75" customHeight="1">
+    <row r="150" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A150" s="13"/>
       <c r="B150" s="14"/>
       <c r="C150" s="13"/>
       <c r="D150" s="14"/>
       <c r="E150" s="14"/>
     </row>
-    <row r="151" ht="15.75" customHeight="1">
+    <row r="151" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A151" s="13"/>
       <c r="B151" s="14"/>
       <c r="C151" s="13"/>
       <c r="D151" s="14"/>
       <c r="E151" s="14"/>
     </row>
-    <row r="152" ht="15.75" customHeight="1">
+    <row r="152" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A152" s="13"/>
       <c r="B152" s="14"/>
       <c r="C152" s="13"/>
       <c r="D152" s="14"/>
       <c r="E152" s="14"/>
     </row>
-    <row r="153" ht="15.75" customHeight="1">
+    <row r="153" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A153" s="13"/>
       <c r="B153" s="14"/>
       <c r="C153" s="13"/>
       <c r="D153" s="14"/>
       <c r="E153" s="14"/>
     </row>
-    <row r="154" ht="15.75" customHeight="1">
+    <row r="154" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A154" s="13"/>
       <c r="B154" s="14"/>
       <c r="C154" s="13"/>
       <c r="D154" s="14"/>
       <c r="E154" s="14"/>
     </row>
-    <row r="155" ht="15.75" customHeight="1">
+    <row r="155" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A155" s="13"/>
       <c r="B155" s="14"/>
       <c r="C155" s="13"/>
       <c r="D155" s="14"/>
       <c r="E155" s="14"/>
     </row>
-    <row r="156" ht="15.75" customHeight="1">
+    <row r="156" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A156" s="13"/>
       <c r="B156" s="14"/>
       <c r="C156" s="13"/>
       <c r="D156" s="14"/>
       <c r="E156" s="14"/>
     </row>
-    <row r="157" ht="15.75" customHeight="1">
+    <row r="157" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A157" s="13"/>
       <c r="B157" s="14"/>
       <c r="C157" s="13"/>
       <c r="D157" s="14"/>
       <c r="E157" s="14"/>
     </row>
-    <row r="158" ht="15.75" customHeight="1">
+    <row r="158" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A158" s="13"/>
       <c r="B158" s="14"/>
       <c r="C158" s="13"/>
       <c r="D158" s="14"/>
       <c r="E158" s="14"/>
     </row>
-    <row r="159" ht="15.75" customHeight="1">
+    <row r="159" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A159" s="13"/>
       <c r="B159" s="14"/>
       <c r="C159" s="13"/>
       <c r="D159" s="14"/>
       <c r="E159" s="14"/>
     </row>
-    <row r="160" ht="15.75" customHeight="1">
+    <row r="160" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A160" s="13"/>
       <c r="B160" s="14"/>
       <c r="C160" s="13"/>
       <c r="D160" s="14"/>
       <c r="E160" s="14"/>
     </row>
-    <row r="161" ht="15.75" customHeight="1">
+    <row r="161" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A161" s="13"/>
       <c r="B161" s="14"/>
       <c r="C161" s="13"/>
       <c r="D161" s="14"/>
       <c r="E161" s="14"/>
     </row>
-    <row r="162" ht="15.75" customHeight="1">
+    <row r="162" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A162" s="13"/>
       <c r="B162" s="14"/>
       <c r="C162" s="13"/>
       <c r="D162" s="14"/>
       <c r="E162" s="14"/>
     </row>
-    <row r="163" ht="15.75" customHeight="1">
+    <row r="163" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A163" s="13"/>
       <c r="B163" s="14"/>
       <c r="C163" s="13"/>
       <c r="D163" s="14"/>
       <c r="E163" s="14"/>
     </row>
-    <row r="164" ht="15.75" customHeight="1">
+    <row r="164" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A164" s="13"/>
       <c r="B164" s="14"/>
       <c r="C164" s="13"/>
       <c r="D164" s="14"/>
       <c r="E164" s="14"/>
     </row>
-    <row r="165" ht="15.75" customHeight="1">
+    <row r="165" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A165" s="13"/>
       <c r="B165" s="14"/>
       <c r="C165" s="13"/>
       <c r="D165" s="14"/>
       <c r="E165" s="14"/>
     </row>
-    <row r="166" ht="15.75" customHeight="1">
+    <row r="166" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A166" s="13"/>
       <c r="B166" s="14"/>
       <c r="C166" s="13"/>
       <c r="D166" s="14"/>
       <c r="E166" s="14"/>
     </row>
-    <row r="167" ht="15.75" customHeight="1">
+    <row r="167" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A167" s="13"/>
       <c r="B167" s="14"/>
       <c r="C167" s="13"/>
       <c r="D167" s="14"/>
       <c r="E167" s="14"/>
     </row>
-    <row r="168" ht="15.75" customHeight="1">
+    <row r="168" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A168" s="13"/>
       <c r="B168" s="14"/>
       <c r="C168" s="13"/>
       <c r="D168" s="14"/>
       <c r="E168" s="14"/>
     </row>
-    <row r="169" ht="15.75" customHeight="1">
+    <row r="169" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A169" s="13"/>
       <c r="B169" s="14"/>
       <c r="C169" s="13"/>
       <c r="D169" s="14"/>
       <c r="E169" s="14"/>
     </row>
-    <row r="170" ht="15.75" customHeight="1">
+    <row r="170" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A170" s="13"/>
       <c r="B170" s="14"/>
       <c r="C170" s="13"/>
       <c r="D170" s="14"/>
       <c r="E170" s="14"/>
     </row>
-    <row r="171" ht="15.75" customHeight="1">
+    <row r="171" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A171" s="13"/>
       <c r="B171" s="14"/>
       <c r="C171" s="13"/>
       <c r="D171" s="14"/>
       <c r="E171" s="14"/>
     </row>
-    <row r="172" ht="15.75" customHeight="1">
+    <row r="172" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A172" s="13"/>
       <c r="B172" s="14"/>
       <c r="C172" s="13"/>
       <c r="D172" s="14"/>
       <c r="E172" s="14"/>
     </row>
-    <row r="173" ht="15.75" customHeight="1">
+    <row r="173" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A173" s="13"/>
       <c r="B173" s="14"/>
       <c r="C173" s="13"/>
       <c r="D173" s="14"/>
       <c r="E173" s="14"/>
     </row>
-    <row r="174" ht="15.75" customHeight="1">
+    <row r="174" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A174" s="13"/>
       <c r="B174" s="14"/>
       <c r="C174" s="13"/>
       <c r="D174" s="14"/>
       <c r="E174" s="14"/>
     </row>
-    <row r="175" ht="15.75" customHeight="1">
+    <row r="175" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A175" s="13"/>
       <c r="B175" s="14"/>
       <c r="C175" s="13"/>
       <c r="D175" s="14"/>
       <c r="E175" s="14"/>
     </row>
-    <row r="176" ht="15.75" customHeight="1">
+    <row r="176" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A176" s="13"/>
       <c r="B176" s="14"/>
       <c r="C176" s="13"/>
       <c r="D176" s="14"/>
       <c r="E176" s="14"/>
     </row>
-    <row r="177" ht="15.75" customHeight="1">
+    <row r="177" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A177" s="13"/>
       <c r="B177" s="14"/>
       <c r="C177" s="13"/>
       <c r="D177" s="14"/>
       <c r="E177" s="14"/>
     </row>
-    <row r="178" ht="15.75" customHeight="1">
+    <row r="178" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A178" s="13"/>
       <c r="B178" s="14"/>
       <c r="C178" s="13"/>
       <c r="D178" s="14"/>
       <c r="E178" s="14"/>
     </row>
-    <row r="179" ht="15.75" customHeight="1">
+    <row r="179" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A179" s="13"/>
       <c r="B179" s="14"/>
       <c r="C179" s="13"/>
       <c r="D179" s="14"/>
       <c r="E179" s="14"/>
     </row>
-    <row r="180" ht="15.75" customHeight="1">
+    <row r="180" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A180" s="13"/>
       <c r="B180" s="14"/>
       <c r="C180" s="13"/>
       <c r="D180" s="14"/>
       <c r="E180" s="14"/>
     </row>
-    <row r="181" ht="15.75" customHeight="1">
+    <row r="181" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A181" s="13"/>
       <c r="B181" s="14"/>
       <c r="C181" s="13"/>
       <c r="D181" s="14"/>
       <c r="E181" s="14"/>
     </row>
-    <row r="182" ht="15.75" customHeight="1">
+    <row r="182" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A182" s="13"/>
       <c r="B182" s="14"/>
       <c r="C182" s="13"/>
       <c r="D182" s="14"/>
       <c r="E182" s="14"/>
     </row>
-    <row r="183" ht="15.75" customHeight="1">
+    <row r="183" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A183" s="13"/>
       <c r="B183" s="14"/>
       <c r="C183" s="13"/>
       <c r="D183" s="14"/>
       <c r="E183" s="14"/>
     </row>
-    <row r="184" ht="15.75" customHeight="1">
+    <row r="184" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A184" s="13"/>
       <c r="B184" s="14"/>
       <c r="C184" s="13"/>
       <c r="D184" s="14"/>
       <c r="E184" s="14"/>
     </row>
-    <row r="185" ht="15.75" customHeight="1">
+    <row r="185" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A185" s="13"/>
       <c r="B185" s="14"/>
       <c r="C185" s="13"/>
       <c r="D185" s="14"/>
       <c r="E185" s="14"/>
     </row>
-    <row r="186" ht="15.75" customHeight="1">
+    <row r="186" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A186" s="13"/>
       <c r="B186" s="14"/>
       <c r="C186" s="13"/>
       <c r="D186" s="14"/>
       <c r="E186" s="14"/>
     </row>
-    <row r="187" ht="15.75" customHeight="1">
+    <row r="187" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A187" s="13"/>
       <c r="B187" s="14"/>
       <c r="C187" s="13"/>
       <c r="D187" s="14"/>
       <c r="E187" s="14"/>
     </row>
-    <row r="188" ht="15.75" customHeight="1">
+    <row r="188" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A188" s="13"/>
       <c r="B188" s="14"/>
       <c r="C188" s="13"/>
       <c r="D188" s="14"/>
       <c r="E188" s="14"/>
     </row>
-    <row r="189" ht="15.75" customHeight="1">
+    <row r="189" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A189" s="13"/>
       <c r="B189" s="14"/>
       <c r="C189" s="13"/>
       <c r="D189" s="14"/>
       <c r="E189" s="14"/>
     </row>
-    <row r="190" ht="15.75" customHeight="1">
+    <row r="190" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A190" s="13"/>
       <c r="B190" s="14"/>
       <c r="C190" s="13"/>
       <c r="D190" s="14"/>
       <c r="E190" s="14"/>
     </row>
-    <row r="191" ht="15.75" customHeight="1">
+    <row r="191" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A191" s="13"/>
       <c r="B191" s="14"/>
       <c r="C191" s="13"/>
       <c r="D191" s="14"/>
       <c r="E191" s="14"/>
     </row>
-    <row r="192" ht="15.75" customHeight="1">
+    <row r="192" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A192" s="13"/>
       <c r="B192" s="14"/>
       <c r="C192" s="13"/>
       <c r="D192" s="14"/>
       <c r="E192" s="14"/>
     </row>
-    <row r="193" ht="15.75" customHeight="1">
+    <row r="193" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A193" s="13"/>
       <c r="B193" s="14"/>
       <c r="C193" s="13"/>
       <c r="D193" s="14"/>
       <c r="E193" s="14"/>
     </row>
-    <row r="194" ht="15.75" customHeight="1">
+    <row r="194" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A194" s="13"/>
       <c r="B194" s="14"/>
       <c r="C194" s="13"/>
       <c r="D194" s="14"/>
       <c r="E194" s="14"/>
     </row>
-    <row r="195" ht="15.75" customHeight="1">
+    <row r="195" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A195" s="13"/>
       <c r="B195" s="14"/>
       <c r="C195" s="13"/>
       <c r="D195" s="14"/>
       <c r="E195" s="14"/>
     </row>
-    <row r="196" ht="15.75" customHeight="1">
+    <row r="196" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A196" s="13"/>
       <c r="B196" s="14"/>
       <c r="C196" s="13"/>
       <c r="D196" s="14"/>
       <c r="E196" s="14"/>
     </row>
-    <row r="197" ht="15.75" customHeight="1">
+    <row r="197" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A197" s="13"/>
       <c r="B197" s="14"/>
       <c r="C197" s="13"/>
       <c r="D197" s="14"/>
       <c r="E197" s="14"/>
     </row>
-    <row r="198" ht="15.75" customHeight="1">
+    <row r="198" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A198" s="13"/>
       <c r="B198" s="14"/>
       <c r="C198" s="13"/>
       <c r="D198" s="14"/>
       <c r="E198" s="14"/>
     </row>
-    <row r="199" ht="15.75" customHeight="1">
+    <row r="199" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A199" s="13"/>
       <c r="B199" s="14"/>
       <c r="C199" s="13"/>
       <c r="D199" s="14"/>
       <c r="E199" s="14"/>
     </row>
-    <row r="200" ht="15.75" customHeight="1">
+    <row r="200" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A200" s="13"/>
       <c r="B200" s="14"/>
       <c r="C200" s="13"/>
       <c r="D200" s="14"/>
       <c r="E200" s="14"/>
     </row>
-    <row r="201" ht="15.75" customHeight="1">
+    <row r="201" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A201" s="13"/>
       <c r="B201" s="14"/>
       <c r="C201" s="13"/>
       <c r="D201" s="14"/>
       <c r="E201" s="14"/>
     </row>
-    <row r="202" ht="15.75" customHeight="1">
+    <row r="202" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A202" s="13"/>
       <c r="B202" s="14"/>
       <c r="C202" s="13"/>
       <c r="D202" s="14"/>
       <c r="E202" s="14"/>
     </row>
-    <row r="203" ht="15.75" customHeight="1">
+    <row r="203" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A203" s="13"/>
       <c r="B203" s="14"/>
       <c r="C203" s="13"/>
       <c r="D203" s="14"/>
       <c r="E203" s="14"/>
     </row>
-    <row r="204" ht="15.75" customHeight="1">
+    <row r="204" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A204" s="13"/>
       <c r="B204" s="14"/>
       <c r="C204" s="13"/>
       <c r="D204" s="14"/>
       <c r="E204" s="14"/>
     </row>
-    <row r="205" ht="15.75" customHeight="1">
+    <row r="205" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A205" s="13"/>
       <c r="B205" s="14"/>
       <c r="C205" s="13"/>
       <c r="D205" s="14"/>
       <c r="E205" s="14"/>
     </row>
-    <row r="206" ht="15.75" customHeight="1">
+    <row r="206" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A206" s="13"/>
       <c r="B206" s="14"/>
       <c r="C206" s="13"/>
       <c r="D206" s="14"/>
       <c r="E206" s="14"/>
     </row>
-    <row r="207" ht="15.75" customHeight="1">
+    <row r="207" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A207" s="13"/>
       <c r="B207" s="14"/>
       <c r="C207" s="13"/>
       <c r="D207" s="14"/>
       <c r="E207" s="14"/>
     </row>
-    <row r="208" ht="15.75" customHeight="1">
+    <row r="208" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A208" s="13"/>
       <c r="B208" s="14"/>
       <c r="C208" s="13"/>
       <c r="D208" s="14"/>
       <c r="E208" s="14"/>
     </row>
-    <row r="209" ht="15.75" customHeight="1">
+    <row r="209" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A209" s="13"/>
       <c r="B209" s="14"/>
       <c r="C209" s="13"/>
       <c r="D209" s="14"/>
       <c r="E209" s="14"/>
     </row>
-    <row r="210" ht="15.75" customHeight="1">
+    <row r="210" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A210" s="13"/>
       <c r="B210" s="14"/>
       <c r="C210" s="13"/>
       <c r="D210" s="14"/>
       <c r="E210" s="14"/>
     </row>
-    <row r="211" ht="15.75" customHeight="1">
+    <row r="211" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A211" s="13"/>
       <c r="B211" s="14"/>
       <c r="C211" s="13"/>
       <c r="D211" s="14"/>
       <c r="E211" s="14"/>
     </row>
-    <row r="212" ht="15.75" customHeight="1">
+    <row r="212" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A212" s="13"/>
       <c r="B212" s="14"/>
       <c r="C212" s="13"/>
       <c r="D212" s="14"/>
       <c r="E212" s="14"/>
     </row>
-    <row r="213" ht="15.75" customHeight="1">
+    <row r="213" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A213" s="13"/>
       <c r="B213" s="14"/>
       <c r="C213" s="13"/>
       <c r="D213" s="14"/>
       <c r="E213" s="14"/>
     </row>
-    <row r="214" ht="15.75" customHeight="1">
+    <row r="214" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A214" s="13"/>
       <c r="B214" s="14"/>
       <c r="C214" s="13"/>
       <c r="D214" s="14"/>
       <c r="E214" s="14"/>
     </row>
-    <row r="215" ht="15.75" customHeight="1">
+    <row r="215" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A215" s="13"/>
       <c r="B215" s="14"/>
       <c r="C215" s="13"/>
       <c r="D215" s="14"/>
       <c r="E215" s="14"/>
     </row>
-    <row r="216" ht="15.75" customHeight="1">
+    <row r="216" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A216" s="13"/>
       <c r="B216" s="14"/>
       <c r="C216" s="13"/>
       <c r="D216" s="14"/>
       <c r="E216" s="14"/>
     </row>
-    <row r="217" ht="15.75" customHeight="1">
+    <row r="217" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A217" s="13"/>
       <c r="B217" s="14"/>
       <c r="C217" s="13"/>
       <c r="D217" s="14"/>
       <c r="E217" s="14"/>
     </row>
-    <row r="218" ht="15.75" customHeight="1">
+    <row r="218" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A218" s="13"/>
       <c r="B218" s="14"/>
       <c r="C218" s="13"/>
       <c r="D218" s="14"/>
       <c r="E218" s="14"/>
     </row>
-    <row r="219" ht="15.75" customHeight="1">
+    <row r="219" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A219" s="13"/>
       <c r="B219" s="14"/>
       <c r="C219" s="13"/>
       <c r="D219" s="14"/>
       <c r="E219" s="14"/>
     </row>
-    <row r="220" ht="15.75" customHeight="1">
+    <row r="220" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A220" s="13"/>
       <c r="B220" s="14"/>
       <c r="C220" s="13"/>
       <c r="D220" s="14"/>
       <c r="E220" s="14"/>
     </row>
-    <row r="221" ht="15.75" customHeight="1">
+    <row r="221" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A221" s="13"/>
       <c r="B221" s="14"/>
       <c r="C221" s="13"/>
       <c r="D221" s="14"/>
       <c r="E221" s="14"/>
     </row>
-    <row r="222" ht="15.75" customHeight="1">
+    <row r="222" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A222" s="13"/>
       <c r="B222" s="14"/>
       <c r="C222" s="13"/>
       <c r="D222" s="14"/>
       <c r="E222" s="14"/>
     </row>
-    <row r="223" ht="15.75" customHeight="1">
+    <row r="223" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A223" s="13"/>
       <c r="B223" s="14"/>
       <c r="C223" s="13"/>
       <c r="D223" s="14"/>
       <c r="E223" s="14"/>
     </row>
-    <row r="224" ht="15.75" customHeight="1">
+    <row r="224" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A224" s="13"/>
       <c r="B224" s="14"/>
       <c r="C224" s="13"/>
       <c r="D224" s="14"/>
       <c r="E224" s="14"/>
     </row>
-    <row r="225" ht="15.75" customHeight="1">
+    <row r="225" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A225" s="13"/>
       <c r="B225" s="14"/>
       <c r="C225" s="13"/>
       <c r="D225" s="14"/>
       <c r="E225" s="14"/>
     </row>
-    <row r="226" ht="15.75" customHeight="1">
+    <row r="226" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A226" s="13"/>
       <c r="B226" s="14"/>
       <c r="C226" s="13"/>
       <c r="D226" s="14"/>
       <c r="E226" s="14"/>
     </row>
-    <row r="227" ht="15.75" customHeight="1">
+    <row r="227" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A227" s="13"/>
       <c r="B227" s="14"/>
       <c r="C227" s="13"/>
       <c r="D227" s="14"/>
       <c r="E227" s="14"/>
     </row>
-    <row r="228" ht="15.75" customHeight="1">
+    <row r="228" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A228" s="13"/>
       <c r="B228" s="14"/>
       <c r="C228" s="13"/>
       <c r="D228" s="14"/>
       <c r="E228" s="14"/>
     </row>
-    <row r="229" ht="15.75" customHeight="1">
+    <row r="229" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A229" s="13"/>
       <c r="B229" s="14"/>
       <c r="C229" s="13"/>
       <c r="D229" s="14"/>
       <c r="E229" s="14"/>
     </row>
-    <row r="230" ht="15.75" customHeight="1">
+    <row r="230" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A230" s="13"/>
       <c r="B230" s="14"/>
       <c r="C230" s="13"/>
       <c r="D230" s="14"/>
       <c r="E230" s="14"/>
     </row>
-    <row r="231" ht="15.75" customHeight="1">
+    <row r="231" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A231" s="13"/>
       <c r="B231" s="14"/>
       <c r="C231" s="13"/>
       <c r="D231" s="14"/>
       <c r="E231" s="14"/>
     </row>
-    <row r="232" ht="15.75" customHeight="1">
+    <row r="232" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A232" s="13"/>
       <c r="B232" s="14"/>
       <c r="C232" s="13"/>
       <c r="D232" s="14"/>
       <c r="E232" s="14"/>
     </row>
-    <row r="233" ht="15.75" customHeight="1">
+    <row r="233" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A233" s="13"/>
       <c r="B233" s="14"/>
       <c r="C233" s="13"/>
       <c r="D233" s="14"/>
       <c r="E233" s="14"/>
     </row>
-    <row r="234" ht="15.75" customHeight="1">
+    <row r="234" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A234" s="13"/>
       <c r="B234" s="14"/>
       <c r="C234" s="13"/>
       <c r="D234" s="14"/>
       <c r="E234" s="14"/>
     </row>
-    <row r="235" ht="15.75" customHeight="1">
+    <row r="235" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A235" s="13"/>
       <c r="B235" s="14"/>
       <c r="C235" s="13"/>
       <c r="D235" s="14"/>
       <c r="E235" s="14"/>
     </row>
-    <row r="236" ht="15.75" customHeight="1">
+    <row r="236" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A236" s="13"/>
       <c r="B236" s="14"/>
       <c r="C236" s="13"/>
       <c r="D236" s="14"/>
       <c r="E236" s="14"/>
     </row>
-    <row r="237" ht="15.75" customHeight="1">
+    <row r="237" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A237" s="13"/>
       <c r="B237" s="14"/>
       <c r="C237" s="13"/>
       <c r="D237" s="14"/>
       <c r="E237" s="14"/>
     </row>
-    <row r="238" ht="15.75" customHeight="1">
+    <row r="238" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A238" s="13"/>
       <c r="B238" s="14"/>
       <c r="C238" s="13"/>
       <c r="D238" s="14"/>
       <c r="E238" s="14"/>
     </row>
-    <row r="239" ht="15.75" customHeight="1">
+    <row r="239" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A239" s="13"/>
       <c r="B239" s="14"/>
       <c r="C239" s="13"/>
       <c r="D239" s="14"/>
       <c r="E239" s="14"/>
     </row>
-    <row r="240" ht="15.75" customHeight="1">
+    <row r="240" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A240" s="13"/>
       <c r="B240" s="14"/>
       <c r="C240" s="13"/>
       <c r="D240" s="14"/>
       <c r="E240" s="14"/>
     </row>
-    <row r="241" ht="15.75" customHeight="1">
+    <row r="241" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A241" s="13"/>
       <c r="B241" s="14"/>
       <c r="C241" s="13"/>
       <c r="D241" s="14"/>
       <c r="E241" s="14"/>
     </row>
-    <row r="242" ht="15.75" customHeight="1">
+    <row r="242" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A242" s="13"/>
       <c r="B242" s="14"/>
       <c r="C242" s="13"/>
       <c r="D242" s="14"/>
       <c r="E242" s="14"/>
     </row>
-    <row r="243" ht="15.75" customHeight="1">
+    <row r="243" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A243" s="13"/>
       <c r="B243" s="14"/>
       <c r="C243" s="13"/>
       <c r="D243" s="14"/>
       <c r="E243" s="14"/>
     </row>
-    <row r="244" ht="15.75" customHeight="1">
+    <row r="244" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A244" s="13"/>
       <c r="B244" s="14"/>
       <c r="C244" s="13"/>
       <c r="D244" s="14"/>
       <c r="E244" s="14"/>
     </row>
-    <row r="245" ht="15.75" customHeight="1">
+    <row r="245" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A245" s="13"/>
       <c r="B245" s="14"/>
       <c r="C245" s="13"/>
       <c r="D245" s="14"/>
       <c r="E245" s="14"/>
     </row>
-    <row r="246" ht="15.75" customHeight="1">
+    <row r="246" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A246" s="13"/>
       <c r="B246" s="14"/>
       <c r="C246" s="13"/>
       <c r="D246" s="14"/>
       <c r="E246" s="14"/>
     </row>
-    <row r="247" ht="15.75" customHeight="1">
+    <row r="247" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A247" s="13"/>
       <c r="B247" s="14"/>
       <c r="C247" s="13"/>
       <c r="D247" s="14"/>
       <c r="E247" s="14"/>
     </row>
-    <row r="248" ht="15.75" customHeight="1">
+    <row r="248" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A248" s="13"/>
       <c r="B248" s="14"/>
       <c r="C248" s="13"/>
       <c r="D248" s="14"/>
       <c r="E248" s="14"/>
     </row>
-    <row r="249" ht="15.75" customHeight="1">
+    <row r="249" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A249" s="13"/>
       <c r="B249" s="14"/>
       <c r="C249" s="13"/>
       <c r="D249" s="14"/>
       <c r="E249" s="14"/>
     </row>
-    <row r="250" ht="15.75" customHeight="1">
+    <row r="250" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A250" s="13"/>
       <c r="B250" s="14"/>
       <c r="C250" s="13"/>
       <c r="D250" s="14"/>
       <c r="E250" s="14"/>
     </row>
-    <row r="251" ht="15.75" customHeight="1">
+    <row r="251" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A251" s="13"/>
       <c r="B251" s="14"/>
       <c r="C251" s="13"/>
       <c r="D251" s="14"/>
       <c r="E251" s="14"/>
     </row>
-    <row r="252" ht="15.75" customHeight="1">
+    <row r="252" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A252" s="13"/>
       <c r="B252" s="14"/>
       <c r="C252" s="13"/>
       <c r="D252" s="14"/>
       <c r="E252" s="14"/>
     </row>
-    <row r="253" ht="15.75" customHeight="1">
+    <row r="253" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A253" s="13"/>
       <c r="B253" s="14"/>
       <c r="C253" s="13"/>
       <c r="D253" s="14"/>
       <c r="E253" s="14"/>
     </row>
-    <row r="254" ht="15.75" customHeight="1">
+    <row r="254" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A254" s="13"/>
       <c r="B254" s="14"/>
       <c r="C254" s="13"/>
       <c r="D254" s="14"/>
       <c r="E254" s="14"/>
     </row>
-    <row r="255" ht="15.75" customHeight="1">
+    <row r="255" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A255" s="13"/>
       <c r="B255" s="14"/>
       <c r="C255" s="13"/>
       <c r="D255" s="14"/>
       <c r="E255" s="14"/>
     </row>
-    <row r="256" ht="15.75" customHeight="1">
+    <row r="256" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A256" s="13"/>
       <c r="B256" s="14"/>
       <c r="C256" s="13"/>
       <c r="D256" s="14"/>
       <c r="E256" s="14"/>
     </row>
-    <row r="257" ht="15.75" customHeight="1">
+    <row r="257" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A257" s="13"/>
       <c r="B257" s="14"/>
       <c r="C257" s="13"/>
       <c r="D257" s="14"/>
       <c r="E257" s="14"/>
     </row>
-    <row r="258" ht="15.75" customHeight="1">
+    <row r="258" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A258" s="13"/>
       <c r="B258" s="14"/>
       <c r="C258" s="13"/>
       <c r="D258" s="14"/>
       <c r="E258" s="14"/>
     </row>
-    <row r="259" ht="15.75" customHeight="1">
+    <row r="259" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A259" s="13"/>
       <c r="B259" s="14"/>
       <c r="C259" s="13"/>
       <c r="D259" s="14"/>
       <c r="E259" s="14"/>
     </row>
-    <row r="260" ht="15.75" customHeight="1">
+    <row r="260" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A260" s="13"/>
       <c r="B260" s="14"/>
       <c r="C260" s="13"/>
@@ -2677,17 +2732,16 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="D4"/>
-    <hyperlink r:id="rId2" ref="D5"/>
-    <hyperlink r:id="rId3" ref="D8"/>
-    <hyperlink r:id="rId4" ref="D9"/>
-    <hyperlink r:id="rId5" ref="D10"/>
-    <hyperlink r:id="rId6" ref="D11"/>
-    <hyperlink r:id="rId7" ref="D12"/>
+    <hyperlink ref="D4" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="D5" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="D8" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="D9" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="D10" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="D11" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="D12" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="D14" r:id="rId8" xr:uid="{AC1C4612-7541-47F6-9BBC-A0AC9D798593}"/>
   </hyperlinks>
-  <printOptions/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <drawing r:id="rId8"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Se agrega el 13 alummno al archivo. (modificado)
</commit_message>
<xml_diff>
--- a/Lista de Alumnos.xlsx
+++ b/Lista de Alumnos.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Temp\nuevo\Alumnos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Temp\Alumnos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55072BD9-E547-429B-A066-FB6D82893E87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D33D9E2-6937-42BE-8731-BD53E09721BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -148,7 +148,7 @@
     <t>alfredo.pc@gmail.com</t>
   </si>
   <si>
-    <t>alfredop</t>
+    <t>alfredop37</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Se agrega el alumno Gonzalez al Archivo
</commit_message>
<xml_diff>
--- a/Lista de Alumnos.xlsx
+++ b/Lista de Alumnos.xlsx
@@ -1,28 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25502"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Temp\Alumnos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Compumar\Documents\Git-Ispc\Alumnos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D0BFBA4D-00E4-43A0-A137-AD3686F93FB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93C2FFF5-8CB5-458A-B6EF-A01A295E674E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Electronica Microcontrolada" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
@@ -32,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
   <si>
     <t>#</t>
   </si>
@@ -170,13 +168,22 @@
   </si>
   <si>
     <t>mariogonzalezispc</t>
+  </si>
+  <si>
+    <t>Ivan Ezequiel Gonzalez</t>
+  </si>
+  <si>
+    <t>ivanezegonza@gmail.com</t>
+  </si>
+  <si>
+    <t>ivansky22</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -222,6 +229,12 @@
       <color theme="10"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -298,7 +311,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -340,6 +353,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -360,7 +376,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -682,11 +698,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E260"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.85546875" customWidth="1"/>
     <col min="2" max="2" width="37.140625" customWidth="1"/>
@@ -696,7 +712,7 @@
     <col min="6" max="6" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="27" customHeight="1">
+    <row r="1" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -713,7 +729,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="19.5" customHeight="1">
+    <row r="2" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -730,7 +746,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="19.5" customHeight="1">
+    <row r="3" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>2</v>
       </c>
@@ -745,7 +761,7 @@
       </c>
       <c r="E3" s="6"/>
     </row>
-    <row r="4" spans="1:5" ht="19.5" customHeight="1">
+    <row r="4" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>3</v>
       </c>
@@ -762,7 +778,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="19.5" customHeight="1">
+    <row r="5" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>4</v>
       </c>
@@ -779,7 +795,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="19.5" customHeight="1">
+    <row r="6" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>5</v>
       </c>
@@ -796,7 +812,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="19.5" customHeight="1">
+    <row r="7" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>6</v>
       </c>
@@ -813,7 +829,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="19.5" customHeight="1">
+    <row r="8" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>7</v>
       </c>
@@ -830,7 +846,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="19.5" customHeight="1">
+    <row r="9" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>8</v>
       </c>
@@ -847,7 +863,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="19.5" customHeight="1">
+    <row r="10" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>9</v>
       </c>
@@ -862,7 +878,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="19.5" customHeight="1">
+    <row r="11" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <v>10</v>
       </c>
@@ -879,7 +895,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="19.5" customHeight="1">
+    <row r="12" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>11</v>
       </c>
@@ -896,7 +912,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="19.5" customHeight="1">
+    <row r="13" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
         <v>12</v>
       </c>
@@ -913,7 +929,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="19.5" customHeight="1">
+    <row r="14" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
         <v>13</v>
       </c>
@@ -930,7 +946,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="19.5" customHeight="1">
+    <row r="15" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
         <v>14</v>
       </c>
@@ -947,16 +963,24 @@
         <v>45</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="19.5" customHeight="1">
+    <row r="16" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
         <v>15</v>
       </c>
-      <c r="B16" s="6"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
-    </row>
-    <row r="17" spans="1:5" ht="19.5" customHeight="1">
+      <c r="B16" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C16" s="5">
+        <v>2</v>
+      </c>
+      <c r="D16" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="E16" s="15" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
         <v>16</v>
       </c>
@@ -965,7 +989,7 @@
       <c r="D17" s="6"/>
       <c r="E17" s="6"/>
     </row>
-    <row r="18" spans="1:5" ht="25.5" customHeight="1">
+    <row r="18" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <v>17</v>
       </c>
@@ -974,7 +998,7 @@
       <c r="D18" s="6"/>
       <c r="E18" s="6"/>
     </row>
-    <row r="19" spans="1:5" ht="25.5" customHeight="1">
+    <row r="19" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
         <v>18</v>
       </c>
@@ -983,7 +1007,7 @@
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
     </row>
-    <row r="20" spans="1:5" ht="25.5" customHeight="1">
+    <row r="20" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
         <v>19</v>
       </c>
@@ -992,7 +1016,7 @@
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
     </row>
-    <row r="21" spans="1:5" ht="25.5" customHeight="1">
+    <row r="21" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="5">
         <v>20</v>
       </c>
@@ -1001,7 +1025,7 @@
       <c r="D21" s="6"/>
       <c r="E21" s="6"/>
     </row>
-    <row r="22" spans="1:5" ht="25.5" customHeight="1">
+    <row r="22" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="5">
         <v>21</v>
       </c>
@@ -1010,7 +1034,7 @@
       <c r="D22" s="6"/>
       <c r="E22" s="6"/>
     </row>
-    <row r="23" spans="1:5" ht="25.5" customHeight="1">
+    <row r="23" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="5">
         <v>22</v>
       </c>
@@ -1019,7 +1043,7 @@
       <c r="D23" s="6"/>
       <c r="E23" s="6"/>
     </row>
-    <row r="24" spans="1:5" ht="25.5" customHeight="1">
+    <row r="24" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="5">
         <v>23</v>
       </c>
@@ -1028,7 +1052,7 @@
       <c r="D24" s="6"/>
       <c r="E24" s="6"/>
     </row>
-    <row r="25" spans="1:5" ht="25.5" customHeight="1">
+    <row r="25" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="5">
         <v>24</v>
       </c>
@@ -1037,7 +1061,7 @@
       <c r="D25" s="6"/>
       <c r="E25" s="6"/>
     </row>
-    <row r="26" spans="1:5" ht="25.5" customHeight="1">
+    <row r="26" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="5">
         <v>25</v>
       </c>
@@ -1046,7 +1070,7 @@
       <c r="D26" s="6"/>
       <c r="E26" s="6"/>
     </row>
-    <row r="27" spans="1:5" ht="25.5" customHeight="1">
+    <row r="27" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="5">
         <v>26</v>
       </c>
@@ -1055,7 +1079,7 @@
       <c r="D27" s="6"/>
       <c r="E27" s="6"/>
     </row>
-    <row r="28" spans="1:5" ht="25.5" customHeight="1">
+    <row r="28" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="5">
         <v>27</v>
       </c>
@@ -1064,7 +1088,7 @@
       <c r="D28" s="6"/>
       <c r="E28" s="6"/>
     </row>
-    <row r="29" spans="1:5" ht="25.5" customHeight="1">
+    <row r="29" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="5">
         <v>28</v>
       </c>
@@ -1073,7 +1097,7 @@
       <c r="D29" s="6"/>
       <c r="E29" s="6"/>
     </row>
-    <row r="30" spans="1:5" ht="25.5" customHeight="1">
+    <row r="30" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="5">
         <v>29</v>
       </c>
@@ -1082,7 +1106,7 @@
       <c r="D30" s="6"/>
       <c r="E30" s="6"/>
     </row>
-    <row r="31" spans="1:5" ht="25.5" customHeight="1">
+    <row r="31" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="5">
         <v>30</v>
       </c>
@@ -1091,7 +1115,7 @@
       <c r="D31" s="6"/>
       <c r="E31" s="6"/>
     </row>
-    <row r="32" spans="1:5" ht="25.5" customHeight="1">
+    <row r="32" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="5">
         <v>31</v>
       </c>
@@ -1100,7 +1124,7 @@
       <c r="D32" s="6"/>
       <c r="E32" s="6"/>
     </row>
-    <row r="33" spans="1:5" ht="25.5" customHeight="1">
+    <row r="33" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="5">
         <v>32</v>
       </c>
@@ -1109,7 +1133,7 @@
       <c r="D33" s="6"/>
       <c r="E33" s="6"/>
     </row>
-    <row r="34" spans="1:5" ht="25.5" customHeight="1">
+    <row r="34" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="5">
         <v>33</v>
       </c>
@@ -1118,7 +1142,7 @@
       <c r="D34" s="6"/>
       <c r="E34" s="6"/>
     </row>
-    <row r="35" spans="1:5" ht="25.5" customHeight="1">
+    <row r="35" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="5">
         <v>34</v>
       </c>
@@ -1127,7 +1151,7 @@
       <c r="D35" s="6"/>
       <c r="E35" s="6"/>
     </row>
-    <row r="36" spans="1:5" ht="25.5" customHeight="1">
+    <row r="36" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="5">
         <v>35</v>
       </c>
@@ -1136,7 +1160,7 @@
       <c r="D36" s="6"/>
       <c r="E36" s="6"/>
     </row>
-    <row r="37" spans="1:5" ht="25.5" customHeight="1">
+    <row r="37" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="5">
         <v>36</v>
       </c>
@@ -1145,7 +1169,7 @@
       <c r="D37" s="6"/>
       <c r="E37" s="6"/>
     </row>
-    <row r="38" spans="1:5" ht="25.5" customHeight="1">
+    <row r="38" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="5">
         <v>37</v>
       </c>
@@ -1154,7 +1178,7 @@
       <c r="D38" s="6"/>
       <c r="E38" s="6"/>
     </row>
-    <row r="39" spans="1:5" ht="25.5" customHeight="1">
+    <row r="39" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="5">
         <v>38</v>
       </c>
@@ -1163,7 +1187,7 @@
       <c r="D39" s="6"/>
       <c r="E39" s="6"/>
     </row>
-    <row r="40" spans="1:5" ht="25.5" customHeight="1">
+    <row r="40" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="5">
         <v>39</v>
       </c>
@@ -1172,7 +1196,7 @@
       <c r="D40" s="6"/>
       <c r="E40" s="6"/>
     </row>
-    <row r="41" spans="1:5" ht="25.5" customHeight="1">
+    <row r="41" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="5">
         <v>40</v>
       </c>
@@ -1181,7 +1205,7 @@
       <c r="D41" s="6"/>
       <c r="E41" s="6"/>
     </row>
-    <row r="42" spans="1:5" ht="25.5" customHeight="1">
+    <row r="42" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="5">
         <v>41</v>
       </c>
@@ -1190,7 +1214,7 @@
       <c r="D42" s="6"/>
       <c r="E42" s="6"/>
     </row>
-    <row r="43" spans="1:5" ht="25.5" customHeight="1">
+    <row r="43" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="5">
         <v>42</v>
       </c>
@@ -1199,7 +1223,7 @@
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
     </row>
-    <row r="44" spans="1:5" ht="25.5" customHeight="1">
+    <row r="44" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="5">
         <v>43</v>
       </c>
@@ -1208,7 +1232,7 @@
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
     </row>
-    <row r="45" spans="1:5" ht="25.5" customHeight="1">
+    <row r="45" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="5">
         <v>44</v>
       </c>
@@ -1217,7 +1241,7 @@
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
     </row>
-    <row r="46" spans="1:5" ht="25.5" customHeight="1">
+    <row r="46" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="5">
         <v>45</v>
       </c>
@@ -1226,7 +1250,7 @@
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
     </row>
-    <row r="47" spans="1:5" ht="25.5" customHeight="1">
+    <row r="47" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="5">
         <v>46</v>
       </c>
@@ -1235,7 +1259,7 @@
       <c r="D47" s="6"/>
       <c r="E47" s="6"/>
     </row>
-    <row r="48" spans="1:5" ht="25.5" customHeight="1">
+    <row r="48" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="5">
         <v>47</v>
       </c>
@@ -1244,7 +1268,7 @@
       <c r="D48" s="6"/>
       <c r="E48" s="6"/>
     </row>
-    <row r="49" spans="1:5" ht="25.5" customHeight="1">
+    <row r="49" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="5">
         <v>48</v>
       </c>
@@ -1253,7 +1277,7 @@
       <c r="D49" s="6"/>
       <c r="E49" s="6"/>
     </row>
-    <row r="50" spans="1:5" ht="25.5" customHeight="1">
+    <row r="50" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="5">
         <v>49</v>
       </c>
@@ -1262,7 +1286,7 @@
       <c r="D50" s="6"/>
       <c r="E50" s="6"/>
     </row>
-    <row r="51" spans="1:5" ht="25.5" customHeight="1">
+    <row r="51" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="5">
         <v>50</v>
       </c>
@@ -1271,7 +1295,7 @@
       <c r="D51" s="6"/>
       <c r="E51" s="6"/>
     </row>
-    <row r="52" spans="1:5" ht="25.5" customHeight="1">
+    <row r="52" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="5">
         <v>51</v>
       </c>
@@ -1280,7 +1304,7 @@
       <c r="D52" s="6"/>
       <c r="E52" s="6"/>
     </row>
-    <row r="53" spans="1:5" ht="25.5" customHeight="1">
+    <row r="53" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="5">
         <v>52</v>
       </c>
@@ -1289,7 +1313,7 @@
       <c r="D53" s="6"/>
       <c r="E53" s="6"/>
     </row>
-    <row r="54" spans="1:5" ht="25.5" customHeight="1">
+    <row r="54" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="5">
         <v>53</v>
       </c>
@@ -1298,7 +1322,7 @@
       <c r="D54" s="6"/>
       <c r="E54" s="6"/>
     </row>
-    <row r="55" spans="1:5" ht="25.5" customHeight="1">
+    <row r="55" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="5">
         <v>54</v>
       </c>
@@ -1307,7 +1331,7 @@
       <c r="D55" s="6"/>
       <c r="E55" s="6"/>
     </row>
-    <row r="56" spans="1:5" ht="25.5" customHeight="1">
+    <row r="56" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="5">
         <v>55</v>
       </c>
@@ -1316,7 +1340,7 @@
       <c r="D56" s="6"/>
       <c r="E56" s="6"/>
     </row>
-    <row r="57" spans="1:5" ht="25.5" customHeight="1">
+    <row r="57" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="5">
         <v>56</v>
       </c>
@@ -1325,7 +1349,7 @@
       <c r="D57" s="6"/>
       <c r="E57" s="6"/>
     </row>
-    <row r="58" spans="1:5" ht="25.5" customHeight="1">
+    <row r="58" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="5">
         <v>57</v>
       </c>
@@ -1334,7 +1358,7 @@
       <c r="D58" s="6"/>
       <c r="E58" s="6"/>
     </row>
-    <row r="59" spans="1:5" ht="25.5" customHeight="1">
+    <row r="59" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="5">
         <v>58</v>
       </c>
@@ -1343,7 +1367,7 @@
       <c r="D59" s="6"/>
       <c r="E59" s="6"/>
     </row>
-    <row r="60" spans="1:5" ht="25.5" customHeight="1">
+    <row r="60" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="5">
         <v>59</v>
       </c>
@@ -1352,1400 +1376,1400 @@
       <c r="D60" s="6"/>
       <c r="E60" s="6"/>
     </row>
-    <row r="61" spans="1:5" ht="15.75" customHeight="1">
+    <row r="61" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="10"/>
       <c r="B61" s="11"/>
       <c r="C61" s="10"/>
       <c r="D61" s="11"/>
       <c r="E61" s="11"/>
     </row>
-    <row r="62" spans="1:5" ht="15.75" customHeight="1">
+    <row r="62" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="10"/>
       <c r="B62" s="11"/>
       <c r="C62" s="10"/>
       <c r="D62" s="11"/>
       <c r="E62" s="11"/>
     </row>
-    <row r="63" spans="1:5" ht="15.75" customHeight="1">
+    <row r="63" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="10"/>
       <c r="B63" s="11"/>
       <c r="C63" s="10"/>
       <c r="D63" s="11"/>
       <c r="E63" s="11"/>
     </row>
-    <row r="64" spans="1:5" ht="15.75" customHeight="1">
+    <row r="64" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="10"/>
       <c r="B64" s="11"/>
       <c r="C64" s="10"/>
       <c r="D64" s="11"/>
       <c r="E64" s="11"/>
     </row>
-    <row r="65" spans="1:5" ht="15.75" customHeight="1">
+    <row r="65" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="10"/>
       <c r="B65" s="11"/>
       <c r="C65" s="10"/>
       <c r="D65" s="11"/>
       <c r="E65" s="11"/>
     </row>
-    <row r="66" spans="1:5" ht="15.75" customHeight="1">
+    <row r="66" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="10"/>
       <c r="B66" s="11"/>
       <c r="C66" s="10"/>
       <c r="D66" s="11"/>
       <c r="E66" s="11"/>
     </row>
-    <row r="67" spans="1:5" ht="15.75" customHeight="1">
+    <row r="67" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="10"/>
       <c r="B67" s="11"/>
       <c r="C67" s="10"/>
       <c r="D67" s="11"/>
       <c r="E67" s="11"/>
     </row>
-    <row r="68" spans="1:5" ht="15.75" customHeight="1">
+    <row r="68" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="10"/>
       <c r="B68" s="11"/>
       <c r="C68" s="10"/>
       <c r="D68" s="11"/>
       <c r="E68" s="11"/>
     </row>
-    <row r="69" spans="1:5" ht="15.75" customHeight="1">
+    <row r="69" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="10"/>
       <c r="B69" s="11"/>
       <c r="C69" s="10"/>
       <c r="D69" s="11"/>
       <c r="E69" s="11"/>
     </row>
-    <row r="70" spans="1:5" ht="15.75" customHeight="1">
+    <row r="70" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="10"/>
       <c r="B70" s="11"/>
       <c r="C70" s="10"/>
       <c r="D70" s="11"/>
       <c r="E70" s="11"/>
     </row>
-    <row r="71" spans="1:5" ht="15.75" customHeight="1">
+    <row r="71" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="10"/>
       <c r="B71" s="11"/>
       <c r="C71" s="10"/>
       <c r="D71" s="11"/>
       <c r="E71" s="11"/>
     </row>
-    <row r="72" spans="1:5" ht="15.75" customHeight="1">
+    <row r="72" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="10"/>
       <c r="B72" s="11"/>
       <c r="C72" s="10"/>
       <c r="D72" s="11"/>
       <c r="E72" s="11"/>
     </row>
-    <row r="73" spans="1:5" ht="15.75" customHeight="1">
+    <row r="73" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="10"/>
       <c r="B73" s="11"/>
       <c r="C73" s="10"/>
       <c r="D73" s="11"/>
       <c r="E73" s="11"/>
     </row>
-    <row r="74" spans="1:5" ht="15.75" customHeight="1">
+    <row r="74" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="10"/>
       <c r="B74" s="11"/>
       <c r="C74" s="10"/>
       <c r="D74" s="11"/>
       <c r="E74" s="11"/>
     </row>
-    <row r="75" spans="1:5" ht="15.75" customHeight="1">
+    <row r="75" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="10"/>
       <c r="B75" s="11"/>
       <c r="C75" s="10"/>
       <c r="D75" s="11"/>
       <c r="E75" s="11"/>
     </row>
-    <row r="76" spans="1:5" ht="15.75" customHeight="1">
+    <row r="76" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="10"/>
       <c r="B76" s="11"/>
       <c r="C76" s="10"/>
       <c r="D76" s="11"/>
       <c r="E76" s="11"/>
     </row>
-    <row r="77" spans="1:5" ht="15.75" customHeight="1">
+    <row r="77" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="10"/>
       <c r="B77" s="11"/>
       <c r="C77" s="10"/>
       <c r="D77" s="11"/>
       <c r="E77" s="11"/>
     </row>
-    <row r="78" spans="1:5" ht="15.75" customHeight="1">
+    <row r="78" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="10"/>
       <c r="B78" s="11"/>
       <c r="C78" s="10"/>
       <c r="D78" s="11"/>
       <c r="E78" s="11"/>
     </row>
-    <row r="79" spans="1:5" ht="15.75" customHeight="1">
+    <row r="79" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="10"/>
       <c r="B79" s="11"/>
       <c r="C79" s="10"/>
       <c r="D79" s="11"/>
       <c r="E79" s="11"/>
     </row>
-    <row r="80" spans="1:5" ht="15.75" customHeight="1">
+    <row r="80" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="10"/>
       <c r="B80" s="11"/>
       <c r="C80" s="10"/>
       <c r="D80" s="11"/>
       <c r="E80" s="11"/>
     </row>
-    <row r="81" spans="1:5" ht="15.75" customHeight="1">
+    <row r="81" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="10"/>
       <c r="B81" s="11"/>
       <c r="C81" s="10"/>
       <c r="D81" s="11"/>
       <c r="E81" s="11"/>
     </row>
-    <row r="82" spans="1:5" ht="15.75" customHeight="1">
+    <row r="82" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="10"/>
       <c r="B82" s="11"/>
       <c r="C82" s="10"/>
       <c r="D82" s="11"/>
       <c r="E82" s="11"/>
     </row>
-    <row r="83" spans="1:5" ht="15.75" customHeight="1">
+    <row r="83" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="10"/>
       <c r="B83" s="11"/>
       <c r="C83" s="10"/>
       <c r="D83" s="11"/>
       <c r="E83" s="11"/>
     </row>
-    <row r="84" spans="1:5" ht="15.75" customHeight="1">
+    <row r="84" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="10"/>
       <c r="B84" s="11"/>
       <c r="C84" s="10"/>
       <c r="D84" s="11"/>
       <c r="E84" s="11"/>
     </row>
-    <row r="85" spans="1:5" ht="15.75" customHeight="1">
+    <row r="85" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="10"/>
       <c r="B85" s="11"/>
       <c r="C85" s="10"/>
       <c r="D85" s="11"/>
       <c r="E85" s="11"/>
     </row>
-    <row r="86" spans="1:5" ht="15.75" customHeight="1">
+    <row r="86" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="10"/>
       <c r="B86" s="11"/>
       <c r="C86" s="10"/>
       <c r="D86" s="11"/>
       <c r="E86" s="11"/>
     </row>
-    <row r="87" spans="1:5" ht="15.75" customHeight="1">
+    <row r="87" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="10"/>
       <c r="B87" s="11"/>
       <c r="C87" s="10"/>
       <c r="D87" s="11"/>
       <c r="E87" s="11"/>
     </row>
-    <row r="88" spans="1:5" ht="15.75" customHeight="1">
+    <row r="88" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="10"/>
       <c r="B88" s="11"/>
       <c r="C88" s="10"/>
       <c r="D88" s="11"/>
       <c r="E88" s="11"/>
     </row>
-    <row r="89" spans="1:5" ht="15.75" customHeight="1">
+    <row r="89" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="10"/>
       <c r="B89" s="11"/>
       <c r="C89" s="10"/>
       <c r="D89" s="11"/>
       <c r="E89" s="11"/>
     </row>
-    <row r="90" spans="1:5" ht="15.75" customHeight="1">
+    <row r="90" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="10"/>
       <c r="B90" s="11"/>
       <c r="C90" s="10"/>
       <c r="D90" s="11"/>
       <c r="E90" s="11"/>
     </row>
-    <row r="91" spans="1:5" ht="15.75" customHeight="1">
+    <row r="91" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="10"/>
       <c r="B91" s="11"/>
       <c r="C91" s="10"/>
       <c r="D91" s="11"/>
       <c r="E91" s="11"/>
     </row>
-    <row r="92" spans="1:5" ht="15.75" customHeight="1">
+    <row r="92" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="10"/>
       <c r="B92" s="11"/>
       <c r="C92" s="10"/>
       <c r="D92" s="11"/>
       <c r="E92" s="11"/>
     </row>
-    <row r="93" spans="1:5" ht="15.75" customHeight="1">
+    <row r="93" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="10"/>
       <c r="B93" s="11"/>
       <c r="C93" s="10"/>
       <c r="D93" s="11"/>
       <c r="E93" s="11"/>
     </row>
-    <row r="94" spans="1:5" ht="15.75" customHeight="1">
+    <row r="94" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="10"/>
       <c r="B94" s="11"/>
       <c r="C94" s="10"/>
       <c r="D94" s="11"/>
       <c r="E94" s="11"/>
     </row>
-    <row r="95" spans="1:5" ht="15.75" customHeight="1">
+    <row r="95" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="10"/>
       <c r="B95" s="11"/>
       <c r="C95" s="10"/>
       <c r="D95" s="11"/>
       <c r="E95" s="11"/>
     </row>
-    <row r="96" spans="1:5" ht="15.75" customHeight="1">
+    <row r="96" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="10"/>
       <c r="B96" s="11"/>
       <c r="C96" s="10"/>
       <c r="D96" s="11"/>
       <c r="E96" s="11"/>
     </row>
-    <row r="97" spans="1:5" ht="15.75" customHeight="1">
+    <row r="97" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="10"/>
       <c r="B97" s="11"/>
       <c r="C97" s="10"/>
       <c r="D97" s="11"/>
       <c r="E97" s="11"/>
     </row>
-    <row r="98" spans="1:5" ht="15.75" customHeight="1">
+    <row r="98" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="10"/>
       <c r="B98" s="11"/>
       <c r="C98" s="10"/>
       <c r="D98" s="11"/>
       <c r="E98" s="11"/>
     </row>
-    <row r="99" spans="1:5" ht="15.75" customHeight="1">
+    <row r="99" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="10"/>
       <c r="B99" s="11"/>
       <c r="C99" s="10"/>
       <c r="D99" s="11"/>
       <c r="E99" s="11"/>
     </row>
-    <row r="100" spans="1:5" ht="15.75" customHeight="1">
+    <row r="100" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="10"/>
       <c r="B100" s="11"/>
       <c r="C100" s="10"/>
       <c r="D100" s="11"/>
       <c r="E100" s="11"/>
     </row>
-    <row r="101" spans="1:5" ht="15.75" customHeight="1">
+    <row r="101" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="10"/>
       <c r="B101" s="11"/>
       <c r="C101" s="10"/>
       <c r="D101" s="11"/>
       <c r="E101" s="11"/>
     </row>
-    <row r="102" spans="1:5" ht="15.75" customHeight="1">
+    <row r="102" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="10"/>
       <c r="B102" s="11"/>
       <c r="C102" s="10"/>
       <c r="D102" s="11"/>
       <c r="E102" s="11"/>
     </row>
-    <row r="103" spans="1:5" ht="15.75" customHeight="1">
+    <row r="103" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" s="10"/>
       <c r="B103" s="11"/>
       <c r="C103" s="10"/>
       <c r="D103" s="11"/>
       <c r="E103" s="11"/>
     </row>
-    <row r="104" spans="1:5" ht="15.75" customHeight="1">
+    <row r="104" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="10"/>
       <c r="B104" s="11"/>
       <c r="C104" s="10"/>
       <c r="D104" s="11"/>
       <c r="E104" s="11"/>
     </row>
-    <row r="105" spans="1:5" ht="15.75" customHeight="1">
+    <row r="105" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" s="10"/>
       <c r="B105" s="11"/>
       <c r="C105" s="10"/>
       <c r="D105" s="11"/>
       <c r="E105" s="11"/>
     </row>
-    <row r="106" spans="1:5" ht="15.75" customHeight="1">
+    <row r="106" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="10"/>
       <c r="B106" s="11"/>
       <c r="C106" s="10"/>
       <c r="D106" s="11"/>
       <c r="E106" s="11"/>
     </row>
-    <row r="107" spans="1:5" ht="15.75" customHeight="1">
+    <row r="107" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" s="10"/>
       <c r="B107" s="11"/>
       <c r="C107" s="10"/>
       <c r="D107" s="11"/>
       <c r="E107" s="11"/>
     </row>
-    <row r="108" spans="1:5" ht="15.75" customHeight="1">
+    <row r="108" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" s="10"/>
       <c r="B108" s="11"/>
       <c r="C108" s="10"/>
       <c r="D108" s="11"/>
       <c r="E108" s="11"/>
     </row>
-    <row r="109" spans="1:5" ht="15.75" customHeight="1">
+    <row r="109" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" s="10"/>
       <c r="B109" s="11"/>
       <c r="C109" s="10"/>
       <c r="D109" s="11"/>
       <c r="E109" s="11"/>
     </row>
-    <row r="110" spans="1:5" ht="15.75" customHeight="1">
+    <row r="110" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" s="10"/>
       <c r="B110" s="11"/>
       <c r="C110" s="10"/>
       <c r="D110" s="11"/>
       <c r="E110" s="11"/>
     </row>
-    <row r="111" spans="1:5" ht="15.75" customHeight="1">
+    <row r="111" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" s="10"/>
       <c r="B111" s="11"/>
       <c r="C111" s="10"/>
       <c r="D111" s="11"/>
       <c r="E111" s="11"/>
     </row>
-    <row r="112" spans="1:5" ht="15.75" customHeight="1">
+    <row r="112" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" s="10"/>
       <c r="B112" s="11"/>
       <c r="C112" s="10"/>
       <c r="D112" s="11"/>
       <c r="E112" s="11"/>
     </row>
-    <row r="113" spans="1:5" ht="15.75" customHeight="1">
+    <row r="113" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" s="10"/>
       <c r="B113" s="11"/>
       <c r="C113" s="10"/>
       <c r="D113" s="11"/>
       <c r="E113" s="11"/>
     </row>
-    <row r="114" spans="1:5" ht="15.75" customHeight="1">
+    <row r="114" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A114" s="10"/>
       <c r="B114" s="11"/>
       <c r="C114" s="10"/>
       <c r="D114" s="11"/>
       <c r="E114" s="11"/>
     </row>
-    <row r="115" spans="1:5" ht="15.75" customHeight="1">
+    <row r="115" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A115" s="10"/>
       <c r="B115" s="11"/>
       <c r="C115" s="10"/>
       <c r="D115" s="11"/>
       <c r="E115" s="11"/>
     </row>
-    <row r="116" spans="1:5" ht="15.75" customHeight="1">
+    <row r="116" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A116" s="10"/>
       <c r="B116" s="11"/>
       <c r="C116" s="10"/>
       <c r="D116" s="11"/>
       <c r="E116" s="11"/>
     </row>
-    <row r="117" spans="1:5" ht="15.75" customHeight="1">
+    <row r="117" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A117" s="10"/>
       <c r="B117" s="11"/>
       <c r="C117" s="10"/>
       <c r="D117" s="11"/>
       <c r="E117" s="11"/>
     </row>
-    <row r="118" spans="1:5" ht="15.75" customHeight="1">
+    <row r="118" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A118" s="10"/>
       <c r="B118" s="11"/>
       <c r="C118" s="10"/>
       <c r="D118" s="11"/>
       <c r="E118" s="11"/>
     </row>
-    <row r="119" spans="1:5" ht="15.75" customHeight="1">
+    <row r="119" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A119" s="10"/>
       <c r="B119" s="11"/>
       <c r="C119" s="10"/>
       <c r="D119" s="11"/>
       <c r="E119" s="11"/>
     </row>
-    <row r="120" spans="1:5" ht="15.75" customHeight="1">
+    <row r="120" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A120" s="10"/>
       <c r="B120" s="11"/>
       <c r="C120" s="10"/>
       <c r="D120" s="11"/>
       <c r="E120" s="11"/>
     </row>
-    <row r="121" spans="1:5" ht="15.75" customHeight="1">
+    <row r="121" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A121" s="10"/>
       <c r="B121" s="11"/>
       <c r="C121" s="10"/>
       <c r="D121" s="11"/>
       <c r="E121" s="11"/>
     </row>
-    <row r="122" spans="1:5" ht="15.75" customHeight="1">
+    <row r="122" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A122" s="10"/>
       <c r="B122" s="11"/>
       <c r="C122" s="10"/>
       <c r="D122" s="11"/>
       <c r="E122" s="11"/>
     </row>
-    <row r="123" spans="1:5" ht="15.75" customHeight="1">
+    <row r="123" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A123" s="10"/>
       <c r="B123" s="11"/>
       <c r="C123" s="10"/>
       <c r="D123" s="11"/>
       <c r="E123" s="11"/>
     </row>
-    <row r="124" spans="1:5" ht="15.75" customHeight="1">
+    <row r="124" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A124" s="10"/>
       <c r="B124" s="11"/>
       <c r="C124" s="10"/>
       <c r="D124" s="11"/>
       <c r="E124" s="11"/>
     </row>
-    <row r="125" spans="1:5" ht="15.75" customHeight="1">
+    <row r="125" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A125" s="10"/>
       <c r="B125" s="11"/>
       <c r="C125" s="10"/>
       <c r="D125" s="11"/>
       <c r="E125" s="11"/>
     </row>
-    <row r="126" spans="1:5" ht="15.75" customHeight="1">
+    <row r="126" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A126" s="10"/>
       <c r="B126" s="11"/>
       <c r="C126" s="10"/>
       <c r="D126" s="11"/>
       <c r="E126" s="11"/>
     </row>
-    <row r="127" spans="1:5" ht="15.75" customHeight="1">
+    <row r="127" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A127" s="10"/>
       <c r="B127" s="11"/>
       <c r="C127" s="10"/>
       <c r="D127" s="11"/>
       <c r="E127" s="11"/>
     </row>
-    <row r="128" spans="1:5" ht="15.75" customHeight="1">
+    <row r="128" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A128" s="10"/>
       <c r="B128" s="11"/>
       <c r="C128" s="10"/>
       <c r="D128" s="11"/>
       <c r="E128" s="11"/>
     </row>
-    <row r="129" spans="1:5" ht="15.75" customHeight="1">
+    <row r="129" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A129" s="10"/>
       <c r="B129" s="11"/>
       <c r="C129" s="10"/>
       <c r="D129" s="11"/>
       <c r="E129" s="11"/>
     </row>
-    <row r="130" spans="1:5" ht="15.75" customHeight="1">
+    <row r="130" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A130" s="10"/>
       <c r="B130" s="11"/>
       <c r="C130" s="10"/>
       <c r="D130" s="11"/>
       <c r="E130" s="11"/>
     </row>
-    <row r="131" spans="1:5" ht="15.75" customHeight="1">
+    <row r="131" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A131" s="10"/>
       <c r="B131" s="11"/>
       <c r="C131" s="10"/>
       <c r="D131" s="11"/>
       <c r="E131" s="11"/>
     </row>
-    <row r="132" spans="1:5" ht="15.75" customHeight="1">
+    <row r="132" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A132" s="10"/>
       <c r="B132" s="11"/>
       <c r="C132" s="10"/>
       <c r="D132" s="11"/>
       <c r="E132" s="11"/>
     </row>
-    <row r="133" spans="1:5" ht="15.75" customHeight="1">
+    <row r="133" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A133" s="10"/>
       <c r="B133" s="11"/>
       <c r="C133" s="10"/>
       <c r="D133" s="11"/>
       <c r="E133" s="11"/>
     </row>
-    <row r="134" spans="1:5" ht="15.75" customHeight="1">
+    <row r="134" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A134" s="10"/>
       <c r="B134" s="11"/>
       <c r="C134" s="10"/>
       <c r="D134" s="11"/>
       <c r="E134" s="11"/>
     </row>
-    <row r="135" spans="1:5" ht="15.75" customHeight="1">
+    <row r="135" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A135" s="10"/>
       <c r="B135" s="11"/>
       <c r="C135" s="10"/>
       <c r="D135" s="11"/>
       <c r="E135" s="11"/>
     </row>
-    <row r="136" spans="1:5" ht="15.75" customHeight="1">
+    <row r="136" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A136" s="10"/>
       <c r="B136" s="11"/>
       <c r="C136" s="10"/>
       <c r="D136" s="11"/>
       <c r="E136" s="11"/>
     </row>
-    <row r="137" spans="1:5" ht="15.75" customHeight="1">
+    <row r="137" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A137" s="10"/>
       <c r="B137" s="11"/>
       <c r="C137" s="10"/>
       <c r="D137" s="11"/>
       <c r="E137" s="11"/>
     </row>
-    <row r="138" spans="1:5" ht="15.75" customHeight="1">
+    <row r="138" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A138" s="10"/>
       <c r="B138" s="11"/>
       <c r="C138" s="10"/>
       <c r="D138" s="11"/>
       <c r="E138" s="11"/>
     </row>
-    <row r="139" spans="1:5" ht="15.75" customHeight="1">
+    <row r="139" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A139" s="10"/>
       <c r="B139" s="11"/>
       <c r="C139" s="10"/>
       <c r="D139" s="11"/>
       <c r="E139" s="11"/>
     </row>
-    <row r="140" spans="1:5" ht="15.75" customHeight="1">
+    <row r="140" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A140" s="10"/>
       <c r="B140" s="11"/>
       <c r="C140" s="10"/>
       <c r="D140" s="11"/>
       <c r="E140" s="11"/>
     </row>
-    <row r="141" spans="1:5" ht="15.75" customHeight="1">
+    <row r="141" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A141" s="10"/>
       <c r="B141" s="11"/>
       <c r="C141" s="10"/>
       <c r="D141" s="11"/>
       <c r="E141" s="11"/>
     </row>
-    <row r="142" spans="1:5" ht="15.75" customHeight="1">
+    <row r="142" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A142" s="10"/>
       <c r="B142" s="11"/>
       <c r="C142" s="10"/>
       <c r="D142" s="11"/>
       <c r="E142" s="11"/>
     </row>
-    <row r="143" spans="1:5" ht="15.75" customHeight="1">
+    <row r="143" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A143" s="10"/>
       <c r="B143" s="11"/>
       <c r="C143" s="10"/>
       <c r="D143" s="11"/>
       <c r="E143" s="11"/>
     </row>
-    <row r="144" spans="1:5" ht="15.75" customHeight="1">
+    <row r="144" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A144" s="10"/>
       <c r="B144" s="11"/>
       <c r="C144" s="10"/>
       <c r="D144" s="11"/>
       <c r="E144" s="11"/>
     </row>
-    <row r="145" spans="1:5" ht="15.75" customHeight="1">
+    <row r="145" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A145" s="10"/>
       <c r="B145" s="11"/>
       <c r="C145" s="10"/>
       <c r="D145" s="11"/>
       <c r="E145" s="11"/>
     </row>
-    <row r="146" spans="1:5" ht="15.75" customHeight="1">
+    <row r="146" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A146" s="10"/>
       <c r="B146" s="11"/>
       <c r="C146" s="10"/>
       <c r="D146" s="11"/>
       <c r="E146" s="11"/>
     </row>
-    <row r="147" spans="1:5" ht="15.75" customHeight="1">
+    <row r="147" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A147" s="10"/>
       <c r="B147" s="11"/>
       <c r="C147" s="10"/>
       <c r="D147" s="11"/>
       <c r="E147" s="11"/>
     </row>
-    <row r="148" spans="1:5" ht="15.75" customHeight="1">
+    <row r="148" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A148" s="10"/>
       <c r="B148" s="11"/>
       <c r="C148" s="10"/>
       <c r="D148" s="11"/>
       <c r="E148" s="11"/>
     </row>
-    <row r="149" spans="1:5" ht="15.75" customHeight="1">
+    <row r="149" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A149" s="10"/>
       <c r="B149" s="11"/>
       <c r="C149" s="10"/>
       <c r="D149" s="11"/>
       <c r="E149" s="11"/>
     </row>
-    <row r="150" spans="1:5" ht="15.75" customHeight="1">
+    <row r="150" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A150" s="10"/>
       <c r="B150" s="11"/>
       <c r="C150" s="10"/>
       <c r="D150" s="11"/>
       <c r="E150" s="11"/>
     </row>
-    <row r="151" spans="1:5" ht="15.75" customHeight="1">
+    <row r="151" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A151" s="10"/>
       <c r="B151" s="11"/>
       <c r="C151" s="10"/>
       <c r="D151" s="11"/>
       <c r="E151" s="11"/>
     </row>
-    <row r="152" spans="1:5" ht="15.75" customHeight="1">
+    <row r="152" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A152" s="10"/>
       <c r="B152" s="11"/>
       <c r="C152" s="10"/>
       <c r="D152" s="11"/>
       <c r="E152" s="11"/>
     </row>
-    <row r="153" spans="1:5" ht="15.75" customHeight="1">
+    <row r="153" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A153" s="10"/>
       <c r="B153" s="11"/>
       <c r="C153" s="10"/>
       <c r="D153" s="11"/>
       <c r="E153" s="11"/>
     </row>
-    <row r="154" spans="1:5" ht="15.75" customHeight="1">
+    <row r="154" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A154" s="10"/>
       <c r="B154" s="11"/>
       <c r="C154" s="10"/>
       <c r="D154" s="11"/>
       <c r="E154" s="11"/>
     </row>
-    <row r="155" spans="1:5" ht="15.75" customHeight="1">
+    <row r="155" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A155" s="10"/>
       <c r="B155" s="11"/>
       <c r="C155" s="10"/>
       <c r="D155" s="11"/>
       <c r="E155" s="11"/>
     </row>
-    <row r="156" spans="1:5" ht="15.75" customHeight="1">
+    <row r="156" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A156" s="10"/>
       <c r="B156" s="11"/>
       <c r="C156" s="10"/>
       <c r="D156" s="11"/>
       <c r="E156" s="11"/>
     </row>
-    <row r="157" spans="1:5" ht="15.75" customHeight="1">
+    <row r="157" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A157" s="10"/>
       <c r="B157" s="11"/>
       <c r="C157" s="10"/>
       <c r="D157" s="11"/>
       <c r="E157" s="11"/>
     </row>
-    <row r="158" spans="1:5" ht="15.75" customHeight="1">
+    <row r="158" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A158" s="10"/>
       <c r="B158" s="11"/>
       <c r="C158" s="10"/>
       <c r="D158" s="11"/>
       <c r="E158" s="11"/>
     </row>
-    <row r="159" spans="1:5" ht="15.75" customHeight="1">
+    <row r="159" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A159" s="10"/>
       <c r="B159" s="11"/>
       <c r="C159" s="10"/>
       <c r="D159" s="11"/>
       <c r="E159" s="11"/>
     </row>
-    <row r="160" spans="1:5" ht="15.75" customHeight="1">
+    <row r="160" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A160" s="10"/>
       <c r="B160" s="11"/>
       <c r="C160" s="10"/>
       <c r="D160" s="11"/>
       <c r="E160" s="11"/>
     </row>
-    <row r="161" spans="1:5" ht="15.75" customHeight="1">
+    <row r="161" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A161" s="10"/>
       <c r="B161" s="11"/>
       <c r="C161" s="10"/>
       <c r="D161" s="11"/>
       <c r="E161" s="11"/>
     </row>
-    <row r="162" spans="1:5" ht="15.75" customHeight="1">
+    <row r="162" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A162" s="10"/>
       <c r="B162" s="11"/>
       <c r="C162" s="10"/>
       <c r="D162" s="11"/>
       <c r="E162" s="11"/>
     </row>
-    <row r="163" spans="1:5" ht="15.75" customHeight="1">
+    <row r="163" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A163" s="10"/>
       <c r="B163" s="11"/>
       <c r="C163" s="10"/>
       <c r="D163" s="11"/>
       <c r="E163" s="11"/>
     </row>
-    <row r="164" spans="1:5" ht="15.75" customHeight="1">
+    <row r="164" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A164" s="10"/>
       <c r="B164" s="11"/>
       <c r="C164" s="10"/>
       <c r="D164" s="11"/>
       <c r="E164" s="11"/>
     </row>
-    <row r="165" spans="1:5" ht="15.75" customHeight="1">
+    <row r="165" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A165" s="10"/>
       <c r="B165" s="11"/>
       <c r="C165" s="10"/>
       <c r="D165" s="11"/>
       <c r="E165" s="11"/>
     </row>
-    <row r="166" spans="1:5" ht="15.75" customHeight="1">
+    <row r="166" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A166" s="10"/>
       <c r="B166" s="11"/>
       <c r="C166" s="10"/>
       <c r="D166" s="11"/>
       <c r="E166" s="11"/>
     </row>
-    <row r="167" spans="1:5" ht="15.75" customHeight="1">
+    <row r="167" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A167" s="10"/>
       <c r="B167" s="11"/>
       <c r="C167" s="10"/>
       <c r="D167" s="11"/>
       <c r="E167" s="11"/>
     </row>
-    <row r="168" spans="1:5" ht="15.75" customHeight="1">
+    <row r="168" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A168" s="10"/>
       <c r="B168" s="11"/>
       <c r="C168" s="10"/>
       <c r="D168" s="11"/>
       <c r="E168" s="11"/>
     </row>
-    <row r="169" spans="1:5" ht="15.75" customHeight="1">
+    <row r="169" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A169" s="10"/>
       <c r="B169" s="11"/>
       <c r="C169" s="10"/>
       <c r="D169" s="11"/>
       <c r="E169" s="11"/>
     </row>
-    <row r="170" spans="1:5" ht="15.75" customHeight="1">
+    <row r="170" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A170" s="10"/>
       <c r="B170" s="11"/>
       <c r="C170" s="10"/>
       <c r="D170" s="11"/>
       <c r="E170" s="11"/>
     </row>
-    <row r="171" spans="1:5" ht="15.75" customHeight="1">
+    <row r="171" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A171" s="10"/>
       <c r="B171" s="11"/>
       <c r="C171" s="10"/>
       <c r="D171" s="11"/>
       <c r="E171" s="11"/>
     </row>
-    <row r="172" spans="1:5" ht="15.75" customHeight="1">
+    <row r="172" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A172" s="10"/>
       <c r="B172" s="11"/>
       <c r="C172" s="10"/>
       <c r="D172" s="11"/>
       <c r="E172" s="11"/>
     </row>
-    <row r="173" spans="1:5" ht="15.75" customHeight="1">
+    <row r="173" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A173" s="10"/>
       <c r="B173" s="11"/>
       <c r="C173" s="10"/>
       <c r="D173" s="11"/>
       <c r="E173" s="11"/>
     </row>
-    <row r="174" spans="1:5" ht="15.75" customHeight="1">
+    <row r="174" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A174" s="10"/>
       <c r="B174" s="11"/>
       <c r="C174" s="10"/>
       <c r="D174" s="11"/>
       <c r="E174" s="11"/>
     </row>
-    <row r="175" spans="1:5" ht="15.75" customHeight="1">
+    <row r="175" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A175" s="10"/>
       <c r="B175" s="11"/>
       <c r="C175" s="10"/>
       <c r="D175" s="11"/>
       <c r="E175" s="11"/>
     </row>
-    <row r="176" spans="1:5" ht="15.75" customHeight="1">
+    <row r="176" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A176" s="10"/>
       <c r="B176" s="11"/>
       <c r="C176" s="10"/>
       <c r="D176" s="11"/>
       <c r="E176" s="11"/>
     </row>
-    <row r="177" spans="1:5" ht="15.75" customHeight="1">
+    <row r="177" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A177" s="10"/>
       <c r="B177" s="11"/>
       <c r="C177" s="10"/>
       <c r="D177" s="11"/>
       <c r="E177" s="11"/>
     </row>
-    <row r="178" spans="1:5" ht="15.75" customHeight="1">
+    <row r="178" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A178" s="10"/>
       <c r="B178" s="11"/>
       <c r="C178" s="10"/>
       <c r="D178" s="11"/>
       <c r="E178" s="11"/>
     </row>
-    <row r="179" spans="1:5" ht="15.75" customHeight="1">
+    <row r="179" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A179" s="10"/>
       <c r="B179" s="11"/>
       <c r="C179" s="10"/>
       <c r="D179" s="11"/>
       <c r="E179" s="11"/>
     </row>
-    <row r="180" spans="1:5" ht="15.75" customHeight="1">
+    <row r="180" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A180" s="10"/>
       <c r="B180" s="11"/>
       <c r="C180" s="10"/>
       <c r="D180" s="11"/>
       <c r="E180" s="11"/>
     </row>
-    <row r="181" spans="1:5" ht="15.75" customHeight="1">
+    <row r="181" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A181" s="10"/>
       <c r="B181" s="11"/>
       <c r="C181" s="10"/>
       <c r="D181" s="11"/>
       <c r="E181" s="11"/>
     </row>
-    <row r="182" spans="1:5" ht="15.75" customHeight="1">
+    <row r="182" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A182" s="10"/>
       <c r="B182" s="11"/>
       <c r="C182" s="10"/>
       <c r="D182" s="11"/>
       <c r="E182" s="11"/>
     </row>
-    <row r="183" spans="1:5" ht="15.75" customHeight="1">
+    <row r="183" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A183" s="10"/>
       <c r="B183" s="11"/>
       <c r="C183" s="10"/>
       <c r="D183" s="11"/>
       <c r="E183" s="11"/>
     </row>
-    <row r="184" spans="1:5" ht="15.75" customHeight="1">
+    <row r="184" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A184" s="10"/>
       <c r="B184" s="11"/>
       <c r="C184" s="10"/>
       <c r="D184" s="11"/>
       <c r="E184" s="11"/>
     </row>
-    <row r="185" spans="1:5" ht="15.75" customHeight="1">
+    <row r="185" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A185" s="10"/>
       <c r="B185" s="11"/>
       <c r="C185" s="10"/>
       <c r="D185" s="11"/>
       <c r="E185" s="11"/>
     </row>
-    <row r="186" spans="1:5" ht="15.75" customHeight="1">
+    <row r="186" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A186" s="10"/>
       <c r="B186" s="11"/>
       <c r="C186" s="10"/>
       <c r="D186" s="11"/>
       <c r="E186" s="11"/>
     </row>
-    <row r="187" spans="1:5" ht="15.75" customHeight="1">
+    <row r="187" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A187" s="10"/>
       <c r="B187" s="11"/>
       <c r="C187" s="10"/>
       <c r="D187" s="11"/>
       <c r="E187" s="11"/>
     </row>
-    <row r="188" spans="1:5" ht="15.75" customHeight="1">
+    <row r="188" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A188" s="10"/>
       <c r="B188" s="11"/>
       <c r="C188" s="10"/>
       <c r="D188" s="11"/>
       <c r="E188" s="11"/>
     </row>
-    <row r="189" spans="1:5" ht="15.75" customHeight="1">
+    <row r="189" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A189" s="10"/>
       <c r="B189" s="11"/>
       <c r="C189" s="10"/>
       <c r="D189" s="11"/>
       <c r="E189" s="11"/>
     </row>
-    <row r="190" spans="1:5" ht="15.75" customHeight="1">
+    <row r="190" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A190" s="10"/>
       <c r="B190" s="11"/>
       <c r="C190" s="10"/>
       <c r="D190" s="11"/>
       <c r="E190" s="11"/>
     </row>
-    <row r="191" spans="1:5" ht="15.75" customHeight="1">
+    <row r="191" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A191" s="10"/>
       <c r="B191" s="11"/>
       <c r="C191" s="10"/>
       <c r="D191" s="11"/>
       <c r="E191" s="11"/>
     </row>
-    <row r="192" spans="1:5" ht="15.75" customHeight="1">
+    <row r="192" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A192" s="10"/>
       <c r="B192" s="11"/>
       <c r="C192" s="10"/>
       <c r="D192" s="11"/>
       <c r="E192" s="11"/>
     </row>
-    <row r="193" spans="1:5" ht="15.75" customHeight="1">
+    <row r="193" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A193" s="10"/>
       <c r="B193" s="11"/>
       <c r="C193" s="10"/>
       <c r="D193" s="11"/>
       <c r="E193" s="11"/>
     </row>
-    <row r="194" spans="1:5" ht="15.75" customHeight="1">
+    <row r="194" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A194" s="10"/>
       <c r="B194" s="11"/>
       <c r="C194" s="10"/>
       <c r="D194" s="11"/>
       <c r="E194" s="11"/>
     </row>
-    <row r="195" spans="1:5" ht="15.75" customHeight="1">
+    <row r="195" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A195" s="10"/>
       <c r="B195" s="11"/>
       <c r="C195" s="10"/>
       <c r="D195" s="11"/>
       <c r="E195" s="11"/>
     </row>
-    <row r="196" spans="1:5" ht="15.75" customHeight="1">
+    <row r="196" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A196" s="10"/>
       <c r="B196" s="11"/>
       <c r="C196" s="10"/>
       <c r="D196" s="11"/>
       <c r="E196" s="11"/>
     </row>
-    <row r="197" spans="1:5" ht="15.75" customHeight="1">
+    <row r="197" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A197" s="10"/>
       <c r="B197" s="11"/>
       <c r="C197" s="10"/>
       <c r="D197" s="11"/>
       <c r="E197" s="11"/>
     </row>
-    <row r="198" spans="1:5" ht="15.75" customHeight="1">
+    <row r="198" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A198" s="10"/>
       <c r="B198" s="11"/>
       <c r="C198" s="10"/>
       <c r="D198" s="11"/>
       <c r="E198" s="11"/>
     </row>
-    <row r="199" spans="1:5" ht="15.75" customHeight="1">
+    <row r="199" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A199" s="10"/>
       <c r="B199" s="11"/>
       <c r="C199" s="10"/>
       <c r="D199" s="11"/>
       <c r="E199" s="11"/>
     </row>
-    <row r="200" spans="1:5" ht="15.75" customHeight="1">
+    <row r="200" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A200" s="10"/>
       <c r="B200" s="11"/>
       <c r="C200" s="10"/>
       <c r="D200" s="11"/>
       <c r="E200" s="11"/>
     </row>
-    <row r="201" spans="1:5" ht="15.75" customHeight="1">
+    <row r="201" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A201" s="10"/>
       <c r="B201" s="11"/>
       <c r="C201" s="10"/>
       <c r="D201" s="11"/>
       <c r="E201" s="11"/>
     </row>
-    <row r="202" spans="1:5" ht="15.75" customHeight="1">
+    <row r="202" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A202" s="10"/>
       <c r="B202" s="11"/>
       <c r="C202" s="10"/>
       <c r="D202" s="11"/>
       <c r="E202" s="11"/>
     </row>
-    <row r="203" spans="1:5" ht="15.75" customHeight="1">
+    <row r="203" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A203" s="10"/>
       <c r="B203" s="11"/>
       <c r="C203" s="10"/>
       <c r="D203" s="11"/>
       <c r="E203" s="11"/>
     </row>
-    <row r="204" spans="1:5" ht="15.75" customHeight="1">
+    <row r="204" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A204" s="10"/>
       <c r="B204" s="11"/>
       <c r="C204" s="10"/>
       <c r="D204" s="11"/>
       <c r="E204" s="11"/>
     </row>
-    <row r="205" spans="1:5" ht="15.75" customHeight="1">
+    <row r="205" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A205" s="10"/>
       <c r="B205" s="11"/>
       <c r="C205" s="10"/>
       <c r="D205" s="11"/>
       <c r="E205" s="11"/>
     </row>
-    <row r="206" spans="1:5" ht="15.75" customHeight="1">
+    <row r="206" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A206" s="10"/>
       <c r="B206" s="11"/>
       <c r="C206" s="10"/>
       <c r="D206" s="11"/>
       <c r="E206" s="11"/>
     </row>
-    <row r="207" spans="1:5" ht="15.75" customHeight="1">
+    <row r="207" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A207" s="10"/>
       <c r="B207" s="11"/>
       <c r="C207" s="10"/>
       <c r="D207" s="11"/>
       <c r="E207" s="11"/>
     </row>
-    <row r="208" spans="1:5" ht="15.75" customHeight="1">
+    <row r="208" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A208" s="10"/>
       <c r="B208" s="11"/>
       <c r="C208" s="10"/>
       <c r="D208" s="11"/>
       <c r="E208" s="11"/>
     </row>
-    <row r="209" spans="1:5" ht="15.75" customHeight="1">
+    <row r="209" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A209" s="10"/>
       <c r="B209" s="11"/>
       <c r="C209" s="10"/>
       <c r="D209" s="11"/>
       <c r="E209" s="11"/>
     </row>
-    <row r="210" spans="1:5" ht="15.75" customHeight="1">
+    <row r="210" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A210" s="10"/>
       <c r="B210" s="11"/>
       <c r="C210" s="10"/>
       <c r="D210" s="11"/>
       <c r="E210" s="11"/>
     </row>
-    <row r="211" spans="1:5" ht="15.75" customHeight="1">
+    <row r="211" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A211" s="10"/>
       <c r="B211" s="11"/>
       <c r="C211" s="10"/>
       <c r="D211" s="11"/>
       <c r="E211" s="11"/>
     </row>
-    <row r="212" spans="1:5" ht="15.75" customHeight="1">
+    <row r="212" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A212" s="10"/>
       <c r="B212" s="11"/>
       <c r="C212" s="10"/>
       <c r="D212" s="11"/>
       <c r="E212" s="11"/>
     </row>
-    <row r="213" spans="1:5" ht="15.75" customHeight="1">
+    <row r="213" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A213" s="10"/>
       <c r="B213" s="11"/>
       <c r="C213" s="10"/>
       <c r="D213" s="11"/>
       <c r="E213" s="11"/>
     </row>
-    <row r="214" spans="1:5" ht="15.75" customHeight="1">
+    <row r="214" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A214" s="10"/>
       <c r="B214" s="11"/>
       <c r="C214" s="10"/>
       <c r="D214" s="11"/>
       <c r="E214" s="11"/>
     </row>
-    <row r="215" spans="1:5" ht="15.75" customHeight="1">
+    <row r="215" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A215" s="10"/>
       <c r="B215" s="11"/>
       <c r="C215" s="10"/>
       <c r="D215" s="11"/>
       <c r="E215" s="11"/>
     </row>
-    <row r="216" spans="1:5" ht="15.75" customHeight="1">
+    <row r="216" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A216" s="10"/>
       <c r="B216" s="11"/>
       <c r="C216" s="10"/>
       <c r="D216" s="11"/>
       <c r="E216" s="11"/>
     </row>
-    <row r="217" spans="1:5" ht="15.75" customHeight="1">
+    <row r="217" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A217" s="10"/>
       <c r="B217" s="11"/>
       <c r="C217" s="10"/>
       <c r="D217" s="11"/>
       <c r="E217" s="11"/>
     </row>
-    <row r="218" spans="1:5" ht="15.75" customHeight="1">
+    <row r="218" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A218" s="10"/>
       <c r="B218" s="11"/>
       <c r="C218" s="10"/>
       <c r="D218" s="11"/>
       <c r="E218" s="11"/>
     </row>
-    <row r="219" spans="1:5" ht="15.75" customHeight="1">
+    <row r="219" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A219" s="10"/>
       <c r="B219" s="11"/>
       <c r="C219" s="10"/>
       <c r="D219" s="11"/>
       <c r="E219" s="11"/>
     </row>
-    <row r="220" spans="1:5" ht="15.75" customHeight="1">
+    <row r="220" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A220" s="10"/>
       <c r="B220" s="11"/>
       <c r="C220" s="10"/>
       <c r="D220" s="11"/>
       <c r="E220" s="11"/>
     </row>
-    <row r="221" spans="1:5" ht="15.75" customHeight="1">
+    <row r="221" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A221" s="10"/>
       <c r="B221" s="11"/>
       <c r="C221" s="10"/>
       <c r="D221" s="11"/>
       <c r="E221" s="11"/>
     </row>
-    <row r="222" spans="1:5" ht="15.75" customHeight="1">
+    <row r="222" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A222" s="10"/>
       <c r="B222" s="11"/>
       <c r="C222" s="10"/>
       <c r="D222" s="11"/>
       <c r="E222" s="11"/>
     </row>
-    <row r="223" spans="1:5" ht="15.75" customHeight="1">
+    <row r="223" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A223" s="10"/>
       <c r="B223" s="11"/>
       <c r="C223" s="10"/>
       <c r="D223" s="11"/>
       <c r="E223" s="11"/>
     </row>
-    <row r="224" spans="1:5" ht="15.75" customHeight="1">
+    <row r="224" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A224" s="10"/>
       <c r="B224" s="11"/>
       <c r="C224" s="10"/>
       <c r="D224" s="11"/>
       <c r="E224" s="11"/>
     </row>
-    <row r="225" spans="1:5" ht="15.75" customHeight="1">
+    <row r="225" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A225" s="10"/>
       <c r="B225" s="11"/>
       <c r="C225" s="10"/>
       <c r="D225" s="11"/>
       <c r="E225" s="11"/>
     </row>
-    <row r="226" spans="1:5" ht="15.75" customHeight="1">
+    <row r="226" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A226" s="10"/>
       <c r="B226" s="11"/>
       <c r="C226" s="10"/>
       <c r="D226" s="11"/>
       <c r="E226" s="11"/>
     </row>
-    <row r="227" spans="1:5" ht="15.75" customHeight="1">
+    <row r="227" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A227" s="10"/>
       <c r="B227" s="11"/>
       <c r="C227" s="10"/>
       <c r="D227" s="11"/>
       <c r="E227" s="11"/>
     </row>
-    <row r="228" spans="1:5" ht="15.75" customHeight="1">
+    <row r="228" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A228" s="10"/>
       <c r="B228" s="11"/>
       <c r="C228" s="10"/>
       <c r="D228" s="11"/>
       <c r="E228" s="11"/>
     </row>
-    <row r="229" spans="1:5" ht="15.75" customHeight="1">
+    <row r="229" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A229" s="10"/>
       <c r="B229" s="11"/>
       <c r="C229" s="10"/>
       <c r="D229" s="11"/>
       <c r="E229" s="11"/>
     </row>
-    <row r="230" spans="1:5" ht="15.75" customHeight="1">
+    <row r="230" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A230" s="10"/>
       <c r="B230" s="11"/>
       <c r="C230" s="10"/>
       <c r="D230" s="11"/>
       <c r="E230" s="11"/>
     </row>
-    <row r="231" spans="1:5" ht="15.75" customHeight="1">
+    <row r="231" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A231" s="10"/>
       <c r="B231" s="11"/>
       <c r="C231" s="10"/>
       <c r="D231" s="11"/>
       <c r="E231" s="11"/>
     </row>
-    <row r="232" spans="1:5" ht="15.75" customHeight="1">
+    <row r="232" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A232" s="10"/>
       <c r="B232" s="11"/>
       <c r="C232" s="10"/>
       <c r="D232" s="11"/>
       <c r="E232" s="11"/>
     </row>
-    <row r="233" spans="1:5" ht="15.75" customHeight="1">
+    <row r="233" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A233" s="10"/>
       <c r="B233" s="11"/>
       <c r="C233" s="10"/>
       <c r="D233" s="11"/>
       <c r="E233" s="11"/>
     </row>
-    <row r="234" spans="1:5" ht="15.75" customHeight="1">
+    <row r="234" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A234" s="10"/>
       <c r="B234" s="11"/>
       <c r="C234" s="10"/>
       <c r="D234" s="11"/>
       <c r="E234" s="11"/>
     </row>
-    <row r="235" spans="1:5" ht="15.75" customHeight="1">
+    <row r="235" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A235" s="10"/>
       <c r="B235" s="11"/>
       <c r="C235" s="10"/>
       <c r="D235" s="11"/>
       <c r="E235" s="11"/>
     </row>
-    <row r="236" spans="1:5" ht="15.75" customHeight="1">
+    <row r="236" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A236" s="10"/>
       <c r="B236" s="11"/>
       <c r="C236" s="10"/>
       <c r="D236" s="11"/>
       <c r="E236" s="11"/>
     </row>
-    <row r="237" spans="1:5" ht="15.75" customHeight="1">
+    <row r="237" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A237" s="10"/>
       <c r="B237" s="11"/>
       <c r="C237" s="10"/>
       <c r="D237" s="11"/>
       <c r="E237" s="11"/>
     </row>
-    <row r="238" spans="1:5" ht="15.75" customHeight="1">
+    <row r="238" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A238" s="10"/>
       <c r="B238" s="11"/>
       <c r="C238" s="10"/>
       <c r="D238" s="11"/>
       <c r="E238" s="11"/>
     </row>
-    <row r="239" spans="1:5" ht="15.75" customHeight="1">
+    <row r="239" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A239" s="10"/>
       <c r="B239" s="11"/>
       <c r="C239" s="10"/>
       <c r="D239" s="11"/>
       <c r="E239" s="11"/>
     </row>
-    <row r="240" spans="1:5" ht="15.75" customHeight="1">
+    <row r="240" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A240" s="10"/>
       <c r="B240" s="11"/>
       <c r="C240" s="10"/>
       <c r="D240" s="11"/>
       <c r="E240" s="11"/>
     </row>
-    <row r="241" spans="1:5" ht="15.75" customHeight="1">
+    <row r="241" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A241" s="10"/>
       <c r="B241" s="11"/>
       <c r="C241" s="10"/>
       <c r="D241" s="11"/>
       <c r="E241" s="11"/>
     </row>
-    <row r="242" spans="1:5" ht="15.75" customHeight="1">
+    <row r="242" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A242" s="10"/>
       <c r="B242" s="11"/>
       <c r="C242" s="10"/>
       <c r="D242" s="11"/>
       <c r="E242" s="11"/>
     </row>
-    <row r="243" spans="1:5" ht="15.75" customHeight="1">
+    <row r="243" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A243" s="10"/>
       <c r="B243" s="11"/>
       <c r="C243" s="10"/>
       <c r="D243" s="11"/>
       <c r="E243" s="11"/>
     </row>
-    <row r="244" spans="1:5" ht="15.75" customHeight="1">
+    <row r="244" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A244" s="10"/>
       <c r="B244" s="11"/>
       <c r="C244" s="10"/>
       <c r="D244" s="11"/>
       <c r="E244" s="11"/>
     </row>
-    <row r="245" spans="1:5" ht="15.75" customHeight="1">
+    <row r="245" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A245" s="10"/>
       <c r="B245" s="11"/>
       <c r="C245" s="10"/>
       <c r="D245" s="11"/>
       <c r="E245" s="11"/>
     </row>
-    <row r="246" spans="1:5" ht="15.75" customHeight="1">
+    <row r="246" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A246" s="10"/>
       <c r="B246" s="11"/>
       <c r="C246" s="10"/>
       <c r="D246" s="11"/>
       <c r="E246" s="11"/>
     </row>
-    <row r="247" spans="1:5" ht="15.75" customHeight="1">
+    <row r="247" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A247" s="10"/>
       <c r="B247" s="11"/>
       <c r="C247" s="10"/>
       <c r="D247" s="11"/>
       <c r="E247" s="11"/>
     </row>
-    <row r="248" spans="1:5" ht="15.75" customHeight="1">
+    <row r="248" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A248" s="10"/>
       <c r="B248" s="11"/>
       <c r="C248" s="10"/>
       <c r="D248" s="11"/>
       <c r="E248" s="11"/>
     </row>
-    <row r="249" spans="1:5" ht="15.75" customHeight="1">
+    <row r="249" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A249" s="10"/>
       <c r="B249" s="11"/>
       <c r="C249" s="10"/>
       <c r="D249" s="11"/>
       <c r="E249" s="11"/>
     </row>
-    <row r="250" spans="1:5" ht="15.75" customHeight="1">
+    <row r="250" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A250" s="10"/>
       <c r="B250" s="11"/>
       <c r="C250" s="10"/>
       <c r="D250" s="11"/>
       <c r="E250" s="11"/>
     </row>
-    <row r="251" spans="1:5" ht="15.75" customHeight="1">
+    <row r="251" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A251" s="10"/>
       <c r="B251" s="11"/>
       <c r="C251" s="10"/>
       <c r="D251" s="11"/>
       <c r="E251" s="11"/>
     </row>
-    <row r="252" spans="1:5" ht="15.75" customHeight="1">
+    <row r="252" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A252" s="10"/>
       <c r="B252" s="11"/>
       <c r="C252" s="10"/>
       <c r="D252" s="11"/>
       <c r="E252" s="11"/>
     </row>
-    <row r="253" spans="1:5" ht="15.75" customHeight="1">
+    <row r="253" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A253" s="10"/>
       <c r="B253" s="11"/>
       <c r="C253" s="10"/>
       <c r="D253" s="11"/>
       <c r="E253" s="11"/>
     </row>
-    <row r="254" spans="1:5" ht="15.75" customHeight="1">
+    <row r="254" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A254" s="10"/>
       <c r="B254" s="11"/>
       <c r="C254" s="10"/>
       <c r="D254" s="11"/>
       <c r="E254" s="11"/>
     </row>
-    <row r="255" spans="1:5" ht="15.75" customHeight="1">
+    <row r="255" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A255" s="10"/>
       <c r="B255" s="11"/>
       <c r="C255" s="10"/>
       <c r="D255" s="11"/>
       <c r="E255" s="11"/>
     </row>
-    <row r="256" spans="1:5" ht="15.75" customHeight="1">
+    <row r="256" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A256" s="10"/>
       <c r="B256" s="11"/>
       <c r="C256" s="10"/>
       <c r="D256" s="11"/>
       <c r="E256" s="11"/>
     </row>
-    <row r="257" spans="1:5" ht="15.75" customHeight="1">
+    <row r="257" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A257" s="10"/>
       <c r="B257" s="11"/>
       <c r="C257" s="10"/>
       <c r="D257" s="11"/>
       <c r="E257" s="11"/>
     </row>
-    <row r="258" spans="1:5" ht="15.75" customHeight="1">
+    <row r="258" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A258" s="10"/>
       <c r="B258" s="11"/>
       <c r="C258" s="10"/>
       <c r="D258" s="11"/>
       <c r="E258" s="11"/>
     </row>
-    <row r="259" spans="1:5" ht="15.75" customHeight="1">
+    <row r="259" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A259" s="10"/>
       <c r="B259" s="11"/>
       <c r="C259" s="10"/>
       <c r="D259" s="11"/>
       <c r="E259" s="11"/>
     </row>
-    <row r="260" spans="1:5" ht="15.75" customHeight="1">
+    <row r="260" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A260" s="10"/>
       <c r="B260" s="11"/>
       <c r="C260" s="10"/>
@@ -2763,8 +2787,9 @@
     <hyperlink ref="D12" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
     <hyperlink ref="D14" r:id="rId8" xr:uid="{AC1C4612-7541-47F6-9BBC-A0AC9D798593}"/>
     <hyperlink ref="D15" r:id="rId9" xr:uid="{25B6CEF9-6B6C-4C14-84CC-92F755087F9D}"/>
+    <hyperlink ref="D16" r:id="rId10" xr:uid="{91A56197-0AD9-4DDC-B0E6-23D73D5A0A07}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId11"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Se agrega el 16 Alumno al archivo
</commit_message>
<xml_diff>
--- a/Lista de Alumnos.xlsx
+++ b/Lista de Alumnos.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Compumar\Documents\Git-Ispc\Alumnos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Titan\Desktop\ElectronicaMicro\Alumnos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93C2FFF5-8CB5-458A-B6EF-A01A295E674E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="Electronica Microcontrolada" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -30,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
   <si>
     <t>#</t>
   </si>
@@ -177,12 +176,21 @@
   </si>
   <si>
     <t>ivansky22</t>
+  </si>
+  <si>
+    <t>Rojas Cristian Ivan</t>
+  </si>
+  <si>
+    <t>rojastitanivan@gmail.com</t>
+  </si>
+  <si>
+    <t>CristianIvanRojas</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -359,7 +367,7 @@
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
-    <cellStyle name="Hyperlink" xfId="2" xr:uid="{00000000-000B-0000-0000-000008000000}"/>
+    <cellStyle name="Hyperlink" xfId="2"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -451,23 +459,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -503,23 +494,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -695,11 +669,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E260"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -984,10 +958,18 @@
       <c r="A17" s="5">
         <v>16</v>
       </c>
-      <c r="B17" s="6"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="6"/>
+      <c r="B17" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C17" s="5">
+        <v>1</v>
+      </c>
+      <c r="D17" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="18" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
@@ -2778,18 +2760,19 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D4" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="D5" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="D8" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="D9" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="D10" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="D11" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="D12" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="D14" r:id="rId8" xr:uid="{AC1C4612-7541-47F6-9BBC-A0AC9D798593}"/>
-    <hyperlink ref="D15" r:id="rId9" xr:uid="{25B6CEF9-6B6C-4C14-84CC-92F755087F9D}"/>
-    <hyperlink ref="D16" r:id="rId10" xr:uid="{91A56197-0AD9-4DDC-B0E6-23D73D5A0A07}"/>
+    <hyperlink ref="D4" r:id="rId1"/>
+    <hyperlink ref="D5" r:id="rId2"/>
+    <hyperlink ref="D8" r:id="rId3"/>
+    <hyperlink ref="D9" r:id="rId4"/>
+    <hyperlink ref="D10" r:id="rId5"/>
+    <hyperlink ref="D11" r:id="rId6"/>
+    <hyperlink ref="D12" r:id="rId7"/>
+    <hyperlink ref="D14" r:id="rId8"/>
+    <hyperlink ref="D15" r:id="rId9"/>
+    <hyperlink ref="D16" r:id="rId10"/>
+    <hyperlink ref="D17" r:id="rId11"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId11"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId12"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Se agrega el 17 Alumno al archivo
</commit_message>
<xml_diff>
--- a/Lista de Alumnos.xlsx
+++ b/Lista de Alumnos.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Titan\Desktop\ElectronicaMicro\Alumnos\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="15600" windowHeight="9240"/>
   </bookViews>
   <sheets>
     <sheet name="Electronica Microcontrolada" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="124519"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -29,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
   <si>
     <t>#</t>
   </si>
@@ -185,13 +180,22 @@
   </si>
   <si>
     <t>CristianIvanRojas</t>
+  </si>
+  <si>
+    <t>Maria Carolina Nis</t>
+  </si>
+  <si>
+    <t>caronis22@gmail.com</t>
+  </si>
+  <si>
+    <t>Mayte2008</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="9" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -426,7 +430,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -458,10 +462,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -493,7 +496,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -669,14 +671,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E260"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="6.85546875" customWidth="1"/>
     <col min="2" max="2" width="37.140625" customWidth="1"/>
@@ -686,7 +688,7 @@
     <col min="6" max="6" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" ht="27" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -703,7 +705,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="19.5" customHeight="1">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -720,7 +722,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="19.5" customHeight="1">
       <c r="A3" s="5">
         <v>2</v>
       </c>
@@ -735,7 +737,7 @@
       </c>
       <c r="E3" s="6"/>
     </row>
-    <row r="4" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="19.5" customHeight="1">
       <c r="A4" s="5">
         <v>3</v>
       </c>
@@ -752,7 +754,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="19.5" customHeight="1">
       <c r="A5" s="5">
         <v>4</v>
       </c>
@@ -769,7 +771,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="19.5" customHeight="1">
       <c r="A6" s="5">
         <v>5</v>
       </c>
@@ -786,7 +788,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="19.5" customHeight="1">
       <c r="A7" s="5">
         <v>6</v>
       </c>
@@ -803,7 +805,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="19.5" customHeight="1">
       <c r="A8" s="5">
         <v>7</v>
       </c>
@@ -820,7 +822,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="19.5" customHeight="1">
       <c r="A9" s="5">
         <v>8</v>
       </c>
@@ -837,7 +839,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="19.5" customHeight="1">
       <c r="A10" s="5">
         <v>9</v>
       </c>
@@ -852,7 +854,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="19.5" customHeight="1">
       <c r="A11" s="5">
         <v>10</v>
       </c>
@@ -869,7 +871,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="19.5" customHeight="1">
       <c r="A12" s="5">
         <v>11</v>
       </c>
@@ -886,7 +888,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" ht="19.5" customHeight="1">
       <c r="A13" s="5">
         <v>12</v>
       </c>
@@ -903,7 +905,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" ht="19.5" customHeight="1">
       <c r="A14" s="5">
         <v>13</v>
       </c>
@@ -920,7 +922,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" ht="19.5" customHeight="1">
       <c r="A15" s="5">
         <v>14</v>
       </c>
@@ -937,7 +939,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" ht="19.5" customHeight="1">
       <c r="A16" s="5">
         <v>15</v>
       </c>
@@ -954,7 +956,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" ht="19.5" customHeight="1">
       <c r="A17" s="5">
         <v>16</v>
       </c>
@@ -971,16 +973,24 @@
         <v>51</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" ht="25.5" customHeight="1">
       <c r="A18" s="5">
         <v>17</v>
       </c>
-      <c r="B18" s="6"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
-    </row>
-    <row r="19" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C18" s="5">
+        <v>4</v>
+      </c>
+      <c r="D18" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="25.5" customHeight="1">
       <c r="A19" s="5">
         <v>18</v>
       </c>
@@ -989,7 +999,7 @@
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
     </row>
-    <row r="20" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" ht="25.5" customHeight="1">
       <c r="A20" s="5">
         <v>19</v>
       </c>
@@ -998,7 +1008,7 @@
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
     </row>
-    <row r="21" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" ht="25.5" customHeight="1">
       <c r="A21" s="5">
         <v>20</v>
       </c>
@@ -1007,7 +1017,7 @@
       <c r="D21" s="6"/>
       <c r="E21" s="6"/>
     </row>
-    <row r="22" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" ht="25.5" customHeight="1">
       <c r="A22" s="5">
         <v>21</v>
       </c>
@@ -1016,7 +1026,7 @@
       <c r="D22" s="6"/>
       <c r="E22" s="6"/>
     </row>
-    <row r="23" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" ht="25.5" customHeight="1">
       <c r="A23" s="5">
         <v>22</v>
       </c>
@@ -1025,7 +1035,7 @@
       <c r="D23" s="6"/>
       <c r="E23" s="6"/>
     </row>
-    <row r="24" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" ht="25.5" customHeight="1">
       <c r="A24" s="5">
         <v>23</v>
       </c>
@@ -1034,7 +1044,7 @@
       <c r="D24" s="6"/>
       <c r="E24" s="6"/>
     </row>
-    <row r="25" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" ht="25.5" customHeight="1">
       <c r="A25" s="5">
         <v>24</v>
       </c>
@@ -1043,7 +1053,7 @@
       <c r="D25" s="6"/>
       <c r="E25" s="6"/>
     </row>
-    <row r="26" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" ht="25.5" customHeight="1">
       <c r="A26" s="5">
         <v>25</v>
       </c>
@@ -1052,7 +1062,7 @@
       <c r="D26" s="6"/>
       <c r="E26" s="6"/>
     </row>
-    <row r="27" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" ht="25.5" customHeight="1">
       <c r="A27" s="5">
         <v>26</v>
       </c>
@@ -1061,7 +1071,7 @@
       <c r="D27" s="6"/>
       <c r="E27" s="6"/>
     </row>
-    <row r="28" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" ht="25.5" customHeight="1">
       <c r="A28" s="5">
         <v>27</v>
       </c>
@@ -1070,7 +1080,7 @@
       <c r="D28" s="6"/>
       <c r="E28" s="6"/>
     </row>
-    <row r="29" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" ht="25.5" customHeight="1">
       <c r="A29" s="5">
         <v>28</v>
       </c>
@@ -1079,7 +1089,7 @@
       <c r="D29" s="6"/>
       <c r="E29" s="6"/>
     </row>
-    <row r="30" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" ht="25.5" customHeight="1">
       <c r="A30" s="5">
         <v>29</v>
       </c>
@@ -1088,7 +1098,7 @@
       <c r="D30" s="6"/>
       <c r="E30" s="6"/>
     </row>
-    <row r="31" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" ht="25.5" customHeight="1">
       <c r="A31" s="5">
         <v>30</v>
       </c>
@@ -1097,7 +1107,7 @@
       <c r="D31" s="6"/>
       <c r="E31" s="6"/>
     </row>
-    <row r="32" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" ht="25.5" customHeight="1">
       <c r="A32" s="5">
         <v>31</v>
       </c>
@@ -1106,7 +1116,7 @@
       <c r="D32" s="6"/>
       <c r="E32" s="6"/>
     </row>
-    <row r="33" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" ht="25.5" customHeight="1">
       <c r="A33" s="5">
         <v>32</v>
       </c>
@@ -1115,7 +1125,7 @@
       <c r="D33" s="6"/>
       <c r="E33" s="6"/>
     </row>
-    <row r="34" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" ht="25.5" customHeight="1">
       <c r="A34" s="5">
         <v>33</v>
       </c>
@@ -1124,7 +1134,7 @@
       <c r="D34" s="6"/>
       <c r="E34" s="6"/>
     </row>
-    <row r="35" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" ht="25.5" customHeight="1">
       <c r="A35" s="5">
         <v>34</v>
       </c>
@@ -1133,7 +1143,7 @@
       <c r="D35" s="6"/>
       <c r="E35" s="6"/>
     </row>
-    <row r="36" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" ht="25.5" customHeight="1">
       <c r="A36" s="5">
         <v>35</v>
       </c>
@@ -1142,7 +1152,7 @@
       <c r="D36" s="6"/>
       <c r="E36" s="6"/>
     </row>
-    <row r="37" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" ht="25.5" customHeight="1">
       <c r="A37" s="5">
         <v>36</v>
       </c>
@@ -1151,7 +1161,7 @@
       <c r="D37" s="6"/>
       <c r="E37" s="6"/>
     </row>
-    <row r="38" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" ht="25.5" customHeight="1">
       <c r="A38" s="5">
         <v>37</v>
       </c>
@@ -1160,7 +1170,7 @@
       <c r="D38" s="6"/>
       <c r="E38" s="6"/>
     </row>
-    <row r="39" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" ht="25.5" customHeight="1">
       <c r="A39" s="5">
         <v>38</v>
       </c>
@@ -1169,7 +1179,7 @@
       <c r="D39" s="6"/>
       <c r="E39" s="6"/>
     </row>
-    <row r="40" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" ht="25.5" customHeight="1">
       <c r="A40" s="5">
         <v>39</v>
       </c>
@@ -1178,7 +1188,7 @@
       <c r="D40" s="6"/>
       <c r="E40" s="6"/>
     </row>
-    <row r="41" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" ht="25.5" customHeight="1">
       <c r="A41" s="5">
         <v>40</v>
       </c>
@@ -1187,7 +1197,7 @@
       <c r="D41" s="6"/>
       <c r="E41" s="6"/>
     </row>
-    <row r="42" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" ht="25.5" customHeight="1">
       <c r="A42" s="5">
         <v>41</v>
       </c>
@@ -1196,7 +1206,7 @@
       <c r="D42" s="6"/>
       <c r="E42" s="6"/>
     </row>
-    <row r="43" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" ht="25.5" customHeight="1">
       <c r="A43" s="5">
         <v>42</v>
       </c>
@@ -1205,7 +1215,7 @@
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
     </row>
-    <row r="44" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" ht="25.5" customHeight="1">
       <c r="A44" s="5">
         <v>43</v>
       </c>
@@ -1214,7 +1224,7 @@
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
     </row>
-    <row r="45" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" ht="25.5" customHeight="1">
       <c r="A45" s="5">
         <v>44</v>
       </c>
@@ -1223,7 +1233,7 @@
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
     </row>
-    <row r="46" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" ht="25.5" customHeight="1">
       <c r="A46" s="5">
         <v>45</v>
       </c>
@@ -1232,7 +1242,7 @@
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
     </row>
-    <row r="47" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" ht="25.5" customHeight="1">
       <c r="A47" s="5">
         <v>46</v>
       </c>
@@ -1241,7 +1251,7 @@
       <c r="D47" s="6"/>
       <c r="E47" s="6"/>
     </row>
-    <row r="48" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" ht="25.5" customHeight="1">
       <c r="A48" s="5">
         <v>47</v>
       </c>
@@ -1250,7 +1260,7 @@
       <c r="D48" s="6"/>
       <c r="E48" s="6"/>
     </row>
-    <row r="49" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" ht="25.5" customHeight="1">
       <c r="A49" s="5">
         <v>48</v>
       </c>
@@ -1259,7 +1269,7 @@
       <c r="D49" s="6"/>
       <c r="E49" s="6"/>
     </row>
-    <row r="50" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" ht="25.5" customHeight="1">
       <c r="A50" s="5">
         <v>49</v>
       </c>
@@ -1268,7 +1278,7 @@
       <c r="D50" s="6"/>
       <c r="E50" s="6"/>
     </row>
-    <row r="51" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" ht="25.5" customHeight="1">
       <c r="A51" s="5">
         <v>50</v>
       </c>
@@ -1277,7 +1287,7 @@
       <c r="D51" s="6"/>
       <c r="E51" s="6"/>
     </row>
-    <row r="52" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" ht="25.5" customHeight="1">
       <c r="A52" s="5">
         <v>51</v>
       </c>
@@ -1286,7 +1296,7 @@
       <c r="D52" s="6"/>
       <c r="E52" s="6"/>
     </row>
-    <row r="53" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" ht="25.5" customHeight="1">
       <c r="A53" s="5">
         <v>52</v>
       </c>
@@ -1295,7 +1305,7 @@
       <c r="D53" s="6"/>
       <c r="E53" s="6"/>
     </row>
-    <row r="54" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" ht="25.5" customHeight="1">
       <c r="A54" s="5">
         <v>53</v>
       </c>
@@ -1304,7 +1314,7 @@
       <c r="D54" s="6"/>
       <c r="E54" s="6"/>
     </row>
-    <row r="55" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" ht="25.5" customHeight="1">
       <c r="A55" s="5">
         <v>54</v>
       </c>
@@ -1313,7 +1323,7 @@
       <c r="D55" s="6"/>
       <c r="E55" s="6"/>
     </row>
-    <row r="56" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" ht="25.5" customHeight="1">
       <c r="A56" s="5">
         <v>55</v>
       </c>
@@ -1322,7 +1332,7 @@
       <c r="D56" s="6"/>
       <c r="E56" s="6"/>
     </row>
-    <row r="57" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" ht="25.5" customHeight="1">
       <c r="A57" s="5">
         <v>56</v>
       </c>
@@ -1331,7 +1341,7 @@
       <c r="D57" s="6"/>
       <c r="E57" s="6"/>
     </row>
-    <row r="58" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" ht="25.5" customHeight="1">
       <c r="A58" s="5">
         <v>57</v>
       </c>
@@ -1340,7 +1350,7 @@
       <c r="D58" s="6"/>
       <c r="E58" s="6"/>
     </row>
-    <row r="59" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" ht="25.5" customHeight="1">
       <c r="A59" s="5">
         <v>58</v>
       </c>
@@ -1349,7 +1359,7 @@
       <c r="D59" s="6"/>
       <c r="E59" s="6"/>
     </row>
-    <row r="60" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" ht="25.5" customHeight="1">
       <c r="A60" s="5">
         <v>59</v>
       </c>
@@ -1358,1400 +1368,1400 @@
       <c r="D60" s="6"/>
       <c r="E60" s="6"/>
     </row>
-    <row r="61" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" ht="15.75" customHeight="1">
       <c r="A61" s="10"/>
       <c r="B61" s="11"/>
       <c r="C61" s="10"/>
       <c r="D61" s="11"/>
       <c r="E61" s="11"/>
     </row>
-    <row r="62" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" ht="15.75" customHeight="1">
       <c r="A62" s="10"/>
       <c r="B62" s="11"/>
       <c r="C62" s="10"/>
       <c r="D62" s="11"/>
       <c r="E62" s="11"/>
     </row>
-    <row r="63" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" ht="15.75" customHeight="1">
       <c r="A63" s="10"/>
       <c r="B63" s="11"/>
       <c r="C63" s="10"/>
       <c r="D63" s="11"/>
       <c r="E63" s="11"/>
     </row>
-    <row r="64" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" ht="15.75" customHeight="1">
       <c r="A64" s="10"/>
       <c r="B64" s="11"/>
       <c r="C64" s="10"/>
       <c r="D64" s="11"/>
       <c r="E64" s="11"/>
     </row>
-    <row r="65" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" ht="15.75" customHeight="1">
       <c r="A65" s="10"/>
       <c r="B65" s="11"/>
       <c r="C65" s="10"/>
       <c r="D65" s="11"/>
       <c r="E65" s="11"/>
     </row>
-    <row r="66" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" ht="15.75" customHeight="1">
       <c r="A66" s="10"/>
       <c r="B66" s="11"/>
       <c r="C66" s="10"/>
       <c r="D66" s="11"/>
       <c r="E66" s="11"/>
     </row>
-    <row r="67" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" ht="15.75" customHeight="1">
       <c r="A67" s="10"/>
       <c r="B67" s="11"/>
       <c r="C67" s="10"/>
       <c r="D67" s="11"/>
       <c r="E67" s="11"/>
     </row>
-    <row r="68" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" ht="15.75" customHeight="1">
       <c r="A68" s="10"/>
       <c r="B68" s="11"/>
       <c r="C68" s="10"/>
       <c r="D68" s="11"/>
       <c r="E68" s="11"/>
     </row>
-    <row r="69" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" ht="15.75" customHeight="1">
       <c r="A69" s="10"/>
       <c r="B69" s="11"/>
       <c r="C69" s="10"/>
       <c r="D69" s="11"/>
       <c r="E69" s="11"/>
     </row>
-    <row r="70" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" ht="15.75" customHeight="1">
       <c r="A70" s="10"/>
       <c r="B70" s="11"/>
       <c r="C70" s="10"/>
       <c r="D70" s="11"/>
       <c r="E70" s="11"/>
     </row>
-    <row r="71" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" ht="15.75" customHeight="1">
       <c r="A71" s="10"/>
       <c r="B71" s="11"/>
       <c r="C71" s="10"/>
       <c r="D71" s="11"/>
       <c r="E71" s="11"/>
     </row>
-    <row r="72" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" ht="15.75" customHeight="1">
       <c r="A72" s="10"/>
       <c r="B72" s="11"/>
       <c r="C72" s="10"/>
       <c r="D72" s="11"/>
       <c r="E72" s="11"/>
     </row>
-    <row r="73" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" ht="15.75" customHeight="1">
       <c r="A73" s="10"/>
       <c r="B73" s="11"/>
       <c r="C73" s="10"/>
       <c r="D73" s="11"/>
       <c r="E73" s="11"/>
     </row>
-    <row r="74" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" ht="15.75" customHeight="1">
       <c r="A74" s="10"/>
       <c r="B74" s="11"/>
       <c r="C74" s="10"/>
       <c r="D74" s="11"/>
       <c r="E74" s="11"/>
     </row>
-    <row r="75" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" ht="15.75" customHeight="1">
       <c r="A75" s="10"/>
       <c r="B75" s="11"/>
       <c r="C75" s="10"/>
       <c r="D75" s="11"/>
       <c r="E75" s="11"/>
     </row>
-    <row r="76" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" ht="15.75" customHeight="1">
       <c r="A76" s="10"/>
       <c r="B76" s="11"/>
       <c r="C76" s="10"/>
       <c r="D76" s="11"/>
       <c r="E76" s="11"/>
     </row>
-    <row r="77" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" ht="15.75" customHeight="1">
       <c r="A77" s="10"/>
       <c r="B77" s="11"/>
       <c r="C77" s="10"/>
       <c r="D77" s="11"/>
       <c r="E77" s="11"/>
     </row>
-    <row r="78" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" ht="15.75" customHeight="1">
       <c r="A78" s="10"/>
       <c r="B78" s="11"/>
       <c r="C78" s="10"/>
       <c r="D78" s="11"/>
       <c r="E78" s="11"/>
     </row>
-    <row r="79" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" ht="15.75" customHeight="1">
       <c r="A79" s="10"/>
       <c r="B79" s="11"/>
       <c r="C79" s="10"/>
       <c r="D79" s="11"/>
       <c r="E79" s="11"/>
     </row>
-    <row r="80" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5" ht="15.75" customHeight="1">
       <c r="A80" s="10"/>
       <c r="B80" s="11"/>
       <c r="C80" s="10"/>
       <c r="D80" s="11"/>
       <c r="E80" s="11"/>
     </row>
-    <row r="81" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5" ht="15.75" customHeight="1">
       <c r="A81" s="10"/>
       <c r="B81" s="11"/>
       <c r="C81" s="10"/>
       <c r="D81" s="11"/>
       <c r="E81" s="11"/>
     </row>
-    <row r="82" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" ht="15.75" customHeight="1">
       <c r="A82" s="10"/>
       <c r="B82" s="11"/>
       <c r="C82" s="10"/>
       <c r="D82" s="11"/>
       <c r="E82" s="11"/>
     </row>
-    <row r="83" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5" ht="15.75" customHeight="1">
       <c r="A83" s="10"/>
       <c r="B83" s="11"/>
       <c r="C83" s="10"/>
       <c r="D83" s="11"/>
       <c r="E83" s="11"/>
     </row>
-    <row r="84" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5" ht="15.75" customHeight="1">
       <c r="A84" s="10"/>
       <c r="B84" s="11"/>
       <c r="C84" s="10"/>
       <c r="D84" s="11"/>
       <c r="E84" s="11"/>
     </row>
-    <row r="85" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5" ht="15.75" customHeight="1">
       <c r="A85" s="10"/>
       <c r="B85" s="11"/>
       <c r="C85" s="10"/>
       <c r="D85" s="11"/>
       <c r="E85" s="11"/>
     </row>
-    <row r="86" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5" ht="15.75" customHeight="1">
       <c r="A86" s="10"/>
       <c r="B86" s="11"/>
       <c r="C86" s="10"/>
       <c r="D86" s="11"/>
       <c r="E86" s="11"/>
     </row>
-    <row r="87" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5" ht="15.75" customHeight="1">
       <c r="A87" s="10"/>
       <c r="B87" s="11"/>
       <c r="C87" s="10"/>
       <c r="D87" s="11"/>
       <c r="E87" s="11"/>
     </row>
-    <row r="88" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:5" ht="15.75" customHeight="1">
       <c r="A88" s="10"/>
       <c r="B88" s="11"/>
       <c r="C88" s="10"/>
       <c r="D88" s="11"/>
       <c r="E88" s="11"/>
     </row>
-    <row r="89" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:5" ht="15.75" customHeight="1">
       <c r="A89" s="10"/>
       <c r="B89" s="11"/>
       <c r="C89" s="10"/>
       <c r="D89" s="11"/>
       <c r="E89" s="11"/>
     </row>
-    <row r="90" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:5" ht="15.75" customHeight="1">
       <c r="A90" s="10"/>
       <c r="B90" s="11"/>
       <c r="C90" s="10"/>
       <c r="D90" s="11"/>
       <c r="E90" s="11"/>
     </row>
-    <row r="91" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:5" ht="15.75" customHeight="1">
       <c r="A91" s="10"/>
       <c r="B91" s="11"/>
       <c r="C91" s="10"/>
       <c r="D91" s="11"/>
       <c r="E91" s="11"/>
     </row>
-    <row r="92" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:5" ht="15.75" customHeight="1">
       <c r="A92" s="10"/>
       <c r="B92" s="11"/>
       <c r="C92" s="10"/>
       <c r="D92" s="11"/>
       <c r="E92" s="11"/>
     </row>
-    <row r="93" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:5" ht="15.75" customHeight="1">
       <c r="A93" s="10"/>
       <c r="B93" s="11"/>
       <c r="C93" s="10"/>
       <c r="D93" s="11"/>
       <c r="E93" s="11"/>
     </row>
-    <row r="94" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:5" ht="15.75" customHeight="1">
       <c r="A94" s="10"/>
       <c r="B94" s="11"/>
       <c r="C94" s="10"/>
       <c r="D94" s="11"/>
       <c r="E94" s="11"/>
     </row>
-    <row r="95" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:5" ht="15.75" customHeight="1">
       <c r="A95" s="10"/>
       <c r="B95" s="11"/>
       <c r="C95" s="10"/>
       <c r="D95" s="11"/>
       <c r="E95" s="11"/>
     </row>
-    <row r="96" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:5" ht="15.75" customHeight="1">
       <c r="A96" s="10"/>
       <c r="B96" s="11"/>
       <c r="C96" s="10"/>
       <c r="D96" s="11"/>
       <c r="E96" s="11"/>
     </row>
-    <row r="97" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:5" ht="15.75" customHeight="1">
       <c r="A97" s="10"/>
       <c r="B97" s="11"/>
       <c r="C97" s="10"/>
       <c r="D97" s="11"/>
       <c r="E97" s="11"/>
     </row>
-    <row r="98" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:5" ht="15.75" customHeight="1">
       <c r="A98" s="10"/>
       <c r="B98" s="11"/>
       <c r="C98" s="10"/>
       <c r="D98" s="11"/>
       <c r="E98" s="11"/>
     </row>
-    <row r="99" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:5" ht="15.75" customHeight="1">
       <c r="A99" s="10"/>
       <c r="B99" s="11"/>
       <c r="C99" s="10"/>
       <c r="D99" s="11"/>
       <c r="E99" s="11"/>
     </row>
-    <row r="100" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:5" ht="15.75" customHeight="1">
       <c r="A100" s="10"/>
       <c r="B100" s="11"/>
       <c r="C100" s="10"/>
       <c r="D100" s="11"/>
       <c r="E100" s="11"/>
     </row>
-    <row r="101" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:5" ht="15.75" customHeight="1">
       <c r="A101" s="10"/>
       <c r="B101" s="11"/>
       <c r="C101" s="10"/>
       <c r="D101" s="11"/>
       <c r="E101" s="11"/>
     </row>
-    <row r="102" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:5" ht="15.75" customHeight="1">
       <c r="A102" s="10"/>
       <c r="B102" s="11"/>
       <c r="C102" s="10"/>
       <c r="D102" s="11"/>
       <c r="E102" s="11"/>
     </row>
-    <row r="103" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:5" ht="15.75" customHeight="1">
       <c r="A103" s="10"/>
       <c r="B103" s="11"/>
       <c r="C103" s="10"/>
       <c r="D103" s="11"/>
       <c r="E103" s="11"/>
     </row>
-    <row r="104" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:5" ht="15.75" customHeight="1">
       <c r="A104" s="10"/>
       <c r="B104" s="11"/>
       <c r="C104" s="10"/>
       <c r="D104" s="11"/>
       <c r="E104" s="11"/>
     </row>
-    <row r="105" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:5" ht="15.75" customHeight="1">
       <c r="A105" s="10"/>
       <c r="B105" s="11"/>
       <c r="C105" s="10"/>
       <c r="D105" s="11"/>
       <c r="E105" s="11"/>
     </row>
-    <row r="106" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:5" ht="15.75" customHeight="1">
       <c r="A106" s="10"/>
       <c r="B106" s="11"/>
       <c r="C106" s="10"/>
       <c r="D106" s="11"/>
       <c r="E106" s="11"/>
     </row>
-    <row r="107" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:5" ht="15.75" customHeight="1">
       <c r="A107" s="10"/>
       <c r="B107" s="11"/>
       <c r="C107" s="10"/>
       <c r="D107" s="11"/>
       <c r="E107" s="11"/>
     </row>
-    <row r="108" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:5" ht="15.75" customHeight="1">
       <c r="A108" s="10"/>
       <c r="B108" s="11"/>
       <c r="C108" s="10"/>
       <c r="D108" s="11"/>
       <c r="E108" s="11"/>
     </row>
-    <row r="109" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:5" ht="15.75" customHeight="1">
       <c r="A109" s="10"/>
       <c r="B109" s="11"/>
       <c r="C109" s="10"/>
       <c r="D109" s="11"/>
       <c r="E109" s="11"/>
     </row>
-    <row r="110" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:5" ht="15.75" customHeight="1">
       <c r="A110" s="10"/>
       <c r="B110" s="11"/>
       <c r="C110" s="10"/>
       <c r="D110" s="11"/>
       <c r="E110" s="11"/>
     </row>
-    <row r="111" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:5" ht="15.75" customHeight="1">
       <c r="A111" s="10"/>
       <c r="B111" s="11"/>
       <c r="C111" s="10"/>
       <c r="D111" s="11"/>
       <c r="E111" s="11"/>
     </row>
-    <row r="112" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:5" ht="15.75" customHeight="1">
       <c r="A112" s="10"/>
       <c r="B112" s="11"/>
       <c r="C112" s="10"/>
       <c r="D112" s="11"/>
       <c r="E112" s="11"/>
     </row>
-    <row r="113" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:5" ht="15.75" customHeight="1">
       <c r="A113" s="10"/>
       <c r="B113" s="11"/>
       <c r="C113" s="10"/>
       <c r="D113" s="11"/>
       <c r="E113" s="11"/>
     </row>
-    <row r="114" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:5" ht="15.75" customHeight="1">
       <c r="A114" s="10"/>
       <c r="B114" s="11"/>
       <c r="C114" s="10"/>
       <c r="D114" s="11"/>
       <c r="E114" s="11"/>
     </row>
-    <row r="115" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:5" ht="15.75" customHeight="1">
       <c r="A115" s="10"/>
       <c r="B115" s="11"/>
       <c r="C115" s="10"/>
       <c r="D115" s="11"/>
       <c r="E115" s="11"/>
     </row>
-    <row r="116" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:5" ht="15.75" customHeight="1">
       <c r="A116" s="10"/>
       <c r="B116" s="11"/>
       <c r="C116" s="10"/>
       <c r="D116" s="11"/>
       <c r="E116" s="11"/>
     </row>
-    <row r="117" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:5" ht="15.75" customHeight="1">
       <c r="A117" s="10"/>
       <c r="B117" s="11"/>
       <c r="C117" s="10"/>
       <c r="D117" s="11"/>
       <c r="E117" s="11"/>
     </row>
-    <row r="118" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:5" ht="15.75" customHeight="1">
       <c r="A118" s="10"/>
       <c r="B118" s="11"/>
       <c r="C118" s="10"/>
       <c r="D118" s="11"/>
       <c r="E118" s="11"/>
     </row>
-    <row r="119" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:5" ht="15.75" customHeight="1">
       <c r="A119" s="10"/>
       <c r="B119" s="11"/>
       <c r="C119" s="10"/>
       <c r="D119" s="11"/>
       <c r="E119" s="11"/>
     </row>
-    <row r="120" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:5" ht="15.75" customHeight="1">
       <c r="A120" s="10"/>
       <c r="B120" s="11"/>
       <c r="C120" s="10"/>
       <c r="D120" s="11"/>
       <c r="E120" s="11"/>
     </row>
-    <row r="121" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:5" ht="15.75" customHeight="1">
       <c r="A121" s="10"/>
       <c r="B121" s="11"/>
       <c r="C121" s="10"/>
       <c r="D121" s="11"/>
       <c r="E121" s="11"/>
     </row>
-    <row r="122" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:5" ht="15.75" customHeight="1">
       <c r="A122" s="10"/>
       <c r="B122" s="11"/>
       <c r="C122" s="10"/>
       <c r="D122" s="11"/>
       <c r="E122" s="11"/>
     </row>
-    <row r="123" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:5" ht="15.75" customHeight="1">
       <c r="A123" s="10"/>
       <c r="B123" s="11"/>
       <c r="C123" s="10"/>
       <c r="D123" s="11"/>
       <c r="E123" s="11"/>
     </row>
-    <row r="124" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:5" ht="15.75" customHeight="1">
       <c r="A124" s="10"/>
       <c r="B124" s="11"/>
       <c r="C124" s="10"/>
       <c r="D124" s="11"/>
       <c r="E124" s="11"/>
     </row>
-    <row r="125" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:5" ht="15.75" customHeight="1">
       <c r="A125" s="10"/>
       <c r="B125" s="11"/>
       <c r="C125" s="10"/>
       <c r="D125" s="11"/>
       <c r="E125" s="11"/>
     </row>
-    <row r="126" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:5" ht="15.75" customHeight="1">
       <c r="A126" s="10"/>
       <c r="B126" s="11"/>
       <c r="C126" s="10"/>
       <c r="D126" s="11"/>
       <c r="E126" s="11"/>
     </row>
-    <row r="127" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:5" ht="15.75" customHeight="1">
       <c r="A127" s="10"/>
       <c r="B127" s="11"/>
       <c r="C127" s="10"/>
       <c r="D127" s="11"/>
       <c r="E127" s="11"/>
     </row>
-    <row r="128" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:5" ht="15.75" customHeight="1">
       <c r="A128" s="10"/>
       <c r="B128" s="11"/>
       <c r="C128" s="10"/>
       <c r="D128" s="11"/>
       <c r="E128" s="11"/>
     </row>
-    <row r="129" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:5" ht="15.75" customHeight="1">
       <c r="A129" s="10"/>
       <c r="B129" s="11"/>
       <c r="C129" s="10"/>
       <c r="D129" s="11"/>
       <c r="E129" s="11"/>
     </row>
-    <row r="130" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:5" ht="15.75" customHeight="1">
       <c r="A130" s="10"/>
       <c r="B130" s="11"/>
       <c r="C130" s="10"/>
       <c r="D130" s="11"/>
       <c r="E130" s="11"/>
     </row>
-    <row r="131" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:5" ht="15.75" customHeight="1">
       <c r="A131" s="10"/>
       <c r="B131" s="11"/>
       <c r="C131" s="10"/>
       <c r="D131" s="11"/>
       <c r="E131" s="11"/>
     </row>
-    <row r="132" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:5" ht="15.75" customHeight="1">
       <c r="A132" s="10"/>
       <c r="B132" s="11"/>
       <c r="C132" s="10"/>
       <c r="D132" s="11"/>
       <c r="E132" s="11"/>
     </row>
-    <row r="133" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:5" ht="15.75" customHeight="1">
       <c r="A133" s="10"/>
       <c r="B133" s="11"/>
       <c r="C133" s="10"/>
       <c r="D133" s="11"/>
       <c r="E133" s="11"/>
     </row>
-    <row r="134" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:5" ht="15.75" customHeight="1">
       <c r="A134" s="10"/>
       <c r="B134" s="11"/>
       <c r="C134" s="10"/>
       <c r="D134" s="11"/>
       <c r="E134" s="11"/>
     </row>
-    <row r="135" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:5" ht="15.75" customHeight="1">
       <c r="A135" s="10"/>
       <c r="B135" s="11"/>
       <c r="C135" s="10"/>
       <c r="D135" s="11"/>
       <c r="E135" s="11"/>
     </row>
-    <row r="136" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:5" ht="15.75" customHeight="1">
       <c r="A136" s="10"/>
       <c r="B136" s="11"/>
       <c r="C136" s="10"/>
       <c r="D136" s="11"/>
       <c r="E136" s="11"/>
     </row>
-    <row r="137" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:5" ht="15.75" customHeight="1">
       <c r="A137" s="10"/>
       <c r="B137" s="11"/>
       <c r="C137" s="10"/>
       <c r="D137" s="11"/>
       <c r="E137" s="11"/>
     </row>
-    <row r="138" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:5" ht="15.75" customHeight="1">
       <c r="A138" s="10"/>
       <c r="B138" s="11"/>
       <c r="C138" s="10"/>
       <c r="D138" s="11"/>
       <c r="E138" s="11"/>
     </row>
-    <row r="139" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:5" ht="15.75" customHeight="1">
       <c r="A139" s="10"/>
       <c r="B139" s="11"/>
       <c r="C139" s="10"/>
       <c r="D139" s="11"/>
       <c r="E139" s="11"/>
     </row>
-    <row r="140" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:5" ht="15.75" customHeight="1">
       <c r="A140" s="10"/>
       <c r="B140" s="11"/>
       <c r="C140" s="10"/>
       <c r="D140" s="11"/>
       <c r="E140" s="11"/>
     </row>
-    <row r="141" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:5" ht="15.75" customHeight="1">
       <c r="A141" s="10"/>
       <c r="B141" s="11"/>
       <c r="C141" s="10"/>
       <c r="D141" s="11"/>
       <c r="E141" s="11"/>
     </row>
-    <row r="142" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:5" ht="15.75" customHeight="1">
       <c r="A142" s="10"/>
       <c r="B142" s="11"/>
       <c r="C142" s="10"/>
       <c r="D142" s="11"/>
       <c r="E142" s="11"/>
     </row>
-    <row r="143" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:5" ht="15.75" customHeight="1">
       <c r="A143" s="10"/>
       <c r="B143" s="11"/>
       <c r="C143" s="10"/>
       <c r="D143" s="11"/>
       <c r="E143" s="11"/>
     </row>
-    <row r="144" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:5" ht="15.75" customHeight="1">
       <c r="A144" s="10"/>
       <c r="B144" s="11"/>
       <c r="C144" s="10"/>
       <c r="D144" s="11"/>
       <c r="E144" s="11"/>
     </row>
-    <row r="145" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:5" ht="15.75" customHeight="1">
       <c r="A145" s="10"/>
       <c r="B145" s="11"/>
       <c r="C145" s="10"/>
       <c r="D145" s="11"/>
       <c r="E145" s="11"/>
     </row>
-    <row r="146" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:5" ht="15.75" customHeight="1">
       <c r="A146" s="10"/>
       <c r="B146" s="11"/>
       <c r="C146" s="10"/>
       <c r="D146" s="11"/>
       <c r="E146" s="11"/>
     </row>
-    <row r="147" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:5" ht="15.75" customHeight="1">
       <c r="A147" s="10"/>
       <c r="B147" s="11"/>
       <c r="C147" s="10"/>
       <c r="D147" s="11"/>
       <c r="E147" s="11"/>
     </row>
-    <row r="148" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:5" ht="15.75" customHeight="1">
       <c r="A148" s="10"/>
       <c r="B148" s="11"/>
       <c r="C148" s="10"/>
       <c r="D148" s="11"/>
       <c r="E148" s="11"/>
     </row>
-    <row r="149" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:5" ht="15.75" customHeight="1">
       <c r="A149" s="10"/>
       <c r="B149" s="11"/>
       <c r="C149" s="10"/>
       <c r="D149" s="11"/>
       <c r="E149" s="11"/>
     </row>
-    <row r="150" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:5" ht="15.75" customHeight="1">
       <c r="A150" s="10"/>
       <c r="B150" s="11"/>
       <c r="C150" s="10"/>
       <c r="D150" s="11"/>
       <c r="E150" s="11"/>
     </row>
-    <row r="151" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:5" ht="15.75" customHeight="1">
       <c r="A151" s="10"/>
       <c r="B151" s="11"/>
       <c r="C151" s="10"/>
       <c r="D151" s="11"/>
       <c r="E151" s="11"/>
     </row>
-    <row r="152" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:5" ht="15.75" customHeight="1">
       <c r="A152" s="10"/>
       <c r="B152" s="11"/>
       <c r="C152" s="10"/>
       <c r="D152" s="11"/>
       <c r="E152" s="11"/>
     </row>
-    <row r="153" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:5" ht="15.75" customHeight="1">
       <c r="A153" s="10"/>
       <c r="B153" s="11"/>
       <c r="C153" s="10"/>
       <c r="D153" s="11"/>
       <c r="E153" s="11"/>
     </row>
-    <row r="154" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:5" ht="15.75" customHeight="1">
       <c r="A154" s="10"/>
       <c r="B154" s="11"/>
       <c r="C154" s="10"/>
       <c r="D154" s="11"/>
       <c r="E154" s="11"/>
     </row>
-    <row r="155" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:5" ht="15.75" customHeight="1">
       <c r="A155" s="10"/>
       <c r="B155" s="11"/>
       <c r="C155" s="10"/>
       <c r="D155" s="11"/>
       <c r="E155" s="11"/>
     </row>
-    <row r="156" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:5" ht="15.75" customHeight="1">
       <c r="A156" s="10"/>
       <c r="B156" s="11"/>
       <c r="C156" s="10"/>
       <c r="D156" s="11"/>
       <c r="E156" s="11"/>
     </row>
-    <row r="157" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:5" ht="15.75" customHeight="1">
       <c r="A157" s="10"/>
       <c r="B157" s="11"/>
       <c r="C157" s="10"/>
       <c r="D157" s="11"/>
       <c r="E157" s="11"/>
     </row>
-    <row r="158" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:5" ht="15.75" customHeight="1">
       <c r="A158" s="10"/>
       <c r="B158" s="11"/>
       <c r="C158" s="10"/>
       <c r="D158" s="11"/>
       <c r="E158" s="11"/>
     </row>
-    <row r="159" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:5" ht="15.75" customHeight="1">
       <c r="A159" s="10"/>
       <c r="B159" s="11"/>
       <c r="C159" s="10"/>
       <c r="D159" s="11"/>
       <c r="E159" s="11"/>
     </row>
-    <row r="160" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:5" ht="15.75" customHeight="1">
       <c r="A160" s="10"/>
       <c r="B160" s="11"/>
       <c r="C160" s="10"/>
       <c r="D160" s="11"/>
       <c r="E160" s="11"/>
     </row>
-    <row r="161" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:5" ht="15.75" customHeight="1">
       <c r="A161" s="10"/>
       <c r="B161" s="11"/>
       <c r="C161" s="10"/>
       <c r="D161" s="11"/>
       <c r="E161" s="11"/>
     </row>
-    <row r="162" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:5" ht="15.75" customHeight="1">
       <c r="A162" s="10"/>
       <c r="B162" s="11"/>
       <c r="C162" s="10"/>
       <c r="D162" s="11"/>
       <c r="E162" s="11"/>
     </row>
-    <row r="163" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:5" ht="15.75" customHeight="1">
       <c r="A163" s="10"/>
       <c r="B163" s="11"/>
       <c r="C163" s="10"/>
       <c r="D163" s="11"/>
       <c r="E163" s="11"/>
     </row>
-    <row r="164" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:5" ht="15.75" customHeight="1">
       <c r="A164" s="10"/>
       <c r="B164" s="11"/>
       <c r="C164" s="10"/>
       <c r="D164" s="11"/>
       <c r="E164" s="11"/>
     </row>
-    <row r="165" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:5" ht="15.75" customHeight="1">
       <c r="A165" s="10"/>
       <c r="B165" s="11"/>
       <c r="C165" s="10"/>
       <c r="D165" s="11"/>
       <c r="E165" s="11"/>
     </row>
-    <row r="166" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:5" ht="15.75" customHeight="1">
       <c r="A166" s="10"/>
       <c r="B166" s="11"/>
       <c r="C166" s="10"/>
       <c r="D166" s="11"/>
       <c r="E166" s="11"/>
     </row>
-    <row r="167" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:5" ht="15.75" customHeight="1">
       <c r="A167" s="10"/>
       <c r="B167" s="11"/>
       <c r="C167" s="10"/>
       <c r="D167" s="11"/>
       <c r="E167" s="11"/>
     </row>
-    <row r="168" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:5" ht="15.75" customHeight="1">
       <c r="A168" s="10"/>
       <c r="B168" s="11"/>
       <c r="C168" s="10"/>
       <c r="D168" s="11"/>
       <c r="E168" s="11"/>
     </row>
-    <row r="169" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:5" ht="15.75" customHeight="1">
       <c r="A169" s="10"/>
       <c r="B169" s="11"/>
       <c r="C169" s="10"/>
       <c r="D169" s="11"/>
       <c r="E169" s="11"/>
     </row>
-    <row r="170" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:5" ht="15.75" customHeight="1">
       <c r="A170" s="10"/>
       <c r="B170" s="11"/>
       <c r="C170" s="10"/>
       <c r="D170" s="11"/>
       <c r="E170" s="11"/>
     </row>
-    <row r="171" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:5" ht="15.75" customHeight="1">
       <c r="A171" s="10"/>
       <c r="B171" s="11"/>
       <c r="C171" s="10"/>
       <c r="D171" s="11"/>
       <c r="E171" s="11"/>
     </row>
-    <row r="172" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:5" ht="15.75" customHeight="1">
       <c r="A172" s="10"/>
       <c r="B172" s="11"/>
       <c r="C172" s="10"/>
       <c r="D172" s="11"/>
       <c r="E172" s="11"/>
     </row>
-    <row r="173" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:5" ht="15.75" customHeight="1">
       <c r="A173" s="10"/>
       <c r="B173" s="11"/>
       <c r="C173" s="10"/>
       <c r="D173" s="11"/>
       <c r="E173" s="11"/>
     </row>
-    <row r="174" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:5" ht="15.75" customHeight="1">
       <c r="A174" s="10"/>
       <c r="B174" s="11"/>
       <c r="C174" s="10"/>
       <c r="D174" s="11"/>
       <c r="E174" s="11"/>
     </row>
-    <row r="175" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:5" ht="15.75" customHeight="1">
       <c r="A175" s="10"/>
       <c r="B175" s="11"/>
       <c r="C175" s="10"/>
       <c r="D175" s="11"/>
       <c r="E175" s="11"/>
     </row>
-    <row r="176" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:5" ht="15.75" customHeight="1">
       <c r="A176" s="10"/>
       <c r="B176" s="11"/>
       <c r="C176" s="10"/>
       <c r="D176" s="11"/>
       <c r="E176" s="11"/>
     </row>
-    <row r="177" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:5" ht="15.75" customHeight="1">
       <c r="A177" s="10"/>
       <c r="B177" s="11"/>
       <c r="C177" s="10"/>
       <c r="D177" s="11"/>
       <c r="E177" s="11"/>
     </row>
-    <row r="178" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:5" ht="15.75" customHeight="1">
       <c r="A178" s="10"/>
       <c r="B178" s="11"/>
       <c r="C178" s="10"/>
       <c r="D178" s="11"/>
       <c r="E178" s="11"/>
     </row>
-    <row r="179" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:5" ht="15.75" customHeight="1">
       <c r="A179" s="10"/>
       <c r="B179" s="11"/>
       <c r="C179" s="10"/>
       <c r="D179" s="11"/>
       <c r="E179" s="11"/>
     </row>
-    <row r="180" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:5" ht="15.75" customHeight="1">
       <c r="A180" s="10"/>
       <c r="B180" s="11"/>
       <c r="C180" s="10"/>
       <c r="D180" s="11"/>
       <c r="E180" s="11"/>
     </row>
-    <row r="181" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:5" ht="15.75" customHeight="1">
       <c r="A181" s="10"/>
       <c r="B181" s="11"/>
       <c r="C181" s="10"/>
       <c r="D181" s="11"/>
       <c r="E181" s="11"/>
     </row>
-    <row r="182" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:5" ht="15.75" customHeight="1">
       <c r="A182" s="10"/>
       <c r="B182" s="11"/>
       <c r="C182" s="10"/>
       <c r="D182" s="11"/>
       <c r="E182" s="11"/>
     </row>
-    <row r="183" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:5" ht="15.75" customHeight="1">
       <c r="A183" s="10"/>
       <c r="B183" s="11"/>
       <c r="C183" s="10"/>
       <c r="D183" s="11"/>
       <c r="E183" s="11"/>
     </row>
-    <row r="184" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:5" ht="15.75" customHeight="1">
       <c r="A184" s="10"/>
       <c r="B184" s="11"/>
       <c r="C184" s="10"/>
       <c r="D184" s="11"/>
       <c r="E184" s="11"/>
     </row>
-    <row r="185" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:5" ht="15.75" customHeight="1">
       <c r="A185" s="10"/>
       <c r="B185" s="11"/>
       <c r="C185" s="10"/>
       <c r="D185" s="11"/>
       <c r="E185" s="11"/>
     </row>
-    <row r="186" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:5" ht="15.75" customHeight="1">
       <c r="A186" s="10"/>
       <c r="B186" s="11"/>
       <c r="C186" s="10"/>
       <c r="D186" s="11"/>
       <c r="E186" s="11"/>
     </row>
-    <row r="187" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:5" ht="15.75" customHeight="1">
       <c r="A187" s="10"/>
       <c r="B187" s="11"/>
       <c r="C187" s="10"/>
       <c r="D187" s="11"/>
       <c r="E187" s="11"/>
     </row>
-    <row r="188" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:5" ht="15.75" customHeight="1">
       <c r="A188" s="10"/>
       <c r="B188" s="11"/>
       <c r="C188" s="10"/>
       <c r="D188" s="11"/>
       <c r="E188" s="11"/>
     </row>
-    <row r="189" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:5" ht="15.75" customHeight="1">
       <c r="A189" s="10"/>
       <c r="B189" s="11"/>
       <c r="C189" s="10"/>
       <c r="D189" s="11"/>
       <c r="E189" s="11"/>
     </row>
-    <row r="190" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:5" ht="15.75" customHeight="1">
       <c r="A190" s="10"/>
       <c r="B190" s="11"/>
       <c r="C190" s="10"/>
       <c r="D190" s="11"/>
       <c r="E190" s="11"/>
     </row>
-    <row r="191" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:5" ht="15.75" customHeight="1">
       <c r="A191" s="10"/>
       <c r="B191" s="11"/>
       <c r="C191" s="10"/>
       <c r="D191" s="11"/>
       <c r="E191" s="11"/>
     </row>
-    <row r="192" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:5" ht="15.75" customHeight="1">
       <c r="A192" s="10"/>
       <c r="B192" s="11"/>
       <c r="C192" s="10"/>
       <c r="D192" s="11"/>
       <c r="E192" s="11"/>
     </row>
-    <row r="193" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:5" ht="15.75" customHeight="1">
       <c r="A193" s="10"/>
       <c r="B193" s="11"/>
       <c r="C193" s="10"/>
       <c r="D193" s="11"/>
       <c r="E193" s="11"/>
     </row>
-    <row r="194" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:5" ht="15.75" customHeight="1">
       <c r="A194" s="10"/>
       <c r="B194" s="11"/>
       <c r="C194" s="10"/>
       <c r="D194" s="11"/>
       <c r="E194" s="11"/>
     </row>
-    <row r="195" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:5" ht="15.75" customHeight="1">
       <c r="A195" s="10"/>
       <c r="B195" s="11"/>
       <c r="C195" s="10"/>
       <c r="D195" s="11"/>
       <c r="E195" s="11"/>
     </row>
-    <row r="196" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:5" ht="15.75" customHeight="1">
       <c r="A196" s="10"/>
       <c r="B196" s="11"/>
       <c r="C196" s="10"/>
       <c r="D196" s="11"/>
       <c r="E196" s="11"/>
     </row>
-    <row r="197" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:5" ht="15.75" customHeight="1">
       <c r="A197" s="10"/>
       <c r="B197" s="11"/>
       <c r="C197" s="10"/>
       <c r="D197" s="11"/>
       <c r="E197" s="11"/>
     </row>
-    <row r="198" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:5" ht="15.75" customHeight="1">
       <c r="A198" s="10"/>
       <c r="B198" s="11"/>
       <c r="C198" s="10"/>
       <c r="D198" s="11"/>
       <c r="E198" s="11"/>
     </row>
-    <row r="199" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:5" ht="15.75" customHeight="1">
       <c r="A199" s="10"/>
       <c r="B199" s="11"/>
       <c r="C199" s="10"/>
       <c r="D199" s="11"/>
       <c r="E199" s="11"/>
     </row>
-    <row r="200" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:5" ht="15.75" customHeight="1">
       <c r="A200" s="10"/>
       <c r="B200" s="11"/>
       <c r="C200" s="10"/>
       <c r="D200" s="11"/>
       <c r="E200" s="11"/>
     </row>
-    <row r="201" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:5" ht="15.75" customHeight="1">
       <c r="A201" s="10"/>
       <c r="B201" s="11"/>
       <c r="C201" s="10"/>
       <c r="D201" s="11"/>
       <c r="E201" s="11"/>
     </row>
-    <row r="202" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:5" ht="15.75" customHeight="1">
       <c r="A202" s="10"/>
       <c r="B202" s="11"/>
       <c r="C202" s="10"/>
       <c r="D202" s="11"/>
       <c r="E202" s="11"/>
     </row>
-    <row r="203" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:5" ht="15.75" customHeight="1">
       <c r="A203" s="10"/>
       <c r="B203" s="11"/>
       <c r="C203" s="10"/>
       <c r="D203" s="11"/>
       <c r="E203" s="11"/>
     </row>
-    <row r="204" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:5" ht="15.75" customHeight="1">
       <c r="A204" s="10"/>
       <c r="B204" s="11"/>
       <c r="C204" s="10"/>
       <c r="D204" s="11"/>
       <c r="E204" s="11"/>
     </row>
-    <row r="205" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:5" ht="15.75" customHeight="1">
       <c r="A205" s="10"/>
       <c r="B205" s="11"/>
       <c r="C205" s="10"/>
       <c r="D205" s="11"/>
       <c r="E205" s="11"/>
     </row>
-    <row r="206" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:5" ht="15.75" customHeight="1">
       <c r="A206" s="10"/>
       <c r="B206" s="11"/>
       <c r="C206" s="10"/>
       <c r="D206" s="11"/>
       <c r="E206" s="11"/>
     </row>
-    <row r="207" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:5" ht="15.75" customHeight="1">
       <c r="A207" s="10"/>
       <c r="B207" s="11"/>
       <c r="C207" s="10"/>
       <c r="D207" s="11"/>
       <c r="E207" s="11"/>
     </row>
-    <row r="208" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:5" ht="15.75" customHeight="1">
       <c r="A208" s="10"/>
       <c r="B208" s="11"/>
       <c r="C208" s="10"/>
       <c r="D208" s="11"/>
       <c r="E208" s="11"/>
     </row>
-    <row r="209" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:5" ht="15.75" customHeight="1">
       <c r="A209" s="10"/>
       <c r="B209" s="11"/>
       <c r="C209" s="10"/>
       <c r="D209" s="11"/>
       <c r="E209" s="11"/>
     </row>
-    <row r="210" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:5" ht="15.75" customHeight="1">
       <c r="A210" s="10"/>
       <c r="B210" s="11"/>
       <c r="C210" s="10"/>
       <c r="D210" s="11"/>
       <c r="E210" s="11"/>
     </row>
-    <row r="211" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:5" ht="15.75" customHeight="1">
       <c r="A211" s="10"/>
       <c r="B211" s="11"/>
       <c r="C211" s="10"/>
       <c r="D211" s="11"/>
       <c r="E211" s="11"/>
     </row>
-    <row r="212" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:5" ht="15.75" customHeight="1">
       <c r="A212" s="10"/>
       <c r="B212" s="11"/>
       <c r="C212" s="10"/>
       <c r="D212" s="11"/>
       <c r="E212" s="11"/>
     </row>
-    <row r="213" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:5" ht="15.75" customHeight="1">
       <c r="A213" s="10"/>
       <c r="B213" s="11"/>
       <c r="C213" s="10"/>
       <c r="D213" s="11"/>
       <c r="E213" s="11"/>
     </row>
-    <row r="214" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:5" ht="15.75" customHeight="1">
       <c r="A214" s="10"/>
       <c r="B214" s="11"/>
       <c r="C214" s="10"/>
       <c r="D214" s="11"/>
       <c r="E214" s="11"/>
     </row>
-    <row r="215" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:5" ht="15.75" customHeight="1">
       <c r="A215" s="10"/>
       <c r="B215" s="11"/>
       <c r="C215" s="10"/>
       <c r="D215" s="11"/>
       <c r="E215" s="11"/>
     </row>
-    <row r="216" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:5" ht="15.75" customHeight="1">
       <c r="A216" s="10"/>
       <c r="B216" s="11"/>
       <c r="C216" s="10"/>
       <c r="D216" s="11"/>
       <c r="E216" s="11"/>
     </row>
-    <row r="217" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:5" ht="15.75" customHeight="1">
       <c r="A217" s="10"/>
       <c r="B217" s="11"/>
       <c r="C217" s="10"/>
       <c r="D217" s="11"/>
       <c r="E217" s="11"/>
     </row>
-    <row r="218" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:5" ht="15.75" customHeight="1">
       <c r="A218" s="10"/>
       <c r="B218" s="11"/>
       <c r="C218" s="10"/>
       <c r="D218" s="11"/>
       <c r="E218" s="11"/>
     </row>
-    <row r="219" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:5" ht="15.75" customHeight="1">
       <c r="A219" s="10"/>
       <c r="B219" s="11"/>
       <c r="C219" s="10"/>
       <c r="D219" s="11"/>
       <c r="E219" s="11"/>
     </row>
-    <row r="220" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:5" ht="15.75" customHeight="1">
       <c r="A220" s="10"/>
       <c r="B220" s="11"/>
       <c r="C220" s="10"/>
       <c r="D220" s="11"/>
       <c r="E220" s="11"/>
     </row>
-    <row r="221" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:5" ht="15.75" customHeight="1">
       <c r="A221" s="10"/>
       <c r="B221" s="11"/>
       <c r="C221" s="10"/>
       <c r="D221" s="11"/>
       <c r="E221" s="11"/>
     </row>
-    <row r="222" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:5" ht="15.75" customHeight="1">
       <c r="A222" s="10"/>
       <c r="B222" s="11"/>
       <c r="C222" s="10"/>
       <c r="D222" s="11"/>
       <c r="E222" s="11"/>
     </row>
-    <row r="223" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:5" ht="15.75" customHeight="1">
       <c r="A223" s="10"/>
       <c r="B223" s="11"/>
       <c r="C223" s="10"/>
       <c r="D223" s="11"/>
       <c r="E223" s="11"/>
     </row>
-    <row r="224" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:5" ht="15.75" customHeight="1">
       <c r="A224" s="10"/>
       <c r="B224" s="11"/>
       <c r="C224" s="10"/>
       <c r="D224" s="11"/>
       <c r="E224" s="11"/>
     </row>
-    <row r="225" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:5" ht="15.75" customHeight="1">
       <c r="A225" s="10"/>
       <c r="B225" s="11"/>
       <c r="C225" s="10"/>
       <c r="D225" s="11"/>
       <c r="E225" s="11"/>
     </row>
-    <row r="226" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:5" ht="15.75" customHeight="1">
       <c r="A226" s="10"/>
       <c r="B226" s="11"/>
       <c r="C226" s="10"/>
       <c r="D226" s="11"/>
       <c r="E226" s="11"/>
     </row>
-    <row r="227" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:5" ht="15.75" customHeight="1">
       <c r="A227" s="10"/>
       <c r="B227" s="11"/>
       <c r="C227" s="10"/>
       <c r="D227" s="11"/>
       <c r="E227" s="11"/>
     </row>
-    <row r="228" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:5" ht="15.75" customHeight="1">
       <c r="A228" s="10"/>
       <c r="B228" s="11"/>
       <c r="C228" s="10"/>
       <c r="D228" s="11"/>
       <c r="E228" s="11"/>
     </row>
-    <row r="229" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:5" ht="15.75" customHeight="1">
       <c r="A229" s="10"/>
       <c r="B229" s="11"/>
       <c r="C229" s="10"/>
       <c r="D229" s="11"/>
       <c r="E229" s="11"/>
     </row>
-    <row r="230" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:5" ht="15.75" customHeight="1">
       <c r="A230" s="10"/>
       <c r="B230" s="11"/>
       <c r="C230" s="10"/>
       <c r="D230" s="11"/>
       <c r="E230" s="11"/>
     </row>
-    <row r="231" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:5" ht="15.75" customHeight="1">
       <c r="A231" s="10"/>
       <c r="B231" s="11"/>
       <c r="C231" s="10"/>
       <c r="D231" s="11"/>
       <c r="E231" s="11"/>
     </row>
-    <row r="232" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:5" ht="15.75" customHeight="1">
       <c r="A232" s="10"/>
       <c r="B232" s="11"/>
       <c r="C232" s="10"/>
       <c r="D232" s="11"/>
       <c r="E232" s="11"/>
     </row>
-    <row r="233" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:5" ht="15.75" customHeight="1">
       <c r="A233" s="10"/>
       <c r="B233" s="11"/>
       <c r="C233" s="10"/>
       <c r="D233" s="11"/>
       <c r="E233" s="11"/>
     </row>
-    <row r="234" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:5" ht="15.75" customHeight="1">
       <c r="A234" s="10"/>
       <c r="B234" s="11"/>
       <c r="C234" s="10"/>
       <c r="D234" s="11"/>
       <c r="E234" s="11"/>
     </row>
-    <row r="235" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:5" ht="15.75" customHeight="1">
       <c r="A235" s="10"/>
       <c r="B235" s="11"/>
       <c r="C235" s="10"/>
       <c r="D235" s="11"/>
       <c r="E235" s="11"/>
     </row>
-    <row r="236" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:5" ht="15.75" customHeight="1">
       <c r="A236" s="10"/>
       <c r="B236" s="11"/>
       <c r="C236" s="10"/>
       <c r="D236" s="11"/>
       <c r="E236" s="11"/>
     </row>
-    <row r="237" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:5" ht="15.75" customHeight="1">
       <c r="A237" s="10"/>
       <c r="B237" s="11"/>
       <c r="C237" s="10"/>
       <c r="D237" s="11"/>
       <c r="E237" s="11"/>
     </row>
-    <row r="238" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:5" ht="15.75" customHeight="1">
       <c r="A238" s="10"/>
       <c r="B238" s="11"/>
       <c r="C238" s="10"/>
       <c r="D238" s="11"/>
       <c r="E238" s="11"/>
     </row>
-    <row r="239" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:5" ht="15.75" customHeight="1">
       <c r="A239" s="10"/>
       <c r="B239" s="11"/>
       <c r="C239" s="10"/>
       <c r="D239" s="11"/>
       <c r="E239" s="11"/>
     </row>
-    <row r="240" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:5" ht="15.75" customHeight="1">
       <c r="A240" s="10"/>
       <c r="B240" s="11"/>
       <c r="C240" s="10"/>
       <c r="D240" s="11"/>
       <c r="E240" s="11"/>
     </row>
-    <row r="241" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:5" ht="15.75" customHeight="1">
       <c r="A241" s="10"/>
       <c r="B241" s="11"/>
       <c r="C241" s="10"/>
       <c r="D241" s="11"/>
       <c r="E241" s="11"/>
     </row>
-    <row r="242" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:5" ht="15.75" customHeight="1">
       <c r="A242" s="10"/>
       <c r="B242" s="11"/>
       <c r="C242" s="10"/>
       <c r="D242" s="11"/>
       <c r="E242" s="11"/>
     </row>
-    <row r="243" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:5" ht="15.75" customHeight="1">
       <c r="A243" s="10"/>
       <c r="B243" s="11"/>
       <c r="C243" s="10"/>
       <c r="D243" s="11"/>
       <c r="E243" s="11"/>
     </row>
-    <row r="244" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:5" ht="15.75" customHeight="1">
       <c r="A244" s="10"/>
       <c r="B244" s="11"/>
       <c r="C244" s="10"/>
       <c r="D244" s="11"/>
       <c r="E244" s="11"/>
     </row>
-    <row r="245" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:5" ht="15.75" customHeight="1">
       <c r="A245" s="10"/>
       <c r="B245" s="11"/>
       <c r="C245" s="10"/>
       <c r="D245" s="11"/>
       <c r="E245" s="11"/>
     </row>
-    <row r="246" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:5" ht="15.75" customHeight="1">
       <c r="A246" s="10"/>
       <c r="B246" s="11"/>
       <c r="C246" s="10"/>
       <c r="D246" s="11"/>
       <c r="E246" s="11"/>
     </row>
-    <row r="247" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:5" ht="15.75" customHeight="1">
       <c r="A247" s="10"/>
       <c r="B247" s="11"/>
       <c r="C247" s="10"/>
       <c r="D247" s="11"/>
       <c r="E247" s="11"/>
     </row>
-    <row r="248" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:5" ht="15.75" customHeight="1">
       <c r="A248" s="10"/>
       <c r="B248" s="11"/>
       <c r="C248" s="10"/>
       <c r="D248" s="11"/>
       <c r="E248" s="11"/>
     </row>
-    <row r="249" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:5" ht="15.75" customHeight="1">
       <c r="A249" s="10"/>
       <c r="B249" s="11"/>
       <c r="C249" s="10"/>
       <c r="D249" s="11"/>
       <c r="E249" s="11"/>
     </row>
-    <row r="250" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:5" ht="15.75" customHeight="1">
       <c r="A250" s="10"/>
       <c r="B250" s="11"/>
       <c r="C250" s="10"/>
       <c r="D250" s="11"/>
       <c r="E250" s="11"/>
     </row>
-    <row r="251" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:5" ht="15.75" customHeight="1">
       <c r="A251" s="10"/>
       <c r="B251" s="11"/>
       <c r="C251" s="10"/>
       <c r="D251" s="11"/>
       <c r="E251" s="11"/>
     </row>
-    <row r="252" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:5" ht="15.75" customHeight="1">
       <c r="A252" s="10"/>
       <c r="B252" s="11"/>
       <c r="C252" s="10"/>
       <c r="D252" s="11"/>
       <c r="E252" s="11"/>
     </row>
-    <row r="253" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:5" ht="15.75" customHeight="1">
       <c r="A253" s="10"/>
       <c r="B253" s="11"/>
       <c r="C253" s="10"/>
       <c r="D253" s="11"/>
       <c r="E253" s="11"/>
     </row>
-    <row r="254" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:5" ht="15.75" customHeight="1">
       <c r="A254" s="10"/>
       <c r="B254" s="11"/>
       <c r="C254" s="10"/>
       <c r="D254" s="11"/>
       <c r="E254" s="11"/>
     </row>
-    <row r="255" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:5" ht="15.75" customHeight="1">
       <c r="A255" s="10"/>
       <c r="B255" s="11"/>
       <c r="C255" s="10"/>
       <c r="D255" s="11"/>
       <c r="E255" s="11"/>
     </row>
-    <row r="256" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:5" ht="15.75" customHeight="1">
       <c r="A256" s="10"/>
       <c r="B256" s="11"/>
       <c r="C256" s="10"/>
       <c r="D256" s="11"/>
       <c r="E256" s="11"/>
     </row>
-    <row r="257" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:5" ht="15.75" customHeight="1">
       <c r="A257" s="10"/>
       <c r="B257" s="11"/>
       <c r="C257" s="10"/>
       <c r="D257" s="11"/>
       <c r="E257" s="11"/>
     </row>
-    <row r="258" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:5" ht="15.75" customHeight="1">
       <c r="A258" s="10"/>
       <c r="B258" s="11"/>
       <c r="C258" s="10"/>
       <c r="D258" s="11"/>
       <c r="E258" s="11"/>
     </row>
-    <row r="259" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:5" ht="15.75" customHeight="1">
       <c r="A259" s="10"/>
       <c r="B259" s="11"/>
       <c r="C259" s="10"/>
       <c r="D259" s="11"/>
       <c r="E259" s="11"/>
     </row>
-    <row r="260" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:5" ht="15.75" customHeight="1">
       <c r="A260" s="10"/>
       <c r="B260" s="11"/>
       <c r="C260" s="10"/>
@@ -2771,8 +2781,9 @@
     <hyperlink ref="D15" r:id="rId9"/>
     <hyperlink ref="D16" r:id="rId10"/>
     <hyperlink ref="D17" r:id="rId11"/>
+    <hyperlink ref="D18" r:id="rId12"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId12"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId13"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Se agrega el 18 Alumno al archivo
</commit_message>
<xml_diff>
--- a/Lista de Alumnos.xlsx
+++ b/Lista de Alumnos.xlsx
@@ -1,30 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CARO-FER\Desktop\Alumnos\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A844082-029F-4AEE-8583-533DB5640F08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="15600" windowHeight="9240"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="15576" windowHeight="8832" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Electronica Microcontrolada" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
   <si>
     <t>#</t>
   </si>
@@ -189,13 +185,22 @@
   </si>
   <si>
     <t>Mayte2008</t>
+  </si>
+  <si>
+    <t>Fernando Javier Vexenat</t>
+  </si>
+  <si>
+    <t>fernandovexenat@gmail.com</t>
+  </si>
+  <si>
+    <t>Fvexe82</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -371,11 +376,39 @@
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
-    <cellStyle name="Hyperlink" xfId="2"/>
+    <cellStyle name="Hyperlink" xfId="2" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{DD085388-3F85-4BAF-9721-319BA6098B72}">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -430,7 +463,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -462,9 +495,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -496,6 +547,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -671,24 +740,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E260"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
       <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.85546875" customWidth="1"/>
-    <col min="2" max="2" width="37.140625" customWidth="1"/>
-    <col min="3" max="3" width="10.5703125" customWidth="1"/>
+    <col min="1" max="1" width="6.88671875" customWidth="1"/>
+    <col min="2" max="2" width="37.109375" customWidth="1"/>
+    <col min="3" max="3" width="10.5546875" customWidth="1"/>
     <col min="4" max="4" width="31" customWidth="1"/>
     <col min="5" max="5" width="29" customWidth="1"/>
-    <col min="6" max="6" width="8.7109375" customWidth="1"/>
+    <col min="6" max="6" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="27" customHeight="1">
+    <row r="1" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -705,7 +774,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="19.5" customHeight="1">
+    <row r="2" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -722,7 +791,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="19.5" customHeight="1">
+    <row r="3" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5">
         <v>2</v>
       </c>
@@ -737,7 +806,7 @@
       </c>
       <c r="E3" s="6"/>
     </row>
-    <row r="4" spans="1:5" ht="19.5" customHeight="1">
+    <row r="4" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5">
         <v>3</v>
       </c>
@@ -754,7 +823,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="19.5" customHeight="1">
+    <row r="5" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="5">
         <v>4</v>
       </c>
@@ -771,7 +840,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="19.5" customHeight="1">
+    <row r="6" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="5">
         <v>5</v>
       </c>
@@ -788,7 +857,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="19.5" customHeight="1">
+    <row r="7" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="5">
         <v>6</v>
       </c>
@@ -805,7 +874,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="19.5" customHeight="1">
+    <row r="8" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5">
         <v>7</v>
       </c>
@@ -822,7 +891,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="19.5" customHeight="1">
+    <row r="9" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="5">
         <v>8</v>
       </c>
@@ -839,7 +908,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="19.5" customHeight="1">
+    <row r="10" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="5">
         <v>9</v>
       </c>
@@ -854,7 +923,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="19.5" customHeight="1">
+    <row r="11" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="5">
         <v>10</v>
       </c>
@@ -871,7 +940,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="19.5" customHeight="1">
+    <row r="12" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="5">
         <v>11</v>
       </c>
@@ -888,7 +957,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="19.5" customHeight="1">
+    <row r="13" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="5">
         <v>12</v>
       </c>
@@ -905,7 +974,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="19.5" customHeight="1">
+    <row r="14" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="5">
         <v>13</v>
       </c>
@@ -922,7 +991,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="19.5" customHeight="1">
+    <row r="15" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="5">
         <v>14</v>
       </c>
@@ -939,7 +1008,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="19.5" customHeight="1">
+    <row r="16" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="5">
         <v>15</v>
       </c>
@@ -956,7 +1025,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="19.5" customHeight="1">
+    <row r="17" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="5">
         <v>16</v>
       </c>
@@ -973,7 +1042,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="25.5" customHeight="1">
+    <row r="18" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="5">
         <v>17</v>
       </c>
@@ -990,16 +1059,24 @@
         <v>54</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="25.5" customHeight="1">
+    <row r="19" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="5">
         <v>18</v>
       </c>
-      <c r="B19" s="6"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="6"/>
-    </row>
-    <row r="20" spans="1:5" ht="25.5" customHeight="1">
+      <c r="B19" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C19" s="5">
+        <v>1</v>
+      </c>
+      <c r="D19" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="5">
         <v>19</v>
       </c>
@@ -1008,7 +1085,7 @@
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
     </row>
-    <row r="21" spans="1:5" ht="25.5" customHeight="1">
+    <row r="21" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="5">
         <v>20</v>
       </c>
@@ -1017,7 +1094,7 @@
       <c r="D21" s="6"/>
       <c r="E21" s="6"/>
     </row>
-    <row r="22" spans="1:5" ht="25.5" customHeight="1">
+    <row r="22" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="5">
         <v>21</v>
       </c>
@@ -1026,7 +1103,7 @@
       <c r="D22" s="6"/>
       <c r="E22" s="6"/>
     </row>
-    <row r="23" spans="1:5" ht="25.5" customHeight="1">
+    <row r="23" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="5">
         <v>22</v>
       </c>
@@ -1035,7 +1112,7 @@
       <c r="D23" s="6"/>
       <c r="E23" s="6"/>
     </row>
-    <row r="24" spans="1:5" ht="25.5" customHeight="1">
+    <row r="24" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="5">
         <v>23</v>
       </c>
@@ -1044,7 +1121,7 @@
       <c r="D24" s="6"/>
       <c r="E24" s="6"/>
     </row>
-    <row r="25" spans="1:5" ht="25.5" customHeight="1">
+    <row r="25" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="5">
         <v>24</v>
       </c>
@@ -1053,7 +1130,7 @@
       <c r="D25" s="6"/>
       <c r="E25" s="6"/>
     </row>
-    <row r="26" spans="1:5" ht="25.5" customHeight="1">
+    <row r="26" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="5">
         <v>25</v>
       </c>
@@ -1062,7 +1139,7 @@
       <c r="D26" s="6"/>
       <c r="E26" s="6"/>
     </row>
-    <row r="27" spans="1:5" ht="25.5" customHeight="1">
+    <row r="27" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="5">
         <v>26</v>
       </c>
@@ -1071,7 +1148,7 @@
       <c r="D27" s="6"/>
       <c r="E27" s="6"/>
     </row>
-    <row r="28" spans="1:5" ht="25.5" customHeight="1">
+    <row r="28" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="5">
         <v>27</v>
       </c>
@@ -1080,7 +1157,7 @@
       <c r="D28" s="6"/>
       <c r="E28" s="6"/>
     </row>
-    <row r="29" spans="1:5" ht="25.5" customHeight="1">
+    <row r="29" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="5">
         <v>28</v>
       </c>
@@ -1089,7 +1166,7 @@
       <c r="D29" s="6"/>
       <c r="E29" s="6"/>
     </row>
-    <row r="30" spans="1:5" ht="25.5" customHeight="1">
+    <row r="30" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="5">
         <v>29</v>
       </c>
@@ -1098,7 +1175,7 @@
       <c r="D30" s="6"/>
       <c r="E30" s="6"/>
     </row>
-    <row r="31" spans="1:5" ht="25.5" customHeight="1">
+    <row r="31" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="5">
         <v>30</v>
       </c>
@@ -1107,7 +1184,7 @@
       <c r="D31" s="6"/>
       <c r="E31" s="6"/>
     </row>
-    <row r="32" spans="1:5" ht="25.5" customHeight="1">
+    <row r="32" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="5">
         <v>31</v>
       </c>
@@ -1116,7 +1193,7 @@
       <c r="D32" s="6"/>
       <c r="E32" s="6"/>
     </row>
-    <row r="33" spans="1:5" ht="25.5" customHeight="1">
+    <row r="33" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="5">
         <v>32</v>
       </c>
@@ -1125,7 +1202,7 @@
       <c r="D33" s="6"/>
       <c r="E33" s="6"/>
     </row>
-    <row r="34" spans="1:5" ht="25.5" customHeight="1">
+    <row r="34" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="5">
         <v>33</v>
       </c>
@@ -1134,7 +1211,7 @@
       <c r="D34" s="6"/>
       <c r="E34" s="6"/>
     </row>
-    <row r="35" spans="1:5" ht="25.5" customHeight="1">
+    <row r="35" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="5">
         <v>34</v>
       </c>
@@ -1143,7 +1220,7 @@
       <c r="D35" s="6"/>
       <c r="E35" s="6"/>
     </row>
-    <row r="36" spans="1:5" ht="25.5" customHeight="1">
+    <row r="36" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="5">
         <v>35</v>
       </c>
@@ -1152,7 +1229,7 @@
       <c r="D36" s="6"/>
       <c r="E36" s="6"/>
     </row>
-    <row r="37" spans="1:5" ht="25.5" customHeight="1">
+    <row r="37" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="5">
         <v>36</v>
       </c>
@@ -1161,7 +1238,7 @@
       <c r="D37" s="6"/>
       <c r="E37" s="6"/>
     </row>
-    <row r="38" spans="1:5" ht="25.5" customHeight="1">
+    <row r="38" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="5">
         <v>37</v>
       </c>
@@ -1170,7 +1247,7 @@
       <c r="D38" s="6"/>
       <c r="E38" s="6"/>
     </row>
-    <row r="39" spans="1:5" ht="25.5" customHeight="1">
+    <row r="39" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="5">
         <v>38</v>
       </c>
@@ -1179,7 +1256,7 @@
       <c r="D39" s="6"/>
       <c r="E39" s="6"/>
     </row>
-    <row r="40" spans="1:5" ht="25.5" customHeight="1">
+    <row r="40" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="5">
         <v>39</v>
       </c>
@@ -1188,7 +1265,7 @@
       <c r="D40" s="6"/>
       <c r="E40" s="6"/>
     </row>
-    <row r="41" spans="1:5" ht="25.5" customHeight="1">
+    <row r="41" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="5">
         <v>40</v>
       </c>
@@ -1197,7 +1274,7 @@
       <c r="D41" s="6"/>
       <c r="E41" s="6"/>
     </row>
-    <row r="42" spans="1:5" ht="25.5" customHeight="1">
+    <row r="42" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="5">
         <v>41</v>
       </c>
@@ -1206,7 +1283,7 @@
       <c r="D42" s="6"/>
       <c r="E42" s="6"/>
     </row>
-    <row r="43" spans="1:5" ht="25.5" customHeight="1">
+    <row r="43" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="5">
         <v>42</v>
       </c>
@@ -1215,7 +1292,7 @@
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
     </row>
-    <row r="44" spans="1:5" ht="25.5" customHeight="1">
+    <row r="44" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="5">
         <v>43</v>
       </c>
@@ -1224,7 +1301,7 @@
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
     </row>
-    <row r="45" spans="1:5" ht="25.5" customHeight="1">
+    <row r="45" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="5">
         <v>44</v>
       </c>
@@ -1233,7 +1310,7 @@
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
     </row>
-    <row r="46" spans="1:5" ht="25.5" customHeight="1">
+    <row r="46" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="5">
         <v>45</v>
       </c>
@@ -1242,7 +1319,7 @@
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
     </row>
-    <row r="47" spans="1:5" ht="25.5" customHeight="1">
+    <row r="47" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="5">
         <v>46</v>
       </c>
@@ -1251,7 +1328,7 @@
       <c r="D47" s="6"/>
       <c r="E47" s="6"/>
     </row>
-    <row r="48" spans="1:5" ht="25.5" customHeight="1">
+    <row r="48" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="5">
         <v>47</v>
       </c>
@@ -1260,7 +1337,7 @@
       <c r="D48" s="6"/>
       <c r="E48" s="6"/>
     </row>
-    <row r="49" spans="1:5" ht="25.5" customHeight="1">
+    <row r="49" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="5">
         <v>48</v>
       </c>
@@ -1269,7 +1346,7 @@
       <c r="D49" s="6"/>
       <c r="E49" s="6"/>
     </row>
-    <row r="50" spans="1:5" ht="25.5" customHeight="1">
+    <row r="50" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="5">
         <v>49</v>
       </c>
@@ -1278,7 +1355,7 @@
       <c r="D50" s="6"/>
       <c r="E50" s="6"/>
     </row>
-    <row r="51" spans="1:5" ht="25.5" customHeight="1">
+    <row r="51" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="5">
         <v>50</v>
       </c>
@@ -1287,7 +1364,7 @@
       <c r="D51" s="6"/>
       <c r="E51" s="6"/>
     </row>
-    <row r="52" spans="1:5" ht="25.5" customHeight="1">
+    <row r="52" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="5">
         <v>51</v>
       </c>
@@ -1296,7 +1373,7 @@
       <c r="D52" s="6"/>
       <c r="E52" s="6"/>
     </row>
-    <row r="53" spans="1:5" ht="25.5" customHeight="1">
+    <row r="53" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="5">
         <v>52</v>
       </c>
@@ -1305,7 +1382,7 @@
       <c r="D53" s="6"/>
       <c r="E53" s="6"/>
     </row>
-    <row r="54" spans="1:5" ht="25.5" customHeight="1">
+    <row r="54" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="5">
         <v>53</v>
       </c>
@@ -1314,7 +1391,7 @@
       <c r="D54" s="6"/>
       <c r="E54" s="6"/>
     </row>
-    <row r="55" spans="1:5" ht="25.5" customHeight="1">
+    <row r="55" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="5">
         <v>54</v>
       </c>
@@ -1323,7 +1400,7 @@
       <c r="D55" s="6"/>
       <c r="E55" s="6"/>
     </row>
-    <row r="56" spans="1:5" ht="25.5" customHeight="1">
+    <row r="56" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="5">
         <v>55</v>
       </c>
@@ -1332,7 +1409,7 @@
       <c r="D56" s="6"/>
       <c r="E56" s="6"/>
     </row>
-    <row r="57" spans="1:5" ht="25.5" customHeight="1">
+    <row r="57" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="5">
         <v>56</v>
       </c>
@@ -1341,7 +1418,7 @@
       <c r="D57" s="6"/>
       <c r="E57" s="6"/>
     </row>
-    <row r="58" spans="1:5" ht="25.5" customHeight="1">
+    <row r="58" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="5">
         <v>57</v>
       </c>
@@ -1350,7 +1427,7 @@
       <c r="D58" s="6"/>
       <c r="E58" s="6"/>
     </row>
-    <row r="59" spans="1:5" ht="25.5" customHeight="1">
+    <row r="59" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="5">
         <v>58</v>
       </c>
@@ -1359,7 +1436,7 @@
       <c r="D59" s="6"/>
       <c r="E59" s="6"/>
     </row>
-    <row r="60" spans="1:5" ht="25.5" customHeight="1">
+    <row r="60" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" s="5">
         <v>59</v>
       </c>
@@ -1368,1400 +1445,1400 @@
       <c r="D60" s="6"/>
       <c r="E60" s="6"/>
     </row>
-    <row r="61" spans="1:5" ht="15.75" customHeight="1">
+    <row r="61" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" s="10"/>
       <c r="B61" s="11"/>
       <c r="C61" s="10"/>
       <c r="D61" s="11"/>
       <c r="E61" s="11"/>
     </row>
-    <row r="62" spans="1:5" ht="15.75" customHeight="1">
+    <row r="62" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" s="10"/>
       <c r="B62" s="11"/>
       <c r="C62" s="10"/>
       <c r="D62" s="11"/>
       <c r="E62" s="11"/>
     </row>
-    <row r="63" spans="1:5" ht="15.75" customHeight="1">
+    <row r="63" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" s="10"/>
       <c r="B63" s="11"/>
       <c r="C63" s="10"/>
       <c r="D63" s="11"/>
       <c r="E63" s="11"/>
     </row>
-    <row r="64" spans="1:5" ht="15.75" customHeight="1">
+    <row r="64" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" s="10"/>
       <c r="B64" s="11"/>
       <c r="C64" s="10"/>
       <c r="D64" s="11"/>
       <c r="E64" s="11"/>
     </row>
-    <row r="65" spans="1:5" ht="15.75" customHeight="1">
+    <row r="65" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A65" s="10"/>
       <c r="B65" s="11"/>
       <c r="C65" s="10"/>
       <c r="D65" s="11"/>
       <c r="E65" s="11"/>
     </row>
-    <row r="66" spans="1:5" ht="15.75" customHeight="1">
+    <row r="66" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A66" s="10"/>
       <c r="B66" s="11"/>
       <c r="C66" s="10"/>
       <c r="D66" s="11"/>
       <c r="E66" s="11"/>
     </row>
-    <row r="67" spans="1:5" ht="15.75" customHeight="1">
+    <row r="67" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67" s="10"/>
       <c r="B67" s="11"/>
       <c r="C67" s="10"/>
       <c r="D67" s="11"/>
       <c r="E67" s="11"/>
     </row>
-    <row r="68" spans="1:5" ht="15.75" customHeight="1">
+    <row r="68" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" s="10"/>
       <c r="B68" s="11"/>
       <c r="C68" s="10"/>
       <c r="D68" s="11"/>
       <c r="E68" s="11"/>
     </row>
-    <row r="69" spans="1:5" ht="15.75" customHeight="1">
+    <row r="69" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69" s="10"/>
       <c r="B69" s="11"/>
       <c r="C69" s="10"/>
       <c r="D69" s="11"/>
       <c r="E69" s="11"/>
     </row>
-    <row r="70" spans="1:5" ht="15.75" customHeight="1">
+    <row r="70" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A70" s="10"/>
       <c r="B70" s="11"/>
       <c r="C70" s="10"/>
       <c r="D70" s="11"/>
       <c r="E70" s="11"/>
     </row>
-    <row r="71" spans="1:5" ht="15.75" customHeight="1">
+    <row r="71" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A71" s="10"/>
       <c r="B71" s="11"/>
       <c r="C71" s="10"/>
       <c r="D71" s="11"/>
       <c r="E71" s="11"/>
     </row>
-    <row r="72" spans="1:5" ht="15.75" customHeight="1">
+    <row r="72" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72" s="10"/>
       <c r="B72" s="11"/>
       <c r="C72" s="10"/>
       <c r="D72" s="11"/>
       <c r="E72" s="11"/>
     </row>
-    <row r="73" spans="1:5" ht="15.75" customHeight="1">
+    <row r="73" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A73" s="10"/>
       <c r="B73" s="11"/>
       <c r="C73" s="10"/>
       <c r="D73" s="11"/>
       <c r="E73" s="11"/>
     </row>
-    <row r="74" spans="1:5" ht="15.75" customHeight="1">
+    <row r="74" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A74" s="10"/>
       <c r="B74" s="11"/>
       <c r="C74" s="10"/>
       <c r="D74" s="11"/>
       <c r="E74" s="11"/>
     </row>
-    <row r="75" spans="1:5" ht="15.75" customHeight="1">
+    <row r="75" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A75" s="10"/>
       <c r="B75" s="11"/>
       <c r="C75" s="10"/>
       <c r="D75" s="11"/>
       <c r="E75" s="11"/>
     </row>
-    <row r="76" spans="1:5" ht="15.75" customHeight="1">
+    <row r="76" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A76" s="10"/>
       <c r="B76" s="11"/>
       <c r="C76" s="10"/>
       <c r="D76" s="11"/>
       <c r="E76" s="11"/>
     </row>
-    <row r="77" spans="1:5" ht="15.75" customHeight="1">
+    <row r="77" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A77" s="10"/>
       <c r="B77" s="11"/>
       <c r="C77" s="10"/>
       <c r="D77" s="11"/>
       <c r="E77" s="11"/>
     </row>
-    <row r="78" spans="1:5" ht="15.75" customHeight="1">
+    <row r="78" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A78" s="10"/>
       <c r="B78" s="11"/>
       <c r="C78" s="10"/>
       <c r="D78" s="11"/>
       <c r="E78" s="11"/>
     </row>
-    <row r="79" spans="1:5" ht="15.75" customHeight="1">
+    <row r="79" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A79" s="10"/>
       <c r="B79" s="11"/>
       <c r="C79" s="10"/>
       <c r="D79" s="11"/>
       <c r="E79" s="11"/>
     </row>
-    <row r="80" spans="1:5" ht="15.75" customHeight="1">
+    <row r="80" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A80" s="10"/>
       <c r="B80" s="11"/>
       <c r="C80" s="10"/>
       <c r="D80" s="11"/>
       <c r="E80" s="11"/>
     </row>
-    <row r="81" spans="1:5" ht="15.75" customHeight="1">
+    <row r="81" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A81" s="10"/>
       <c r="B81" s="11"/>
       <c r="C81" s="10"/>
       <c r="D81" s="11"/>
       <c r="E81" s="11"/>
     </row>
-    <row r="82" spans="1:5" ht="15.75" customHeight="1">
+    <row r="82" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A82" s="10"/>
       <c r="B82" s="11"/>
       <c r="C82" s="10"/>
       <c r="D82" s="11"/>
       <c r="E82" s="11"/>
     </row>
-    <row r="83" spans="1:5" ht="15.75" customHeight="1">
+    <row r="83" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A83" s="10"/>
       <c r="B83" s="11"/>
       <c r="C83" s="10"/>
       <c r="D83" s="11"/>
       <c r="E83" s="11"/>
     </row>
-    <row r="84" spans="1:5" ht="15.75" customHeight="1">
+    <row r="84" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A84" s="10"/>
       <c r="B84" s="11"/>
       <c r="C84" s="10"/>
       <c r="D84" s="11"/>
       <c r="E84" s="11"/>
     </row>
-    <row r="85" spans="1:5" ht="15.75" customHeight="1">
+    <row r="85" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A85" s="10"/>
       <c r="B85" s="11"/>
       <c r="C85" s="10"/>
       <c r="D85" s="11"/>
       <c r="E85" s="11"/>
     </row>
-    <row r="86" spans="1:5" ht="15.75" customHeight="1">
+    <row r="86" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A86" s="10"/>
       <c r="B86" s="11"/>
       <c r="C86" s="10"/>
       <c r="D86" s="11"/>
       <c r="E86" s="11"/>
     </row>
-    <row r="87" spans="1:5" ht="15.75" customHeight="1">
+    <row r="87" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A87" s="10"/>
       <c r="B87" s="11"/>
       <c r="C87" s="10"/>
       <c r="D87" s="11"/>
       <c r="E87" s="11"/>
     </row>
-    <row r="88" spans="1:5" ht="15.75" customHeight="1">
+    <row r="88" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A88" s="10"/>
       <c r="B88" s="11"/>
       <c r="C88" s="10"/>
       <c r="D88" s="11"/>
       <c r="E88" s="11"/>
     </row>
-    <row r="89" spans="1:5" ht="15.75" customHeight="1">
+    <row r="89" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A89" s="10"/>
       <c r="B89" s="11"/>
       <c r="C89" s="10"/>
       <c r="D89" s="11"/>
       <c r="E89" s="11"/>
     </row>
-    <row r="90" spans="1:5" ht="15.75" customHeight="1">
+    <row r="90" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A90" s="10"/>
       <c r="B90" s="11"/>
       <c r="C90" s="10"/>
       <c r="D90" s="11"/>
       <c r="E90" s="11"/>
     </row>
-    <row r="91" spans="1:5" ht="15.75" customHeight="1">
+    <row r="91" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A91" s="10"/>
       <c r="B91" s="11"/>
       <c r="C91" s="10"/>
       <c r="D91" s="11"/>
       <c r="E91" s="11"/>
     </row>
-    <row r="92" spans="1:5" ht="15.75" customHeight="1">
+    <row r="92" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A92" s="10"/>
       <c r="B92" s="11"/>
       <c r="C92" s="10"/>
       <c r="D92" s="11"/>
       <c r="E92" s="11"/>
     </row>
-    <row r="93" spans="1:5" ht="15.75" customHeight="1">
+    <row r="93" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A93" s="10"/>
       <c r="B93" s="11"/>
       <c r="C93" s="10"/>
       <c r="D93" s="11"/>
       <c r="E93" s="11"/>
     </row>
-    <row r="94" spans="1:5" ht="15.75" customHeight="1">
+    <row r="94" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A94" s="10"/>
       <c r="B94" s="11"/>
       <c r="C94" s="10"/>
       <c r="D94" s="11"/>
       <c r="E94" s="11"/>
     </row>
-    <row r="95" spans="1:5" ht="15.75" customHeight="1">
+    <row r="95" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A95" s="10"/>
       <c r="B95" s="11"/>
       <c r="C95" s="10"/>
       <c r="D95" s="11"/>
       <c r="E95" s="11"/>
     </row>
-    <row r="96" spans="1:5" ht="15.75" customHeight="1">
+    <row r="96" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A96" s="10"/>
       <c r="B96" s="11"/>
       <c r="C96" s="10"/>
       <c r="D96" s="11"/>
       <c r="E96" s="11"/>
     </row>
-    <row r="97" spans="1:5" ht="15.75" customHeight="1">
+    <row r="97" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A97" s="10"/>
       <c r="B97" s="11"/>
       <c r="C97" s="10"/>
       <c r="D97" s="11"/>
       <c r="E97" s="11"/>
     </row>
-    <row r="98" spans="1:5" ht="15.75" customHeight="1">
+    <row r="98" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A98" s="10"/>
       <c r="B98" s="11"/>
       <c r="C98" s="10"/>
       <c r="D98" s="11"/>
       <c r="E98" s="11"/>
     </row>
-    <row r="99" spans="1:5" ht="15.75" customHeight="1">
+    <row r="99" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A99" s="10"/>
       <c r="B99" s="11"/>
       <c r="C99" s="10"/>
       <c r="D99" s="11"/>
       <c r="E99" s="11"/>
     </row>
-    <row r="100" spans="1:5" ht="15.75" customHeight="1">
+    <row r="100" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A100" s="10"/>
       <c r="B100" s="11"/>
       <c r="C100" s="10"/>
       <c r="D100" s="11"/>
       <c r="E100" s="11"/>
     </row>
-    <row r="101" spans="1:5" ht="15.75" customHeight="1">
+    <row r="101" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A101" s="10"/>
       <c r="B101" s="11"/>
       <c r="C101" s="10"/>
       <c r="D101" s="11"/>
       <c r="E101" s="11"/>
     </row>
-    <row r="102" spans="1:5" ht="15.75" customHeight="1">
+    <row r="102" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A102" s="10"/>
       <c r="B102" s="11"/>
       <c r="C102" s="10"/>
       <c r="D102" s="11"/>
       <c r="E102" s="11"/>
     </row>
-    <row r="103" spans="1:5" ht="15.75" customHeight="1">
+    <row r="103" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A103" s="10"/>
       <c r="B103" s="11"/>
       <c r="C103" s="10"/>
       <c r="D103" s="11"/>
       <c r="E103" s="11"/>
     </row>
-    <row r="104" spans="1:5" ht="15.75" customHeight="1">
+    <row r="104" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A104" s="10"/>
       <c r="B104" s="11"/>
       <c r="C104" s="10"/>
       <c r="D104" s="11"/>
       <c r="E104" s="11"/>
     </row>
-    <row r="105" spans="1:5" ht="15.75" customHeight="1">
+    <row r="105" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A105" s="10"/>
       <c r="B105" s="11"/>
       <c r="C105" s="10"/>
       <c r="D105" s="11"/>
       <c r="E105" s="11"/>
     </row>
-    <row r="106" spans="1:5" ht="15.75" customHeight="1">
+    <row r="106" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A106" s="10"/>
       <c r="B106" s="11"/>
       <c r="C106" s="10"/>
       <c r="D106" s="11"/>
       <c r="E106" s="11"/>
     </row>
-    <row r="107" spans="1:5" ht="15.75" customHeight="1">
+    <row r="107" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A107" s="10"/>
       <c r="B107" s="11"/>
       <c r="C107" s="10"/>
       <c r="D107" s="11"/>
       <c r="E107" s="11"/>
     </row>
-    <row r="108" spans="1:5" ht="15.75" customHeight="1">
+    <row r="108" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A108" s="10"/>
       <c r="B108" s="11"/>
       <c r="C108" s="10"/>
       <c r="D108" s="11"/>
       <c r="E108" s="11"/>
     </row>
-    <row r="109" spans="1:5" ht="15.75" customHeight="1">
+    <row r="109" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A109" s="10"/>
       <c r="B109" s="11"/>
       <c r="C109" s="10"/>
       <c r="D109" s="11"/>
       <c r="E109" s="11"/>
     </row>
-    <row r="110" spans="1:5" ht="15.75" customHeight="1">
+    <row r="110" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A110" s="10"/>
       <c r="B110" s="11"/>
       <c r="C110" s="10"/>
       <c r="D110" s="11"/>
       <c r="E110" s="11"/>
     </row>
-    <row r="111" spans="1:5" ht="15.75" customHeight="1">
+    <row r="111" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A111" s="10"/>
       <c r="B111" s="11"/>
       <c r="C111" s="10"/>
       <c r="D111" s="11"/>
       <c r="E111" s="11"/>
     </row>
-    <row r="112" spans="1:5" ht="15.75" customHeight="1">
+    <row r="112" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A112" s="10"/>
       <c r="B112" s="11"/>
       <c r="C112" s="10"/>
       <c r="D112" s="11"/>
       <c r="E112" s="11"/>
     </row>
-    <row r="113" spans="1:5" ht="15.75" customHeight="1">
+    <row r="113" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A113" s="10"/>
       <c r="B113" s="11"/>
       <c r="C113" s="10"/>
       <c r="D113" s="11"/>
       <c r="E113" s="11"/>
     </row>
-    <row r="114" spans="1:5" ht="15.75" customHeight="1">
+    <row r="114" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A114" s="10"/>
       <c r="B114" s="11"/>
       <c r="C114" s="10"/>
       <c r="D114" s="11"/>
       <c r="E114" s="11"/>
     </row>
-    <row r="115" spans="1:5" ht="15.75" customHeight="1">
+    <row r="115" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A115" s="10"/>
       <c r="B115" s="11"/>
       <c r="C115" s="10"/>
       <c r="D115" s="11"/>
       <c r="E115" s="11"/>
     </row>
-    <row r="116" spans="1:5" ht="15.75" customHeight="1">
+    <row r="116" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A116" s="10"/>
       <c r="B116" s="11"/>
       <c r="C116" s="10"/>
       <c r="D116" s="11"/>
       <c r="E116" s="11"/>
     </row>
-    <row r="117" spans="1:5" ht="15.75" customHeight="1">
+    <row r="117" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A117" s="10"/>
       <c r="B117" s="11"/>
       <c r="C117" s="10"/>
       <c r="D117" s="11"/>
       <c r="E117" s="11"/>
     </row>
-    <row r="118" spans="1:5" ht="15.75" customHeight="1">
+    <row r="118" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A118" s="10"/>
       <c r="B118" s="11"/>
       <c r="C118" s="10"/>
       <c r="D118" s="11"/>
       <c r="E118" s="11"/>
     </row>
-    <row r="119" spans="1:5" ht="15.75" customHeight="1">
+    <row r="119" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A119" s="10"/>
       <c r="B119" s="11"/>
       <c r="C119" s="10"/>
       <c r="D119" s="11"/>
       <c r="E119" s="11"/>
     </row>
-    <row r="120" spans="1:5" ht="15.75" customHeight="1">
+    <row r="120" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A120" s="10"/>
       <c r="B120" s="11"/>
       <c r="C120" s="10"/>
       <c r="D120" s="11"/>
       <c r="E120" s="11"/>
     </row>
-    <row r="121" spans="1:5" ht="15.75" customHeight="1">
+    <row r="121" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A121" s="10"/>
       <c r="B121" s="11"/>
       <c r="C121" s="10"/>
       <c r="D121" s="11"/>
       <c r="E121" s="11"/>
     </row>
-    <row r="122" spans="1:5" ht="15.75" customHeight="1">
+    <row r="122" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A122" s="10"/>
       <c r="B122" s="11"/>
       <c r="C122" s="10"/>
       <c r="D122" s="11"/>
       <c r="E122" s="11"/>
     </row>
-    <row r="123" spans="1:5" ht="15.75" customHeight="1">
+    <row r="123" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A123" s="10"/>
       <c r="B123" s="11"/>
       <c r="C123" s="10"/>
       <c r="D123" s="11"/>
       <c r="E123" s="11"/>
     </row>
-    <row r="124" spans="1:5" ht="15.75" customHeight="1">
+    <row r="124" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A124" s="10"/>
       <c r="B124" s="11"/>
       <c r="C124" s="10"/>
       <c r="D124" s="11"/>
       <c r="E124" s="11"/>
     </row>
-    <row r="125" spans="1:5" ht="15.75" customHeight="1">
+    <row r="125" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A125" s="10"/>
       <c r="B125" s="11"/>
       <c r="C125" s="10"/>
       <c r="D125" s="11"/>
       <c r="E125" s="11"/>
     </row>
-    <row r="126" spans="1:5" ht="15.75" customHeight="1">
+    <row r="126" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A126" s="10"/>
       <c r="B126" s="11"/>
       <c r="C126" s="10"/>
       <c r="D126" s="11"/>
       <c r="E126" s="11"/>
     </row>
-    <row r="127" spans="1:5" ht="15.75" customHeight="1">
+    <row r="127" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A127" s="10"/>
       <c r="B127" s="11"/>
       <c r="C127" s="10"/>
       <c r="D127" s="11"/>
       <c r="E127" s="11"/>
     </row>
-    <row r="128" spans="1:5" ht="15.75" customHeight="1">
+    <row r="128" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A128" s="10"/>
       <c r="B128" s="11"/>
       <c r="C128" s="10"/>
       <c r="D128" s="11"/>
       <c r="E128" s="11"/>
     </row>
-    <row r="129" spans="1:5" ht="15.75" customHeight="1">
+    <row r="129" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A129" s="10"/>
       <c r="B129" s="11"/>
       <c r="C129" s="10"/>
       <c r="D129" s="11"/>
       <c r="E129" s="11"/>
     </row>
-    <row r="130" spans="1:5" ht="15.75" customHeight="1">
+    <row r="130" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A130" s="10"/>
       <c r="B130" s="11"/>
       <c r="C130" s="10"/>
       <c r="D130" s="11"/>
       <c r="E130" s="11"/>
     </row>
-    <row r="131" spans="1:5" ht="15.75" customHeight="1">
+    <row r="131" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A131" s="10"/>
       <c r="B131" s="11"/>
       <c r="C131" s="10"/>
       <c r="D131" s="11"/>
       <c r="E131" s="11"/>
     </row>
-    <row r="132" spans="1:5" ht="15.75" customHeight="1">
+    <row r="132" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A132" s="10"/>
       <c r="B132" s="11"/>
       <c r="C132" s="10"/>
       <c r="D132" s="11"/>
       <c r="E132" s="11"/>
     </row>
-    <row r="133" spans="1:5" ht="15.75" customHeight="1">
+    <row r="133" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A133" s="10"/>
       <c r="B133" s="11"/>
       <c r="C133" s="10"/>
       <c r="D133" s="11"/>
       <c r="E133" s="11"/>
     </row>
-    <row r="134" spans="1:5" ht="15.75" customHeight="1">
+    <row r="134" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A134" s="10"/>
       <c r="B134" s="11"/>
       <c r="C134" s="10"/>
       <c r="D134" s="11"/>
       <c r="E134" s="11"/>
     </row>
-    <row r="135" spans="1:5" ht="15.75" customHeight="1">
+    <row r="135" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A135" s="10"/>
       <c r="B135" s="11"/>
       <c r="C135" s="10"/>
       <c r="D135" s="11"/>
       <c r="E135" s="11"/>
     </row>
-    <row r="136" spans="1:5" ht="15.75" customHeight="1">
+    <row r="136" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A136" s="10"/>
       <c r="B136" s="11"/>
       <c r="C136" s="10"/>
       <c r="D136" s="11"/>
       <c r="E136" s="11"/>
     </row>
-    <row r="137" spans="1:5" ht="15.75" customHeight="1">
+    <row r="137" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A137" s="10"/>
       <c r="B137" s="11"/>
       <c r="C137" s="10"/>
       <c r="D137" s="11"/>
       <c r="E137" s="11"/>
     </row>
-    <row r="138" spans="1:5" ht="15.75" customHeight="1">
+    <row r="138" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A138" s="10"/>
       <c r="B138" s="11"/>
       <c r="C138" s="10"/>
       <c r="D138" s="11"/>
       <c r="E138" s="11"/>
     </row>
-    <row r="139" spans="1:5" ht="15.75" customHeight="1">
+    <row r="139" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A139" s="10"/>
       <c r="B139" s="11"/>
       <c r="C139" s="10"/>
       <c r="D139" s="11"/>
       <c r="E139" s="11"/>
     </row>
-    <row r="140" spans="1:5" ht="15.75" customHeight="1">
+    <row r="140" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A140" s="10"/>
       <c r="B140" s="11"/>
       <c r="C140" s="10"/>
       <c r="D140" s="11"/>
       <c r="E140" s="11"/>
     </row>
-    <row r="141" spans="1:5" ht="15.75" customHeight="1">
+    <row r="141" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A141" s="10"/>
       <c r="B141" s="11"/>
       <c r="C141" s="10"/>
       <c r="D141" s="11"/>
       <c r="E141" s="11"/>
     </row>
-    <row r="142" spans="1:5" ht="15.75" customHeight="1">
+    <row r="142" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A142" s="10"/>
       <c r="B142" s="11"/>
       <c r="C142" s="10"/>
       <c r="D142" s="11"/>
       <c r="E142" s="11"/>
     </row>
-    <row r="143" spans="1:5" ht="15.75" customHeight="1">
+    <row r="143" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A143" s="10"/>
       <c r="B143" s="11"/>
       <c r="C143" s="10"/>
       <c r="D143" s="11"/>
       <c r="E143" s="11"/>
     </row>
-    <row r="144" spans="1:5" ht="15.75" customHeight="1">
+    <row r="144" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A144" s="10"/>
       <c r="B144" s="11"/>
       <c r="C144" s="10"/>
       <c r="D144" s="11"/>
       <c r="E144" s="11"/>
     </row>
-    <row r="145" spans="1:5" ht="15.75" customHeight="1">
+    <row r="145" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A145" s="10"/>
       <c r="B145" s="11"/>
       <c r="C145" s="10"/>
       <c r="D145" s="11"/>
       <c r="E145" s="11"/>
     </row>
-    <row r="146" spans="1:5" ht="15.75" customHeight="1">
+    <row r="146" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A146" s="10"/>
       <c r="B146" s="11"/>
       <c r="C146" s="10"/>
       <c r="D146" s="11"/>
       <c r="E146" s="11"/>
     </row>
-    <row r="147" spans="1:5" ht="15.75" customHeight="1">
+    <row r="147" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A147" s="10"/>
       <c r="B147" s="11"/>
       <c r="C147" s="10"/>
       <c r="D147" s="11"/>
       <c r="E147" s="11"/>
     </row>
-    <row r="148" spans="1:5" ht="15.75" customHeight="1">
+    <row r="148" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A148" s="10"/>
       <c r="B148" s="11"/>
       <c r="C148" s="10"/>
       <c r="D148" s="11"/>
       <c r="E148" s="11"/>
     </row>
-    <row r="149" spans="1:5" ht="15.75" customHeight="1">
+    <row r="149" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A149" s="10"/>
       <c r="B149" s="11"/>
       <c r="C149" s="10"/>
       <c r="D149" s="11"/>
       <c r="E149" s="11"/>
     </row>
-    <row r="150" spans="1:5" ht="15.75" customHeight="1">
+    <row r="150" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A150" s="10"/>
       <c r="B150" s="11"/>
       <c r="C150" s="10"/>
       <c r="D150" s="11"/>
       <c r="E150" s="11"/>
     </row>
-    <row r="151" spans="1:5" ht="15.75" customHeight="1">
+    <row r="151" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A151" s="10"/>
       <c r="B151" s="11"/>
       <c r="C151" s="10"/>
       <c r="D151" s="11"/>
       <c r="E151" s="11"/>
     </row>
-    <row r="152" spans="1:5" ht="15.75" customHeight="1">
+    <row r="152" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A152" s="10"/>
       <c r="B152" s="11"/>
       <c r="C152" s="10"/>
       <c r="D152" s="11"/>
       <c r="E152" s="11"/>
     </row>
-    <row r="153" spans="1:5" ht="15.75" customHeight="1">
+    <row r="153" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A153" s="10"/>
       <c r="B153" s="11"/>
       <c r="C153" s="10"/>
       <c r="D153" s="11"/>
       <c r="E153" s="11"/>
     </row>
-    <row r="154" spans="1:5" ht="15.75" customHeight="1">
+    <row r="154" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A154" s="10"/>
       <c r="B154" s="11"/>
       <c r="C154" s="10"/>
       <c r="D154" s="11"/>
       <c r="E154" s="11"/>
     </row>
-    <row r="155" spans="1:5" ht="15.75" customHeight="1">
+    <row r="155" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A155" s="10"/>
       <c r="B155" s="11"/>
       <c r="C155" s="10"/>
       <c r="D155" s="11"/>
       <c r="E155" s="11"/>
     </row>
-    <row r="156" spans="1:5" ht="15.75" customHeight="1">
+    <row r="156" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A156" s="10"/>
       <c r="B156" s="11"/>
       <c r="C156" s="10"/>
       <c r="D156" s="11"/>
       <c r="E156" s="11"/>
     </row>
-    <row r="157" spans="1:5" ht="15.75" customHeight="1">
+    <row r="157" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A157" s="10"/>
       <c r="B157" s="11"/>
       <c r="C157" s="10"/>
       <c r="D157" s="11"/>
       <c r="E157" s="11"/>
     </row>
-    <row r="158" spans="1:5" ht="15.75" customHeight="1">
+    <row r="158" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A158" s="10"/>
       <c r="B158" s="11"/>
       <c r="C158" s="10"/>
       <c r="D158" s="11"/>
       <c r="E158" s="11"/>
     </row>
-    <row r="159" spans="1:5" ht="15.75" customHeight="1">
+    <row r="159" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A159" s="10"/>
       <c r="B159" s="11"/>
       <c r="C159" s="10"/>
       <c r="D159" s="11"/>
       <c r="E159" s="11"/>
     </row>
-    <row r="160" spans="1:5" ht="15.75" customHeight="1">
+    <row r="160" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A160" s="10"/>
       <c r="B160" s="11"/>
       <c r="C160" s="10"/>
       <c r="D160" s="11"/>
       <c r="E160" s="11"/>
     </row>
-    <row r="161" spans="1:5" ht="15.75" customHeight="1">
+    <row r="161" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A161" s="10"/>
       <c r="B161" s="11"/>
       <c r="C161" s="10"/>
       <c r="D161" s="11"/>
       <c r="E161" s="11"/>
     </row>
-    <row r="162" spans="1:5" ht="15.75" customHeight="1">
+    <row r="162" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A162" s="10"/>
       <c r="B162" s="11"/>
       <c r="C162" s="10"/>
       <c r="D162" s="11"/>
       <c r="E162" s="11"/>
     </row>
-    <row r="163" spans="1:5" ht="15.75" customHeight="1">
+    <row r="163" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A163" s="10"/>
       <c r="B163" s="11"/>
       <c r="C163" s="10"/>
       <c r="D163" s="11"/>
       <c r="E163" s="11"/>
     </row>
-    <row r="164" spans="1:5" ht="15.75" customHeight="1">
+    <row r="164" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A164" s="10"/>
       <c r="B164" s="11"/>
       <c r="C164" s="10"/>
       <c r="D164" s="11"/>
       <c r="E164" s="11"/>
     </row>
-    <row r="165" spans="1:5" ht="15.75" customHeight="1">
+    <row r="165" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A165" s="10"/>
       <c r="B165" s="11"/>
       <c r="C165" s="10"/>
       <c r="D165" s="11"/>
       <c r="E165" s="11"/>
     </row>
-    <row r="166" spans="1:5" ht="15.75" customHeight="1">
+    <row r="166" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A166" s="10"/>
       <c r="B166" s="11"/>
       <c r="C166" s="10"/>
       <c r="D166" s="11"/>
       <c r="E166" s="11"/>
     </row>
-    <row r="167" spans="1:5" ht="15.75" customHeight="1">
+    <row r="167" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A167" s="10"/>
       <c r="B167" s="11"/>
       <c r="C167" s="10"/>
       <c r="D167" s="11"/>
       <c r="E167" s="11"/>
     </row>
-    <row r="168" spans="1:5" ht="15.75" customHeight="1">
+    <row r="168" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A168" s="10"/>
       <c r="B168" s="11"/>
       <c r="C168" s="10"/>
       <c r="D168" s="11"/>
       <c r="E168" s="11"/>
     </row>
-    <row r="169" spans="1:5" ht="15.75" customHeight="1">
+    <row r="169" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A169" s="10"/>
       <c r="B169" s="11"/>
       <c r="C169" s="10"/>
       <c r="D169" s="11"/>
       <c r="E169" s="11"/>
     </row>
-    <row r="170" spans="1:5" ht="15.75" customHeight="1">
+    <row r="170" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A170" s="10"/>
       <c r="B170" s="11"/>
       <c r="C170" s="10"/>
       <c r="D170" s="11"/>
       <c r="E170" s="11"/>
     </row>
-    <row r="171" spans="1:5" ht="15.75" customHeight="1">
+    <row r="171" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A171" s="10"/>
       <c r="B171" s="11"/>
       <c r="C171" s="10"/>
       <c r="D171" s="11"/>
       <c r="E171" s="11"/>
     </row>
-    <row r="172" spans="1:5" ht="15.75" customHeight="1">
+    <row r="172" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A172" s="10"/>
       <c r="B172" s="11"/>
       <c r="C172" s="10"/>
       <c r="D172" s="11"/>
       <c r="E172" s="11"/>
     </row>
-    <row r="173" spans="1:5" ht="15.75" customHeight="1">
+    <row r="173" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A173" s="10"/>
       <c r="B173" s="11"/>
       <c r="C173" s="10"/>
       <c r="D173" s="11"/>
       <c r="E173" s="11"/>
     </row>
-    <row r="174" spans="1:5" ht="15.75" customHeight="1">
+    <row r="174" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A174" s="10"/>
       <c r="B174" s="11"/>
       <c r="C174" s="10"/>
       <c r="D174" s="11"/>
       <c r="E174" s="11"/>
     </row>
-    <row r="175" spans="1:5" ht="15.75" customHeight="1">
+    <row r="175" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A175" s="10"/>
       <c r="B175" s="11"/>
       <c r="C175" s="10"/>
       <c r="D175" s="11"/>
       <c r="E175" s="11"/>
     </row>
-    <row r="176" spans="1:5" ht="15.75" customHeight="1">
+    <row r="176" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A176" s="10"/>
       <c r="B176" s="11"/>
       <c r="C176" s="10"/>
       <c r="D176" s="11"/>
       <c r="E176" s="11"/>
     </row>
-    <row r="177" spans="1:5" ht="15.75" customHeight="1">
+    <row r="177" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A177" s="10"/>
       <c r="B177" s="11"/>
       <c r="C177" s="10"/>
       <c r="D177" s="11"/>
       <c r="E177" s="11"/>
     </row>
-    <row r="178" spans="1:5" ht="15.75" customHeight="1">
+    <row r="178" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A178" s="10"/>
       <c r="B178" s="11"/>
       <c r="C178" s="10"/>
       <c r="D178" s="11"/>
       <c r="E178" s="11"/>
     </row>
-    <row r="179" spans="1:5" ht="15.75" customHeight="1">
+    <row r="179" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A179" s="10"/>
       <c r="B179" s="11"/>
       <c r="C179" s="10"/>
       <c r="D179" s="11"/>
       <c r="E179" s="11"/>
     </row>
-    <row r="180" spans="1:5" ht="15.75" customHeight="1">
+    <row r="180" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A180" s="10"/>
       <c r="B180" s="11"/>
       <c r="C180" s="10"/>
       <c r="D180" s="11"/>
       <c r="E180" s="11"/>
     </row>
-    <row r="181" spans="1:5" ht="15.75" customHeight="1">
+    <row r="181" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A181" s="10"/>
       <c r="B181" s="11"/>
       <c r="C181" s="10"/>
       <c r="D181" s="11"/>
       <c r="E181" s="11"/>
     </row>
-    <row r="182" spans="1:5" ht="15.75" customHeight="1">
+    <row r="182" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A182" s="10"/>
       <c r="B182" s="11"/>
       <c r="C182" s="10"/>
       <c r="D182" s="11"/>
       <c r="E182" s="11"/>
     </row>
-    <row r="183" spans="1:5" ht="15.75" customHeight="1">
+    <row r="183" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A183" s="10"/>
       <c r="B183" s="11"/>
       <c r="C183" s="10"/>
       <c r="D183" s="11"/>
       <c r="E183" s="11"/>
     </row>
-    <row r="184" spans="1:5" ht="15.75" customHeight="1">
+    <row r="184" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A184" s="10"/>
       <c r="B184" s="11"/>
       <c r="C184" s="10"/>
       <c r="D184" s="11"/>
       <c r="E184" s="11"/>
     </row>
-    <row r="185" spans="1:5" ht="15.75" customHeight="1">
+    <row r="185" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A185" s="10"/>
       <c r="B185" s="11"/>
       <c r="C185" s="10"/>
       <c r="D185" s="11"/>
       <c r="E185" s="11"/>
     </row>
-    <row r="186" spans="1:5" ht="15.75" customHeight="1">
+    <row r="186" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A186" s="10"/>
       <c r="B186" s="11"/>
       <c r="C186" s="10"/>
       <c r="D186" s="11"/>
       <c r="E186" s="11"/>
     </row>
-    <row r="187" spans="1:5" ht="15.75" customHeight="1">
+    <row r="187" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A187" s="10"/>
       <c r="B187" s="11"/>
       <c r="C187" s="10"/>
       <c r="D187" s="11"/>
       <c r="E187" s="11"/>
     </row>
-    <row r="188" spans="1:5" ht="15.75" customHeight="1">
+    <row r="188" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A188" s="10"/>
       <c r="B188" s="11"/>
       <c r="C188" s="10"/>
       <c r="D188" s="11"/>
       <c r="E188" s="11"/>
     </row>
-    <row r="189" spans="1:5" ht="15.75" customHeight="1">
+    <row r="189" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A189" s="10"/>
       <c r="B189" s="11"/>
       <c r="C189" s="10"/>
       <c r="D189" s="11"/>
       <c r="E189" s="11"/>
     </row>
-    <row r="190" spans="1:5" ht="15.75" customHeight="1">
+    <row r="190" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A190" s="10"/>
       <c r="B190" s="11"/>
       <c r="C190" s="10"/>
       <c r="D190" s="11"/>
       <c r="E190" s="11"/>
     </row>
-    <row r="191" spans="1:5" ht="15.75" customHeight="1">
+    <row r="191" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A191" s="10"/>
       <c r="B191" s="11"/>
       <c r="C191" s="10"/>
       <c r="D191" s="11"/>
       <c r="E191" s="11"/>
     </row>
-    <row r="192" spans="1:5" ht="15.75" customHeight="1">
+    <row r="192" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A192" s="10"/>
       <c r="B192" s="11"/>
       <c r="C192" s="10"/>
       <c r="D192" s="11"/>
       <c r="E192" s="11"/>
     </row>
-    <row r="193" spans="1:5" ht="15.75" customHeight="1">
+    <row r="193" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A193" s="10"/>
       <c r="B193" s="11"/>
       <c r="C193" s="10"/>
       <c r="D193" s="11"/>
       <c r="E193" s="11"/>
     </row>
-    <row r="194" spans="1:5" ht="15.75" customHeight="1">
+    <row r="194" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A194" s="10"/>
       <c r="B194" s="11"/>
       <c r="C194" s="10"/>
       <c r="D194" s="11"/>
       <c r="E194" s="11"/>
     </row>
-    <row r="195" spans="1:5" ht="15.75" customHeight="1">
+    <row r="195" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A195" s="10"/>
       <c r="B195" s="11"/>
       <c r="C195" s="10"/>
       <c r="D195" s="11"/>
       <c r="E195" s="11"/>
     </row>
-    <row r="196" spans="1:5" ht="15.75" customHeight="1">
+    <row r="196" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A196" s="10"/>
       <c r="B196" s="11"/>
       <c r="C196" s="10"/>
       <c r="D196" s="11"/>
       <c r="E196" s="11"/>
     </row>
-    <row r="197" spans="1:5" ht="15.75" customHeight="1">
+    <row r="197" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A197" s="10"/>
       <c r="B197" s="11"/>
       <c r="C197" s="10"/>
       <c r="D197" s="11"/>
       <c r="E197" s="11"/>
     </row>
-    <row r="198" spans="1:5" ht="15.75" customHeight="1">
+    <row r="198" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A198" s="10"/>
       <c r="B198" s="11"/>
       <c r="C198" s="10"/>
       <c r="D198" s="11"/>
       <c r="E198" s="11"/>
     </row>
-    <row r="199" spans="1:5" ht="15.75" customHeight="1">
+    <row r="199" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A199" s="10"/>
       <c r="B199" s="11"/>
       <c r="C199" s="10"/>
       <c r="D199" s="11"/>
       <c r="E199" s="11"/>
     </row>
-    <row r="200" spans="1:5" ht="15.75" customHeight="1">
+    <row r="200" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A200" s="10"/>
       <c r="B200" s="11"/>
       <c r="C200" s="10"/>
       <c r="D200" s="11"/>
       <c r="E200" s="11"/>
     </row>
-    <row r="201" spans="1:5" ht="15.75" customHeight="1">
+    <row r="201" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A201" s="10"/>
       <c r="B201" s="11"/>
       <c r="C201" s="10"/>
       <c r="D201" s="11"/>
       <c r="E201" s="11"/>
     </row>
-    <row r="202" spans="1:5" ht="15.75" customHeight="1">
+    <row r="202" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A202" s="10"/>
       <c r="B202" s="11"/>
       <c r="C202" s="10"/>
       <c r="D202" s="11"/>
       <c r="E202" s="11"/>
     </row>
-    <row r="203" spans="1:5" ht="15.75" customHeight="1">
+    <row r="203" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A203" s="10"/>
       <c r="B203" s="11"/>
       <c r="C203" s="10"/>
       <c r="D203" s="11"/>
       <c r="E203" s="11"/>
     </row>
-    <row r="204" spans="1:5" ht="15.75" customHeight="1">
+    <row r="204" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A204" s="10"/>
       <c r="B204" s="11"/>
       <c r="C204" s="10"/>
       <c r="D204" s="11"/>
       <c r="E204" s="11"/>
     </row>
-    <row r="205" spans="1:5" ht="15.75" customHeight="1">
+    <row r="205" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A205" s="10"/>
       <c r="B205" s="11"/>
       <c r="C205" s="10"/>
       <c r="D205" s="11"/>
       <c r="E205" s="11"/>
     </row>
-    <row r="206" spans="1:5" ht="15.75" customHeight="1">
+    <row r="206" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A206" s="10"/>
       <c r="B206" s="11"/>
       <c r="C206" s="10"/>
       <c r="D206" s="11"/>
       <c r="E206" s="11"/>
     </row>
-    <row r="207" spans="1:5" ht="15.75" customHeight="1">
+    <row r="207" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A207" s="10"/>
       <c r="B207" s="11"/>
       <c r="C207" s="10"/>
       <c r="D207" s="11"/>
       <c r="E207" s="11"/>
     </row>
-    <row r="208" spans="1:5" ht="15.75" customHeight="1">
+    <row r="208" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A208" s="10"/>
       <c r="B208" s="11"/>
       <c r="C208" s="10"/>
       <c r="D208" s="11"/>
       <c r="E208" s="11"/>
     </row>
-    <row r="209" spans="1:5" ht="15.75" customHeight="1">
+    <row r="209" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A209" s="10"/>
       <c r="B209" s="11"/>
       <c r="C209" s="10"/>
       <c r="D209" s="11"/>
       <c r="E209" s="11"/>
     </row>
-    <row r="210" spans="1:5" ht="15.75" customHeight="1">
+    <row r="210" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A210" s="10"/>
       <c r="B210" s="11"/>
       <c r="C210" s="10"/>
       <c r="D210" s="11"/>
       <c r="E210" s="11"/>
     </row>
-    <row r="211" spans="1:5" ht="15.75" customHeight="1">
+    <row r="211" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A211" s="10"/>
       <c r="B211" s="11"/>
       <c r="C211" s="10"/>
       <c r="D211" s="11"/>
       <c r="E211" s="11"/>
     </row>
-    <row r="212" spans="1:5" ht="15.75" customHeight="1">
+    <row r="212" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A212" s="10"/>
       <c r="B212" s="11"/>
       <c r="C212" s="10"/>
       <c r="D212" s="11"/>
       <c r="E212" s="11"/>
     </row>
-    <row r="213" spans="1:5" ht="15.75" customHeight="1">
+    <row r="213" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A213" s="10"/>
       <c r="B213" s="11"/>
       <c r="C213" s="10"/>
       <c r="D213" s="11"/>
       <c r="E213" s="11"/>
     </row>
-    <row r="214" spans="1:5" ht="15.75" customHeight="1">
+    <row r="214" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A214" s="10"/>
       <c r="B214" s="11"/>
       <c r="C214" s="10"/>
       <c r="D214" s="11"/>
       <c r="E214" s="11"/>
     </row>
-    <row r="215" spans="1:5" ht="15.75" customHeight="1">
+    <row r="215" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A215" s="10"/>
       <c r="B215" s="11"/>
       <c r="C215" s="10"/>
       <c r="D215" s="11"/>
       <c r="E215" s="11"/>
     </row>
-    <row r="216" spans="1:5" ht="15.75" customHeight="1">
+    <row r="216" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A216" s="10"/>
       <c r="B216" s="11"/>
       <c r="C216" s="10"/>
       <c r="D216" s="11"/>
       <c r="E216" s="11"/>
     </row>
-    <row r="217" spans="1:5" ht="15.75" customHeight="1">
+    <row r="217" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A217" s="10"/>
       <c r="B217" s="11"/>
       <c r="C217" s="10"/>
       <c r="D217" s="11"/>
       <c r="E217" s="11"/>
     </row>
-    <row r="218" spans="1:5" ht="15.75" customHeight="1">
+    <row r="218" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A218" s="10"/>
       <c r="B218" s="11"/>
       <c r="C218" s="10"/>
       <c r="D218" s="11"/>
       <c r="E218" s="11"/>
     </row>
-    <row r="219" spans="1:5" ht="15.75" customHeight="1">
+    <row r="219" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A219" s="10"/>
       <c r="B219" s="11"/>
       <c r="C219" s="10"/>
       <c r="D219" s="11"/>
       <c r="E219" s="11"/>
     </row>
-    <row r="220" spans="1:5" ht="15.75" customHeight="1">
+    <row r="220" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A220" s="10"/>
       <c r="B220" s="11"/>
       <c r="C220" s="10"/>
       <c r="D220" s="11"/>
       <c r="E220" s="11"/>
     </row>
-    <row r="221" spans="1:5" ht="15.75" customHeight="1">
+    <row r="221" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A221" s="10"/>
       <c r="B221" s="11"/>
       <c r="C221" s="10"/>
       <c r="D221" s="11"/>
       <c r="E221" s="11"/>
     </row>
-    <row r="222" spans="1:5" ht="15.75" customHeight="1">
+    <row r="222" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A222" s="10"/>
       <c r="B222" s="11"/>
       <c r="C222" s="10"/>
       <c r="D222" s="11"/>
       <c r="E222" s="11"/>
     </row>
-    <row r="223" spans="1:5" ht="15.75" customHeight="1">
+    <row r="223" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A223" s="10"/>
       <c r="B223" s="11"/>
       <c r="C223" s="10"/>
       <c r="D223" s="11"/>
       <c r="E223" s="11"/>
     </row>
-    <row r="224" spans="1:5" ht="15.75" customHeight="1">
+    <row r="224" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A224" s="10"/>
       <c r="B224" s="11"/>
       <c r="C224" s="10"/>
       <c r="D224" s="11"/>
       <c r="E224" s="11"/>
     </row>
-    <row r="225" spans="1:5" ht="15.75" customHeight="1">
+    <row r="225" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A225" s="10"/>
       <c r="B225" s="11"/>
       <c r="C225" s="10"/>
       <c r="D225" s="11"/>
       <c r="E225" s="11"/>
     </row>
-    <row r="226" spans="1:5" ht="15.75" customHeight="1">
+    <row r="226" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A226" s="10"/>
       <c r="B226" s="11"/>
       <c r="C226" s="10"/>
       <c r="D226" s="11"/>
       <c r="E226" s="11"/>
     </row>
-    <row r="227" spans="1:5" ht="15.75" customHeight="1">
+    <row r="227" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A227" s="10"/>
       <c r="B227" s="11"/>
       <c r="C227" s="10"/>
       <c r="D227" s="11"/>
       <c r="E227" s="11"/>
     </row>
-    <row r="228" spans="1:5" ht="15.75" customHeight="1">
+    <row r="228" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A228" s="10"/>
       <c r="B228" s="11"/>
       <c r="C228" s="10"/>
       <c r="D228" s="11"/>
       <c r="E228" s="11"/>
     </row>
-    <row r="229" spans="1:5" ht="15.75" customHeight="1">
+    <row r="229" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A229" s="10"/>
       <c r="B229" s="11"/>
       <c r="C229" s="10"/>
       <c r="D229" s="11"/>
       <c r="E229" s="11"/>
     </row>
-    <row r="230" spans="1:5" ht="15.75" customHeight="1">
+    <row r="230" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A230" s="10"/>
       <c r="B230" s="11"/>
       <c r="C230" s="10"/>
       <c r="D230" s="11"/>
       <c r="E230" s="11"/>
     </row>
-    <row r="231" spans="1:5" ht="15.75" customHeight="1">
+    <row r="231" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A231" s="10"/>
       <c r="B231" s="11"/>
       <c r="C231" s="10"/>
       <c r="D231" s="11"/>
       <c r="E231" s="11"/>
     </row>
-    <row r="232" spans="1:5" ht="15.75" customHeight="1">
+    <row r="232" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A232" s="10"/>
       <c r="B232" s="11"/>
       <c r="C232" s="10"/>
       <c r="D232" s="11"/>
       <c r="E232" s="11"/>
     </row>
-    <row r="233" spans="1:5" ht="15.75" customHeight="1">
+    <row r="233" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A233" s="10"/>
       <c r="B233" s="11"/>
       <c r="C233" s="10"/>
       <c r="D233" s="11"/>
       <c r="E233" s="11"/>
     </row>
-    <row r="234" spans="1:5" ht="15.75" customHeight="1">
+    <row r="234" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A234" s="10"/>
       <c r="B234" s="11"/>
       <c r="C234" s="10"/>
       <c r="D234" s="11"/>
       <c r="E234" s="11"/>
     </row>
-    <row r="235" spans="1:5" ht="15.75" customHeight="1">
+    <row r="235" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A235" s="10"/>
       <c r="B235" s="11"/>
       <c r="C235" s="10"/>
       <c r="D235" s="11"/>
       <c r="E235" s="11"/>
     </row>
-    <row r="236" spans="1:5" ht="15.75" customHeight="1">
+    <row r="236" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A236" s="10"/>
       <c r="B236" s="11"/>
       <c r="C236" s="10"/>
       <c r="D236" s="11"/>
       <c r="E236" s="11"/>
     </row>
-    <row r="237" spans="1:5" ht="15.75" customHeight="1">
+    <row r="237" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A237" s="10"/>
       <c r="B237" s="11"/>
       <c r="C237" s="10"/>
       <c r="D237" s="11"/>
       <c r="E237" s="11"/>
     </row>
-    <row r="238" spans="1:5" ht="15.75" customHeight="1">
+    <row r="238" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A238" s="10"/>
       <c r="B238" s="11"/>
       <c r="C238" s="10"/>
       <c r="D238" s="11"/>
       <c r="E238" s="11"/>
     </row>
-    <row r="239" spans="1:5" ht="15.75" customHeight="1">
+    <row r="239" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A239" s="10"/>
       <c r="B239" s="11"/>
       <c r="C239" s="10"/>
       <c r="D239" s="11"/>
       <c r="E239" s="11"/>
     </row>
-    <row r="240" spans="1:5" ht="15.75" customHeight="1">
+    <row r="240" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A240" s="10"/>
       <c r="B240" s="11"/>
       <c r="C240" s="10"/>
       <c r="D240" s="11"/>
       <c r="E240" s="11"/>
     </row>
-    <row r="241" spans="1:5" ht="15.75" customHeight="1">
+    <row r="241" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A241" s="10"/>
       <c r="B241" s="11"/>
       <c r="C241" s="10"/>
       <c r="D241" s="11"/>
       <c r="E241" s="11"/>
     </row>
-    <row r="242" spans="1:5" ht="15.75" customHeight="1">
+    <row r="242" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A242" s="10"/>
       <c r="B242" s="11"/>
       <c r="C242" s="10"/>
       <c r="D242" s="11"/>
       <c r="E242" s="11"/>
     </row>
-    <row r="243" spans="1:5" ht="15.75" customHeight="1">
+    <row r="243" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A243" s="10"/>
       <c r="B243" s="11"/>
       <c r="C243" s="10"/>
       <c r="D243" s="11"/>
       <c r="E243" s="11"/>
     </row>
-    <row r="244" spans="1:5" ht="15.75" customHeight="1">
+    <row r="244" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A244" s="10"/>
       <c r="B244" s="11"/>
       <c r="C244" s="10"/>
       <c r="D244" s="11"/>
       <c r="E244" s="11"/>
     </row>
-    <row r="245" spans="1:5" ht="15.75" customHeight="1">
+    <row r="245" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A245" s="10"/>
       <c r="B245" s="11"/>
       <c r="C245" s="10"/>
       <c r="D245" s="11"/>
       <c r="E245" s="11"/>
     </row>
-    <row r="246" spans="1:5" ht="15.75" customHeight="1">
+    <row r="246" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A246" s="10"/>
       <c r="B246" s="11"/>
       <c r="C246" s="10"/>
       <c r="D246" s="11"/>
       <c r="E246" s="11"/>
     </row>
-    <row r="247" spans="1:5" ht="15.75" customHeight="1">
+    <row r="247" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A247" s="10"/>
       <c r="B247" s="11"/>
       <c r="C247" s="10"/>
       <c r="D247" s="11"/>
       <c r="E247" s="11"/>
     </row>
-    <row r="248" spans="1:5" ht="15.75" customHeight="1">
+    <row r="248" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A248" s="10"/>
       <c r="B248" s="11"/>
       <c r="C248" s="10"/>
       <c r="D248" s="11"/>
       <c r="E248" s="11"/>
     </row>
-    <row r="249" spans="1:5" ht="15.75" customHeight="1">
+    <row r="249" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A249" s="10"/>
       <c r="B249" s="11"/>
       <c r="C249" s="10"/>
       <c r="D249" s="11"/>
       <c r="E249" s="11"/>
     </row>
-    <row r="250" spans="1:5" ht="15.75" customHeight="1">
+    <row r="250" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A250" s="10"/>
       <c r="B250" s="11"/>
       <c r="C250" s="10"/>
       <c r="D250" s="11"/>
       <c r="E250" s="11"/>
     </row>
-    <row r="251" spans="1:5" ht="15.75" customHeight="1">
+    <row r="251" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A251" s="10"/>
       <c r="B251" s="11"/>
       <c r="C251" s="10"/>
       <c r="D251" s="11"/>
       <c r="E251" s="11"/>
     </row>
-    <row r="252" spans="1:5" ht="15.75" customHeight="1">
+    <row r="252" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A252" s="10"/>
       <c r="B252" s="11"/>
       <c r="C252" s="10"/>
       <c r="D252" s="11"/>
       <c r="E252" s="11"/>
     </row>
-    <row r="253" spans="1:5" ht="15.75" customHeight="1">
+    <row r="253" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A253" s="10"/>
       <c r="B253" s="11"/>
       <c r="C253" s="10"/>
       <c r="D253" s="11"/>
       <c r="E253" s="11"/>
     </row>
-    <row r="254" spans="1:5" ht="15.75" customHeight="1">
+    <row r="254" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A254" s="10"/>
       <c r="B254" s="11"/>
       <c r="C254" s="10"/>
       <c r="D254" s="11"/>
       <c r="E254" s="11"/>
     </row>
-    <row r="255" spans="1:5" ht="15.75" customHeight="1">
+    <row r="255" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A255" s="10"/>
       <c r="B255" s="11"/>
       <c r="C255" s="10"/>
       <c r="D255" s="11"/>
       <c r="E255" s="11"/>
     </row>
-    <row r="256" spans="1:5" ht="15.75" customHeight="1">
+    <row r="256" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A256" s="10"/>
       <c r="B256" s="11"/>
       <c r="C256" s="10"/>
       <c r="D256" s="11"/>
       <c r="E256" s="11"/>
     </row>
-    <row r="257" spans="1:5" ht="15.75" customHeight="1">
+    <row r="257" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A257" s="10"/>
       <c r="B257" s="11"/>
       <c r="C257" s="10"/>
       <c r="D257" s="11"/>
       <c r="E257" s="11"/>
     </row>
-    <row r="258" spans="1:5" ht="15.75" customHeight="1">
+    <row r="258" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A258" s="10"/>
       <c r="B258" s="11"/>
       <c r="C258" s="10"/>
       <c r="D258" s="11"/>
       <c r="E258" s="11"/>
     </row>
-    <row r="259" spans="1:5" ht="15.75" customHeight="1">
+    <row r="259" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A259" s="10"/>
       <c r="B259" s="11"/>
       <c r="C259" s="10"/>
       <c r="D259" s="11"/>
       <c r="E259" s="11"/>
     </row>
-    <row r="260" spans="1:5" ht="15.75" customHeight="1">
+    <row r="260" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A260" s="10"/>
       <c r="B260" s="11"/>
       <c r="C260" s="10"/>
@@ -2770,20 +2847,21 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D4" r:id="rId1"/>
-    <hyperlink ref="D5" r:id="rId2"/>
-    <hyperlink ref="D8" r:id="rId3"/>
-    <hyperlink ref="D9" r:id="rId4"/>
-    <hyperlink ref="D10" r:id="rId5"/>
-    <hyperlink ref="D11" r:id="rId6"/>
-    <hyperlink ref="D12" r:id="rId7"/>
-    <hyperlink ref="D14" r:id="rId8"/>
-    <hyperlink ref="D15" r:id="rId9"/>
-    <hyperlink ref="D16" r:id="rId10"/>
-    <hyperlink ref="D17" r:id="rId11"/>
-    <hyperlink ref="D18" r:id="rId12"/>
+    <hyperlink ref="D4" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="D5" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="D8" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="D9" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="D10" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="D11" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="D12" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="D14" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="D15" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="D16" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="D17" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="D18" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="D19" r:id="rId13" xr:uid="{FF36A996-8431-4AEB-BF38-25B60907EB7E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId13"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId14"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Se agrega el 22 Alumno al archivo
</commit_message>
<xml_diff>
--- a/Lista de Alumnos.xlsx
+++ b/Lista de Alumnos.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25330"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Tecnicatura\Electronica\Git clase alumnos\Alumnos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pedro\Alumnos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E546AC4-84FA-4913-BFA5-13AE547E481A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040"/>
   </bookViews>
   <sheets>
     <sheet name="Electronica Microcontrolada" sheetId="1" r:id="rId1"/>
@@ -20,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="67">
   <si>
     <t>#</t>
   </si>
@@ -212,12 +211,21 @@
   </si>
   <si>
     <t>Enrique Alfredo Ripoli</t>
+  </si>
+  <si>
+    <t>Pedro Omar Rojo</t>
+  </si>
+  <si>
+    <t>tecnosisnet@gmail.com</t>
+  </si>
+  <si>
+    <t>tecnosisnet</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -713,14 +721,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:E260"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B16" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView tabSelected="1" topLeftCell="B7" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1089,10 +1097,18 @@
       <c r="A22" s="5">
         <v>21</v>
       </c>
-      <c r="B22" s="6"/>
-      <c r="C22" s="5"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="6"/>
+      <c r="B22" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="C22" s="5">
+        <v>4</v>
+      </c>
+      <c r="D22" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="23" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="5">
@@ -2838,7 +2854,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D21" r:id="rId1" xr:uid="{9CB016FB-33A8-4342-AE7E-94E75E7BAF0F}"/>
+    <hyperlink ref="D21" r:id="rId1"/>
+    <hyperlink ref="D22" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Se agrega el 23 Alumno al archivo
</commit_message>
<xml_diff>
--- a/Lista de Alumnos.xlsx
+++ b/Lista de Alumnos.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25505"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pedro\Alumnos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Juan Diego\Documents\GitHub\ISPC\Electronica Microcontrolada\Alumnos\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE887227-A142-43D1-83CD-CFF66BC72418}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Electronica Microcontrolada" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="70">
   <si>
     <t>#</t>
   </si>
@@ -220,12 +221,21 @@
   </si>
   <si>
     <t>tecnosisnet</t>
+  </si>
+  <si>
+    <t>Juan Diego Gonzalez Antoniazzi</t>
+  </si>
+  <si>
+    <t>jdgaprogrammer@gmail.com</t>
+  </si>
+  <si>
+    <t>JDGA1997</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -721,14 +731,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:E260"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B7" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" topLeftCell="B9" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1114,10 +1124,18 @@
       <c r="A23" s="5">
         <v>22</v>
       </c>
-      <c r="B23" s="6"/>
-      <c r="C23" s="5"/>
-      <c r="D23" s="6"/>
-      <c r="E23" s="6"/>
+      <c r="B23" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="C23" s="5">
+        <v>3</v>
+      </c>
+      <c r="D23" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="24" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="5">
@@ -2854,8 +2872,9 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D21" r:id="rId1"/>
-    <hyperlink ref="D22" r:id="rId2"/>
+    <hyperlink ref="D21" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="D22" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="D23" r:id="rId3" xr:uid="{AF4704A2-EBC1-4DE2-8CA7-F14F49C851B1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Se agrega el 24 Alumno al archivo
</commit_message>
<xml_diff>
--- a/Lista de Alumnos.xlsx
+++ b/Lista de Alumnos.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Juan Diego\Documents\GitHub\ISPC\Electronica Microcontrolada\Alumnos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\TELECOMUNICACIONES\00 ISPC - TECNICATURA\00 PROYECTO INTEGRADOR\GIT\Alumnos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE887227-A142-43D1-83CD-CFF66BC72418}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Electronica Microcontrolada" sheetId="1" r:id="rId1"/>
@@ -20,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="73">
   <si>
     <t>#</t>
   </si>
@@ -230,12 +229,21 @@
   </si>
   <si>
     <t>JDGA1997</t>
+  </si>
+  <si>
+    <t>Pablo Noseda</t>
+  </si>
+  <si>
+    <t>pablonoseda1@gmail.com</t>
+  </si>
+  <si>
+    <t>pablonoseda</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -731,14 +739,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:E260"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B9" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1141,10 +1149,18 @@
       <c r="A24" s="5">
         <v>23</v>
       </c>
-      <c r="B24" s="6"/>
-      <c r="C24" s="5"/>
-      <c r="D24" s="6"/>
-      <c r="E24" s="6"/>
+      <c r="B24" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="C24" s="5">
+        <v>1</v>
+      </c>
+      <c r="D24" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="25" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="5">
@@ -2872,9 +2888,10 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D21" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="D22" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="D23" r:id="rId3" xr:uid="{AF4704A2-EBC1-4DE2-8CA7-F14F49C851B1}"/>
+    <hyperlink ref="D21" r:id="rId1"/>
+    <hyperlink ref="D22" r:id="rId2"/>
+    <hyperlink ref="D23" r:id="rId3"/>
+    <hyperlink ref="D24" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Se agrego el 25 Alumno al archivo
</commit_message>
<xml_diff>
--- a/Lista de Alumnos.xlsx
+++ b/Lista de Alumnos.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\TELECOMUNICACIONES\00 ISPC - TECNICATURA\00 PROYECTO INTEGRADOR\GIT\Alumnos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PerfLogs\Proyecto\Alumnos\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="76">
   <si>
     <t>#</t>
   </si>
@@ -238,12 +238,21 @@
   </si>
   <si>
     <t>pablonoseda</t>
+  </si>
+  <si>
+    <t>Vera Emilio Andres</t>
+  </si>
+  <si>
+    <t>evera8@hotmail.com</t>
+  </si>
+  <si>
+    <t>evera8</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -745,8 +754,8 @@
   </sheetPr>
   <dimension ref="A1:E260"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B9" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView tabSelected="1" topLeftCell="B7" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1166,10 +1175,18 @@
       <c r="A25" s="5">
         <v>24</v>
       </c>
-      <c r="B25" s="6"/>
-      <c r="C25" s="5"/>
-      <c r="D25" s="6"/>
-      <c r="E25" s="6"/>
+      <c r="B25" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="C25" s="5">
+        <v>4</v>
+      </c>
+      <c r="D25" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="26" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="5">
@@ -2892,6 +2909,7 @@
     <hyperlink ref="D22" r:id="rId2"/>
     <hyperlink ref="D23" r:id="rId3"/>
     <hyperlink ref="D24" r:id="rId4"/>
+    <hyperlink ref="D25" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Se agrega el 25 Alumno al archivo
</commit_message>
<xml_diff>
--- a/Lista de Alumnos.xlsx
+++ b/Lista de Alumnos.xlsx
@@ -1,25 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PerfLogs\Proyecto\Alumnos\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Electronica Microcontrolada" sheetId="1" r:id="rId1"/>
+    <sheet r:id="rId1" sheetId="1" name="Electronica Microcontrolada"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="79">
   <si>
     <t>#</t>
   </si>
@@ -204,15 +199,15 @@
     <t>matiluajn</t>
   </si>
   <si>
+    <t>Enrique Alfredo Ripoli</t>
+  </si>
+  <si>
     <t>enriqueripoli01@gmail.com</t>
   </si>
   <si>
     <t>enriqueripoli</t>
   </si>
   <si>
-    <t>Enrique Alfredo Ripoli</t>
-  </si>
-  <si>
     <t>Pedro Omar Rojo</t>
   </si>
   <si>
@@ -247,13 +242,23 @@
   </si>
   <si>
     <t>evera8</t>
+  </si>
+  <si>
+    <t>Andrea Celeste Suarez</t>
+  </si>
+  <si>
+    <t>celestessuarez00@gmail.com</t>
+  </si>
+  <si>
+    <t>CelesteSuarezz</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -290,7 +295,7 @@
     <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF0563C1"/>
+      <color rgb="FF0563c1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -306,14 +311,6 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -392,73 +389,65 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+  <cellXfs count="16">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="4" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="4" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="4" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="4" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="4" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="4" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="4" applyBorder="1" fontId="6" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="7" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="5" applyBorder="1" fontId="7" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="5" applyBorder="1" fontId="7" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  <cellStyles count="1">
+    <cellStyle xfId="0" builtinId="0" name="Normal"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -469,10 +458,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -510,71 +499,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Times New Roman" script="Arab"/>
+        <a:font typeface="Times New Roman" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="MoolBoran" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Times New Roman" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Arial" script="Arab"/>
+        <a:font typeface="Arial" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="DaunPenh" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Arial" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -602,7 +591,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -625,11 +614,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -638,13 +627,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -654,7 +643,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -663,7 +652,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -672,7 +661,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -680,10 +669,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
+              <a:rot rev="0" lon="0" lat="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
+            <a:lightRig dir="t" rig="threePt">
+              <a:rot rev="1200000" lon="0" lat="0"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -754,20 +743,18 @@
   </sheetPr>
   <dimension ref="A1:E260"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B7" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
-    </sheetView>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.85546875" style="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="37.140625" style="15" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.5703125" style="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="31" style="15" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="29" style="15" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" style="14" width="6.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="15" width="37.14785714285715" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="14" width="10.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="15" width="31.005" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="15" width="29.005" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="27">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -784,7 +771,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -801,7 +788,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="5">
         <v>2</v>
       </c>
@@ -816,7 +803,7 @@
       </c>
       <c r="E3" s="6"/>
     </row>
-    <row r="4" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="5">
         <v>3</v>
       </c>
@@ -833,7 +820,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
       <c r="A5" s="5">
         <v>4</v>
       </c>
@@ -850,7 +837,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
       <c r="A6" s="5">
         <v>5</v>
       </c>
@@ -867,7 +854,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
       <c r="A7" s="5">
         <v>6</v>
       </c>
@@ -884,7 +871,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
       <c r="A8" s="5">
         <v>7</v>
       </c>
@@ -901,7 +888,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
       <c r="A9" s="5">
         <v>8</v>
       </c>
@@ -918,7 +905,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
       <c r="A10" s="5">
         <v>9</v>
       </c>
@@ -933,7 +920,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
       <c r="A11" s="5">
         <v>10</v>
       </c>
@@ -950,7 +937,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
       <c r="A12" s="5">
         <v>11</v>
       </c>
@@ -967,7 +954,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
       <c r="A13" s="5">
         <v>12</v>
       </c>
@@ -984,7 +971,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
       <c r="A14" s="5">
         <v>13</v>
       </c>
@@ -1001,7 +988,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
       <c r="A15" s="5">
         <v>14</v>
       </c>
@@ -1018,7 +1005,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
       <c r="A16" s="5">
         <v>15</v>
       </c>
@@ -1035,7 +1022,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
       <c r="A17" s="5">
         <v>16</v>
       </c>
@@ -1052,7 +1039,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
       <c r="A18" s="5">
         <v>17</v>
       </c>
@@ -1069,7 +1056,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
       <c r="A19" s="5">
         <v>18</v>
       </c>
@@ -1086,7 +1073,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5">
       <c r="A20" s="5">
         <v>19</v>
       </c>
@@ -1103,24 +1090,24 @@
         <v>60</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5">
       <c r="A21" s="5">
         <v>20</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C21" s="5">
         <v>2</v>
       </c>
-      <c r="D21" s="16" t="s">
-        <v>61</v>
+      <c r="D21" s="11" t="s">
+        <v>62</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="25.5">
       <c r="A22" s="5">
         <v>21</v>
       </c>
@@ -1130,14 +1117,14 @@
       <c r="C22" s="5">
         <v>4</v>
       </c>
-      <c r="D22" s="16" t="s">
+      <c r="D22" s="11" t="s">
         <v>65</v>
       </c>
       <c r="E22" s="6" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="25.5">
       <c r="A23" s="5">
         <v>22</v>
       </c>
@@ -1147,14 +1134,14 @@
       <c r="C23" s="5">
         <v>3</v>
       </c>
-      <c r="D23" s="16" t="s">
+      <c r="D23" s="11" t="s">
         <v>68</v>
       </c>
       <c r="E23" s="6" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="25.5">
       <c r="A24" s="5">
         <v>23</v>
       </c>
@@ -1164,14 +1151,14 @@
       <c r="C24" s="5">
         <v>1</v>
       </c>
-      <c r="D24" s="16" t="s">
+      <c r="D24" s="11" t="s">
         <v>71</v>
       </c>
       <c r="E24" s="6" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="25.5">
       <c r="A25" s="5">
         <v>24</v>
       </c>
@@ -1181,23 +1168,31 @@
       <c r="C25" s="5">
         <v>4</v>
       </c>
-      <c r="D25" s="16" t="s">
+      <c r="D25" s="11" t="s">
         <v>74</v>
       </c>
       <c r="E25" s="6" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="25.5">
       <c r="A26" s="5">
         <v>25</v>
       </c>
-      <c r="B26" s="6"/>
-      <c r="C26" s="5"/>
-      <c r="D26" s="6"/>
-      <c r="E26" s="6"/>
-    </row>
-    <row r="27" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="C26" s="5">
+        <v>2</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="25.5">
       <c r="A27" s="5">
         <v>26</v>
       </c>
@@ -1206,7 +1201,7 @@
       <c r="D27" s="6"/>
       <c r="E27" s="6"/>
     </row>
-    <row r="28" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="25.5">
       <c r="A28" s="5">
         <v>27</v>
       </c>
@@ -1215,7 +1210,7 @@
       <c r="D28" s="6"/>
       <c r="E28" s="6"/>
     </row>
-    <row r="29" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="25.5">
       <c r="A29" s="5">
         <v>28</v>
       </c>
@@ -1224,7 +1219,7 @@
       <c r="D29" s="6"/>
       <c r="E29" s="6"/>
     </row>
-    <row r="30" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="25.5">
       <c r="A30" s="5">
         <v>29</v>
       </c>
@@ -1233,7 +1228,7 @@
       <c r="D30" s="6"/>
       <c r="E30" s="6"/>
     </row>
-    <row r="31" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="25.5">
       <c r="A31" s="5">
         <v>30</v>
       </c>
@@ -1242,7 +1237,7 @@
       <c r="D31" s="6"/>
       <c r="E31" s="6"/>
     </row>
-    <row r="32" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="25.5">
       <c r="A32" s="5">
         <v>31</v>
       </c>
@@ -1251,7 +1246,7 @@
       <c r="D32" s="6"/>
       <c r="E32" s="6"/>
     </row>
-    <row r="33" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="25.5">
       <c r="A33" s="5">
         <v>32</v>
       </c>
@@ -1260,7 +1255,7 @@
       <c r="D33" s="6"/>
       <c r="E33" s="6"/>
     </row>
-    <row r="34" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="25.5">
       <c r="A34" s="5">
         <v>33</v>
       </c>
@@ -1269,7 +1264,7 @@
       <c r="D34" s="6"/>
       <c r="E34" s="6"/>
     </row>
-    <row r="35" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="25.5">
       <c r="A35" s="5">
         <v>34</v>
       </c>
@@ -1278,7 +1273,7 @@
       <c r="D35" s="6"/>
       <c r="E35" s="6"/>
     </row>
-    <row r="36" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="25.5">
       <c r="A36" s="5">
         <v>35</v>
       </c>
@@ -1287,7 +1282,7 @@
       <c r="D36" s="6"/>
       <c r="E36" s="6"/>
     </row>
-    <row r="37" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="25.5">
       <c r="A37" s="5">
         <v>36</v>
       </c>
@@ -1296,7 +1291,7 @@
       <c r="D37" s="6"/>
       <c r="E37" s="6"/>
     </row>
-    <row r="38" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="25.5">
       <c r="A38" s="5">
         <v>37</v>
       </c>
@@ -1305,7 +1300,7 @@
       <c r="D38" s="6"/>
       <c r="E38" s="6"/>
     </row>
-    <row r="39" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="25.5">
       <c r="A39" s="5">
         <v>38</v>
       </c>
@@ -1314,7 +1309,7 @@
       <c r="D39" s="6"/>
       <c r="E39" s="6"/>
     </row>
-    <row r="40" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="25.5">
       <c r="A40" s="5">
         <v>39</v>
       </c>
@@ -1323,7 +1318,7 @@
       <c r="D40" s="6"/>
       <c r="E40" s="6"/>
     </row>
-    <row r="41" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="25.5">
       <c r="A41" s="5">
         <v>40</v>
       </c>
@@ -1332,7 +1327,7 @@
       <c r="D41" s="6"/>
       <c r="E41" s="6"/>
     </row>
-    <row r="42" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="25.5">
       <c r="A42" s="5">
         <v>41</v>
       </c>
@@ -1341,7 +1336,7 @@
       <c r="D42" s="6"/>
       <c r="E42" s="6"/>
     </row>
-    <row r="43" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="25.5">
       <c r="A43" s="5">
         <v>42</v>
       </c>
@@ -1350,7 +1345,7 @@
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
     </row>
-    <row r="44" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="25.5">
       <c r="A44" s="5">
         <v>43</v>
       </c>
@@ -1359,7 +1354,7 @@
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
     </row>
-    <row r="45" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="25.5">
       <c r="A45" s="5">
         <v>44</v>
       </c>
@@ -1368,7 +1363,7 @@
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
     </row>
-    <row r="46" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="25.5">
       <c r="A46" s="5">
         <v>45</v>
       </c>
@@ -1377,7 +1372,7 @@
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
     </row>
-    <row r="47" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="25.5">
       <c r="A47" s="5">
         <v>46</v>
       </c>
@@ -1386,7 +1381,7 @@
       <c r="D47" s="6"/>
       <c r="E47" s="6"/>
     </row>
-    <row r="48" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="25.5">
       <c r="A48" s="5">
         <v>47</v>
       </c>
@@ -1395,7 +1390,7 @@
       <c r="D48" s="6"/>
       <c r="E48" s="6"/>
     </row>
-    <row r="49" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="25.5">
       <c r="A49" s="5">
         <v>48</v>
       </c>
@@ -1404,7 +1399,7 @@
       <c r="D49" s="6"/>
       <c r="E49" s="6"/>
     </row>
-    <row r="50" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="25.5">
       <c r="A50" s="5">
         <v>49</v>
       </c>
@@ -1413,7 +1408,7 @@
       <c r="D50" s="6"/>
       <c r="E50" s="6"/>
     </row>
-    <row r="51" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="51" customHeight="1" ht="25.5">
       <c r="A51" s="5">
         <v>50</v>
       </c>
@@ -1422,7 +1417,7 @@
       <c r="D51" s="6"/>
       <c r="E51" s="6"/>
     </row>
-    <row r="52" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="52" customHeight="1" ht="25.5">
       <c r="A52" s="5">
         <v>51</v>
       </c>
@@ -1431,7 +1426,7 @@
       <c r="D52" s="6"/>
       <c r="E52" s="6"/>
     </row>
-    <row r="53" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="53" customHeight="1" ht="25.5">
       <c r="A53" s="5">
         <v>52</v>
       </c>
@@ -1440,7 +1435,7 @@
       <c r="D53" s="6"/>
       <c r="E53" s="6"/>
     </row>
-    <row r="54" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="54" customHeight="1" ht="25.5">
       <c r="A54" s="5">
         <v>53</v>
       </c>
@@ -1449,7 +1444,7 @@
       <c r="D54" s="6"/>
       <c r="E54" s="6"/>
     </row>
-    <row r="55" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="55" customHeight="1" ht="25.5">
       <c r="A55" s="5">
         <v>54</v>
       </c>
@@ -1458,7 +1453,7 @@
       <c r="D55" s="6"/>
       <c r="E55" s="6"/>
     </row>
-    <row r="56" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="56" customHeight="1" ht="25.5">
       <c r="A56" s="5">
         <v>55</v>
       </c>
@@ -1467,7 +1462,7 @@
       <c r="D56" s="6"/>
       <c r="E56" s="6"/>
     </row>
-    <row r="57" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="57" customHeight="1" ht="25.5">
       <c r="A57" s="5">
         <v>56</v>
       </c>
@@ -1476,7 +1471,7 @@
       <c r="D57" s="6"/>
       <c r="E57" s="6"/>
     </row>
-    <row r="58" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="58" customHeight="1" ht="25.5">
       <c r="A58" s="5">
         <v>57</v>
       </c>
@@ -1485,7 +1480,7 @@
       <c r="D58" s="6"/>
       <c r="E58" s="6"/>
     </row>
-    <row r="59" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="59" customHeight="1" ht="25.5">
       <c r="A59" s="5">
         <v>58</v>
       </c>
@@ -1494,7 +1489,7 @@
       <c r="D59" s="6"/>
       <c r="E59" s="6"/>
     </row>
-    <row r="60" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="60" customHeight="1" ht="25.5">
       <c r="A60" s="5">
         <v>59</v>
       </c>
@@ -1503,1400 +1498,1400 @@
       <c r="D60" s="6"/>
       <c r="E60" s="6"/>
     </row>
-    <row r="61" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="61" customHeight="1" ht="15.75">
       <c r="A61" s="12"/>
       <c r="B61" s="13"/>
       <c r="C61" s="12"/>
       <c r="D61" s="13"/>
       <c r="E61" s="13"/>
     </row>
-    <row r="62" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="62" customHeight="1" ht="15.75">
       <c r="A62" s="12"/>
       <c r="B62" s="13"/>
       <c r="C62" s="12"/>
       <c r="D62" s="13"/>
       <c r="E62" s="13"/>
     </row>
-    <row r="63" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="63" customHeight="1" ht="15.75">
       <c r="A63" s="12"/>
       <c r="B63" s="13"/>
       <c r="C63" s="12"/>
       <c r="D63" s="13"/>
       <c r="E63" s="13"/>
     </row>
-    <row r="64" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="64" customHeight="1" ht="15.75">
       <c r="A64" s="12"/>
       <c r="B64" s="13"/>
       <c r="C64" s="12"/>
       <c r="D64" s="13"/>
       <c r="E64" s="13"/>
     </row>
-    <row r="65" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="65" customHeight="1" ht="15.75">
       <c r="A65" s="12"/>
       <c r="B65" s="13"/>
       <c r="C65" s="12"/>
       <c r="D65" s="13"/>
       <c r="E65" s="13"/>
     </row>
-    <row r="66" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="66" customHeight="1" ht="15.75">
       <c r="A66" s="12"/>
       <c r="B66" s="13"/>
       <c r="C66" s="12"/>
       <c r="D66" s="13"/>
       <c r="E66" s="13"/>
     </row>
-    <row r="67" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="67" customHeight="1" ht="15.75">
       <c r="A67" s="12"/>
       <c r="B67" s="13"/>
       <c r="C67" s="12"/>
       <c r="D67" s="13"/>
       <c r="E67" s="13"/>
     </row>
-    <row r="68" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="68" customHeight="1" ht="15.75">
       <c r="A68" s="12"/>
       <c r="B68" s="13"/>
       <c r="C68" s="12"/>
       <c r="D68" s="13"/>
       <c r="E68" s="13"/>
     </row>
-    <row r="69" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="69" customHeight="1" ht="15.75">
       <c r="A69" s="12"/>
       <c r="B69" s="13"/>
       <c r="C69" s="12"/>
       <c r="D69" s="13"/>
       <c r="E69" s="13"/>
     </row>
-    <row r="70" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="70" customHeight="1" ht="15.75">
       <c r="A70" s="12"/>
       <c r="B70" s="13"/>
       <c r="C70" s="12"/>
       <c r="D70" s="13"/>
       <c r="E70" s="13"/>
     </row>
-    <row r="71" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="71" customHeight="1" ht="15.75">
       <c r="A71" s="12"/>
       <c r="B71" s="13"/>
       <c r="C71" s="12"/>
       <c r="D71" s="13"/>
       <c r="E71" s="13"/>
     </row>
-    <row r="72" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="72" customHeight="1" ht="15.75">
       <c r="A72" s="12"/>
       <c r="B72" s="13"/>
       <c r="C72" s="12"/>
       <c r="D72" s="13"/>
       <c r="E72" s="13"/>
     </row>
-    <row r="73" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="73" customHeight="1" ht="15.75">
       <c r="A73" s="12"/>
       <c r="B73" s="13"/>
       <c r="C73" s="12"/>
       <c r="D73" s="13"/>
       <c r="E73" s="13"/>
     </row>
-    <row r="74" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="74" customHeight="1" ht="15.75">
       <c r="A74" s="12"/>
       <c r="B74" s="13"/>
       <c r="C74" s="12"/>
       <c r="D74" s="13"/>
       <c r="E74" s="13"/>
     </row>
-    <row r="75" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="75" customHeight="1" ht="15.75">
       <c r="A75" s="12"/>
       <c r="B75" s="13"/>
       <c r="C75" s="12"/>
       <c r="D75" s="13"/>
       <c r="E75" s="13"/>
     </row>
-    <row r="76" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="76" customHeight="1" ht="15.75">
       <c r="A76" s="12"/>
       <c r="B76" s="13"/>
       <c r="C76" s="12"/>
       <c r="D76" s="13"/>
       <c r="E76" s="13"/>
     </row>
-    <row r="77" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="77" customHeight="1" ht="15.75">
       <c r="A77" s="12"/>
       <c r="B77" s="13"/>
       <c r="C77" s="12"/>
       <c r="D77" s="13"/>
       <c r="E77" s="13"/>
     </row>
-    <row r="78" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="78" customHeight="1" ht="15.75">
       <c r="A78" s="12"/>
       <c r="B78" s="13"/>
       <c r="C78" s="12"/>
       <c r="D78" s="13"/>
       <c r="E78" s="13"/>
     </row>
-    <row r="79" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="79" customHeight="1" ht="15.75">
       <c r="A79" s="12"/>
       <c r="B79" s="13"/>
       <c r="C79" s="12"/>
       <c r="D79" s="13"/>
       <c r="E79" s="13"/>
     </row>
-    <row r="80" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="80" customHeight="1" ht="15.75">
       <c r="A80" s="12"/>
       <c r="B80" s="13"/>
       <c r="C80" s="12"/>
       <c r="D80" s="13"/>
       <c r="E80" s="13"/>
     </row>
-    <row r="81" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="81" customHeight="1" ht="15.75">
       <c r="A81" s="12"/>
       <c r="B81" s="13"/>
       <c r="C81" s="12"/>
       <c r="D81" s="13"/>
       <c r="E81" s="13"/>
     </row>
-    <row r="82" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="82" customHeight="1" ht="15.75">
       <c r="A82" s="12"/>
       <c r="B82" s="13"/>
       <c r="C82" s="12"/>
       <c r="D82" s="13"/>
       <c r="E82" s="13"/>
     </row>
-    <row r="83" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="83" customHeight="1" ht="15.75">
       <c r="A83" s="12"/>
       <c r="B83" s="13"/>
       <c r="C83" s="12"/>
       <c r="D83" s="13"/>
       <c r="E83" s="13"/>
     </row>
-    <row r="84" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="84" customHeight="1" ht="15.75">
       <c r="A84" s="12"/>
       <c r="B84" s="13"/>
       <c r="C84" s="12"/>
       <c r="D84" s="13"/>
       <c r="E84" s="13"/>
     </row>
-    <row r="85" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="85" customHeight="1" ht="15.75">
       <c r="A85" s="12"/>
       <c r="B85" s="13"/>
       <c r="C85" s="12"/>
       <c r="D85" s="13"/>
       <c r="E85" s="13"/>
     </row>
-    <row r="86" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="86" customHeight="1" ht="15.75">
       <c r="A86" s="12"/>
       <c r="B86" s="13"/>
       <c r="C86" s="12"/>
       <c r="D86" s="13"/>
       <c r="E86" s="13"/>
     </row>
-    <row r="87" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="87" customHeight="1" ht="15.75">
       <c r="A87" s="12"/>
       <c r="B87" s="13"/>
       <c r="C87" s="12"/>
       <c r="D87" s="13"/>
       <c r="E87" s="13"/>
     </row>
-    <row r="88" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="88" customHeight="1" ht="15.75">
       <c r="A88" s="12"/>
       <c r="B88" s="13"/>
       <c r="C88" s="12"/>
       <c r="D88" s="13"/>
       <c r="E88" s="13"/>
     </row>
-    <row r="89" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="89" customHeight="1" ht="15.75">
       <c r="A89" s="12"/>
       <c r="B89" s="13"/>
       <c r="C89" s="12"/>
       <c r="D89" s="13"/>
       <c r="E89" s="13"/>
     </row>
-    <row r="90" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="90" customHeight="1" ht="15.75">
       <c r="A90" s="12"/>
       <c r="B90" s="13"/>
       <c r="C90" s="12"/>
       <c r="D90" s="13"/>
       <c r="E90" s="13"/>
     </row>
-    <row r="91" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="91" customHeight="1" ht="15.75">
       <c r="A91" s="12"/>
       <c r="B91" s="13"/>
       <c r="C91" s="12"/>
       <c r="D91" s="13"/>
       <c r="E91" s="13"/>
     </row>
-    <row r="92" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="92" customHeight="1" ht="15.75">
       <c r="A92" s="12"/>
       <c r="B92" s="13"/>
       <c r="C92" s="12"/>
       <c r="D92" s="13"/>
       <c r="E92" s="13"/>
     </row>
-    <row r="93" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="93" customHeight="1" ht="15.75">
       <c r="A93" s="12"/>
       <c r="B93" s="13"/>
       <c r="C93" s="12"/>
       <c r="D93" s="13"/>
       <c r="E93" s="13"/>
     </row>
-    <row r="94" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="94" customHeight="1" ht="15.75">
       <c r="A94" s="12"/>
       <c r="B94" s="13"/>
       <c r="C94" s="12"/>
       <c r="D94" s="13"/>
       <c r="E94" s="13"/>
     </row>
-    <row r="95" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="95" customHeight="1" ht="15.75">
       <c r="A95" s="12"/>
       <c r="B95" s="13"/>
       <c r="C95" s="12"/>
       <c r="D95" s="13"/>
       <c r="E95" s="13"/>
     </row>
-    <row r="96" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="96" customHeight="1" ht="15.75">
       <c r="A96" s="12"/>
       <c r="B96" s="13"/>
       <c r="C96" s="12"/>
       <c r="D96" s="13"/>
       <c r="E96" s="13"/>
     </row>
-    <row r="97" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="97" customHeight="1" ht="15.75">
       <c r="A97" s="12"/>
       <c r="B97" s="13"/>
       <c r="C97" s="12"/>
       <c r="D97" s="13"/>
       <c r="E97" s="13"/>
     </row>
-    <row r="98" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="98" customHeight="1" ht="15.75">
       <c r="A98" s="12"/>
       <c r="B98" s="13"/>
       <c r="C98" s="12"/>
       <c r="D98" s="13"/>
       <c r="E98" s="13"/>
     </row>
-    <row r="99" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="99" customHeight="1" ht="15.75">
       <c r="A99" s="12"/>
       <c r="B99" s="13"/>
       <c r="C99" s="12"/>
       <c r="D99" s="13"/>
       <c r="E99" s="13"/>
     </row>
-    <row r="100" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="100" customHeight="1" ht="15.75">
       <c r="A100" s="12"/>
       <c r="B100" s="13"/>
       <c r="C100" s="12"/>
       <c r="D100" s="13"/>
       <c r="E100" s="13"/>
     </row>
-    <row r="101" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="101" customHeight="1" ht="15.75">
       <c r="A101" s="12"/>
       <c r="B101" s="13"/>
       <c r="C101" s="12"/>
       <c r="D101" s="13"/>
       <c r="E101" s="13"/>
     </row>
-    <row r="102" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="102" customHeight="1" ht="15.75">
       <c r="A102" s="12"/>
       <c r="B102" s="13"/>
       <c r="C102" s="12"/>
       <c r="D102" s="13"/>
       <c r="E102" s="13"/>
     </row>
-    <row r="103" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="103" customHeight="1" ht="15.75">
       <c r="A103" s="12"/>
       <c r="B103" s="13"/>
       <c r="C103" s="12"/>
       <c r="D103" s="13"/>
       <c r="E103" s="13"/>
     </row>
-    <row r="104" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="104" customHeight="1" ht="15.75">
       <c r="A104" s="12"/>
       <c r="B104" s="13"/>
       <c r="C104" s="12"/>
       <c r="D104" s="13"/>
       <c r="E104" s="13"/>
     </row>
-    <row r="105" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="105" customHeight="1" ht="15.75">
       <c r="A105" s="12"/>
       <c r="B105" s="13"/>
       <c r="C105" s="12"/>
       <c r="D105" s="13"/>
       <c r="E105" s="13"/>
     </row>
-    <row r="106" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="106" customHeight="1" ht="15.75">
       <c r="A106" s="12"/>
       <c r="B106" s="13"/>
       <c r="C106" s="12"/>
       <c r="D106" s="13"/>
       <c r="E106" s="13"/>
     </row>
-    <row r="107" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="107" customHeight="1" ht="15.75">
       <c r="A107" s="12"/>
       <c r="B107" s="13"/>
       <c r="C107" s="12"/>
       <c r="D107" s="13"/>
       <c r="E107" s="13"/>
     </row>
-    <row r="108" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="108" customHeight="1" ht="15.75">
       <c r="A108" s="12"/>
       <c r="B108" s="13"/>
       <c r="C108" s="12"/>
       <c r="D108" s="13"/>
       <c r="E108" s="13"/>
     </row>
-    <row r="109" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="109" customHeight="1" ht="15.75">
       <c r="A109" s="12"/>
       <c r="B109" s="13"/>
       <c r="C109" s="12"/>
       <c r="D109" s="13"/>
       <c r="E109" s="13"/>
     </row>
-    <row r="110" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="110" customHeight="1" ht="15.75">
       <c r="A110" s="12"/>
       <c r="B110" s="13"/>
       <c r="C110" s="12"/>
       <c r="D110" s="13"/>
       <c r="E110" s="13"/>
     </row>
-    <row r="111" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="111" customHeight="1" ht="15.75">
       <c r="A111" s="12"/>
       <c r="B111" s="13"/>
       <c r="C111" s="12"/>
       <c r="D111" s="13"/>
       <c r="E111" s="13"/>
     </row>
-    <row r="112" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="112" customHeight="1" ht="15.75">
       <c r="A112" s="12"/>
       <c r="B112" s="13"/>
       <c r="C112" s="12"/>
       <c r="D112" s="13"/>
       <c r="E112" s="13"/>
     </row>
-    <row r="113" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="113" customHeight="1" ht="15.75">
       <c r="A113" s="12"/>
       <c r="B113" s="13"/>
       <c r="C113" s="12"/>
       <c r="D113" s="13"/>
       <c r="E113" s="13"/>
     </row>
-    <row r="114" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="114" customHeight="1" ht="15.75">
       <c r="A114" s="12"/>
       <c r="B114" s="13"/>
       <c r="C114" s="12"/>
       <c r="D114" s="13"/>
       <c r="E114" s="13"/>
     </row>
-    <row r="115" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="115" customHeight="1" ht="15.75">
       <c r="A115" s="12"/>
       <c r="B115" s="13"/>
       <c r="C115" s="12"/>
       <c r="D115" s="13"/>
       <c r="E115" s="13"/>
     </row>
-    <row r="116" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="116" customHeight="1" ht="15.75">
       <c r="A116" s="12"/>
       <c r="B116" s="13"/>
       <c r="C116" s="12"/>
       <c r="D116" s="13"/>
       <c r="E116" s="13"/>
     </row>
-    <row r="117" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="117" customHeight="1" ht="15.75">
       <c r="A117" s="12"/>
       <c r="B117" s="13"/>
       <c r="C117" s="12"/>
       <c r="D117" s="13"/>
       <c r="E117" s="13"/>
     </row>
-    <row r="118" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="118" customHeight="1" ht="15.75">
       <c r="A118" s="12"/>
       <c r="B118" s="13"/>
       <c r="C118" s="12"/>
       <c r="D118" s="13"/>
       <c r="E118" s="13"/>
     </row>
-    <row r="119" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="119" customHeight="1" ht="15.75">
       <c r="A119" s="12"/>
       <c r="B119" s="13"/>
       <c r="C119" s="12"/>
       <c r="D119" s="13"/>
       <c r="E119" s="13"/>
     </row>
-    <row r="120" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="120" customHeight="1" ht="15.75">
       <c r="A120" s="12"/>
       <c r="B120" s="13"/>
       <c r="C120" s="12"/>
       <c r="D120" s="13"/>
       <c r="E120" s="13"/>
     </row>
-    <row r="121" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="121" customHeight="1" ht="15.75">
       <c r="A121" s="12"/>
       <c r="B121" s="13"/>
       <c r="C121" s="12"/>
       <c r="D121" s="13"/>
       <c r="E121" s="13"/>
     </row>
-    <row r="122" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="122" customHeight="1" ht="15.75">
       <c r="A122" s="12"/>
       <c r="B122" s="13"/>
       <c r="C122" s="12"/>
       <c r="D122" s="13"/>
       <c r="E122" s="13"/>
     </row>
-    <row r="123" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="123" customHeight="1" ht="15.75">
       <c r="A123" s="12"/>
       <c r="B123" s="13"/>
       <c r="C123" s="12"/>
       <c r="D123" s="13"/>
       <c r="E123" s="13"/>
     </row>
-    <row r="124" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="124" customHeight="1" ht="15.75">
       <c r="A124" s="12"/>
       <c r="B124" s="13"/>
       <c r="C124" s="12"/>
       <c r="D124" s="13"/>
       <c r="E124" s="13"/>
     </row>
-    <row r="125" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="125" customHeight="1" ht="15.75">
       <c r="A125" s="12"/>
       <c r="B125" s="13"/>
       <c r="C125" s="12"/>
       <c r="D125" s="13"/>
       <c r="E125" s="13"/>
     </row>
-    <row r="126" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="126" customHeight="1" ht="15.75">
       <c r="A126" s="12"/>
       <c r="B126" s="13"/>
       <c r="C126" s="12"/>
       <c r="D126" s="13"/>
       <c r="E126" s="13"/>
     </row>
-    <row r="127" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="127" customHeight="1" ht="15.75">
       <c r="A127" s="12"/>
       <c r="B127" s="13"/>
       <c r="C127" s="12"/>
       <c r="D127" s="13"/>
       <c r="E127" s="13"/>
     </row>
-    <row r="128" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="128" customHeight="1" ht="15.75">
       <c r="A128" s="12"/>
       <c r="B128" s="13"/>
       <c r="C128" s="12"/>
       <c r="D128" s="13"/>
       <c r="E128" s="13"/>
     </row>
-    <row r="129" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="129" customHeight="1" ht="15.75">
       <c r="A129" s="12"/>
       <c r="B129" s="13"/>
       <c r="C129" s="12"/>
       <c r="D129" s="13"/>
       <c r="E129" s="13"/>
     </row>
-    <row r="130" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="130" customHeight="1" ht="15.75">
       <c r="A130" s="12"/>
       <c r="B130" s="13"/>
       <c r="C130" s="12"/>
       <c r="D130" s="13"/>
       <c r="E130" s="13"/>
     </row>
-    <row r="131" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="131" customHeight="1" ht="15.75">
       <c r="A131" s="12"/>
       <c r="B131" s="13"/>
       <c r="C131" s="12"/>
       <c r="D131" s="13"/>
       <c r="E131" s="13"/>
     </row>
-    <row r="132" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="132" customHeight="1" ht="15.75">
       <c r="A132" s="12"/>
       <c r="B132" s="13"/>
       <c r="C132" s="12"/>
       <c r="D132" s="13"/>
       <c r="E132" s="13"/>
     </row>
-    <row r="133" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="133" customHeight="1" ht="15.75">
       <c r="A133" s="12"/>
       <c r="B133" s="13"/>
       <c r="C133" s="12"/>
       <c r="D133" s="13"/>
       <c r="E133" s="13"/>
     </row>
-    <row r="134" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="134" customHeight="1" ht="15.75">
       <c r="A134" s="12"/>
       <c r="B134" s="13"/>
       <c r="C134" s="12"/>
       <c r="D134" s="13"/>
       <c r="E134" s="13"/>
     </row>
-    <row r="135" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="135" customHeight="1" ht="15.75">
       <c r="A135" s="12"/>
       <c r="B135" s="13"/>
       <c r="C135" s="12"/>
       <c r="D135" s="13"/>
       <c r="E135" s="13"/>
     </row>
-    <row r="136" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="136" customHeight="1" ht="15.75">
       <c r="A136" s="12"/>
       <c r="B136" s="13"/>
       <c r="C136" s="12"/>
       <c r="D136" s="13"/>
       <c r="E136" s="13"/>
     </row>
-    <row r="137" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="137" customHeight="1" ht="15.75">
       <c r="A137" s="12"/>
       <c r="B137" s="13"/>
       <c r="C137" s="12"/>
       <c r="D137" s="13"/>
       <c r="E137" s="13"/>
     </row>
-    <row r="138" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="138" customHeight="1" ht="15.75">
       <c r="A138" s="12"/>
       <c r="B138" s="13"/>
       <c r="C138" s="12"/>
       <c r="D138" s="13"/>
       <c r="E138" s="13"/>
     </row>
-    <row r="139" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="139" customHeight="1" ht="15.75">
       <c r="A139" s="12"/>
       <c r="B139" s="13"/>
       <c r="C139" s="12"/>
       <c r="D139" s="13"/>
       <c r="E139" s="13"/>
     </row>
-    <row r="140" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="140" customHeight="1" ht="15.75">
       <c r="A140" s="12"/>
       <c r="B140" s="13"/>
       <c r="C140" s="12"/>
       <c r="D140" s="13"/>
       <c r="E140" s="13"/>
     </row>
-    <row r="141" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="141" customHeight="1" ht="15.75">
       <c r="A141" s="12"/>
       <c r="B141" s="13"/>
       <c r="C141" s="12"/>
       <c r="D141" s="13"/>
       <c r="E141" s="13"/>
     </row>
-    <row r="142" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="142" customHeight="1" ht="15.75">
       <c r="A142" s="12"/>
       <c r="B142" s="13"/>
       <c r="C142" s="12"/>
       <c r="D142" s="13"/>
       <c r="E142" s="13"/>
     </row>
-    <row r="143" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="143" customHeight="1" ht="15.75">
       <c r="A143" s="12"/>
       <c r="B143" s="13"/>
       <c r="C143" s="12"/>
       <c r="D143" s="13"/>
       <c r="E143" s="13"/>
     </row>
-    <row r="144" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="144" customHeight="1" ht="15.75">
       <c r="A144" s="12"/>
       <c r="B144" s="13"/>
       <c r="C144" s="12"/>
       <c r="D144" s="13"/>
       <c r="E144" s="13"/>
     </row>
-    <row r="145" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="145" customHeight="1" ht="15.75">
       <c r="A145" s="12"/>
       <c r="B145" s="13"/>
       <c r="C145" s="12"/>
       <c r="D145" s="13"/>
       <c r="E145" s="13"/>
     </row>
-    <row r="146" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="146" customHeight="1" ht="15.75">
       <c r="A146" s="12"/>
       <c r="B146" s="13"/>
       <c r="C146" s="12"/>
       <c r="D146" s="13"/>
       <c r="E146" s="13"/>
     </row>
-    <row r="147" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="147" customHeight="1" ht="15.75">
       <c r="A147" s="12"/>
       <c r="B147" s="13"/>
       <c r="C147" s="12"/>
       <c r="D147" s="13"/>
       <c r="E147" s="13"/>
     </row>
-    <row r="148" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="148" customHeight="1" ht="15.75">
       <c r="A148" s="12"/>
       <c r="B148" s="13"/>
       <c r="C148" s="12"/>
       <c r="D148" s="13"/>
       <c r="E148" s="13"/>
     </row>
-    <row r="149" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="149" customHeight="1" ht="15.75">
       <c r="A149" s="12"/>
       <c r="B149" s="13"/>
       <c r="C149" s="12"/>
       <c r="D149" s="13"/>
       <c r="E149" s="13"/>
     </row>
-    <row r="150" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="150" customHeight="1" ht="15.75">
       <c r="A150" s="12"/>
       <c r="B150" s="13"/>
       <c r="C150" s="12"/>
       <c r="D150" s="13"/>
       <c r="E150" s="13"/>
     </row>
-    <row r="151" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="151" customHeight="1" ht="15.75">
       <c r="A151" s="12"/>
       <c r="B151" s="13"/>
       <c r="C151" s="12"/>
       <c r="D151" s="13"/>
       <c r="E151" s="13"/>
     </row>
-    <row r="152" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="152" customHeight="1" ht="15.75">
       <c r="A152" s="12"/>
       <c r="B152" s="13"/>
       <c r="C152" s="12"/>
       <c r="D152" s="13"/>
       <c r="E152" s="13"/>
     </row>
-    <row r="153" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="153" customHeight="1" ht="15.75">
       <c r="A153" s="12"/>
       <c r="B153" s="13"/>
       <c r="C153" s="12"/>
       <c r="D153" s="13"/>
       <c r="E153" s="13"/>
     </row>
-    <row r="154" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="154" customHeight="1" ht="15.75">
       <c r="A154" s="12"/>
       <c r="B154" s="13"/>
       <c r="C154" s="12"/>
       <c r="D154" s="13"/>
       <c r="E154" s="13"/>
     </row>
-    <row r="155" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="155" customHeight="1" ht="15.75">
       <c r="A155" s="12"/>
       <c r="B155" s="13"/>
       <c r="C155" s="12"/>
       <c r="D155" s="13"/>
       <c r="E155" s="13"/>
     </row>
-    <row r="156" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="156" customHeight="1" ht="15.75">
       <c r="A156" s="12"/>
       <c r="B156" s="13"/>
       <c r="C156" s="12"/>
       <c r="D156" s="13"/>
       <c r="E156" s="13"/>
     </row>
-    <row r="157" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="157" customHeight="1" ht="15.75">
       <c r="A157" s="12"/>
       <c r="B157" s="13"/>
       <c r="C157" s="12"/>
       <c r="D157" s="13"/>
       <c r="E157" s="13"/>
     </row>
-    <row r="158" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="158" customHeight="1" ht="15.75">
       <c r="A158" s="12"/>
       <c r="B158" s="13"/>
       <c r="C158" s="12"/>
       <c r="D158" s="13"/>
       <c r="E158" s="13"/>
     </row>
-    <row r="159" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="159" customHeight="1" ht="15.75">
       <c r="A159" s="12"/>
       <c r="B159" s="13"/>
       <c r="C159" s="12"/>
       <c r="D159" s="13"/>
       <c r="E159" s="13"/>
     </row>
-    <row r="160" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="160" customHeight="1" ht="15.75">
       <c r="A160" s="12"/>
       <c r="B160" s="13"/>
       <c r="C160" s="12"/>
       <c r="D160" s="13"/>
       <c r="E160" s="13"/>
     </row>
-    <row r="161" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="161" customHeight="1" ht="15.75">
       <c r="A161" s="12"/>
       <c r="B161" s="13"/>
       <c r="C161" s="12"/>
       <c r="D161" s="13"/>
       <c r="E161" s="13"/>
     </row>
-    <row r="162" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="162" customHeight="1" ht="15.75">
       <c r="A162" s="12"/>
       <c r="B162" s="13"/>
       <c r="C162" s="12"/>
       <c r="D162" s="13"/>
       <c r="E162" s="13"/>
     </row>
-    <row r="163" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="163" customHeight="1" ht="15.75">
       <c r="A163" s="12"/>
       <c r="B163" s="13"/>
       <c r="C163" s="12"/>
       <c r="D163" s="13"/>
       <c r="E163" s="13"/>
     </row>
-    <row r="164" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="164" customHeight="1" ht="15.75">
       <c r="A164" s="12"/>
       <c r="B164" s="13"/>
       <c r="C164" s="12"/>
       <c r="D164" s="13"/>
       <c r="E164" s="13"/>
     </row>
-    <row r="165" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="165" customHeight="1" ht="15.75">
       <c r="A165" s="12"/>
       <c r="B165" s="13"/>
       <c r="C165" s="12"/>
       <c r="D165" s="13"/>
       <c r="E165" s="13"/>
     </row>
-    <row r="166" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="166" customHeight="1" ht="15.75">
       <c r="A166" s="12"/>
       <c r="B166" s="13"/>
       <c r="C166" s="12"/>
       <c r="D166" s="13"/>
       <c r="E166" s="13"/>
     </row>
-    <row r="167" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="167" customHeight="1" ht="15.75">
       <c r="A167" s="12"/>
       <c r="B167" s="13"/>
       <c r="C167" s="12"/>
       <c r="D167" s="13"/>
       <c r="E167" s="13"/>
     </row>
-    <row r="168" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="168" customHeight="1" ht="15.75">
       <c r="A168" s="12"/>
       <c r="B168" s="13"/>
       <c r="C168" s="12"/>
       <c r="D168" s="13"/>
       <c r="E168" s="13"/>
     </row>
-    <row r="169" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="169" customHeight="1" ht="15.75">
       <c r="A169" s="12"/>
       <c r="B169" s="13"/>
       <c r="C169" s="12"/>
       <c r="D169" s="13"/>
       <c r="E169" s="13"/>
     </row>
-    <row r="170" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="170" customHeight="1" ht="15.75">
       <c r="A170" s="12"/>
       <c r="B170" s="13"/>
       <c r="C170" s="12"/>
       <c r="D170" s="13"/>
       <c r="E170" s="13"/>
     </row>
-    <row r="171" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="171" customHeight="1" ht="15.75">
       <c r="A171" s="12"/>
       <c r="B171" s="13"/>
       <c r="C171" s="12"/>
       <c r="D171" s="13"/>
       <c r="E171" s="13"/>
     </row>
-    <row r="172" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="172" customHeight="1" ht="15.75">
       <c r="A172" s="12"/>
       <c r="B172" s="13"/>
       <c r="C172" s="12"/>
       <c r="D172" s="13"/>
       <c r="E172" s="13"/>
     </row>
-    <row r="173" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="173" customHeight="1" ht="15.75">
       <c r="A173" s="12"/>
       <c r="B173" s="13"/>
       <c r="C173" s="12"/>
       <c r="D173" s="13"/>
       <c r="E173" s="13"/>
     </row>
-    <row r="174" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="174" customHeight="1" ht="15.75">
       <c r="A174" s="12"/>
       <c r="B174" s="13"/>
       <c r="C174" s="12"/>
       <c r="D174" s="13"/>
       <c r="E174" s="13"/>
     </row>
-    <row r="175" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="175" customHeight="1" ht="15.75">
       <c r="A175" s="12"/>
       <c r="B175" s="13"/>
       <c r="C175" s="12"/>
       <c r="D175" s="13"/>
       <c r="E175" s="13"/>
     </row>
-    <row r="176" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="176" customHeight="1" ht="15.75">
       <c r="A176" s="12"/>
       <c r="B176" s="13"/>
       <c r="C176" s="12"/>
       <c r="D176" s="13"/>
       <c r="E176" s="13"/>
     </row>
-    <row r="177" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="177" customHeight="1" ht="15.75">
       <c r="A177" s="12"/>
       <c r="B177" s="13"/>
       <c r="C177" s="12"/>
       <c r="D177" s="13"/>
       <c r="E177" s="13"/>
     </row>
-    <row r="178" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="178" customHeight="1" ht="15.75">
       <c r="A178" s="12"/>
       <c r="B178" s="13"/>
       <c r="C178" s="12"/>
       <c r="D178" s="13"/>
       <c r="E178" s="13"/>
     </row>
-    <row r="179" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="179" customHeight="1" ht="15.75">
       <c r="A179" s="12"/>
       <c r="B179" s="13"/>
       <c r="C179" s="12"/>
       <c r="D179" s="13"/>
       <c r="E179" s="13"/>
     </row>
-    <row r="180" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="180" customHeight="1" ht="15.75">
       <c r="A180" s="12"/>
       <c r="B180" s="13"/>
       <c r="C180" s="12"/>
       <c r="D180" s="13"/>
       <c r="E180" s="13"/>
     </row>
-    <row r="181" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="181" customHeight="1" ht="15.75">
       <c r="A181" s="12"/>
       <c r="B181" s="13"/>
       <c r="C181" s="12"/>
       <c r="D181" s="13"/>
       <c r="E181" s="13"/>
     </row>
-    <row r="182" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="182" customHeight="1" ht="15.75">
       <c r="A182" s="12"/>
       <c r="B182" s="13"/>
       <c r="C182" s="12"/>
       <c r="D182" s="13"/>
       <c r="E182" s="13"/>
     </row>
-    <row r="183" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="183" customHeight="1" ht="15.75">
       <c r="A183" s="12"/>
       <c r="B183" s="13"/>
       <c r="C183" s="12"/>
       <c r="D183" s="13"/>
       <c r="E183" s="13"/>
     </row>
-    <row r="184" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="184" customHeight="1" ht="15.75">
       <c r="A184" s="12"/>
       <c r="B184" s="13"/>
       <c r="C184" s="12"/>
       <c r="D184" s="13"/>
       <c r="E184" s="13"/>
     </row>
-    <row r="185" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="185" customHeight="1" ht="15.75">
       <c r="A185" s="12"/>
       <c r="B185" s="13"/>
       <c r="C185" s="12"/>
       <c r="D185" s="13"/>
       <c r="E185" s="13"/>
     </row>
-    <row r="186" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="186" customHeight="1" ht="15.75">
       <c r="A186" s="12"/>
       <c r="B186" s="13"/>
       <c r="C186" s="12"/>
       <c r="D186" s="13"/>
       <c r="E186" s="13"/>
     </row>
-    <row r="187" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="187" customHeight="1" ht="15.75">
       <c r="A187" s="12"/>
       <c r="B187" s="13"/>
       <c r="C187" s="12"/>
       <c r="D187" s="13"/>
       <c r="E187" s="13"/>
     </row>
-    <row r="188" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="188" customHeight="1" ht="15.75">
       <c r="A188" s="12"/>
       <c r="B188" s="13"/>
       <c r="C188" s="12"/>
       <c r="D188" s="13"/>
       <c r="E188" s="13"/>
     </row>
-    <row r="189" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="189" customHeight="1" ht="15.75">
       <c r="A189" s="12"/>
       <c r="B189" s="13"/>
       <c r="C189" s="12"/>
       <c r="D189" s="13"/>
       <c r="E189" s="13"/>
     </row>
-    <row r="190" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="190" customHeight="1" ht="15.75">
       <c r="A190" s="12"/>
       <c r="B190" s="13"/>
       <c r="C190" s="12"/>
       <c r="D190" s="13"/>
       <c r="E190" s="13"/>
     </row>
-    <row r="191" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="191" customHeight="1" ht="15.75">
       <c r="A191" s="12"/>
       <c r="B191" s="13"/>
       <c r="C191" s="12"/>
       <c r="D191" s="13"/>
       <c r="E191" s="13"/>
     </row>
-    <row r="192" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="192" customHeight="1" ht="15.75">
       <c r="A192" s="12"/>
       <c r="B192" s="13"/>
       <c r="C192" s="12"/>
       <c r="D192" s="13"/>
       <c r="E192" s="13"/>
     </row>
-    <row r="193" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="193" customHeight="1" ht="15.75">
       <c r="A193" s="12"/>
       <c r="B193" s="13"/>
       <c r="C193" s="12"/>
       <c r="D193" s="13"/>
       <c r="E193" s="13"/>
     </row>
-    <row r="194" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="194" customHeight="1" ht="15.75">
       <c r="A194" s="12"/>
       <c r="B194" s="13"/>
       <c r="C194" s="12"/>
       <c r="D194" s="13"/>
       <c r="E194" s="13"/>
     </row>
-    <row r="195" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="195" customHeight="1" ht="15.75">
       <c r="A195" s="12"/>
       <c r="B195" s="13"/>
       <c r="C195" s="12"/>
       <c r="D195" s="13"/>
       <c r="E195" s="13"/>
     </row>
-    <row r="196" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="196" customHeight="1" ht="15.75">
       <c r="A196" s="12"/>
       <c r="B196" s="13"/>
       <c r="C196" s="12"/>
       <c r="D196" s="13"/>
       <c r="E196" s="13"/>
     </row>
-    <row r="197" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="197" customHeight="1" ht="15.75">
       <c r="A197" s="12"/>
       <c r="B197" s="13"/>
       <c r="C197" s="12"/>
       <c r="D197" s="13"/>
       <c r="E197" s="13"/>
     </row>
-    <row r="198" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="198" customHeight="1" ht="15.75">
       <c r="A198" s="12"/>
       <c r="B198" s="13"/>
       <c r="C198" s="12"/>
       <c r="D198" s="13"/>
       <c r="E198" s="13"/>
     </row>
-    <row r="199" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="199" customHeight="1" ht="15.75">
       <c r="A199" s="12"/>
       <c r="B199" s="13"/>
       <c r="C199" s="12"/>
       <c r="D199" s="13"/>
       <c r="E199" s="13"/>
     </row>
-    <row r="200" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="200" customHeight="1" ht="15.75">
       <c r="A200" s="12"/>
       <c r="B200" s="13"/>
       <c r="C200" s="12"/>
       <c r="D200" s="13"/>
       <c r="E200" s="13"/>
     </row>
-    <row r="201" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="201" customHeight="1" ht="15.75">
       <c r="A201" s="12"/>
       <c r="B201" s="13"/>
       <c r="C201" s="12"/>
       <c r="D201" s="13"/>
       <c r="E201" s="13"/>
     </row>
-    <row r="202" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="202" customHeight="1" ht="15.75">
       <c r="A202" s="12"/>
       <c r="B202" s="13"/>
       <c r="C202" s="12"/>
       <c r="D202" s="13"/>
       <c r="E202" s="13"/>
     </row>
-    <row r="203" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="203" customHeight="1" ht="15.75">
       <c r="A203" s="12"/>
       <c r="B203" s="13"/>
       <c r="C203" s="12"/>
       <c r="D203" s="13"/>
       <c r="E203" s="13"/>
     </row>
-    <row r="204" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="204" customHeight="1" ht="15.75">
       <c r="A204" s="12"/>
       <c r="B204" s="13"/>
       <c r="C204" s="12"/>
       <c r="D204" s="13"/>
       <c r="E204" s="13"/>
     </row>
-    <row r="205" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="205" customHeight="1" ht="15.75">
       <c r="A205" s="12"/>
       <c r="B205" s="13"/>
       <c r="C205" s="12"/>
       <c r="D205" s="13"/>
       <c r="E205" s="13"/>
     </row>
-    <row r="206" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="206" customHeight="1" ht="15.75">
       <c r="A206" s="12"/>
       <c r="B206" s="13"/>
       <c r="C206" s="12"/>
       <c r="D206" s="13"/>
       <c r="E206" s="13"/>
     </row>
-    <row r="207" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="207" customHeight="1" ht="15.75">
       <c r="A207" s="12"/>
       <c r="B207" s="13"/>
       <c r="C207" s="12"/>
       <c r="D207" s="13"/>
       <c r="E207" s="13"/>
     </row>
-    <row r="208" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="208" customHeight="1" ht="15.75">
       <c r="A208" s="12"/>
       <c r="B208" s="13"/>
       <c r="C208" s="12"/>
       <c r="D208" s="13"/>
       <c r="E208" s="13"/>
     </row>
-    <row r="209" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="209" customHeight="1" ht="15.75">
       <c r="A209" s="12"/>
       <c r="B209" s="13"/>
       <c r="C209" s="12"/>
       <c r="D209" s="13"/>
       <c r="E209" s="13"/>
     </row>
-    <row r="210" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="210" customHeight="1" ht="15.75">
       <c r="A210" s="12"/>
       <c r="B210" s="13"/>
       <c r="C210" s="12"/>
       <c r="D210" s="13"/>
       <c r="E210" s="13"/>
     </row>
-    <row r="211" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="211" customHeight="1" ht="15.75">
       <c r="A211" s="12"/>
       <c r="B211" s="13"/>
       <c r="C211" s="12"/>
       <c r="D211" s="13"/>
       <c r="E211" s="13"/>
     </row>
-    <row r="212" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="212" customHeight="1" ht="15.75">
       <c r="A212" s="12"/>
       <c r="B212" s="13"/>
       <c r="C212" s="12"/>
       <c r="D212" s="13"/>
       <c r="E212" s="13"/>
     </row>
-    <row r="213" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="213" customHeight="1" ht="15.75">
       <c r="A213" s="12"/>
       <c r="B213" s="13"/>
       <c r="C213" s="12"/>
       <c r="D213" s="13"/>
       <c r="E213" s="13"/>
     </row>
-    <row r="214" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="214" customHeight="1" ht="15.75">
       <c r="A214" s="12"/>
       <c r="B214" s="13"/>
       <c r="C214" s="12"/>
       <c r="D214" s="13"/>
       <c r="E214" s="13"/>
     </row>
-    <row r="215" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="215" customHeight="1" ht="15.75">
       <c r="A215" s="12"/>
       <c r="B215" s="13"/>
       <c r="C215" s="12"/>
       <c r="D215" s="13"/>
       <c r="E215" s="13"/>
     </row>
-    <row r="216" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="216" customHeight="1" ht="15.75">
       <c r="A216" s="12"/>
       <c r="B216" s="13"/>
       <c r="C216" s="12"/>
       <c r="D216" s="13"/>
       <c r="E216" s="13"/>
     </row>
-    <row r="217" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="217" customHeight="1" ht="15.75">
       <c r="A217" s="12"/>
       <c r="B217" s="13"/>
       <c r="C217" s="12"/>
       <c r="D217" s="13"/>
       <c r="E217" s="13"/>
     </row>
-    <row r="218" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="218" customHeight="1" ht="15.75">
       <c r="A218" s="12"/>
       <c r="B218" s="13"/>
       <c r="C218" s="12"/>
       <c r="D218" s="13"/>
       <c r="E218" s="13"/>
     </row>
-    <row r="219" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="219" customHeight="1" ht="15.75">
       <c r="A219" s="12"/>
       <c r="B219" s="13"/>
       <c r="C219" s="12"/>
       <c r="D219" s="13"/>
       <c r="E219" s="13"/>
     </row>
-    <row r="220" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="220" customHeight="1" ht="15.75">
       <c r="A220" s="12"/>
       <c r="B220" s="13"/>
       <c r="C220" s="12"/>
       <c r="D220" s="13"/>
       <c r="E220" s="13"/>
     </row>
-    <row r="221" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="221" customHeight="1" ht="15.75">
       <c r="A221" s="12"/>
       <c r="B221" s="13"/>
       <c r="C221" s="12"/>
       <c r="D221" s="13"/>
       <c r="E221" s="13"/>
     </row>
-    <row r="222" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="222" customHeight="1" ht="15.75">
       <c r="A222" s="12"/>
       <c r="B222" s="13"/>
       <c r="C222" s="12"/>
       <c r="D222" s="13"/>
       <c r="E222" s="13"/>
     </row>
-    <row r="223" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="223" customHeight="1" ht="15.75">
       <c r="A223" s="12"/>
       <c r="B223" s="13"/>
       <c r="C223" s="12"/>
       <c r="D223" s="13"/>
       <c r="E223" s="13"/>
     </row>
-    <row r="224" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="224" customHeight="1" ht="15.75">
       <c r="A224" s="12"/>
       <c r="B224" s="13"/>
       <c r="C224" s="12"/>
       <c r="D224" s="13"/>
       <c r="E224" s="13"/>
     </row>
-    <row r="225" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="225" customHeight="1" ht="15.75">
       <c r="A225" s="12"/>
       <c r="B225" s="13"/>
       <c r="C225" s="12"/>
       <c r="D225" s="13"/>
       <c r="E225" s="13"/>
     </row>
-    <row r="226" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="226" customHeight="1" ht="15.75">
       <c r="A226" s="12"/>
       <c r="B226" s="13"/>
       <c r="C226" s="12"/>
       <c r="D226" s="13"/>
       <c r="E226" s="13"/>
     </row>
-    <row r="227" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="227" customHeight="1" ht="15.75">
       <c r="A227" s="12"/>
       <c r="B227" s="13"/>
       <c r="C227" s="12"/>
       <c r="D227" s="13"/>
       <c r="E227" s="13"/>
     </row>
-    <row r="228" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="228" customHeight="1" ht="15.75">
       <c r="A228" s="12"/>
       <c r="B228" s="13"/>
       <c r="C228" s="12"/>
       <c r="D228" s="13"/>
       <c r="E228" s="13"/>
     </row>
-    <row r="229" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="229" customHeight="1" ht="15.75">
       <c r="A229" s="12"/>
       <c r="B229" s="13"/>
       <c r="C229" s="12"/>
       <c r="D229" s="13"/>
       <c r="E229" s="13"/>
     </row>
-    <row r="230" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="230" customHeight="1" ht="15.75">
       <c r="A230" s="12"/>
       <c r="B230" s="13"/>
       <c r="C230" s="12"/>
       <c r="D230" s="13"/>
       <c r="E230" s="13"/>
     </row>
-    <row r="231" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="231" customHeight="1" ht="15.75">
       <c r="A231" s="12"/>
       <c r="B231" s="13"/>
       <c r="C231" s="12"/>
       <c r="D231" s="13"/>
       <c r="E231" s="13"/>
     </row>
-    <row r="232" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="232" customHeight="1" ht="15.75">
       <c r="A232" s="12"/>
       <c r="B232" s="13"/>
       <c r="C232" s="12"/>
       <c r="D232" s="13"/>
       <c r="E232" s="13"/>
     </row>
-    <row r="233" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="233" customHeight="1" ht="15.75">
       <c r="A233" s="12"/>
       <c r="B233" s="13"/>
       <c r="C233" s="12"/>
       <c r="D233" s="13"/>
       <c r="E233" s="13"/>
     </row>
-    <row r="234" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="234" customHeight="1" ht="15.75">
       <c r="A234" s="12"/>
       <c r="B234" s="13"/>
       <c r="C234" s="12"/>
       <c r="D234" s="13"/>
       <c r="E234" s="13"/>
     </row>
-    <row r="235" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="235" customHeight="1" ht="15.75">
       <c r="A235" s="12"/>
       <c r="B235" s="13"/>
       <c r="C235" s="12"/>
       <c r="D235" s="13"/>
       <c r="E235" s="13"/>
     </row>
-    <row r="236" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="236" customHeight="1" ht="15.75">
       <c r="A236" s="12"/>
       <c r="B236" s="13"/>
       <c r="C236" s="12"/>
       <c r="D236" s="13"/>
       <c r="E236" s="13"/>
     </row>
-    <row r="237" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="237" customHeight="1" ht="15.75">
       <c r="A237" s="12"/>
       <c r="B237" s="13"/>
       <c r="C237" s="12"/>
       <c r="D237" s="13"/>
       <c r="E237" s="13"/>
     </row>
-    <row r="238" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="238" customHeight="1" ht="15.75">
       <c r="A238" s="12"/>
       <c r="B238" s="13"/>
       <c r="C238" s="12"/>
       <c r="D238" s="13"/>
       <c r="E238" s="13"/>
     </row>
-    <row r="239" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="239" customHeight="1" ht="15.75">
       <c r="A239" s="12"/>
       <c r="B239" s="13"/>
       <c r="C239" s="12"/>
       <c r="D239" s="13"/>
       <c r="E239" s="13"/>
     </row>
-    <row r="240" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="240" customHeight="1" ht="15.75">
       <c r="A240" s="12"/>
       <c r="B240" s="13"/>
       <c r="C240" s="12"/>
       <c r="D240" s="13"/>
       <c r="E240" s="13"/>
     </row>
-    <row r="241" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="241" customHeight="1" ht="15.75">
       <c r="A241" s="12"/>
       <c r="B241" s="13"/>
       <c r="C241" s="12"/>
       <c r="D241" s="13"/>
       <c r="E241" s="13"/>
     </row>
-    <row r="242" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="242" customHeight="1" ht="15.75">
       <c r="A242" s="12"/>
       <c r="B242" s="13"/>
       <c r="C242" s="12"/>
       <c r="D242" s="13"/>
       <c r="E242" s="13"/>
     </row>
-    <row r="243" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="243" customHeight="1" ht="15.75">
       <c r="A243" s="12"/>
       <c r="B243" s="13"/>
       <c r="C243" s="12"/>
       <c r="D243" s="13"/>
       <c r="E243" s="13"/>
     </row>
-    <row r="244" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="244" customHeight="1" ht="15.75">
       <c r="A244" s="12"/>
       <c r="B244" s="13"/>
       <c r="C244" s="12"/>
       <c r="D244" s="13"/>
       <c r="E244" s="13"/>
     </row>
-    <row r="245" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="245" customHeight="1" ht="15.75">
       <c r="A245" s="12"/>
       <c r="B245" s="13"/>
       <c r="C245" s="12"/>
       <c r="D245" s="13"/>
       <c r="E245" s="13"/>
     </row>
-    <row r="246" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="246" customHeight="1" ht="15.75">
       <c r="A246" s="12"/>
       <c r="B246" s="13"/>
       <c r="C246" s="12"/>
       <c r="D246" s="13"/>
       <c r="E246" s="13"/>
     </row>
-    <row r="247" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="247" customHeight="1" ht="15.75">
       <c r="A247" s="12"/>
       <c r="B247" s="13"/>
       <c r="C247" s="12"/>
       <c r="D247" s="13"/>
       <c r="E247" s="13"/>
     </row>
-    <row r="248" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="248" customHeight="1" ht="15.75">
       <c r="A248" s="12"/>
       <c r="B248" s="13"/>
       <c r="C248" s="12"/>
       <c r="D248" s="13"/>
       <c r="E248" s="13"/>
     </row>
-    <row r="249" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="249" customHeight="1" ht="15.75">
       <c r="A249" s="12"/>
       <c r="B249" s="13"/>
       <c r="C249" s="12"/>
       <c r="D249" s="13"/>
       <c r="E249" s="13"/>
     </row>
-    <row r="250" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="250" customHeight="1" ht="15.75">
       <c r="A250" s="12"/>
       <c r="B250" s="13"/>
       <c r="C250" s="12"/>
       <c r="D250" s="13"/>
       <c r="E250" s="13"/>
     </row>
-    <row r="251" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="251" customHeight="1" ht="15.75">
       <c r="A251" s="12"/>
       <c r="B251" s="13"/>
       <c r="C251" s="12"/>
       <c r="D251" s="13"/>
       <c r="E251" s="13"/>
     </row>
-    <row r="252" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="252" customHeight="1" ht="15.75">
       <c r="A252" s="12"/>
       <c r="B252" s="13"/>
       <c r="C252" s="12"/>
       <c r="D252" s="13"/>
       <c r="E252" s="13"/>
     </row>
-    <row r="253" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="253" customHeight="1" ht="15.75">
       <c r="A253" s="12"/>
       <c r="B253" s="13"/>
       <c r="C253" s="12"/>
       <c r="D253" s="13"/>
       <c r="E253" s="13"/>
     </row>
-    <row r="254" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="254" customHeight="1" ht="15.75">
       <c r="A254" s="12"/>
       <c r="B254" s="13"/>
       <c r="C254" s="12"/>
       <c r="D254" s="13"/>
       <c r="E254" s="13"/>
     </row>
-    <row r="255" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="255" customHeight="1" ht="15.75">
       <c r="A255" s="12"/>
       <c r="B255" s="13"/>
       <c r="C255" s="12"/>
       <c r="D255" s="13"/>
       <c r="E255" s="13"/>
     </row>
-    <row r="256" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="256" customHeight="1" ht="15.75">
       <c r="A256" s="12"/>
       <c r="B256" s="13"/>
       <c r="C256" s="12"/>
       <c r="D256" s="13"/>
       <c r="E256" s="13"/>
     </row>
-    <row r="257" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="257" customHeight="1" ht="15.75">
       <c r="A257" s="12"/>
       <c r="B257" s="13"/>
       <c r="C257" s="12"/>
       <c r="D257" s="13"/>
       <c r="E257" s="13"/>
     </row>
-    <row r="258" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="258" customHeight="1" ht="15.75">
       <c r="A258" s="12"/>
       <c r="B258" s="13"/>
       <c r="C258" s="12"/>
       <c r="D258" s="13"/>
       <c r="E258" s="13"/>
     </row>
-    <row r="259" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="259" customHeight="1" ht="15.75">
       <c r="A259" s="12"/>
       <c r="B259" s="13"/>
       <c r="C259" s="12"/>
       <c r="D259" s="13"/>
       <c r="E259" s="13"/>
     </row>
-    <row r="260" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="260" customHeight="1" ht="15.75">
       <c r="A260" s="12"/>
       <c r="B260" s="13"/>
       <c r="C260" s="12"/>
@@ -2904,13 +2899,6 @@
       <c r="E260" s="13"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="D21" r:id="rId1"/>
-    <hyperlink ref="D22" r:id="rId2"/>
-    <hyperlink ref="D23" r:id="rId3"/>
-    <hyperlink ref="D24" r:id="rId4"/>
-    <hyperlink ref="D25" r:id="rId5"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Se agrega el 26 Alumno al archivo
</commit_message>
<xml_diff>
--- a/Lista de Alumnos.xlsx
+++ b/Lista de Alumnos.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505"/>
   </bookViews>
   <sheets>
-    <sheet r:id="rId1" sheetId="1" name="Electronica Microcontrolada"/>
+    <sheet name="Electronica Microcontrolada" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="82">
   <si>
     <t>#</t>
   </si>
@@ -251,14 +251,22 @@
   </si>
   <si>
     <t>CelesteSuarezz</t>
+  </si>
+  <si>
+    <t>Mauro Yamil Martinez</t>
+  </si>
+  <si>
+    <t>mauromartinez10.mtz@gmail.com</t>
+  </si>
+  <si>
+    <t>Mauro-Martinez</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
-  <fonts count="8" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -295,7 +303,7 @@
     <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF0563c1"/>
+      <color rgb="FF0563C1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -311,6 +319,14 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -389,65 +405,70 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+  <cellXfs count="17">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="4" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="4" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="4" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="4" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="4" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="4" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="4" applyBorder="1" fontId="6" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="5" applyBorder="1" fontId="7" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="7" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="5" applyBorder="1" fontId="7" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle xfId="0" builtinId="0" name="Normal"/>
+  <cellStyles count="2">
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -458,10 +479,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -499,71 +520,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Times New Roman" script="Arab"/>
-        <a:font typeface="Times New Roman" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="MoolBoran" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Times New Roman" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Arial" script="Arab"/>
-        <a:font typeface="Arial" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="DaunPenh" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Arial" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -591,7 +612,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -614,11 +635,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -627,13 +648,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -643,7 +664,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -652,7 +673,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -661,7 +682,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -669,10 +690,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot rev="0" lon="0" lat="0"/>
+              <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
-              <a:rot rev="1200000" lon="0" lat="0"/>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -743,18 +764,20 @@
   </sheetPr>
   <dimension ref="A1:E260"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="14" width="6.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="15" width="37.14785714285715" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="14" width="10.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="15" width="31.005" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="15" width="29.005" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="6.85546875" style="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.140625" style="15" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" style="14" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31" style="15" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29" style="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="27">
+    <row r="1" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -771,7 +794,7 @@
         <v>4</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
+    <row r="2" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -788,7 +811,7 @@
         <v>7</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
+    <row r="3" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>2</v>
       </c>
@@ -803,7 +826,7 @@
       </c>
       <c r="E3" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
+    <row r="4" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>3</v>
       </c>
@@ -820,7 +843,7 @@
         <v>12</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
+    <row r="5" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>4</v>
       </c>
@@ -837,7 +860,7 @@
         <v>15</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
+    <row r="6" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>5</v>
       </c>
@@ -854,7 +877,7 @@
         <v>18</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
+    <row r="7" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>6</v>
       </c>
@@ -871,7 +894,7 @@
         <v>21</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
+    <row r="8" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>7</v>
       </c>
@@ -888,7 +911,7 @@
         <v>24</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
+    <row r="9" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>8</v>
       </c>
@@ -905,7 +928,7 @@
         <v>27</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
+    <row r="10" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>9</v>
       </c>
@@ -920,7 +943,7 @@
         <v>30</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
+    <row r="11" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <v>10</v>
       </c>
@@ -937,7 +960,7 @@
         <v>33</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
+    <row r="12" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>11</v>
       </c>
@@ -954,7 +977,7 @@
         <v>36</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
+    <row r="13" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
         <v>12</v>
       </c>
@@ -971,7 +994,7 @@
         <v>39</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
+    <row r="14" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
         <v>13</v>
       </c>
@@ -988,7 +1011,7 @@
         <v>42</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
+    <row r="15" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
         <v>14</v>
       </c>
@@ -1005,7 +1028,7 @@
         <v>45</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
+    <row r="16" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
         <v>15</v>
       </c>
@@ -1022,7 +1045,7 @@
         <v>48</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
+    <row r="17" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
         <v>16</v>
       </c>
@@ -1039,7 +1062,7 @@
         <v>51</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
+    <row r="18" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <v>17</v>
       </c>
@@ -1056,7 +1079,7 @@
         <v>54</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
+    <row r="19" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
         <v>18</v>
       </c>
@@ -1073,7 +1096,7 @@
         <v>57</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5">
+    <row r="20" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
         <v>19</v>
       </c>
@@ -1090,7 +1113,7 @@
         <v>60</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5">
+    <row r="21" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="5">
         <v>20</v>
       </c>
@@ -1107,7 +1130,7 @@
         <v>63</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="25.5">
+    <row r="22" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="5">
         <v>21</v>
       </c>
@@ -1124,7 +1147,7 @@
         <v>66</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="25.5">
+    <row r="23" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="5">
         <v>22</v>
       </c>
@@ -1141,7 +1164,7 @@
         <v>69</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="25.5">
+    <row r="24" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="5">
         <v>23</v>
       </c>
@@ -1158,7 +1181,7 @@
         <v>72</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="25.5">
+    <row r="25" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="5">
         <v>24</v>
       </c>
@@ -1175,7 +1198,7 @@
         <v>75</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="25.5">
+    <row r="26" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="5">
         <v>25</v>
       </c>
@@ -1192,16 +1215,24 @@
         <v>78</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="25.5">
+    <row r="27" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="5">
         <v>26</v>
       </c>
-      <c r="B27" s="6"/>
-      <c r="C27" s="5"/>
-      <c r="D27" s="6"/>
-      <c r="E27" s="6"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="25.5">
+      <c r="B27" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="C27" s="5">
+        <v>2</v>
+      </c>
+      <c r="D27" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="E27" s="6" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="5">
         <v>27</v>
       </c>
@@ -1210,7 +1241,7 @@
       <c r="D28" s="6"/>
       <c r="E28" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="25.5">
+    <row r="29" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="5">
         <v>28</v>
       </c>
@@ -1219,7 +1250,7 @@
       <c r="D29" s="6"/>
       <c r="E29" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="25.5">
+    <row r="30" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="5">
         <v>29</v>
       </c>
@@ -1228,7 +1259,7 @@
       <c r="D30" s="6"/>
       <c r="E30" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="25.5">
+    <row r="31" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="5">
         <v>30</v>
       </c>
@@ -1237,7 +1268,7 @@
       <c r="D31" s="6"/>
       <c r="E31" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="25.5">
+    <row r="32" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="5">
         <v>31</v>
       </c>
@@ -1246,7 +1277,7 @@
       <c r="D32" s="6"/>
       <c r="E32" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="25.5">
+    <row r="33" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="5">
         <v>32</v>
       </c>
@@ -1255,7 +1286,7 @@
       <c r="D33" s="6"/>
       <c r="E33" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="25.5">
+    <row r="34" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="5">
         <v>33</v>
       </c>
@@ -1264,7 +1295,7 @@
       <c r="D34" s="6"/>
       <c r="E34" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="25.5">
+    <row r="35" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="5">
         <v>34</v>
       </c>
@@ -1273,7 +1304,7 @@
       <c r="D35" s="6"/>
       <c r="E35" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="25.5">
+    <row r="36" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="5">
         <v>35</v>
       </c>
@@ -1282,7 +1313,7 @@
       <c r="D36" s="6"/>
       <c r="E36" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="25.5">
+    <row r="37" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="5">
         <v>36</v>
       </c>
@@ -1291,7 +1322,7 @@
       <c r="D37" s="6"/>
       <c r="E37" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="25.5">
+    <row r="38" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="5">
         <v>37</v>
       </c>
@@ -1300,7 +1331,7 @@
       <c r="D38" s="6"/>
       <c r="E38" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="25.5">
+    <row r="39" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="5">
         <v>38</v>
       </c>
@@ -1309,7 +1340,7 @@
       <c r="D39" s="6"/>
       <c r="E39" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="25.5">
+    <row r="40" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="5">
         <v>39</v>
       </c>
@@ -1318,7 +1349,7 @@
       <c r="D40" s="6"/>
       <c r="E40" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="25.5">
+    <row r="41" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="5">
         <v>40</v>
       </c>
@@ -1327,7 +1358,7 @@
       <c r="D41" s="6"/>
       <c r="E41" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="25.5">
+    <row r="42" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="5">
         <v>41</v>
       </c>
@@ -1336,7 +1367,7 @@
       <c r="D42" s="6"/>
       <c r="E42" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="25.5">
+    <row r="43" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="5">
         <v>42</v>
       </c>
@@ -1345,7 +1376,7 @@
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="25.5">
+    <row r="44" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="5">
         <v>43</v>
       </c>
@@ -1354,7 +1385,7 @@
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="25.5">
+    <row r="45" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="5">
         <v>44</v>
       </c>
@@ -1363,7 +1394,7 @@
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="25.5">
+    <row r="46" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="5">
         <v>45</v>
       </c>
@@ -1372,7 +1403,7 @@
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="25.5">
+    <row r="47" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="5">
         <v>46</v>
       </c>
@@ -1381,7 +1412,7 @@
       <c r="D47" s="6"/>
       <c r="E47" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="25.5">
+    <row r="48" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="5">
         <v>47</v>
       </c>
@@ -1390,7 +1421,7 @@
       <c r="D48" s="6"/>
       <c r="E48" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="25.5">
+    <row r="49" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="5">
         <v>48</v>
       </c>
@@ -1399,7 +1430,7 @@
       <c r="D49" s="6"/>
       <c r="E49" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="25.5">
+    <row r="50" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="5">
         <v>49</v>
       </c>
@@ -1408,7 +1439,7 @@
       <c r="D50" s="6"/>
       <c r="E50" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="51" customHeight="1" ht="25.5">
+    <row r="51" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="5">
         <v>50</v>
       </c>
@@ -1417,7 +1448,7 @@
       <c r="D51" s="6"/>
       <c r="E51" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="52" customHeight="1" ht="25.5">
+    <row r="52" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="5">
         <v>51</v>
       </c>
@@ -1426,7 +1457,7 @@
       <c r="D52" s="6"/>
       <c r="E52" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="53" customHeight="1" ht="25.5">
+    <row r="53" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="5">
         <v>52</v>
       </c>
@@ -1435,7 +1466,7 @@
       <c r="D53" s="6"/>
       <c r="E53" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="54" customHeight="1" ht="25.5">
+    <row r="54" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="5">
         <v>53</v>
       </c>
@@ -1444,7 +1475,7 @@
       <c r="D54" s="6"/>
       <c r="E54" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="55" customHeight="1" ht="25.5">
+    <row r="55" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="5">
         <v>54</v>
       </c>
@@ -1453,7 +1484,7 @@
       <c r="D55" s="6"/>
       <c r="E55" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="56" customHeight="1" ht="25.5">
+    <row r="56" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="5">
         <v>55</v>
       </c>
@@ -1462,7 +1493,7 @@
       <c r="D56" s="6"/>
       <c r="E56" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="57" customHeight="1" ht="25.5">
+    <row r="57" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="5">
         <v>56</v>
       </c>
@@ -1471,7 +1502,7 @@
       <c r="D57" s="6"/>
       <c r="E57" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="58" customHeight="1" ht="25.5">
+    <row r="58" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="5">
         <v>57</v>
       </c>
@@ -1480,7 +1511,7 @@
       <c r="D58" s="6"/>
       <c r="E58" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="59" customHeight="1" ht="25.5">
+    <row r="59" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="5">
         <v>58</v>
       </c>
@@ -1489,7 +1520,7 @@
       <c r="D59" s="6"/>
       <c r="E59" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="60" customHeight="1" ht="25.5">
+    <row r="60" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="5">
         <v>59</v>
       </c>
@@ -1498,1400 +1529,1400 @@
       <c r="D60" s="6"/>
       <c r="E60" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="61" customHeight="1" ht="15.75">
+    <row r="61" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="12"/>
       <c r="B61" s="13"/>
       <c r="C61" s="12"/>
       <c r="D61" s="13"/>
       <c r="E61" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="62" customHeight="1" ht="15.75">
+    <row r="62" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="12"/>
       <c r="B62" s="13"/>
       <c r="C62" s="12"/>
       <c r="D62" s="13"/>
       <c r="E62" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="63" customHeight="1" ht="15.75">
+    <row r="63" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="12"/>
       <c r="B63" s="13"/>
       <c r="C63" s="12"/>
       <c r="D63" s="13"/>
       <c r="E63" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="64" customHeight="1" ht="15.75">
+    <row r="64" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="12"/>
       <c r="B64" s="13"/>
       <c r="C64" s="12"/>
       <c r="D64" s="13"/>
       <c r="E64" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="65" customHeight="1" ht="15.75">
+    <row r="65" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="12"/>
       <c r="B65" s="13"/>
       <c r="C65" s="12"/>
       <c r="D65" s="13"/>
       <c r="E65" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="66" customHeight="1" ht="15.75">
+    <row r="66" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="12"/>
       <c r="B66" s="13"/>
       <c r="C66" s="12"/>
       <c r="D66" s="13"/>
       <c r="E66" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="67" customHeight="1" ht="15.75">
+    <row r="67" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="12"/>
       <c r="B67" s="13"/>
       <c r="C67" s="12"/>
       <c r="D67" s="13"/>
       <c r="E67" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="68" customHeight="1" ht="15.75">
+    <row r="68" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="12"/>
       <c r="B68" s="13"/>
       <c r="C68" s="12"/>
       <c r="D68" s="13"/>
       <c r="E68" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="69" customHeight="1" ht="15.75">
+    <row r="69" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="12"/>
       <c r="B69" s="13"/>
       <c r="C69" s="12"/>
       <c r="D69" s="13"/>
       <c r="E69" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="70" customHeight="1" ht="15.75">
+    <row r="70" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="12"/>
       <c r="B70" s="13"/>
       <c r="C70" s="12"/>
       <c r="D70" s="13"/>
       <c r="E70" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="71" customHeight="1" ht="15.75">
+    <row r="71" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="12"/>
       <c r="B71" s="13"/>
       <c r="C71" s="12"/>
       <c r="D71" s="13"/>
       <c r="E71" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="72" customHeight="1" ht="15.75">
+    <row r="72" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="12"/>
       <c r="B72" s="13"/>
       <c r="C72" s="12"/>
       <c r="D72" s="13"/>
       <c r="E72" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="73" customHeight="1" ht="15.75">
+    <row r="73" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="12"/>
       <c r="B73" s="13"/>
       <c r="C73" s="12"/>
       <c r="D73" s="13"/>
       <c r="E73" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="74" customHeight="1" ht="15.75">
+    <row r="74" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="12"/>
       <c r="B74" s="13"/>
       <c r="C74" s="12"/>
       <c r="D74" s="13"/>
       <c r="E74" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="75" customHeight="1" ht="15.75">
+    <row r="75" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="12"/>
       <c r="B75" s="13"/>
       <c r="C75" s="12"/>
       <c r="D75" s="13"/>
       <c r="E75" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="76" customHeight="1" ht="15.75">
+    <row r="76" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="12"/>
       <c r="B76" s="13"/>
       <c r="C76" s="12"/>
       <c r="D76" s="13"/>
       <c r="E76" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="77" customHeight="1" ht="15.75">
+    <row r="77" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="12"/>
       <c r="B77" s="13"/>
       <c r="C77" s="12"/>
       <c r="D77" s="13"/>
       <c r="E77" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="78" customHeight="1" ht="15.75">
+    <row r="78" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="12"/>
       <c r="B78" s="13"/>
       <c r="C78" s="12"/>
       <c r="D78" s="13"/>
       <c r="E78" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="79" customHeight="1" ht="15.75">
+    <row r="79" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="12"/>
       <c r="B79" s="13"/>
       <c r="C79" s="12"/>
       <c r="D79" s="13"/>
       <c r="E79" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="80" customHeight="1" ht="15.75">
+    <row r="80" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="12"/>
       <c r="B80" s="13"/>
       <c r="C80" s="12"/>
       <c r="D80" s="13"/>
       <c r="E80" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="81" customHeight="1" ht="15.75">
+    <row r="81" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="12"/>
       <c r="B81" s="13"/>
       <c r="C81" s="12"/>
       <c r="D81" s="13"/>
       <c r="E81" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="82" customHeight="1" ht="15.75">
+    <row r="82" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="12"/>
       <c r="B82" s="13"/>
       <c r="C82" s="12"/>
       <c r="D82" s="13"/>
       <c r="E82" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="83" customHeight="1" ht="15.75">
+    <row r="83" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="12"/>
       <c r="B83" s="13"/>
       <c r="C83" s="12"/>
       <c r="D83" s="13"/>
       <c r="E83" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="84" customHeight="1" ht="15.75">
+    <row r="84" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="12"/>
       <c r="B84" s="13"/>
       <c r="C84" s="12"/>
       <c r="D84" s="13"/>
       <c r="E84" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="85" customHeight="1" ht="15.75">
+    <row r="85" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="12"/>
       <c r="B85" s="13"/>
       <c r="C85" s="12"/>
       <c r="D85" s="13"/>
       <c r="E85" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="86" customHeight="1" ht="15.75">
+    <row r="86" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="12"/>
       <c r="B86" s="13"/>
       <c r="C86" s="12"/>
       <c r="D86" s="13"/>
       <c r="E86" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="87" customHeight="1" ht="15.75">
+    <row r="87" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="12"/>
       <c r="B87" s="13"/>
       <c r="C87" s="12"/>
       <c r="D87" s="13"/>
       <c r="E87" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="88" customHeight="1" ht="15.75">
+    <row r="88" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="12"/>
       <c r="B88" s="13"/>
       <c r="C88" s="12"/>
       <c r="D88" s="13"/>
       <c r="E88" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="89" customHeight="1" ht="15.75">
+    <row r="89" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="12"/>
       <c r="B89" s="13"/>
       <c r="C89" s="12"/>
       <c r="D89" s="13"/>
       <c r="E89" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="90" customHeight="1" ht="15.75">
+    <row r="90" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="12"/>
       <c r="B90" s="13"/>
       <c r="C90" s="12"/>
       <c r="D90" s="13"/>
       <c r="E90" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="91" customHeight="1" ht="15.75">
+    <row r="91" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="12"/>
       <c r="B91" s="13"/>
       <c r="C91" s="12"/>
       <c r="D91" s="13"/>
       <c r="E91" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="92" customHeight="1" ht="15.75">
+    <row r="92" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="12"/>
       <c r="B92" s="13"/>
       <c r="C92" s="12"/>
       <c r="D92" s="13"/>
       <c r="E92" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="93" customHeight="1" ht="15.75">
+    <row r="93" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="12"/>
       <c r="B93" s="13"/>
       <c r="C93" s="12"/>
       <c r="D93" s="13"/>
       <c r="E93" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="94" customHeight="1" ht="15.75">
+    <row r="94" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="12"/>
       <c r="B94" s="13"/>
       <c r="C94" s="12"/>
       <c r="D94" s="13"/>
       <c r="E94" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="95" customHeight="1" ht="15.75">
+    <row r="95" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="12"/>
       <c r="B95" s="13"/>
       <c r="C95" s="12"/>
       <c r="D95" s="13"/>
       <c r="E95" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="96" customHeight="1" ht="15.75">
+    <row r="96" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="12"/>
       <c r="B96" s="13"/>
       <c r="C96" s="12"/>
       <c r="D96" s="13"/>
       <c r="E96" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="97" customHeight="1" ht="15.75">
+    <row r="97" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="12"/>
       <c r="B97" s="13"/>
       <c r="C97" s="12"/>
       <c r="D97" s="13"/>
       <c r="E97" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="98" customHeight="1" ht="15.75">
+    <row r="98" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="12"/>
       <c r="B98" s="13"/>
       <c r="C98" s="12"/>
       <c r="D98" s="13"/>
       <c r="E98" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="99" customHeight="1" ht="15.75">
+    <row r="99" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="12"/>
       <c r="B99" s="13"/>
       <c r="C99" s="12"/>
       <c r="D99" s="13"/>
       <c r="E99" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="100" customHeight="1" ht="15.75">
+    <row r="100" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="12"/>
       <c r="B100" s="13"/>
       <c r="C100" s="12"/>
       <c r="D100" s="13"/>
       <c r="E100" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="101" customHeight="1" ht="15.75">
+    <row r="101" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="12"/>
       <c r="B101" s="13"/>
       <c r="C101" s="12"/>
       <c r="D101" s="13"/>
       <c r="E101" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="102" customHeight="1" ht="15.75">
+    <row r="102" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="12"/>
       <c r="B102" s="13"/>
       <c r="C102" s="12"/>
       <c r="D102" s="13"/>
       <c r="E102" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="103" customHeight="1" ht="15.75">
+    <row r="103" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" s="12"/>
       <c r="B103" s="13"/>
       <c r="C103" s="12"/>
       <c r="D103" s="13"/>
       <c r="E103" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="104" customHeight="1" ht="15.75">
+    <row r="104" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="12"/>
       <c r="B104" s="13"/>
       <c r="C104" s="12"/>
       <c r="D104" s="13"/>
       <c r="E104" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="105" customHeight="1" ht="15.75">
+    <row r="105" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" s="12"/>
       <c r="B105" s="13"/>
       <c r="C105" s="12"/>
       <c r="D105" s="13"/>
       <c r="E105" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="106" customHeight="1" ht="15.75">
+    <row r="106" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="12"/>
       <c r="B106" s="13"/>
       <c r="C106" s="12"/>
       <c r="D106" s="13"/>
       <c r="E106" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="107" customHeight="1" ht="15.75">
+    <row r="107" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" s="12"/>
       <c r="B107" s="13"/>
       <c r="C107" s="12"/>
       <c r="D107" s="13"/>
       <c r="E107" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="108" customHeight="1" ht="15.75">
+    <row r="108" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" s="12"/>
       <c r="B108" s="13"/>
       <c r="C108" s="12"/>
       <c r="D108" s="13"/>
       <c r="E108" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="109" customHeight="1" ht="15.75">
+    <row r="109" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" s="12"/>
       <c r="B109" s="13"/>
       <c r="C109" s="12"/>
       <c r="D109" s="13"/>
       <c r="E109" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="110" customHeight="1" ht="15.75">
+    <row r="110" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" s="12"/>
       <c r="B110" s="13"/>
       <c r="C110" s="12"/>
       <c r="D110" s="13"/>
       <c r="E110" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="111" customHeight="1" ht="15.75">
+    <row r="111" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" s="12"/>
       <c r="B111" s="13"/>
       <c r="C111" s="12"/>
       <c r="D111" s="13"/>
       <c r="E111" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="112" customHeight="1" ht="15.75">
+    <row r="112" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" s="12"/>
       <c r="B112" s="13"/>
       <c r="C112" s="12"/>
       <c r="D112" s="13"/>
       <c r="E112" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="113" customHeight="1" ht="15.75">
+    <row r="113" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" s="12"/>
       <c r="B113" s="13"/>
       <c r="C113" s="12"/>
       <c r="D113" s="13"/>
       <c r="E113" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="114" customHeight="1" ht="15.75">
+    <row r="114" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A114" s="12"/>
       <c r="B114" s="13"/>
       <c r="C114" s="12"/>
       <c r="D114" s="13"/>
       <c r="E114" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="115" customHeight="1" ht="15.75">
+    <row r="115" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A115" s="12"/>
       <c r="B115" s="13"/>
       <c r="C115" s="12"/>
       <c r="D115" s="13"/>
       <c r="E115" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="116" customHeight="1" ht="15.75">
+    <row r="116" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A116" s="12"/>
       <c r="B116" s="13"/>
       <c r="C116" s="12"/>
       <c r="D116" s="13"/>
       <c r="E116" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="117" customHeight="1" ht="15.75">
+    <row r="117" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A117" s="12"/>
       <c r="B117" s="13"/>
       <c r="C117" s="12"/>
       <c r="D117" s="13"/>
       <c r="E117" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="118" customHeight="1" ht="15.75">
+    <row r="118" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A118" s="12"/>
       <c r="B118" s="13"/>
       <c r="C118" s="12"/>
       <c r="D118" s="13"/>
       <c r="E118" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="119" customHeight="1" ht="15.75">
+    <row r="119" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A119" s="12"/>
       <c r="B119" s="13"/>
       <c r="C119" s="12"/>
       <c r="D119" s="13"/>
       <c r="E119" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="120" customHeight="1" ht="15.75">
+    <row r="120" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A120" s="12"/>
       <c r="B120" s="13"/>
       <c r="C120" s="12"/>
       <c r="D120" s="13"/>
       <c r="E120" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="121" customHeight="1" ht="15.75">
+    <row r="121" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A121" s="12"/>
       <c r="B121" s="13"/>
       <c r="C121" s="12"/>
       <c r="D121" s="13"/>
       <c r="E121" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="122" customHeight="1" ht="15.75">
+    <row r="122" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A122" s="12"/>
       <c r="B122" s="13"/>
       <c r="C122" s="12"/>
       <c r="D122" s="13"/>
       <c r="E122" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="123" customHeight="1" ht="15.75">
+    <row r="123" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A123" s="12"/>
       <c r="B123" s="13"/>
       <c r="C123" s="12"/>
       <c r="D123" s="13"/>
       <c r="E123" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="124" customHeight="1" ht="15.75">
+    <row r="124" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A124" s="12"/>
       <c r="B124" s="13"/>
       <c r="C124" s="12"/>
       <c r="D124" s="13"/>
       <c r="E124" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="125" customHeight="1" ht="15.75">
+    <row r="125" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A125" s="12"/>
       <c r="B125" s="13"/>
       <c r="C125" s="12"/>
       <c r="D125" s="13"/>
       <c r="E125" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="126" customHeight="1" ht="15.75">
+    <row r="126" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A126" s="12"/>
       <c r="B126" s="13"/>
       <c r="C126" s="12"/>
       <c r="D126" s="13"/>
       <c r="E126" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="127" customHeight="1" ht="15.75">
+    <row r="127" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A127" s="12"/>
       <c r="B127" s="13"/>
       <c r="C127" s="12"/>
       <c r="D127" s="13"/>
       <c r="E127" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="128" customHeight="1" ht="15.75">
+    <row r="128" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A128" s="12"/>
       <c r="B128" s="13"/>
       <c r="C128" s="12"/>
       <c r="D128" s="13"/>
       <c r="E128" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="129" customHeight="1" ht="15.75">
+    <row r="129" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A129" s="12"/>
       <c r="B129" s="13"/>
       <c r="C129" s="12"/>
       <c r="D129" s="13"/>
       <c r="E129" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="130" customHeight="1" ht="15.75">
+    <row r="130" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A130" s="12"/>
       <c r="B130" s="13"/>
       <c r="C130" s="12"/>
       <c r="D130" s="13"/>
       <c r="E130" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="131" customHeight="1" ht="15.75">
+    <row r="131" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A131" s="12"/>
       <c r="B131" s="13"/>
       <c r="C131" s="12"/>
       <c r="D131" s="13"/>
       <c r="E131" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="132" customHeight="1" ht="15.75">
+    <row r="132" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A132" s="12"/>
       <c r="B132" s="13"/>
       <c r="C132" s="12"/>
       <c r="D132" s="13"/>
       <c r="E132" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="133" customHeight="1" ht="15.75">
+    <row r="133" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A133" s="12"/>
       <c r="B133" s="13"/>
       <c r="C133" s="12"/>
       <c r="D133" s="13"/>
       <c r="E133" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="134" customHeight="1" ht="15.75">
+    <row r="134" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A134" s="12"/>
       <c r="B134" s="13"/>
       <c r="C134" s="12"/>
       <c r="D134" s="13"/>
       <c r="E134" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="135" customHeight="1" ht="15.75">
+    <row r="135" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A135" s="12"/>
       <c r="B135" s="13"/>
       <c r="C135" s="12"/>
       <c r="D135" s="13"/>
       <c r="E135" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="136" customHeight="1" ht="15.75">
+    <row r="136" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A136" s="12"/>
       <c r="B136" s="13"/>
       <c r="C136" s="12"/>
       <c r="D136" s="13"/>
       <c r="E136" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="137" customHeight="1" ht="15.75">
+    <row r="137" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A137" s="12"/>
       <c r="B137" s="13"/>
       <c r="C137" s="12"/>
       <c r="D137" s="13"/>
       <c r="E137" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="138" customHeight="1" ht="15.75">
+    <row r="138" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A138" s="12"/>
       <c r="B138" s="13"/>
       <c r="C138" s="12"/>
       <c r="D138" s="13"/>
       <c r="E138" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="139" customHeight="1" ht="15.75">
+    <row r="139" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A139" s="12"/>
       <c r="B139" s="13"/>
       <c r="C139" s="12"/>
       <c r="D139" s="13"/>
       <c r="E139" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="140" customHeight="1" ht="15.75">
+    <row r="140" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A140" s="12"/>
       <c r="B140" s="13"/>
       <c r="C140" s="12"/>
       <c r="D140" s="13"/>
       <c r="E140" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="141" customHeight="1" ht="15.75">
+    <row r="141" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A141" s="12"/>
       <c r="B141" s="13"/>
       <c r="C141" s="12"/>
       <c r="D141" s="13"/>
       <c r="E141" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="142" customHeight="1" ht="15.75">
+    <row r="142" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A142" s="12"/>
       <c r="B142" s="13"/>
       <c r="C142" s="12"/>
       <c r="D142" s="13"/>
       <c r="E142" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="143" customHeight="1" ht="15.75">
+    <row r="143" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A143" s="12"/>
       <c r="B143" s="13"/>
       <c r="C143" s="12"/>
       <c r="D143" s="13"/>
       <c r="E143" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="144" customHeight="1" ht="15.75">
+    <row r="144" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A144" s="12"/>
       <c r="B144" s="13"/>
       <c r="C144" s="12"/>
       <c r="D144" s="13"/>
       <c r="E144" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="145" customHeight="1" ht="15.75">
+    <row r="145" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A145" s="12"/>
       <c r="B145" s="13"/>
       <c r="C145" s="12"/>
       <c r="D145" s="13"/>
       <c r="E145" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="146" customHeight="1" ht="15.75">
+    <row r="146" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A146" s="12"/>
       <c r="B146" s="13"/>
       <c r="C146" s="12"/>
       <c r="D146" s="13"/>
       <c r="E146" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="147" customHeight="1" ht="15.75">
+    <row r="147" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A147" s="12"/>
       <c r="B147" s="13"/>
       <c r="C147" s="12"/>
       <c r="D147" s="13"/>
       <c r="E147" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="148" customHeight="1" ht="15.75">
+    <row r="148" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A148" s="12"/>
       <c r="B148" s="13"/>
       <c r="C148" s="12"/>
       <c r="D148" s="13"/>
       <c r="E148" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="149" customHeight="1" ht="15.75">
+    <row r="149" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A149" s="12"/>
       <c r="B149" s="13"/>
       <c r="C149" s="12"/>
       <c r="D149" s="13"/>
       <c r="E149" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="150" customHeight="1" ht="15.75">
+    <row r="150" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A150" s="12"/>
       <c r="B150" s="13"/>
       <c r="C150" s="12"/>
       <c r="D150" s="13"/>
       <c r="E150" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="151" customHeight="1" ht="15.75">
+    <row r="151" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A151" s="12"/>
       <c r="B151" s="13"/>
       <c r="C151" s="12"/>
       <c r="D151" s="13"/>
       <c r="E151" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="152" customHeight="1" ht="15.75">
+    <row r="152" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A152" s="12"/>
       <c r="B152" s="13"/>
       <c r="C152" s="12"/>
       <c r="D152" s="13"/>
       <c r="E152" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="153" customHeight="1" ht="15.75">
+    <row r="153" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A153" s="12"/>
       <c r="B153" s="13"/>
       <c r="C153" s="12"/>
       <c r="D153" s="13"/>
       <c r="E153" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="154" customHeight="1" ht="15.75">
+    <row r="154" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A154" s="12"/>
       <c r="B154" s="13"/>
       <c r="C154" s="12"/>
       <c r="D154" s="13"/>
       <c r="E154" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="155" customHeight="1" ht="15.75">
+    <row r="155" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A155" s="12"/>
       <c r="B155" s="13"/>
       <c r="C155" s="12"/>
       <c r="D155" s="13"/>
       <c r="E155" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="156" customHeight="1" ht="15.75">
+    <row r="156" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A156" s="12"/>
       <c r="B156" s="13"/>
       <c r="C156" s="12"/>
       <c r="D156" s="13"/>
       <c r="E156" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="157" customHeight="1" ht="15.75">
+    <row r="157" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A157" s="12"/>
       <c r="B157" s="13"/>
       <c r="C157" s="12"/>
       <c r="D157" s="13"/>
       <c r="E157" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="158" customHeight="1" ht="15.75">
+    <row r="158" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A158" s="12"/>
       <c r="B158" s="13"/>
       <c r="C158" s="12"/>
       <c r="D158" s="13"/>
       <c r="E158" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="159" customHeight="1" ht="15.75">
+    <row r="159" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A159" s="12"/>
       <c r="B159" s="13"/>
       <c r="C159" s="12"/>
       <c r="D159" s="13"/>
       <c r="E159" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="160" customHeight="1" ht="15.75">
+    <row r="160" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A160" s="12"/>
       <c r="B160" s="13"/>
       <c r="C160" s="12"/>
       <c r="D160" s="13"/>
       <c r="E160" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="161" customHeight="1" ht="15.75">
+    <row r="161" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A161" s="12"/>
       <c r="B161" s="13"/>
       <c r="C161" s="12"/>
       <c r="D161" s="13"/>
       <c r="E161" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="162" customHeight="1" ht="15.75">
+    <row r="162" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A162" s="12"/>
       <c r="B162" s="13"/>
       <c r="C162" s="12"/>
       <c r="D162" s="13"/>
       <c r="E162" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="163" customHeight="1" ht="15.75">
+    <row r="163" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A163" s="12"/>
       <c r="B163" s="13"/>
       <c r="C163" s="12"/>
       <c r="D163" s="13"/>
       <c r="E163" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="164" customHeight="1" ht="15.75">
+    <row r="164" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A164" s="12"/>
       <c r="B164" s="13"/>
       <c r="C164" s="12"/>
       <c r="D164" s="13"/>
       <c r="E164" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="165" customHeight="1" ht="15.75">
+    <row r="165" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A165" s="12"/>
       <c r="B165" s="13"/>
       <c r="C165" s="12"/>
       <c r="D165" s="13"/>
       <c r="E165" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="166" customHeight="1" ht="15.75">
+    <row r="166" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A166" s="12"/>
       <c r="B166" s="13"/>
       <c r="C166" s="12"/>
       <c r="D166" s="13"/>
       <c r="E166" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="167" customHeight="1" ht="15.75">
+    <row r="167" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A167" s="12"/>
       <c r="B167" s="13"/>
       <c r="C167" s="12"/>
       <c r="D167" s="13"/>
       <c r="E167" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="168" customHeight="1" ht="15.75">
+    <row r="168" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A168" s="12"/>
       <c r="B168" s="13"/>
       <c r="C168" s="12"/>
       <c r="D168" s="13"/>
       <c r="E168" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="169" customHeight="1" ht="15.75">
+    <row r="169" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A169" s="12"/>
       <c r="B169" s="13"/>
       <c r="C169" s="12"/>
       <c r="D169" s="13"/>
       <c r="E169" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="170" customHeight="1" ht="15.75">
+    <row r="170" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A170" s="12"/>
       <c r="B170" s="13"/>
       <c r="C170" s="12"/>
       <c r="D170" s="13"/>
       <c r="E170" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="171" customHeight="1" ht="15.75">
+    <row r="171" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A171" s="12"/>
       <c r="B171" s="13"/>
       <c r="C171" s="12"/>
       <c r="D171" s="13"/>
       <c r="E171" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="172" customHeight="1" ht="15.75">
+    <row r="172" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A172" s="12"/>
       <c r="B172" s="13"/>
       <c r="C172" s="12"/>
       <c r="D172" s="13"/>
       <c r="E172" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="173" customHeight="1" ht="15.75">
+    <row r="173" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A173" s="12"/>
       <c r="B173" s="13"/>
       <c r="C173" s="12"/>
       <c r="D173" s="13"/>
       <c r="E173" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="174" customHeight="1" ht="15.75">
+    <row r="174" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A174" s="12"/>
       <c r="B174" s="13"/>
       <c r="C174" s="12"/>
       <c r="D174" s="13"/>
       <c r="E174" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="175" customHeight="1" ht="15.75">
+    <row r="175" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A175" s="12"/>
       <c r="B175" s="13"/>
       <c r="C175" s="12"/>
       <c r="D175" s="13"/>
       <c r="E175" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="176" customHeight="1" ht="15.75">
+    <row r="176" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A176" s="12"/>
       <c r="B176" s="13"/>
       <c r="C176" s="12"/>
       <c r="D176" s="13"/>
       <c r="E176" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="177" customHeight="1" ht="15.75">
+    <row r="177" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A177" s="12"/>
       <c r="B177" s="13"/>
       <c r="C177" s="12"/>
       <c r="D177" s="13"/>
       <c r="E177" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="178" customHeight="1" ht="15.75">
+    <row r="178" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A178" s="12"/>
       <c r="B178" s="13"/>
       <c r="C178" s="12"/>
       <c r="D178" s="13"/>
       <c r="E178" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="179" customHeight="1" ht="15.75">
+    <row r="179" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A179" s="12"/>
       <c r="B179" s="13"/>
       <c r="C179" s="12"/>
       <c r="D179" s="13"/>
       <c r="E179" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="180" customHeight="1" ht="15.75">
+    <row r="180" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A180" s="12"/>
       <c r="B180" s="13"/>
       <c r="C180" s="12"/>
       <c r="D180" s="13"/>
       <c r="E180" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="181" customHeight="1" ht="15.75">
+    <row r="181" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A181" s="12"/>
       <c r="B181" s="13"/>
       <c r="C181" s="12"/>
       <c r="D181" s="13"/>
       <c r="E181" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="182" customHeight="1" ht="15.75">
+    <row r="182" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A182" s="12"/>
       <c r="B182" s="13"/>
       <c r="C182" s="12"/>
       <c r="D182" s="13"/>
       <c r="E182" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="183" customHeight="1" ht="15.75">
+    <row r="183" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A183" s="12"/>
       <c r="B183" s="13"/>
       <c r="C183" s="12"/>
       <c r="D183" s="13"/>
       <c r="E183" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="184" customHeight="1" ht="15.75">
+    <row r="184" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A184" s="12"/>
       <c r="B184" s="13"/>
       <c r="C184" s="12"/>
       <c r="D184" s="13"/>
       <c r="E184" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="185" customHeight="1" ht="15.75">
+    <row r="185" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A185" s="12"/>
       <c r="B185" s="13"/>
       <c r="C185" s="12"/>
       <c r="D185" s="13"/>
       <c r="E185" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="186" customHeight="1" ht="15.75">
+    <row r="186" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A186" s="12"/>
       <c r="B186" s="13"/>
       <c r="C186" s="12"/>
       <c r="D186" s="13"/>
       <c r="E186" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="187" customHeight="1" ht="15.75">
+    <row r="187" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A187" s="12"/>
       <c r="B187" s="13"/>
       <c r="C187" s="12"/>
       <c r="D187" s="13"/>
       <c r="E187" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="188" customHeight="1" ht="15.75">
+    <row r="188" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A188" s="12"/>
       <c r="B188" s="13"/>
       <c r="C188" s="12"/>
       <c r="D188" s="13"/>
       <c r="E188" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="189" customHeight="1" ht="15.75">
+    <row r="189" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A189" s="12"/>
       <c r="B189" s="13"/>
       <c r="C189" s="12"/>
       <c r="D189" s="13"/>
       <c r="E189" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="190" customHeight="1" ht="15.75">
+    <row r="190" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A190" s="12"/>
       <c r="B190" s="13"/>
       <c r="C190" s="12"/>
       <c r="D190" s="13"/>
       <c r="E190" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="191" customHeight="1" ht="15.75">
+    <row r="191" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A191" s="12"/>
       <c r="B191" s="13"/>
       <c r="C191" s="12"/>
       <c r="D191" s="13"/>
       <c r="E191" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="192" customHeight="1" ht="15.75">
+    <row r="192" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A192" s="12"/>
       <c r="B192" s="13"/>
       <c r="C192" s="12"/>
       <c r="D192" s="13"/>
       <c r="E192" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="193" customHeight="1" ht="15.75">
+    <row r="193" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A193" s="12"/>
       <c r="B193" s="13"/>
       <c r="C193" s="12"/>
       <c r="D193" s="13"/>
       <c r="E193" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="194" customHeight="1" ht="15.75">
+    <row r="194" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A194" s="12"/>
       <c r="B194" s="13"/>
       <c r="C194" s="12"/>
       <c r="D194" s="13"/>
       <c r="E194" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="195" customHeight="1" ht="15.75">
+    <row r="195" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A195" s="12"/>
       <c r="B195" s="13"/>
       <c r="C195" s="12"/>
       <c r="D195" s="13"/>
       <c r="E195" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="196" customHeight="1" ht="15.75">
+    <row r="196" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A196" s="12"/>
       <c r="B196" s="13"/>
       <c r="C196" s="12"/>
       <c r="D196" s="13"/>
       <c r="E196" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="197" customHeight="1" ht="15.75">
+    <row r="197" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A197" s="12"/>
       <c r="B197" s="13"/>
       <c r="C197" s="12"/>
       <c r="D197" s="13"/>
       <c r="E197" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="198" customHeight="1" ht="15.75">
+    <row r="198" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A198" s="12"/>
       <c r="B198" s="13"/>
       <c r="C198" s="12"/>
       <c r="D198" s="13"/>
       <c r="E198" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="199" customHeight="1" ht="15.75">
+    <row r="199" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A199" s="12"/>
       <c r="B199" s="13"/>
       <c r="C199" s="12"/>
       <c r="D199" s="13"/>
       <c r="E199" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="200" customHeight="1" ht="15.75">
+    <row r="200" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A200" s="12"/>
       <c r="B200" s="13"/>
       <c r="C200" s="12"/>
       <c r="D200" s="13"/>
       <c r="E200" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="201" customHeight="1" ht="15.75">
+    <row r="201" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A201" s="12"/>
       <c r="B201" s="13"/>
       <c r="C201" s="12"/>
       <c r="D201" s="13"/>
       <c r="E201" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="202" customHeight="1" ht="15.75">
+    <row r="202" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A202" s="12"/>
       <c r="B202" s="13"/>
       <c r="C202" s="12"/>
       <c r="D202" s="13"/>
       <c r="E202" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="203" customHeight="1" ht="15.75">
+    <row r="203" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A203" s="12"/>
       <c r="B203" s="13"/>
       <c r="C203" s="12"/>
       <c r="D203" s="13"/>
       <c r="E203" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="204" customHeight="1" ht="15.75">
+    <row r="204" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A204" s="12"/>
       <c r="B204" s="13"/>
       <c r="C204" s="12"/>
       <c r="D204" s="13"/>
       <c r="E204" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="205" customHeight="1" ht="15.75">
+    <row r="205" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A205" s="12"/>
       <c r="B205" s="13"/>
       <c r="C205" s="12"/>
       <c r="D205" s="13"/>
       <c r="E205" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="206" customHeight="1" ht="15.75">
+    <row r="206" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A206" s="12"/>
       <c r="B206" s="13"/>
       <c r="C206" s="12"/>
       <c r="D206" s="13"/>
       <c r="E206" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="207" customHeight="1" ht="15.75">
+    <row r="207" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A207" s="12"/>
       <c r="B207" s="13"/>
       <c r="C207" s="12"/>
       <c r="D207" s="13"/>
       <c r="E207" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="208" customHeight="1" ht="15.75">
+    <row r="208" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A208" s="12"/>
       <c r="B208" s="13"/>
       <c r="C208" s="12"/>
       <c r="D208" s="13"/>
       <c r="E208" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="209" customHeight="1" ht="15.75">
+    <row r="209" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A209" s="12"/>
       <c r="B209" s="13"/>
       <c r="C209" s="12"/>
       <c r="D209" s="13"/>
       <c r="E209" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="210" customHeight="1" ht="15.75">
+    <row r="210" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A210" s="12"/>
       <c r="B210" s="13"/>
       <c r="C210" s="12"/>
       <c r="D210" s="13"/>
       <c r="E210" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="211" customHeight="1" ht="15.75">
+    <row r="211" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A211" s="12"/>
       <c r="B211" s="13"/>
       <c r="C211" s="12"/>
       <c r="D211" s="13"/>
       <c r="E211" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="212" customHeight="1" ht="15.75">
+    <row r="212" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A212" s="12"/>
       <c r="B212" s="13"/>
       <c r="C212" s="12"/>
       <c r="D212" s="13"/>
       <c r="E212" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="213" customHeight="1" ht="15.75">
+    <row r="213" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A213" s="12"/>
       <c r="B213" s="13"/>
       <c r="C213" s="12"/>
       <c r="D213" s="13"/>
       <c r="E213" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="214" customHeight="1" ht="15.75">
+    <row r="214" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A214" s="12"/>
       <c r="B214" s="13"/>
       <c r="C214" s="12"/>
       <c r="D214" s="13"/>
       <c r="E214" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="215" customHeight="1" ht="15.75">
+    <row r="215" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A215" s="12"/>
       <c r="B215" s="13"/>
       <c r="C215" s="12"/>
       <c r="D215" s="13"/>
       <c r="E215" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="216" customHeight="1" ht="15.75">
+    <row r="216" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A216" s="12"/>
       <c r="B216" s="13"/>
       <c r="C216" s="12"/>
       <c r="D216" s="13"/>
       <c r="E216" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="217" customHeight="1" ht="15.75">
+    <row r="217" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A217" s="12"/>
       <c r="B217" s="13"/>
       <c r="C217" s="12"/>
       <c r="D217" s="13"/>
       <c r="E217" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="218" customHeight="1" ht="15.75">
+    <row r="218" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A218" s="12"/>
       <c r="B218" s="13"/>
       <c r="C218" s="12"/>
       <c r="D218" s="13"/>
       <c r="E218" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="219" customHeight="1" ht="15.75">
+    <row r="219" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A219" s="12"/>
       <c r="B219" s="13"/>
       <c r="C219" s="12"/>
       <c r="D219" s="13"/>
       <c r="E219" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="220" customHeight="1" ht="15.75">
+    <row r="220" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A220" s="12"/>
       <c r="B220" s="13"/>
       <c r="C220" s="12"/>
       <c r="D220" s="13"/>
       <c r="E220" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="221" customHeight="1" ht="15.75">
+    <row r="221" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A221" s="12"/>
       <c r="B221" s="13"/>
       <c r="C221" s="12"/>
       <c r="D221" s="13"/>
       <c r="E221" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="222" customHeight="1" ht="15.75">
+    <row r="222" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A222" s="12"/>
       <c r="B222" s="13"/>
       <c r="C222" s="12"/>
       <c r="D222" s="13"/>
       <c r="E222" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="223" customHeight="1" ht="15.75">
+    <row r="223" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A223" s="12"/>
       <c r="B223" s="13"/>
       <c r="C223" s="12"/>
       <c r="D223" s="13"/>
       <c r="E223" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="224" customHeight="1" ht="15.75">
+    <row r="224" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A224" s="12"/>
       <c r="B224" s="13"/>
       <c r="C224" s="12"/>
       <c r="D224" s="13"/>
       <c r="E224" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="225" customHeight="1" ht="15.75">
+    <row r="225" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A225" s="12"/>
       <c r="B225" s="13"/>
       <c r="C225" s="12"/>
       <c r="D225" s="13"/>
       <c r="E225" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="226" customHeight="1" ht="15.75">
+    <row r="226" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A226" s="12"/>
       <c r="B226" s="13"/>
       <c r="C226" s="12"/>
       <c r="D226" s="13"/>
       <c r="E226" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="227" customHeight="1" ht="15.75">
+    <row r="227" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A227" s="12"/>
       <c r="B227" s="13"/>
       <c r="C227" s="12"/>
       <c r="D227" s="13"/>
       <c r="E227" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="228" customHeight="1" ht="15.75">
+    <row r="228" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A228" s="12"/>
       <c r="B228" s="13"/>
       <c r="C228" s="12"/>
       <c r="D228" s="13"/>
       <c r="E228" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="229" customHeight="1" ht="15.75">
+    <row r="229" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A229" s="12"/>
       <c r="B229" s="13"/>
       <c r="C229" s="12"/>
       <c r="D229" s="13"/>
       <c r="E229" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="230" customHeight="1" ht="15.75">
+    <row r="230" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A230" s="12"/>
       <c r="B230" s="13"/>
       <c r="C230" s="12"/>
       <c r="D230" s="13"/>
       <c r="E230" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="231" customHeight="1" ht="15.75">
+    <row r="231" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A231" s="12"/>
       <c r="B231" s="13"/>
       <c r="C231" s="12"/>
       <c r="D231" s="13"/>
       <c r="E231" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="232" customHeight="1" ht="15.75">
+    <row r="232" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A232" s="12"/>
       <c r="B232" s="13"/>
       <c r="C232" s="12"/>
       <c r="D232" s="13"/>
       <c r="E232" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="233" customHeight="1" ht="15.75">
+    <row r="233" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A233" s="12"/>
       <c r="B233" s="13"/>
       <c r="C233" s="12"/>
       <c r="D233" s="13"/>
       <c r="E233" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="234" customHeight="1" ht="15.75">
+    <row r="234" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A234" s="12"/>
       <c r="B234" s="13"/>
       <c r="C234" s="12"/>
       <c r="D234" s="13"/>
       <c r="E234" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="235" customHeight="1" ht="15.75">
+    <row r="235" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A235" s="12"/>
       <c r="B235" s="13"/>
       <c r="C235" s="12"/>
       <c r="D235" s="13"/>
       <c r="E235" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="236" customHeight="1" ht="15.75">
+    <row r="236" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A236" s="12"/>
       <c r="B236" s="13"/>
       <c r="C236" s="12"/>
       <c r="D236" s="13"/>
       <c r="E236" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="237" customHeight="1" ht="15.75">
+    <row r="237" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A237" s="12"/>
       <c r="B237" s="13"/>
       <c r="C237" s="12"/>
       <c r="D237" s="13"/>
       <c r="E237" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="238" customHeight="1" ht="15.75">
+    <row r="238" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A238" s="12"/>
       <c r="B238" s="13"/>
       <c r="C238" s="12"/>
       <c r="D238" s="13"/>
       <c r="E238" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="239" customHeight="1" ht="15.75">
+    <row r="239" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A239" s="12"/>
       <c r="B239" s="13"/>
       <c r="C239" s="12"/>
       <c r="D239" s="13"/>
       <c r="E239" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="240" customHeight="1" ht="15.75">
+    <row r="240" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A240" s="12"/>
       <c r="B240" s="13"/>
       <c r="C240" s="12"/>
       <c r="D240" s="13"/>
       <c r="E240" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="241" customHeight="1" ht="15.75">
+    <row r="241" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A241" s="12"/>
       <c r="B241" s="13"/>
       <c r="C241" s="12"/>
       <c r="D241" s="13"/>
       <c r="E241" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="242" customHeight="1" ht="15.75">
+    <row r="242" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A242" s="12"/>
       <c r="B242" s="13"/>
       <c r="C242" s="12"/>
       <c r="D242" s="13"/>
       <c r="E242" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="243" customHeight="1" ht="15.75">
+    <row r="243" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A243" s="12"/>
       <c r="B243" s="13"/>
       <c r="C243" s="12"/>
       <c r="D243" s="13"/>
       <c r="E243" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="244" customHeight="1" ht="15.75">
+    <row r="244" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A244" s="12"/>
       <c r="B244" s="13"/>
       <c r="C244" s="12"/>
       <c r="D244" s="13"/>
       <c r="E244" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="245" customHeight="1" ht="15.75">
+    <row r="245" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A245" s="12"/>
       <c r="B245" s="13"/>
       <c r="C245" s="12"/>
       <c r="D245" s="13"/>
       <c r="E245" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="246" customHeight="1" ht="15.75">
+    <row r="246" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A246" s="12"/>
       <c r="B246" s="13"/>
       <c r="C246" s="12"/>
       <c r="D246" s="13"/>
       <c r="E246" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="247" customHeight="1" ht="15.75">
+    <row r="247" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A247" s="12"/>
       <c r="B247" s="13"/>
       <c r="C247" s="12"/>
       <c r="D247" s="13"/>
       <c r="E247" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="248" customHeight="1" ht="15.75">
+    <row r="248" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A248" s="12"/>
       <c r="B248" s="13"/>
       <c r="C248" s="12"/>
       <c r="D248" s="13"/>
       <c r="E248" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="249" customHeight="1" ht="15.75">
+    <row r="249" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A249" s="12"/>
       <c r="B249" s="13"/>
       <c r="C249" s="12"/>
       <c r="D249" s="13"/>
       <c r="E249" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="250" customHeight="1" ht="15.75">
+    <row r="250" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A250" s="12"/>
       <c r="B250" s="13"/>
       <c r="C250" s="12"/>
       <c r="D250" s="13"/>
       <c r="E250" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="251" customHeight="1" ht="15.75">
+    <row r="251" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A251" s="12"/>
       <c r="B251" s="13"/>
       <c r="C251" s="12"/>
       <c r="D251" s="13"/>
       <c r="E251" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="252" customHeight="1" ht="15.75">
+    <row r="252" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A252" s="12"/>
       <c r="B252" s="13"/>
       <c r="C252" s="12"/>
       <c r="D252" s="13"/>
       <c r="E252" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="253" customHeight="1" ht="15.75">
+    <row r="253" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A253" s="12"/>
       <c r="B253" s="13"/>
       <c r="C253" s="12"/>
       <c r="D253" s="13"/>
       <c r="E253" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="254" customHeight="1" ht="15.75">
+    <row r="254" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A254" s="12"/>
       <c r="B254" s="13"/>
       <c r="C254" s="12"/>
       <c r="D254" s="13"/>
       <c r="E254" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="255" customHeight="1" ht="15.75">
+    <row r="255" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A255" s="12"/>
       <c r="B255" s="13"/>
       <c r="C255" s="12"/>
       <c r="D255" s="13"/>
       <c r="E255" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="256" customHeight="1" ht="15.75">
+    <row r="256" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A256" s="12"/>
       <c r="B256" s="13"/>
       <c r="C256" s="12"/>
       <c r="D256" s="13"/>
       <c r="E256" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="257" customHeight="1" ht="15.75">
+    <row r="257" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A257" s="12"/>
       <c r="B257" s="13"/>
       <c r="C257" s="12"/>
       <c r="D257" s="13"/>
       <c r="E257" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="258" customHeight="1" ht="15.75">
+    <row r="258" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A258" s="12"/>
       <c r="B258" s="13"/>
       <c r="C258" s="12"/>
       <c r="D258" s="13"/>
       <c r="E258" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="259" customHeight="1" ht="15.75">
+    <row r="259" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A259" s="12"/>
       <c r="B259" s="13"/>
       <c r="C259" s="12"/>
       <c r="D259" s="13"/>
       <c r="E259" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="260" customHeight="1" ht="15.75">
+    <row r="260" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A260" s="12"/>
       <c r="B260" s="13"/>
       <c r="C260" s="12"/>
@@ -2899,6 +2930,9 @@
       <c r="E260" s="13"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D27" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Se agrega el 27 Alumno al archivo
</commit_message>
<xml_diff>
--- a/Lista de Alumnos.xlsx
+++ b/Lista de Alumnos.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25330"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mhect\OneDrive\Escritorio\pp12021grupo7_a2-grupo7_a2-main\Alumnos\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E8CC4E3-61A2-422C-8B7B-58CB9E4E07C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Electronica Microcontrolada" sheetId="1" r:id="rId1"/>
@@ -14,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="85">
   <si>
     <t>#</t>
   </si>
@@ -260,12 +266,21 @@
   </si>
   <si>
     <t>Mauro-Martinez</t>
+  </si>
+  <si>
+    <t>Emilio Noel Moyano</t>
+  </si>
+  <si>
+    <t>emi.moyano.95@gmail.com</t>
+  </si>
+  <si>
+    <t>TerraWolf</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -469,6 +484,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -758,26 +776,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:E260"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.85546875" style="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="37.140625" style="15" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.5703125" style="14" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.88671875" style="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.109375" style="15" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5546875" style="14" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="31" style="15" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="29" style="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -794,7 +812,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -811,7 +829,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5">
         <v>2</v>
       </c>
@@ -826,7 +844,7 @@
       </c>
       <c r="E3" s="6"/>
     </row>
-    <row r="4" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5">
         <v>3</v>
       </c>
@@ -843,7 +861,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="5">
         <v>4</v>
       </c>
@@ -860,7 +878,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="5">
         <v>5</v>
       </c>
@@ -877,7 +895,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="5">
         <v>6</v>
       </c>
@@ -894,7 +912,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5">
         <v>7</v>
       </c>
@@ -911,7 +929,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="5">
         <v>8</v>
       </c>
@@ -928,7 +946,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="5">
         <v>9</v>
       </c>
@@ -943,7 +961,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="5">
         <v>10</v>
       </c>
@@ -960,7 +978,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="5">
         <v>11</v>
       </c>
@@ -977,7 +995,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="5">
         <v>12</v>
       </c>
@@ -994,7 +1012,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="5">
         <v>13</v>
       </c>
@@ -1011,7 +1029,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="5">
         <v>14</v>
       </c>
@@ -1028,7 +1046,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="5">
         <v>15</v>
       </c>
@@ -1045,7 +1063,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="5">
         <v>16</v>
       </c>
@@ -1062,7 +1080,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="5">
         <v>17</v>
       </c>
@@ -1079,7 +1097,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="5">
         <v>18</v>
       </c>
@@ -1096,7 +1114,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="5">
         <v>19</v>
       </c>
@@ -1113,7 +1131,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="5">
         <v>20</v>
       </c>
@@ -1130,7 +1148,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="5">
         <v>21</v>
       </c>
@@ -1147,7 +1165,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="5">
         <v>22</v>
       </c>
@@ -1164,7 +1182,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="5">
         <v>23</v>
       </c>
@@ -1181,7 +1199,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="5">
         <v>24</v>
       </c>
@@ -1198,7 +1216,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="5">
         <v>25</v>
       </c>
@@ -1215,7 +1233,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="5">
         <v>26</v>
       </c>
@@ -1232,16 +1250,24 @@
         <v>81</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="5">
         <v>27</v>
       </c>
-      <c r="B28" s="6"/>
-      <c r="C28" s="5"/>
-      <c r="D28" s="6"/>
-      <c r="E28" s="6"/>
-    </row>
-    <row r="29" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="C28" s="5">
+        <v>2</v>
+      </c>
+      <c r="D28" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="E28" s="6" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="5">
         <v>28</v>
       </c>
@@ -1250,7 +1276,7 @@
       <c r="D29" s="6"/>
       <c r="E29" s="6"/>
     </row>
-    <row r="30" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="5">
         <v>29</v>
       </c>
@@ -1259,7 +1285,7 @@
       <c r="D30" s="6"/>
       <c r="E30" s="6"/>
     </row>
-    <row r="31" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="5">
         <v>30</v>
       </c>
@@ -1268,7 +1294,7 @@
       <c r="D31" s="6"/>
       <c r="E31" s="6"/>
     </row>
-    <row r="32" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="5">
         <v>31</v>
       </c>
@@ -1277,7 +1303,7 @@
       <c r="D32" s="6"/>
       <c r="E32" s="6"/>
     </row>
-    <row r="33" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="5">
         <v>32</v>
       </c>
@@ -1286,7 +1312,7 @@
       <c r="D33" s="6"/>
       <c r="E33" s="6"/>
     </row>
-    <row r="34" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="5">
         <v>33</v>
       </c>
@@ -1295,7 +1321,7 @@
       <c r="D34" s="6"/>
       <c r="E34" s="6"/>
     </row>
-    <row r="35" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="5">
         <v>34</v>
       </c>
@@ -1304,7 +1330,7 @@
       <c r="D35" s="6"/>
       <c r="E35" s="6"/>
     </row>
-    <row r="36" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="5">
         <v>35</v>
       </c>
@@ -1313,7 +1339,7 @@
       <c r="D36" s="6"/>
       <c r="E36" s="6"/>
     </row>
-    <row r="37" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="5">
         <v>36</v>
       </c>
@@ -1322,7 +1348,7 @@
       <c r="D37" s="6"/>
       <c r="E37" s="6"/>
     </row>
-    <row r="38" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="5">
         <v>37</v>
       </c>
@@ -1331,7 +1357,7 @@
       <c r="D38" s="6"/>
       <c r="E38" s="6"/>
     </row>
-    <row r="39" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="5">
         <v>38</v>
       </c>
@@ -1340,7 +1366,7 @@
       <c r="D39" s="6"/>
       <c r="E39" s="6"/>
     </row>
-    <row r="40" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="5">
         <v>39</v>
       </c>
@@ -1349,7 +1375,7 @@
       <c r="D40" s="6"/>
       <c r="E40" s="6"/>
     </row>
-    <row r="41" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="5">
         <v>40</v>
       </c>
@@ -1358,7 +1384,7 @@
       <c r="D41" s="6"/>
       <c r="E41" s="6"/>
     </row>
-    <row r="42" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="5">
         <v>41</v>
       </c>
@@ -1367,7 +1393,7 @@
       <c r="D42" s="6"/>
       <c r="E42" s="6"/>
     </row>
-    <row r="43" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="5">
         <v>42</v>
       </c>
@@ -1376,7 +1402,7 @@
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
     </row>
-    <row r="44" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="5">
         <v>43</v>
       </c>
@@ -1385,7 +1411,7 @@
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
     </row>
-    <row r="45" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="5">
         <v>44</v>
       </c>
@@ -1394,7 +1420,7 @@
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
     </row>
-    <row r="46" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="5">
         <v>45</v>
       </c>
@@ -1403,7 +1429,7 @@
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
     </row>
-    <row r="47" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="5">
         <v>46</v>
       </c>
@@ -1412,7 +1438,7 @@
       <c r="D47" s="6"/>
       <c r="E47" s="6"/>
     </row>
-    <row r="48" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="5">
         <v>47</v>
       </c>
@@ -1421,7 +1447,7 @@
       <c r="D48" s="6"/>
       <c r="E48" s="6"/>
     </row>
-    <row r="49" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="5">
         <v>48</v>
       </c>
@@ -1430,7 +1456,7 @@
       <c r="D49" s="6"/>
       <c r="E49" s="6"/>
     </row>
-    <row r="50" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="5">
         <v>49</v>
       </c>
@@ -1439,7 +1465,7 @@
       <c r="D50" s="6"/>
       <c r="E50" s="6"/>
     </row>
-    <row r="51" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="5">
         <v>50</v>
       </c>
@@ -1448,7 +1474,7 @@
       <c r="D51" s="6"/>
       <c r="E51" s="6"/>
     </row>
-    <row r="52" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="5">
         <v>51</v>
       </c>
@@ -1457,7 +1483,7 @@
       <c r="D52" s="6"/>
       <c r="E52" s="6"/>
     </row>
-    <row r="53" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="5">
         <v>52</v>
       </c>
@@ -1466,7 +1492,7 @@
       <c r="D53" s="6"/>
       <c r="E53" s="6"/>
     </row>
-    <row r="54" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="5">
         <v>53</v>
       </c>
@@ -1475,7 +1501,7 @@
       <c r="D54" s="6"/>
       <c r="E54" s="6"/>
     </row>
-    <row r="55" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="5">
         <v>54</v>
       </c>
@@ -1484,7 +1510,7 @@
       <c r="D55" s="6"/>
       <c r="E55" s="6"/>
     </row>
-    <row r="56" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="5">
         <v>55</v>
       </c>
@@ -1493,7 +1519,7 @@
       <c r="D56" s="6"/>
       <c r="E56" s="6"/>
     </row>
-    <row r="57" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="5">
         <v>56</v>
       </c>
@@ -1502,7 +1528,7 @@
       <c r="D57" s="6"/>
       <c r="E57" s="6"/>
     </row>
-    <row r="58" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="5">
         <v>57</v>
       </c>
@@ -1511,7 +1537,7 @@
       <c r="D58" s="6"/>
       <c r="E58" s="6"/>
     </row>
-    <row r="59" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="5">
         <v>58</v>
       </c>
@@ -1520,7 +1546,7 @@
       <c r="D59" s="6"/>
       <c r="E59" s="6"/>
     </row>
-    <row r="60" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" s="5">
         <v>59</v>
       </c>
@@ -1529,1400 +1555,1400 @@
       <c r="D60" s="6"/>
       <c r="E60" s="6"/>
     </row>
-    <row r="61" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" s="12"/>
       <c r="B61" s="13"/>
       <c r="C61" s="12"/>
       <c r="D61" s="13"/>
       <c r="E61" s="13"/>
     </row>
-    <row r="62" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" s="12"/>
       <c r="B62" s="13"/>
       <c r="C62" s="12"/>
       <c r="D62" s="13"/>
       <c r="E62" s="13"/>
     </row>
-    <row r="63" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" s="12"/>
       <c r="B63" s="13"/>
       <c r="C63" s="12"/>
       <c r="D63" s="13"/>
       <c r="E63" s="13"/>
     </row>
-    <row r="64" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" s="12"/>
       <c r="B64" s="13"/>
       <c r="C64" s="12"/>
       <c r="D64" s="13"/>
       <c r="E64" s="13"/>
     </row>
-    <row r="65" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A65" s="12"/>
       <c r="B65" s="13"/>
       <c r="C65" s="12"/>
       <c r="D65" s="13"/>
       <c r="E65" s="13"/>
     </row>
-    <row r="66" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A66" s="12"/>
       <c r="B66" s="13"/>
       <c r="C66" s="12"/>
       <c r="D66" s="13"/>
       <c r="E66" s="13"/>
     </row>
-    <row r="67" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67" s="12"/>
       <c r="B67" s="13"/>
       <c r="C67" s="12"/>
       <c r="D67" s="13"/>
       <c r="E67" s="13"/>
     </row>
-    <row r="68" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" s="12"/>
       <c r="B68" s="13"/>
       <c r="C68" s="12"/>
       <c r="D68" s="13"/>
       <c r="E68" s="13"/>
     </row>
-    <row r="69" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69" s="12"/>
       <c r="B69" s="13"/>
       <c r="C69" s="12"/>
       <c r="D69" s="13"/>
       <c r="E69" s="13"/>
     </row>
-    <row r="70" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A70" s="12"/>
       <c r="B70" s="13"/>
       <c r="C70" s="12"/>
       <c r="D70" s="13"/>
       <c r="E70" s="13"/>
     </row>
-    <row r="71" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A71" s="12"/>
       <c r="B71" s="13"/>
       <c r="C71" s="12"/>
       <c r="D71" s="13"/>
       <c r="E71" s="13"/>
     </row>
-    <row r="72" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72" s="12"/>
       <c r="B72" s="13"/>
       <c r="C72" s="12"/>
       <c r="D72" s="13"/>
       <c r="E72" s="13"/>
     </row>
-    <row r="73" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A73" s="12"/>
       <c r="B73" s="13"/>
       <c r="C73" s="12"/>
       <c r="D73" s="13"/>
       <c r="E73" s="13"/>
     </row>
-    <row r="74" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A74" s="12"/>
       <c r="B74" s="13"/>
       <c r="C74" s="12"/>
       <c r="D74" s="13"/>
       <c r="E74" s="13"/>
     </row>
-    <row r="75" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A75" s="12"/>
       <c r="B75" s="13"/>
       <c r="C75" s="12"/>
       <c r="D75" s="13"/>
       <c r="E75" s="13"/>
     </row>
-    <row r="76" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A76" s="12"/>
       <c r="B76" s="13"/>
       <c r="C76" s="12"/>
       <c r="D76" s="13"/>
       <c r="E76" s="13"/>
     </row>
-    <row r="77" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A77" s="12"/>
       <c r="B77" s="13"/>
       <c r="C77" s="12"/>
       <c r="D77" s="13"/>
       <c r="E77" s="13"/>
     </row>
-    <row r="78" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A78" s="12"/>
       <c r="B78" s="13"/>
       <c r="C78" s="12"/>
       <c r="D78" s="13"/>
       <c r="E78" s="13"/>
     </row>
-    <row r="79" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A79" s="12"/>
       <c r="B79" s="13"/>
       <c r="C79" s="12"/>
       <c r="D79" s="13"/>
       <c r="E79" s="13"/>
     </row>
-    <row r="80" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A80" s="12"/>
       <c r="B80" s="13"/>
       <c r="C80" s="12"/>
       <c r="D80" s="13"/>
       <c r="E80" s="13"/>
     </row>
-    <row r="81" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A81" s="12"/>
       <c r="B81" s="13"/>
       <c r="C81" s="12"/>
       <c r="D81" s="13"/>
       <c r="E81" s="13"/>
     </row>
-    <row r="82" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A82" s="12"/>
       <c r="B82" s="13"/>
       <c r="C82" s="12"/>
       <c r="D82" s="13"/>
       <c r="E82" s="13"/>
     </row>
-    <row r="83" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A83" s="12"/>
       <c r="B83" s="13"/>
       <c r="C83" s="12"/>
       <c r="D83" s="13"/>
       <c r="E83" s="13"/>
     </row>
-    <row r="84" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A84" s="12"/>
       <c r="B84" s="13"/>
       <c r="C84" s="12"/>
       <c r="D84" s="13"/>
       <c r="E84" s="13"/>
     </row>
-    <row r="85" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A85" s="12"/>
       <c r="B85" s="13"/>
       <c r="C85" s="12"/>
       <c r="D85" s="13"/>
       <c r="E85" s="13"/>
     </row>
-    <row r="86" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A86" s="12"/>
       <c r="B86" s="13"/>
       <c r="C86" s="12"/>
       <c r="D86" s="13"/>
       <c r="E86" s="13"/>
     </row>
-    <row r="87" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A87" s="12"/>
       <c r="B87" s="13"/>
       <c r="C87" s="12"/>
       <c r="D87" s="13"/>
       <c r="E87" s="13"/>
     </row>
-    <row r="88" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A88" s="12"/>
       <c r="B88" s="13"/>
       <c r="C88" s="12"/>
       <c r="D88" s="13"/>
       <c r="E88" s="13"/>
     </row>
-    <row r="89" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A89" s="12"/>
       <c r="B89" s="13"/>
       <c r="C89" s="12"/>
       <c r="D89" s="13"/>
       <c r="E89" s="13"/>
     </row>
-    <row r="90" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A90" s="12"/>
       <c r="B90" s="13"/>
       <c r="C90" s="12"/>
       <c r="D90" s="13"/>
       <c r="E90" s="13"/>
     </row>
-    <row r="91" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A91" s="12"/>
       <c r="B91" s="13"/>
       <c r="C91" s="12"/>
       <c r="D91" s="13"/>
       <c r="E91" s="13"/>
     </row>
-    <row r="92" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A92" s="12"/>
       <c r="B92" s="13"/>
       <c r="C92" s="12"/>
       <c r="D92" s="13"/>
       <c r="E92" s="13"/>
     </row>
-    <row r="93" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A93" s="12"/>
       <c r="B93" s="13"/>
       <c r="C93" s="12"/>
       <c r="D93" s="13"/>
       <c r="E93" s="13"/>
     </row>
-    <row r="94" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A94" s="12"/>
       <c r="B94" s="13"/>
       <c r="C94" s="12"/>
       <c r="D94" s="13"/>
       <c r="E94" s="13"/>
     </row>
-    <row r="95" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A95" s="12"/>
       <c r="B95" s="13"/>
       <c r="C95" s="12"/>
       <c r="D95" s="13"/>
       <c r="E95" s="13"/>
     </row>
-    <row r="96" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A96" s="12"/>
       <c r="B96" s="13"/>
       <c r="C96" s="12"/>
       <c r="D96" s="13"/>
       <c r="E96" s="13"/>
     </row>
-    <row r="97" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A97" s="12"/>
       <c r="B97" s="13"/>
       <c r="C97" s="12"/>
       <c r="D97" s="13"/>
       <c r="E97" s="13"/>
     </row>
-    <row r="98" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A98" s="12"/>
       <c r="B98" s="13"/>
       <c r="C98" s="12"/>
       <c r="D98" s="13"/>
       <c r="E98" s="13"/>
     </row>
-    <row r="99" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A99" s="12"/>
       <c r="B99" s="13"/>
       <c r="C99" s="12"/>
       <c r="D99" s="13"/>
       <c r="E99" s="13"/>
     </row>
-    <row r="100" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A100" s="12"/>
       <c r="B100" s="13"/>
       <c r="C100" s="12"/>
       <c r="D100" s="13"/>
       <c r="E100" s="13"/>
     </row>
-    <row r="101" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A101" s="12"/>
       <c r="B101" s="13"/>
       <c r="C101" s="12"/>
       <c r="D101" s="13"/>
       <c r="E101" s="13"/>
     </row>
-    <row r="102" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A102" s="12"/>
       <c r="B102" s="13"/>
       <c r="C102" s="12"/>
       <c r="D102" s="13"/>
       <c r="E102" s="13"/>
     </row>
-    <row r="103" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A103" s="12"/>
       <c r="B103" s="13"/>
       <c r="C103" s="12"/>
       <c r="D103" s="13"/>
       <c r="E103" s="13"/>
     </row>
-    <row r="104" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A104" s="12"/>
       <c r="B104" s="13"/>
       <c r="C104" s="12"/>
       <c r="D104" s="13"/>
       <c r="E104" s="13"/>
     </row>
-    <row r="105" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A105" s="12"/>
       <c r="B105" s="13"/>
       <c r="C105" s="12"/>
       <c r="D105" s="13"/>
       <c r="E105" s="13"/>
     </row>
-    <row r="106" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A106" s="12"/>
       <c r="B106" s="13"/>
       <c r="C106" s="12"/>
       <c r="D106" s="13"/>
       <c r="E106" s="13"/>
     </row>
-    <row r="107" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A107" s="12"/>
       <c r="B107" s="13"/>
       <c r="C107" s="12"/>
       <c r="D107" s="13"/>
       <c r="E107" s="13"/>
     </row>
-    <row r="108" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A108" s="12"/>
       <c r="B108" s="13"/>
       <c r="C108" s="12"/>
       <c r="D108" s="13"/>
       <c r="E108" s="13"/>
     </row>
-    <row r="109" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A109" s="12"/>
       <c r="B109" s="13"/>
       <c r="C109" s="12"/>
       <c r="D109" s="13"/>
       <c r="E109" s="13"/>
     </row>
-    <row r="110" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A110" s="12"/>
       <c r="B110" s="13"/>
       <c r="C110" s="12"/>
       <c r="D110" s="13"/>
       <c r="E110" s="13"/>
     </row>
-    <row r="111" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A111" s="12"/>
       <c r="B111" s="13"/>
       <c r="C111" s="12"/>
       <c r="D111" s="13"/>
       <c r="E111" s="13"/>
     </row>
-    <row r="112" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A112" s="12"/>
       <c r="B112" s="13"/>
       <c r="C112" s="12"/>
       <c r="D112" s="13"/>
       <c r="E112" s="13"/>
     </row>
-    <row r="113" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A113" s="12"/>
       <c r="B113" s="13"/>
       <c r="C113" s="12"/>
       <c r="D113" s="13"/>
       <c r="E113" s="13"/>
     </row>
-    <row r="114" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A114" s="12"/>
       <c r="B114" s="13"/>
       <c r="C114" s="12"/>
       <c r="D114" s="13"/>
       <c r="E114" s="13"/>
     </row>
-    <row r="115" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A115" s="12"/>
       <c r="B115" s="13"/>
       <c r="C115" s="12"/>
       <c r="D115" s="13"/>
       <c r="E115" s="13"/>
     </row>
-    <row r="116" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A116" s="12"/>
       <c r="B116" s="13"/>
       <c r="C116" s="12"/>
       <c r="D116" s="13"/>
       <c r="E116" s="13"/>
     </row>
-    <row r="117" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A117" s="12"/>
       <c r="B117" s="13"/>
       <c r="C117" s="12"/>
       <c r="D117" s="13"/>
       <c r="E117" s="13"/>
     </row>
-    <row r="118" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A118" s="12"/>
       <c r="B118" s="13"/>
       <c r="C118" s="12"/>
       <c r="D118" s="13"/>
       <c r="E118" s="13"/>
     </row>
-    <row r="119" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A119" s="12"/>
       <c r="B119" s="13"/>
       <c r="C119" s="12"/>
       <c r="D119" s="13"/>
       <c r="E119" s="13"/>
     </row>
-    <row r="120" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A120" s="12"/>
       <c r="B120" s="13"/>
       <c r="C120" s="12"/>
       <c r="D120" s="13"/>
       <c r="E120" s="13"/>
     </row>
-    <row r="121" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A121" s="12"/>
       <c r="B121" s="13"/>
       <c r="C121" s="12"/>
       <c r="D121" s="13"/>
       <c r="E121" s="13"/>
     </row>
-    <row r="122" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A122" s="12"/>
       <c r="B122" s="13"/>
       <c r="C122" s="12"/>
       <c r="D122" s="13"/>
       <c r="E122" s="13"/>
     </row>
-    <row r="123" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A123" s="12"/>
       <c r="B123" s="13"/>
       <c r="C123" s="12"/>
       <c r="D123" s="13"/>
       <c r="E123" s="13"/>
     </row>
-    <row r="124" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A124" s="12"/>
       <c r="B124" s="13"/>
       <c r="C124" s="12"/>
       <c r="D124" s="13"/>
       <c r="E124" s="13"/>
     </row>
-    <row r="125" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A125" s="12"/>
       <c r="B125" s="13"/>
       <c r="C125" s="12"/>
       <c r="D125" s="13"/>
       <c r="E125" s="13"/>
     </row>
-    <row r="126" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A126" s="12"/>
       <c r="B126" s="13"/>
       <c r="C126" s="12"/>
       <c r="D126" s="13"/>
       <c r="E126" s="13"/>
     </row>
-    <row r="127" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A127" s="12"/>
       <c r="B127" s="13"/>
       <c r="C127" s="12"/>
       <c r="D127" s="13"/>
       <c r="E127" s="13"/>
     </row>
-    <row r="128" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A128" s="12"/>
       <c r="B128" s="13"/>
       <c r="C128" s="12"/>
       <c r="D128" s="13"/>
       <c r="E128" s="13"/>
     </row>
-    <row r="129" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A129" s="12"/>
       <c r="B129" s="13"/>
       <c r="C129" s="12"/>
       <c r="D129" s="13"/>
       <c r="E129" s="13"/>
     </row>
-    <row r="130" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A130" s="12"/>
       <c r="B130" s="13"/>
       <c r="C130" s="12"/>
       <c r="D130" s="13"/>
       <c r="E130" s="13"/>
     </row>
-    <row r="131" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A131" s="12"/>
       <c r="B131" s="13"/>
       <c r="C131" s="12"/>
       <c r="D131" s="13"/>
       <c r="E131" s="13"/>
     </row>
-    <row r="132" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A132" s="12"/>
       <c r="B132" s="13"/>
       <c r="C132" s="12"/>
       <c r="D132" s="13"/>
       <c r="E132" s="13"/>
     </row>
-    <row r="133" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A133" s="12"/>
       <c r="B133" s="13"/>
       <c r="C133" s="12"/>
       <c r="D133" s="13"/>
       <c r="E133" s="13"/>
     </row>
-    <row r="134" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A134" s="12"/>
       <c r="B134" s="13"/>
       <c r="C134" s="12"/>
       <c r="D134" s="13"/>
       <c r="E134" s="13"/>
     </row>
-    <row r="135" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A135" s="12"/>
       <c r="B135" s="13"/>
       <c r="C135" s="12"/>
       <c r="D135" s="13"/>
       <c r="E135" s="13"/>
     </row>
-    <row r="136" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A136" s="12"/>
       <c r="B136" s="13"/>
       <c r="C136" s="12"/>
       <c r="D136" s="13"/>
       <c r="E136" s="13"/>
     </row>
-    <row r="137" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A137" s="12"/>
       <c r="B137" s="13"/>
       <c r="C137" s="12"/>
       <c r="D137" s="13"/>
       <c r="E137" s="13"/>
     </row>
-    <row r="138" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A138" s="12"/>
       <c r="B138" s="13"/>
       <c r="C138" s="12"/>
       <c r="D138" s="13"/>
       <c r="E138" s="13"/>
     </row>
-    <row r="139" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A139" s="12"/>
       <c r="B139" s="13"/>
       <c r="C139" s="12"/>
       <c r="D139" s="13"/>
       <c r="E139" s="13"/>
     </row>
-    <row r="140" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A140" s="12"/>
       <c r="B140" s="13"/>
       <c r="C140" s="12"/>
       <c r="D140" s="13"/>
       <c r="E140" s="13"/>
     </row>
-    <row r="141" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A141" s="12"/>
       <c r="B141" s="13"/>
       <c r="C141" s="12"/>
       <c r="D141" s="13"/>
       <c r="E141" s="13"/>
     </row>
-    <row r="142" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A142" s="12"/>
       <c r="B142" s="13"/>
       <c r="C142" s="12"/>
       <c r="D142" s="13"/>
       <c r="E142" s="13"/>
     </row>
-    <row r="143" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A143" s="12"/>
       <c r="B143" s="13"/>
       <c r="C143" s="12"/>
       <c r="D143" s="13"/>
       <c r="E143" s="13"/>
     </row>
-    <row r="144" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A144" s="12"/>
       <c r="B144" s="13"/>
       <c r="C144" s="12"/>
       <c r="D144" s="13"/>
       <c r="E144" s="13"/>
     </row>
-    <row r="145" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A145" s="12"/>
       <c r="B145" s="13"/>
       <c r="C145" s="12"/>
       <c r="D145" s="13"/>
       <c r="E145" s="13"/>
     </row>
-    <row r="146" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A146" s="12"/>
       <c r="B146" s="13"/>
       <c r="C146" s="12"/>
       <c r="D146" s="13"/>
       <c r="E146" s="13"/>
     </row>
-    <row r="147" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A147" s="12"/>
       <c r="B147" s="13"/>
       <c r="C147" s="12"/>
       <c r="D147" s="13"/>
       <c r="E147" s="13"/>
     </row>
-    <row r="148" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A148" s="12"/>
       <c r="B148" s="13"/>
       <c r="C148" s="12"/>
       <c r="D148" s="13"/>
       <c r="E148" s="13"/>
     </row>
-    <row r="149" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A149" s="12"/>
       <c r="B149" s="13"/>
       <c r="C149" s="12"/>
       <c r="D149" s="13"/>
       <c r="E149" s="13"/>
     </row>
-    <row r="150" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A150" s="12"/>
       <c r="B150" s="13"/>
       <c r="C150" s="12"/>
       <c r="D150" s="13"/>
       <c r="E150" s="13"/>
     </row>
-    <row r="151" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A151" s="12"/>
       <c r="B151" s="13"/>
       <c r="C151" s="12"/>
       <c r="D151" s="13"/>
       <c r="E151" s="13"/>
     </row>
-    <row r="152" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A152" s="12"/>
       <c r="B152" s="13"/>
       <c r="C152" s="12"/>
       <c r="D152" s="13"/>
       <c r="E152" s="13"/>
     </row>
-    <row r="153" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A153" s="12"/>
       <c r="B153" s="13"/>
       <c r="C153" s="12"/>
       <c r="D153" s="13"/>
       <c r="E153" s="13"/>
     </row>
-    <row r="154" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A154" s="12"/>
       <c r="B154" s="13"/>
       <c r="C154" s="12"/>
       <c r="D154" s="13"/>
       <c r="E154" s="13"/>
     </row>
-    <row r="155" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A155" s="12"/>
       <c r="B155" s="13"/>
       <c r="C155" s="12"/>
       <c r="D155" s="13"/>
       <c r="E155" s="13"/>
     </row>
-    <row r="156" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A156" s="12"/>
       <c r="B156" s="13"/>
       <c r="C156" s="12"/>
       <c r="D156" s="13"/>
       <c r="E156" s="13"/>
     </row>
-    <row r="157" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A157" s="12"/>
       <c r="B157" s="13"/>
       <c r="C157" s="12"/>
       <c r="D157" s="13"/>
       <c r="E157" s="13"/>
     </row>
-    <row r="158" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A158" s="12"/>
       <c r="B158" s="13"/>
       <c r="C158" s="12"/>
       <c r="D158" s="13"/>
       <c r="E158" s="13"/>
     </row>
-    <row r="159" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A159" s="12"/>
       <c r="B159" s="13"/>
       <c r="C159" s="12"/>
       <c r="D159" s="13"/>
       <c r="E159" s="13"/>
     </row>
-    <row r="160" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A160" s="12"/>
       <c r="B160" s="13"/>
       <c r="C160" s="12"/>
       <c r="D160" s="13"/>
       <c r="E160" s="13"/>
     </row>
-    <row r="161" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A161" s="12"/>
       <c r="B161" s="13"/>
       <c r="C161" s="12"/>
       <c r="D161" s="13"/>
       <c r="E161" s="13"/>
     </row>
-    <row r="162" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A162" s="12"/>
       <c r="B162" s="13"/>
       <c r="C162" s="12"/>
       <c r="D162" s="13"/>
       <c r="E162" s="13"/>
     </row>
-    <row r="163" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A163" s="12"/>
       <c r="B163" s="13"/>
       <c r="C163" s="12"/>
       <c r="D163" s="13"/>
       <c r="E163" s="13"/>
     </row>
-    <row r="164" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A164" s="12"/>
       <c r="B164" s="13"/>
       <c r="C164" s="12"/>
       <c r="D164" s="13"/>
       <c r="E164" s="13"/>
     </row>
-    <row r="165" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A165" s="12"/>
       <c r="B165" s="13"/>
       <c r="C165" s="12"/>
       <c r="D165" s="13"/>
       <c r="E165" s="13"/>
     </row>
-    <row r="166" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A166" s="12"/>
       <c r="B166" s="13"/>
       <c r="C166" s="12"/>
       <c r="D166" s="13"/>
       <c r="E166" s="13"/>
     </row>
-    <row r="167" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A167" s="12"/>
       <c r="B167" s="13"/>
       <c r="C167" s="12"/>
       <c r="D167" s="13"/>
       <c r="E167" s="13"/>
     </row>
-    <row r="168" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A168" s="12"/>
       <c r="B168" s="13"/>
       <c r="C168" s="12"/>
       <c r="D168" s="13"/>
       <c r="E168" s="13"/>
     </row>
-    <row r="169" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A169" s="12"/>
       <c r="B169" s="13"/>
       <c r="C169" s="12"/>
       <c r="D169" s="13"/>
       <c r="E169" s="13"/>
     </row>
-    <row r="170" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A170" s="12"/>
       <c r="B170" s="13"/>
       <c r="C170" s="12"/>
       <c r="D170" s="13"/>
       <c r="E170" s="13"/>
     </row>
-    <row r="171" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A171" s="12"/>
       <c r="B171" s="13"/>
       <c r="C171" s="12"/>
       <c r="D171" s="13"/>
       <c r="E171" s="13"/>
     </row>
-    <row r="172" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A172" s="12"/>
       <c r="B172" s="13"/>
       <c r="C172" s="12"/>
       <c r="D172" s="13"/>
       <c r="E172" s="13"/>
     </row>
-    <row r="173" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A173" s="12"/>
       <c r="B173" s="13"/>
       <c r="C173" s="12"/>
       <c r="D173" s="13"/>
       <c r="E173" s="13"/>
     </row>
-    <row r="174" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A174" s="12"/>
       <c r="B174" s="13"/>
       <c r="C174" s="12"/>
       <c r="D174" s="13"/>
       <c r="E174" s="13"/>
     </row>
-    <row r="175" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A175" s="12"/>
       <c r="B175" s="13"/>
       <c r="C175" s="12"/>
       <c r="D175" s="13"/>
       <c r="E175" s="13"/>
     </row>
-    <row r="176" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A176" s="12"/>
       <c r="B176" s="13"/>
       <c r="C176" s="12"/>
       <c r="D176" s="13"/>
       <c r="E176" s="13"/>
     </row>
-    <row r="177" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A177" s="12"/>
       <c r="B177" s="13"/>
       <c r="C177" s="12"/>
       <c r="D177" s="13"/>
       <c r="E177" s="13"/>
     </row>
-    <row r="178" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A178" s="12"/>
       <c r="B178" s="13"/>
       <c r="C178" s="12"/>
       <c r="D178" s="13"/>
       <c r="E178" s="13"/>
     </row>
-    <row r="179" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A179" s="12"/>
       <c r="B179" s="13"/>
       <c r="C179" s="12"/>
       <c r="D179" s="13"/>
       <c r="E179" s="13"/>
     </row>
-    <row r="180" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A180" s="12"/>
       <c r="B180" s="13"/>
       <c r="C180" s="12"/>
       <c r="D180" s="13"/>
       <c r="E180" s="13"/>
     </row>
-    <row r="181" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A181" s="12"/>
       <c r="B181" s="13"/>
       <c r="C181" s="12"/>
       <c r="D181" s="13"/>
       <c r="E181" s="13"/>
     </row>
-    <row r="182" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A182" s="12"/>
       <c r="B182" s="13"/>
       <c r="C182" s="12"/>
       <c r="D182" s="13"/>
       <c r="E182" s="13"/>
     </row>
-    <row r="183" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A183" s="12"/>
       <c r="B183" s="13"/>
       <c r="C183" s="12"/>
       <c r="D183" s="13"/>
       <c r="E183" s="13"/>
     </row>
-    <row r="184" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A184" s="12"/>
       <c r="B184" s="13"/>
       <c r="C184" s="12"/>
       <c r="D184" s="13"/>
       <c r="E184" s="13"/>
     </row>
-    <row r="185" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A185" s="12"/>
       <c r="B185" s="13"/>
       <c r="C185" s="12"/>
       <c r="D185" s="13"/>
       <c r="E185" s="13"/>
     </row>
-    <row r="186" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A186" s="12"/>
       <c r="B186" s="13"/>
       <c r="C186" s="12"/>
       <c r="D186" s="13"/>
       <c r="E186" s="13"/>
     </row>
-    <row r="187" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A187" s="12"/>
       <c r="B187" s="13"/>
       <c r="C187" s="12"/>
       <c r="D187" s="13"/>
       <c r="E187" s="13"/>
     </row>
-    <row r="188" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A188" s="12"/>
       <c r="B188" s="13"/>
       <c r="C188" s="12"/>
       <c r="D188" s="13"/>
       <c r="E188" s="13"/>
     </row>
-    <row r="189" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A189" s="12"/>
       <c r="B189" s="13"/>
       <c r="C189" s="12"/>
       <c r="D189" s="13"/>
       <c r="E189" s="13"/>
     </row>
-    <row r="190" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A190" s="12"/>
       <c r="B190" s="13"/>
       <c r="C190" s="12"/>
       <c r="D190" s="13"/>
       <c r="E190" s="13"/>
     </row>
-    <row r="191" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A191" s="12"/>
       <c r="B191" s="13"/>
       <c r="C191" s="12"/>
       <c r="D191" s="13"/>
       <c r="E191" s="13"/>
     </row>
-    <row r="192" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A192" s="12"/>
       <c r="B192" s="13"/>
       <c r="C192" s="12"/>
       <c r="D192" s="13"/>
       <c r="E192" s="13"/>
     </row>
-    <row r="193" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A193" s="12"/>
       <c r="B193" s="13"/>
       <c r="C193" s="12"/>
       <c r="D193" s="13"/>
       <c r="E193" s="13"/>
     </row>
-    <row r="194" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A194" s="12"/>
       <c r="B194" s="13"/>
       <c r="C194" s="12"/>
       <c r="D194" s="13"/>
       <c r="E194" s="13"/>
     </row>
-    <row r="195" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A195" s="12"/>
       <c r="B195" s="13"/>
       <c r="C195" s="12"/>
       <c r="D195" s="13"/>
       <c r="E195" s="13"/>
     </row>
-    <row r="196" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A196" s="12"/>
       <c r="B196" s="13"/>
       <c r="C196" s="12"/>
       <c r="D196" s="13"/>
       <c r="E196" s="13"/>
     </row>
-    <row r="197" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A197" s="12"/>
       <c r="B197" s="13"/>
       <c r="C197" s="12"/>
       <c r="D197" s="13"/>
       <c r="E197" s="13"/>
     </row>
-    <row r="198" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A198" s="12"/>
       <c r="B198" s="13"/>
       <c r="C198" s="12"/>
       <c r="D198" s="13"/>
       <c r="E198" s="13"/>
     </row>
-    <row r="199" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A199" s="12"/>
       <c r="B199" s="13"/>
       <c r="C199" s="12"/>
       <c r="D199" s="13"/>
       <c r="E199" s="13"/>
     </row>
-    <row r="200" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A200" s="12"/>
       <c r="B200" s="13"/>
       <c r="C200" s="12"/>
       <c r="D200" s="13"/>
       <c r="E200" s="13"/>
     </row>
-    <row r="201" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A201" s="12"/>
       <c r="B201" s="13"/>
       <c r="C201" s="12"/>
       <c r="D201" s="13"/>
       <c r="E201" s="13"/>
     </row>
-    <row r="202" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A202" s="12"/>
       <c r="B202" s="13"/>
       <c r="C202" s="12"/>
       <c r="D202" s="13"/>
       <c r="E202" s="13"/>
     </row>
-    <row r="203" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A203" s="12"/>
       <c r="B203" s="13"/>
       <c r="C203" s="12"/>
       <c r="D203" s="13"/>
       <c r="E203" s="13"/>
     </row>
-    <row r="204" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A204" s="12"/>
       <c r="B204" s="13"/>
       <c r="C204" s="12"/>
       <c r="D204" s="13"/>
       <c r="E204" s="13"/>
     </row>
-    <row r="205" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A205" s="12"/>
       <c r="B205" s="13"/>
       <c r="C205" s="12"/>
       <c r="D205" s="13"/>
       <c r="E205" s="13"/>
     </row>
-    <row r="206" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A206" s="12"/>
       <c r="B206" s="13"/>
       <c r="C206" s="12"/>
       <c r="D206" s="13"/>
       <c r="E206" s="13"/>
     </row>
-    <row r="207" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A207" s="12"/>
       <c r="B207" s="13"/>
       <c r="C207" s="12"/>
       <c r="D207" s="13"/>
       <c r="E207" s="13"/>
     </row>
-    <row r="208" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A208" s="12"/>
       <c r="B208" s="13"/>
       <c r="C208" s="12"/>
       <c r="D208" s="13"/>
       <c r="E208" s="13"/>
     </row>
-    <row r="209" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A209" s="12"/>
       <c r="B209" s="13"/>
       <c r="C209" s="12"/>
       <c r="D209" s="13"/>
       <c r="E209" s="13"/>
     </row>
-    <row r="210" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A210" s="12"/>
       <c r="B210" s="13"/>
       <c r="C210" s="12"/>
       <c r="D210" s="13"/>
       <c r="E210" s="13"/>
     </row>
-    <row r="211" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A211" s="12"/>
       <c r="B211" s="13"/>
       <c r="C211" s="12"/>
       <c r="D211" s="13"/>
       <c r="E211" s="13"/>
     </row>
-    <row r="212" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A212" s="12"/>
       <c r="B212" s="13"/>
       <c r="C212" s="12"/>
       <c r="D212" s="13"/>
       <c r="E212" s="13"/>
     </row>
-    <row r="213" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A213" s="12"/>
       <c r="B213" s="13"/>
       <c r="C213" s="12"/>
       <c r="D213" s="13"/>
       <c r="E213" s="13"/>
     </row>
-    <row r="214" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A214" s="12"/>
       <c r="B214" s="13"/>
       <c r="C214" s="12"/>
       <c r="D214" s="13"/>
       <c r="E214" s="13"/>
     </row>
-    <row r="215" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A215" s="12"/>
       <c r="B215" s="13"/>
       <c r="C215" s="12"/>
       <c r="D215" s="13"/>
       <c r="E215" s="13"/>
     </row>
-    <row r="216" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A216" s="12"/>
       <c r="B216" s="13"/>
       <c r="C216" s="12"/>
       <c r="D216" s="13"/>
       <c r="E216" s="13"/>
     </row>
-    <row r="217" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A217" s="12"/>
       <c r="B217" s="13"/>
       <c r="C217" s="12"/>
       <c r="D217" s="13"/>
       <c r="E217" s="13"/>
     </row>
-    <row r="218" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A218" s="12"/>
       <c r="B218" s="13"/>
       <c r="C218" s="12"/>
       <c r="D218" s="13"/>
       <c r="E218" s="13"/>
     </row>
-    <row r="219" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A219" s="12"/>
       <c r="B219" s="13"/>
       <c r="C219" s="12"/>
       <c r="D219" s="13"/>
       <c r="E219" s="13"/>
     </row>
-    <row r="220" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A220" s="12"/>
       <c r="B220" s="13"/>
       <c r="C220" s="12"/>
       <c r="D220" s="13"/>
       <c r="E220" s="13"/>
     </row>
-    <row r="221" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A221" s="12"/>
       <c r="B221" s="13"/>
       <c r="C221" s="12"/>
       <c r="D221" s="13"/>
       <c r="E221" s="13"/>
     </row>
-    <row r="222" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A222" s="12"/>
       <c r="B222" s="13"/>
       <c r="C222" s="12"/>
       <c r="D222" s="13"/>
       <c r="E222" s="13"/>
     </row>
-    <row r="223" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A223" s="12"/>
       <c r="B223" s="13"/>
       <c r="C223" s="12"/>
       <c r="D223" s="13"/>
       <c r="E223" s="13"/>
     </row>
-    <row r="224" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A224" s="12"/>
       <c r="B224" s="13"/>
       <c r="C224" s="12"/>
       <c r="D224" s="13"/>
       <c r="E224" s="13"/>
     </row>
-    <row r="225" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A225" s="12"/>
       <c r="B225" s="13"/>
       <c r="C225" s="12"/>
       <c r="D225" s="13"/>
       <c r="E225" s="13"/>
     </row>
-    <row r="226" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A226" s="12"/>
       <c r="B226" s="13"/>
       <c r="C226" s="12"/>
       <c r="D226" s="13"/>
       <c r="E226" s="13"/>
     </row>
-    <row r="227" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A227" s="12"/>
       <c r="B227" s="13"/>
       <c r="C227" s="12"/>
       <c r="D227" s="13"/>
       <c r="E227" s="13"/>
     </row>
-    <row r="228" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A228" s="12"/>
       <c r="B228" s="13"/>
       <c r="C228" s="12"/>
       <c r="D228" s="13"/>
       <c r="E228" s="13"/>
     </row>
-    <row r="229" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A229" s="12"/>
       <c r="B229" s="13"/>
       <c r="C229" s="12"/>
       <c r="D229" s="13"/>
       <c r="E229" s="13"/>
     </row>
-    <row r="230" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A230" s="12"/>
       <c r="B230" s="13"/>
       <c r="C230" s="12"/>
       <c r="D230" s="13"/>
       <c r="E230" s="13"/>
     </row>
-    <row r="231" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A231" s="12"/>
       <c r="B231" s="13"/>
       <c r="C231" s="12"/>
       <c r="D231" s="13"/>
       <c r="E231" s="13"/>
     </row>
-    <row r="232" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A232" s="12"/>
       <c r="B232" s="13"/>
       <c r="C232" s="12"/>
       <c r="D232" s="13"/>
       <c r="E232" s="13"/>
     </row>
-    <row r="233" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A233" s="12"/>
       <c r="B233" s="13"/>
       <c r="C233" s="12"/>
       <c r="D233" s="13"/>
       <c r="E233" s="13"/>
     </row>
-    <row r="234" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A234" s="12"/>
       <c r="B234" s="13"/>
       <c r="C234" s="12"/>
       <c r="D234" s="13"/>
       <c r="E234" s="13"/>
     </row>
-    <row r="235" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A235" s="12"/>
       <c r="B235" s="13"/>
       <c r="C235" s="12"/>
       <c r="D235" s="13"/>
       <c r="E235" s="13"/>
     </row>
-    <row r="236" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A236" s="12"/>
       <c r="B236" s="13"/>
       <c r="C236" s="12"/>
       <c r="D236" s="13"/>
       <c r="E236" s="13"/>
     </row>
-    <row r="237" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A237" s="12"/>
       <c r="B237" s="13"/>
       <c r="C237" s="12"/>
       <c r="D237" s="13"/>
       <c r="E237" s="13"/>
     </row>
-    <row r="238" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A238" s="12"/>
       <c r="B238" s="13"/>
       <c r="C238" s="12"/>
       <c r="D238" s="13"/>
       <c r="E238" s="13"/>
     </row>
-    <row r="239" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A239" s="12"/>
       <c r="B239" s="13"/>
       <c r="C239" s="12"/>
       <c r="D239" s="13"/>
       <c r="E239" s="13"/>
     </row>
-    <row r="240" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A240" s="12"/>
       <c r="B240" s="13"/>
       <c r="C240" s="12"/>
       <c r="D240" s="13"/>
       <c r="E240" s="13"/>
     </row>
-    <row r="241" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A241" s="12"/>
       <c r="B241" s="13"/>
       <c r="C241" s="12"/>
       <c r="D241" s="13"/>
       <c r="E241" s="13"/>
     </row>
-    <row r="242" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A242" s="12"/>
       <c r="B242" s="13"/>
       <c r="C242" s="12"/>
       <c r="D242" s="13"/>
       <c r="E242" s="13"/>
     </row>
-    <row r="243" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A243" s="12"/>
       <c r="B243" s="13"/>
       <c r="C243" s="12"/>
       <c r="D243" s="13"/>
       <c r="E243" s="13"/>
     </row>
-    <row r="244" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A244" s="12"/>
       <c r="B244" s="13"/>
       <c r="C244" s="12"/>
       <c r="D244" s="13"/>
       <c r="E244" s="13"/>
     </row>
-    <row r="245" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A245" s="12"/>
       <c r="B245" s="13"/>
       <c r="C245" s="12"/>
       <c r="D245" s="13"/>
       <c r="E245" s="13"/>
     </row>
-    <row r="246" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A246" s="12"/>
       <c r="B246" s="13"/>
       <c r="C246" s="12"/>
       <c r="D246" s="13"/>
       <c r="E246" s="13"/>
     </row>
-    <row r="247" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A247" s="12"/>
       <c r="B247" s="13"/>
       <c r="C247" s="12"/>
       <c r="D247" s="13"/>
       <c r="E247" s="13"/>
     </row>
-    <row r="248" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A248" s="12"/>
       <c r="B248" s="13"/>
       <c r="C248" s="12"/>
       <c r="D248" s="13"/>
       <c r="E248" s="13"/>
     </row>
-    <row r="249" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A249" s="12"/>
       <c r="B249" s="13"/>
       <c r="C249" s="12"/>
       <c r="D249" s="13"/>
       <c r="E249" s="13"/>
     </row>
-    <row r="250" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A250" s="12"/>
       <c r="B250" s="13"/>
       <c r="C250" s="12"/>
       <c r="D250" s="13"/>
       <c r="E250" s="13"/>
     </row>
-    <row r="251" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A251" s="12"/>
       <c r="B251" s="13"/>
       <c r="C251" s="12"/>
       <c r="D251" s="13"/>
       <c r="E251" s="13"/>
     </row>
-    <row r="252" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A252" s="12"/>
       <c r="B252" s="13"/>
       <c r="C252" s="12"/>
       <c r="D252" s="13"/>
       <c r="E252" s="13"/>
     </row>
-    <row r="253" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A253" s="12"/>
       <c r="B253" s="13"/>
       <c r="C253" s="12"/>
       <c r="D253" s="13"/>
       <c r="E253" s="13"/>
     </row>
-    <row r="254" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A254" s="12"/>
       <c r="B254" s="13"/>
       <c r="C254" s="12"/>
       <c r="D254" s="13"/>
       <c r="E254" s="13"/>
     </row>
-    <row r="255" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A255" s="12"/>
       <c r="B255" s="13"/>
       <c r="C255" s="12"/>
       <c r="D255" s="13"/>
       <c r="E255" s="13"/>
     </row>
-    <row r="256" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A256" s="12"/>
       <c r="B256" s="13"/>
       <c r="C256" s="12"/>
       <c r="D256" s="13"/>
       <c r="E256" s="13"/>
     </row>
-    <row r="257" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A257" s="12"/>
       <c r="B257" s="13"/>
       <c r="C257" s="12"/>
       <c r="D257" s="13"/>
       <c r="E257" s="13"/>
     </row>
-    <row r="258" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A258" s="12"/>
       <c r="B258" s="13"/>
       <c r="C258" s="12"/>
       <c r="D258" s="13"/>
       <c r="E258" s="13"/>
     </row>
-    <row r="259" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A259" s="12"/>
       <c r="B259" s="13"/>
       <c r="C259" s="12"/>
       <c r="D259" s="13"/>
       <c r="E259" s="13"/>
     </row>
-    <row r="260" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A260" s="12"/>
       <c r="B260" s="13"/>
       <c r="C260" s="12"/>
@@ -2931,7 +2957,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D27" r:id="rId1"/>
+    <hyperlink ref="D27" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="D28" r:id="rId2" xr:uid="{4877334E-7528-4DFA-87BA-7232CC222E39}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Se agrega el 28 Alumno al archivo
</commit_message>
<xml_diff>
--- a/Lista de Alumnos.xlsx
+++ b/Lista de Alumnos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24931"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mhect\OneDrive\Escritorio\pp12021grupo7_a2-grupo7_a2-main\Alumnos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Leonardo\Alumnos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E8CC4E3-61A2-422C-8B7B-58CB9E4E07C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9750FE42-F856-4D81-B757-57DCD39B530B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Electronica Microcontrolada" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="88">
   <si>
     <t>#</t>
   </si>
@@ -275,6 +275,15 @@
   </si>
   <si>
     <t>TerraWolf</t>
+  </si>
+  <si>
+    <t>Leonardo Gonzalez</t>
+  </si>
+  <si>
+    <t>leogb37@gmail.com</t>
+  </si>
+  <si>
+    <t>leolgonzalez</t>
   </si>
 </sst>
 </file>
@@ -782,20 +791,20 @@
   </sheetPr>
   <dimension ref="A1:E260"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.88671875" style="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="37.109375" style="15" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.5546875" style="14" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.85546875" style="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.140625" style="15" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" style="14" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="31" style="15" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="29" style="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -812,7 +821,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -829,7 +838,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>2</v>
       </c>
@@ -844,7 +853,7 @@
       </c>
       <c r="E3" s="6"/>
     </row>
-    <row r="4" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>3</v>
       </c>
@@ -861,7 +870,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>4</v>
       </c>
@@ -878,7 +887,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>5</v>
       </c>
@@ -895,7 +904,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>6</v>
       </c>
@@ -912,7 +921,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>7</v>
       </c>
@@ -929,7 +938,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>8</v>
       </c>
@@ -946,7 +955,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>9</v>
       </c>
@@ -961,7 +970,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <v>10</v>
       </c>
@@ -978,7 +987,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>11</v>
       </c>
@@ -995,7 +1004,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
         <v>12</v>
       </c>
@@ -1012,7 +1021,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
         <v>13</v>
       </c>
@@ -1029,7 +1038,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
         <v>14</v>
       </c>
@@ -1046,7 +1055,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
         <v>15</v>
       </c>
@@ -1063,7 +1072,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
         <v>16</v>
       </c>
@@ -1080,7 +1089,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <v>17</v>
       </c>
@@ -1097,7 +1106,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
         <v>18</v>
       </c>
@@ -1114,7 +1123,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
         <v>19</v>
       </c>
@@ -1131,7 +1140,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="5">
         <v>20</v>
       </c>
@@ -1148,7 +1157,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="5">
         <v>21</v>
       </c>
@@ -1165,7 +1174,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="5">
         <v>22</v>
       </c>
@@ -1182,7 +1191,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="5">
         <v>23</v>
       </c>
@@ -1199,7 +1208,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="5">
         <v>24</v>
       </c>
@@ -1216,7 +1225,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="5">
         <v>25</v>
       </c>
@@ -1233,7 +1242,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="5">
         <v>26</v>
       </c>
@@ -1250,7 +1259,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="5">
         <v>27</v>
       </c>
@@ -1267,16 +1276,24 @@
         <v>84</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="5">
         <v>28</v>
       </c>
-      <c r="B29" s="6"/>
-      <c r="C29" s="5"/>
-      <c r="D29" s="6"/>
-      <c r="E29" s="6"/>
-    </row>
-    <row r="30" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="C29" s="5">
+        <v>2</v>
+      </c>
+      <c r="D29" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="E29" s="6" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="5">
         <v>29</v>
       </c>
@@ -1285,7 +1302,7 @@
       <c r="D30" s="6"/>
       <c r="E30" s="6"/>
     </row>
-    <row r="31" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="5">
         <v>30</v>
       </c>
@@ -1294,7 +1311,7 @@
       <c r="D31" s="6"/>
       <c r="E31" s="6"/>
     </row>
-    <row r="32" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="5">
         <v>31</v>
       </c>
@@ -1303,7 +1320,7 @@
       <c r="D32" s="6"/>
       <c r="E32" s="6"/>
     </row>
-    <row r="33" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="5">
         <v>32</v>
       </c>
@@ -1312,7 +1329,7 @@
       <c r="D33" s="6"/>
       <c r="E33" s="6"/>
     </row>
-    <row r="34" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="5">
         <v>33</v>
       </c>
@@ -1321,7 +1338,7 @@
       <c r="D34" s="6"/>
       <c r="E34" s="6"/>
     </row>
-    <row r="35" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="5">
         <v>34</v>
       </c>
@@ -1330,7 +1347,7 @@
       <c r="D35" s="6"/>
       <c r="E35" s="6"/>
     </row>
-    <row r="36" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="5">
         <v>35</v>
       </c>
@@ -1339,7 +1356,7 @@
       <c r="D36" s="6"/>
       <c r="E36" s="6"/>
     </row>
-    <row r="37" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="5">
         <v>36</v>
       </c>
@@ -1348,7 +1365,7 @@
       <c r="D37" s="6"/>
       <c r="E37" s="6"/>
     </row>
-    <row r="38" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="5">
         <v>37</v>
       </c>
@@ -1357,7 +1374,7 @@
       <c r="D38" s="6"/>
       <c r="E38" s="6"/>
     </row>
-    <row r="39" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="5">
         <v>38</v>
       </c>
@@ -1366,7 +1383,7 @@
       <c r="D39" s="6"/>
       <c r="E39" s="6"/>
     </row>
-    <row r="40" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="5">
         <v>39</v>
       </c>
@@ -1375,7 +1392,7 @@
       <c r="D40" s="6"/>
       <c r="E40" s="6"/>
     </row>
-    <row r="41" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="5">
         <v>40</v>
       </c>
@@ -1384,7 +1401,7 @@
       <c r="D41" s="6"/>
       <c r="E41" s="6"/>
     </row>
-    <row r="42" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="5">
         <v>41</v>
       </c>
@@ -1393,7 +1410,7 @@
       <c r="D42" s="6"/>
       <c r="E42" s="6"/>
     </row>
-    <row r="43" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="5">
         <v>42</v>
       </c>
@@ -1402,7 +1419,7 @@
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
     </row>
-    <row r="44" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="5">
         <v>43</v>
       </c>
@@ -1411,7 +1428,7 @@
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
     </row>
-    <row r="45" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="5">
         <v>44</v>
       </c>
@@ -1420,7 +1437,7 @@
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
     </row>
-    <row r="46" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="5">
         <v>45</v>
       </c>
@@ -1429,7 +1446,7 @@
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
     </row>
-    <row r="47" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="5">
         <v>46</v>
       </c>
@@ -1438,7 +1455,7 @@
       <c r="D47" s="6"/>
       <c r="E47" s="6"/>
     </row>
-    <row r="48" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="5">
         <v>47</v>
       </c>
@@ -1447,7 +1464,7 @@
       <c r="D48" s="6"/>
       <c r="E48" s="6"/>
     </row>
-    <row r="49" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="5">
         <v>48</v>
       </c>
@@ -1456,7 +1473,7 @@
       <c r="D49" s="6"/>
       <c r="E49" s="6"/>
     </row>
-    <row r="50" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="5">
         <v>49</v>
       </c>
@@ -1465,7 +1482,7 @@
       <c r="D50" s="6"/>
       <c r="E50" s="6"/>
     </row>
-    <row r="51" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="5">
         <v>50</v>
       </c>
@@ -1474,7 +1491,7 @@
       <c r="D51" s="6"/>
       <c r="E51" s="6"/>
     </row>
-    <row r="52" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="5">
         <v>51</v>
       </c>
@@ -1483,7 +1500,7 @@
       <c r="D52" s="6"/>
       <c r="E52" s="6"/>
     </row>
-    <row r="53" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="5">
         <v>52</v>
       </c>
@@ -1492,7 +1509,7 @@
       <c r="D53" s="6"/>
       <c r="E53" s="6"/>
     </row>
-    <row r="54" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="5">
         <v>53</v>
       </c>
@@ -1501,7 +1518,7 @@
       <c r="D54" s="6"/>
       <c r="E54" s="6"/>
     </row>
-    <row r="55" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="5">
         <v>54</v>
       </c>
@@ -1510,7 +1527,7 @@
       <c r="D55" s="6"/>
       <c r="E55" s="6"/>
     </row>
-    <row r="56" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="5">
         <v>55</v>
       </c>
@@ -1519,7 +1536,7 @@
       <c r="D56" s="6"/>
       <c r="E56" s="6"/>
     </row>
-    <row r="57" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="5">
         <v>56</v>
       </c>
@@ -1528,7 +1545,7 @@
       <c r="D57" s="6"/>
       <c r="E57" s="6"/>
     </row>
-    <row r="58" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="5">
         <v>57</v>
       </c>
@@ -1537,7 +1554,7 @@
       <c r="D58" s="6"/>
       <c r="E58" s="6"/>
     </row>
-    <row r="59" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="5">
         <v>58</v>
       </c>
@@ -1546,7 +1563,7 @@
       <c r="D59" s="6"/>
       <c r="E59" s="6"/>
     </row>
-    <row r="60" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="5">
         <v>59</v>
       </c>
@@ -1555,1400 +1572,1400 @@
       <c r="D60" s="6"/>
       <c r="E60" s="6"/>
     </row>
-    <row r="61" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="12"/>
       <c r="B61" s="13"/>
       <c r="C61" s="12"/>
       <c r="D61" s="13"/>
       <c r="E61" s="13"/>
     </row>
-    <row r="62" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="12"/>
       <c r="B62" s="13"/>
       <c r="C62" s="12"/>
       <c r="D62" s="13"/>
       <c r="E62" s="13"/>
     </row>
-    <row r="63" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="12"/>
       <c r="B63" s="13"/>
       <c r="C63" s="12"/>
       <c r="D63" s="13"/>
       <c r="E63" s="13"/>
     </row>
-    <row r="64" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="12"/>
       <c r="B64" s="13"/>
       <c r="C64" s="12"/>
       <c r="D64" s="13"/>
       <c r="E64" s="13"/>
     </row>
-    <row r="65" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="12"/>
       <c r="B65" s="13"/>
       <c r="C65" s="12"/>
       <c r="D65" s="13"/>
       <c r="E65" s="13"/>
     </row>
-    <row r="66" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="12"/>
       <c r="B66" s="13"/>
       <c r="C66" s="12"/>
       <c r="D66" s="13"/>
       <c r="E66" s="13"/>
     </row>
-    <row r="67" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="12"/>
       <c r="B67" s="13"/>
       <c r="C67" s="12"/>
       <c r="D67" s="13"/>
       <c r="E67" s="13"/>
     </row>
-    <row r="68" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="12"/>
       <c r="B68" s="13"/>
       <c r="C68" s="12"/>
       <c r="D68" s="13"/>
       <c r="E68" s="13"/>
     </row>
-    <row r="69" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="12"/>
       <c r="B69" s="13"/>
       <c r="C69" s="12"/>
       <c r="D69" s="13"/>
       <c r="E69" s="13"/>
     </row>
-    <row r="70" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="12"/>
       <c r="B70" s="13"/>
       <c r="C70" s="12"/>
       <c r="D70" s="13"/>
       <c r="E70" s="13"/>
     </row>
-    <row r="71" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="12"/>
       <c r="B71" s="13"/>
       <c r="C71" s="12"/>
       <c r="D71" s="13"/>
       <c r="E71" s="13"/>
     </row>
-    <row r="72" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="12"/>
       <c r="B72" s="13"/>
       <c r="C72" s="12"/>
       <c r="D72" s="13"/>
       <c r="E72" s="13"/>
     </row>
-    <row r="73" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="12"/>
       <c r="B73" s="13"/>
       <c r="C73" s="12"/>
       <c r="D73" s="13"/>
       <c r="E73" s="13"/>
     </row>
-    <row r="74" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="12"/>
       <c r="B74" s="13"/>
       <c r="C74" s="12"/>
       <c r="D74" s="13"/>
       <c r="E74" s="13"/>
     </row>
-    <row r="75" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="12"/>
       <c r="B75" s="13"/>
       <c r="C75" s="12"/>
       <c r="D75" s="13"/>
       <c r="E75" s="13"/>
     </row>
-    <row r="76" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="12"/>
       <c r="B76" s="13"/>
       <c r="C76" s="12"/>
       <c r="D76" s="13"/>
       <c r="E76" s="13"/>
     </row>
-    <row r="77" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="12"/>
       <c r="B77" s="13"/>
       <c r="C77" s="12"/>
       <c r="D77" s="13"/>
       <c r="E77" s="13"/>
     </row>
-    <row r="78" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="12"/>
       <c r="B78" s="13"/>
       <c r="C78" s="12"/>
       <c r="D78" s="13"/>
       <c r="E78" s="13"/>
     </row>
-    <row r="79" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="12"/>
       <c r="B79" s="13"/>
       <c r="C79" s="12"/>
       <c r="D79" s="13"/>
       <c r="E79" s="13"/>
     </row>
-    <row r="80" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="12"/>
       <c r="B80" s="13"/>
       <c r="C80" s="12"/>
       <c r="D80" s="13"/>
       <c r="E80" s="13"/>
     </row>
-    <row r="81" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="12"/>
       <c r="B81" s="13"/>
       <c r="C81" s="12"/>
       <c r="D81" s="13"/>
       <c r="E81" s="13"/>
     </row>
-    <row r="82" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="12"/>
       <c r="B82" s="13"/>
       <c r="C82" s="12"/>
       <c r="D82" s="13"/>
       <c r="E82" s="13"/>
     </row>
-    <row r="83" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="12"/>
       <c r="B83" s="13"/>
       <c r="C83" s="12"/>
       <c r="D83" s="13"/>
       <c r="E83" s="13"/>
     </row>
-    <row r="84" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="12"/>
       <c r="B84" s="13"/>
       <c r="C84" s="12"/>
       <c r="D84" s="13"/>
       <c r="E84" s="13"/>
     </row>
-    <row r="85" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="12"/>
       <c r="B85" s="13"/>
       <c r="C85" s="12"/>
       <c r="D85" s="13"/>
       <c r="E85" s="13"/>
     </row>
-    <row r="86" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="12"/>
       <c r="B86" s="13"/>
       <c r="C86" s="12"/>
       <c r="D86" s="13"/>
       <c r="E86" s="13"/>
     </row>
-    <row r="87" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="12"/>
       <c r="B87" s="13"/>
       <c r="C87" s="12"/>
       <c r="D87" s="13"/>
       <c r="E87" s="13"/>
     </row>
-    <row r="88" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="12"/>
       <c r="B88" s="13"/>
       <c r="C88" s="12"/>
       <c r="D88" s="13"/>
       <c r="E88" s="13"/>
     </row>
-    <row r="89" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="12"/>
       <c r="B89" s="13"/>
       <c r="C89" s="12"/>
       <c r="D89" s="13"/>
       <c r="E89" s="13"/>
     </row>
-    <row r="90" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="12"/>
       <c r="B90" s="13"/>
       <c r="C90" s="12"/>
       <c r="D90" s="13"/>
       <c r="E90" s="13"/>
     </row>
-    <row r="91" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="12"/>
       <c r="B91" s="13"/>
       <c r="C91" s="12"/>
       <c r="D91" s="13"/>
       <c r="E91" s="13"/>
     </row>
-    <row r="92" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="12"/>
       <c r="B92" s="13"/>
       <c r="C92" s="12"/>
       <c r="D92" s="13"/>
       <c r="E92" s="13"/>
     </row>
-    <row r="93" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="12"/>
       <c r="B93" s="13"/>
       <c r="C93" s="12"/>
       <c r="D93" s="13"/>
       <c r="E93" s="13"/>
     </row>
-    <row r="94" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="12"/>
       <c r="B94" s="13"/>
       <c r="C94" s="12"/>
       <c r="D94" s="13"/>
       <c r="E94" s="13"/>
     </row>
-    <row r="95" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="12"/>
       <c r="B95" s="13"/>
       <c r="C95" s="12"/>
       <c r="D95" s="13"/>
       <c r="E95" s="13"/>
     </row>
-    <row r="96" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="12"/>
       <c r="B96" s="13"/>
       <c r="C96" s="12"/>
       <c r="D96" s="13"/>
       <c r="E96" s="13"/>
     </row>
-    <row r="97" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="12"/>
       <c r="B97" s="13"/>
       <c r="C97" s="12"/>
       <c r="D97" s="13"/>
       <c r="E97" s="13"/>
     </row>
-    <row r="98" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="12"/>
       <c r="B98" s="13"/>
       <c r="C98" s="12"/>
       <c r="D98" s="13"/>
       <c r="E98" s="13"/>
     </row>
-    <row r="99" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="12"/>
       <c r="B99" s="13"/>
       <c r="C99" s="12"/>
       <c r="D99" s="13"/>
       <c r="E99" s="13"/>
     </row>
-    <row r="100" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="12"/>
       <c r="B100" s="13"/>
       <c r="C100" s="12"/>
       <c r="D100" s="13"/>
       <c r="E100" s="13"/>
     </row>
-    <row r="101" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="12"/>
       <c r="B101" s="13"/>
       <c r="C101" s="12"/>
       <c r="D101" s="13"/>
       <c r="E101" s="13"/>
     </row>
-    <row r="102" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="12"/>
       <c r="B102" s="13"/>
       <c r="C102" s="12"/>
       <c r="D102" s="13"/>
       <c r="E102" s="13"/>
     </row>
-    <row r="103" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" s="12"/>
       <c r="B103" s="13"/>
       <c r="C103" s="12"/>
       <c r="D103" s="13"/>
       <c r="E103" s="13"/>
     </row>
-    <row r="104" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="12"/>
       <c r="B104" s="13"/>
       <c r="C104" s="12"/>
       <c r="D104" s="13"/>
       <c r="E104" s="13"/>
     </row>
-    <row r="105" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" s="12"/>
       <c r="B105" s="13"/>
       <c r="C105" s="12"/>
       <c r="D105" s="13"/>
       <c r="E105" s="13"/>
     </row>
-    <row r="106" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="12"/>
       <c r="B106" s="13"/>
       <c r="C106" s="12"/>
       <c r="D106" s="13"/>
       <c r="E106" s="13"/>
     </row>
-    <row r="107" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" s="12"/>
       <c r="B107" s="13"/>
       <c r="C107" s="12"/>
       <c r="D107" s="13"/>
       <c r="E107" s="13"/>
     </row>
-    <row r="108" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" s="12"/>
       <c r="B108" s="13"/>
       <c r="C108" s="12"/>
       <c r="D108" s="13"/>
       <c r="E108" s="13"/>
     </row>
-    <row r="109" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" s="12"/>
       <c r="B109" s="13"/>
       <c r="C109" s="12"/>
       <c r="D109" s="13"/>
       <c r="E109" s="13"/>
     </row>
-    <row r="110" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" s="12"/>
       <c r="B110" s="13"/>
       <c r="C110" s="12"/>
       <c r="D110" s="13"/>
       <c r="E110" s="13"/>
     </row>
-    <row r="111" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" s="12"/>
       <c r="B111" s="13"/>
       <c r="C111" s="12"/>
       <c r="D111" s="13"/>
       <c r="E111" s="13"/>
     </row>
-    <row r="112" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" s="12"/>
       <c r="B112" s="13"/>
       <c r="C112" s="12"/>
       <c r="D112" s="13"/>
       <c r="E112" s="13"/>
     </row>
-    <row r="113" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" s="12"/>
       <c r="B113" s="13"/>
       <c r="C113" s="12"/>
       <c r="D113" s="13"/>
       <c r="E113" s="13"/>
     </row>
-    <row r="114" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A114" s="12"/>
       <c r="B114" s="13"/>
       <c r="C114" s="12"/>
       <c r="D114" s="13"/>
       <c r="E114" s="13"/>
     </row>
-    <row r="115" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A115" s="12"/>
       <c r="B115" s="13"/>
       <c r="C115" s="12"/>
       <c r="D115" s="13"/>
       <c r="E115" s="13"/>
     </row>
-    <row r="116" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A116" s="12"/>
       <c r="B116" s="13"/>
       <c r="C116" s="12"/>
       <c r="D116" s="13"/>
       <c r="E116" s="13"/>
     </row>
-    <row r="117" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A117" s="12"/>
       <c r="B117" s="13"/>
       <c r="C117" s="12"/>
       <c r="D117" s="13"/>
       <c r="E117" s="13"/>
     </row>
-    <row r="118" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A118" s="12"/>
       <c r="B118" s="13"/>
       <c r="C118" s="12"/>
       <c r="D118" s="13"/>
       <c r="E118" s="13"/>
     </row>
-    <row r="119" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A119" s="12"/>
       <c r="B119" s="13"/>
       <c r="C119" s="12"/>
       <c r="D119" s="13"/>
       <c r="E119" s="13"/>
     </row>
-    <row r="120" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A120" s="12"/>
       <c r="B120" s="13"/>
       <c r="C120" s="12"/>
       <c r="D120" s="13"/>
       <c r="E120" s="13"/>
     </row>
-    <row r="121" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A121" s="12"/>
       <c r="B121" s="13"/>
       <c r="C121" s="12"/>
       <c r="D121" s="13"/>
       <c r="E121" s="13"/>
     </row>
-    <row r="122" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A122" s="12"/>
       <c r="B122" s="13"/>
       <c r="C122" s="12"/>
       <c r="D122" s="13"/>
       <c r="E122" s="13"/>
     </row>
-    <row r="123" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A123" s="12"/>
       <c r="B123" s="13"/>
       <c r="C123" s="12"/>
       <c r="D123" s="13"/>
       <c r="E123" s="13"/>
     </row>
-    <row r="124" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A124" s="12"/>
       <c r="B124" s="13"/>
       <c r="C124" s="12"/>
       <c r="D124" s="13"/>
       <c r="E124" s="13"/>
     </row>
-    <row r="125" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A125" s="12"/>
       <c r="B125" s="13"/>
       <c r="C125" s="12"/>
       <c r="D125" s="13"/>
       <c r="E125" s="13"/>
     </row>
-    <row r="126" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A126" s="12"/>
       <c r="B126" s="13"/>
       <c r="C126" s="12"/>
       <c r="D126" s="13"/>
       <c r="E126" s="13"/>
     </row>
-    <row r="127" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A127" s="12"/>
       <c r="B127" s="13"/>
       <c r="C127" s="12"/>
       <c r="D127" s="13"/>
       <c r="E127" s="13"/>
     </row>
-    <row r="128" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A128" s="12"/>
       <c r="B128" s="13"/>
       <c r="C128" s="12"/>
       <c r="D128" s="13"/>
       <c r="E128" s="13"/>
     </row>
-    <row r="129" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A129" s="12"/>
       <c r="B129" s="13"/>
       <c r="C129" s="12"/>
       <c r="D129" s="13"/>
       <c r="E129" s="13"/>
     </row>
-    <row r="130" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A130" s="12"/>
       <c r="B130" s="13"/>
       <c r="C130" s="12"/>
       <c r="D130" s="13"/>
       <c r="E130" s="13"/>
     </row>
-    <row r="131" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A131" s="12"/>
       <c r="B131" s="13"/>
       <c r="C131" s="12"/>
       <c r="D131" s="13"/>
       <c r="E131" s="13"/>
     </row>
-    <row r="132" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A132" s="12"/>
       <c r="B132" s="13"/>
       <c r="C132" s="12"/>
       <c r="D132" s="13"/>
       <c r="E132" s="13"/>
     </row>
-    <row r="133" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A133" s="12"/>
       <c r="B133" s="13"/>
       <c r="C133" s="12"/>
       <c r="D133" s="13"/>
       <c r="E133" s="13"/>
     </row>
-    <row r="134" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A134" s="12"/>
       <c r="B134" s="13"/>
       <c r="C134" s="12"/>
       <c r="D134" s="13"/>
       <c r="E134" s="13"/>
     </row>
-    <row r="135" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A135" s="12"/>
       <c r="B135" s="13"/>
       <c r="C135" s="12"/>
       <c r="D135" s="13"/>
       <c r="E135" s="13"/>
     </row>
-    <row r="136" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A136" s="12"/>
       <c r="B136" s="13"/>
       <c r="C136" s="12"/>
       <c r="D136" s="13"/>
       <c r="E136" s="13"/>
     </row>
-    <row r="137" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A137" s="12"/>
       <c r="B137" s="13"/>
       <c r="C137" s="12"/>
       <c r="D137" s="13"/>
       <c r="E137" s="13"/>
     </row>
-    <row r="138" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A138" s="12"/>
       <c r="B138" s="13"/>
       <c r="C138" s="12"/>
       <c r="D138" s="13"/>
       <c r="E138" s="13"/>
     </row>
-    <row r="139" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A139" s="12"/>
       <c r="B139" s="13"/>
       <c r="C139" s="12"/>
       <c r="D139" s="13"/>
       <c r="E139" s="13"/>
     </row>
-    <row r="140" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A140" s="12"/>
       <c r="B140" s="13"/>
       <c r="C140" s="12"/>
       <c r="D140" s="13"/>
       <c r="E140" s="13"/>
     </row>
-    <row r="141" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A141" s="12"/>
       <c r="B141" s="13"/>
       <c r="C141" s="12"/>
       <c r="D141" s="13"/>
       <c r="E141" s="13"/>
     </row>
-    <row r="142" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A142" s="12"/>
       <c r="B142" s="13"/>
       <c r="C142" s="12"/>
       <c r="D142" s="13"/>
       <c r="E142" s="13"/>
     </row>
-    <row r="143" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A143" s="12"/>
       <c r="B143" s="13"/>
       <c r="C143" s="12"/>
       <c r="D143" s="13"/>
       <c r="E143" s="13"/>
     </row>
-    <row r="144" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A144" s="12"/>
       <c r="B144" s="13"/>
       <c r="C144" s="12"/>
       <c r="D144" s="13"/>
       <c r="E144" s="13"/>
     </row>
-    <row r="145" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A145" s="12"/>
       <c r="B145" s="13"/>
       <c r="C145" s="12"/>
       <c r="D145" s="13"/>
       <c r="E145" s="13"/>
     </row>
-    <row r="146" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A146" s="12"/>
       <c r="B146" s="13"/>
       <c r="C146" s="12"/>
       <c r="D146" s="13"/>
       <c r="E146" s="13"/>
     </row>
-    <row r="147" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A147" s="12"/>
       <c r="B147" s="13"/>
       <c r="C147" s="12"/>
       <c r="D147" s="13"/>
       <c r="E147" s="13"/>
     </row>
-    <row r="148" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A148" s="12"/>
       <c r="B148" s="13"/>
       <c r="C148" s="12"/>
       <c r="D148" s="13"/>
       <c r="E148" s="13"/>
     </row>
-    <row r="149" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A149" s="12"/>
       <c r="B149" s="13"/>
       <c r="C149" s="12"/>
       <c r="D149" s="13"/>
       <c r="E149" s="13"/>
     </row>
-    <row r="150" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A150" s="12"/>
       <c r="B150" s="13"/>
       <c r="C150" s="12"/>
       <c r="D150" s="13"/>
       <c r="E150" s="13"/>
     </row>
-    <row r="151" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A151" s="12"/>
       <c r="B151" s="13"/>
       <c r="C151" s="12"/>
       <c r="D151" s="13"/>
       <c r="E151" s="13"/>
     </row>
-    <row r="152" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A152" s="12"/>
       <c r="B152" s="13"/>
       <c r="C152" s="12"/>
       <c r="D152" s="13"/>
       <c r="E152" s="13"/>
     </row>
-    <row r="153" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A153" s="12"/>
       <c r="B153" s="13"/>
       <c r="C153" s="12"/>
       <c r="D153" s="13"/>
       <c r="E153" s="13"/>
     </row>
-    <row r="154" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A154" s="12"/>
       <c r="B154" s="13"/>
       <c r="C154" s="12"/>
       <c r="D154" s="13"/>
       <c r="E154" s="13"/>
     </row>
-    <row r="155" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A155" s="12"/>
       <c r="B155" s="13"/>
       <c r="C155" s="12"/>
       <c r="D155" s="13"/>
       <c r="E155" s="13"/>
     </row>
-    <row r="156" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A156" s="12"/>
       <c r="B156" s="13"/>
       <c r="C156" s="12"/>
       <c r="D156" s="13"/>
       <c r="E156" s="13"/>
     </row>
-    <row r="157" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A157" s="12"/>
       <c r="B157" s="13"/>
       <c r="C157" s="12"/>
       <c r="D157" s="13"/>
       <c r="E157" s="13"/>
     </row>
-    <row r="158" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A158" s="12"/>
       <c r="B158" s="13"/>
       <c r="C158" s="12"/>
       <c r="D158" s="13"/>
       <c r="E158" s="13"/>
     </row>
-    <row r="159" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A159" s="12"/>
       <c r="B159" s="13"/>
       <c r="C159" s="12"/>
       <c r="D159" s="13"/>
       <c r="E159" s="13"/>
     </row>
-    <row r="160" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A160" s="12"/>
       <c r="B160" s="13"/>
       <c r="C160" s="12"/>
       <c r="D160" s="13"/>
       <c r="E160" s="13"/>
     </row>
-    <row r="161" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A161" s="12"/>
       <c r="B161" s="13"/>
       <c r="C161" s="12"/>
       <c r="D161" s="13"/>
       <c r="E161" s="13"/>
     </row>
-    <row r="162" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A162" s="12"/>
       <c r="B162" s="13"/>
       <c r="C162" s="12"/>
       <c r="D162" s="13"/>
       <c r="E162" s="13"/>
     </row>
-    <row r="163" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A163" s="12"/>
       <c r="B163" s="13"/>
       <c r="C163" s="12"/>
       <c r="D163" s="13"/>
       <c r="E163" s="13"/>
     </row>
-    <row r="164" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A164" s="12"/>
       <c r="B164" s="13"/>
       <c r="C164" s="12"/>
       <c r="D164" s="13"/>
       <c r="E164" s="13"/>
     </row>
-    <row r="165" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A165" s="12"/>
       <c r="B165" s="13"/>
       <c r="C165" s="12"/>
       <c r="D165" s="13"/>
       <c r="E165" s="13"/>
     </row>
-    <row r="166" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A166" s="12"/>
       <c r="B166" s="13"/>
       <c r="C166" s="12"/>
       <c r="D166" s="13"/>
       <c r="E166" s="13"/>
     </row>
-    <row r="167" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A167" s="12"/>
       <c r="B167" s="13"/>
       <c r="C167" s="12"/>
       <c r="D167" s="13"/>
       <c r="E167" s="13"/>
     </row>
-    <row r="168" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A168" s="12"/>
       <c r="B168" s="13"/>
       <c r="C168" s="12"/>
       <c r="D168" s="13"/>
       <c r="E168" s="13"/>
     </row>
-    <row r="169" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A169" s="12"/>
       <c r="B169" s="13"/>
       <c r="C169" s="12"/>
       <c r="D169" s="13"/>
       <c r="E169" s="13"/>
     </row>
-    <row r="170" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A170" s="12"/>
       <c r="B170" s="13"/>
       <c r="C170" s="12"/>
       <c r="D170" s="13"/>
       <c r="E170" s="13"/>
     </row>
-    <row r="171" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A171" s="12"/>
       <c r="B171" s="13"/>
       <c r="C171" s="12"/>
       <c r="D171" s="13"/>
       <c r="E171" s="13"/>
     </row>
-    <row r="172" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A172" s="12"/>
       <c r="B172" s="13"/>
       <c r="C172" s="12"/>
       <c r="D172" s="13"/>
       <c r="E172" s="13"/>
     </row>
-    <row r="173" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A173" s="12"/>
       <c r="B173" s="13"/>
       <c r="C173" s="12"/>
       <c r="D173" s="13"/>
       <c r="E173" s="13"/>
     </row>
-    <row r="174" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A174" s="12"/>
       <c r="B174" s="13"/>
       <c r="C174" s="12"/>
       <c r="D174" s="13"/>
       <c r="E174" s="13"/>
     </row>
-    <row r="175" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A175" s="12"/>
       <c r="B175" s="13"/>
       <c r="C175" s="12"/>
       <c r="D175" s="13"/>
       <c r="E175" s="13"/>
     </row>
-    <row r="176" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A176" s="12"/>
       <c r="B176" s="13"/>
       <c r="C176" s="12"/>
       <c r="D176" s="13"/>
       <c r="E176" s="13"/>
     </row>
-    <row r="177" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A177" s="12"/>
       <c r="B177" s="13"/>
       <c r="C177" s="12"/>
       <c r="D177" s="13"/>
       <c r="E177" s="13"/>
     </row>
-    <row r="178" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A178" s="12"/>
       <c r="B178" s="13"/>
       <c r="C178" s="12"/>
       <c r="D178" s="13"/>
       <c r="E178" s="13"/>
     </row>
-    <row r="179" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A179" s="12"/>
       <c r="B179" s="13"/>
       <c r="C179" s="12"/>
       <c r="D179" s="13"/>
       <c r="E179" s="13"/>
     </row>
-    <row r="180" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A180" s="12"/>
       <c r="B180" s="13"/>
       <c r="C180" s="12"/>
       <c r="D180" s="13"/>
       <c r="E180" s="13"/>
     </row>
-    <row r="181" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A181" s="12"/>
       <c r="B181" s="13"/>
       <c r="C181" s="12"/>
       <c r="D181" s="13"/>
       <c r="E181" s="13"/>
     </row>
-    <row r="182" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A182" s="12"/>
       <c r="B182" s="13"/>
       <c r="C182" s="12"/>
       <c r="D182" s="13"/>
       <c r="E182" s="13"/>
     </row>
-    <row r="183" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A183" s="12"/>
       <c r="B183" s="13"/>
       <c r="C183" s="12"/>
       <c r="D183" s="13"/>
       <c r="E183" s="13"/>
     </row>
-    <row r="184" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A184" s="12"/>
       <c r="B184" s="13"/>
       <c r="C184" s="12"/>
       <c r="D184" s="13"/>
       <c r="E184" s="13"/>
     </row>
-    <row r="185" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A185" s="12"/>
       <c r="B185" s="13"/>
       <c r="C185" s="12"/>
       <c r="D185" s="13"/>
       <c r="E185" s="13"/>
     </row>
-    <row r="186" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A186" s="12"/>
       <c r="B186" s="13"/>
       <c r="C186" s="12"/>
       <c r="D186" s="13"/>
       <c r="E186" s="13"/>
     </row>
-    <row r="187" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A187" s="12"/>
       <c r="B187" s="13"/>
       <c r="C187" s="12"/>
       <c r="D187" s="13"/>
       <c r="E187" s="13"/>
     </row>
-    <row r="188" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A188" s="12"/>
       <c r="B188" s="13"/>
       <c r="C188" s="12"/>
       <c r="D188" s="13"/>
       <c r="E188" s="13"/>
     </row>
-    <row r="189" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A189" s="12"/>
       <c r="B189" s="13"/>
       <c r="C189" s="12"/>
       <c r="D189" s="13"/>
       <c r="E189" s="13"/>
     </row>
-    <row r="190" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A190" s="12"/>
       <c r="B190" s="13"/>
       <c r="C190" s="12"/>
       <c r="D190" s="13"/>
       <c r="E190" s="13"/>
     </row>
-    <row r="191" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A191" s="12"/>
       <c r="B191" s="13"/>
       <c r="C191" s="12"/>
       <c r="D191" s="13"/>
       <c r="E191" s="13"/>
     </row>
-    <row r="192" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A192" s="12"/>
       <c r="B192" s="13"/>
       <c r="C192" s="12"/>
       <c r="D192" s="13"/>
       <c r="E192" s="13"/>
     </row>
-    <row r="193" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A193" s="12"/>
       <c r="B193" s="13"/>
       <c r="C193" s="12"/>
       <c r="D193" s="13"/>
       <c r="E193" s="13"/>
     </row>
-    <row r="194" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A194" s="12"/>
       <c r="B194" s="13"/>
       <c r="C194" s="12"/>
       <c r="D194" s="13"/>
       <c r="E194" s="13"/>
     </row>
-    <row r="195" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A195" s="12"/>
       <c r="B195" s="13"/>
       <c r="C195" s="12"/>
       <c r="D195" s="13"/>
       <c r="E195" s="13"/>
     </row>
-    <row r="196" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A196" s="12"/>
       <c r="B196" s="13"/>
       <c r="C196" s="12"/>
       <c r="D196" s="13"/>
       <c r="E196" s="13"/>
     </row>
-    <row r="197" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A197" s="12"/>
       <c r="B197" s="13"/>
       <c r="C197" s="12"/>
       <c r="D197" s="13"/>
       <c r="E197" s="13"/>
     </row>
-    <row r="198" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A198" s="12"/>
       <c r="B198" s="13"/>
       <c r="C198" s="12"/>
       <c r="D198" s="13"/>
       <c r="E198" s="13"/>
     </row>
-    <row r="199" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A199" s="12"/>
       <c r="B199" s="13"/>
       <c r="C199" s="12"/>
       <c r="D199" s="13"/>
       <c r="E199" s="13"/>
     </row>
-    <row r="200" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A200" s="12"/>
       <c r="B200" s="13"/>
       <c r="C200" s="12"/>
       <c r="D200" s="13"/>
       <c r="E200" s="13"/>
     </row>
-    <row r="201" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A201" s="12"/>
       <c r="B201" s="13"/>
       <c r="C201" s="12"/>
       <c r="D201" s="13"/>
       <c r="E201" s="13"/>
     </row>
-    <row r="202" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A202" s="12"/>
       <c r="B202" s="13"/>
       <c r="C202" s="12"/>
       <c r="D202" s="13"/>
       <c r="E202" s="13"/>
     </row>
-    <row r="203" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A203" s="12"/>
       <c r="B203" s="13"/>
       <c r="C203" s="12"/>
       <c r="D203" s="13"/>
       <c r="E203" s="13"/>
     </row>
-    <row r="204" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A204" s="12"/>
       <c r="B204" s="13"/>
       <c r="C204" s="12"/>
       <c r="D204" s="13"/>
       <c r="E204" s="13"/>
     </row>
-    <row r="205" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A205" s="12"/>
       <c r="B205" s="13"/>
       <c r="C205" s="12"/>
       <c r="D205" s="13"/>
       <c r="E205" s="13"/>
     </row>
-    <row r="206" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A206" s="12"/>
       <c r="B206" s="13"/>
       <c r="C206" s="12"/>
       <c r="D206" s="13"/>
       <c r="E206" s="13"/>
     </row>
-    <row r="207" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A207" s="12"/>
       <c r="B207" s="13"/>
       <c r="C207" s="12"/>
       <c r="D207" s="13"/>
       <c r="E207" s="13"/>
     </row>
-    <row r="208" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A208" s="12"/>
       <c r="B208" s="13"/>
       <c r="C208" s="12"/>
       <c r="D208" s="13"/>
       <c r="E208" s="13"/>
     </row>
-    <row r="209" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A209" s="12"/>
       <c r="B209" s="13"/>
       <c r="C209" s="12"/>
       <c r="D209" s="13"/>
       <c r="E209" s="13"/>
     </row>
-    <row r="210" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A210" s="12"/>
       <c r="B210" s="13"/>
       <c r="C210" s="12"/>
       <c r="D210" s="13"/>
       <c r="E210" s="13"/>
     </row>
-    <row r="211" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A211" s="12"/>
       <c r="B211" s="13"/>
       <c r="C211" s="12"/>
       <c r="D211" s="13"/>
       <c r="E211" s="13"/>
     </row>
-    <row r="212" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A212" s="12"/>
       <c r="B212" s="13"/>
       <c r="C212" s="12"/>
       <c r="D212" s="13"/>
       <c r="E212" s="13"/>
     </row>
-    <row r="213" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A213" s="12"/>
       <c r="B213" s="13"/>
       <c r="C213" s="12"/>
       <c r="D213" s="13"/>
       <c r="E213" s="13"/>
     </row>
-    <row r="214" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A214" s="12"/>
       <c r="B214" s="13"/>
       <c r="C214" s="12"/>
       <c r="D214" s="13"/>
       <c r="E214" s="13"/>
     </row>
-    <row r="215" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A215" s="12"/>
       <c r="B215" s="13"/>
       <c r="C215" s="12"/>
       <c r="D215" s="13"/>
       <c r="E215" s="13"/>
     </row>
-    <row r="216" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A216" s="12"/>
       <c r="B216" s="13"/>
       <c r="C216" s="12"/>
       <c r="D216" s="13"/>
       <c r="E216" s="13"/>
     </row>
-    <row r="217" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A217" s="12"/>
       <c r="B217" s="13"/>
       <c r="C217" s="12"/>
       <c r="D217" s="13"/>
       <c r="E217" s="13"/>
     </row>
-    <row r="218" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A218" s="12"/>
       <c r="B218" s="13"/>
       <c r="C218" s="12"/>
       <c r="D218" s="13"/>
       <c r="E218" s="13"/>
     </row>
-    <row r="219" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A219" s="12"/>
       <c r="B219" s="13"/>
       <c r="C219" s="12"/>
       <c r="D219" s="13"/>
       <c r="E219" s="13"/>
     </row>
-    <row r="220" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A220" s="12"/>
       <c r="B220" s="13"/>
       <c r="C220" s="12"/>
       <c r="D220" s="13"/>
       <c r="E220" s="13"/>
     </row>
-    <row r="221" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A221" s="12"/>
       <c r="B221" s="13"/>
       <c r="C221" s="12"/>
       <c r="D221" s="13"/>
       <c r="E221" s="13"/>
     </row>
-    <row r="222" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A222" s="12"/>
       <c r="B222" s="13"/>
       <c r="C222" s="12"/>
       <c r="D222" s="13"/>
       <c r="E222" s="13"/>
     </row>
-    <row r="223" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A223" s="12"/>
       <c r="B223" s="13"/>
       <c r="C223" s="12"/>
       <c r="D223" s="13"/>
       <c r="E223" s="13"/>
     </row>
-    <row r="224" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A224" s="12"/>
       <c r="B224" s="13"/>
       <c r="C224" s="12"/>
       <c r="D224" s="13"/>
       <c r="E224" s="13"/>
     </row>
-    <row r="225" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A225" s="12"/>
       <c r="B225" s="13"/>
       <c r="C225" s="12"/>
       <c r="D225" s="13"/>
       <c r="E225" s="13"/>
     </row>
-    <row r="226" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A226" s="12"/>
       <c r="B226" s="13"/>
       <c r="C226" s="12"/>
       <c r="D226" s="13"/>
       <c r="E226" s="13"/>
     </row>
-    <row r="227" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A227" s="12"/>
       <c r="B227" s="13"/>
       <c r="C227" s="12"/>
       <c r="D227" s="13"/>
       <c r="E227" s="13"/>
     </row>
-    <row r="228" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A228" s="12"/>
       <c r="B228" s="13"/>
       <c r="C228" s="12"/>
       <c r="D228" s="13"/>
       <c r="E228" s="13"/>
     </row>
-    <row r="229" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A229" s="12"/>
       <c r="B229" s="13"/>
       <c r="C229" s="12"/>
       <c r="D229" s="13"/>
       <c r="E229" s="13"/>
     </row>
-    <row r="230" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A230" s="12"/>
       <c r="B230" s="13"/>
       <c r="C230" s="12"/>
       <c r="D230" s="13"/>
       <c r="E230" s="13"/>
     </row>
-    <row r="231" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A231" s="12"/>
       <c r="B231" s="13"/>
       <c r="C231" s="12"/>
       <c r="D231" s="13"/>
       <c r="E231" s="13"/>
     </row>
-    <row r="232" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A232" s="12"/>
       <c r="B232" s="13"/>
       <c r="C232" s="12"/>
       <c r="D232" s="13"/>
       <c r="E232" s="13"/>
     </row>
-    <row r="233" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A233" s="12"/>
       <c r="B233" s="13"/>
       <c r="C233" s="12"/>
       <c r="D233" s="13"/>
       <c r="E233" s="13"/>
     </row>
-    <row r="234" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A234" s="12"/>
       <c r="B234" s="13"/>
       <c r="C234" s="12"/>
       <c r="D234" s="13"/>
       <c r="E234" s="13"/>
     </row>
-    <row r="235" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A235" s="12"/>
       <c r="B235" s="13"/>
       <c r="C235" s="12"/>
       <c r="D235" s="13"/>
       <c r="E235" s="13"/>
     </row>
-    <row r="236" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A236" s="12"/>
       <c r="B236" s="13"/>
       <c r="C236" s="12"/>
       <c r="D236" s="13"/>
       <c r="E236" s="13"/>
     </row>
-    <row r="237" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A237" s="12"/>
       <c r="B237" s="13"/>
       <c r="C237" s="12"/>
       <c r="D237" s="13"/>
       <c r="E237" s="13"/>
     </row>
-    <row r="238" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A238" s="12"/>
       <c r="B238" s="13"/>
       <c r="C238" s="12"/>
       <c r="D238" s="13"/>
       <c r="E238" s="13"/>
     </row>
-    <row r="239" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A239" s="12"/>
       <c r="B239" s="13"/>
       <c r="C239" s="12"/>
       <c r="D239" s="13"/>
       <c r="E239" s="13"/>
     </row>
-    <row r="240" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A240" s="12"/>
       <c r="B240" s="13"/>
       <c r="C240" s="12"/>
       <c r="D240" s="13"/>
       <c r="E240" s="13"/>
     </row>
-    <row r="241" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A241" s="12"/>
       <c r="B241" s="13"/>
       <c r="C241" s="12"/>
       <c r="D241" s="13"/>
       <c r="E241" s="13"/>
     </row>
-    <row r="242" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A242" s="12"/>
       <c r="B242" s="13"/>
       <c r="C242" s="12"/>
       <c r="D242" s="13"/>
       <c r="E242" s="13"/>
     </row>
-    <row r="243" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A243" s="12"/>
       <c r="B243" s="13"/>
       <c r="C243" s="12"/>
       <c r="D243" s="13"/>
       <c r="E243" s="13"/>
     </row>
-    <row r="244" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A244" s="12"/>
       <c r="B244" s="13"/>
       <c r="C244" s="12"/>
       <c r="D244" s="13"/>
       <c r="E244" s="13"/>
     </row>
-    <row r="245" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A245" s="12"/>
       <c r="B245" s="13"/>
       <c r="C245" s="12"/>
       <c r="D245" s="13"/>
       <c r="E245" s="13"/>
     </row>
-    <row r="246" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A246" s="12"/>
       <c r="B246" s="13"/>
       <c r="C246" s="12"/>
       <c r="D246" s="13"/>
       <c r="E246" s="13"/>
     </row>
-    <row r="247" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A247" s="12"/>
       <c r="B247" s="13"/>
       <c r="C247" s="12"/>
       <c r="D247" s="13"/>
       <c r="E247" s="13"/>
     </row>
-    <row r="248" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A248" s="12"/>
       <c r="B248" s="13"/>
       <c r="C248" s="12"/>
       <c r="D248" s="13"/>
       <c r="E248" s="13"/>
     </row>
-    <row r="249" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A249" s="12"/>
       <c r="B249" s="13"/>
       <c r="C249" s="12"/>
       <c r="D249" s="13"/>
       <c r="E249" s="13"/>
     </row>
-    <row r="250" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A250" s="12"/>
       <c r="B250" s="13"/>
       <c r="C250" s="12"/>
       <c r="D250" s="13"/>
       <c r="E250" s="13"/>
     </row>
-    <row r="251" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A251" s="12"/>
       <c r="B251" s="13"/>
       <c r="C251" s="12"/>
       <c r="D251" s="13"/>
       <c r="E251" s="13"/>
     </row>
-    <row r="252" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A252" s="12"/>
       <c r="B252" s="13"/>
       <c r="C252" s="12"/>
       <c r="D252" s="13"/>
       <c r="E252" s="13"/>
     </row>
-    <row r="253" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A253" s="12"/>
       <c r="B253" s="13"/>
       <c r="C253" s="12"/>
       <c r="D253" s="13"/>
       <c r="E253" s="13"/>
     </row>
-    <row r="254" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A254" s="12"/>
       <c r="B254" s="13"/>
       <c r="C254" s="12"/>
       <c r="D254" s="13"/>
       <c r="E254" s="13"/>
     </row>
-    <row r="255" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A255" s="12"/>
       <c r="B255" s="13"/>
       <c r="C255" s="12"/>
       <c r="D255" s="13"/>
       <c r="E255" s="13"/>
     </row>
-    <row r="256" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A256" s="12"/>
       <c r="B256" s="13"/>
       <c r="C256" s="12"/>
       <c r="D256" s="13"/>
       <c r="E256" s="13"/>
     </row>
-    <row r="257" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A257" s="12"/>
       <c r="B257" s="13"/>
       <c r="C257" s="12"/>
       <c r="D257" s="13"/>
       <c r="E257" s="13"/>
     </row>
-    <row r="258" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="258" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A258" s="12"/>
       <c r="B258" s="13"/>
       <c r="C258" s="12"/>
       <c r="D258" s="13"/>
       <c r="E258" s="13"/>
     </row>
-    <row r="259" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="259" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A259" s="12"/>
       <c r="B259" s="13"/>
       <c r="C259" s="12"/>
       <c r="D259" s="13"/>
       <c r="E259" s="13"/>
     </row>
-    <row r="260" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="260" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A260" s="12"/>
       <c r="B260" s="13"/>
       <c r="C260" s="12"/>
@@ -2959,6 +2976,7 @@
   <hyperlinks>
     <hyperlink ref="D27" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
     <hyperlink ref="D28" r:id="rId2" xr:uid="{4877334E-7528-4DFA-87BA-7232CC222E39}"/>
+    <hyperlink ref="D29" r:id="rId3" xr:uid="{BD98EB24-72D1-47EA-9C38-88A632EFC407}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Se agrega el 29 Alumno al archivo
</commit_message>
<xml_diff>
--- a/Lista de Alumnos.xlsx
+++ b/Lista de Alumnos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25330"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Leonardo\Alumnos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mhect\OneDrive\Escritorio\pp12021grupo7_a2-grupo7_a2-main\Alumnos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9750FE42-F856-4D81-B757-57DCD39B530B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EB75262-340B-4510-8E68-B93EF4B66A5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Electronica Microcontrolada" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="91">
   <si>
     <t>#</t>
   </si>
@@ -284,6 +284,15 @@
   </si>
   <si>
     <t>leolgonzalez</t>
+  </si>
+  <si>
+    <t>Marina Soledad Ramos</t>
+  </si>
+  <si>
+    <t>marinaramos1118@gmail.com</t>
+  </si>
+  <si>
+    <t>MarinaSR11</t>
   </si>
 </sst>
 </file>
@@ -791,20 +800,20 @@
   </sheetPr>
   <dimension ref="A1:E260"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.85546875" style="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="37.140625" style="15" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.5703125" style="14" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.88671875" style="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.109375" style="15" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5546875" style="14" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="31" style="15" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="29" style="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -821,7 +830,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -838,7 +847,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5">
         <v>2</v>
       </c>
@@ -853,7 +862,7 @@
       </c>
       <c r="E3" s="6"/>
     </row>
-    <row r="4" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5">
         <v>3</v>
       </c>
@@ -870,7 +879,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="5">
         <v>4</v>
       </c>
@@ -887,7 +896,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="5">
         <v>5</v>
       </c>
@@ -904,7 +913,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="5">
         <v>6</v>
       </c>
@@ -921,7 +930,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5">
         <v>7</v>
       </c>
@@ -938,7 +947,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="5">
         <v>8</v>
       </c>
@@ -955,7 +964,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="5">
         <v>9</v>
       </c>
@@ -970,7 +979,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="5">
         <v>10</v>
       </c>
@@ -987,7 +996,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="5">
         <v>11</v>
       </c>
@@ -1004,7 +1013,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="5">
         <v>12</v>
       </c>
@@ -1021,7 +1030,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="5">
         <v>13</v>
       </c>
@@ -1038,7 +1047,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="5">
         <v>14</v>
       </c>
@@ -1055,7 +1064,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="5">
         <v>15</v>
       </c>
@@ -1072,7 +1081,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="5">
         <v>16</v>
       </c>
@@ -1089,7 +1098,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="5">
         <v>17</v>
       </c>
@@ -1106,7 +1115,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="5">
         <v>18</v>
       </c>
@@ -1123,7 +1132,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="5">
         <v>19</v>
       </c>
@@ -1140,7 +1149,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="5">
         <v>20</v>
       </c>
@@ -1157,7 +1166,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="5">
         <v>21</v>
       </c>
@@ -1174,7 +1183,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="5">
         <v>22</v>
       </c>
@@ -1191,7 +1200,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="5">
         <v>23</v>
       </c>
@@ -1208,7 +1217,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="5">
         <v>24</v>
       </c>
@@ -1225,7 +1234,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="5">
         <v>25</v>
       </c>
@@ -1242,7 +1251,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="5">
         <v>26</v>
       </c>
@@ -1259,7 +1268,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="5">
         <v>27</v>
       </c>
@@ -1276,7 +1285,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="5">
         <v>28</v>
       </c>
@@ -1293,16 +1302,24 @@
         <v>87</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="5">
         <v>29</v>
       </c>
-      <c r="B30" s="6"/>
-      <c r="C30" s="5"/>
-      <c r="D30" s="6"/>
-      <c r="E30" s="6"/>
-    </row>
-    <row r="31" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="C30" s="5">
+        <v>1</v>
+      </c>
+      <c r="D30" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="5">
         <v>30</v>
       </c>
@@ -1311,7 +1328,7 @@
       <c r="D31" s="6"/>
       <c r="E31" s="6"/>
     </row>
-    <row r="32" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="5">
         <v>31</v>
       </c>
@@ -1320,7 +1337,7 @@
       <c r="D32" s="6"/>
       <c r="E32" s="6"/>
     </row>
-    <row r="33" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="5">
         <v>32</v>
       </c>
@@ -1329,7 +1346,7 @@
       <c r="D33" s="6"/>
       <c r="E33" s="6"/>
     </row>
-    <row r="34" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="5">
         <v>33</v>
       </c>
@@ -1338,7 +1355,7 @@
       <c r="D34" s="6"/>
       <c r="E34" s="6"/>
     </row>
-    <row r="35" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="5">
         <v>34</v>
       </c>
@@ -1347,7 +1364,7 @@
       <c r="D35" s="6"/>
       <c r="E35" s="6"/>
     </row>
-    <row r="36" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="5">
         <v>35</v>
       </c>
@@ -1356,7 +1373,7 @@
       <c r="D36" s="6"/>
       <c r="E36" s="6"/>
     </row>
-    <row r="37" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="5">
         <v>36</v>
       </c>
@@ -1365,7 +1382,7 @@
       <c r="D37" s="6"/>
       <c r="E37" s="6"/>
     </row>
-    <row r="38" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="5">
         <v>37</v>
       </c>
@@ -1374,7 +1391,7 @@
       <c r="D38" s="6"/>
       <c r="E38" s="6"/>
     </row>
-    <row r="39" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="5">
         <v>38</v>
       </c>
@@ -1383,7 +1400,7 @@
       <c r="D39" s="6"/>
       <c r="E39" s="6"/>
     </row>
-    <row r="40" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="5">
         <v>39</v>
       </c>
@@ -1392,7 +1409,7 @@
       <c r="D40" s="6"/>
       <c r="E40" s="6"/>
     </row>
-    <row r="41" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="5">
         <v>40</v>
       </c>
@@ -1401,7 +1418,7 @@
       <c r="D41" s="6"/>
       <c r="E41" s="6"/>
     </row>
-    <row r="42" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="5">
         <v>41</v>
       </c>
@@ -1410,7 +1427,7 @@
       <c r="D42" s="6"/>
       <c r="E42" s="6"/>
     </row>
-    <row r="43" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="5">
         <v>42</v>
       </c>
@@ -1419,7 +1436,7 @@
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
     </row>
-    <row r="44" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="5">
         <v>43</v>
       </c>
@@ -1428,7 +1445,7 @@
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
     </row>
-    <row r="45" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="5">
         <v>44</v>
       </c>
@@ -1437,7 +1454,7 @@
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
     </row>
-    <row r="46" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="5">
         <v>45</v>
       </c>
@@ -1446,7 +1463,7 @@
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
     </row>
-    <row r="47" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="5">
         <v>46</v>
       </c>
@@ -1455,7 +1472,7 @@
       <c r="D47" s="6"/>
       <c r="E47" s="6"/>
     </row>
-    <row r="48" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="5">
         <v>47</v>
       </c>
@@ -1464,7 +1481,7 @@
       <c r="D48" s="6"/>
       <c r="E48" s="6"/>
     </row>
-    <row r="49" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="5">
         <v>48</v>
       </c>
@@ -1473,7 +1490,7 @@
       <c r="D49" s="6"/>
       <c r="E49" s="6"/>
     </row>
-    <row r="50" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="5">
         <v>49</v>
       </c>
@@ -1482,7 +1499,7 @@
       <c r="D50" s="6"/>
       <c r="E50" s="6"/>
     </row>
-    <row r="51" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="5">
         <v>50</v>
       </c>
@@ -1491,7 +1508,7 @@
       <c r="D51" s="6"/>
       <c r="E51" s="6"/>
     </row>
-    <row r="52" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="5">
         <v>51</v>
       </c>
@@ -1500,7 +1517,7 @@
       <c r="D52" s="6"/>
       <c r="E52" s="6"/>
     </row>
-    <row r="53" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="5">
         <v>52</v>
       </c>
@@ -1509,7 +1526,7 @@
       <c r="D53" s="6"/>
       <c r="E53" s="6"/>
     </row>
-    <row r="54" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="5">
         <v>53</v>
       </c>
@@ -1518,7 +1535,7 @@
       <c r="D54" s="6"/>
       <c r="E54" s="6"/>
     </row>
-    <row r="55" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="5">
         <v>54</v>
       </c>
@@ -1527,7 +1544,7 @@
       <c r="D55" s="6"/>
       <c r="E55" s="6"/>
     </row>
-    <row r="56" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="5">
         <v>55</v>
       </c>
@@ -1536,7 +1553,7 @@
       <c r="D56" s="6"/>
       <c r="E56" s="6"/>
     </row>
-    <row r="57" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="5">
         <v>56</v>
       </c>
@@ -1545,7 +1562,7 @@
       <c r="D57" s="6"/>
       <c r="E57" s="6"/>
     </row>
-    <row r="58" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="5">
         <v>57</v>
       </c>
@@ -1554,7 +1571,7 @@
       <c r="D58" s="6"/>
       <c r="E58" s="6"/>
     </row>
-    <row r="59" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="5">
         <v>58</v>
       </c>
@@ -1563,7 +1580,7 @@
       <c r="D59" s="6"/>
       <c r="E59" s="6"/>
     </row>
-    <row r="60" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" s="5">
         <v>59</v>
       </c>
@@ -1572,1400 +1589,1400 @@
       <c r="D60" s="6"/>
       <c r="E60" s="6"/>
     </row>
-    <row r="61" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" s="12"/>
       <c r="B61" s="13"/>
       <c r="C61" s="12"/>
       <c r="D61" s="13"/>
       <c r="E61" s="13"/>
     </row>
-    <row r="62" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" s="12"/>
       <c r="B62" s="13"/>
       <c r="C62" s="12"/>
       <c r="D62" s="13"/>
       <c r="E62" s="13"/>
     </row>
-    <row r="63" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" s="12"/>
       <c r="B63" s="13"/>
       <c r="C63" s="12"/>
       <c r="D63" s="13"/>
       <c r="E63" s="13"/>
     </row>
-    <row r="64" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" s="12"/>
       <c r="B64" s="13"/>
       <c r="C64" s="12"/>
       <c r="D64" s="13"/>
       <c r="E64" s="13"/>
     </row>
-    <row r="65" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A65" s="12"/>
       <c r="B65" s="13"/>
       <c r="C65" s="12"/>
       <c r="D65" s="13"/>
       <c r="E65" s="13"/>
     </row>
-    <row r="66" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A66" s="12"/>
       <c r="B66" s="13"/>
       <c r="C66" s="12"/>
       <c r="D66" s="13"/>
       <c r="E66" s="13"/>
     </row>
-    <row r="67" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67" s="12"/>
       <c r="B67" s="13"/>
       <c r="C67" s="12"/>
       <c r="D67" s="13"/>
       <c r="E67" s="13"/>
     </row>
-    <row r="68" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" s="12"/>
       <c r="B68" s="13"/>
       <c r="C68" s="12"/>
       <c r="D68" s="13"/>
       <c r="E68" s="13"/>
     </row>
-    <row r="69" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69" s="12"/>
       <c r="B69" s="13"/>
       <c r="C69" s="12"/>
       <c r="D69" s="13"/>
       <c r="E69" s="13"/>
     </row>
-    <row r="70" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A70" s="12"/>
       <c r="B70" s="13"/>
       <c r="C70" s="12"/>
       <c r="D70" s="13"/>
       <c r="E70" s="13"/>
     </row>
-    <row r="71" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A71" s="12"/>
       <c r="B71" s="13"/>
       <c r="C71" s="12"/>
       <c r="D71" s="13"/>
       <c r="E71" s="13"/>
     </row>
-    <row r="72" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72" s="12"/>
       <c r="B72" s="13"/>
       <c r="C72" s="12"/>
       <c r="D72" s="13"/>
       <c r="E72" s="13"/>
     </row>
-    <row r="73" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A73" s="12"/>
       <c r="B73" s="13"/>
       <c r="C73" s="12"/>
       <c r="D73" s="13"/>
       <c r="E73" s="13"/>
     </row>
-    <row r="74" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A74" s="12"/>
       <c r="B74" s="13"/>
       <c r="C74" s="12"/>
       <c r="D74" s="13"/>
       <c r="E74" s="13"/>
     </row>
-    <row r="75" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A75" s="12"/>
       <c r="B75" s="13"/>
       <c r="C75" s="12"/>
       <c r="D75" s="13"/>
       <c r="E75" s="13"/>
     </row>
-    <row r="76" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A76" s="12"/>
       <c r="B76" s="13"/>
       <c r="C76" s="12"/>
       <c r="D76" s="13"/>
       <c r="E76" s="13"/>
     </row>
-    <row r="77" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A77" s="12"/>
       <c r="B77" s="13"/>
       <c r="C77" s="12"/>
       <c r="D77" s="13"/>
       <c r="E77" s="13"/>
     </row>
-    <row r="78" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A78" s="12"/>
       <c r="B78" s="13"/>
       <c r="C78" s="12"/>
       <c r="D78" s="13"/>
       <c r="E78" s="13"/>
     </row>
-    <row r="79" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A79" s="12"/>
       <c r="B79" s="13"/>
       <c r="C79" s="12"/>
       <c r="D79" s="13"/>
       <c r="E79" s="13"/>
     </row>
-    <row r="80" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A80" s="12"/>
       <c r="B80" s="13"/>
       <c r="C80" s="12"/>
       <c r="D80" s="13"/>
       <c r="E80" s="13"/>
     </row>
-    <row r="81" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A81" s="12"/>
       <c r="B81" s="13"/>
       <c r="C81" s="12"/>
       <c r="D81" s="13"/>
       <c r="E81" s="13"/>
     </row>
-    <row r="82" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A82" s="12"/>
       <c r="B82" s="13"/>
       <c r="C82" s="12"/>
       <c r="D82" s="13"/>
       <c r="E82" s="13"/>
     </row>
-    <row r="83" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A83" s="12"/>
       <c r="B83" s="13"/>
       <c r="C83" s="12"/>
       <c r="D83" s="13"/>
       <c r="E83" s="13"/>
     </row>
-    <row r="84" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A84" s="12"/>
       <c r="B84" s="13"/>
       <c r="C84" s="12"/>
       <c r="D84" s="13"/>
       <c r="E84" s="13"/>
     </row>
-    <row r="85" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A85" s="12"/>
       <c r="B85" s="13"/>
       <c r="C85" s="12"/>
       <c r="D85" s="13"/>
       <c r="E85" s="13"/>
     </row>
-    <row r="86" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A86" s="12"/>
       <c r="B86" s="13"/>
       <c r="C86" s="12"/>
       <c r="D86" s="13"/>
       <c r="E86" s="13"/>
     </row>
-    <row r="87" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A87" s="12"/>
       <c r="B87" s="13"/>
       <c r="C87" s="12"/>
       <c r="D87" s="13"/>
       <c r="E87" s="13"/>
     </row>
-    <row r="88" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A88" s="12"/>
       <c r="B88" s="13"/>
       <c r="C88" s="12"/>
       <c r="D88" s="13"/>
       <c r="E88" s="13"/>
     </row>
-    <row r="89" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A89" s="12"/>
       <c r="B89" s="13"/>
       <c r="C89" s="12"/>
       <c r="D89" s="13"/>
       <c r="E89" s="13"/>
     </row>
-    <row r="90" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A90" s="12"/>
       <c r="B90" s="13"/>
       <c r="C90" s="12"/>
       <c r="D90" s="13"/>
       <c r="E90" s="13"/>
     </row>
-    <row r="91" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A91" s="12"/>
       <c r="B91" s="13"/>
       <c r="C91" s="12"/>
       <c r="D91" s="13"/>
       <c r="E91" s="13"/>
     </row>
-    <row r="92" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A92" s="12"/>
       <c r="B92" s="13"/>
       <c r="C92" s="12"/>
       <c r="D92" s="13"/>
       <c r="E92" s="13"/>
     </row>
-    <row r="93" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A93" s="12"/>
       <c r="B93" s="13"/>
       <c r="C93" s="12"/>
       <c r="D93" s="13"/>
       <c r="E93" s="13"/>
     </row>
-    <row r="94" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A94" s="12"/>
       <c r="B94" s="13"/>
       <c r="C94" s="12"/>
       <c r="D94" s="13"/>
       <c r="E94" s="13"/>
     </row>
-    <row r="95" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A95" s="12"/>
       <c r="B95" s="13"/>
       <c r="C95" s="12"/>
       <c r="D95" s="13"/>
       <c r="E95" s="13"/>
     </row>
-    <row r="96" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A96" s="12"/>
       <c r="B96" s="13"/>
       <c r="C96" s="12"/>
       <c r="D96" s="13"/>
       <c r="E96" s="13"/>
     </row>
-    <row r="97" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A97" s="12"/>
       <c r="B97" s="13"/>
       <c r="C97" s="12"/>
       <c r="D97" s="13"/>
       <c r="E97" s="13"/>
     </row>
-    <row r="98" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A98" s="12"/>
       <c r="B98" s="13"/>
       <c r="C98" s="12"/>
       <c r="D98" s="13"/>
       <c r="E98" s="13"/>
     </row>
-    <row r="99" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A99" s="12"/>
       <c r="B99" s="13"/>
       <c r="C99" s="12"/>
       <c r="D99" s="13"/>
       <c r="E99" s="13"/>
     </row>
-    <row r="100" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A100" s="12"/>
       <c r="B100" s="13"/>
       <c r="C100" s="12"/>
       <c r="D100" s="13"/>
       <c r="E100" s="13"/>
     </row>
-    <row r="101" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A101" s="12"/>
       <c r="B101" s="13"/>
       <c r="C101" s="12"/>
       <c r="D101" s="13"/>
       <c r="E101" s="13"/>
     </row>
-    <row r="102" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A102" s="12"/>
       <c r="B102" s="13"/>
       <c r="C102" s="12"/>
       <c r="D102" s="13"/>
       <c r="E102" s="13"/>
     </row>
-    <row r="103" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A103" s="12"/>
       <c r="B103" s="13"/>
       <c r="C103" s="12"/>
       <c r="D103" s="13"/>
       <c r="E103" s="13"/>
     </row>
-    <row r="104" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A104" s="12"/>
       <c r="B104" s="13"/>
       <c r="C104" s="12"/>
       <c r="D104" s="13"/>
       <c r="E104" s="13"/>
     </row>
-    <row r="105" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A105" s="12"/>
       <c r="B105" s="13"/>
       <c r="C105" s="12"/>
       <c r="D105" s="13"/>
       <c r="E105" s="13"/>
     </row>
-    <row r="106" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A106" s="12"/>
       <c r="B106" s="13"/>
       <c r="C106" s="12"/>
       <c r="D106" s="13"/>
       <c r="E106" s="13"/>
     </row>
-    <row r="107" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A107" s="12"/>
       <c r="B107" s="13"/>
       <c r="C107" s="12"/>
       <c r="D107" s="13"/>
       <c r="E107" s="13"/>
     </row>
-    <row r="108" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A108" s="12"/>
       <c r="B108" s="13"/>
       <c r="C108" s="12"/>
       <c r="D108" s="13"/>
       <c r="E108" s="13"/>
     </row>
-    <row r="109" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A109" s="12"/>
       <c r="B109" s="13"/>
       <c r="C109" s="12"/>
       <c r="D109" s="13"/>
       <c r="E109" s="13"/>
     </row>
-    <row r="110" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A110" s="12"/>
       <c r="B110" s="13"/>
       <c r="C110" s="12"/>
       <c r="D110" s="13"/>
       <c r="E110" s="13"/>
     </row>
-    <row r="111" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A111" s="12"/>
       <c r="B111" s="13"/>
       <c r="C111" s="12"/>
       <c r="D111" s="13"/>
       <c r="E111" s="13"/>
     </row>
-    <row r="112" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A112" s="12"/>
       <c r="B112" s="13"/>
       <c r="C112" s="12"/>
       <c r="D112" s="13"/>
       <c r="E112" s="13"/>
     </row>
-    <row r="113" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A113" s="12"/>
       <c r="B113" s="13"/>
       <c r="C113" s="12"/>
       <c r="D113" s="13"/>
       <c r="E113" s="13"/>
     </row>
-    <row r="114" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A114" s="12"/>
       <c r="B114" s="13"/>
       <c r="C114" s="12"/>
       <c r="D114" s="13"/>
       <c r="E114" s="13"/>
     </row>
-    <row r="115" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A115" s="12"/>
       <c r="B115" s="13"/>
       <c r="C115" s="12"/>
       <c r="D115" s="13"/>
       <c r="E115" s="13"/>
     </row>
-    <row r="116" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A116" s="12"/>
       <c r="B116" s="13"/>
       <c r="C116" s="12"/>
       <c r="D116" s="13"/>
       <c r="E116" s="13"/>
     </row>
-    <row r="117" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A117" s="12"/>
       <c r="B117" s="13"/>
       <c r="C117" s="12"/>
       <c r="D117" s="13"/>
       <c r="E117" s="13"/>
     </row>
-    <row r="118" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A118" s="12"/>
       <c r="B118" s="13"/>
       <c r="C118" s="12"/>
       <c r="D118" s="13"/>
       <c r="E118" s="13"/>
     </row>
-    <row r="119" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A119" s="12"/>
       <c r="B119" s="13"/>
       <c r="C119" s="12"/>
       <c r="D119" s="13"/>
       <c r="E119" s="13"/>
     </row>
-    <row r="120" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A120" s="12"/>
       <c r="B120" s="13"/>
       <c r="C120" s="12"/>
       <c r="D120" s="13"/>
       <c r="E120" s="13"/>
     </row>
-    <row r="121" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A121" s="12"/>
       <c r="B121" s="13"/>
       <c r="C121" s="12"/>
       <c r="D121" s="13"/>
       <c r="E121" s="13"/>
     </row>
-    <row r="122" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A122" s="12"/>
       <c r="B122" s="13"/>
       <c r="C122" s="12"/>
       <c r="D122" s="13"/>
       <c r="E122" s="13"/>
     </row>
-    <row r="123" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A123" s="12"/>
       <c r="B123" s="13"/>
       <c r="C123" s="12"/>
       <c r="D123" s="13"/>
       <c r="E123" s="13"/>
     </row>
-    <row r="124" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A124" s="12"/>
       <c r="B124" s="13"/>
       <c r="C124" s="12"/>
       <c r="D124" s="13"/>
       <c r="E124" s="13"/>
     </row>
-    <row r="125" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A125" s="12"/>
       <c r="B125" s="13"/>
       <c r="C125" s="12"/>
       <c r="D125" s="13"/>
       <c r="E125" s="13"/>
     </row>
-    <row r="126" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A126" s="12"/>
       <c r="B126" s="13"/>
       <c r="C126" s="12"/>
       <c r="D126" s="13"/>
       <c r="E126" s="13"/>
     </row>
-    <row r="127" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A127" s="12"/>
       <c r="B127" s="13"/>
       <c r="C127" s="12"/>
       <c r="D127" s="13"/>
       <c r="E127" s="13"/>
     </row>
-    <row r="128" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A128" s="12"/>
       <c r="B128" s="13"/>
       <c r="C128" s="12"/>
       <c r="D128" s="13"/>
       <c r="E128" s="13"/>
     </row>
-    <row r="129" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A129" s="12"/>
       <c r="B129" s="13"/>
       <c r="C129" s="12"/>
       <c r="D129" s="13"/>
       <c r="E129" s="13"/>
     </row>
-    <row r="130" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A130" s="12"/>
       <c r="B130" s="13"/>
       <c r="C130" s="12"/>
       <c r="D130" s="13"/>
       <c r="E130" s="13"/>
     </row>
-    <row r="131" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A131" s="12"/>
       <c r="B131" s="13"/>
       <c r="C131" s="12"/>
       <c r="D131" s="13"/>
       <c r="E131" s="13"/>
     </row>
-    <row r="132" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A132" s="12"/>
       <c r="B132" s="13"/>
       <c r="C132" s="12"/>
       <c r="D132" s="13"/>
       <c r="E132" s="13"/>
     </row>
-    <row r="133" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A133" s="12"/>
       <c r="B133" s="13"/>
       <c r="C133" s="12"/>
       <c r="D133" s="13"/>
       <c r="E133" s="13"/>
     </row>
-    <row r="134" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A134" s="12"/>
       <c r="B134" s="13"/>
       <c r="C134" s="12"/>
       <c r="D134" s="13"/>
       <c r="E134" s="13"/>
     </row>
-    <row r="135" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A135" s="12"/>
       <c r="B135" s="13"/>
       <c r="C135" s="12"/>
       <c r="D135" s="13"/>
       <c r="E135" s="13"/>
     </row>
-    <row r="136" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A136" s="12"/>
       <c r="B136" s="13"/>
       <c r="C136" s="12"/>
       <c r="D136" s="13"/>
       <c r="E136" s="13"/>
     </row>
-    <row r="137" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A137" s="12"/>
       <c r="B137" s="13"/>
       <c r="C137" s="12"/>
       <c r="D137" s="13"/>
       <c r="E137" s="13"/>
     </row>
-    <row r="138" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A138" s="12"/>
       <c r="B138" s="13"/>
       <c r="C138" s="12"/>
       <c r="D138" s="13"/>
       <c r="E138" s="13"/>
     </row>
-    <row r="139" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A139" s="12"/>
       <c r="B139" s="13"/>
       <c r="C139" s="12"/>
       <c r="D139" s="13"/>
       <c r="E139" s="13"/>
     </row>
-    <row r="140" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A140" s="12"/>
       <c r="B140" s="13"/>
       <c r="C140" s="12"/>
       <c r="D140" s="13"/>
       <c r="E140" s="13"/>
     </row>
-    <row r="141" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A141" s="12"/>
       <c r="B141" s="13"/>
       <c r="C141" s="12"/>
       <c r="D141" s="13"/>
       <c r="E141" s="13"/>
     </row>
-    <row r="142" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A142" s="12"/>
       <c r="B142" s="13"/>
       <c r="C142" s="12"/>
       <c r="D142" s="13"/>
       <c r="E142" s="13"/>
     </row>
-    <row r="143" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A143" s="12"/>
       <c r="B143" s="13"/>
       <c r="C143" s="12"/>
       <c r="D143" s="13"/>
       <c r="E143" s="13"/>
     </row>
-    <row r="144" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A144" s="12"/>
       <c r="B144" s="13"/>
       <c r="C144" s="12"/>
       <c r="D144" s="13"/>
       <c r="E144" s="13"/>
     </row>
-    <row r="145" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A145" s="12"/>
       <c r="B145" s="13"/>
       <c r="C145" s="12"/>
       <c r="D145" s="13"/>
       <c r="E145" s="13"/>
     </row>
-    <row r="146" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A146" s="12"/>
       <c r="B146" s="13"/>
       <c r="C146" s="12"/>
       <c r="D146" s="13"/>
       <c r="E146" s="13"/>
     </row>
-    <row r="147" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A147" s="12"/>
       <c r="B147" s="13"/>
       <c r="C147" s="12"/>
       <c r="D147" s="13"/>
       <c r="E147" s="13"/>
     </row>
-    <row r="148" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A148" s="12"/>
       <c r="B148" s="13"/>
       <c r="C148" s="12"/>
       <c r="D148" s="13"/>
       <c r="E148" s="13"/>
     </row>
-    <row r="149" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A149" s="12"/>
       <c r="B149" s="13"/>
       <c r="C149" s="12"/>
       <c r="D149" s="13"/>
       <c r="E149" s="13"/>
     </row>
-    <row r="150" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A150" s="12"/>
       <c r="B150" s="13"/>
       <c r="C150" s="12"/>
       <c r="D150" s="13"/>
       <c r="E150" s="13"/>
     </row>
-    <row r="151" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A151" s="12"/>
       <c r="B151" s="13"/>
       <c r="C151" s="12"/>
       <c r="D151" s="13"/>
       <c r="E151" s="13"/>
     </row>
-    <row r="152" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A152" s="12"/>
       <c r="B152" s="13"/>
       <c r="C152" s="12"/>
       <c r="D152" s="13"/>
       <c r="E152" s="13"/>
     </row>
-    <row r="153" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A153" s="12"/>
       <c r="B153" s="13"/>
       <c r="C153" s="12"/>
       <c r="D153" s="13"/>
       <c r="E153" s="13"/>
     </row>
-    <row r="154" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A154" s="12"/>
       <c r="B154" s="13"/>
       <c r="C154" s="12"/>
       <c r="D154" s="13"/>
       <c r="E154" s="13"/>
     </row>
-    <row r="155" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A155" s="12"/>
       <c r="B155" s="13"/>
       <c r="C155" s="12"/>
       <c r="D155" s="13"/>
       <c r="E155" s="13"/>
     </row>
-    <row r="156" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A156" s="12"/>
       <c r="B156" s="13"/>
       <c r="C156" s="12"/>
       <c r="D156" s="13"/>
       <c r="E156" s="13"/>
     </row>
-    <row r="157" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A157" s="12"/>
       <c r="B157" s="13"/>
       <c r="C157" s="12"/>
       <c r="D157" s="13"/>
       <c r="E157" s="13"/>
     </row>
-    <row r="158" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A158" s="12"/>
       <c r="B158" s="13"/>
       <c r="C158" s="12"/>
       <c r="D158" s="13"/>
       <c r="E158" s="13"/>
     </row>
-    <row r="159" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A159" s="12"/>
       <c r="B159" s="13"/>
       <c r="C159" s="12"/>
       <c r="D159" s="13"/>
       <c r="E159" s="13"/>
     </row>
-    <row r="160" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A160" s="12"/>
       <c r="B160" s="13"/>
       <c r="C160" s="12"/>
       <c r="D160" s="13"/>
       <c r="E160" s="13"/>
     </row>
-    <row r="161" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A161" s="12"/>
       <c r="B161" s="13"/>
       <c r="C161" s="12"/>
       <c r="D161" s="13"/>
       <c r="E161" s="13"/>
     </row>
-    <row r="162" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A162" s="12"/>
       <c r="B162" s="13"/>
       <c r="C162" s="12"/>
       <c r="D162" s="13"/>
       <c r="E162" s="13"/>
     </row>
-    <row r="163" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A163" s="12"/>
       <c r="B163" s="13"/>
       <c r="C163" s="12"/>
       <c r="D163" s="13"/>
       <c r="E163" s="13"/>
     </row>
-    <row r="164" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A164" s="12"/>
       <c r="B164" s="13"/>
       <c r="C164" s="12"/>
       <c r="D164" s="13"/>
       <c r="E164" s="13"/>
     </row>
-    <row r="165" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A165" s="12"/>
       <c r="B165" s="13"/>
       <c r="C165" s="12"/>
       <c r="D165" s="13"/>
       <c r="E165" s="13"/>
     </row>
-    <row r="166" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A166" s="12"/>
       <c r="B166" s="13"/>
       <c r="C166" s="12"/>
       <c r="D166" s="13"/>
       <c r="E166" s="13"/>
     </row>
-    <row r="167" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A167" s="12"/>
       <c r="B167" s="13"/>
       <c r="C167" s="12"/>
       <c r="D167" s="13"/>
       <c r="E167" s="13"/>
     </row>
-    <row r="168" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A168" s="12"/>
       <c r="B168" s="13"/>
       <c r="C168" s="12"/>
       <c r="D168" s="13"/>
       <c r="E168" s="13"/>
     </row>
-    <row r="169" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A169" s="12"/>
       <c r="B169" s="13"/>
       <c r="C169" s="12"/>
       <c r="D169" s="13"/>
       <c r="E169" s="13"/>
     </row>
-    <row r="170" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A170" s="12"/>
       <c r="B170" s="13"/>
       <c r="C170" s="12"/>
       <c r="D170" s="13"/>
       <c r="E170" s="13"/>
     </row>
-    <row r="171" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A171" s="12"/>
       <c r="B171" s="13"/>
       <c r="C171" s="12"/>
       <c r="D171" s="13"/>
       <c r="E171" s="13"/>
     </row>
-    <row r="172" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A172" s="12"/>
       <c r="B172" s="13"/>
       <c r="C172" s="12"/>
       <c r="D172" s="13"/>
       <c r="E172" s="13"/>
     </row>
-    <row r="173" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A173" s="12"/>
       <c r="B173" s="13"/>
       <c r="C173" s="12"/>
       <c r="D173" s="13"/>
       <c r="E173" s="13"/>
     </row>
-    <row r="174" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A174" s="12"/>
       <c r="B174" s="13"/>
       <c r="C174" s="12"/>
       <c r="D174" s="13"/>
       <c r="E174" s="13"/>
     </row>
-    <row r="175" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A175" s="12"/>
       <c r="B175" s="13"/>
       <c r="C175" s="12"/>
       <c r="D175" s="13"/>
       <c r="E175" s="13"/>
     </row>
-    <row r="176" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A176" s="12"/>
       <c r="B176" s="13"/>
       <c r="C176" s="12"/>
       <c r="D176" s="13"/>
       <c r="E176" s="13"/>
     </row>
-    <row r="177" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A177" s="12"/>
       <c r="B177" s="13"/>
       <c r="C177" s="12"/>
       <c r="D177" s="13"/>
       <c r="E177" s="13"/>
     </row>
-    <row r="178" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A178" s="12"/>
       <c r="B178" s="13"/>
       <c r="C178" s="12"/>
       <c r="D178" s="13"/>
       <c r="E178" s="13"/>
     </row>
-    <row r="179" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A179" s="12"/>
       <c r="B179" s="13"/>
       <c r="C179" s="12"/>
       <c r="D179" s="13"/>
       <c r="E179" s="13"/>
     </row>
-    <row r="180" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A180" s="12"/>
       <c r="B180" s="13"/>
       <c r="C180" s="12"/>
       <c r="D180" s="13"/>
       <c r="E180" s="13"/>
     </row>
-    <row r="181" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A181" s="12"/>
       <c r="B181" s="13"/>
       <c r="C181" s="12"/>
       <c r="D181" s="13"/>
       <c r="E181" s="13"/>
     </row>
-    <row r="182" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A182" s="12"/>
       <c r="B182" s="13"/>
       <c r="C182" s="12"/>
       <c r="D182" s="13"/>
       <c r="E182" s="13"/>
     </row>
-    <row r="183" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A183" s="12"/>
       <c r="B183" s="13"/>
       <c r="C183" s="12"/>
       <c r="D183" s="13"/>
       <c r="E183" s="13"/>
     </row>
-    <row r="184" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A184" s="12"/>
       <c r="B184" s="13"/>
       <c r="C184" s="12"/>
       <c r="D184" s="13"/>
       <c r="E184" s="13"/>
     </row>
-    <row r="185" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A185" s="12"/>
       <c r="B185" s="13"/>
       <c r="C185" s="12"/>
       <c r="D185" s="13"/>
       <c r="E185" s="13"/>
     </row>
-    <row r="186" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A186" s="12"/>
       <c r="B186" s="13"/>
       <c r="C186" s="12"/>
       <c r="D186" s="13"/>
       <c r="E186" s="13"/>
     </row>
-    <row r="187" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A187" s="12"/>
       <c r="B187" s="13"/>
       <c r="C187" s="12"/>
       <c r="D187" s="13"/>
       <c r="E187" s="13"/>
     </row>
-    <row r="188" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A188" s="12"/>
       <c r="B188" s="13"/>
       <c r="C188" s="12"/>
       <c r="D188" s="13"/>
       <c r="E188" s="13"/>
     </row>
-    <row r="189" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A189" s="12"/>
       <c r="B189" s="13"/>
       <c r="C189" s="12"/>
       <c r="D189" s="13"/>
       <c r="E189" s="13"/>
     </row>
-    <row r="190" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A190" s="12"/>
       <c r="B190" s="13"/>
       <c r="C190" s="12"/>
       <c r="D190" s="13"/>
       <c r="E190" s="13"/>
     </row>
-    <row r="191" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A191" s="12"/>
       <c r="B191" s="13"/>
       <c r="C191" s="12"/>
       <c r="D191" s="13"/>
       <c r="E191" s="13"/>
     </row>
-    <row r="192" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A192" s="12"/>
       <c r="B192" s="13"/>
       <c r="C192" s="12"/>
       <c r="D192" s="13"/>
       <c r="E192" s="13"/>
     </row>
-    <row r="193" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A193" s="12"/>
       <c r="B193" s="13"/>
       <c r="C193" s="12"/>
       <c r="D193" s="13"/>
       <c r="E193" s="13"/>
     </row>
-    <row r="194" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A194" s="12"/>
       <c r="B194" s="13"/>
       <c r="C194" s="12"/>
       <c r="D194" s="13"/>
       <c r="E194" s="13"/>
     </row>
-    <row r="195" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A195" s="12"/>
       <c r="B195" s="13"/>
       <c r="C195" s="12"/>
       <c r="D195" s="13"/>
       <c r="E195" s="13"/>
     </row>
-    <row r="196" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A196" s="12"/>
       <c r="B196" s="13"/>
       <c r="C196" s="12"/>
       <c r="D196" s="13"/>
       <c r="E196" s="13"/>
     </row>
-    <row r="197" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A197" s="12"/>
       <c r="B197" s="13"/>
       <c r="C197" s="12"/>
       <c r="D197" s="13"/>
       <c r="E197" s="13"/>
     </row>
-    <row r="198" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A198" s="12"/>
       <c r="B198" s="13"/>
       <c r="C198" s="12"/>
       <c r="D198" s="13"/>
       <c r="E198" s="13"/>
     </row>
-    <row r="199" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A199" s="12"/>
       <c r="B199" s="13"/>
       <c r="C199" s="12"/>
       <c r="D199" s="13"/>
       <c r="E199" s="13"/>
     </row>
-    <row r="200" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A200" s="12"/>
       <c r="B200" s="13"/>
       <c r="C200" s="12"/>
       <c r="D200" s="13"/>
       <c r="E200" s="13"/>
     </row>
-    <row r="201" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A201" s="12"/>
       <c r="B201" s="13"/>
       <c r="C201" s="12"/>
       <c r="D201" s="13"/>
       <c r="E201" s="13"/>
     </row>
-    <row r="202" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A202" s="12"/>
       <c r="B202" s="13"/>
       <c r="C202" s="12"/>
       <c r="D202" s="13"/>
       <c r="E202" s="13"/>
     </row>
-    <row r="203" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A203" s="12"/>
       <c r="B203" s="13"/>
       <c r="C203" s="12"/>
       <c r="D203" s="13"/>
       <c r="E203" s="13"/>
     </row>
-    <row r="204" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A204" s="12"/>
       <c r="B204" s="13"/>
       <c r="C204" s="12"/>
       <c r="D204" s="13"/>
       <c r="E204" s="13"/>
     </row>
-    <row r="205" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A205" s="12"/>
       <c r="B205" s="13"/>
       <c r="C205" s="12"/>
       <c r="D205" s="13"/>
       <c r="E205" s="13"/>
     </row>
-    <row r="206" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A206" s="12"/>
       <c r="B206" s="13"/>
       <c r="C206" s="12"/>
       <c r="D206" s="13"/>
       <c r="E206" s="13"/>
     </row>
-    <row r="207" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A207" s="12"/>
       <c r="B207" s="13"/>
       <c r="C207" s="12"/>
       <c r="D207" s="13"/>
       <c r="E207" s="13"/>
     </row>
-    <row r="208" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A208" s="12"/>
       <c r="B208" s="13"/>
       <c r="C208" s="12"/>
       <c r="D208" s="13"/>
       <c r="E208" s="13"/>
     </row>
-    <row r="209" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A209" s="12"/>
       <c r="B209" s="13"/>
       <c r="C209" s="12"/>
       <c r="D209" s="13"/>
       <c r="E209" s="13"/>
     </row>
-    <row r="210" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A210" s="12"/>
       <c r="B210" s="13"/>
       <c r="C210" s="12"/>
       <c r="D210" s="13"/>
       <c r="E210" s="13"/>
     </row>
-    <row r="211" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A211" s="12"/>
       <c r="B211" s="13"/>
       <c r="C211" s="12"/>
       <c r="D211" s="13"/>
       <c r="E211" s="13"/>
     </row>
-    <row r="212" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A212" s="12"/>
       <c r="B212" s="13"/>
       <c r="C212" s="12"/>
       <c r="D212" s="13"/>
       <c r="E212" s="13"/>
     </row>
-    <row r="213" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A213" s="12"/>
       <c r="B213" s="13"/>
       <c r="C213" s="12"/>
       <c r="D213" s="13"/>
       <c r="E213" s="13"/>
     </row>
-    <row r="214" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A214" s="12"/>
       <c r="B214" s="13"/>
       <c r="C214" s="12"/>
       <c r="D214" s="13"/>
       <c r="E214" s="13"/>
     </row>
-    <row r="215" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A215" s="12"/>
       <c r="B215" s="13"/>
       <c r="C215" s="12"/>
       <c r="D215" s="13"/>
       <c r="E215" s="13"/>
     </row>
-    <row r="216" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A216" s="12"/>
       <c r="B216" s="13"/>
       <c r="C216" s="12"/>
       <c r="D216" s="13"/>
       <c r="E216" s="13"/>
     </row>
-    <row r="217" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A217" s="12"/>
       <c r="B217" s="13"/>
       <c r="C217" s="12"/>
       <c r="D217" s="13"/>
       <c r="E217" s="13"/>
     </row>
-    <row r="218" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A218" s="12"/>
       <c r="B218" s="13"/>
       <c r="C218" s="12"/>
       <c r="D218" s="13"/>
       <c r="E218" s="13"/>
     </row>
-    <row r="219" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A219" s="12"/>
       <c r="B219" s="13"/>
       <c r="C219" s="12"/>
       <c r="D219" s="13"/>
       <c r="E219" s="13"/>
     </row>
-    <row r="220" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A220" s="12"/>
       <c r="B220" s="13"/>
       <c r="C220" s="12"/>
       <c r="D220" s="13"/>
       <c r="E220" s="13"/>
     </row>
-    <row r="221" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A221" s="12"/>
       <c r="B221" s="13"/>
       <c r="C221" s="12"/>
       <c r="D221" s="13"/>
       <c r="E221" s="13"/>
     </row>
-    <row r="222" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A222" s="12"/>
       <c r="B222" s="13"/>
       <c r="C222" s="12"/>
       <c r="D222" s="13"/>
       <c r="E222" s="13"/>
     </row>
-    <row r="223" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A223" s="12"/>
       <c r="B223" s="13"/>
       <c r="C223" s="12"/>
       <c r="D223" s="13"/>
       <c r="E223" s="13"/>
     </row>
-    <row r="224" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A224" s="12"/>
       <c r="B224" s="13"/>
       <c r="C224" s="12"/>
       <c r="D224" s="13"/>
       <c r="E224" s="13"/>
     </row>
-    <row r="225" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A225" s="12"/>
       <c r="B225" s="13"/>
       <c r="C225" s="12"/>
       <c r="D225" s="13"/>
       <c r="E225" s="13"/>
     </row>
-    <row r="226" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A226" s="12"/>
       <c r="B226" s="13"/>
       <c r="C226" s="12"/>
       <c r="D226" s="13"/>
       <c r="E226" s="13"/>
     </row>
-    <row r="227" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A227" s="12"/>
       <c r="B227" s="13"/>
       <c r="C227" s="12"/>
       <c r="D227" s="13"/>
       <c r="E227" s="13"/>
     </row>
-    <row r="228" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A228" s="12"/>
       <c r="B228" s="13"/>
       <c r="C228" s="12"/>
       <c r="D228" s="13"/>
       <c r="E228" s="13"/>
     </row>
-    <row r="229" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A229" s="12"/>
       <c r="B229" s="13"/>
       <c r="C229" s="12"/>
       <c r="D229" s="13"/>
       <c r="E229" s="13"/>
     </row>
-    <row r="230" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A230" s="12"/>
       <c r="B230" s="13"/>
       <c r="C230" s="12"/>
       <c r="D230" s="13"/>
       <c r="E230" s="13"/>
     </row>
-    <row r="231" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A231" s="12"/>
       <c r="B231" s="13"/>
       <c r="C231" s="12"/>
       <c r="D231" s="13"/>
       <c r="E231" s="13"/>
     </row>
-    <row r="232" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A232" s="12"/>
       <c r="B232" s="13"/>
       <c r="C232" s="12"/>
       <c r="D232" s="13"/>
       <c r="E232" s="13"/>
     </row>
-    <row r="233" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A233" s="12"/>
       <c r="B233" s="13"/>
       <c r="C233" s="12"/>
       <c r="D233" s="13"/>
       <c r="E233" s="13"/>
     </row>
-    <row r="234" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A234" s="12"/>
       <c r="B234" s="13"/>
       <c r="C234" s="12"/>
       <c r="D234" s="13"/>
       <c r="E234" s="13"/>
     </row>
-    <row r="235" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A235" s="12"/>
       <c r="B235" s="13"/>
       <c r="C235" s="12"/>
       <c r="D235" s="13"/>
       <c r="E235" s="13"/>
     </row>
-    <row r="236" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A236" s="12"/>
       <c r="B236" s="13"/>
       <c r="C236" s="12"/>
       <c r="D236" s="13"/>
       <c r="E236" s="13"/>
     </row>
-    <row r="237" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A237" s="12"/>
       <c r="B237" s="13"/>
       <c r="C237" s="12"/>
       <c r="D237" s="13"/>
       <c r="E237" s="13"/>
     </row>
-    <row r="238" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A238" s="12"/>
       <c r="B238" s="13"/>
       <c r="C238" s="12"/>
       <c r="D238" s="13"/>
       <c r="E238" s="13"/>
     </row>
-    <row r="239" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A239" s="12"/>
       <c r="B239" s="13"/>
       <c r="C239" s="12"/>
       <c r="D239" s="13"/>
       <c r="E239" s="13"/>
     </row>
-    <row r="240" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A240" s="12"/>
       <c r="B240" s="13"/>
       <c r="C240" s="12"/>
       <c r="D240" s="13"/>
       <c r="E240" s="13"/>
     </row>
-    <row r="241" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A241" s="12"/>
       <c r="B241" s="13"/>
       <c r="C241" s="12"/>
       <c r="D241" s="13"/>
       <c r="E241" s="13"/>
     </row>
-    <row r="242" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A242" s="12"/>
       <c r="B242" s="13"/>
       <c r="C242" s="12"/>
       <c r="D242" s="13"/>
       <c r="E242" s="13"/>
     </row>
-    <row r="243" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A243" s="12"/>
       <c r="B243" s="13"/>
       <c r="C243" s="12"/>
       <c r="D243" s="13"/>
       <c r="E243" s="13"/>
     </row>
-    <row r="244" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A244" s="12"/>
       <c r="B244" s="13"/>
       <c r="C244" s="12"/>
       <c r="D244" s="13"/>
       <c r="E244" s="13"/>
     </row>
-    <row r="245" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A245" s="12"/>
       <c r="B245" s="13"/>
       <c r="C245" s="12"/>
       <c r="D245" s="13"/>
       <c r="E245" s="13"/>
     </row>
-    <row r="246" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A246" s="12"/>
       <c r="B246" s="13"/>
       <c r="C246" s="12"/>
       <c r="D246" s="13"/>
       <c r="E246" s="13"/>
     </row>
-    <row r="247" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A247" s="12"/>
       <c r="B247" s="13"/>
       <c r="C247" s="12"/>
       <c r="D247" s="13"/>
       <c r="E247" s="13"/>
     </row>
-    <row r="248" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A248" s="12"/>
       <c r="B248" s="13"/>
       <c r="C248" s="12"/>
       <c r="D248" s="13"/>
       <c r="E248" s="13"/>
     </row>
-    <row r="249" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A249" s="12"/>
       <c r="B249" s="13"/>
       <c r="C249" s="12"/>
       <c r="D249" s="13"/>
       <c r="E249" s="13"/>
     </row>
-    <row r="250" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A250" s="12"/>
       <c r="B250" s="13"/>
       <c r="C250" s="12"/>
       <c r="D250" s="13"/>
       <c r="E250" s="13"/>
     </row>
-    <row r="251" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A251" s="12"/>
       <c r="B251" s="13"/>
       <c r="C251" s="12"/>
       <c r="D251" s="13"/>
       <c r="E251" s="13"/>
     </row>
-    <row r="252" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A252" s="12"/>
       <c r="B252" s="13"/>
       <c r="C252" s="12"/>
       <c r="D252" s="13"/>
       <c r="E252" s="13"/>
     </row>
-    <row r="253" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A253" s="12"/>
       <c r="B253" s="13"/>
       <c r="C253" s="12"/>
       <c r="D253" s="13"/>
       <c r="E253" s="13"/>
     </row>
-    <row r="254" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A254" s="12"/>
       <c r="B254" s="13"/>
       <c r="C254" s="12"/>
       <c r="D254" s="13"/>
       <c r="E254" s="13"/>
     </row>
-    <row r="255" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A255" s="12"/>
       <c r="B255" s="13"/>
       <c r="C255" s="12"/>
       <c r="D255" s="13"/>
       <c r="E255" s="13"/>
     </row>
-    <row r="256" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A256" s="12"/>
       <c r="B256" s="13"/>
       <c r="C256" s="12"/>
       <c r="D256" s="13"/>
       <c r="E256" s="13"/>
     </row>
-    <row r="257" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A257" s="12"/>
       <c r="B257" s="13"/>
       <c r="C257" s="12"/>
       <c r="D257" s="13"/>
       <c r="E257" s="13"/>
     </row>
-    <row r="258" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A258" s="12"/>
       <c r="B258" s="13"/>
       <c r="C258" s="12"/>
       <c r="D258" s="13"/>
       <c r="E258" s="13"/>
     </row>
-    <row r="259" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A259" s="12"/>
       <c r="B259" s="13"/>
       <c r="C259" s="12"/>
       <c r="D259" s="13"/>
       <c r="E259" s="13"/>
     </row>
-    <row r="260" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A260" s="12"/>
       <c r="B260" s="13"/>
       <c r="C260" s="12"/>
@@ -2977,6 +2994,7 @@
     <hyperlink ref="D27" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
     <hyperlink ref="D28" r:id="rId2" xr:uid="{4877334E-7528-4DFA-87BA-7232CC222E39}"/>
     <hyperlink ref="D29" r:id="rId3" xr:uid="{BD98EB24-72D1-47EA-9C38-88A632EFC407}"/>
+    <hyperlink ref="D30" r:id="rId4" xr:uid="{2B1F1BE8-9B38-49F3-BF80-B549935EB25B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Se agrega el [30] Alumno al archivo
</commit_message>
<xml_diff>
--- a/Lista de Alumnos.xlsx
+++ b/Lista de Alumnos.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25330"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mhect\OneDrive\Escritorio\pp12021grupo7_a2-grupo7_a2-main\Alumnos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MONTAÑO ANDRES\Desktop\proyecto1\Alumnos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EB75262-340B-4510-8E68-B93EF4B66A5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570"/>
   </bookViews>
   <sheets>
     <sheet name="Electronica Microcontrolada" sheetId="1" r:id="rId1"/>
@@ -20,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="94">
   <si>
     <t>#</t>
   </si>
@@ -293,12 +292,21 @@
   </si>
   <si>
     <t>MarinaSR11</t>
+  </si>
+  <si>
+    <t>Andres Montaño</t>
+  </si>
+  <si>
+    <t>maj3210@gmail.com</t>
+  </si>
+  <si>
+    <t>maj3210</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -794,26 +802,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:E260"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="H29" sqref="H29"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.88671875" style="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="37.109375" style="15" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.5546875" style="14" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.85546875" style="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.140625" style="15" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" style="14" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="31" style="15" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="29" style="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -830,7 +838,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -847,7 +855,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>2</v>
       </c>
@@ -862,7 +870,7 @@
       </c>
       <c r="E3" s="6"/>
     </row>
-    <row r="4" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>3</v>
       </c>
@@ -879,7 +887,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>4</v>
       </c>
@@ -896,7 +904,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>5</v>
       </c>
@@ -913,7 +921,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>6</v>
       </c>
@@ -930,7 +938,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>7</v>
       </c>
@@ -947,7 +955,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>8</v>
       </c>
@@ -964,7 +972,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>9</v>
       </c>
@@ -979,7 +987,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <v>10</v>
       </c>
@@ -996,7 +1004,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>11</v>
       </c>
@@ -1013,7 +1021,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
         <v>12</v>
       </c>
@@ -1030,7 +1038,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
         <v>13</v>
       </c>
@@ -1047,7 +1055,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
         <v>14</v>
       </c>
@@ -1064,7 +1072,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
         <v>15</v>
       </c>
@@ -1081,7 +1089,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
         <v>16</v>
       </c>
@@ -1098,7 +1106,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <v>17</v>
       </c>
@@ -1115,7 +1123,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
         <v>18</v>
       </c>
@@ -1132,7 +1140,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
         <v>19</v>
       </c>
@@ -1149,7 +1157,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="5">
         <v>20</v>
       </c>
@@ -1166,7 +1174,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="5">
         <v>21</v>
       </c>
@@ -1183,7 +1191,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="5">
         <v>22</v>
       </c>
@@ -1200,7 +1208,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="5">
         <v>23</v>
       </c>
@@ -1217,7 +1225,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="5">
         <v>24</v>
       </c>
@@ -1234,7 +1242,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="5">
         <v>25</v>
       </c>
@@ -1251,7 +1259,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="5">
         <v>26</v>
       </c>
@@ -1268,7 +1276,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="5">
         <v>27</v>
       </c>
@@ -1285,7 +1293,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="5">
         <v>28</v>
       </c>
@@ -1302,7 +1310,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="5">
         <v>29</v>
       </c>
@@ -1319,16 +1327,24 @@
         <v>90</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="5">
         <v>30</v>
       </c>
-      <c r="B31" s="6"/>
-      <c r="C31" s="5"/>
-      <c r="D31" s="6"/>
-      <c r="E31" s="6"/>
-    </row>
-    <row r="32" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B31" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="C31" s="5">
+        <v>2</v>
+      </c>
+      <c r="D31" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="E31" s="6" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="5">
         <v>31</v>
       </c>
@@ -1337,7 +1353,7 @@
       <c r="D32" s="6"/>
       <c r="E32" s="6"/>
     </row>
-    <row r="33" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="5">
         <v>32</v>
       </c>
@@ -1346,7 +1362,7 @@
       <c r="D33" s="6"/>
       <c r="E33" s="6"/>
     </row>
-    <row r="34" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="5">
         <v>33</v>
       </c>
@@ -1355,7 +1371,7 @@
       <c r="D34" s="6"/>
       <c r="E34" s="6"/>
     </row>
-    <row r="35" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="5">
         <v>34</v>
       </c>
@@ -1364,7 +1380,7 @@
       <c r="D35" s="6"/>
       <c r="E35" s="6"/>
     </row>
-    <row r="36" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="5">
         <v>35</v>
       </c>
@@ -1373,7 +1389,7 @@
       <c r="D36" s="6"/>
       <c r="E36" s="6"/>
     </row>
-    <row r="37" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="5">
         <v>36</v>
       </c>
@@ -1382,7 +1398,7 @@
       <c r="D37" s="6"/>
       <c r="E37" s="6"/>
     </row>
-    <row r="38" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="5">
         <v>37</v>
       </c>
@@ -1391,7 +1407,7 @@
       <c r="D38" s="6"/>
       <c r="E38" s="6"/>
     </row>
-    <row r="39" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="5">
         <v>38</v>
       </c>
@@ -1400,7 +1416,7 @@
       <c r="D39" s="6"/>
       <c r="E39" s="6"/>
     </row>
-    <row r="40" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="5">
         <v>39</v>
       </c>
@@ -1409,7 +1425,7 @@
       <c r="D40" s="6"/>
       <c r="E40" s="6"/>
     </row>
-    <row r="41" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="5">
         <v>40</v>
       </c>
@@ -1418,7 +1434,7 @@
       <c r="D41" s="6"/>
       <c r="E41" s="6"/>
     </row>
-    <row r="42" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="5">
         <v>41</v>
       </c>
@@ -1427,7 +1443,7 @@
       <c r="D42" s="6"/>
       <c r="E42" s="6"/>
     </row>
-    <row r="43" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="5">
         <v>42</v>
       </c>
@@ -1436,7 +1452,7 @@
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
     </row>
-    <row r="44" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="5">
         <v>43</v>
       </c>
@@ -1445,7 +1461,7 @@
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
     </row>
-    <row r="45" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="5">
         <v>44</v>
       </c>
@@ -1454,7 +1470,7 @@
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
     </row>
-    <row r="46" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="5">
         <v>45</v>
       </c>
@@ -1463,7 +1479,7 @@
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
     </row>
-    <row r="47" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="5">
         <v>46</v>
       </c>
@@ -1472,7 +1488,7 @@
       <c r="D47" s="6"/>
       <c r="E47" s="6"/>
     </row>
-    <row r="48" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="5">
         <v>47</v>
       </c>
@@ -1481,7 +1497,7 @@
       <c r="D48" s="6"/>
       <c r="E48" s="6"/>
     </row>
-    <row r="49" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="5">
         <v>48</v>
       </c>
@@ -1490,7 +1506,7 @@
       <c r="D49" s="6"/>
       <c r="E49" s="6"/>
     </row>
-    <row r="50" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="5">
         <v>49</v>
       </c>
@@ -1499,7 +1515,7 @@
       <c r="D50" s="6"/>
       <c r="E50" s="6"/>
     </row>
-    <row r="51" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="5">
         <v>50</v>
       </c>
@@ -1508,7 +1524,7 @@
       <c r="D51" s="6"/>
       <c r="E51" s="6"/>
     </row>
-    <row r="52" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="5">
         <v>51</v>
       </c>
@@ -1517,7 +1533,7 @@
       <c r="D52" s="6"/>
       <c r="E52" s="6"/>
     </row>
-    <row r="53" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="5">
         <v>52</v>
       </c>
@@ -1526,7 +1542,7 @@
       <c r="D53" s="6"/>
       <c r="E53" s="6"/>
     </row>
-    <row r="54" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="5">
         <v>53</v>
       </c>
@@ -1535,7 +1551,7 @@
       <c r="D54" s="6"/>
       <c r="E54" s="6"/>
     </row>
-    <row r="55" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="5">
         <v>54</v>
       </c>
@@ -1544,7 +1560,7 @@
       <c r="D55" s="6"/>
       <c r="E55" s="6"/>
     </row>
-    <row r="56" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="5">
         <v>55</v>
       </c>
@@ -1553,7 +1569,7 @@
       <c r="D56" s="6"/>
       <c r="E56" s="6"/>
     </row>
-    <row r="57" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="5">
         <v>56</v>
       </c>
@@ -1562,7 +1578,7 @@
       <c r="D57" s="6"/>
       <c r="E57" s="6"/>
     </row>
-    <row r="58" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="5">
         <v>57</v>
       </c>
@@ -1571,7 +1587,7 @@
       <c r="D58" s="6"/>
       <c r="E58" s="6"/>
     </row>
-    <row r="59" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="5">
         <v>58</v>
       </c>
@@ -1580,7 +1596,7 @@
       <c r="D59" s="6"/>
       <c r="E59" s="6"/>
     </row>
-    <row r="60" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="5">
         <v>59</v>
       </c>
@@ -1589,1400 +1605,1400 @@
       <c r="D60" s="6"/>
       <c r="E60" s="6"/>
     </row>
-    <row r="61" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="12"/>
       <c r="B61" s="13"/>
       <c r="C61" s="12"/>
       <c r="D61" s="13"/>
       <c r="E61" s="13"/>
     </row>
-    <row r="62" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="12"/>
       <c r="B62" s="13"/>
       <c r="C62" s="12"/>
       <c r="D62" s="13"/>
       <c r="E62" s="13"/>
     </row>
-    <row r="63" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="12"/>
       <c r="B63" s="13"/>
       <c r="C63" s="12"/>
       <c r="D63" s="13"/>
       <c r="E63" s="13"/>
     </row>
-    <row r="64" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="12"/>
       <c r="B64" s="13"/>
       <c r="C64" s="12"/>
       <c r="D64" s="13"/>
       <c r="E64" s="13"/>
     </row>
-    <row r="65" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="12"/>
       <c r="B65" s="13"/>
       <c r="C65" s="12"/>
       <c r="D65" s="13"/>
       <c r="E65" s="13"/>
     </row>
-    <row r="66" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="12"/>
       <c r="B66" s="13"/>
       <c r="C66" s="12"/>
       <c r="D66" s="13"/>
       <c r="E66" s="13"/>
     </row>
-    <row r="67" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="12"/>
       <c r="B67" s="13"/>
       <c r="C67" s="12"/>
       <c r="D67" s="13"/>
       <c r="E67" s="13"/>
     </row>
-    <row r="68" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="12"/>
       <c r="B68" s="13"/>
       <c r="C68" s="12"/>
       <c r="D68" s="13"/>
       <c r="E68" s="13"/>
     </row>
-    <row r="69" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="12"/>
       <c r="B69" s="13"/>
       <c r="C69" s="12"/>
       <c r="D69" s="13"/>
       <c r="E69" s="13"/>
     </row>
-    <row r="70" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="12"/>
       <c r="B70" s="13"/>
       <c r="C70" s="12"/>
       <c r="D70" s="13"/>
       <c r="E70" s="13"/>
     </row>
-    <row r="71" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="12"/>
       <c r="B71" s="13"/>
       <c r="C71" s="12"/>
       <c r="D71" s="13"/>
       <c r="E71" s="13"/>
     </row>
-    <row r="72" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="12"/>
       <c r="B72" s="13"/>
       <c r="C72" s="12"/>
       <c r="D72" s="13"/>
       <c r="E72" s="13"/>
     </row>
-    <row r="73" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="12"/>
       <c r="B73" s="13"/>
       <c r="C73" s="12"/>
       <c r="D73" s="13"/>
       <c r="E73" s="13"/>
     </row>
-    <row r="74" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="12"/>
       <c r="B74" s="13"/>
       <c r="C74" s="12"/>
       <c r="D74" s="13"/>
       <c r="E74" s="13"/>
     </row>
-    <row r="75" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="12"/>
       <c r="B75" s="13"/>
       <c r="C75" s="12"/>
       <c r="D75" s="13"/>
       <c r="E75" s="13"/>
     </row>
-    <row r="76" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="12"/>
       <c r="B76" s="13"/>
       <c r="C76" s="12"/>
       <c r="D76" s="13"/>
       <c r="E76" s="13"/>
     </row>
-    <row r="77" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="12"/>
       <c r="B77" s="13"/>
       <c r="C77" s="12"/>
       <c r="D77" s="13"/>
       <c r="E77" s="13"/>
     </row>
-    <row r="78" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="12"/>
       <c r="B78" s="13"/>
       <c r="C78" s="12"/>
       <c r="D78" s="13"/>
       <c r="E78" s="13"/>
     </row>
-    <row r="79" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="12"/>
       <c r="B79" s="13"/>
       <c r="C79" s="12"/>
       <c r="D79" s="13"/>
       <c r="E79" s="13"/>
     </row>
-    <row r="80" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="12"/>
       <c r="B80" s="13"/>
       <c r="C80" s="12"/>
       <c r="D80" s="13"/>
       <c r="E80" s="13"/>
     </row>
-    <row r="81" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="12"/>
       <c r="B81" s="13"/>
       <c r="C81" s="12"/>
       <c r="D81" s="13"/>
       <c r="E81" s="13"/>
     </row>
-    <row r="82" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="12"/>
       <c r="B82" s="13"/>
       <c r="C82" s="12"/>
       <c r="D82" s="13"/>
       <c r="E82" s="13"/>
     </row>
-    <row r="83" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="12"/>
       <c r="B83" s="13"/>
       <c r="C83" s="12"/>
       <c r="D83" s="13"/>
       <c r="E83" s="13"/>
     </row>
-    <row r="84" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="12"/>
       <c r="B84" s="13"/>
       <c r="C84" s="12"/>
       <c r="D84" s="13"/>
       <c r="E84" s="13"/>
     </row>
-    <row r="85" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="12"/>
       <c r="B85" s="13"/>
       <c r="C85" s="12"/>
       <c r="D85" s="13"/>
       <c r="E85" s="13"/>
     </row>
-    <row r="86" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="12"/>
       <c r="B86" s="13"/>
       <c r="C86" s="12"/>
       <c r="D86" s="13"/>
       <c r="E86" s="13"/>
     </row>
-    <row r="87" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="12"/>
       <c r="B87" s="13"/>
       <c r="C87" s="12"/>
       <c r="D87" s="13"/>
       <c r="E87" s="13"/>
     </row>
-    <row r="88" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="12"/>
       <c r="B88" s="13"/>
       <c r="C88" s="12"/>
       <c r="D88" s="13"/>
       <c r="E88" s="13"/>
     </row>
-    <row r="89" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="12"/>
       <c r="B89" s="13"/>
       <c r="C89" s="12"/>
       <c r="D89" s="13"/>
       <c r="E89" s="13"/>
     </row>
-    <row r="90" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="12"/>
       <c r="B90" s="13"/>
       <c r="C90" s="12"/>
       <c r="D90" s="13"/>
       <c r="E90" s="13"/>
     </row>
-    <row r="91" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="12"/>
       <c r="B91" s="13"/>
       <c r="C91" s="12"/>
       <c r="D91" s="13"/>
       <c r="E91" s="13"/>
     </row>
-    <row r="92" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="12"/>
       <c r="B92" s="13"/>
       <c r="C92" s="12"/>
       <c r="D92" s="13"/>
       <c r="E92" s="13"/>
     </row>
-    <row r="93" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="12"/>
       <c r="B93" s="13"/>
       <c r="C93" s="12"/>
       <c r="D93" s="13"/>
       <c r="E93" s="13"/>
     </row>
-    <row r="94" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="12"/>
       <c r="B94" s="13"/>
       <c r="C94" s="12"/>
       <c r="D94" s="13"/>
       <c r="E94" s="13"/>
     </row>
-    <row r="95" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="12"/>
       <c r="B95" s="13"/>
       <c r="C95" s="12"/>
       <c r="D95" s="13"/>
       <c r="E95" s="13"/>
     </row>
-    <row r="96" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="12"/>
       <c r="B96" s="13"/>
       <c r="C96" s="12"/>
       <c r="D96" s="13"/>
       <c r="E96" s="13"/>
     </row>
-    <row r="97" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="12"/>
       <c r="B97" s="13"/>
       <c r="C97" s="12"/>
       <c r="D97" s="13"/>
       <c r="E97" s="13"/>
     </row>
-    <row r="98" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="12"/>
       <c r="B98" s="13"/>
       <c r="C98" s="12"/>
       <c r="D98" s="13"/>
       <c r="E98" s="13"/>
     </row>
-    <row r="99" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="12"/>
       <c r="B99" s="13"/>
       <c r="C99" s="12"/>
       <c r="D99" s="13"/>
       <c r="E99" s="13"/>
     </row>
-    <row r="100" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="12"/>
       <c r="B100" s="13"/>
       <c r="C100" s="12"/>
       <c r="D100" s="13"/>
       <c r="E100" s="13"/>
     </row>
-    <row r="101" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="12"/>
       <c r="B101" s="13"/>
       <c r="C101" s="12"/>
       <c r="D101" s="13"/>
       <c r="E101" s="13"/>
     </row>
-    <row r="102" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="12"/>
       <c r="B102" s="13"/>
       <c r="C102" s="12"/>
       <c r="D102" s="13"/>
       <c r="E102" s="13"/>
     </row>
-    <row r="103" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" s="12"/>
       <c r="B103" s="13"/>
       <c r="C103" s="12"/>
       <c r="D103" s="13"/>
       <c r="E103" s="13"/>
     </row>
-    <row r="104" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="12"/>
       <c r="B104" s="13"/>
       <c r="C104" s="12"/>
       <c r="D104" s="13"/>
       <c r="E104" s="13"/>
     </row>
-    <row r="105" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" s="12"/>
       <c r="B105" s="13"/>
       <c r="C105" s="12"/>
       <c r="D105" s="13"/>
       <c r="E105" s="13"/>
     </row>
-    <row r="106" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="12"/>
       <c r="B106" s="13"/>
       <c r="C106" s="12"/>
       <c r="D106" s="13"/>
       <c r="E106" s="13"/>
     </row>
-    <row r="107" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" s="12"/>
       <c r="B107" s="13"/>
       <c r="C107" s="12"/>
       <c r="D107" s="13"/>
       <c r="E107" s="13"/>
     </row>
-    <row r="108" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" s="12"/>
       <c r="B108" s="13"/>
       <c r="C108" s="12"/>
       <c r="D108" s="13"/>
       <c r="E108" s="13"/>
     </row>
-    <row r="109" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" s="12"/>
       <c r="B109" s="13"/>
       <c r="C109" s="12"/>
       <c r="D109" s="13"/>
       <c r="E109" s="13"/>
     </row>
-    <row r="110" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" s="12"/>
       <c r="B110" s="13"/>
       <c r="C110" s="12"/>
       <c r="D110" s="13"/>
       <c r="E110" s="13"/>
     </row>
-    <row r="111" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" s="12"/>
       <c r="B111" s="13"/>
       <c r="C111" s="12"/>
       <c r="D111" s="13"/>
       <c r="E111" s="13"/>
     </row>
-    <row r="112" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" s="12"/>
       <c r="B112" s="13"/>
       <c r="C112" s="12"/>
       <c r="D112" s="13"/>
       <c r="E112" s="13"/>
     </row>
-    <row r="113" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" s="12"/>
       <c r="B113" s="13"/>
       <c r="C113" s="12"/>
       <c r="D113" s="13"/>
       <c r="E113" s="13"/>
     </row>
-    <row r="114" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A114" s="12"/>
       <c r="B114" s="13"/>
       <c r="C114" s="12"/>
       <c r="D114" s="13"/>
       <c r="E114" s="13"/>
     </row>
-    <row r="115" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A115" s="12"/>
       <c r="B115" s="13"/>
       <c r="C115" s="12"/>
       <c r="D115" s="13"/>
       <c r="E115" s="13"/>
     </row>
-    <row r="116" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A116" s="12"/>
       <c r="B116" s="13"/>
       <c r="C116" s="12"/>
       <c r="D116" s="13"/>
       <c r="E116" s="13"/>
     </row>
-    <row r="117" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A117" s="12"/>
       <c r="B117" s="13"/>
       <c r="C117" s="12"/>
       <c r="D117" s="13"/>
       <c r="E117" s="13"/>
     </row>
-    <row r="118" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A118" s="12"/>
       <c r="B118" s="13"/>
       <c r="C118" s="12"/>
       <c r="D118" s="13"/>
       <c r="E118" s="13"/>
     </row>
-    <row r="119" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A119" s="12"/>
       <c r="B119" s="13"/>
       <c r="C119" s="12"/>
       <c r="D119" s="13"/>
       <c r="E119" s="13"/>
     </row>
-    <row r="120" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A120" s="12"/>
       <c r="B120" s="13"/>
       <c r="C120" s="12"/>
       <c r="D120" s="13"/>
       <c r="E120" s="13"/>
     </row>
-    <row r="121" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A121" s="12"/>
       <c r="B121" s="13"/>
       <c r="C121" s="12"/>
       <c r="D121" s="13"/>
       <c r="E121" s="13"/>
     </row>
-    <row r="122" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A122" s="12"/>
       <c r="B122" s="13"/>
       <c r="C122" s="12"/>
       <c r="D122" s="13"/>
       <c r="E122" s="13"/>
     </row>
-    <row r="123" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A123" s="12"/>
       <c r="B123" s="13"/>
       <c r="C123" s="12"/>
       <c r="D123" s="13"/>
       <c r="E123" s="13"/>
     </row>
-    <row r="124" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A124" s="12"/>
       <c r="B124" s="13"/>
       <c r="C124" s="12"/>
       <c r="D124" s="13"/>
       <c r="E124" s="13"/>
     </row>
-    <row r="125" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A125" s="12"/>
       <c r="B125" s="13"/>
       <c r="C125" s="12"/>
       <c r="D125" s="13"/>
       <c r="E125" s="13"/>
     </row>
-    <row r="126" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A126" s="12"/>
       <c r="B126" s="13"/>
       <c r="C126" s="12"/>
       <c r="D126" s="13"/>
       <c r="E126" s="13"/>
     </row>
-    <row r="127" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A127" s="12"/>
       <c r="B127" s="13"/>
       <c r="C127" s="12"/>
       <c r="D127" s="13"/>
       <c r="E127" s="13"/>
     </row>
-    <row r="128" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A128" s="12"/>
       <c r="B128" s="13"/>
       <c r="C128" s="12"/>
       <c r="D128" s="13"/>
       <c r="E128" s="13"/>
     </row>
-    <row r="129" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A129" s="12"/>
       <c r="B129" s="13"/>
       <c r="C129" s="12"/>
       <c r="D129" s="13"/>
       <c r="E129" s="13"/>
     </row>
-    <row r="130" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A130" s="12"/>
       <c r="B130" s="13"/>
       <c r="C130" s="12"/>
       <c r="D130" s="13"/>
       <c r="E130" s="13"/>
     </row>
-    <row r="131" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A131" s="12"/>
       <c r="B131" s="13"/>
       <c r="C131" s="12"/>
       <c r="D131" s="13"/>
       <c r="E131" s="13"/>
     </row>
-    <row r="132" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A132" s="12"/>
       <c r="B132" s="13"/>
       <c r="C132" s="12"/>
       <c r="D132" s="13"/>
       <c r="E132" s="13"/>
     </row>
-    <row r="133" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A133" s="12"/>
       <c r="B133" s="13"/>
       <c r="C133" s="12"/>
       <c r="D133" s="13"/>
       <c r="E133" s="13"/>
     </row>
-    <row r="134" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A134" s="12"/>
       <c r="B134" s="13"/>
       <c r="C134" s="12"/>
       <c r="D134" s="13"/>
       <c r="E134" s="13"/>
     </row>
-    <row r="135" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A135" s="12"/>
       <c r="B135" s="13"/>
       <c r="C135" s="12"/>
       <c r="D135" s="13"/>
       <c r="E135" s="13"/>
     </row>
-    <row r="136" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A136" s="12"/>
       <c r="B136" s="13"/>
       <c r="C136" s="12"/>
       <c r="D136" s="13"/>
       <c r="E136" s="13"/>
     </row>
-    <row r="137" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A137" s="12"/>
       <c r="B137" s="13"/>
       <c r="C137" s="12"/>
       <c r="D137" s="13"/>
       <c r="E137" s="13"/>
     </row>
-    <row r="138" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A138" s="12"/>
       <c r="B138" s="13"/>
       <c r="C138" s="12"/>
       <c r="D138" s="13"/>
       <c r="E138" s="13"/>
     </row>
-    <row r="139" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A139" s="12"/>
       <c r="B139" s="13"/>
       <c r="C139" s="12"/>
       <c r="D139" s="13"/>
       <c r="E139" s="13"/>
     </row>
-    <row r="140" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A140" s="12"/>
       <c r="B140" s="13"/>
       <c r="C140" s="12"/>
       <c r="D140" s="13"/>
       <c r="E140" s="13"/>
     </row>
-    <row r="141" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A141" s="12"/>
       <c r="B141" s="13"/>
       <c r="C141" s="12"/>
       <c r="D141" s="13"/>
       <c r="E141" s="13"/>
     </row>
-    <row r="142" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A142" s="12"/>
       <c r="B142" s="13"/>
       <c r="C142" s="12"/>
       <c r="D142" s="13"/>
       <c r="E142" s="13"/>
     </row>
-    <row r="143" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A143" s="12"/>
       <c r="B143" s="13"/>
       <c r="C143" s="12"/>
       <c r="D143" s="13"/>
       <c r="E143" s="13"/>
     </row>
-    <row r="144" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A144" s="12"/>
       <c r="B144" s="13"/>
       <c r="C144" s="12"/>
       <c r="D144" s="13"/>
       <c r="E144" s="13"/>
     </row>
-    <row r="145" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A145" s="12"/>
       <c r="B145" s="13"/>
       <c r="C145" s="12"/>
       <c r="D145" s="13"/>
       <c r="E145" s="13"/>
     </row>
-    <row r="146" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A146" s="12"/>
       <c r="B146" s="13"/>
       <c r="C146" s="12"/>
       <c r="D146" s="13"/>
       <c r="E146" s="13"/>
     </row>
-    <row r="147" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A147" s="12"/>
       <c r="B147" s="13"/>
       <c r="C147" s="12"/>
       <c r="D147" s="13"/>
       <c r="E147" s="13"/>
     </row>
-    <row r="148" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A148" s="12"/>
       <c r="B148" s="13"/>
       <c r="C148" s="12"/>
       <c r="D148" s="13"/>
       <c r="E148" s="13"/>
     </row>
-    <row r="149" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A149" s="12"/>
       <c r="B149" s="13"/>
       <c r="C149" s="12"/>
       <c r="D149" s="13"/>
       <c r="E149" s="13"/>
     </row>
-    <row r="150" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A150" s="12"/>
       <c r="B150" s="13"/>
       <c r="C150" s="12"/>
       <c r="D150" s="13"/>
       <c r="E150" s="13"/>
     </row>
-    <row r="151" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A151" s="12"/>
       <c r="B151" s="13"/>
       <c r="C151" s="12"/>
       <c r="D151" s="13"/>
       <c r="E151" s="13"/>
     </row>
-    <row r="152" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A152" s="12"/>
       <c r="B152" s="13"/>
       <c r="C152" s="12"/>
       <c r="D152" s="13"/>
       <c r="E152" s="13"/>
     </row>
-    <row r="153" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A153" s="12"/>
       <c r="B153" s="13"/>
       <c r="C153" s="12"/>
       <c r="D153" s="13"/>
       <c r="E153" s="13"/>
     </row>
-    <row r="154" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A154" s="12"/>
       <c r="B154" s="13"/>
       <c r="C154" s="12"/>
       <c r="D154" s="13"/>
       <c r="E154" s="13"/>
     </row>
-    <row r="155" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A155" s="12"/>
       <c r="B155" s="13"/>
       <c r="C155" s="12"/>
       <c r="D155" s="13"/>
       <c r="E155" s="13"/>
     </row>
-    <row r="156" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A156" s="12"/>
       <c r="B156" s="13"/>
       <c r="C156" s="12"/>
       <c r="D156" s="13"/>
       <c r="E156" s="13"/>
     </row>
-    <row r="157" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A157" s="12"/>
       <c r="B157" s="13"/>
       <c r="C157" s="12"/>
       <c r="D157" s="13"/>
       <c r="E157" s="13"/>
     </row>
-    <row r="158" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A158" s="12"/>
       <c r="B158" s="13"/>
       <c r="C158" s="12"/>
       <c r="D158" s="13"/>
       <c r="E158" s="13"/>
     </row>
-    <row r="159" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A159" s="12"/>
       <c r="B159" s="13"/>
       <c r="C159" s="12"/>
       <c r="D159" s="13"/>
       <c r="E159" s="13"/>
     </row>
-    <row r="160" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A160" s="12"/>
       <c r="B160" s="13"/>
       <c r="C160" s="12"/>
       <c r="D160" s="13"/>
       <c r="E160" s="13"/>
     </row>
-    <row r="161" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A161" s="12"/>
       <c r="B161" s="13"/>
       <c r="C161" s="12"/>
       <c r="D161" s="13"/>
       <c r="E161" s="13"/>
     </row>
-    <row r="162" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A162" s="12"/>
       <c r="B162" s="13"/>
       <c r="C162" s="12"/>
       <c r="D162" s="13"/>
       <c r="E162" s="13"/>
     </row>
-    <row r="163" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A163" s="12"/>
       <c r="B163" s="13"/>
       <c r="C163" s="12"/>
       <c r="D163" s="13"/>
       <c r="E163" s="13"/>
     </row>
-    <row r="164" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A164" s="12"/>
       <c r="B164" s="13"/>
       <c r="C164" s="12"/>
       <c r="D164" s="13"/>
       <c r="E164" s="13"/>
     </row>
-    <row r="165" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A165" s="12"/>
       <c r="B165" s="13"/>
       <c r="C165" s="12"/>
       <c r="D165" s="13"/>
       <c r="E165" s="13"/>
     </row>
-    <row r="166" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A166" s="12"/>
       <c r="B166" s="13"/>
       <c r="C166" s="12"/>
       <c r="D166" s="13"/>
       <c r="E166" s="13"/>
     </row>
-    <row r="167" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A167" s="12"/>
       <c r="B167" s="13"/>
       <c r="C167" s="12"/>
       <c r="D167" s="13"/>
       <c r="E167" s="13"/>
     </row>
-    <row r="168" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A168" s="12"/>
       <c r="B168" s="13"/>
       <c r="C168" s="12"/>
       <c r="D168" s="13"/>
       <c r="E168" s="13"/>
     </row>
-    <row r="169" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A169" s="12"/>
       <c r="B169" s="13"/>
       <c r="C169" s="12"/>
       <c r="D169" s="13"/>
       <c r="E169" s="13"/>
     </row>
-    <row r="170" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A170" s="12"/>
       <c r="B170" s="13"/>
       <c r="C170" s="12"/>
       <c r="D170" s="13"/>
       <c r="E170" s="13"/>
     </row>
-    <row r="171" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A171" s="12"/>
       <c r="B171" s="13"/>
       <c r="C171" s="12"/>
       <c r="D171" s="13"/>
       <c r="E171" s="13"/>
     </row>
-    <row r="172" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A172" s="12"/>
       <c r="B172" s="13"/>
       <c r="C172" s="12"/>
       <c r="D172" s="13"/>
       <c r="E172" s="13"/>
     </row>
-    <row r="173" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A173" s="12"/>
       <c r="B173" s="13"/>
       <c r="C173" s="12"/>
       <c r="D173" s="13"/>
       <c r="E173" s="13"/>
     </row>
-    <row r="174" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A174" s="12"/>
       <c r="B174" s="13"/>
       <c r="C174" s="12"/>
       <c r="D174" s="13"/>
       <c r="E174" s="13"/>
     </row>
-    <row r="175" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A175" s="12"/>
       <c r="B175" s="13"/>
       <c r="C175" s="12"/>
       <c r="D175" s="13"/>
       <c r="E175" s="13"/>
     </row>
-    <row r="176" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A176" s="12"/>
       <c r="B176" s="13"/>
       <c r="C176" s="12"/>
       <c r="D176" s="13"/>
       <c r="E176" s="13"/>
     </row>
-    <row r="177" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A177" s="12"/>
       <c r="B177" s="13"/>
       <c r="C177" s="12"/>
       <c r="D177" s="13"/>
       <c r="E177" s="13"/>
     </row>
-    <row r="178" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A178" s="12"/>
       <c r="B178" s="13"/>
       <c r="C178" s="12"/>
       <c r="D178" s="13"/>
       <c r="E178" s="13"/>
     </row>
-    <row r="179" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A179" s="12"/>
       <c r="B179" s="13"/>
       <c r="C179" s="12"/>
       <c r="D179" s="13"/>
       <c r="E179" s="13"/>
     </row>
-    <row r="180" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A180" s="12"/>
       <c r="B180" s="13"/>
       <c r="C180" s="12"/>
       <c r="D180" s="13"/>
       <c r="E180" s="13"/>
     </row>
-    <row r="181" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A181" s="12"/>
       <c r="B181" s="13"/>
       <c r="C181" s="12"/>
       <c r="D181" s="13"/>
       <c r="E181" s="13"/>
     </row>
-    <row r="182" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A182" s="12"/>
       <c r="B182" s="13"/>
       <c r="C182" s="12"/>
       <c r="D182" s="13"/>
       <c r="E182" s="13"/>
     </row>
-    <row r="183" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A183" s="12"/>
       <c r="B183" s="13"/>
       <c r="C183" s="12"/>
       <c r="D183" s="13"/>
       <c r="E183" s="13"/>
     </row>
-    <row r="184" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A184" s="12"/>
       <c r="B184" s="13"/>
       <c r="C184" s="12"/>
       <c r="D184" s="13"/>
       <c r="E184" s="13"/>
     </row>
-    <row r="185" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A185" s="12"/>
       <c r="B185" s="13"/>
       <c r="C185" s="12"/>
       <c r="D185" s="13"/>
       <c r="E185" s="13"/>
     </row>
-    <row r="186" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A186" s="12"/>
       <c r="B186" s="13"/>
       <c r="C186" s="12"/>
       <c r="D186" s="13"/>
       <c r="E186" s="13"/>
     </row>
-    <row r="187" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A187" s="12"/>
       <c r="B187" s="13"/>
       <c r="C187" s="12"/>
       <c r="D187" s="13"/>
       <c r="E187" s="13"/>
     </row>
-    <row r="188" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A188" s="12"/>
       <c r="B188" s="13"/>
       <c r="C188" s="12"/>
       <c r="D188" s="13"/>
       <c r="E188" s="13"/>
     </row>
-    <row r="189" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A189" s="12"/>
       <c r="B189" s="13"/>
       <c r="C189" s="12"/>
       <c r="D189" s="13"/>
       <c r="E189" s="13"/>
     </row>
-    <row r="190" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A190" s="12"/>
       <c r="B190" s="13"/>
       <c r="C190" s="12"/>
       <c r="D190" s="13"/>
       <c r="E190" s="13"/>
     </row>
-    <row r="191" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A191" s="12"/>
       <c r="B191" s="13"/>
       <c r="C191" s="12"/>
       <c r="D191" s="13"/>
       <c r="E191" s="13"/>
     </row>
-    <row r="192" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A192" s="12"/>
       <c r="B192" s="13"/>
       <c r="C192" s="12"/>
       <c r="D192" s="13"/>
       <c r="E192" s="13"/>
     </row>
-    <row r="193" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A193" s="12"/>
       <c r="B193" s="13"/>
       <c r="C193" s="12"/>
       <c r="D193" s="13"/>
       <c r="E193" s="13"/>
     </row>
-    <row r="194" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A194" s="12"/>
       <c r="B194" s="13"/>
       <c r="C194" s="12"/>
       <c r="D194" s="13"/>
       <c r="E194" s="13"/>
     </row>
-    <row r="195" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A195" s="12"/>
       <c r="B195" s="13"/>
       <c r="C195" s="12"/>
       <c r="D195" s="13"/>
       <c r="E195" s="13"/>
     </row>
-    <row r="196" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A196" s="12"/>
       <c r="B196" s="13"/>
       <c r="C196" s="12"/>
       <c r="D196" s="13"/>
       <c r="E196" s="13"/>
     </row>
-    <row r="197" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A197" s="12"/>
       <c r="B197" s="13"/>
       <c r="C197" s="12"/>
       <c r="D197" s="13"/>
       <c r="E197" s="13"/>
     </row>
-    <row r="198" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A198" s="12"/>
       <c r="B198" s="13"/>
       <c r="C198" s="12"/>
       <c r="D198" s="13"/>
       <c r="E198" s="13"/>
     </row>
-    <row r="199" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A199" s="12"/>
       <c r="B199" s="13"/>
       <c r="C199" s="12"/>
       <c r="D199" s="13"/>
       <c r="E199" s="13"/>
     </row>
-    <row r="200" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A200" s="12"/>
       <c r="B200" s="13"/>
       <c r="C200" s="12"/>
       <c r="D200" s="13"/>
       <c r="E200" s="13"/>
     </row>
-    <row r="201" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A201" s="12"/>
       <c r="B201" s="13"/>
       <c r="C201" s="12"/>
       <c r="D201" s="13"/>
       <c r="E201" s="13"/>
     </row>
-    <row r="202" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A202" s="12"/>
       <c r="B202" s="13"/>
       <c r="C202" s="12"/>
       <c r="D202" s="13"/>
       <c r="E202" s="13"/>
     </row>
-    <row r="203" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A203" s="12"/>
       <c r="B203" s="13"/>
       <c r="C203" s="12"/>
       <c r="D203" s="13"/>
       <c r="E203" s="13"/>
     </row>
-    <row r="204" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A204" s="12"/>
       <c r="B204" s="13"/>
       <c r="C204" s="12"/>
       <c r="D204" s="13"/>
       <c r="E204" s="13"/>
     </row>
-    <row r="205" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A205" s="12"/>
       <c r="B205" s="13"/>
       <c r="C205" s="12"/>
       <c r="D205" s="13"/>
       <c r="E205" s="13"/>
     </row>
-    <row r="206" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A206" s="12"/>
       <c r="B206" s="13"/>
       <c r="C206" s="12"/>
       <c r="D206" s="13"/>
       <c r="E206" s="13"/>
     </row>
-    <row r="207" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A207" s="12"/>
       <c r="B207" s="13"/>
       <c r="C207" s="12"/>
       <c r="D207" s="13"/>
       <c r="E207" s="13"/>
     </row>
-    <row r="208" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A208" s="12"/>
       <c r="B208" s="13"/>
       <c r="C208" s="12"/>
       <c r="D208" s="13"/>
       <c r="E208" s="13"/>
     </row>
-    <row r="209" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A209" s="12"/>
       <c r="B209" s="13"/>
       <c r="C209" s="12"/>
       <c r="D209" s="13"/>
       <c r="E209" s="13"/>
     </row>
-    <row r="210" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A210" s="12"/>
       <c r="B210" s="13"/>
       <c r="C210" s="12"/>
       <c r="D210" s="13"/>
       <c r="E210" s="13"/>
     </row>
-    <row r="211" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A211" s="12"/>
       <c r="B211" s="13"/>
       <c r="C211" s="12"/>
       <c r="D211" s="13"/>
       <c r="E211" s="13"/>
     </row>
-    <row r="212" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A212" s="12"/>
       <c r="B212" s="13"/>
       <c r="C212" s="12"/>
       <c r="D212" s="13"/>
       <c r="E212" s="13"/>
     </row>
-    <row r="213" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A213" s="12"/>
       <c r="B213" s="13"/>
       <c r="C213" s="12"/>
       <c r="D213" s="13"/>
       <c r="E213" s="13"/>
     </row>
-    <row r="214" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A214" s="12"/>
       <c r="B214" s="13"/>
       <c r="C214" s="12"/>
       <c r="D214" s="13"/>
       <c r="E214" s="13"/>
     </row>
-    <row r="215" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A215" s="12"/>
       <c r="B215" s="13"/>
       <c r="C215" s="12"/>
       <c r="D215" s="13"/>
       <c r="E215" s="13"/>
     </row>
-    <row r="216" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A216" s="12"/>
       <c r="B216" s="13"/>
       <c r="C216" s="12"/>
       <c r="D216" s="13"/>
       <c r="E216" s="13"/>
     </row>
-    <row r="217" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A217" s="12"/>
       <c r="B217" s="13"/>
       <c r="C217" s="12"/>
       <c r="D217" s="13"/>
       <c r="E217" s="13"/>
     </row>
-    <row r="218" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A218" s="12"/>
       <c r="B218" s="13"/>
       <c r="C218" s="12"/>
       <c r="D218" s="13"/>
       <c r="E218" s="13"/>
     </row>
-    <row r="219" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A219" s="12"/>
       <c r="B219" s="13"/>
       <c r="C219" s="12"/>
       <c r="D219" s="13"/>
       <c r="E219" s="13"/>
     </row>
-    <row r="220" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A220" s="12"/>
       <c r="B220" s="13"/>
       <c r="C220" s="12"/>
       <c r="D220" s="13"/>
       <c r="E220" s="13"/>
     </row>
-    <row r="221" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A221" s="12"/>
       <c r="B221" s="13"/>
       <c r="C221" s="12"/>
       <c r="D221" s="13"/>
       <c r="E221" s="13"/>
     </row>
-    <row r="222" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A222" s="12"/>
       <c r="B222" s="13"/>
       <c r="C222" s="12"/>
       <c r="D222" s="13"/>
       <c r="E222" s="13"/>
     </row>
-    <row r="223" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A223" s="12"/>
       <c r="B223" s="13"/>
       <c r="C223" s="12"/>
       <c r="D223" s="13"/>
       <c r="E223" s="13"/>
     </row>
-    <row r="224" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A224" s="12"/>
       <c r="B224" s="13"/>
       <c r="C224" s="12"/>
       <c r="D224" s="13"/>
       <c r="E224" s="13"/>
     </row>
-    <row r="225" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A225" s="12"/>
       <c r="B225" s="13"/>
       <c r="C225" s="12"/>
       <c r="D225" s="13"/>
       <c r="E225" s="13"/>
     </row>
-    <row r="226" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A226" s="12"/>
       <c r="B226" s="13"/>
       <c r="C226" s="12"/>
       <c r="D226" s="13"/>
       <c r="E226" s="13"/>
     </row>
-    <row r="227" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A227" s="12"/>
       <c r="B227" s="13"/>
       <c r="C227" s="12"/>
       <c r="D227" s="13"/>
       <c r="E227" s="13"/>
     </row>
-    <row r="228" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A228" s="12"/>
       <c r="B228" s="13"/>
       <c r="C228" s="12"/>
       <c r="D228" s="13"/>
       <c r="E228" s="13"/>
     </row>
-    <row r="229" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A229" s="12"/>
       <c r="B229" s="13"/>
       <c r="C229" s="12"/>
       <c r="D229" s="13"/>
       <c r="E229" s="13"/>
     </row>
-    <row r="230" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A230" s="12"/>
       <c r="B230" s="13"/>
       <c r="C230" s="12"/>
       <c r="D230" s="13"/>
       <c r="E230" s="13"/>
     </row>
-    <row r="231" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A231" s="12"/>
       <c r="B231" s="13"/>
       <c r="C231" s="12"/>
       <c r="D231" s="13"/>
       <c r="E231" s="13"/>
     </row>
-    <row r="232" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A232" s="12"/>
       <c r="B232" s="13"/>
       <c r="C232" s="12"/>
       <c r="D232" s="13"/>
       <c r="E232" s="13"/>
     </row>
-    <row r="233" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A233" s="12"/>
       <c r="B233" s="13"/>
       <c r="C233" s="12"/>
       <c r="D233" s="13"/>
       <c r="E233" s="13"/>
     </row>
-    <row r="234" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A234" s="12"/>
       <c r="B234" s="13"/>
       <c r="C234" s="12"/>
       <c r="D234" s="13"/>
       <c r="E234" s="13"/>
     </row>
-    <row r="235" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A235" s="12"/>
       <c r="B235" s="13"/>
       <c r="C235" s="12"/>
       <c r="D235" s="13"/>
       <c r="E235" s="13"/>
     </row>
-    <row r="236" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A236" s="12"/>
       <c r="B236" s="13"/>
       <c r="C236" s="12"/>
       <c r="D236" s="13"/>
       <c r="E236" s="13"/>
     </row>
-    <row r="237" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A237" s="12"/>
       <c r="B237" s="13"/>
       <c r="C237" s="12"/>
       <c r="D237" s="13"/>
       <c r="E237" s="13"/>
     </row>
-    <row r="238" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A238" s="12"/>
       <c r="B238" s="13"/>
       <c r="C238" s="12"/>
       <c r="D238" s="13"/>
       <c r="E238" s="13"/>
     </row>
-    <row r="239" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A239" s="12"/>
       <c r="B239" s="13"/>
       <c r="C239" s="12"/>
       <c r="D239" s="13"/>
       <c r="E239" s="13"/>
     </row>
-    <row r="240" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A240" s="12"/>
       <c r="B240" s="13"/>
       <c r="C240" s="12"/>
       <c r="D240" s="13"/>
       <c r="E240" s="13"/>
     </row>
-    <row r="241" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A241" s="12"/>
       <c r="B241" s="13"/>
       <c r="C241" s="12"/>
       <c r="D241" s="13"/>
       <c r="E241" s="13"/>
     </row>
-    <row r="242" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A242" s="12"/>
       <c r="B242" s="13"/>
       <c r="C242" s="12"/>
       <c r="D242" s="13"/>
       <c r="E242" s="13"/>
     </row>
-    <row r="243" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A243" s="12"/>
       <c r="B243" s="13"/>
       <c r="C243" s="12"/>
       <c r="D243" s="13"/>
       <c r="E243" s="13"/>
     </row>
-    <row r="244" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A244" s="12"/>
       <c r="B244" s="13"/>
       <c r="C244" s="12"/>
       <c r="D244" s="13"/>
       <c r="E244" s="13"/>
     </row>
-    <row r="245" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A245" s="12"/>
       <c r="B245" s="13"/>
       <c r="C245" s="12"/>
       <c r="D245" s="13"/>
       <c r="E245" s="13"/>
     </row>
-    <row r="246" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A246" s="12"/>
       <c r="B246" s="13"/>
       <c r="C246" s="12"/>
       <c r="D246" s="13"/>
       <c r="E246" s="13"/>
     </row>
-    <row r="247" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A247" s="12"/>
       <c r="B247" s="13"/>
       <c r="C247" s="12"/>
       <c r="D247" s="13"/>
       <c r="E247" s="13"/>
     </row>
-    <row r="248" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A248" s="12"/>
       <c r="B248" s="13"/>
       <c r="C248" s="12"/>
       <c r="D248" s="13"/>
       <c r="E248" s="13"/>
     </row>
-    <row r="249" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A249" s="12"/>
       <c r="B249" s="13"/>
       <c r="C249" s="12"/>
       <c r="D249" s="13"/>
       <c r="E249" s="13"/>
     </row>
-    <row r="250" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A250" s="12"/>
       <c r="B250" s="13"/>
       <c r="C250" s="12"/>
       <c r="D250" s="13"/>
       <c r="E250" s="13"/>
     </row>
-    <row r="251" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A251" s="12"/>
       <c r="B251" s="13"/>
       <c r="C251" s="12"/>
       <c r="D251" s="13"/>
       <c r="E251" s="13"/>
     </row>
-    <row r="252" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A252" s="12"/>
       <c r="B252" s="13"/>
       <c r="C252" s="12"/>
       <c r="D252" s="13"/>
       <c r="E252" s="13"/>
     </row>
-    <row r="253" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A253" s="12"/>
       <c r="B253" s="13"/>
       <c r="C253" s="12"/>
       <c r="D253" s="13"/>
       <c r="E253" s="13"/>
     </row>
-    <row r="254" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A254" s="12"/>
       <c r="B254" s="13"/>
       <c r="C254" s="12"/>
       <c r="D254" s="13"/>
       <c r="E254" s="13"/>
     </row>
-    <row r="255" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A255" s="12"/>
       <c r="B255" s="13"/>
       <c r="C255" s="12"/>
       <c r="D255" s="13"/>
       <c r="E255" s="13"/>
     </row>
-    <row r="256" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A256" s="12"/>
       <c r="B256" s="13"/>
       <c r="C256" s="12"/>
       <c r="D256" s="13"/>
       <c r="E256" s="13"/>
     </row>
-    <row r="257" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A257" s="12"/>
       <c r="B257" s="13"/>
       <c r="C257" s="12"/>
       <c r="D257" s="13"/>
       <c r="E257" s="13"/>
     </row>
-    <row r="258" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="258" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A258" s="12"/>
       <c r="B258" s="13"/>
       <c r="C258" s="12"/>
       <c r="D258" s="13"/>
       <c r="E258" s="13"/>
     </row>
-    <row r="259" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="259" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A259" s="12"/>
       <c r="B259" s="13"/>
       <c r="C259" s="12"/>
       <c r="D259" s="13"/>
       <c r="E259" s="13"/>
     </row>
-    <row r="260" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="260" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A260" s="12"/>
       <c r="B260" s="13"/>
       <c r="C260" s="12"/>
@@ -2991,10 +3007,11 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D27" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="D28" r:id="rId2" xr:uid="{4877334E-7528-4DFA-87BA-7232CC222E39}"/>
-    <hyperlink ref="D29" r:id="rId3" xr:uid="{BD98EB24-72D1-47EA-9C38-88A632EFC407}"/>
-    <hyperlink ref="D30" r:id="rId4" xr:uid="{2B1F1BE8-9B38-49F3-BF80-B549935EB25B}"/>
+    <hyperlink ref="D27" r:id="rId1"/>
+    <hyperlink ref="D28" r:id="rId2"/>
+    <hyperlink ref="D29" r:id="rId3"/>
+    <hyperlink ref="D30" r:id="rId4"/>
+    <hyperlink ref="D31" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Se agrega  Alumno N° 31
</commit_message>
<xml_diff>
--- a/Lista de Alumnos.xlsx
+++ b/Lista de Alumnos.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MONTAÑO ANDRES\Desktop\proyecto1\Alumnos\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570"/>
+    <workbookView xWindow="-102" yWindow="-102" windowWidth="18580" windowHeight="11698"/>
   </bookViews>
   <sheets>
     <sheet name="Electronica Microcontrolada" sheetId="1" r:id="rId1"/>
@@ -19,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="97">
   <si>
     <t>#</t>
   </si>
@@ -301,6 +296,15 @@
   </si>
   <si>
     <t>maj3210</t>
+  </si>
+  <si>
+    <t>Fede Birge</t>
+  </si>
+  <si>
+    <t>fedeikky@gmail.com</t>
+  </si>
+  <si>
+    <t>FedeBirge</t>
   </si>
 </sst>
 </file>
@@ -809,19 +813,19 @@
   <dimension ref="A1:E260"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.65" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.85546875" style="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="37.140625" style="15" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.5703125" style="14" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.88671875" style="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.109375" style="15" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5546875" style="14" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="31" style="15" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="29" style="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" ht="27.1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -838,7 +842,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="19.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -855,7 +859,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="19.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>2</v>
       </c>
@@ -870,7 +874,7 @@
       </c>
       <c r="E3" s="6"/>
     </row>
-    <row r="4" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="19.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>3</v>
       </c>
@@ -887,7 +891,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="19.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>4</v>
       </c>
@@ -904,7 +908,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="19.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>5</v>
       </c>
@@ -921,7 +925,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="19.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>6</v>
       </c>
@@ -938,7 +942,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="19.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>7</v>
       </c>
@@ -955,7 +959,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="19.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>8</v>
       </c>
@@ -972,7 +976,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="19.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>9</v>
       </c>
@@ -987,7 +991,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="19.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <v>10</v>
       </c>
@@ -1004,7 +1008,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="19.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>11</v>
       </c>
@@ -1021,7 +1025,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" ht="19.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="5">
         <v>12</v>
       </c>
@@ -1038,7 +1042,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" ht="19.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
         <v>13</v>
       </c>
@@ -1055,7 +1059,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" ht="19.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
         <v>14</v>
       </c>
@@ -1072,7 +1076,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" ht="19.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
         <v>15</v>
       </c>
@@ -1089,7 +1093,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" ht="19.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
         <v>16</v>
       </c>
@@ -1106,7 +1110,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" ht="19.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <v>17</v>
       </c>
@@ -1123,7 +1127,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" ht="19.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
         <v>18</v>
       </c>
@@ -1140,7 +1144,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" ht="19.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
         <v>19</v>
       </c>
@@ -1157,7 +1161,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" ht="19.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="5">
         <v>20</v>
       </c>
@@ -1327,7 +1331,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="5">
         <v>30</v>
       </c>
@@ -1344,14 +1348,22 @@
         <v>93</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="5">
         <v>31</v>
       </c>
-      <c r="B32" s="6"/>
-      <c r="C32" s="5"/>
-      <c r="D32" s="6"/>
-      <c r="E32" s="6"/>
+      <c r="B32" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="C32" s="5">
+        <v>2</v>
+      </c>
+      <c r="D32" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="E32" s="6" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="33" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="5">
@@ -1389,7 +1401,7 @@
       <c r="D36" s="6"/>
       <c r="E36" s="6"/>
     </row>
-    <row r="37" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="5">
         <v>36</v>
       </c>
@@ -1398,7 +1410,7 @@
       <c r="D37" s="6"/>
       <c r="E37" s="6"/>
     </row>
-    <row r="38" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="5">
         <v>37</v>
       </c>
@@ -1407,7 +1419,7 @@
       <c r="D38" s="6"/>
       <c r="E38" s="6"/>
     </row>
-    <row r="39" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="5">
         <v>38</v>
       </c>
@@ -1416,7 +1428,7 @@
       <c r="D39" s="6"/>
       <c r="E39" s="6"/>
     </row>
-    <row r="40" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="5">
         <v>39</v>
       </c>
@@ -1425,7 +1437,7 @@
       <c r="D40" s="6"/>
       <c r="E40" s="6"/>
     </row>
-    <row r="41" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="5">
         <v>40</v>
       </c>
@@ -1434,7 +1446,7 @@
       <c r="D41" s="6"/>
       <c r="E41" s="6"/>
     </row>
-    <row r="42" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="5">
         <v>41</v>
       </c>
@@ -1443,7 +1455,7 @@
       <c r="D42" s="6"/>
       <c r="E42" s="6"/>
     </row>
-    <row r="43" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="5">
         <v>42</v>
       </c>
@@ -1452,7 +1464,7 @@
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
     </row>
-    <row r="44" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="5">
         <v>43</v>
       </c>
@@ -1461,7 +1473,7 @@
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
     </row>
-    <row r="45" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="5">
         <v>44</v>
       </c>
@@ -1470,7 +1482,7 @@
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
     </row>
-    <row r="46" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="5">
         <v>45</v>
       </c>
@@ -1479,7 +1491,7 @@
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
     </row>
-    <row r="47" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="5">
         <v>46</v>
       </c>
@@ -1488,7 +1500,7 @@
       <c r="D47" s="6"/>
       <c r="E47" s="6"/>
     </row>
-    <row r="48" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="5">
         <v>47</v>
       </c>
@@ -1497,7 +1509,7 @@
       <c r="D48" s="6"/>
       <c r="E48" s="6"/>
     </row>
-    <row r="49" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="5">
         <v>48</v>
       </c>
@@ -1506,7 +1518,7 @@
       <c r="D49" s="6"/>
       <c r="E49" s="6"/>
     </row>
-    <row r="50" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="5">
         <v>49</v>
       </c>
@@ -1515,7 +1527,7 @@
       <c r="D50" s="6"/>
       <c r="E50" s="6"/>
     </row>
-    <row r="51" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="5">
         <v>50</v>
       </c>
@@ -1524,7 +1536,7 @@
       <c r="D51" s="6"/>
       <c r="E51" s="6"/>
     </row>
-    <row r="52" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="5">
         <v>51</v>
       </c>
@@ -1533,7 +1545,7 @@
       <c r="D52" s="6"/>
       <c r="E52" s="6"/>
     </row>
-    <row r="53" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="5">
         <v>52</v>
       </c>
@@ -1542,7 +1554,7 @@
       <c r="D53" s="6"/>
       <c r="E53" s="6"/>
     </row>
-    <row r="54" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="5">
         <v>53</v>
       </c>
@@ -1551,7 +1563,7 @@
       <c r="D54" s="6"/>
       <c r="E54" s="6"/>
     </row>
-    <row r="55" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="5">
         <v>54</v>
       </c>
@@ -1560,7 +1572,7 @@
       <c r="D55" s="6"/>
       <c r="E55" s="6"/>
     </row>
-    <row r="56" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="5">
         <v>55</v>
       </c>
@@ -1569,7 +1581,7 @@
       <c r="D56" s="6"/>
       <c r="E56" s="6"/>
     </row>
-    <row r="57" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="5">
         <v>56</v>
       </c>
@@ -1578,7 +1590,7 @@
       <c r="D57" s="6"/>
       <c r="E57" s="6"/>
     </row>
-    <row r="58" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="5">
         <v>57</v>
       </c>
@@ -1587,7 +1599,7 @@
       <c r="D58" s="6"/>
       <c r="E58" s="6"/>
     </row>
-    <row r="59" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="5">
         <v>58</v>
       </c>
@@ -1596,7 +1608,7 @@
       <c r="D59" s="6"/>
       <c r="E59" s="6"/>
     </row>
-    <row r="60" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" s="5">
         <v>59</v>
       </c>
@@ -1605,1400 +1617,1400 @@
       <c r="D60" s="6"/>
       <c r="E60" s="6"/>
     </row>
-    <row r="61" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" s="12"/>
       <c r="B61" s="13"/>
       <c r="C61" s="12"/>
       <c r="D61" s="13"/>
       <c r="E61" s="13"/>
     </row>
-    <row r="62" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" s="12"/>
       <c r="B62" s="13"/>
       <c r="C62" s="12"/>
       <c r="D62" s="13"/>
       <c r="E62" s="13"/>
     </row>
-    <row r="63" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" s="12"/>
       <c r="B63" s="13"/>
       <c r="C63" s="12"/>
       <c r="D63" s="13"/>
       <c r="E63" s="13"/>
     </row>
-    <row r="64" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" s="12"/>
       <c r="B64" s="13"/>
       <c r="C64" s="12"/>
       <c r="D64" s="13"/>
       <c r="E64" s="13"/>
     </row>
-    <row r="65" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A65" s="12"/>
       <c r="B65" s="13"/>
       <c r="C65" s="12"/>
       <c r="D65" s="13"/>
       <c r="E65" s="13"/>
     </row>
-    <row r="66" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A66" s="12"/>
       <c r="B66" s="13"/>
       <c r="C66" s="12"/>
       <c r="D66" s="13"/>
       <c r="E66" s="13"/>
     </row>
-    <row r="67" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67" s="12"/>
       <c r="B67" s="13"/>
       <c r="C67" s="12"/>
       <c r="D67" s="13"/>
       <c r="E67" s="13"/>
     </row>
-    <row r="68" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" s="12"/>
       <c r="B68" s="13"/>
       <c r="C68" s="12"/>
       <c r="D68" s="13"/>
       <c r="E68" s="13"/>
     </row>
-    <row r="69" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69" s="12"/>
       <c r="B69" s="13"/>
       <c r="C69" s="12"/>
       <c r="D69" s="13"/>
       <c r="E69" s="13"/>
     </row>
-    <row r="70" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A70" s="12"/>
       <c r="B70" s="13"/>
       <c r="C70" s="12"/>
       <c r="D70" s="13"/>
       <c r="E70" s="13"/>
     </row>
-    <row r="71" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A71" s="12"/>
       <c r="B71" s="13"/>
       <c r="C71" s="12"/>
       <c r="D71" s="13"/>
       <c r="E71" s="13"/>
     </row>
-    <row r="72" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72" s="12"/>
       <c r="B72" s="13"/>
       <c r="C72" s="12"/>
       <c r="D72" s="13"/>
       <c r="E72" s="13"/>
     </row>
-    <row r="73" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A73" s="12"/>
       <c r="B73" s="13"/>
       <c r="C73" s="12"/>
       <c r="D73" s="13"/>
       <c r="E73" s="13"/>
     </row>
-    <row r="74" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A74" s="12"/>
       <c r="B74" s="13"/>
       <c r="C74" s="12"/>
       <c r="D74" s="13"/>
       <c r="E74" s="13"/>
     </row>
-    <row r="75" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A75" s="12"/>
       <c r="B75" s="13"/>
       <c r="C75" s="12"/>
       <c r="D75" s="13"/>
       <c r="E75" s="13"/>
     </row>
-    <row r="76" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A76" s="12"/>
       <c r="B76" s="13"/>
       <c r="C76" s="12"/>
       <c r="D76" s="13"/>
       <c r="E76" s="13"/>
     </row>
-    <row r="77" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A77" s="12"/>
       <c r="B77" s="13"/>
       <c r="C77" s="12"/>
       <c r="D77" s="13"/>
       <c r="E77" s="13"/>
     </row>
-    <row r="78" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A78" s="12"/>
       <c r="B78" s="13"/>
       <c r="C78" s="12"/>
       <c r="D78" s="13"/>
       <c r="E78" s="13"/>
     </row>
-    <row r="79" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A79" s="12"/>
       <c r="B79" s="13"/>
       <c r="C79" s="12"/>
       <c r="D79" s="13"/>
       <c r="E79" s="13"/>
     </row>
-    <row r="80" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A80" s="12"/>
       <c r="B80" s="13"/>
       <c r="C80" s="12"/>
       <c r="D80" s="13"/>
       <c r="E80" s="13"/>
     </row>
-    <row r="81" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A81" s="12"/>
       <c r="B81" s="13"/>
       <c r="C81" s="12"/>
       <c r="D81" s="13"/>
       <c r="E81" s="13"/>
     </row>
-    <row r="82" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A82" s="12"/>
       <c r="B82" s="13"/>
       <c r="C82" s="12"/>
       <c r="D82" s="13"/>
       <c r="E82" s="13"/>
     </row>
-    <row r="83" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A83" s="12"/>
       <c r="B83" s="13"/>
       <c r="C83" s="12"/>
       <c r="D83" s="13"/>
       <c r="E83" s="13"/>
     </row>
-    <row r="84" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A84" s="12"/>
       <c r="B84" s="13"/>
       <c r="C84" s="12"/>
       <c r="D84" s="13"/>
       <c r="E84" s="13"/>
     </row>
-    <row r="85" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A85" s="12"/>
       <c r="B85" s="13"/>
       <c r="C85" s="12"/>
       <c r="D85" s="13"/>
       <c r="E85" s="13"/>
     </row>
-    <row r="86" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A86" s="12"/>
       <c r="B86" s="13"/>
       <c r="C86" s="12"/>
       <c r="D86" s="13"/>
       <c r="E86" s="13"/>
     </row>
-    <row r="87" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A87" s="12"/>
       <c r="B87" s="13"/>
       <c r="C87" s="12"/>
       <c r="D87" s="13"/>
       <c r="E87" s="13"/>
     </row>
-    <row r="88" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A88" s="12"/>
       <c r="B88" s="13"/>
       <c r="C88" s="12"/>
       <c r="D88" s="13"/>
       <c r="E88" s="13"/>
     </row>
-    <row r="89" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A89" s="12"/>
       <c r="B89" s="13"/>
       <c r="C89" s="12"/>
       <c r="D89" s="13"/>
       <c r="E89" s="13"/>
     </row>
-    <row r="90" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A90" s="12"/>
       <c r="B90" s="13"/>
       <c r="C90" s="12"/>
       <c r="D90" s="13"/>
       <c r="E90" s="13"/>
     </row>
-    <row r="91" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A91" s="12"/>
       <c r="B91" s="13"/>
       <c r="C91" s="12"/>
       <c r="D91" s="13"/>
       <c r="E91" s="13"/>
     </row>
-    <row r="92" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A92" s="12"/>
       <c r="B92" s="13"/>
       <c r="C92" s="12"/>
       <c r="D92" s="13"/>
       <c r="E92" s="13"/>
     </row>
-    <row r="93" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A93" s="12"/>
       <c r="B93" s="13"/>
       <c r="C93" s="12"/>
       <c r="D93" s="13"/>
       <c r="E93" s="13"/>
     </row>
-    <row r="94" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A94" s="12"/>
       <c r="B94" s="13"/>
       <c r="C94" s="12"/>
       <c r="D94" s="13"/>
       <c r="E94" s="13"/>
     </row>
-    <row r="95" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A95" s="12"/>
       <c r="B95" s="13"/>
       <c r="C95" s="12"/>
       <c r="D95" s="13"/>
       <c r="E95" s="13"/>
     </row>
-    <row r="96" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A96" s="12"/>
       <c r="B96" s="13"/>
       <c r="C96" s="12"/>
       <c r="D96" s="13"/>
       <c r="E96" s="13"/>
     </row>
-    <row r="97" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A97" s="12"/>
       <c r="B97" s="13"/>
       <c r="C97" s="12"/>
       <c r="D97" s="13"/>
       <c r="E97" s="13"/>
     </row>
-    <row r="98" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A98" s="12"/>
       <c r="B98" s="13"/>
       <c r="C98" s="12"/>
       <c r="D98" s="13"/>
       <c r="E98" s="13"/>
     </row>
-    <row r="99" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A99" s="12"/>
       <c r="B99" s="13"/>
       <c r="C99" s="12"/>
       <c r="D99" s="13"/>
       <c r="E99" s="13"/>
     </row>
-    <row r="100" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A100" s="12"/>
       <c r="B100" s="13"/>
       <c r="C100" s="12"/>
       <c r="D100" s="13"/>
       <c r="E100" s="13"/>
     </row>
-    <row r="101" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A101" s="12"/>
       <c r="B101" s="13"/>
       <c r="C101" s="12"/>
       <c r="D101" s="13"/>
       <c r="E101" s="13"/>
     </row>
-    <row r="102" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A102" s="12"/>
       <c r="B102" s="13"/>
       <c r="C102" s="12"/>
       <c r="D102" s="13"/>
       <c r="E102" s="13"/>
     </row>
-    <row r="103" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A103" s="12"/>
       <c r="B103" s="13"/>
       <c r="C103" s="12"/>
       <c r="D103" s="13"/>
       <c r="E103" s="13"/>
     </row>
-    <row r="104" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A104" s="12"/>
       <c r="B104" s="13"/>
       <c r="C104" s="12"/>
       <c r="D104" s="13"/>
       <c r="E104" s="13"/>
     </row>
-    <row r="105" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A105" s="12"/>
       <c r="B105" s="13"/>
       <c r="C105" s="12"/>
       <c r="D105" s="13"/>
       <c r="E105" s="13"/>
     </row>
-    <row r="106" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A106" s="12"/>
       <c r="B106" s="13"/>
       <c r="C106" s="12"/>
       <c r="D106" s="13"/>
       <c r="E106" s="13"/>
     </row>
-    <row r="107" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A107" s="12"/>
       <c r="B107" s="13"/>
       <c r="C107" s="12"/>
       <c r="D107" s="13"/>
       <c r="E107" s="13"/>
     </row>
-    <row r="108" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A108" s="12"/>
       <c r="B108" s="13"/>
       <c r="C108" s="12"/>
       <c r="D108" s="13"/>
       <c r="E108" s="13"/>
     </row>
-    <row r="109" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A109" s="12"/>
       <c r="B109" s="13"/>
       <c r="C109" s="12"/>
       <c r="D109" s="13"/>
       <c r="E109" s="13"/>
     </row>
-    <row r="110" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A110" s="12"/>
       <c r="B110" s="13"/>
       <c r="C110" s="12"/>
       <c r="D110" s="13"/>
       <c r="E110" s="13"/>
     </row>
-    <row r="111" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A111" s="12"/>
       <c r="B111" s="13"/>
       <c r="C111" s="12"/>
       <c r="D111" s="13"/>
       <c r="E111" s="13"/>
     </row>
-    <row r="112" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A112" s="12"/>
       <c r="B112" s="13"/>
       <c r="C112" s="12"/>
       <c r="D112" s="13"/>
       <c r="E112" s="13"/>
     </row>
-    <row r="113" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A113" s="12"/>
       <c r="B113" s="13"/>
       <c r="C113" s="12"/>
       <c r="D113" s="13"/>
       <c r="E113" s="13"/>
     </row>
-    <row r="114" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A114" s="12"/>
       <c r="B114" s="13"/>
       <c r="C114" s="12"/>
       <c r="D114" s="13"/>
       <c r="E114" s="13"/>
     </row>
-    <row r="115" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A115" s="12"/>
       <c r="B115" s="13"/>
       <c r="C115" s="12"/>
       <c r="D115" s="13"/>
       <c r="E115" s="13"/>
     </row>
-    <row r="116" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A116" s="12"/>
       <c r="B116" s="13"/>
       <c r="C116" s="12"/>
       <c r="D116" s="13"/>
       <c r="E116" s="13"/>
     </row>
-    <row r="117" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A117" s="12"/>
       <c r="B117" s="13"/>
       <c r="C117" s="12"/>
       <c r="D117" s="13"/>
       <c r="E117" s="13"/>
     </row>
-    <row r="118" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A118" s="12"/>
       <c r="B118" s="13"/>
       <c r="C118" s="12"/>
       <c r="D118" s="13"/>
       <c r="E118" s="13"/>
     </row>
-    <row r="119" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A119" s="12"/>
       <c r="B119" s="13"/>
       <c r="C119" s="12"/>
       <c r="D119" s="13"/>
       <c r="E119" s="13"/>
     </row>
-    <row r="120" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A120" s="12"/>
       <c r="B120" s="13"/>
       <c r="C120" s="12"/>
       <c r="D120" s="13"/>
       <c r="E120" s="13"/>
     </row>
-    <row r="121" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A121" s="12"/>
       <c r="B121" s="13"/>
       <c r="C121" s="12"/>
       <c r="D121" s="13"/>
       <c r="E121" s="13"/>
     </row>
-    <row r="122" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A122" s="12"/>
       <c r="B122" s="13"/>
       <c r="C122" s="12"/>
       <c r="D122" s="13"/>
       <c r="E122" s="13"/>
     </row>
-    <row r="123" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A123" s="12"/>
       <c r="B123" s="13"/>
       <c r="C123" s="12"/>
       <c r="D123" s="13"/>
       <c r="E123" s="13"/>
     </row>
-    <row r="124" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A124" s="12"/>
       <c r="B124" s="13"/>
       <c r="C124" s="12"/>
       <c r="D124" s="13"/>
       <c r="E124" s="13"/>
     </row>
-    <row r="125" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A125" s="12"/>
       <c r="B125" s="13"/>
       <c r="C125" s="12"/>
       <c r="D125" s="13"/>
       <c r="E125" s="13"/>
     </row>
-    <row r="126" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A126" s="12"/>
       <c r="B126" s="13"/>
       <c r="C126" s="12"/>
       <c r="D126" s="13"/>
       <c r="E126" s="13"/>
     </row>
-    <row r="127" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A127" s="12"/>
       <c r="B127" s="13"/>
       <c r="C127" s="12"/>
       <c r="D127" s="13"/>
       <c r="E127" s="13"/>
     </row>
-    <row r="128" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A128" s="12"/>
       <c r="B128" s="13"/>
       <c r="C128" s="12"/>
       <c r="D128" s="13"/>
       <c r="E128" s="13"/>
     </row>
-    <row r="129" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A129" s="12"/>
       <c r="B129" s="13"/>
       <c r="C129" s="12"/>
       <c r="D129" s="13"/>
       <c r="E129" s="13"/>
     </row>
-    <row r="130" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A130" s="12"/>
       <c r="B130" s="13"/>
       <c r="C130" s="12"/>
       <c r="D130" s="13"/>
       <c r="E130" s="13"/>
     </row>
-    <row r="131" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A131" s="12"/>
       <c r="B131" s="13"/>
       <c r="C131" s="12"/>
       <c r="D131" s="13"/>
       <c r="E131" s="13"/>
     </row>
-    <row r="132" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A132" s="12"/>
       <c r="B132" s="13"/>
       <c r="C132" s="12"/>
       <c r="D132" s="13"/>
       <c r="E132" s="13"/>
     </row>
-    <row r="133" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A133" s="12"/>
       <c r="B133" s="13"/>
       <c r="C133" s="12"/>
       <c r="D133" s="13"/>
       <c r="E133" s="13"/>
     </row>
-    <row r="134" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A134" s="12"/>
       <c r="B134" s="13"/>
       <c r="C134" s="12"/>
       <c r="D134" s="13"/>
       <c r="E134" s="13"/>
     </row>
-    <row r="135" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A135" s="12"/>
       <c r="B135" s="13"/>
       <c r="C135" s="12"/>
       <c r="D135" s="13"/>
       <c r="E135" s="13"/>
     </row>
-    <row r="136" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A136" s="12"/>
       <c r="B136" s="13"/>
       <c r="C136" s="12"/>
       <c r="D136" s="13"/>
       <c r="E136" s="13"/>
     </row>
-    <row r="137" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A137" s="12"/>
       <c r="B137" s="13"/>
       <c r="C137" s="12"/>
       <c r="D137" s="13"/>
       <c r="E137" s="13"/>
     </row>
-    <row r="138" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A138" s="12"/>
       <c r="B138" s="13"/>
       <c r="C138" s="12"/>
       <c r="D138" s="13"/>
       <c r="E138" s="13"/>
     </row>
-    <row r="139" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A139" s="12"/>
       <c r="B139" s="13"/>
       <c r="C139" s="12"/>
       <c r="D139" s="13"/>
       <c r="E139" s="13"/>
     </row>
-    <row r="140" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A140" s="12"/>
       <c r="B140" s="13"/>
       <c r="C140" s="12"/>
       <c r="D140" s="13"/>
       <c r="E140" s="13"/>
     </row>
-    <row r="141" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A141" s="12"/>
       <c r="B141" s="13"/>
       <c r="C141" s="12"/>
       <c r="D141" s="13"/>
       <c r="E141" s="13"/>
     </row>
-    <row r="142" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A142" s="12"/>
       <c r="B142" s="13"/>
       <c r="C142" s="12"/>
       <c r="D142" s="13"/>
       <c r="E142" s="13"/>
     </row>
-    <row r="143" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A143" s="12"/>
       <c r="B143" s="13"/>
       <c r="C143" s="12"/>
       <c r="D143" s="13"/>
       <c r="E143" s="13"/>
     </row>
-    <row r="144" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A144" s="12"/>
       <c r="B144" s="13"/>
       <c r="C144" s="12"/>
       <c r="D144" s="13"/>
       <c r="E144" s="13"/>
     </row>
-    <row r="145" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A145" s="12"/>
       <c r="B145" s="13"/>
       <c r="C145" s="12"/>
       <c r="D145" s="13"/>
       <c r="E145" s="13"/>
     </row>
-    <row r="146" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A146" s="12"/>
       <c r="B146" s="13"/>
       <c r="C146" s="12"/>
       <c r="D146" s="13"/>
       <c r="E146" s="13"/>
     </row>
-    <row r="147" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A147" s="12"/>
       <c r="B147" s="13"/>
       <c r="C147" s="12"/>
       <c r="D147" s="13"/>
       <c r="E147" s="13"/>
     </row>
-    <row r="148" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A148" s="12"/>
       <c r="B148" s="13"/>
       <c r="C148" s="12"/>
       <c r="D148" s="13"/>
       <c r="E148" s="13"/>
     </row>
-    <row r="149" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A149" s="12"/>
       <c r="B149" s="13"/>
       <c r="C149" s="12"/>
       <c r="D149" s="13"/>
       <c r="E149" s="13"/>
     </row>
-    <row r="150" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A150" s="12"/>
       <c r="B150" s="13"/>
       <c r="C150" s="12"/>
       <c r="D150" s="13"/>
       <c r="E150" s="13"/>
     </row>
-    <row r="151" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A151" s="12"/>
       <c r="B151" s="13"/>
       <c r="C151" s="12"/>
       <c r="D151" s="13"/>
       <c r="E151" s="13"/>
     </row>
-    <row r="152" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A152" s="12"/>
       <c r="B152" s="13"/>
       <c r="C152" s="12"/>
       <c r="D152" s="13"/>
       <c r="E152" s="13"/>
     </row>
-    <row r="153" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A153" s="12"/>
       <c r="B153" s="13"/>
       <c r="C153" s="12"/>
       <c r="D153" s="13"/>
       <c r="E153" s="13"/>
     </row>
-    <row r="154" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A154" s="12"/>
       <c r="B154" s="13"/>
       <c r="C154" s="12"/>
       <c r="D154" s="13"/>
       <c r="E154" s="13"/>
     </row>
-    <row r="155" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A155" s="12"/>
       <c r="B155" s="13"/>
       <c r="C155" s="12"/>
       <c r="D155" s="13"/>
       <c r="E155" s="13"/>
     </row>
-    <row r="156" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A156" s="12"/>
       <c r="B156" s="13"/>
       <c r="C156" s="12"/>
       <c r="D156" s="13"/>
       <c r="E156" s="13"/>
     </row>
-    <row r="157" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A157" s="12"/>
       <c r="B157" s="13"/>
       <c r="C157" s="12"/>
       <c r="D157" s="13"/>
       <c r="E157" s="13"/>
     </row>
-    <row r="158" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A158" s="12"/>
       <c r="B158" s="13"/>
       <c r="C158" s="12"/>
       <c r="D158" s="13"/>
       <c r="E158" s="13"/>
     </row>
-    <row r="159" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A159" s="12"/>
       <c r="B159" s="13"/>
       <c r="C159" s="12"/>
       <c r="D159" s="13"/>
       <c r="E159" s="13"/>
     </row>
-    <row r="160" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A160" s="12"/>
       <c r="B160" s="13"/>
       <c r="C160" s="12"/>
       <c r="D160" s="13"/>
       <c r="E160" s="13"/>
     </row>
-    <row r="161" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A161" s="12"/>
       <c r="B161" s="13"/>
       <c r="C161" s="12"/>
       <c r="D161" s="13"/>
       <c r="E161" s="13"/>
     </row>
-    <row r="162" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A162" s="12"/>
       <c r="B162" s="13"/>
       <c r="C162" s="12"/>
       <c r="D162" s="13"/>
       <c r="E162" s="13"/>
     </row>
-    <row r="163" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A163" s="12"/>
       <c r="B163" s="13"/>
       <c r="C163" s="12"/>
       <c r="D163" s="13"/>
       <c r="E163" s="13"/>
     </row>
-    <row r="164" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A164" s="12"/>
       <c r="B164" s="13"/>
       <c r="C164" s="12"/>
       <c r="D164" s="13"/>
       <c r="E164" s="13"/>
     </row>
-    <row r="165" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A165" s="12"/>
       <c r="B165" s="13"/>
       <c r="C165" s="12"/>
       <c r="D165" s="13"/>
       <c r="E165" s="13"/>
     </row>
-    <row r="166" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A166" s="12"/>
       <c r="B166" s="13"/>
       <c r="C166" s="12"/>
       <c r="D166" s="13"/>
       <c r="E166" s="13"/>
     </row>
-    <row r="167" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A167" s="12"/>
       <c r="B167" s="13"/>
       <c r="C167" s="12"/>
       <c r="D167" s="13"/>
       <c r="E167" s="13"/>
     </row>
-    <row r="168" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A168" s="12"/>
       <c r="B168" s="13"/>
       <c r="C168" s="12"/>
       <c r="D168" s="13"/>
       <c r="E168" s="13"/>
     </row>
-    <row r="169" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A169" s="12"/>
       <c r="B169" s="13"/>
       <c r="C169" s="12"/>
       <c r="D169" s="13"/>
       <c r="E169" s="13"/>
     </row>
-    <row r="170" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A170" s="12"/>
       <c r="B170" s="13"/>
       <c r="C170" s="12"/>
       <c r="D170" s="13"/>
       <c r="E170" s="13"/>
     </row>
-    <row r="171" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A171" s="12"/>
       <c r="B171" s="13"/>
       <c r="C171" s="12"/>
       <c r="D171" s="13"/>
       <c r="E171" s="13"/>
     </row>
-    <row r="172" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A172" s="12"/>
       <c r="B172" s="13"/>
       <c r="C172" s="12"/>
       <c r="D172" s="13"/>
       <c r="E172" s="13"/>
     </row>
-    <row r="173" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A173" s="12"/>
       <c r="B173" s="13"/>
       <c r="C173" s="12"/>
       <c r="D173" s="13"/>
       <c r="E173" s="13"/>
     </row>
-    <row r="174" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A174" s="12"/>
       <c r="B174" s="13"/>
       <c r="C174" s="12"/>
       <c r="D174" s="13"/>
       <c r="E174" s="13"/>
     </row>
-    <row r="175" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A175" s="12"/>
       <c r="B175" s="13"/>
       <c r="C175" s="12"/>
       <c r="D175" s="13"/>
       <c r="E175" s="13"/>
     </row>
-    <row r="176" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A176" s="12"/>
       <c r="B176" s="13"/>
       <c r="C176" s="12"/>
       <c r="D176" s="13"/>
       <c r="E176" s="13"/>
     </row>
-    <row r="177" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A177" s="12"/>
       <c r="B177" s="13"/>
       <c r="C177" s="12"/>
       <c r="D177" s="13"/>
       <c r="E177" s="13"/>
     </row>
-    <row r="178" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A178" s="12"/>
       <c r="B178" s="13"/>
       <c r="C178" s="12"/>
       <c r="D178" s="13"/>
       <c r="E178" s="13"/>
     </row>
-    <row r="179" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A179" s="12"/>
       <c r="B179" s="13"/>
       <c r="C179" s="12"/>
       <c r="D179" s="13"/>
       <c r="E179" s="13"/>
     </row>
-    <row r="180" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A180" s="12"/>
       <c r="B180" s="13"/>
       <c r="C180" s="12"/>
       <c r="D180" s="13"/>
       <c r="E180" s="13"/>
     </row>
-    <row r="181" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A181" s="12"/>
       <c r="B181" s="13"/>
       <c r="C181" s="12"/>
       <c r="D181" s="13"/>
       <c r="E181" s="13"/>
     </row>
-    <row r="182" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A182" s="12"/>
       <c r="B182" s="13"/>
       <c r="C182" s="12"/>
       <c r="D182" s="13"/>
       <c r="E182" s="13"/>
     </row>
-    <row r="183" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A183" s="12"/>
       <c r="B183" s="13"/>
       <c r="C183" s="12"/>
       <c r="D183" s="13"/>
       <c r="E183" s="13"/>
     </row>
-    <row r="184" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A184" s="12"/>
       <c r="B184" s="13"/>
       <c r="C184" s="12"/>
       <c r="D184" s="13"/>
       <c r="E184" s="13"/>
     </row>
-    <row r="185" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A185" s="12"/>
       <c r="B185" s="13"/>
       <c r="C185" s="12"/>
       <c r="D185" s="13"/>
       <c r="E185" s="13"/>
     </row>
-    <row r="186" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A186" s="12"/>
       <c r="B186" s="13"/>
       <c r="C186" s="12"/>
       <c r="D186" s="13"/>
       <c r="E186" s="13"/>
     </row>
-    <row r="187" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A187" s="12"/>
       <c r="B187" s="13"/>
       <c r="C187" s="12"/>
       <c r="D187" s="13"/>
       <c r="E187" s="13"/>
     </row>
-    <row r="188" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A188" s="12"/>
       <c r="B188" s="13"/>
       <c r="C188" s="12"/>
       <c r="D188" s="13"/>
       <c r="E188" s="13"/>
     </row>
-    <row r="189" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A189" s="12"/>
       <c r="B189" s="13"/>
       <c r="C189" s="12"/>
       <c r="D189" s="13"/>
       <c r="E189" s="13"/>
     </row>
-    <row r="190" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A190" s="12"/>
       <c r="B190" s="13"/>
       <c r="C190" s="12"/>
       <c r="D190" s="13"/>
       <c r="E190" s="13"/>
     </row>
-    <row r="191" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A191" s="12"/>
       <c r="B191" s="13"/>
       <c r="C191" s="12"/>
       <c r="D191" s="13"/>
       <c r="E191" s="13"/>
     </row>
-    <row r="192" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A192" s="12"/>
       <c r="B192" s="13"/>
       <c r="C192" s="12"/>
       <c r="D192" s="13"/>
       <c r="E192" s="13"/>
     </row>
-    <row r="193" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A193" s="12"/>
       <c r="B193" s="13"/>
       <c r="C193" s="12"/>
       <c r="D193" s="13"/>
       <c r="E193" s="13"/>
     </row>
-    <row r="194" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A194" s="12"/>
       <c r="B194" s="13"/>
       <c r="C194" s="12"/>
       <c r="D194" s="13"/>
       <c r="E194" s="13"/>
     </row>
-    <row r="195" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A195" s="12"/>
       <c r="B195" s="13"/>
       <c r="C195" s="12"/>
       <c r="D195" s="13"/>
       <c r="E195" s="13"/>
     </row>
-    <row r="196" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A196" s="12"/>
       <c r="B196" s="13"/>
       <c r="C196" s="12"/>
       <c r="D196" s="13"/>
       <c r="E196" s="13"/>
     </row>
-    <row r="197" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A197" s="12"/>
       <c r="B197" s="13"/>
       <c r="C197" s="12"/>
       <c r="D197" s="13"/>
       <c r="E197" s="13"/>
     </row>
-    <row r="198" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A198" s="12"/>
       <c r="B198" s="13"/>
       <c r="C198" s="12"/>
       <c r="D198" s="13"/>
       <c r="E198" s="13"/>
     </row>
-    <row r="199" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A199" s="12"/>
       <c r="B199" s="13"/>
       <c r="C199" s="12"/>
       <c r="D199" s="13"/>
       <c r="E199" s="13"/>
     </row>
-    <row r="200" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A200" s="12"/>
       <c r="B200" s="13"/>
       <c r="C200" s="12"/>
       <c r="D200" s="13"/>
       <c r="E200" s="13"/>
     </row>
-    <row r="201" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A201" s="12"/>
       <c r="B201" s="13"/>
       <c r="C201" s="12"/>
       <c r="D201" s="13"/>
       <c r="E201" s="13"/>
     </row>
-    <row r="202" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A202" s="12"/>
       <c r="B202" s="13"/>
       <c r="C202" s="12"/>
       <c r="D202" s="13"/>
       <c r="E202" s="13"/>
     </row>
-    <row r="203" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A203" s="12"/>
       <c r="B203" s="13"/>
       <c r="C203" s="12"/>
       <c r="D203" s="13"/>
       <c r="E203" s="13"/>
     </row>
-    <row r="204" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A204" s="12"/>
       <c r="B204" s="13"/>
       <c r="C204" s="12"/>
       <c r="D204" s="13"/>
       <c r="E204" s="13"/>
     </row>
-    <row r="205" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A205" s="12"/>
       <c r="B205" s="13"/>
       <c r="C205" s="12"/>
       <c r="D205" s="13"/>
       <c r="E205" s="13"/>
     </row>
-    <row r="206" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A206" s="12"/>
       <c r="B206" s="13"/>
       <c r="C206" s="12"/>
       <c r="D206" s="13"/>
       <c r="E206" s="13"/>
     </row>
-    <row r="207" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A207" s="12"/>
       <c r="B207" s="13"/>
       <c r="C207" s="12"/>
       <c r="D207" s="13"/>
       <c r="E207" s="13"/>
     </row>
-    <row r="208" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A208" s="12"/>
       <c r="B208" s="13"/>
       <c r="C208" s="12"/>
       <c r="D208" s="13"/>
       <c r="E208" s="13"/>
     </row>
-    <row r="209" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A209" s="12"/>
       <c r="B209" s="13"/>
       <c r="C209" s="12"/>
       <c r="D209" s="13"/>
       <c r="E209" s="13"/>
     </row>
-    <row r="210" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A210" s="12"/>
       <c r="B210" s="13"/>
       <c r="C210" s="12"/>
       <c r="D210" s="13"/>
       <c r="E210" s="13"/>
     </row>
-    <row r="211" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A211" s="12"/>
       <c r="B211" s="13"/>
       <c r="C211" s="12"/>
       <c r="D211" s="13"/>
       <c r="E211" s="13"/>
     </row>
-    <row r="212" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A212" s="12"/>
       <c r="B212" s="13"/>
       <c r="C212" s="12"/>
       <c r="D212" s="13"/>
       <c r="E212" s="13"/>
     </row>
-    <row r="213" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A213" s="12"/>
       <c r="B213" s="13"/>
       <c r="C213" s="12"/>
       <c r="D213" s="13"/>
       <c r="E213" s="13"/>
     </row>
-    <row r="214" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A214" s="12"/>
       <c r="B214" s="13"/>
       <c r="C214" s="12"/>
       <c r="D214" s="13"/>
       <c r="E214" s="13"/>
     </row>
-    <row r="215" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A215" s="12"/>
       <c r="B215" s="13"/>
       <c r="C215" s="12"/>
       <c r="D215" s="13"/>
       <c r="E215" s="13"/>
     </row>
-    <row r="216" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A216" s="12"/>
       <c r="B216" s="13"/>
       <c r="C216" s="12"/>
       <c r="D216" s="13"/>
       <c r="E216" s="13"/>
     </row>
-    <row r="217" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A217" s="12"/>
       <c r="B217" s="13"/>
       <c r="C217" s="12"/>
       <c r="D217" s="13"/>
       <c r="E217" s="13"/>
     </row>
-    <row r="218" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A218" s="12"/>
       <c r="B218" s="13"/>
       <c r="C218" s="12"/>
       <c r="D218" s="13"/>
       <c r="E218" s="13"/>
     </row>
-    <row r="219" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A219" s="12"/>
       <c r="B219" s="13"/>
       <c r="C219" s="12"/>
       <c r="D219" s="13"/>
       <c r="E219" s="13"/>
     </row>
-    <row r="220" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A220" s="12"/>
       <c r="B220" s="13"/>
       <c r="C220" s="12"/>
       <c r="D220" s="13"/>
       <c r="E220" s="13"/>
     </row>
-    <row r="221" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A221" s="12"/>
       <c r="B221" s="13"/>
       <c r="C221" s="12"/>
       <c r="D221" s="13"/>
       <c r="E221" s="13"/>
     </row>
-    <row r="222" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A222" s="12"/>
       <c r="B222" s="13"/>
       <c r="C222" s="12"/>
       <c r="D222" s="13"/>
       <c r="E222" s="13"/>
     </row>
-    <row r="223" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A223" s="12"/>
       <c r="B223" s="13"/>
       <c r="C223" s="12"/>
       <c r="D223" s="13"/>
       <c r="E223" s="13"/>
     </row>
-    <row r="224" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A224" s="12"/>
       <c r="B224" s="13"/>
       <c r="C224" s="12"/>
       <c r="D224" s="13"/>
       <c r="E224" s="13"/>
     </row>
-    <row r="225" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A225" s="12"/>
       <c r="B225" s="13"/>
       <c r="C225" s="12"/>
       <c r="D225" s="13"/>
       <c r="E225" s="13"/>
     </row>
-    <row r="226" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A226" s="12"/>
       <c r="B226" s="13"/>
       <c r="C226" s="12"/>
       <c r="D226" s="13"/>
       <c r="E226" s="13"/>
     </row>
-    <row r="227" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A227" s="12"/>
       <c r="B227" s="13"/>
       <c r="C227" s="12"/>
       <c r="D227" s="13"/>
       <c r="E227" s="13"/>
     </row>
-    <row r="228" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A228" s="12"/>
       <c r="B228" s="13"/>
       <c r="C228" s="12"/>
       <c r="D228" s="13"/>
       <c r="E228" s="13"/>
     </row>
-    <row r="229" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A229" s="12"/>
       <c r="B229" s="13"/>
       <c r="C229" s="12"/>
       <c r="D229" s="13"/>
       <c r="E229" s="13"/>
     </row>
-    <row r="230" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A230" s="12"/>
       <c r="B230" s="13"/>
       <c r="C230" s="12"/>
       <c r="D230" s="13"/>
       <c r="E230" s="13"/>
     </row>
-    <row r="231" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A231" s="12"/>
       <c r="B231" s="13"/>
       <c r="C231" s="12"/>
       <c r="D231" s="13"/>
       <c r="E231" s="13"/>
     </row>
-    <row r="232" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A232" s="12"/>
       <c r="B232" s="13"/>
       <c r="C232" s="12"/>
       <c r="D232" s="13"/>
       <c r="E232" s="13"/>
     </row>
-    <row r="233" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A233" s="12"/>
       <c r="B233" s="13"/>
       <c r="C233" s="12"/>
       <c r="D233" s="13"/>
       <c r="E233" s="13"/>
     </row>
-    <row r="234" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A234" s="12"/>
       <c r="B234" s="13"/>
       <c r="C234" s="12"/>
       <c r="D234" s="13"/>
       <c r="E234" s="13"/>
     </row>
-    <row r="235" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A235" s="12"/>
       <c r="B235" s="13"/>
       <c r="C235" s="12"/>
       <c r="D235" s="13"/>
       <c r="E235" s="13"/>
     </row>
-    <row r="236" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A236" s="12"/>
       <c r="B236" s="13"/>
       <c r="C236" s="12"/>
       <c r="D236" s="13"/>
       <c r="E236" s="13"/>
     </row>
-    <row r="237" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A237" s="12"/>
       <c r="B237" s="13"/>
       <c r="C237" s="12"/>
       <c r="D237" s="13"/>
       <c r="E237" s="13"/>
     </row>
-    <row r="238" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A238" s="12"/>
       <c r="B238" s="13"/>
       <c r="C238" s="12"/>
       <c r="D238" s="13"/>
       <c r="E238" s="13"/>
     </row>
-    <row r="239" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A239" s="12"/>
       <c r="B239" s="13"/>
       <c r="C239" s="12"/>
       <c r="D239" s="13"/>
       <c r="E239" s="13"/>
     </row>
-    <row r="240" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A240" s="12"/>
       <c r="B240" s="13"/>
       <c r="C240" s="12"/>
       <c r="D240" s="13"/>
       <c r="E240" s="13"/>
     </row>
-    <row r="241" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A241" s="12"/>
       <c r="B241" s="13"/>
       <c r="C241" s="12"/>
       <c r="D241" s="13"/>
       <c r="E241" s="13"/>
     </row>
-    <row r="242" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A242" s="12"/>
       <c r="B242" s="13"/>
       <c r="C242" s="12"/>
       <c r="D242" s="13"/>
       <c r="E242" s="13"/>
     </row>
-    <row r="243" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A243" s="12"/>
       <c r="B243" s="13"/>
       <c r="C243" s="12"/>
       <c r="D243" s="13"/>
       <c r="E243" s="13"/>
     </row>
-    <row r="244" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A244" s="12"/>
       <c r="B244" s="13"/>
       <c r="C244" s="12"/>
       <c r="D244" s="13"/>
       <c r="E244" s="13"/>
     </row>
-    <row r="245" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A245" s="12"/>
       <c r="B245" s="13"/>
       <c r="C245" s="12"/>
       <c r="D245" s="13"/>
       <c r="E245" s="13"/>
     </row>
-    <row r="246" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A246" s="12"/>
       <c r="B246" s="13"/>
       <c r="C246" s="12"/>
       <c r="D246" s="13"/>
       <c r="E246" s="13"/>
     </row>
-    <row r="247" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A247" s="12"/>
       <c r="B247" s="13"/>
       <c r="C247" s="12"/>
       <c r="D247" s="13"/>
       <c r="E247" s="13"/>
     </row>
-    <row r="248" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A248" s="12"/>
       <c r="B248" s="13"/>
       <c r="C248" s="12"/>
       <c r="D248" s="13"/>
       <c r="E248" s="13"/>
     </row>
-    <row r="249" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A249" s="12"/>
       <c r="B249" s="13"/>
       <c r="C249" s="12"/>
       <c r="D249" s="13"/>
       <c r="E249" s="13"/>
     </row>
-    <row r="250" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A250" s="12"/>
       <c r="B250" s="13"/>
       <c r="C250" s="12"/>
       <c r="D250" s="13"/>
       <c r="E250" s="13"/>
     </row>
-    <row r="251" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A251" s="12"/>
       <c r="B251" s="13"/>
       <c r="C251" s="12"/>
       <c r="D251" s="13"/>
       <c r="E251" s="13"/>
     </row>
-    <row r="252" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A252" s="12"/>
       <c r="B252" s="13"/>
       <c r="C252" s="12"/>
       <c r="D252" s="13"/>
       <c r="E252" s="13"/>
     </row>
-    <row r="253" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A253" s="12"/>
       <c r="B253" s="13"/>
       <c r="C253" s="12"/>
       <c r="D253" s="13"/>
       <c r="E253" s="13"/>
     </row>
-    <row r="254" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A254" s="12"/>
       <c r="B254" s="13"/>
       <c r="C254" s="12"/>
       <c r="D254" s="13"/>
       <c r="E254" s="13"/>
     </row>
-    <row r="255" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A255" s="12"/>
       <c r="B255" s="13"/>
       <c r="C255" s="12"/>
       <c r="D255" s="13"/>
       <c r="E255" s="13"/>
     </row>
-    <row r="256" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A256" s="12"/>
       <c r="B256" s="13"/>
       <c r="C256" s="12"/>
       <c r="D256" s="13"/>
       <c r="E256" s="13"/>
     </row>
-    <row r="257" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A257" s="12"/>
       <c r="B257" s="13"/>
       <c r="C257" s="12"/>
       <c r="D257" s="13"/>
       <c r="E257" s="13"/>
     </row>
-    <row r="258" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A258" s="12"/>
       <c r="B258" s="13"/>
       <c r="C258" s="12"/>
       <c r="D258" s="13"/>
       <c r="E258" s="13"/>
     </row>
-    <row r="259" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A259" s="12"/>
       <c r="B259" s="13"/>
       <c r="C259" s="12"/>
       <c r="D259" s="13"/>
       <c r="E259" s="13"/>
     </row>
-    <row r="260" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A260" s="12"/>
       <c r="B260" s="13"/>
       <c r="C260" s="12"/>
@@ -3012,6 +3024,7 @@
     <hyperlink ref="D29" r:id="rId3"/>
     <hyperlink ref="D30" r:id="rId4"/>
     <hyperlink ref="D31" r:id="rId5"/>
+    <hyperlink ref="D32" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
se agrega el 32 Alumno al archivo
</commit_message>
<xml_diff>
--- a/Lista de Alumnos.xlsx
+++ b/Lista de Alumnos.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25330"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LILEN\Desktop\ISPC !!\carrera TELECOMUNICACIONES aula1\ELECTRONICA\electronica vacaciones\Alumnos\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{451EB38E-7C65-4641-88AA-18D387720696}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-102" yWindow="-102" windowWidth="18580" windowHeight="11698"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Electronica Microcontrolada" sheetId="1" r:id="rId1"/>
@@ -14,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="100">
   <si>
     <t>#</t>
   </si>
@@ -305,12 +311,21 @@
   </si>
   <si>
     <t>FedeBirge</t>
+  </si>
+  <si>
+    <t>Guzman, Maria Lilen</t>
+  </si>
+  <si>
+    <t>lilenguzman2015@gmail.com</t>
+  </si>
+  <si>
+    <t>lilenguzman01</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -806,26 +821,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:E260"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.65" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.88671875" style="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="37.109375" style="15" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.5546875" style="14" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.85546875" style="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.140625" style="15" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" style="14" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="31" style="15" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="29" style="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="27.1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" ht="27.2" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -842,7 +857,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="19.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -859,7 +874,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="19.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>2</v>
       </c>
@@ -874,7 +889,7 @@
       </c>
       <c r="E3" s="6"/>
     </row>
-    <row r="4" spans="1:5" ht="19.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>3</v>
       </c>
@@ -891,7 +906,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="19.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>4</v>
       </c>
@@ -908,7 +923,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="19.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>5</v>
       </c>
@@ -925,7 +940,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="19.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>6</v>
       </c>
@@ -942,7 +957,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="19.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>7</v>
       </c>
@@ -959,7 +974,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="19.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>8</v>
       </c>
@@ -976,7 +991,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="19.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>9</v>
       </c>
@@ -991,7 +1006,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="19.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <v>10</v>
       </c>
@@ -1008,7 +1023,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="19.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>11</v>
       </c>
@@ -1025,7 +1040,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="19.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
         <v>12</v>
       </c>
@@ -1042,7 +1057,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="19.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
         <v>13</v>
       </c>
@@ -1059,7 +1074,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="19.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
         <v>14</v>
       </c>
@@ -1076,7 +1091,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="19.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
         <v>15</v>
       </c>
@@ -1093,7 +1108,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="19.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
         <v>16</v>
       </c>
@@ -1110,7 +1125,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="19.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <v>17</v>
       </c>
@@ -1127,7 +1142,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="19.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
         <v>18</v>
       </c>
@@ -1144,7 +1159,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="19.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
         <v>19</v>
       </c>
@@ -1161,7 +1176,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="19.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="5">
         <v>20</v>
       </c>
@@ -1331,7 +1346,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="5">
         <v>30</v>
       </c>
@@ -1348,7 +1363,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="5">
         <v>31</v>
       </c>
@@ -1369,10 +1384,18 @@
       <c r="A33" s="5">
         <v>32</v>
       </c>
-      <c r="B33" s="6"/>
-      <c r="C33" s="5"/>
-      <c r="D33" s="6"/>
-      <c r="E33" s="6"/>
+      <c r="B33" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="C33" s="5">
+        <v>1</v>
+      </c>
+      <c r="D33" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="E33" s="6" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="34" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="5">
@@ -1401,7 +1424,7 @@
       <c r="D36" s="6"/>
       <c r="E36" s="6"/>
     </row>
-    <row r="37" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="5">
         <v>36</v>
       </c>
@@ -1410,7 +1433,7 @@
       <c r="D37" s="6"/>
       <c r="E37" s="6"/>
     </row>
-    <row r="38" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="5">
         <v>37</v>
       </c>
@@ -1419,7 +1442,7 @@
       <c r="D38" s="6"/>
       <c r="E38" s="6"/>
     </row>
-    <row r="39" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="5">
         <v>38</v>
       </c>
@@ -1428,7 +1451,7 @@
       <c r="D39" s="6"/>
       <c r="E39" s="6"/>
     </row>
-    <row r="40" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="5">
         <v>39</v>
       </c>
@@ -1437,7 +1460,7 @@
       <c r="D40" s="6"/>
       <c r="E40" s="6"/>
     </row>
-    <row r="41" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="5">
         <v>40</v>
       </c>
@@ -1446,7 +1469,7 @@
       <c r="D41" s="6"/>
       <c r="E41" s="6"/>
     </row>
-    <row r="42" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="5">
         <v>41</v>
       </c>
@@ -1455,7 +1478,7 @@
       <c r="D42" s="6"/>
       <c r="E42" s="6"/>
     </row>
-    <row r="43" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="5">
         <v>42</v>
       </c>
@@ -1464,7 +1487,7 @@
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
     </row>
-    <row r="44" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="5">
         <v>43</v>
       </c>
@@ -1473,7 +1496,7 @@
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
     </row>
-    <row r="45" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="5">
         <v>44</v>
       </c>
@@ -1482,7 +1505,7 @@
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
     </row>
-    <row r="46" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="5">
         <v>45</v>
       </c>
@@ -1491,7 +1514,7 @@
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
     </row>
-    <row r="47" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="5">
         <v>46</v>
       </c>
@@ -1500,7 +1523,7 @@
       <c r="D47" s="6"/>
       <c r="E47" s="6"/>
     </row>
-    <row r="48" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="5">
         <v>47</v>
       </c>
@@ -1509,7 +1532,7 @@
       <c r="D48" s="6"/>
       <c r="E48" s="6"/>
     </row>
-    <row r="49" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="5">
         <v>48</v>
       </c>
@@ -1518,7 +1541,7 @@
       <c r="D49" s="6"/>
       <c r="E49" s="6"/>
     </row>
-    <row r="50" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="5">
         <v>49</v>
       </c>
@@ -1527,7 +1550,7 @@
       <c r="D50" s="6"/>
       <c r="E50" s="6"/>
     </row>
-    <row r="51" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="5">
         <v>50</v>
       </c>
@@ -1536,7 +1559,7 @@
       <c r="D51" s="6"/>
       <c r="E51" s="6"/>
     </row>
-    <row r="52" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="5">
         <v>51</v>
       </c>
@@ -1545,7 +1568,7 @@
       <c r="D52" s="6"/>
       <c r="E52" s="6"/>
     </row>
-    <row r="53" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="5">
         <v>52</v>
       </c>
@@ -1554,7 +1577,7 @@
       <c r="D53" s="6"/>
       <c r="E53" s="6"/>
     </row>
-    <row r="54" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="5">
         <v>53</v>
       </c>
@@ -1563,7 +1586,7 @@
       <c r="D54" s="6"/>
       <c r="E54" s="6"/>
     </row>
-    <row r="55" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="5">
         <v>54</v>
       </c>
@@ -1572,7 +1595,7 @@
       <c r="D55" s="6"/>
       <c r="E55" s="6"/>
     </row>
-    <row r="56" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="5">
         <v>55</v>
       </c>
@@ -1581,7 +1604,7 @@
       <c r="D56" s="6"/>
       <c r="E56" s="6"/>
     </row>
-    <row r="57" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="5">
         <v>56</v>
       </c>
@@ -1590,7 +1613,7 @@
       <c r="D57" s="6"/>
       <c r="E57" s="6"/>
     </row>
-    <row r="58" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="5">
         <v>57</v>
       </c>
@@ -1599,7 +1622,7 @@
       <c r="D58" s="6"/>
       <c r="E58" s="6"/>
     </row>
-    <row r="59" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="5">
         <v>58</v>
       </c>
@@ -1608,7 +1631,7 @@
       <c r="D59" s="6"/>
       <c r="E59" s="6"/>
     </row>
-    <row r="60" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="5">
         <v>59</v>
       </c>
@@ -1617,1400 +1640,1400 @@
       <c r="D60" s="6"/>
       <c r="E60" s="6"/>
     </row>
-    <row r="61" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="12"/>
       <c r="B61" s="13"/>
       <c r="C61" s="12"/>
       <c r="D61" s="13"/>
       <c r="E61" s="13"/>
     </row>
-    <row r="62" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="12"/>
       <c r="B62" s="13"/>
       <c r="C62" s="12"/>
       <c r="D62" s="13"/>
       <c r="E62" s="13"/>
     </row>
-    <row r="63" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="12"/>
       <c r="B63" s="13"/>
       <c r="C63" s="12"/>
       <c r="D63" s="13"/>
       <c r="E63" s="13"/>
     </row>
-    <row r="64" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="12"/>
       <c r="B64" s="13"/>
       <c r="C64" s="12"/>
       <c r="D64" s="13"/>
       <c r="E64" s="13"/>
     </row>
-    <row r="65" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="12"/>
       <c r="B65" s="13"/>
       <c r="C65" s="12"/>
       <c r="D65" s="13"/>
       <c r="E65" s="13"/>
     </row>
-    <row r="66" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="12"/>
       <c r="B66" s="13"/>
       <c r="C66" s="12"/>
       <c r="D66" s="13"/>
       <c r="E66" s="13"/>
     </row>
-    <row r="67" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="12"/>
       <c r="B67" s="13"/>
       <c r="C67" s="12"/>
       <c r="D67" s="13"/>
       <c r="E67" s="13"/>
     </row>
-    <row r="68" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="12"/>
       <c r="B68" s="13"/>
       <c r="C68" s="12"/>
       <c r="D68" s="13"/>
       <c r="E68" s="13"/>
     </row>
-    <row r="69" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="12"/>
       <c r="B69" s="13"/>
       <c r="C69" s="12"/>
       <c r="D69" s="13"/>
       <c r="E69" s="13"/>
     </row>
-    <row r="70" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="12"/>
       <c r="B70" s="13"/>
       <c r="C70" s="12"/>
       <c r="D70" s="13"/>
       <c r="E70" s="13"/>
     </row>
-    <row r="71" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="12"/>
       <c r="B71" s="13"/>
       <c r="C71" s="12"/>
       <c r="D71" s="13"/>
       <c r="E71" s="13"/>
     </row>
-    <row r="72" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="12"/>
       <c r="B72" s="13"/>
       <c r="C72" s="12"/>
       <c r="D72" s="13"/>
       <c r="E72" s="13"/>
     </row>
-    <row r="73" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="12"/>
       <c r="B73" s="13"/>
       <c r="C73" s="12"/>
       <c r="D73" s="13"/>
       <c r="E73" s="13"/>
     </row>
-    <row r="74" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="12"/>
       <c r="B74" s="13"/>
       <c r="C74" s="12"/>
       <c r="D74" s="13"/>
       <c r="E74" s="13"/>
     </row>
-    <row r="75" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="12"/>
       <c r="B75" s="13"/>
       <c r="C75" s="12"/>
       <c r="D75" s="13"/>
       <c r="E75" s="13"/>
     </row>
-    <row r="76" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="12"/>
       <c r="B76" s="13"/>
       <c r="C76" s="12"/>
       <c r="D76" s="13"/>
       <c r="E76" s="13"/>
     </row>
-    <row r="77" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="12"/>
       <c r="B77" s="13"/>
       <c r="C77" s="12"/>
       <c r="D77" s="13"/>
       <c r="E77" s="13"/>
     </row>
-    <row r="78" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="12"/>
       <c r="B78" s="13"/>
       <c r="C78" s="12"/>
       <c r="D78" s="13"/>
       <c r="E78" s="13"/>
     </row>
-    <row r="79" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="12"/>
       <c r="B79" s="13"/>
       <c r="C79" s="12"/>
       <c r="D79" s="13"/>
       <c r="E79" s="13"/>
     </row>
-    <row r="80" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="12"/>
       <c r="B80" s="13"/>
       <c r="C80" s="12"/>
       <c r="D80" s="13"/>
       <c r="E80" s="13"/>
     </row>
-    <row r="81" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="12"/>
       <c r="B81" s="13"/>
       <c r="C81" s="12"/>
       <c r="D81" s="13"/>
       <c r="E81" s="13"/>
     </row>
-    <row r="82" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="12"/>
       <c r="B82" s="13"/>
       <c r="C82" s="12"/>
       <c r="D82" s="13"/>
       <c r="E82" s="13"/>
     </row>
-    <row r="83" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="12"/>
       <c r="B83" s="13"/>
       <c r="C83" s="12"/>
       <c r="D83" s="13"/>
       <c r="E83" s="13"/>
     </row>
-    <row r="84" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="12"/>
       <c r="B84" s="13"/>
       <c r="C84" s="12"/>
       <c r="D84" s="13"/>
       <c r="E84" s="13"/>
     </row>
-    <row r="85" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="12"/>
       <c r="B85" s="13"/>
       <c r="C85" s="12"/>
       <c r="D85" s="13"/>
       <c r="E85" s="13"/>
     </row>
-    <row r="86" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="12"/>
       <c r="B86" s="13"/>
       <c r="C86" s="12"/>
       <c r="D86" s="13"/>
       <c r="E86" s="13"/>
     </row>
-    <row r="87" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="12"/>
       <c r="B87" s="13"/>
       <c r="C87" s="12"/>
       <c r="D87" s="13"/>
       <c r="E87" s="13"/>
     </row>
-    <row r="88" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="12"/>
       <c r="B88" s="13"/>
       <c r="C88" s="12"/>
       <c r="D88" s="13"/>
       <c r="E88" s="13"/>
     </row>
-    <row r="89" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="12"/>
       <c r="B89" s="13"/>
       <c r="C89" s="12"/>
       <c r="D89" s="13"/>
       <c r="E89" s="13"/>
     </row>
-    <row r="90" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="12"/>
       <c r="B90" s="13"/>
       <c r="C90" s="12"/>
       <c r="D90" s="13"/>
       <c r="E90" s="13"/>
     </row>
-    <row r="91" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="12"/>
       <c r="B91" s="13"/>
       <c r="C91" s="12"/>
       <c r="D91" s="13"/>
       <c r="E91" s="13"/>
     </row>
-    <row r="92" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="12"/>
       <c r="B92" s="13"/>
       <c r="C92" s="12"/>
       <c r="D92" s="13"/>
       <c r="E92" s="13"/>
     </row>
-    <row r="93" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="12"/>
       <c r="B93" s="13"/>
       <c r="C93" s="12"/>
       <c r="D93" s="13"/>
       <c r="E93" s="13"/>
     </row>
-    <row r="94" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="12"/>
       <c r="B94" s="13"/>
       <c r="C94" s="12"/>
       <c r="D94" s="13"/>
       <c r="E94" s="13"/>
     </row>
-    <row r="95" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="12"/>
       <c r="B95" s="13"/>
       <c r="C95" s="12"/>
       <c r="D95" s="13"/>
       <c r="E95" s="13"/>
     </row>
-    <row r="96" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="12"/>
       <c r="B96" s="13"/>
       <c r="C96" s="12"/>
       <c r="D96" s="13"/>
       <c r="E96" s="13"/>
     </row>
-    <row r="97" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="12"/>
       <c r="B97" s="13"/>
       <c r="C97" s="12"/>
       <c r="D97" s="13"/>
       <c r="E97" s="13"/>
     </row>
-    <row r="98" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="12"/>
       <c r="B98" s="13"/>
       <c r="C98" s="12"/>
       <c r="D98" s="13"/>
       <c r="E98" s="13"/>
     </row>
-    <row r="99" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="12"/>
       <c r="B99" s="13"/>
       <c r="C99" s="12"/>
       <c r="D99" s="13"/>
       <c r="E99" s="13"/>
     </row>
-    <row r="100" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="12"/>
       <c r="B100" s="13"/>
       <c r="C100" s="12"/>
       <c r="D100" s="13"/>
       <c r="E100" s="13"/>
     </row>
-    <row r="101" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="12"/>
       <c r="B101" s="13"/>
       <c r="C101" s="12"/>
       <c r="D101" s="13"/>
       <c r="E101" s="13"/>
     </row>
-    <row r="102" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="12"/>
       <c r="B102" s="13"/>
       <c r="C102" s="12"/>
       <c r="D102" s="13"/>
       <c r="E102" s="13"/>
     </row>
-    <row r="103" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" s="12"/>
       <c r="B103" s="13"/>
       <c r="C103" s="12"/>
       <c r="D103" s="13"/>
       <c r="E103" s="13"/>
     </row>
-    <row r="104" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="12"/>
       <c r="B104" s="13"/>
       <c r="C104" s="12"/>
       <c r="D104" s="13"/>
       <c r="E104" s="13"/>
     </row>
-    <row r="105" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" s="12"/>
       <c r="B105" s="13"/>
       <c r="C105" s="12"/>
       <c r="D105" s="13"/>
       <c r="E105" s="13"/>
     </row>
-    <row r="106" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="12"/>
       <c r="B106" s="13"/>
       <c r="C106" s="12"/>
       <c r="D106" s="13"/>
       <c r="E106" s="13"/>
     </row>
-    <row r="107" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" s="12"/>
       <c r="B107" s="13"/>
       <c r="C107" s="12"/>
       <c r="D107" s="13"/>
       <c r="E107" s="13"/>
     </row>
-    <row r="108" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" s="12"/>
       <c r="B108" s="13"/>
       <c r="C108" s="12"/>
       <c r="D108" s="13"/>
       <c r="E108" s="13"/>
     </row>
-    <row r="109" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" s="12"/>
       <c r="B109" s="13"/>
       <c r="C109" s="12"/>
       <c r="D109" s="13"/>
       <c r="E109" s="13"/>
     </row>
-    <row r="110" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" s="12"/>
       <c r="B110" s="13"/>
       <c r="C110" s="12"/>
       <c r="D110" s="13"/>
       <c r="E110" s="13"/>
     </row>
-    <row r="111" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" s="12"/>
       <c r="B111" s="13"/>
       <c r="C111" s="12"/>
       <c r="D111" s="13"/>
       <c r="E111" s="13"/>
     </row>
-    <row r="112" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" s="12"/>
       <c r="B112" s="13"/>
       <c r="C112" s="12"/>
       <c r="D112" s="13"/>
       <c r="E112" s="13"/>
     </row>
-    <row r="113" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" s="12"/>
       <c r="B113" s="13"/>
       <c r="C113" s="12"/>
       <c r="D113" s="13"/>
       <c r="E113" s="13"/>
     </row>
-    <row r="114" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A114" s="12"/>
       <c r="B114" s="13"/>
       <c r="C114" s="12"/>
       <c r="D114" s="13"/>
       <c r="E114" s="13"/>
     </row>
-    <row r="115" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A115" s="12"/>
       <c r="B115" s="13"/>
       <c r="C115" s="12"/>
       <c r="D115" s="13"/>
       <c r="E115" s="13"/>
     </row>
-    <row r="116" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A116" s="12"/>
       <c r="B116" s="13"/>
       <c r="C116" s="12"/>
       <c r="D116" s="13"/>
       <c r="E116" s="13"/>
     </row>
-    <row r="117" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A117" s="12"/>
       <c r="B117" s="13"/>
       <c r="C117" s="12"/>
       <c r="D117" s="13"/>
       <c r="E117" s="13"/>
     </row>
-    <row r="118" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A118" s="12"/>
       <c r="B118" s="13"/>
       <c r="C118" s="12"/>
       <c r="D118" s="13"/>
       <c r="E118" s="13"/>
     </row>
-    <row r="119" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A119" s="12"/>
       <c r="B119" s="13"/>
       <c r="C119" s="12"/>
       <c r="D119" s="13"/>
       <c r="E119" s="13"/>
     </row>
-    <row r="120" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A120" s="12"/>
       <c r="B120" s="13"/>
       <c r="C120" s="12"/>
       <c r="D120" s="13"/>
       <c r="E120" s="13"/>
     </row>
-    <row r="121" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A121" s="12"/>
       <c r="B121" s="13"/>
       <c r="C121" s="12"/>
       <c r="D121" s="13"/>
       <c r="E121" s="13"/>
     </row>
-    <row r="122" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A122" s="12"/>
       <c r="B122" s="13"/>
       <c r="C122" s="12"/>
       <c r="D122" s="13"/>
       <c r="E122" s="13"/>
     </row>
-    <row r="123" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A123" s="12"/>
       <c r="B123" s="13"/>
       <c r="C123" s="12"/>
       <c r="D123" s="13"/>
       <c r="E123" s="13"/>
     </row>
-    <row r="124" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A124" s="12"/>
       <c r="B124" s="13"/>
       <c r="C124" s="12"/>
       <c r="D124" s="13"/>
       <c r="E124" s="13"/>
     </row>
-    <row r="125" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A125" s="12"/>
       <c r="B125" s="13"/>
       <c r="C125" s="12"/>
       <c r="D125" s="13"/>
       <c r="E125" s="13"/>
     </row>
-    <row r="126" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A126" s="12"/>
       <c r="B126" s="13"/>
       <c r="C126" s="12"/>
       <c r="D126" s="13"/>
       <c r="E126" s="13"/>
     </row>
-    <row r="127" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A127" s="12"/>
       <c r="B127" s="13"/>
       <c r="C127" s="12"/>
       <c r="D127" s="13"/>
       <c r="E127" s="13"/>
     </row>
-    <row r="128" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A128" s="12"/>
       <c r="B128" s="13"/>
       <c r="C128" s="12"/>
       <c r="D128" s="13"/>
       <c r="E128" s="13"/>
     </row>
-    <row r="129" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A129" s="12"/>
       <c r="B129" s="13"/>
       <c r="C129" s="12"/>
       <c r="D129" s="13"/>
       <c r="E129" s="13"/>
     </row>
-    <row r="130" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A130" s="12"/>
       <c r="B130" s="13"/>
       <c r="C130" s="12"/>
       <c r="D130" s="13"/>
       <c r="E130" s="13"/>
     </row>
-    <row r="131" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A131" s="12"/>
       <c r="B131" s="13"/>
       <c r="C131" s="12"/>
       <c r="D131" s="13"/>
       <c r="E131" s="13"/>
     </row>
-    <row r="132" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A132" s="12"/>
       <c r="B132" s="13"/>
       <c r="C132" s="12"/>
       <c r="D132" s="13"/>
       <c r="E132" s="13"/>
     </row>
-    <row r="133" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A133" s="12"/>
       <c r="B133" s="13"/>
       <c r="C133" s="12"/>
       <c r="D133" s="13"/>
       <c r="E133" s="13"/>
     </row>
-    <row r="134" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A134" s="12"/>
       <c r="B134" s="13"/>
       <c r="C134" s="12"/>
       <c r="D134" s="13"/>
       <c r="E134" s="13"/>
     </row>
-    <row r="135" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A135" s="12"/>
       <c r="B135" s="13"/>
       <c r="C135" s="12"/>
       <c r="D135" s="13"/>
       <c r="E135" s="13"/>
     </row>
-    <row r="136" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A136" s="12"/>
       <c r="B136" s="13"/>
       <c r="C136" s="12"/>
       <c r="D136" s="13"/>
       <c r="E136" s="13"/>
     </row>
-    <row r="137" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A137" s="12"/>
       <c r="B137" s="13"/>
       <c r="C137" s="12"/>
       <c r="D137" s="13"/>
       <c r="E137" s="13"/>
     </row>
-    <row r="138" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A138" s="12"/>
       <c r="B138" s="13"/>
       <c r="C138" s="12"/>
       <c r="D138" s="13"/>
       <c r="E138" s="13"/>
     </row>
-    <row r="139" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A139" s="12"/>
       <c r="B139" s="13"/>
       <c r="C139" s="12"/>
       <c r="D139" s="13"/>
       <c r="E139" s="13"/>
     </row>
-    <row r="140" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A140" s="12"/>
       <c r="B140" s="13"/>
       <c r="C140" s="12"/>
       <c r="D140" s="13"/>
       <c r="E140" s="13"/>
     </row>
-    <row r="141" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A141" s="12"/>
       <c r="B141" s="13"/>
       <c r="C141" s="12"/>
       <c r="D141" s="13"/>
       <c r="E141" s="13"/>
     </row>
-    <row r="142" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A142" s="12"/>
       <c r="B142" s="13"/>
       <c r="C142" s="12"/>
       <c r="D142" s="13"/>
       <c r="E142" s="13"/>
     </row>
-    <row r="143" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A143" s="12"/>
       <c r="B143" s="13"/>
       <c r="C143" s="12"/>
       <c r="D143" s="13"/>
       <c r="E143" s="13"/>
     </row>
-    <row r="144" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A144" s="12"/>
       <c r="B144" s="13"/>
       <c r="C144" s="12"/>
       <c r="D144" s="13"/>
       <c r="E144" s="13"/>
     </row>
-    <row r="145" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A145" s="12"/>
       <c r="B145" s="13"/>
       <c r="C145" s="12"/>
       <c r="D145" s="13"/>
       <c r="E145" s="13"/>
     </row>
-    <row r="146" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A146" s="12"/>
       <c r="B146" s="13"/>
       <c r="C146" s="12"/>
       <c r="D146" s="13"/>
       <c r="E146" s="13"/>
     </row>
-    <row r="147" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A147" s="12"/>
       <c r="B147" s="13"/>
       <c r="C147" s="12"/>
       <c r="D147" s="13"/>
       <c r="E147" s="13"/>
     </row>
-    <row r="148" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A148" s="12"/>
       <c r="B148" s="13"/>
       <c r="C148" s="12"/>
       <c r="D148" s="13"/>
       <c r="E148" s="13"/>
     </row>
-    <row r="149" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A149" s="12"/>
       <c r="B149" s="13"/>
       <c r="C149" s="12"/>
       <c r="D149" s="13"/>
       <c r="E149" s="13"/>
     </row>
-    <row r="150" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A150" s="12"/>
       <c r="B150" s="13"/>
       <c r="C150" s="12"/>
       <c r="D150" s="13"/>
       <c r="E150" s="13"/>
     </row>
-    <row r="151" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A151" s="12"/>
       <c r="B151" s="13"/>
       <c r="C151" s="12"/>
       <c r="D151" s="13"/>
       <c r="E151" s="13"/>
     </row>
-    <row r="152" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A152" s="12"/>
       <c r="B152" s="13"/>
       <c r="C152" s="12"/>
       <c r="D152" s="13"/>
       <c r="E152" s="13"/>
     </row>
-    <row r="153" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A153" s="12"/>
       <c r="B153" s="13"/>
       <c r="C153" s="12"/>
       <c r="D153" s="13"/>
       <c r="E153" s="13"/>
     </row>
-    <row r="154" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A154" s="12"/>
       <c r="B154" s="13"/>
       <c r="C154" s="12"/>
       <c r="D154" s="13"/>
       <c r="E154" s="13"/>
     </row>
-    <row r="155" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A155" s="12"/>
       <c r="B155" s="13"/>
       <c r="C155" s="12"/>
       <c r="D155" s="13"/>
       <c r="E155" s="13"/>
     </row>
-    <row r="156" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A156" s="12"/>
       <c r="B156" s="13"/>
       <c r="C156" s="12"/>
       <c r="D156" s="13"/>
       <c r="E156" s="13"/>
     </row>
-    <row r="157" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A157" s="12"/>
       <c r="B157" s="13"/>
       <c r="C157" s="12"/>
       <c r="D157" s="13"/>
       <c r="E157" s="13"/>
     </row>
-    <row r="158" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A158" s="12"/>
       <c r="B158" s="13"/>
       <c r="C158" s="12"/>
       <c r="D158" s="13"/>
       <c r="E158" s="13"/>
     </row>
-    <row r="159" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A159" s="12"/>
       <c r="B159" s="13"/>
       <c r="C159" s="12"/>
       <c r="D159" s="13"/>
       <c r="E159" s="13"/>
     </row>
-    <row r="160" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A160" s="12"/>
       <c r="B160" s="13"/>
       <c r="C160" s="12"/>
       <c r="D160" s="13"/>
       <c r="E160" s="13"/>
     </row>
-    <row r="161" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A161" s="12"/>
       <c r="B161" s="13"/>
       <c r="C161" s="12"/>
       <c r="D161" s="13"/>
       <c r="E161" s="13"/>
     </row>
-    <row r="162" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A162" s="12"/>
       <c r="B162" s="13"/>
       <c r="C162" s="12"/>
       <c r="D162" s="13"/>
       <c r="E162" s="13"/>
     </row>
-    <row r="163" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A163" s="12"/>
       <c r="B163" s="13"/>
       <c r="C163" s="12"/>
       <c r="D163" s="13"/>
       <c r="E163" s="13"/>
     </row>
-    <row r="164" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A164" s="12"/>
       <c r="B164" s="13"/>
       <c r="C164" s="12"/>
       <c r="D164" s="13"/>
       <c r="E164" s="13"/>
     </row>
-    <row r="165" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A165" s="12"/>
       <c r="B165" s="13"/>
       <c r="C165" s="12"/>
       <c r="D165" s="13"/>
       <c r="E165" s="13"/>
     </row>
-    <row r="166" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A166" s="12"/>
       <c r="B166" s="13"/>
       <c r="C166" s="12"/>
       <c r="D166" s="13"/>
       <c r="E166" s="13"/>
     </row>
-    <row r="167" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A167" s="12"/>
       <c r="B167" s="13"/>
       <c r="C167" s="12"/>
       <c r="D167" s="13"/>
       <c r="E167" s="13"/>
     </row>
-    <row r="168" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A168" s="12"/>
       <c r="B168" s="13"/>
       <c r="C168" s="12"/>
       <c r="D168" s="13"/>
       <c r="E168" s="13"/>
     </row>
-    <row r="169" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A169" s="12"/>
       <c r="B169" s="13"/>
       <c r="C169" s="12"/>
       <c r="D169" s="13"/>
       <c r="E169" s="13"/>
     </row>
-    <row r="170" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A170" s="12"/>
       <c r="B170" s="13"/>
       <c r="C170" s="12"/>
       <c r="D170" s="13"/>
       <c r="E170" s="13"/>
     </row>
-    <row r="171" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A171" s="12"/>
       <c r="B171" s="13"/>
       <c r="C171" s="12"/>
       <c r="D171" s="13"/>
       <c r="E171" s="13"/>
     </row>
-    <row r="172" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A172" s="12"/>
       <c r="B172" s="13"/>
       <c r="C172" s="12"/>
       <c r="D172" s="13"/>
       <c r="E172" s="13"/>
     </row>
-    <row r="173" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A173" s="12"/>
       <c r="B173" s="13"/>
       <c r="C173" s="12"/>
       <c r="D173" s="13"/>
       <c r="E173" s="13"/>
     </row>
-    <row r="174" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A174" s="12"/>
       <c r="B174" s="13"/>
       <c r="C174" s="12"/>
       <c r="D174" s="13"/>
       <c r="E174" s="13"/>
     </row>
-    <row r="175" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A175" s="12"/>
       <c r="B175" s="13"/>
       <c r="C175" s="12"/>
       <c r="D175" s="13"/>
       <c r="E175" s="13"/>
     </row>
-    <row r="176" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A176" s="12"/>
       <c r="B176" s="13"/>
       <c r="C176" s="12"/>
       <c r="D176" s="13"/>
       <c r="E176" s="13"/>
     </row>
-    <row r="177" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A177" s="12"/>
       <c r="B177" s="13"/>
       <c r="C177" s="12"/>
       <c r="D177" s="13"/>
       <c r="E177" s="13"/>
     </row>
-    <row r="178" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A178" s="12"/>
       <c r="B178" s="13"/>
       <c r="C178" s="12"/>
       <c r="D178" s="13"/>
       <c r="E178" s="13"/>
     </row>
-    <row r="179" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A179" s="12"/>
       <c r="B179" s="13"/>
       <c r="C179" s="12"/>
       <c r="D179" s="13"/>
       <c r="E179" s="13"/>
     </row>
-    <row r="180" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A180" s="12"/>
       <c r="B180" s="13"/>
       <c r="C180" s="12"/>
       <c r="D180" s="13"/>
       <c r="E180" s="13"/>
     </row>
-    <row r="181" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A181" s="12"/>
       <c r="B181" s="13"/>
       <c r="C181" s="12"/>
       <c r="D181" s="13"/>
       <c r="E181" s="13"/>
     </row>
-    <row r="182" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A182" s="12"/>
       <c r="B182" s="13"/>
       <c r="C182" s="12"/>
       <c r="D182" s="13"/>
       <c r="E182" s="13"/>
     </row>
-    <row r="183" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A183" s="12"/>
       <c r="B183" s="13"/>
       <c r="C183" s="12"/>
       <c r="D183" s="13"/>
       <c r="E183" s="13"/>
     </row>
-    <row r="184" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A184" s="12"/>
       <c r="B184" s="13"/>
       <c r="C184" s="12"/>
       <c r="D184" s="13"/>
       <c r="E184" s="13"/>
     </row>
-    <row r="185" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A185" s="12"/>
       <c r="B185" s="13"/>
       <c r="C185" s="12"/>
       <c r="D185" s="13"/>
       <c r="E185" s="13"/>
     </row>
-    <row r="186" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A186" s="12"/>
       <c r="B186" s="13"/>
       <c r="C186" s="12"/>
       <c r="D186" s="13"/>
       <c r="E186" s="13"/>
     </row>
-    <row r="187" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A187" s="12"/>
       <c r="B187" s="13"/>
       <c r="C187" s="12"/>
       <c r="D187" s="13"/>
       <c r="E187" s="13"/>
     </row>
-    <row r="188" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A188" s="12"/>
       <c r="B188" s="13"/>
       <c r="C188" s="12"/>
       <c r="D188" s="13"/>
       <c r="E188" s="13"/>
     </row>
-    <row r="189" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A189" s="12"/>
       <c r="B189" s="13"/>
       <c r="C189" s="12"/>
       <c r="D189" s="13"/>
       <c r="E189" s="13"/>
     </row>
-    <row r="190" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A190" s="12"/>
       <c r="B190" s="13"/>
       <c r="C190" s="12"/>
       <c r="D190" s="13"/>
       <c r="E190" s="13"/>
     </row>
-    <row r="191" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A191" s="12"/>
       <c r="B191" s="13"/>
       <c r="C191" s="12"/>
       <c r="D191" s="13"/>
       <c r="E191" s="13"/>
     </row>
-    <row r="192" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A192" s="12"/>
       <c r="B192" s="13"/>
       <c r="C192" s="12"/>
       <c r="D192" s="13"/>
       <c r="E192" s="13"/>
     </row>
-    <row r="193" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A193" s="12"/>
       <c r="B193" s="13"/>
       <c r="C193" s="12"/>
       <c r="D193" s="13"/>
       <c r="E193" s="13"/>
     </row>
-    <row r="194" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A194" s="12"/>
       <c r="B194" s="13"/>
       <c r="C194" s="12"/>
       <c r="D194" s="13"/>
       <c r="E194" s="13"/>
     </row>
-    <row r="195" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A195" s="12"/>
       <c r="B195" s="13"/>
       <c r="C195" s="12"/>
       <c r="D195" s="13"/>
       <c r="E195" s="13"/>
     </row>
-    <row r="196" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A196" s="12"/>
       <c r="B196" s="13"/>
       <c r="C196" s="12"/>
       <c r="D196" s="13"/>
       <c r="E196" s="13"/>
     </row>
-    <row r="197" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A197" s="12"/>
       <c r="B197" s="13"/>
       <c r="C197" s="12"/>
       <c r="D197" s="13"/>
       <c r="E197" s="13"/>
     </row>
-    <row r="198" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A198" s="12"/>
       <c r="B198" s="13"/>
       <c r="C198" s="12"/>
       <c r="D198" s="13"/>
       <c r="E198" s="13"/>
     </row>
-    <row r="199" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A199" s="12"/>
       <c r="B199" s="13"/>
       <c r="C199" s="12"/>
       <c r="D199" s="13"/>
       <c r="E199" s="13"/>
     </row>
-    <row r="200" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A200" s="12"/>
       <c r="B200" s="13"/>
       <c r="C200" s="12"/>
       <c r="D200" s="13"/>
       <c r="E200" s="13"/>
     </row>
-    <row r="201" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A201" s="12"/>
       <c r="B201" s="13"/>
       <c r="C201" s="12"/>
       <c r="D201" s="13"/>
       <c r="E201" s="13"/>
     </row>
-    <row r="202" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A202" s="12"/>
       <c r="B202" s="13"/>
       <c r="C202" s="12"/>
       <c r="D202" s="13"/>
       <c r="E202" s="13"/>
     </row>
-    <row r="203" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A203" s="12"/>
       <c r="B203" s="13"/>
       <c r="C203" s="12"/>
       <c r="D203" s="13"/>
       <c r="E203" s="13"/>
     </row>
-    <row r="204" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A204" s="12"/>
       <c r="B204" s="13"/>
       <c r="C204" s="12"/>
       <c r="D204" s="13"/>
       <c r="E204" s="13"/>
     </row>
-    <row r="205" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A205" s="12"/>
       <c r="B205" s="13"/>
       <c r="C205" s="12"/>
       <c r="D205" s="13"/>
       <c r="E205" s="13"/>
     </row>
-    <row r="206" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A206" s="12"/>
       <c r="B206" s="13"/>
       <c r="C206" s="12"/>
       <c r="D206" s="13"/>
       <c r="E206" s="13"/>
     </row>
-    <row r="207" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A207" s="12"/>
       <c r="B207" s="13"/>
       <c r="C207" s="12"/>
       <c r="D207" s="13"/>
       <c r="E207" s="13"/>
     </row>
-    <row r="208" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A208" s="12"/>
       <c r="B208" s="13"/>
       <c r="C208" s="12"/>
       <c r="D208" s="13"/>
       <c r="E208" s="13"/>
     </row>
-    <row r="209" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A209" s="12"/>
       <c r="B209" s="13"/>
       <c r="C209" s="12"/>
       <c r="D209" s="13"/>
       <c r="E209" s="13"/>
     </row>
-    <row r="210" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A210" s="12"/>
       <c r="B210" s="13"/>
       <c r="C210" s="12"/>
       <c r="D210" s="13"/>
       <c r="E210" s="13"/>
     </row>
-    <row r="211" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A211" s="12"/>
       <c r="B211" s="13"/>
       <c r="C211" s="12"/>
       <c r="D211" s="13"/>
       <c r="E211" s="13"/>
     </row>
-    <row r="212" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A212" s="12"/>
       <c r="B212" s="13"/>
       <c r="C212" s="12"/>
       <c r="D212" s="13"/>
       <c r="E212" s="13"/>
     </row>
-    <row r="213" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A213" s="12"/>
       <c r="B213" s="13"/>
       <c r="C213" s="12"/>
       <c r="D213" s="13"/>
       <c r="E213" s="13"/>
     </row>
-    <row r="214" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A214" s="12"/>
       <c r="B214" s="13"/>
       <c r="C214" s="12"/>
       <c r="D214" s="13"/>
       <c r="E214" s="13"/>
     </row>
-    <row r="215" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A215" s="12"/>
       <c r="B215" s="13"/>
       <c r="C215" s="12"/>
       <c r="D215" s="13"/>
       <c r="E215" s="13"/>
     </row>
-    <row r="216" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A216" s="12"/>
       <c r="B216" s="13"/>
       <c r="C216" s="12"/>
       <c r="D216" s="13"/>
       <c r="E216" s="13"/>
     </row>
-    <row r="217" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A217" s="12"/>
       <c r="B217" s="13"/>
       <c r="C217" s="12"/>
       <c r="D217" s="13"/>
       <c r="E217" s="13"/>
     </row>
-    <row r="218" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A218" s="12"/>
       <c r="B218" s="13"/>
       <c r="C218" s="12"/>
       <c r="D218" s="13"/>
       <c r="E218" s="13"/>
     </row>
-    <row r="219" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A219" s="12"/>
       <c r="B219" s="13"/>
       <c r="C219" s="12"/>
       <c r="D219" s="13"/>
       <c r="E219" s="13"/>
     </row>
-    <row r="220" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A220" s="12"/>
       <c r="B220" s="13"/>
       <c r="C220" s="12"/>
       <c r="D220" s="13"/>
       <c r="E220" s="13"/>
     </row>
-    <row r="221" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A221" s="12"/>
       <c r="B221" s="13"/>
       <c r="C221" s="12"/>
       <c r="D221" s="13"/>
       <c r="E221" s="13"/>
     </row>
-    <row r="222" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A222" s="12"/>
       <c r="B222" s="13"/>
       <c r="C222" s="12"/>
       <c r="D222" s="13"/>
       <c r="E222" s="13"/>
     </row>
-    <row r="223" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A223" s="12"/>
       <c r="B223" s="13"/>
       <c r="C223" s="12"/>
       <c r="D223" s="13"/>
       <c r="E223" s="13"/>
     </row>
-    <row r="224" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A224" s="12"/>
       <c r="B224" s="13"/>
       <c r="C224" s="12"/>
       <c r="D224" s="13"/>
       <c r="E224" s="13"/>
     </row>
-    <row r="225" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A225" s="12"/>
       <c r="B225" s="13"/>
       <c r="C225" s="12"/>
       <c r="D225" s="13"/>
       <c r="E225" s="13"/>
     </row>
-    <row r="226" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A226" s="12"/>
       <c r="B226" s="13"/>
       <c r="C226" s="12"/>
       <c r="D226" s="13"/>
       <c r="E226" s="13"/>
     </row>
-    <row r="227" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A227" s="12"/>
       <c r="B227" s="13"/>
       <c r="C227" s="12"/>
       <c r="D227" s="13"/>
       <c r="E227" s="13"/>
     </row>
-    <row r="228" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A228" s="12"/>
       <c r="B228" s="13"/>
       <c r="C228" s="12"/>
       <c r="D228" s="13"/>
       <c r="E228" s="13"/>
     </row>
-    <row r="229" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A229" s="12"/>
       <c r="B229" s="13"/>
       <c r="C229" s="12"/>
       <c r="D229" s="13"/>
       <c r="E229" s="13"/>
     </row>
-    <row r="230" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A230" s="12"/>
       <c r="B230" s="13"/>
       <c r="C230" s="12"/>
       <c r="D230" s="13"/>
       <c r="E230" s="13"/>
     </row>
-    <row r="231" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A231" s="12"/>
       <c r="B231" s="13"/>
       <c r="C231" s="12"/>
       <c r="D231" s="13"/>
       <c r="E231" s="13"/>
     </row>
-    <row r="232" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A232" s="12"/>
       <c r="B232" s="13"/>
       <c r="C232" s="12"/>
       <c r="D232" s="13"/>
       <c r="E232" s="13"/>
     </row>
-    <row r="233" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A233" s="12"/>
       <c r="B233" s="13"/>
       <c r="C233" s="12"/>
       <c r="D233" s="13"/>
       <c r="E233" s="13"/>
     </row>
-    <row r="234" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A234" s="12"/>
       <c r="B234" s="13"/>
       <c r="C234" s="12"/>
       <c r="D234" s="13"/>
       <c r="E234" s="13"/>
     </row>
-    <row r="235" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A235" s="12"/>
       <c r="B235" s="13"/>
       <c r="C235" s="12"/>
       <c r="D235" s="13"/>
       <c r="E235" s="13"/>
     </row>
-    <row r="236" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A236" s="12"/>
       <c r="B236" s="13"/>
       <c r="C236" s="12"/>
       <c r="D236" s="13"/>
       <c r="E236" s="13"/>
     </row>
-    <row r="237" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A237" s="12"/>
       <c r="B237" s="13"/>
       <c r="C237" s="12"/>
       <c r="D237" s="13"/>
       <c r="E237" s="13"/>
     </row>
-    <row r="238" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A238" s="12"/>
       <c r="B238" s="13"/>
       <c r="C238" s="12"/>
       <c r="D238" s="13"/>
       <c r="E238" s="13"/>
     </row>
-    <row r="239" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A239" s="12"/>
       <c r="B239" s="13"/>
       <c r="C239" s="12"/>
       <c r="D239" s="13"/>
       <c r="E239" s="13"/>
     </row>
-    <row r="240" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A240" s="12"/>
       <c r="B240" s="13"/>
       <c r="C240" s="12"/>
       <c r="D240" s="13"/>
       <c r="E240" s="13"/>
     </row>
-    <row r="241" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A241" s="12"/>
       <c r="B241" s="13"/>
       <c r="C241" s="12"/>
       <c r="D241" s="13"/>
       <c r="E241" s="13"/>
     </row>
-    <row r="242" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A242" s="12"/>
       <c r="B242" s="13"/>
       <c r="C242" s="12"/>
       <c r="D242" s="13"/>
       <c r="E242" s="13"/>
     </row>
-    <row r="243" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A243" s="12"/>
       <c r="B243" s="13"/>
       <c r="C243" s="12"/>
       <c r="D243" s="13"/>
       <c r="E243" s="13"/>
     </row>
-    <row r="244" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A244" s="12"/>
       <c r="B244" s="13"/>
       <c r="C244" s="12"/>
       <c r="D244" s="13"/>
       <c r="E244" s="13"/>
     </row>
-    <row r="245" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A245" s="12"/>
       <c r="B245" s="13"/>
       <c r="C245" s="12"/>
       <c r="D245" s="13"/>
       <c r="E245" s="13"/>
     </row>
-    <row r="246" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A246" s="12"/>
       <c r="B246" s="13"/>
       <c r="C246" s="12"/>
       <c r="D246" s="13"/>
       <c r="E246" s="13"/>
     </row>
-    <row r="247" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A247" s="12"/>
       <c r="B247" s="13"/>
       <c r="C247" s="12"/>
       <c r="D247" s="13"/>
       <c r="E247" s="13"/>
     </row>
-    <row r="248" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A248" s="12"/>
       <c r="B248" s="13"/>
       <c r="C248" s="12"/>
       <c r="D248" s="13"/>
       <c r="E248" s="13"/>
     </row>
-    <row r="249" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A249" s="12"/>
       <c r="B249" s="13"/>
       <c r="C249" s="12"/>
       <c r="D249" s="13"/>
       <c r="E249" s="13"/>
     </row>
-    <row r="250" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A250" s="12"/>
       <c r="B250" s="13"/>
       <c r="C250" s="12"/>
       <c r="D250" s="13"/>
       <c r="E250" s="13"/>
     </row>
-    <row r="251" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A251" s="12"/>
       <c r="B251" s="13"/>
       <c r="C251" s="12"/>
       <c r="D251" s="13"/>
       <c r="E251" s="13"/>
     </row>
-    <row r="252" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A252" s="12"/>
       <c r="B252" s="13"/>
       <c r="C252" s="12"/>
       <c r="D252" s="13"/>
       <c r="E252" s="13"/>
     </row>
-    <row r="253" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A253" s="12"/>
       <c r="B253" s="13"/>
       <c r="C253" s="12"/>
       <c r="D253" s="13"/>
       <c r="E253" s="13"/>
     </row>
-    <row r="254" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A254" s="12"/>
       <c r="B254" s="13"/>
       <c r="C254" s="12"/>
       <c r="D254" s="13"/>
       <c r="E254" s="13"/>
     </row>
-    <row r="255" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A255" s="12"/>
       <c r="B255" s="13"/>
       <c r="C255" s="12"/>
       <c r="D255" s="13"/>
       <c r="E255" s="13"/>
     </row>
-    <row r="256" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A256" s="12"/>
       <c r="B256" s="13"/>
       <c r="C256" s="12"/>
       <c r="D256" s="13"/>
       <c r="E256" s="13"/>
     </row>
-    <row r="257" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A257" s="12"/>
       <c r="B257" s="13"/>
       <c r="C257" s="12"/>
       <c r="D257" s="13"/>
       <c r="E257" s="13"/>
     </row>
-    <row r="258" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="258" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A258" s="12"/>
       <c r="B258" s="13"/>
       <c r="C258" s="12"/>
       <c r="D258" s="13"/>
       <c r="E258" s="13"/>
     </row>
-    <row r="259" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="259" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A259" s="12"/>
       <c r="B259" s="13"/>
       <c r="C259" s="12"/>
       <c r="D259" s="13"/>
       <c r="E259" s="13"/>
     </row>
-    <row r="260" spans="1:5" ht="15.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="260" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A260" s="12"/>
       <c r="B260" s="13"/>
       <c r="C260" s="12"/>
@@ -3019,12 +3042,13 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D27" r:id="rId1"/>
-    <hyperlink ref="D28" r:id="rId2"/>
-    <hyperlink ref="D29" r:id="rId3"/>
-    <hyperlink ref="D30" r:id="rId4"/>
-    <hyperlink ref="D31" r:id="rId5"/>
-    <hyperlink ref="D32" r:id="rId6"/>
+    <hyperlink ref="D27" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="D28" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="D29" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="D30" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="D31" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="D32" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="D33" r:id="rId7" xr:uid="{BBC1248B-06CC-4E1E-8932-721BE97320AF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
se agrega el alumno 33 al archivo
</commit_message>
<xml_diff>
--- a/Lista de Alumnos.xlsx
+++ b/Lista de Alumnos.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LILEN\Desktop\ISPC !!\carrera TELECOMUNICACIONES aula1\ELECTRONICA\electronica vacaciones\Alumnos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ISPC CORDOBA\CARRERAS\TEC. EN TELECOMUNICACIONES\CURSO ELECTRONICA MICROCONTROLADA TST\PROYECTO\Alumnos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{451EB38E-7C65-4641-88AA-18D387720696}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C75395B0-C4DA-4FC8-AF3E-5A15536D30FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="103">
   <si>
     <t>#</t>
   </si>
@@ -320,6 +320,15 @@
   </si>
   <si>
     <t>lilenguzman01</t>
+  </si>
+  <si>
+    <t>Juan Carlos Narvaez</t>
+  </si>
+  <si>
+    <t>jackelectronico@gmail.com</t>
+  </si>
+  <si>
+    <t>ProgramadorPegasus</t>
   </si>
 </sst>
 </file>
@@ -827,8 +836,8 @@
   </sheetPr>
   <dimension ref="A1:E260"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1401,10 +1410,18 @@
       <c r="A34" s="5">
         <v>33</v>
       </c>
-      <c r="B34" s="6"/>
-      <c r="C34" s="5"/>
-      <c r="D34" s="6"/>
-      <c r="E34" s="6"/>
+      <c r="B34" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="C34" s="5">
+        <v>4</v>
+      </c>
+      <c r="D34" s="16" t="s">
+        <v>101</v>
+      </c>
+      <c r="E34" s="6" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="35" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="5">
@@ -3049,6 +3066,7 @@
     <hyperlink ref="D31" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
     <hyperlink ref="D32" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
     <hyperlink ref="D33" r:id="rId7" xr:uid="{BBC1248B-06CC-4E1E-8932-721BE97320AF}"/>
+    <hyperlink ref="D34" r:id="rId8" xr:uid="{FA76FA2B-5206-4A3D-AB9B-DF08FEDB8744}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Se agrega el 35 alumno al archivo
</commit_message>
<xml_diff>
--- a/Lista de Alumnos.xlsx
+++ b/Lista de Alumnos.xlsx
@@ -835,7 +835,7 @@
     <col min="5" max="5" style="15" width="29.005" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="27.2">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="27">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1188,7 +1188,7 @@
         <v>63</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="25.5">
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="19.5">
       <c r="A22" s="5">
         <v>21</v>
       </c>

</xml_diff>

<commit_message>
nuevo commit de mi nueva rama
</commit_message>
<xml_diff>
--- a/Lista de Alumnos.xlsx
+++ b/Lista de Alumnos.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\Electronica micro\Alumnos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\PRACTICAS\Alumnos\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="112">
   <si>
     <t>#</t>
   </si>
@@ -346,13 +346,22 @@
   </si>
   <si>
     <t>GiseRomero</t>
+  </si>
+  <si>
+    <t>Esteban Dario Carrizo</t>
+  </si>
+  <si>
+    <t>carrizoe68@gmail.com</t>
+  </si>
+  <si>
+    <t>estebancarrizo</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -405,6 +414,14 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -483,10 +500,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -534,8 +552,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -841,8 +863,8 @@
   </sheetPr>
   <dimension ref="A1:E260"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="G34" sqref="G34"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1466,10 +1488,18 @@
       <c r="A37" s="5">
         <v>36</v>
       </c>
-      <c r="B37" s="6"/>
-      <c r="C37" s="5"/>
-      <c r="D37" s="6"/>
-      <c r="E37" s="6"/>
+      <c r="B37" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="C37" s="5">
+        <v>2</v>
+      </c>
+      <c r="D37" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="E37" s="6" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="38" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="5">
@@ -3079,6 +3109,9 @@
       <c r="E260" s="13"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D37" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Se agrega  Alumno N° [37]
</commit_message>
<xml_diff>
--- a/Lista de Alumnos.xlsx
+++ b/Lista de Alumnos.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\PRACTICAS\Alumnos\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505"/>
   </bookViews>
@@ -19,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="115">
   <si>
     <t>#</t>
   </si>
@@ -355,12 +350,21 @@
   </si>
   <si>
     <t>estebancarrizo</t>
+  </si>
+  <si>
+    <t>Ruiz Gloria Beatriz</t>
+  </si>
+  <si>
+    <t>gloriabeatrizruiz0@gmail.com</t>
+  </si>
+  <si>
+    <t>ruizgb</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -864,7 +868,7 @@
   <dimension ref="A1:E260"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="E37" sqref="E37"/>
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1505,10 +1509,18 @@
       <c r="A38" s="5">
         <v>37</v>
       </c>
-      <c r="B38" s="6"/>
-      <c r="C38" s="5"/>
-      <c r="D38" s="6"/>
-      <c r="E38" s="6"/>
+      <c r="B38" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="C38" s="5">
+        <v>2</v>
+      </c>
+      <c r="D38" s="17" t="s">
+        <v>113</v>
+      </c>
+      <c r="E38" s="6" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="39" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="5">
@@ -3111,6 +3123,7 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D37" r:id="rId1"/>
+    <hyperlink ref="D38" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Se agrega fila de prueba por porblemas con una compañera
</commit_message>
<xml_diff>
--- a/Lista de Alumnos.xlsx
+++ b/Lista de Alumnos.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PerfLogs\Proyecto\Practicas\Alumnos\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505"/>
   </bookViews>
@@ -14,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="116">
   <si>
     <t>#</t>
   </si>
@@ -359,6 +364,9 @@
   </si>
   <si>
     <t>ruizgb</t>
+  </si>
+  <si>
+    <t>Victoria MAVI</t>
   </si>
 </sst>
 </file>
@@ -1526,7 +1534,9 @@
       <c r="A39" s="5">
         <v>38</v>
       </c>
-      <c r="B39" s="6"/>
+      <c r="B39" s="6" t="s">
+        <v>115</v>
+      </c>
       <c r="C39" s="5"/>
       <c r="D39" s="6"/>
       <c r="E39" s="6"/>

</xml_diff>

<commit_message>
Se agrega el [39] Alumno al archivo
</commit_message>
<xml_diff>
--- a/Lista de Alumnos.xlsx
+++ b/Lista de Alumnos.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PerfLogs\Proyecto\Practicas\Alumnos\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18200" windowHeight="8510"/>
   </bookViews>
   <sheets>
     <sheet name="Electronica Microcontrolada" sheetId="1" r:id="rId1"/>
@@ -19,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="119">
   <si>
     <t>#</t>
   </si>
@@ -367,6 +362,15 @@
   </si>
   <si>
     <t>Victoria MAVI</t>
+  </si>
+  <si>
+    <t>Dario Maldonado</t>
+  </si>
+  <si>
+    <t>d-maldo9@hotmail.com</t>
+  </si>
+  <si>
+    <t>darman82</t>
   </si>
 </sst>
 </file>
@@ -876,14 +880,14 @@
   <dimension ref="A1:E260"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+      <selection activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="6.85546875" style="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="37.140625" style="15" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.5703125" style="14" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.81640625" style="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.1796875" style="15" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.54296875" style="14" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="31" style="15" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="29" style="15" bestFit="1" customWidth="1"/>
   </cols>
@@ -1088,7 +1092,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="5">
         <v>12</v>
       </c>
@@ -1394,7 +1398,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="5">
         <v>30</v>
       </c>
@@ -1541,14 +1545,22 @@
       <c r="D39" s="6"/>
       <c r="E39" s="6"/>
     </row>
-    <row r="40" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" s="5">
         <v>39</v>
       </c>
-      <c r="B40" s="6"/>
-      <c r="C40" s="5"/>
-      <c r="D40" s="6"/>
-      <c r="E40" s="6"/>
+      <c r="B40" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="C40" s="5">
+        <v>2</v>
+      </c>
+      <c r="D40" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="E40" s="6" t="s">
+        <v>118</v>
+      </c>
     </row>
     <row r="41" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="5">
@@ -1631,7 +1643,7 @@
       <c r="D49" s="6"/>
       <c r="E49" s="6"/>
     </row>
-    <row r="50" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A50" s="5">
         <v>49</v>
       </c>
@@ -1640,7 +1652,7 @@
       <c r="D50" s="6"/>
       <c r="E50" s="6"/>
     </row>
-    <row r="51" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A51" s="5">
         <v>50</v>
       </c>
@@ -1649,7 +1661,7 @@
       <c r="D51" s="6"/>
       <c r="E51" s="6"/>
     </row>
-    <row r="52" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A52" s="5">
         <v>51</v>
       </c>
@@ -1658,7 +1670,7 @@
       <c r="D52" s="6"/>
       <c r="E52" s="6"/>
     </row>
-    <row r="53" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A53" s="5">
         <v>52</v>
       </c>
@@ -1667,7 +1679,7 @@
       <c r="D53" s="6"/>
       <c r="E53" s="6"/>
     </row>
-    <row r="54" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A54" s="5">
         <v>53</v>
       </c>
@@ -1676,7 +1688,7 @@
       <c r="D54" s="6"/>
       <c r="E54" s="6"/>
     </row>
-    <row r="55" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A55" s="5">
         <v>54</v>
       </c>
@@ -1685,7 +1697,7 @@
       <c r="D55" s="6"/>
       <c r="E55" s="6"/>
     </row>
-    <row r="56" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A56" s="5">
         <v>55</v>
       </c>
@@ -1694,7 +1706,7 @@
       <c r="D56" s="6"/>
       <c r="E56" s="6"/>
     </row>
-    <row r="57" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A57" s="5">
         <v>56</v>
       </c>
@@ -1703,7 +1715,7 @@
       <c r="D57" s="6"/>
       <c r="E57" s="6"/>
     </row>
-    <row r="58" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A58" s="5">
         <v>57</v>
       </c>
@@ -1712,7 +1724,7 @@
       <c r="D58" s="6"/>
       <c r="E58" s="6"/>
     </row>
-    <row r="59" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A59" s="5">
         <v>58</v>
       </c>
@@ -1721,7 +1733,7 @@
       <c r="D59" s="6"/>
       <c r="E59" s="6"/>
     </row>
-    <row r="60" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A60" s="5">
         <v>59</v>
       </c>
@@ -1730,1400 +1742,1400 @@
       <c r="D60" s="6"/>
       <c r="E60" s="6"/>
     </row>
-    <row r="61" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A61" s="12"/>
       <c r="B61" s="13"/>
       <c r="C61" s="12"/>
       <c r="D61" s="13"/>
       <c r="E61" s="13"/>
     </row>
-    <row r="62" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A62" s="12"/>
       <c r="B62" s="13"/>
       <c r="C62" s="12"/>
       <c r="D62" s="13"/>
       <c r="E62" s="13"/>
     </row>
-    <row r="63" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A63" s="12"/>
       <c r="B63" s="13"/>
       <c r="C63" s="12"/>
       <c r="D63" s="13"/>
       <c r="E63" s="13"/>
     </row>
-    <row r="64" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A64" s="12"/>
       <c r="B64" s="13"/>
       <c r="C64" s="12"/>
       <c r="D64" s="13"/>
       <c r="E64" s="13"/>
     </row>
-    <row r="65" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A65" s="12"/>
       <c r="B65" s="13"/>
       <c r="C65" s="12"/>
       <c r="D65" s="13"/>
       <c r="E65" s="13"/>
     </row>
-    <row r="66" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A66" s="12"/>
       <c r="B66" s="13"/>
       <c r="C66" s="12"/>
       <c r="D66" s="13"/>
       <c r="E66" s="13"/>
     </row>
-    <row r="67" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A67" s="12"/>
       <c r="B67" s="13"/>
       <c r="C67" s="12"/>
       <c r="D67" s="13"/>
       <c r="E67" s="13"/>
     </row>
-    <row r="68" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A68" s="12"/>
       <c r="B68" s="13"/>
       <c r="C68" s="12"/>
       <c r="D68" s="13"/>
       <c r="E68" s="13"/>
     </row>
-    <row r="69" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A69" s="12"/>
       <c r="B69" s="13"/>
       <c r="C69" s="12"/>
       <c r="D69" s="13"/>
       <c r="E69" s="13"/>
     </row>
-    <row r="70" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A70" s="12"/>
       <c r="B70" s="13"/>
       <c r="C70" s="12"/>
       <c r="D70" s="13"/>
       <c r="E70" s="13"/>
     </row>
-    <row r="71" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A71" s="12"/>
       <c r="B71" s="13"/>
       <c r="C71" s="12"/>
       <c r="D71" s="13"/>
       <c r="E71" s="13"/>
     </row>
-    <row r="72" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A72" s="12"/>
       <c r="B72" s="13"/>
       <c r="C72" s="12"/>
       <c r="D72" s="13"/>
       <c r="E72" s="13"/>
     </row>
-    <row r="73" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A73" s="12"/>
       <c r="B73" s="13"/>
       <c r="C73" s="12"/>
       <c r="D73" s="13"/>
       <c r="E73" s="13"/>
     </row>
-    <row r="74" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A74" s="12"/>
       <c r="B74" s="13"/>
       <c r="C74" s="12"/>
       <c r="D74" s="13"/>
       <c r="E74" s="13"/>
     </row>
-    <row r="75" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A75" s="12"/>
       <c r="B75" s="13"/>
       <c r="C75" s="12"/>
       <c r="D75" s="13"/>
       <c r="E75" s="13"/>
     </row>
-    <row r="76" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A76" s="12"/>
       <c r="B76" s="13"/>
       <c r="C76" s="12"/>
       <c r="D76" s="13"/>
       <c r="E76" s="13"/>
     </row>
-    <row r="77" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A77" s="12"/>
       <c r="B77" s="13"/>
       <c r="C77" s="12"/>
       <c r="D77" s="13"/>
       <c r="E77" s="13"/>
     </row>
-    <row r="78" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A78" s="12"/>
       <c r="B78" s="13"/>
       <c r="C78" s="12"/>
       <c r="D78" s="13"/>
       <c r="E78" s="13"/>
     </row>
-    <row r="79" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A79" s="12"/>
       <c r="B79" s="13"/>
       <c r="C79" s="12"/>
       <c r="D79" s="13"/>
       <c r="E79" s="13"/>
     </row>
-    <row r="80" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A80" s="12"/>
       <c r="B80" s="13"/>
       <c r="C80" s="12"/>
       <c r="D80" s="13"/>
       <c r="E80" s="13"/>
     </row>
-    <row r="81" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A81" s="12"/>
       <c r="B81" s="13"/>
       <c r="C81" s="12"/>
       <c r="D81" s="13"/>
       <c r="E81" s="13"/>
     </row>
-    <row r="82" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A82" s="12"/>
       <c r="B82" s="13"/>
       <c r="C82" s="12"/>
       <c r="D82" s="13"/>
       <c r="E82" s="13"/>
     </row>
-    <row r="83" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A83" s="12"/>
       <c r="B83" s="13"/>
       <c r="C83" s="12"/>
       <c r="D83" s="13"/>
       <c r="E83" s="13"/>
     </row>
-    <row r="84" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A84" s="12"/>
       <c r="B84" s="13"/>
       <c r="C84" s="12"/>
       <c r="D84" s="13"/>
       <c r="E84" s="13"/>
     </row>
-    <row r="85" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A85" s="12"/>
       <c r="B85" s="13"/>
       <c r="C85" s="12"/>
       <c r="D85" s="13"/>
       <c r="E85" s="13"/>
     </row>
-    <row r="86" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A86" s="12"/>
       <c r="B86" s="13"/>
       <c r="C86" s="12"/>
       <c r="D86" s="13"/>
       <c r="E86" s="13"/>
     </row>
-    <row r="87" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A87" s="12"/>
       <c r="B87" s="13"/>
       <c r="C87" s="12"/>
       <c r="D87" s="13"/>
       <c r="E87" s="13"/>
     </row>
-    <row r="88" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A88" s="12"/>
       <c r="B88" s="13"/>
       <c r="C88" s="12"/>
       <c r="D88" s="13"/>
       <c r="E88" s="13"/>
     </row>
-    <row r="89" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A89" s="12"/>
       <c r="B89" s="13"/>
       <c r="C89" s="12"/>
       <c r="D89" s="13"/>
       <c r="E89" s="13"/>
     </row>
-    <row r="90" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A90" s="12"/>
       <c r="B90" s="13"/>
       <c r="C90" s="12"/>
       <c r="D90" s="13"/>
       <c r="E90" s="13"/>
     </row>
-    <row r="91" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A91" s="12"/>
       <c r="B91" s="13"/>
       <c r="C91" s="12"/>
       <c r="D91" s="13"/>
       <c r="E91" s="13"/>
     </row>
-    <row r="92" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A92" s="12"/>
       <c r="B92" s="13"/>
       <c r="C92" s="12"/>
       <c r="D92" s="13"/>
       <c r="E92" s="13"/>
     </row>
-    <row r="93" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A93" s="12"/>
       <c r="B93" s="13"/>
       <c r="C93" s="12"/>
       <c r="D93" s="13"/>
       <c r="E93" s="13"/>
     </row>
-    <row r="94" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A94" s="12"/>
       <c r="B94" s="13"/>
       <c r="C94" s="12"/>
       <c r="D94" s="13"/>
       <c r="E94" s="13"/>
     </row>
-    <row r="95" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A95" s="12"/>
       <c r="B95" s="13"/>
       <c r="C95" s="12"/>
       <c r="D95" s="13"/>
       <c r="E95" s="13"/>
     </row>
-    <row r="96" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A96" s="12"/>
       <c r="B96" s="13"/>
       <c r="C96" s="12"/>
       <c r="D96" s="13"/>
       <c r="E96" s="13"/>
     </row>
-    <row r="97" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A97" s="12"/>
       <c r="B97" s="13"/>
       <c r="C97" s="12"/>
       <c r="D97" s="13"/>
       <c r="E97" s="13"/>
     </row>
-    <row r="98" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A98" s="12"/>
       <c r="B98" s="13"/>
       <c r="C98" s="12"/>
       <c r="D98" s="13"/>
       <c r="E98" s="13"/>
     </row>
-    <row r="99" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A99" s="12"/>
       <c r="B99" s="13"/>
       <c r="C99" s="12"/>
       <c r="D99" s="13"/>
       <c r="E99" s="13"/>
     </row>
-    <row r="100" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A100" s="12"/>
       <c r="B100" s="13"/>
       <c r="C100" s="12"/>
       <c r="D100" s="13"/>
       <c r="E100" s="13"/>
     </row>
-    <row r="101" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A101" s="12"/>
       <c r="B101" s="13"/>
       <c r="C101" s="12"/>
       <c r="D101" s="13"/>
       <c r="E101" s="13"/>
     </row>
-    <row r="102" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A102" s="12"/>
       <c r="B102" s="13"/>
       <c r="C102" s="12"/>
       <c r="D102" s="13"/>
       <c r="E102" s="13"/>
     </row>
-    <row r="103" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A103" s="12"/>
       <c r="B103" s="13"/>
       <c r="C103" s="12"/>
       <c r="D103" s="13"/>
       <c r="E103" s="13"/>
     </row>
-    <row r="104" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A104" s="12"/>
       <c r="B104" s="13"/>
       <c r="C104" s="12"/>
       <c r="D104" s="13"/>
       <c r="E104" s="13"/>
     </row>
-    <row r="105" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A105" s="12"/>
       <c r="B105" s="13"/>
       <c r="C105" s="12"/>
       <c r="D105" s="13"/>
       <c r="E105" s="13"/>
     </row>
-    <row r="106" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A106" s="12"/>
       <c r="B106" s="13"/>
       <c r="C106" s="12"/>
       <c r="D106" s="13"/>
       <c r="E106" s="13"/>
     </row>
-    <row r="107" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A107" s="12"/>
       <c r="B107" s="13"/>
       <c r="C107" s="12"/>
       <c r="D107" s="13"/>
       <c r="E107" s="13"/>
     </row>
-    <row r="108" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A108" s="12"/>
       <c r="B108" s="13"/>
       <c r="C108" s="12"/>
       <c r="D108" s="13"/>
       <c r="E108" s="13"/>
     </row>
-    <row r="109" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A109" s="12"/>
       <c r="B109" s="13"/>
       <c r="C109" s="12"/>
       <c r="D109" s="13"/>
       <c r="E109" s="13"/>
     </row>
-    <row r="110" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A110" s="12"/>
       <c r="B110" s="13"/>
       <c r="C110" s="12"/>
       <c r="D110" s="13"/>
       <c r="E110" s="13"/>
     </row>
-    <row r="111" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A111" s="12"/>
       <c r="B111" s="13"/>
       <c r="C111" s="12"/>
       <c r="D111" s="13"/>
       <c r="E111" s="13"/>
     </row>
-    <row r="112" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A112" s="12"/>
       <c r="B112" s="13"/>
       <c r="C112" s="12"/>
       <c r="D112" s="13"/>
       <c r="E112" s="13"/>
     </row>
-    <row r="113" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A113" s="12"/>
       <c r="B113" s="13"/>
       <c r="C113" s="12"/>
       <c r="D113" s="13"/>
       <c r="E113" s="13"/>
     </row>
-    <row r="114" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A114" s="12"/>
       <c r="B114" s="13"/>
       <c r="C114" s="12"/>
       <c r="D114" s="13"/>
       <c r="E114" s="13"/>
     </row>
-    <row r="115" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A115" s="12"/>
       <c r="B115" s="13"/>
       <c r="C115" s="12"/>
       <c r="D115" s="13"/>
       <c r="E115" s="13"/>
     </row>
-    <row r="116" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A116" s="12"/>
       <c r="B116" s="13"/>
       <c r="C116" s="12"/>
       <c r="D116" s="13"/>
       <c r="E116" s="13"/>
     </row>
-    <row r="117" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A117" s="12"/>
       <c r="B117" s="13"/>
       <c r="C117" s="12"/>
       <c r="D117" s="13"/>
       <c r="E117" s="13"/>
     </row>
-    <row r="118" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A118" s="12"/>
       <c r="B118" s="13"/>
       <c r="C118" s="12"/>
       <c r="D118" s="13"/>
       <c r="E118" s="13"/>
     </row>
-    <row r="119" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A119" s="12"/>
       <c r="B119" s="13"/>
       <c r="C119" s="12"/>
       <c r="D119" s="13"/>
       <c r="E119" s="13"/>
     </row>
-    <row r="120" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A120" s="12"/>
       <c r="B120" s="13"/>
       <c r="C120" s="12"/>
       <c r="D120" s="13"/>
       <c r="E120" s="13"/>
     </row>
-    <row r="121" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A121" s="12"/>
       <c r="B121" s="13"/>
       <c r="C121" s="12"/>
       <c r="D121" s="13"/>
       <c r="E121" s="13"/>
     </row>
-    <row r="122" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A122" s="12"/>
       <c r="B122" s="13"/>
       <c r="C122" s="12"/>
       <c r="D122" s="13"/>
       <c r="E122" s="13"/>
     </row>
-    <row r="123" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A123" s="12"/>
       <c r="B123" s="13"/>
       <c r="C123" s="12"/>
       <c r="D123" s="13"/>
       <c r="E123" s="13"/>
     </row>
-    <row r="124" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A124" s="12"/>
       <c r="B124" s="13"/>
       <c r="C124" s="12"/>
       <c r="D124" s="13"/>
       <c r="E124" s="13"/>
     </row>
-    <row r="125" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A125" s="12"/>
       <c r="B125" s="13"/>
       <c r="C125" s="12"/>
       <c r="D125" s="13"/>
       <c r="E125" s="13"/>
     </row>
-    <row r="126" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A126" s="12"/>
       <c r="B126" s="13"/>
       <c r="C126" s="12"/>
       <c r="D126" s="13"/>
       <c r="E126" s="13"/>
     </row>
-    <row r="127" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A127" s="12"/>
       <c r="B127" s="13"/>
       <c r="C127" s="12"/>
       <c r="D127" s="13"/>
       <c r="E127" s="13"/>
     </row>
-    <row r="128" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A128" s="12"/>
       <c r="B128" s="13"/>
       <c r="C128" s="12"/>
       <c r="D128" s="13"/>
       <c r="E128" s="13"/>
     </row>
-    <row r="129" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A129" s="12"/>
       <c r="B129" s="13"/>
       <c r="C129" s="12"/>
       <c r="D129" s="13"/>
       <c r="E129" s="13"/>
     </row>
-    <row r="130" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A130" s="12"/>
       <c r="B130" s="13"/>
       <c r="C130" s="12"/>
       <c r="D130" s="13"/>
       <c r="E130" s="13"/>
     </row>
-    <row r="131" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A131" s="12"/>
       <c r="B131" s="13"/>
       <c r="C131" s="12"/>
       <c r="D131" s="13"/>
       <c r="E131" s="13"/>
     </row>
-    <row r="132" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A132" s="12"/>
       <c r="B132" s="13"/>
       <c r="C132" s="12"/>
       <c r="D132" s="13"/>
       <c r="E132" s="13"/>
     </row>
-    <row r="133" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A133" s="12"/>
       <c r="B133" s="13"/>
       <c r="C133" s="12"/>
       <c r="D133" s="13"/>
       <c r="E133" s="13"/>
     </row>
-    <row r="134" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A134" s="12"/>
       <c r="B134" s="13"/>
       <c r="C134" s="12"/>
       <c r="D134" s="13"/>
       <c r="E134" s="13"/>
     </row>
-    <row r="135" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A135" s="12"/>
       <c r="B135" s="13"/>
       <c r="C135" s="12"/>
       <c r="D135" s="13"/>
       <c r="E135" s="13"/>
     </row>
-    <row r="136" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A136" s="12"/>
       <c r="B136" s="13"/>
       <c r="C136" s="12"/>
       <c r="D136" s="13"/>
       <c r="E136" s="13"/>
     </row>
-    <row r="137" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A137" s="12"/>
       <c r="B137" s="13"/>
       <c r="C137" s="12"/>
       <c r="D137" s="13"/>
       <c r="E137" s="13"/>
     </row>
-    <row r="138" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A138" s="12"/>
       <c r="B138" s="13"/>
       <c r="C138" s="12"/>
       <c r="D138" s="13"/>
       <c r="E138" s="13"/>
     </row>
-    <row r="139" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A139" s="12"/>
       <c r="B139" s="13"/>
       <c r="C139" s="12"/>
       <c r="D139" s="13"/>
       <c r="E139" s="13"/>
     </row>
-    <row r="140" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A140" s="12"/>
       <c r="B140" s="13"/>
       <c r="C140" s="12"/>
       <c r="D140" s="13"/>
       <c r="E140" s="13"/>
     </row>
-    <row r="141" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A141" s="12"/>
       <c r="B141" s="13"/>
       <c r="C141" s="12"/>
       <c r="D141" s="13"/>
       <c r="E141" s="13"/>
     </row>
-    <row r="142" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A142" s="12"/>
       <c r="B142" s="13"/>
       <c r="C142" s="12"/>
       <c r="D142" s="13"/>
       <c r="E142" s="13"/>
     </row>
-    <row r="143" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A143" s="12"/>
       <c r="B143" s="13"/>
       <c r="C143" s="12"/>
       <c r="D143" s="13"/>
       <c r="E143" s="13"/>
     </row>
-    <row r="144" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A144" s="12"/>
       <c r="B144" s="13"/>
       <c r="C144" s="12"/>
       <c r="D144" s="13"/>
       <c r="E144" s="13"/>
     </row>
-    <row r="145" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A145" s="12"/>
       <c r="B145" s="13"/>
       <c r="C145" s="12"/>
       <c r="D145" s="13"/>
       <c r="E145" s="13"/>
     </row>
-    <row r="146" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A146" s="12"/>
       <c r="B146" s="13"/>
       <c r="C146" s="12"/>
       <c r="D146" s="13"/>
       <c r="E146" s="13"/>
     </row>
-    <row r="147" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A147" s="12"/>
       <c r="B147" s="13"/>
       <c r="C147" s="12"/>
       <c r="D147" s="13"/>
       <c r="E147" s="13"/>
     </row>
-    <row r="148" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A148" s="12"/>
       <c r="B148" s="13"/>
       <c r="C148" s="12"/>
       <c r="D148" s="13"/>
       <c r="E148" s="13"/>
     </row>
-    <row r="149" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A149" s="12"/>
       <c r="B149" s="13"/>
       <c r="C149" s="12"/>
       <c r="D149" s="13"/>
       <c r="E149" s="13"/>
     </row>
-    <row r="150" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A150" s="12"/>
       <c r="B150" s="13"/>
       <c r="C150" s="12"/>
       <c r="D150" s="13"/>
       <c r="E150" s="13"/>
     </row>
-    <row r="151" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A151" s="12"/>
       <c r="B151" s="13"/>
       <c r="C151" s="12"/>
       <c r="D151" s="13"/>
       <c r="E151" s="13"/>
     </row>
-    <row r="152" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A152" s="12"/>
       <c r="B152" s="13"/>
       <c r="C152" s="12"/>
       <c r="D152" s="13"/>
       <c r="E152" s="13"/>
     </row>
-    <row r="153" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A153" s="12"/>
       <c r="B153" s="13"/>
       <c r="C153" s="12"/>
       <c r="D153" s="13"/>
       <c r="E153" s="13"/>
     </row>
-    <row r="154" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A154" s="12"/>
       <c r="B154" s="13"/>
       <c r="C154" s="12"/>
       <c r="D154" s="13"/>
       <c r="E154" s="13"/>
     </row>
-    <row r="155" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A155" s="12"/>
       <c r="B155" s="13"/>
       <c r="C155" s="12"/>
       <c r="D155" s="13"/>
       <c r="E155" s="13"/>
     </row>
-    <row r="156" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A156" s="12"/>
       <c r="B156" s="13"/>
       <c r="C156" s="12"/>
       <c r="D156" s="13"/>
       <c r="E156" s="13"/>
     </row>
-    <row r="157" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A157" s="12"/>
       <c r="B157" s="13"/>
       <c r="C157" s="12"/>
       <c r="D157" s="13"/>
       <c r="E157" s="13"/>
     </row>
-    <row r="158" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A158" s="12"/>
       <c r="B158" s="13"/>
       <c r="C158" s="12"/>
       <c r="D158" s="13"/>
       <c r="E158" s="13"/>
     </row>
-    <row r="159" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A159" s="12"/>
       <c r="B159" s="13"/>
       <c r="C159" s="12"/>
       <c r="D159" s="13"/>
       <c r="E159" s="13"/>
     </row>
-    <row r="160" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A160" s="12"/>
       <c r="B160" s="13"/>
       <c r="C160" s="12"/>
       <c r="D160" s="13"/>
       <c r="E160" s="13"/>
     </row>
-    <row r="161" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A161" s="12"/>
       <c r="B161" s="13"/>
       <c r="C161" s="12"/>
       <c r="D161" s="13"/>
       <c r="E161" s="13"/>
     </row>
-    <row r="162" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A162" s="12"/>
       <c r="B162" s="13"/>
       <c r="C162" s="12"/>
       <c r="D162" s="13"/>
       <c r="E162" s="13"/>
     </row>
-    <row r="163" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A163" s="12"/>
       <c r="B163" s="13"/>
       <c r="C163" s="12"/>
       <c r="D163" s="13"/>
       <c r="E163" s="13"/>
     </row>
-    <row r="164" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A164" s="12"/>
       <c r="B164" s="13"/>
       <c r="C164" s="12"/>
       <c r="D164" s="13"/>
       <c r="E164" s="13"/>
     </row>
-    <row r="165" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A165" s="12"/>
       <c r="B165" s="13"/>
       <c r="C165" s="12"/>
       <c r="D165" s="13"/>
       <c r="E165" s="13"/>
     </row>
-    <row r="166" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A166" s="12"/>
       <c r="B166" s="13"/>
       <c r="C166" s="12"/>
       <c r="D166" s="13"/>
       <c r="E166" s="13"/>
     </row>
-    <row r="167" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A167" s="12"/>
       <c r="B167" s="13"/>
       <c r="C167" s="12"/>
       <c r="D167" s="13"/>
       <c r="E167" s="13"/>
     </row>
-    <row r="168" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A168" s="12"/>
       <c r="B168" s="13"/>
       <c r="C168" s="12"/>
       <c r="D168" s="13"/>
       <c r="E168" s="13"/>
     </row>
-    <row r="169" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A169" s="12"/>
       <c r="B169" s="13"/>
       <c r="C169" s="12"/>
       <c r="D169" s="13"/>
       <c r="E169" s="13"/>
     </row>
-    <row r="170" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A170" s="12"/>
       <c r="B170" s="13"/>
       <c r="C170" s="12"/>
       <c r="D170" s="13"/>
       <c r="E170" s="13"/>
     </row>
-    <row r="171" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A171" s="12"/>
       <c r="B171" s="13"/>
       <c r="C171" s="12"/>
       <c r="D171" s="13"/>
       <c r="E171" s="13"/>
     </row>
-    <row r="172" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A172" s="12"/>
       <c r="B172" s="13"/>
       <c r="C172" s="12"/>
       <c r="D172" s="13"/>
       <c r="E172" s="13"/>
     </row>
-    <row r="173" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A173" s="12"/>
       <c r="B173" s="13"/>
       <c r="C173" s="12"/>
       <c r="D173" s="13"/>
       <c r="E173" s="13"/>
     </row>
-    <row r="174" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A174" s="12"/>
       <c r="B174" s="13"/>
       <c r="C174" s="12"/>
       <c r="D174" s="13"/>
       <c r="E174" s="13"/>
     </row>
-    <row r="175" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A175" s="12"/>
       <c r="B175" s="13"/>
       <c r="C175" s="12"/>
       <c r="D175" s="13"/>
       <c r="E175" s="13"/>
     </row>
-    <row r="176" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A176" s="12"/>
       <c r="B176" s="13"/>
       <c r="C176" s="12"/>
       <c r="D176" s="13"/>
       <c r="E176" s="13"/>
     </row>
-    <row r="177" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A177" s="12"/>
       <c r="B177" s="13"/>
       <c r="C177" s="12"/>
       <c r="D177" s="13"/>
       <c r="E177" s="13"/>
     </row>
-    <row r="178" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A178" s="12"/>
       <c r="B178" s="13"/>
       <c r="C178" s="12"/>
       <c r="D178" s="13"/>
       <c r="E178" s="13"/>
     </row>
-    <row r="179" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A179" s="12"/>
       <c r="B179" s="13"/>
       <c r="C179" s="12"/>
       <c r="D179" s="13"/>
       <c r="E179" s="13"/>
     </row>
-    <row r="180" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A180" s="12"/>
       <c r="B180" s="13"/>
       <c r="C180" s="12"/>
       <c r="D180" s="13"/>
       <c r="E180" s="13"/>
     </row>
-    <row r="181" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A181" s="12"/>
       <c r="B181" s="13"/>
       <c r="C181" s="12"/>
       <c r="D181" s="13"/>
       <c r="E181" s="13"/>
     </row>
-    <row r="182" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A182" s="12"/>
       <c r="B182" s="13"/>
       <c r="C182" s="12"/>
       <c r="D182" s="13"/>
       <c r="E182" s="13"/>
     </row>
-    <row r="183" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A183" s="12"/>
       <c r="B183" s="13"/>
       <c r="C183" s="12"/>
       <c r="D183" s="13"/>
       <c r="E183" s="13"/>
     </row>
-    <row r="184" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A184" s="12"/>
       <c r="B184" s="13"/>
       <c r="C184" s="12"/>
       <c r="D184" s="13"/>
       <c r="E184" s="13"/>
     </row>
-    <row r="185" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A185" s="12"/>
       <c r="B185" s="13"/>
       <c r="C185" s="12"/>
       <c r="D185" s="13"/>
       <c r="E185" s="13"/>
     </row>
-    <row r="186" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A186" s="12"/>
       <c r="B186" s="13"/>
       <c r="C186" s="12"/>
       <c r="D186" s="13"/>
       <c r="E186" s="13"/>
     </row>
-    <row r="187" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A187" s="12"/>
       <c r="B187" s="13"/>
       <c r="C187" s="12"/>
       <c r="D187" s="13"/>
       <c r="E187" s="13"/>
     </row>
-    <row r="188" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A188" s="12"/>
       <c r="B188" s="13"/>
       <c r="C188" s="12"/>
       <c r="D188" s="13"/>
       <c r="E188" s="13"/>
     </row>
-    <row r="189" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A189" s="12"/>
       <c r="B189" s="13"/>
       <c r="C189" s="12"/>
       <c r="D189" s="13"/>
       <c r="E189" s="13"/>
     </row>
-    <row r="190" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A190" s="12"/>
       <c r="B190" s="13"/>
       <c r="C190" s="12"/>
       <c r="D190" s="13"/>
       <c r="E190" s="13"/>
     </row>
-    <row r="191" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A191" s="12"/>
       <c r="B191" s="13"/>
       <c r="C191" s="12"/>
       <c r="D191" s="13"/>
       <c r="E191" s="13"/>
     </row>
-    <row r="192" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A192" s="12"/>
       <c r="B192" s="13"/>
       <c r="C192" s="12"/>
       <c r="D192" s="13"/>
       <c r="E192" s="13"/>
     </row>
-    <row r="193" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A193" s="12"/>
       <c r="B193" s="13"/>
       <c r="C193" s="12"/>
       <c r="D193" s="13"/>
       <c r="E193" s="13"/>
     </row>
-    <row r="194" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A194" s="12"/>
       <c r="B194" s="13"/>
       <c r="C194" s="12"/>
       <c r="D194" s="13"/>
       <c r="E194" s="13"/>
     </row>
-    <row r="195" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A195" s="12"/>
       <c r="B195" s="13"/>
       <c r="C195" s="12"/>
       <c r="D195" s="13"/>
       <c r="E195" s="13"/>
     </row>
-    <row r="196" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A196" s="12"/>
       <c r="B196" s="13"/>
       <c r="C196" s="12"/>
       <c r="D196" s="13"/>
       <c r="E196" s="13"/>
     </row>
-    <row r="197" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A197" s="12"/>
       <c r="B197" s="13"/>
       <c r="C197" s="12"/>
       <c r="D197" s="13"/>
       <c r="E197" s="13"/>
     </row>
-    <row r="198" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A198" s="12"/>
       <c r="B198" s="13"/>
       <c r="C198" s="12"/>
       <c r="D198" s="13"/>
       <c r="E198" s="13"/>
     </row>
-    <row r="199" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A199" s="12"/>
       <c r="B199" s="13"/>
       <c r="C199" s="12"/>
       <c r="D199" s="13"/>
       <c r="E199" s="13"/>
     </row>
-    <row r="200" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A200" s="12"/>
       <c r="B200" s="13"/>
       <c r="C200" s="12"/>
       <c r="D200" s="13"/>
       <c r="E200" s="13"/>
     </row>
-    <row r="201" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A201" s="12"/>
       <c r="B201" s="13"/>
       <c r="C201" s="12"/>
       <c r="D201" s="13"/>
       <c r="E201" s="13"/>
     </row>
-    <row r="202" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A202" s="12"/>
       <c r="B202" s="13"/>
       <c r="C202" s="12"/>
       <c r="D202" s="13"/>
       <c r="E202" s="13"/>
     </row>
-    <row r="203" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A203" s="12"/>
       <c r="B203" s="13"/>
       <c r="C203" s="12"/>
       <c r="D203" s="13"/>
       <c r="E203" s="13"/>
     </row>
-    <row r="204" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A204" s="12"/>
       <c r="B204" s="13"/>
       <c r="C204" s="12"/>
       <c r="D204" s="13"/>
       <c r="E204" s="13"/>
     </row>
-    <row r="205" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A205" s="12"/>
       <c r="B205" s="13"/>
       <c r="C205" s="12"/>
       <c r="D205" s="13"/>
       <c r="E205" s="13"/>
     </row>
-    <row r="206" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A206" s="12"/>
       <c r="B206" s="13"/>
       <c r="C206" s="12"/>
       <c r="D206" s="13"/>
       <c r="E206" s="13"/>
     </row>
-    <row r="207" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A207" s="12"/>
       <c r="B207" s="13"/>
       <c r="C207" s="12"/>
       <c r="D207" s="13"/>
       <c r="E207" s="13"/>
     </row>
-    <row r="208" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A208" s="12"/>
       <c r="B208" s="13"/>
       <c r="C208" s="12"/>
       <c r="D208" s="13"/>
       <c r="E208" s="13"/>
     </row>
-    <row r="209" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A209" s="12"/>
       <c r="B209" s="13"/>
       <c r="C209" s="12"/>
       <c r="D209" s="13"/>
       <c r="E209" s="13"/>
     </row>
-    <row r="210" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A210" s="12"/>
       <c r="B210" s="13"/>
       <c r="C210" s="12"/>
       <c r="D210" s="13"/>
       <c r="E210" s="13"/>
     </row>
-    <row r="211" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A211" s="12"/>
       <c r="B211" s="13"/>
       <c r="C211" s="12"/>
       <c r="D211" s="13"/>
       <c r="E211" s="13"/>
     </row>
-    <row r="212" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A212" s="12"/>
       <c r="B212" s="13"/>
       <c r="C212" s="12"/>
       <c r="D212" s="13"/>
       <c r="E212" s="13"/>
     </row>
-    <row r="213" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A213" s="12"/>
       <c r="B213" s="13"/>
       <c r="C213" s="12"/>
       <c r="D213" s="13"/>
       <c r="E213" s="13"/>
     </row>
-    <row r="214" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A214" s="12"/>
       <c r="B214" s="13"/>
       <c r="C214" s="12"/>
       <c r="D214" s="13"/>
       <c r="E214" s="13"/>
     </row>
-    <row r="215" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A215" s="12"/>
       <c r="B215" s="13"/>
       <c r="C215" s="12"/>
       <c r="D215" s="13"/>
       <c r="E215" s="13"/>
     </row>
-    <row r="216" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A216" s="12"/>
       <c r="B216" s="13"/>
       <c r="C216" s="12"/>
       <c r="D216" s="13"/>
       <c r="E216" s="13"/>
     </row>
-    <row r="217" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A217" s="12"/>
       <c r="B217" s="13"/>
       <c r="C217" s="12"/>
       <c r="D217" s="13"/>
       <c r="E217" s="13"/>
     </row>
-    <row r="218" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A218" s="12"/>
       <c r="B218" s="13"/>
       <c r="C218" s="12"/>
       <c r="D218" s="13"/>
       <c r="E218" s="13"/>
     </row>
-    <row r="219" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A219" s="12"/>
       <c r="B219" s="13"/>
       <c r="C219" s="12"/>
       <c r="D219" s="13"/>
       <c r="E219" s="13"/>
     </row>
-    <row r="220" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A220" s="12"/>
       <c r="B220" s="13"/>
       <c r="C220" s="12"/>
       <c r="D220" s="13"/>
       <c r="E220" s="13"/>
     </row>
-    <row r="221" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A221" s="12"/>
       <c r="B221" s="13"/>
       <c r="C221" s="12"/>
       <c r="D221" s="13"/>
       <c r="E221" s="13"/>
     </row>
-    <row r="222" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A222" s="12"/>
       <c r="B222" s="13"/>
       <c r="C222" s="12"/>
       <c r="D222" s="13"/>
       <c r="E222" s="13"/>
     </row>
-    <row r="223" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A223" s="12"/>
       <c r="B223" s="13"/>
       <c r="C223" s="12"/>
       <c r="D223" s="13"/>
       <c r="E223" s="13"/>
     </row>
-    <row r="224" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A224" s="12"/>
       <c r="B224" s="13"/>
       <c r="C224" s="12"/>
       <c r="D224" s="13"/>
       <c r="E224" s="13"/>
     </row>
-    <row r="225" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A225" s="12"/>
       <c r="B225" s="13"/>
       <c r="C225" s="12"/>
       <c r="D225" s="13"/>
       <c r="E225" s="13"/>
     </row>
-    <row r="226" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A226" s="12"/>
       <c r="B226" s="13"/>
       <c r="C226" s="12"/>
       <c r="D226" s="13"/>
       <c r="E226" s="13"/>
     </row>
-    <row r="227" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A227" s="12"/>
       <c r="B227" s="13"/>
       <c r="C227" s="12"/>
       <c r="D227" s="13"/>
       <c r="E227" s="13"/>
     </row>
-    <row r="228" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A228" s="12"/>
       <c r="B228" s="13"/>
       <c r="C228" s="12"/>
       <c r="D228" s="13"/>
       <c r="E228" s="13"/>
     </row>
-    <row r="229" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A229" s="12"/>
       <c r="B229" s="13"/>
       <c r="C229" s="12"/>
       <c r="D229" s="13"/>
       <c r="E229" s="13"/>
     </row>
-    <row r="230" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A230" s="12"/>
       <c r="B230" s="13"/>
       <c r="C230" s="12"/>
       <c r="D230" s="13"/>
       <c r="E230" s="13"/>
     </row>
-    <row r="231" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A231" s="12"/>
       <c r="B231" s="13"/>
       <c r="C231" s="12"/>
       <c r="D231" s="13"/>
       <c r="E231" s="13"/>
     </row>
-    <row r="232" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A232" s="12"/>
       <c r="B232" s="13"/>
       <c r="C232" s="12"/>
       <c r="D232" s="13"/>
       <c r="E232" s="13"/>
     </row>
-    <row r="233" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A233" s="12"/>
       <c r="B233" s="13"/>
       <c r="C233" s="12"/>
       <c r="D233" s="13"/>
       <c r="E233" s="13"/>
     </row>
-    <row r="234" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A234" s="12"/>
       <c r="B234" s="13"/>
       <c r="C234" s="12"/>
       <c r="D234" s="13"/>
       <c r="E234" s="13"/>
     </row>
-    <row r="235" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A235" s="12"/>
       <c r="B235" s="13"/>
       <c r="C235" s="12"/>
       <c r="D235" s="13"/>
       <c r="E235" s="13"/>
     </row>
-    <row r="236" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A236" s="12"/>
       <c r="B236" s="13"/>
       <c r="C236" s="12"/>
       <c r="D236" s="13"/>
       <c r="E236" s="13"/>
     </row>
-    <row r="237" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A237" s="12"/>
       <c r="B237" s="13"/>
       <c r="C237" s="12"/>
       <c r="D237" s="13"/>
       <c r="E237" s="13"/>
     </row>
-    <row r="238" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A238" s="12"/>
       <c r="B238" s="13"/>
       <c r="C238" s="12"/>
       <c r="D238" s="13"/>
       <c r="E238" s="13"/>
     </row>
-    <row r="239" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A239" s="12"/>
       <c r="B239" s="13"/>
       <c r="C239" s="12"/>
       <c r="D239" s="13"/>
       <c r="E239" s="13"/>
     </row>
-    <row r="240" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A240" s="12"/>
       <c r="B240" s="13"/>
       <c r="C240" s="12"/>
       <c r="D240" s="13"/>
       <c r="E240" s="13"/>
     </row>
-    <row r="241" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A241" s="12"/>
       <c r="B241" s="13"/>
       <c r="C241" s="12"/>
       <c r="D241" s="13"/>
       <c r="E241" s="13"/>
     </row>
-    <row r="242" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A242" s="12"/>
       <c r="B242" s="13"/>
       <c r="C242" s="12"/>
       <c r="D242" s="13"/>
       <c r="E242" s="13"/>
     </row>
-    <row r="243" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A243" s="12"/>
       <c r="B243" s="13"/>
       <c r="C243" s="12"/>
       <c r="D243" s="13"/>
       <c r="E243" s="13"/>
     </row>
-    <row r="244" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A244" s="12"/>
       <c r="B244" s="13"/>
       <c r="C244" s="12"/>
       <c r="D244" s="13"/>
       <c r="E244" s="13"/>
     </row>
-    <row r="245" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A245" s="12"/>
       <c r="B245" s="13"/>
       <c r="C245" s="12"/>
       <c r="D245" s="13"/>
       <c r="E245" s="13"/>
     </row>
-    <row r="246" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A246" s="12"/>
       <c r="B246" s="13"/>
       <c r="C246" s="12"/>
       <c r="D246" s="13"/>
       <c r="E246" s="13"/>
     </row>
-    <row r="247" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A247" s="12"/>
       <c r="B247" s="13"/>
       <c r="C247" s="12"/>
       <c r="D247" s="13"/>
       <c r="E247" s="13"/>
     </row>
-    <row r="248" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A248" s="12"/>
       <c r="B248" s="13"/>
       <c r="C248" s="12"/>
       <c r="D248" s="13"/>
       <c r="E248" s="13"/>
     </row>
-    <row r="249" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A249" s="12"/>
       <c r="B249" s="13"/>
       <c r="C249" s="12"/>
       <c r="D249" s="13"/>
       <c r="E249" s="13"/>
     </row>
-    <row r="250" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A250" s="12"/>
       <c r="B250" s="13"/>
       <c r="C250" s="12"/>
       <c r="D250" s="13"/>
       <c r="E250" s="13"/>
     </row>
-    <row r="251" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A251" s="12"/>
       <c r="B251" s="13"/>
       <c r="C251" s="12"/>
       <c r="D251" s="13"/>
       <c r="E251" s="13"/>
     </row>
-    <row r="252" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A252" s="12"/>
       <c r="B252" s="13"/>
       <c r="C252" s="12"/>
       <c r="D252" s="13"/>
       <c r="E252" s="13"/>
     </row>
-    <row r="253" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A253" s="12"/>
       <c r="B253" s="13"/>
       <c r="C253" s="12"/>
       <c r="D253" s="13"/>
       <c r="E253" s="13"/>
     </row>
-    <row r="254" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A254" s="12"/>
       <c r="B254" s="13"/>
       <c r="C254" s="12"/>
       <c r="D254" s="13"/>
       <c r="E254" s="13"/>
     </row>
-    <row r="255" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A255" s="12"/>
       <c r="B255" s="13"/>
       <c r="C255" s="12"/>
       <c r="D255" s="13"/>
       <c r="E255" s="13"/>
     </row>
-    <row r="256" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A256" s="12"/>
       <c r="B256" s="13"/>
       <c r="C256" s="12"/>
       <c r="D256" s="13"/>
       <c r="E256" s="13"/>
     </row>
-    <row r="257" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A257" s="12"/>
       <c r="B257" s="13"/>
       <c r="C257" s="12"/>
       <c r="D257" s="13"/>
       <c r="E257" s="13"/>
     </row>
-    <row r="258" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A258" s="12"/>
       <c r="B258" s="13"/>
       <c r="C258" s="12"/>
       <c r="D258" s="13"/>
       <c r="E258" s="13"/>
     </row>
-    <row r="259" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A259" s="12"/>
       <c r="B259" s="13"/>
       <c r="C259" s="12"/>
       <c r="D259" s="13"/>
       <c r="E259" s="13"/>
     </row>
-    <row r="260" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A260" s="12"/>
       <c r="B260" s="13"/>
       <c r="C260" s="12"/>
@@ -3134,6 +3146,7 @@
   <hyperlinks>
     <hyperlink ref="D37" r:id="rId1"/>
     <hyperlink ref="D38" r:id="rId2"/>
+    <hyperlink ref="D40" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
se agrega el [38] alumno al archivo
</commit_message>
<xml_diff>
--- a/Lista de Alumnos.xlsx
+++ b/Lista de Alumnos.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25330"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\Alumnos\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{018E02CB-CF3D-42CF-83C5-6922162C2121}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18200" windowHeight="8510"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Electronica Microcontrolada" sheetId="1" r:id="rId1"/>
@@ -14,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="121">
   <si>
     <t>#</t>
   </si>
@@ -361,9 +367,6 @@
     <t>ruizgb</t>
   </si>
   <si>
-    <t>Victoria MAVI</t>
-  </si>
-  <si>
     <t>Dario Maldonado</t>
   </si>
   <si>
@@ -371,12 +374,21 @@
   </si>
   <si>
     <t>darman82</t>
+  </si>
+  <si>
+    <t>Schafrik Maria Victoria</t>
+  </si>
+  <si>
+    <t>mavsschafrik@gmail.com</t>
+  </si>
+  <si>
+    <t>MaviSchaf</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -873,14 +885,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:E260"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="D41" sqref="D41"/>
+      <selection activeCell="E39" sqref="E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1534,32 +1546,38 @@
         <v>114</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" s="5">
         <v>38</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="C39" s="5"/>
-      <c r="D39" s="6"/>
-      <c r="E39" s="6"/>
+        <v>118</v>
+      </c>
+      <c r="C39" s="5">
+        <v>4</v>
+      </c>
+      <c r="D39" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="E39" s="6" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="40" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" s="5">
         <v>39</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C40" s="5">
         <v>2</v>
       </c>
       <c r="D40" s="17" t="s">
+        <v>116</v>
+      </c>
+      <c r="E40" s="6" t="s">
         <v>117</v>
-      </c>
-      <c r="E40" s="6" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1625,7 +1643,7 @@
       <c r="D47" s="6"/>
       <c r="E47" s="6"/>
     </row>
-    <row r="48" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A48" s="5">
         <v>47</v>
       </c>
@@ -1634,7 +1652,7 @@
       <c r="D48" s="6"/>
       <c r="E48" s="6"/>
     </row>
-    <row r="49" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A49" s="5">
         <v>48</v>
       </c>
@@ -3144,9 +3162,10 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D37" r:id="rId1"/>
-    <hyperlink ref="D38" r:id="rId2"/>
-    <hyperlink ref="D40" r:id="rId3"/>
+    <hyperlink ref="D37" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="D38" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="D40" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="D39" r:id="rId4" xr:uid="{722F356C-977B-46FD-B20C-ABCDA98A141D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Se agrega el [41] Alumno al archivo
</commit_message>
<xml_diff>
--- a/Lista de Alumnos.xlsx
+++ b/Lista de Alumnos.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25330"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\Alumnos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\DOCUMENTOS\TECNICATURA EN TELECOMUNICACIONES\Electronica microcontrolada\ELECTRONICA MICROCONTROLADA\Alumnos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{018E02CB-CF3D-42CF-83C5-6922162C2121}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="345" windowWidth="19425" windowHeight="10305"/>
   </bookViews>
   <sheets>
     <sheet name="Electronica Microcontrolada" sheetId="1" r:id="rId1"/>
@@ -20,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="124">
   <si>
     <t>#</t>
   </si>
@@ -383,12 +382,21 @@
   </si>
   <si>
     <t>MaviSchaf</t>
+  </si>
+  <si>
+    <t>Lot Brian Llanos Garcia</t>
+  </si>
+  <si>
+    <t>brianllanosbuzon@gmail.com</t>
+  </si>
+  <si>
+    <t>BrianLlanos</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -885,26 +893,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:E260"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="E39" sqref="E39"/>
+      <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.81640625" style="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="37.1796875" style="15" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.54296875" style="14" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.85546875" style="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.140625" style="15" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" style="14" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="31" style="15" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="29" style="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1104,7 +1112,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
         <v>12</v>
       </c>
@@ -1410,7 +1418,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="5">
         <v>30</v>
       </c>
@@ -1546,7 +1554,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="5">
         <v>38</v>
       </c>
@@ -1563,7 +1571,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="5">
         <v>39</v>
       </c>
@@ -1584,10 +1592,18 @@
       <c r="A41" s="5">
         <v>40</v>
       </c>
-      <c r="B41" s="6"/>
-      <c r="C41" s="5"/>
-      <c r="D41" s="6"/>
-      <c r="E41" s="6"/>
+      <c r="B41" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="C41" s="5">
+        <v>1</v>
+      </c>
+      <c r="D41" s="17" t="s">
+        <v>122</v>
+      </c>
+      <c r="E41" s="6" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="42" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="5">
@@ -1643,7 +1659,7 @@
       <c r="D47" s="6"/>
       <c r="E47" s="6"/>
     </row>
-    <row r="48" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="5">
         <v>47</v>
       </c>
@@ -1652,7 +1668,7 @@
       <c r="D48" s="6"/>
       <c r="E48" s="6"/>
     </row>
-    <row r="49" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="5">
         <v>48</v>
       </c>
@@ -1661,7 +1677,7 @@
       <c r="D49" s="6"/>
       <c r="E49" s="6"/>
     </row>
-    <row r="50" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="5">
         <v>49</v>
       </c>
@@ -1670,7 +1686,7 @@
       <c r="D50" s="6"/>
       <c r="E50" s="6"/>
     </row>
-    <row r="51" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="5">
         <v>50</v>
       </c>
@@ -1679,7 +1695,7 @@
       <c r="D51" s="6"/>
       <c r="E51" s="6"/>
     </row>
-    <row r="52" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="5">
         <v>51</v>
       </c>
@@ -1688,7 +1704,7 @@
       <c r="D52" s="6"/>
       <c r="E52" s="6"/>
     </row>
-    <row r="53" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="5">
         <v>52</v>
       </c>
@@ -1697,7 +1713,7 @@
       <c r="D53" s="6"/>
       <c r="E53" s="6"/>
     </row>
-    <row r="54" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="5">
         <v>53</v>
       </c>
@@ -1706,7 +1722,7 @@
       <c r="D54" s="6"/>
       <c r="E54" s="6"/>
     </row>
-    <row r="55" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="5">
         <v>54</v>
       </c>
@@ -1715,7 +1731,7 @@
       <c r="D55" s="6"/>
       <c r="E55" s="6"/>
     </row>
-    <row r="56" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="5">
         <v>55</v>
       </c>
@@ -1724,7 +1740,7 @@
       <c r="D56" s="6"/>
       <c r="E56" s="6"/>
     </row>
-    <row r="57" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="5">
         <v>56</v>
       </c>
@@ -1733,7 +1749,7 @@
       <c r="D57" s="6"/>
       <c r="E57" s="6"/>
     </row>
-    <row r="58" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="5">
         <v>57</v>
       </c>
@@ -1742,7 +1758,7 @@
       <c r="D58" s="6"/>
       <c r="E58" s="6"/>
     </row>
-    <row r="59" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="5">
         <v>58</v>
       </c>
@@ -1751,7 +1767,7 @@
       <c r="D59" s="6"/>
       <c r="E59" s="6"/>
     </row>
-    <row r="60" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="5">
         <v>59</v>
       </c>
@@ -1760,1400 +1776,1400 @@
       <c r="D60" s="6"/>
       <c r="E60" s="6"/>
     </row>
-    <row r="61" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="12"/>
       <c r="B61" s="13"/>
       <c r="C61" s="12"/>
       <c r="D61" s="13"/>
       <c r="E61" s="13"/>
     </row>
-    <row r="62" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="12"/>
       <c r="B62" s="13"/>
       <c r="C62" s="12"/>
       <c r="D62" s="13"/>
       <c r="E62" s="13"/>
     </row>
-    <row r="63" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="12"/>
       <c r="B63" s="13"/>
       <c r="C63" s="12"/>
       <c r="D63" s="13"/>
       <c r="E63" s="13"/>
     </row>
-    <row r="64" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="12"/>
       <c r="B64" s="13"/>
       <c r="C64" s="12"/>
       <c r="D64" s="13"/>
       <c r="E64" s="13"/>
     </row>
-    <row r="65" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="12"/>
       <c r="B65" s="13"/>
       <c r="C65" s="12"/>
       <c r="D65" s="13"/>
       <c r="E65" s="13"/>
     </row>
-    <row r="66" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="12"/>
       <c r="B66" s="13"/>
       <c r="C66" s="12"/>
       <c r="D66" s="13"/>
       <c r="E66" s="13"/>
     </row>
-    <row r="67" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="12"/>
       <c r="B67" s="13"/>
       <c r="C67" s="12"/>
       <c r="D67" s="13"/>
       <c r="E67" s="13"/>
     </row>
-    <row r="68" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="12"/>
       <c r="B68" s="13"/>
       <c r="C68" s="12"/>
       <c r="D68" s="13"/>
       <c r="E68" s="13"/>
     </row>
-    <row r="69" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="12"/>
       <c r="B69" s="13"/>
       <c r="C69" s="12"/>
       <c r="D69" s="13"/>
       <c r="E69" s="13"/>
     </row>
-    <row r="70" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="12"/>
       <c r="B70" s="13"/>
       <c r="C70" s="12"/>
       <c r="D70" s="13"/>
       <c r="E70" s="13"/>
     </row>
-    <row r="71" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="12"/>
       <c r="B71" s="13"/>
       <c r="C71" s="12"/>
       <c r="D71" s="13"/>
       <c r="E71" s="13"/>
     </row>
-    <row r="72" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="12"/>
       <c r="B72" s="13"/>
       <c r="C72" s="12"/>
       <c r="D72" s="13"/>
       <c r="E72" s="13"/>
     </row>
-    <row r="73" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="12"/>
       <c r="B73" s="13"/>
       <c r="C73" s="12"/>
       <c r="D73" s="13"/>
       <c r="E73" s="13"/>
     </row>
-    <row r="74" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="12"/>
       <c r="B74" s="13"/>
       <c r="C74" s="12"/>
       <c r="D74" s="13"/>
       <c r="E74" s="13"/>
     </row>
-    <row r="75" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="12"/>
       <c r="B75" s="13"/>
       <c r="C75" s="12"/>
       <c r="D75" s="13"/>
       <c r="E75" s="13"/>
     </row>
-    <row r="76" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="12"/>
       <c r="B76" s="13"/>
       <c r="C76" s="12"/>
       <c r="D76" s="13"/>
       <c r="E76" s="13"/>
     </row>
-    <row r="77" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="12"/>
       <c r="B77" s="13"/>
       <c r="C77" s="12"/>
       <c r="D77" s="13"/>
       <c r="E77" s="13"/>
     </row>
-    <row r="78" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="12"/>
       <c r="B78" s="13"/>
       <c r="C78" s="12"/>
       <c r="D78" s="13"/>
       <c r="E78" s="13"/>
     </row>
-    <row r="79" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="12"/>
       <c r="B79" s="13"/>
       <c r="C79" s="12"/>
       <c r="D79" s="13"/>
       <c r="E79" s="13"/>
     </row>
-    <row r="80" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="12"/>
       <c r="B80" s="13"/>
       <c r="C80" s="12"/>
       <c r="D80" s="13"/>
       <c r="E80" s="13"/>
     </row>
-    <row r="81" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="12"/>
       <c r="B81" s="13"/>
       <c r="C81" s="12"/>
       <c r="D81" s="13"/>
       <c r="E81" s="13"/>
     </row>
-    <row r="82" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="12"/>
       <c r="B82" s="13"/>
       <c r="C82" s="12"/>
       <c r="D82" s="13"/>
       <c r="E82" s="13"/>
     </row>
-    <row r="83" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="12"/>
       <c r="B83" s="13"/>
       <c r="C83" s="12"/>
       <c r="D83" s="13"/>
       <c r="E83" s="13"/>
     </row>
-    <row r="84" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="12"/>
       <c r="B84" s="13"/>
       <c r="C84" s="12"/>
       <c r="D84" s="13"/>
       <c r="E84" s="13"/>
     </row>
-    <row r="85" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="12"/>
       <c r="B85" s="13"/>
       <c r="C85" s="12"/>
       <c r="D85" s="13"/>
       <c r="E85" s="13"/>
     </row>
-    <row r="86" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="12"/>
       <c r="B86" s="13"/>
       <c r="C86" s="12"/>
       <c r="D86" s="13"/>
       <c r="E86" s="13"/>
     </row>
-    <row r="87" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="12"/>
       <c r="B87" s="13"/>
       <c r="C87" s="12"/>
       <c r="D87" s="13"/>
       <c r="E87" s="13"/>
     </row>
-    <row r="88" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="12"/>
       <c r="B88" s="13"/>
       <c r="C88" s="12"/>
       <c r="D88" s="13"/>
       <c r="E88" s="13"/>
     </row>
-    <row r="89" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="12"/>
       <c r="B89" s="13"/>
       <c r="C89" s="12"/>
       <c r="D89" s="13"/>
       <c r="E89" s="13"/>
     </row>
-    <row r="90" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="12"/>
       <c r="B90" s="13"/>
       <c r="C90" s="12"/>
       <c r="D90" s="13"/>
       <c r="E90" s="13"/>
     </row>
-    <row r="91" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="12"/>
       <c r="B91" s="13"/>
       <c r="C91" s="12"/>
       <c r="D91" s="13"/>
       <c r="E91" s="13"/>
     </row>
-    <row r="92" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="12"/>
       <c r="B92" s="13"/>
       <c r="C92" s="12"/>
       <c r="D92" s="13"/>
       <c r="E92" s="13"/>
     </row>
-    <row r="93" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="12"/>
       <c r="B93" s="13"/>
       <c r="C93" s="12"/>
       <c r="D93" s="13"/>
       <c r="E93" s="13"/>
     </row>
-    <row r="94" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="12"/>
       <c r="B94" s="13"/>
       <c r="C94" s="12"/>
       <c r="D94" s="13"/>
       <c r="E94" s="13"/>
     </row>
-    <row r="95" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="12"/>
       <c r="B95" s="13"/>
       <c r="C95" s="12"/>
       <c r="D95" s="13"/>
       <c r="E95" s="13"/>
     </row>
-    <row r="96" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="12"/>
       <c r="B96" s="13"/>
       <c r="C96" s="12"/>
       <c r="D96" s="13"/>
       <c r="E96" s="13"/>
     </row>
-    <row r="97" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="12"/>
       <c r="B97" s="13"/>
       <c r="C97" s="12"/>
       <c r="D97" s="13"/>
       <c r="E97" s="13"/>
     </row>
-    <row r="98" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="12"/>
       <c r="B98" s="13"/>
       <c r="C98" s="12"/>
       <c r="D98" s="13"/>
       <c r="E98" s="13"/>
     </row>
-    <row r="99" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="12"/>
       <c r="B99" s="13"/>
       <c r="C99" s="12"/>
       <c r="D99" s="13"/>
       <c r="E99" s="13"/>
     </row>
-    <row r="100" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="12"/>
       <c r="B100" s="13"/>
       <c r="C100" s="12"/>
       <c r="D100" s="13"/>
       <c r="E100" s="13"/>
     </row>
-    <row r="101" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="12"/>
       <c r="B101" s="13"/>
       <c r="C101" s="12"/>
       <c r="D101" s="13"/>
       <c r="E101" s="13"/>
     </row>
-    <row r="102" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="12"/>
       <c r="B102" s="13"/>
       <c r="C102" s="12"/>
       <c r="D102" s="13"/>
       <c r="E102" s="13"/>
     </row>
-    <row r="103" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" s="12"/>
       <c r="B103" s="13"/>
       <c r="C103" s="12"/>
       <c r="D103" s="13"/>
       <c r="E103" s="13"/>
     </row>
-    <row r="104" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="12"/>
       <c r="B104" s="13"/>
       <c r="C104" s="12"/>
       <c r="D104" s="13"/>
       <c r="E104" s="13"/>
     </row>
-    <row r="105" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" s="12"/>
       <c r="B105" s="13"/>
       <c r="C105" s="12"/>
       <c r="D105" s="13"/>
       <c r="E105" s="13"/>
     </row>
-    <row r="106" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="12"/>
       <c r="B106" s="13"/>
       <c r="C106" s="12"/>
       <c r="D106" s="13"/>
       <c r="E106" s="13"/>
     </row>
-    <row r="107" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" s="12"/>
       <c r="B107" s="13"/>
       <c r="C107" s="12"/>
       <c r="D107" s="13"/>
       <c r="E107" s="13"/>
     </row>
-    <row r="108" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" s="12"/>
       <c r="B108" s="13"/>
       <c r="C108" s="12"/>
       <c r="D108" s="13"/>
       <c r="E108" s="13"/>
     </row>
-    <row r="109" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" s="12"/>
       <c r="B109" s="13"/>
       <c r="C109" s="12"/>
       <c r="D109" s="13"/>
       <c r="E109" s="13"/>
     </row>
-    <row r="110" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" s="12"/>
       <c r="B110" s="13"/>
       <c r="C110" s="12"/>
       <c r="D110" s="13"/>
       <c r="E110" s="13"/>
     </row>
-    <row r="111" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" s="12"/>
       <c r="B111" s="13"/>
       <c r="C111" s="12"/>
       <c r="D111" s="13"/>
       <c r="E111" s="13"/>
     </row>
-    <row r="112" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" s="12"/>
       <c r="B112" s="13"/>
       <c r="C112" s="12"/>
       <c r="D112" s="13"/>
       <c r="E112" s="13"/>
     </row>
-    <row r="113" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" s="12"/>
       <c r="B113" s="13"/>
       <c r="C113" s="12"/>
       <c r="D113" s="13"/>
       <c r="E113" s="13"/>
     </row>
-    <row r="114" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A114" s="12"/>
       <c r="B114" s="13"/>
       <c r="C114" s="12"/>
       <c r="D114" s="13"/>
       <c r="E114" s="13"/>
     </row>
-    <row r="115" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A115" s="12"/>
       <c r="B115" s="13"/>
       <c r="C115" s="12"/>
       <c r="D115" s="13"/>
       <c r="E115" s="13"/>
     </row>
-    <row r="116" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A116" s="12"/>
       <c r="B116" s="13"/>
       <c r="C116" s="12"/>
       <c r="D116" s="13"/>
       <c r="E116" s="13"/>
     </row>
-    <row r="117" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A117" s="12"/>
       <c r="B117" s="13"/>
       <c r="C117" s="12"/>
       <c r="D117" s="13"/>
       <c r="E117" s="13"/>
     </row>
-    <row r="118" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A118" s="12"/>
       <c r="B118" s="13"/>
       <c r="C118" s="12"/>
       <c r="D118" s="13"/>
       <c r="E118" s="13"/>
     </row>
-    <row r="119" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A119" s="12"/>
       <c r="B119" s="13"/>
       <c r="C119" s="12"/>
       <c r="D119" s="13"/>
       <c r="E119" s="13"/>
     </row>
-    <row r="120" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A120" s="12"/>
       <c r="B120" s="13"/>
       <c r="C120" s="12"/>
       <c r="D120" s="13"/>
       <c r="E120" s="13"/>
     </row>
-    <row r="121" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A121" s="12"/>
       <c r="B121" s="13"/>
       <c r="C121" s="12"/>
       <c r="D121" s="13"/>
       <c r="E121" s="13"/>
     </row>
-    <row r="122" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A122" s="12"/>
       <c r="B122" s="13"/>
       <c r="C122" s="12"/>
       <c r="D122" s="13"/>
       <c r="E122" s="13"/>
     </row>
-    <row r="123" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A123" s="12"/>
       <c r="B123" s="13"/>
       <c r="C123" s="12"/>
       <c r="D123" s="13"/>
       <c r="E123" s="13"/>
     </row>
-    <row r="124" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A124" s="12"/>
       <c r="B124" s="13"/>
       <c r="C124" s="12"/>
       <c r="D124" s="13"/>
       <c r="E124" s="13"/>
     </row>
-    <row r="125" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A125" s="12"/>
       <c r="B125" s="13"/>
       <c r="C125" s="12"/>
       <c r="D125" s="13"/>
       <c r="E125" s="13"/>
     </row>
-    <row r="126" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A126" s="12"/>
       <c r="B126" s="13"/>
       <c r="C126" s="12"/>
       <c r="D126" s="13"/>
       <c r="E126" s="13"/>
     </row>
-    <row r="127" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A127" s="12"/>
       <c r="B127" s="13"/>
       <c r="C127" s="12"/>
       <c r="D127" s="13"/>
       <c r="E127" s="13"/>
     </row>
-    <row r="128" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A128" s="12"/>
       <c r="B128" s="13"/>
       <c r="C128" s="12"/>
       <c r="D128" s="13"/>
       <c r="E128" s="13"/>
     </row>
-    <row r="129" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A129" s="12"/>
       <c r="B129" s="13"/>
       <c r="C129" s="12"/>
       <c r="D129" s="13"/>
       <c r="E129" s="13"/>
     </row>
-    <row r="130" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A130" s="12"/>
       <c r="B130" s="13"/>
       <c r="C130" s="12"/>
       <c r="D130" s="13"/>
       <c r="E130" s="13"/>
     </row>
-    <row r="131" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A131" s="12"/>
       <c r="B131" s="13"/>
       <c r="C131" s="12"/>
       <c r="D131" s="13"/>
       <c r="E131" s="13"/>
     </row>
-    <row r="132" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A132" s="12"/>
       <c r="B132" s="13"/>
       <c r="C132" s="12"/>
       <c r="D132" s="13"/>
       <c r="E132" s="13"/>
     </row>
-    <row r="133" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A133" s="12"/>
       <c r="B133" s="13"/>
       <c r="C133" s="12"/>
       <c r="D133" s="13"/>
       <c r="E133" s="13"/>
     </row>
-    <row r="134" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A134" s="12"/>
       <c r="B134" s="13"/>
       <c r="C134" s="12"/>
       <c r="D134" s="13"/>
       <c r="E134" s="13"/>
     </row>
-    <row r="135" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A135" s="12"/>
       <c r="B135" s="13"/>
       <c r="C135" s="12"/>
       <c r="D135" s="13"/>
       <c r="E135" s="13"/>
     </row>
-    <row r="136" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A136" s="12"/>
       <c r="B136" s="13"/>
       <c r="C136" s="12"/>
       <c r="D136" s="13"/>
       <c r="E136" s="13"/>
     </row>
-    <row r="137" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A137" s="12"/>
       <c r="B137" s="13"/>
       <c r="C137" s="12"/>
       <c r="D137" s="13"/>
       <c r="E137" s="13"/>
     </row>
-    <row r="138" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A138" s="12"/>
       <c r="B138" s="13"/>
       <c r="C138" s="12"/>
       <c r="D138" s="13"/>
       <c r="E138" s="13"/>
     </row>
-    <row r="139" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A139" s="12"/>
       <c r="B139" s="13"/>
       <c r="C139" s="12"/>
       <c r="D139" s="13"/>
       <c r="E139" s="13"/>
     </row>
-    <row r="140" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A140" s="12"/>
       <c r="B140" s="13"/>
       <c r="C140" s="12"/>
       <c r="D140" s="13"/>
       <c r="E140" s="13"/>
     </row>
-    <row r="141" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A141" s="12"/>
       <c r="B141" s="13"/>
       <c r="C141" s="12"/>
       <c r="D141" s="13"/>
       <c r="E141" s="13"/>
     </row>
-    <row r="142" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A142" s="12"/>
       <c r="B142" s="13"/>
       <c r="C142" s="12"/>
       <c r="D142" s="13"/>
       <c r="E142" s="13"/>
     </row>
-    <row r="143" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A143" s="12"/>
       <c r="B143" s="13"/>
       <c r="C143" s="12"/>
       <c r="D143" s="13"/>
       <c r="E143" s="13"/>
     </row>
-    <row r="144" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A144" s="12"/>
       <c r="B144" s="13"/>
       <c r="C144" s="12"/>
       <c r="D144" s="13"/>
       <c r="E144" s="13"/>
     </row>
-    <row r="145" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A145" s="12"/>
       <c r="B145" s="13"/>
       <c r="C145" s="12"/>
       <c r="D145" s="13"/>
       <c r="E145" s="13"/>
     </row>
-    <row r="146" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A146" s="12"/>
       <c r="B146" s="13"/>
       <c r="C146" s="12"/>
       <c r="D146" s="13"/>
       <c r="E146" s="13"/>
     </row>
-    <row r="147" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A147" s="12"/>
       <c r="B147" s="13"/>
       <c r="C147" s="12"/>
       <c r="D147" s="13"/>
       <c r="E147" s="13"/>
     </row>
-    <row r="148" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A148" s="12"/>
       <c r="B148" s="13"/>
       <c r="C148" s="12"/>
       <c r="D148" s="13"/>
       <c r="E148" s="13"/>
     </row>
-    <row r="149" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A149" s="12"/>
       <c r="B149" s="13"/>
       <c r="C149" s="12"/>
       <c r="D149" s="13"/>
       <c r="E149" s="13"/>
     </row>
-    <row r="150" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A150" s="12"/>
       <c r="B150" s="13"/>
       <c r="C150" s="12"/>
       <c r="D150" s="13"/>
       <c r="E150" s="13"/>
     </row>
-    <row r="151" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A151" s="12"/>
       <c r="B151" s="13"/>
       <c r="C151" s="12"/>
       <c r="D151" s="13"/>
       <c r="E151" s="13"/>
     </row>
-    <row r="152" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A152" s="12"/>
       <c r="B152" s="13"/>
       <c r="C152" s="12"/>
       <c r="D152" s="13"/>
       <c r="E152" s="13"/>
     </row>
-    <row r="153" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A153" s="12"/>
       <c r="B153" s="13"/>
       <c r="C153" s="12"/>
       <c r="D153" s="13"/>
       <c r="E153" s="13"/>
     </row>
-    <row r="154" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A154" s="12"/>
       <c r="B154" s="13"/>
       <c r="C154" s="12"/>
       <c r="D154" s="13"/>
       <c r="E154" s="13"/>
     </row>
-    <row r="155" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A155" s="12"/>
       <c r="B155" s="13"/>
       <c r="C155" s="12"/>
       <c r="D155" s="13"/>
       <c r="E155" s="13"/>
     </row>
-    <row r="156" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A156" s="12"/>
       <c r="B156" s="13"/>
       <c r="C156" s="12"/>
       <c r="D156" s="13"/>
       <c r="E156" s="13"/>
     </row>
-    <row r="157" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A157" s="12"/>
       <c r="B157" s="13"/>
       <c r="C157" s="12"/>
       <c r="D157" s="13"/>
       <c r="E157" s="13"/>
     </row>
-    <row r="158" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A158" s="12"/>
       <c r="B158" s="13"/>
       <c r="C158" s="12"/>
       <c r="D158" s="13"/>
       <c r="E158" s="13"/>
     </row>
-    <row r="159" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A159" s="12"/>
       <c r="B159" s="13"/>
       <c r="C159" s="12"/>
       <c r="D159" s="13"/>
       <c r="E159" s="13"/>
     </row>
-    <row r="160" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A160" s="12"/>
       <c r="B160" s="13"/>
       <c r="C160" s="12"/>
       <c r="D160" s="13"/>
       <c r="E160" s="13"/>
     </row>
-    <row r="161" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A161" s="12"/>
       <c r="B161" s="13"/>
       <c r="C161" s="12"/>
       <c r="D161" s="13"/>
       <c r="E161" s="13"/>
     </row>
-    <row r="162" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A162" s="12"/>
       <c r="B162" s="13"/>
       <c r="C162" s="12"/>
       <c r="D162" s="13"/>
       <c r="E162" s="13"/>
     </row>
-    <row r="163" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A163" s="12"/>
       <c r="B163" s="13"/>
       <c r="C163" s="12"/>
       <c r="D163" s="13"/>
       <c r="E163" s="13"/>
     </row>
-    <row r="164" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A164" s="12"/>
       <c r="B164" s="13"/>
       <c r="C164" s="12"/>
       <c r="D164" s="13"/>
       <c r="E164" s="13"/>
     </row>
-    <row r="165" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A165" s="12"/>
       <c r="B165" s="13"/>
       <c r="C165" s="12"/>
       <c r="D165" s="13"/>
       <c r="E165" s="13"/>
     </row>
-    <row r="166" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A166" s="12"/>
       <c r="B166" s="13"/>
       <c r="C166" s="12"/>
       <c r="D166" s="13"/>
       <c r="E166" s="13"/>
     </row>
-    <row r="167" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A167" s="12"/>
       <c r="B167" s="13"/>
       <c r="C167" s="12"/>
       <c r="D167" s="13"/>
       <c r="E167" s="13"/>
     </row>
-    <row r="168" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A168" s="12"/>
       <c r="B168" s="13"/>
       <c r="C168" s="12"/>
       <c r="D168" s="13"/>
       <c r="E168" s="13"/>
     </row>
-    <row r="169" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A169" s="12"/>
       <c r="B169" s="13"/>
       <c r="C169" s="12"/>
       <c r="D169" s="13"/>
       <c r="E169" s="13"/>
     </row>
-    <row r="170" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A170" s="12"/>
       <c r="B170" s="13"/>
       <c r="C170" s="12"/>
       <c r="D170" s="13"/>
       <c r="E170" s="13"/>
     </row>
-    <row r="171" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A171" s="12"/>
       <c r="B171" s="13"/>
       <c r="C171" s="12"/>
       <c r="D171" s="13"/>
       <c r="E171" s="13"/>
     </row>
-    <row r="172" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A172" s="12"/>
       <c r="B172" s="13"/>
       <c r="C172" s="12"/>
       <c r="D172" s="13"/>
       <c r="E172" s="13"/>
     </row>
-    <row r="173" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A173" s="12"/>
       <c r="B173" s="13"/>
       <c r="C173" s="12"/>
       <c r="D173" s="13"/>
       <c r="E173" s="13"/>
     </row>
-    <row r="174" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A174" s="12"/>
       <c r="B174" s="13"/>
       <c r="C174" s="12"/>
       <c r="D174" s="13"/>
       <c r="E174" s="13"/>
     </row>
-    <row r="175" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A175" s="12"/>
       <c r="B175" s="13"/>
       <c r="C175" s="12"/>
       <c r="D175" s="13"/>
       <c r="E175" s="13"/>
     </row>
-    <row r="176" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A176" s="12"/>
       <c r="B176" s="13"/>
       <c r="C176" s="12"/>
       <c r="D176" s="13"/>
       <c r="E176" s="13"/>
     </row>
-    <row r="177" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A177" s="12"/>
       <c r="B177" s="13"/>
       <c r="C177" s="12"/>
       <c r="D177" s="13"/>
       <c r="E177" s="13"/>
     </row>
-    <row r="178" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A178" s="12"/>
       <c r="B178" s="13"/>
       <c r="C178" s="12"/>
       <c r="D178" s="13"/>
       <c r="E178" s="13"/>
     </row>
-    <row r="179" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A179" s="12"/>
       <c r="B179" s="13"/>
       <c r="C179" s="12"/>
       <c r="D179" s="13"/>
       <c r="E179" s="13"/>
     </row>
-    <row r="180" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A180" s="12"/>
       <c r="B180" s="13"/>
       <c r="C180" s="12"/>
       <c r="D180" s="13"/>
       <c r="E180" s="13"/>
     </row>
-    <row r="181" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A181" s="12"/>
       <c r="B181" s="13"/>
       <c r="C181" s="12"/>
       <c r="D181" s="13"/>
       <c r="E181" s="13"/>
     </row>
-    <row r="182" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A182" s="12"/>
       <c r="B182" s="13"/>
       <c r="C182" s="12"/>
       <c r="D182" s="13"/>
       <c r="E182" s="13"/>
     </row>
-    <row r="183" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A183" s="12"/>
       <c r="B183" s="13"/>
       <c r="C183" s="12"/>
       <c r="D183" s="13"/>
       <c r="E183" s="13"/>
     </row>
-    <row r="184" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A184" s="12"/>
       <c r="B184" s="13"/>
       <c r="C184" s="12"/>
       <c r="D184" s="13"/>
       <c r="E184" s="13"/>
     </row>
-    <row r="185" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A185" s="12"/>
       <c r="B185" s="13"/>
       <c r="C185" s="12"/>
       <c r="D185" s="13"/>
       <c r="E185" s="13"/>
     </row>
-    <row r="186" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A186" s="12"/>
       <c r="B186" s="13"/>
       <c r="C186" s="12"/>
       <c r="D186" s="13"/>
       <c r="E186" s="13"/>
     </row>
-    <row r="187" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A187" s="12"/>
       <c r="B187" s="13"/>
       <c r="C187" s="12"/>
       <c r="D187" s="13"/>
       <c r="E187" s="13"/>
     </row>
-    <row r="188" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A188" s="12"/>
       <c r="B188" s="13"/>
       <c r="C188" s="12"/>
       <c r="D188" s="13"/>
       <c r="E188" s="13"/>
     </row>
-    <row r="189" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A189" s="12"/>
       <c r="B189" s="13"/>
       <c r="C189" s="12"/>
       <c r="D189" s="13"/>
       <c r="E189" s="13"/>
     </row>
-    <row r="190" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A190" s="12"/>
       <c r="B190" s="13"/>
       <c r="C190" s="12"/>
       <c r="D190" s="13"/>
       <c r="E190" s="13"/>
     </row>
-    <row r="191" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A191" s="12"/>
       <c r="B191" s="13"/>
       <c r="C191" s="12"/>
       <c r="D191" s="13"/>
       <c r="E191" s="13"/>
     </row>
-    <row r="192" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A192" s="12"/>
       <c r="B192" s="13"/>
       <c r="C192" s="12"/>
       <c r="D192" s="13"/>
       <c r="E192" s="13"/>
     </row>
-    <row r="193" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A193" s="12"/>
       <c r="B193" s="13"/>
       <c r="C193" s="12"/>
       <c r="D193" s="13"/>
       <c r="E193" s="13"/>
     </row>
-    <row r="194" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A194" s="12"/>
       <c r="B194" s="13"/>
       <c r="C194" s="12"/>
       <c r="D194" s="13"/>
       <c r="E194" s="13"/>
     </row>
-    <row r="195" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A195" s="12"/>
       <c r="B195" s="13"/>
       <c r="C195" s="12"/>
       <c r="D195" s="13"/>
       <c r="E195" s="13"/>
     </row>
-    <row r="196" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A196" s="12"/>
       <c r="B196" s="13"/>
       <c r="C196" s="12"/>
       <c r="D196" s="13"/>
       <c r="E196" s="13"/>
     </row>
-    <row r="197" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A197" s="12"/>
       <c r="B197" s="13"/>
       <c r="C197" s="12"/>
       <c r="D197" s="13"/>
       <c r="E197" s="13"/>
     </row>
-    <row r="198" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A198" s="12"/>
       <c r="B198" s="13"/>
       <c r="C198" s="12"/>
       <c r="D198" s="13"/>
       <c r="E198" s="13"/>
     </row>
-    <row r="199" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A199" s="12"/>
       <c r="B199" s="13"/>
       <c r="C199" s="12"/>
       <c r="D199" s="13"/>
       <c r="E199" s="13"/>
     </row>
-    <row r="200" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A200" s="12"/>
       <c r="B200" s="13"/>
       <c r="C200" s="12"/>
       <c r="D200" s="13"/>
       <c r="E200" s="13"/>
     </row>
-    <row r="201" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A201" s="12"/>
       <c r="B201" s="13"/>
       <c r="C201" s="12"/>
       <c r="D201" s="13"/>
       <c r="E201" s="13"/>
     </row>
-    <row r="202" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A202" s="12"/>
       <c r="B202" s="13"/>
       <c r="C202" s="12"/>
       <c r="D202" s="13"/>
       <c r="E202" s="13"/>
     </row>
-    <row r="203" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A203" s="12"/>
       <c r="B203" s="13"/>
       <c r="C203" s="12"/>
       <c r="D203" s="13"/>
       <c r="E203" s="13"/>
     </row>
-    <row r="204" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A204" s="12"/>
       <c r="B204" s="13"/>
       <c r="C204" s="12"/>
       <c r="D204" s="13"/>
       <c r="E204" s="13"/>
     </row>
-    <row r="205" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A205" s="12"/>
       <c r="B205" s="13"/>
       <c r="C205" s="12"/>
       <c r="D205" s="13"/>
       <c r="E205" s="13"/>
     </row>
-    <row r="206" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A206" s="12"/>
       <c r="B206" s="13"/>
       <c r="C206" s="12"/>
       <c r="D206" s="13"/>
       <c r="E206" s="13"/>
     </row>
-    <row r="207" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A207" s="12"/>
       <c r="B207" s="13"/>
       <c r="C207" s="12"/>
       <c r="D207" s="13"/>
       <c r="E207" s="13"/>
     </row>
-    <row r="208" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A208" s="12"/>
       <c r="B208" s="13"/>
       <c r="C208" s="12"/>
       <c r="D208" s="13"/>
       <c r="E208" s="13"/>
     </row>
-    <row r="209" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A209" s="12"/>
       <c r="B209" s="13"/>
       <c r="C209" s="12"/>
       <c r="D209" s="13"/>
       <c r="E209" s="13"/>
     </row>
-    <row r="210" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A210" s="12"/>
       <c r="B210" s="13"/>
       <c r="C210" s="12"/>
       <c r="D210" s="13"/>
       <c r="E210" s="13"/>
     </row>
-    <row r="211" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="211" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A211" s="12"/>
       <c r="B211" s="13"/>
       <c r="C211" s="12"/>
       <c r="D211" s="13"/>
       <c r="E211" s="13"/>
     </row>
-    <row r="212" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="212" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A212" s="12"/>
       <c r="B212" s="13"/>
       <c r="C212" s="12"/>
       <c r="D212" s="13"/>
       <c r="E212" s="13"/>
     </row>
-    <row r="213" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="213" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A213" s="12"/>
       <c r="B213" s="13"/>
       <c r="C213" s="12"/>
       <c r="D213" s="13"/>
       <c r="E213" s="13"/>
     </row>
-    <row r="214" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="214" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A214" s="12"/>
       <c r="B214" s="13"/>
       <c r="C214" s="12"/>
       <c r="D214" s="13"/>
       <c r="E214" s="13"/>
     </row>
-    <row r="215" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="215" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A215" s="12"/>
       <c r="B215" s="13"/>
       <c r="C215" s="12"/>
       <c r="D215" s="13"/>
       <c r="E215" s="13"/>
     </row>
-    <row r="216" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="216" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A216" s="12"/>
       <c r="B216" s="13"/>
       <c r="C216" s="12"/>
       <c r="D216" s="13"/>
       <c r="E216" s="13"/>
     </row>
-    <row r="217" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A217" s="12"/>
       <c r="B217" s="13"/>
       <c r="C217" s="12"/>
       <c r="D217" s="13"/>
       <c r="E217" s="13"/>
     </row>
-    <row r="218" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="218" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A218" s="12"/>
       <c r="B218" s="13"/>
       <c r="C218" s="12"/>
       <c r="D218" s="13"/>
       <c r="E218" s="13"/>
     </row>
-    <row r="219" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="219" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A219" s="12"/>
       <c r="B219" s="13"/>
       <c r="C219" s="12"/>
       <c r="D219" s="13"/>
       <c r="E219" s="13"/>
     </row>
-    <row r="220" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="220" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A220" s="12"/>
       <c r="B220" s="13"/>
       <c r="C220" s="12"/>
       <c r="D220" s="13"/>
       <c r="E220" s="13"/>
     </row>
-    <row r="221" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="221" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A221" s="12"/>
       <c r="B221" s="13"/>
       <c r="C221" s="12"/>
       <c r="D221" s="13"/>
       <c r="E221" s="13"/>
     </row>
-    <row r="222" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A222" s="12"/>
       <c r="B222" s="13"/>
       <c r="C222" s="12"/>
       <c r="D222" s="13"/>
       <c r="E222" s="13"/>
     </row>
-    <row r="223" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="223" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A223" s="12"/>
       <c r="B223" s="13"/>
       <c r="C223" s="12"/>
       <c r="D223" s="13"/>
       <c r="E223" s="13"/>
     </row>
-    <row r="224" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="224" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A224" s="12"/>
       <c r="B224" s="13"/>
       <c r="C224" s="12"/>
       <c r="D224" s="13"/>
       <c r="E224" s="13"/>
     </row>
-    <row r="225" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="225" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A225" s="12"/>
       <c r="B225" s="13"/>
       <c r="C225" s="12"/>
       <c r="D225" s="13"/>
       <c r="E225" s="13"/>
     </row>
-    <row r="226" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="226" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A226" s="12"/>
       <c r="B226" s="13"/>
       <c r="C226" s="12"/>
       <c r="D226" s="13"/>
       <c r="E226" s="13"/>
     </row>
-    <row r="227" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="227" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A227" s="12"/>
       <c r="B227" s="13"/>
       <c r="C227" s="12"/>
       <c r="D227" s="13"/>
       <c r="E227" s="13"/>
     </row>
-    <row r="228" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="228" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A228" s="12"/>
       <c r="B228" s="13"/>
       <c r="C228" s="12"/>
       <c r="D228" s="13"/>
       <c r="E228" s="13"/>
     </row>
-    <row r="229" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="229" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A229" s="12"/>
       <c r="B229" s="13"/>
       <c r="C229" s="12"/>
       <c r="D229" s="13"/>
       <c r="E229" s="13"/>
     </row>
-    <row r="230" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="230" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A230" s="12"/>
       <c r="B230" s="13"/>
       <c r="C230" s="12"/>
       <c r="D230" s="13"/>
       <c r="E230" s="13"/>
     </row>
-    <row r="231" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="231" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A231" s="12"/>
       <c r="B231" s="13"/>
       <c r="C231" s="12"/>
       <c r="D231" s="13"/>
       <c r="E231" s="13"/>
     </row>
-    <row r="232" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="232" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A232" s="12"/>
       <c r="B232" s="13"/>
       <c r="C232" s="12"/>
       <c r="D232" s="13"/>
       <c r="E232" s="13"/>
     </row>
-    <row r="233" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="233" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A233" s="12"/>
       <c r="B233" s="13"/>
       <c r="C233" s="12"/>
       <c r="D233" s="13"/>
       <c r="E233" s="13"/>
     </row>
-    <row r="234" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="234" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A234" s="12"/>
       <c r="B234" s="13"/>
       <c r="C234" s="12"/>
       <c r="D234" s="13"/>
       <c r="E234" s="13"/>
     </row>
-    <row r="235" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="235" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A235" s="12"/>
       <c r="B235" s="13"/>
       <c r="C235" s="12"/>
       <c r="D235" s="13"/>
       <c r="E235" s="13"/>
     </row>
-    <row r="236" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="236" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A236" s="12"/>
       <c r="B236" s="13"/>
       <c r="C236" s="12"/>
       <c r="D236" s="13"/>
       <c r="E236" s="13"/>
     </row>
-    <row r="237" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="237" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A237" s="12"/>
       <c r="B237" s="13"/>
       <c r="C237" s="12"/>
       <c r="D237" s="13"/>
       <c r="E237" s="13"/>
     </row>
-    <row r="238" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="238" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A238" s="12"/>
       <c r="B238" s="13"/>
       <c r="C238" s="12"/>
       <c r="D238" s="13"/>
       <c r="E238" s="13"/>
     </row>
-    <row r="239" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="239" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A239" s="12"/>
       <c r="B239" s="13"/>
       <c r="C239" s="12"/>
       <c r="D239" s="13"/>
       <c r="E239" s="13"/>
     </row>
-    <row r="240" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="240" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A240" s="12"/>
       <c r="B240" s="13"/>
       <c r="C240" s="12"/>
       <c r="D240" s="13"/>
       <c r="E240" s="13"/>
     </row>
-    <row r="241" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="241" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A241" s="12"/>
       <c r="B241" s="13"/>
       <c r="C241" s="12"/>
       <c r="D241" s="13"/>
       <c r="E241" s="13"/>
     </row>
-    <row r="242" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="242" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A242" s="12"/>
       <c r="B242" s="13"/>
       <c r="C242" s="12"/>
       <c r="D242" s="13"/>
       <c r="E242" s="13"/>
     </row>
-    <row r="243" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="243" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A243" s="12"/>
       <c r="B243" s="13"/>
       <c r="C243" s="12"/>
       <c r="D243" s="13"/>
       <c r="E243" s="13"/>
     </row>
-    <row r="244" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="244" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A244" s="12"/>
       <c r="B244" s="13"/>
       <c r="C244" s="12"/>
       <c r="D244" s="13"/>
       <c r="E244" s="13"/>
     </row>
-    <row r="245" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="245" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A245" s="12"/>
       <c r="B245" s="13"/>
       <c r="C245" s="12"/>
       <c r="D245" s="13"/>
       <c r="E245" s="13"/>
     </row>
-    <row r="246" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="246" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A246" s="12"/>
       <c r="B246" s="13"/>
       <c r="C246" s="12"/>
       <c r="D246" s="13"/>
       <c r="E246" s="13"/>
     </row>
-    <row r="247" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="247" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A247" s="12"/>
       <c r="B247" s="13"/>
       <c r="C247" s="12"/>
       <c r="D247" s="13"/>
       <c r="E247" s="13"/>
     </row>
-    <row r="248" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="248" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A248" s="12"/>
       <c r="B248" s="13"/>
       <c r="C248" s="12"/>
       <c r="D248" s="13"/>
       <c r="E248" s="13"/>
     </row>
-    <row r="249" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="249" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A249" s="12"/>
       <c r="B249" s="13"/>
       <c r="C249" s="12"/>
       <c r="D249" s="13"/>
       <c r="E249" s="13"/>
     </row>
-    <row r="250" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="250" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A250" s="12"/>
       <c r="B250" s="13"/>
       <c r="C250" s="12"/>
       <c r="D250" s="13"/>
       <c r="E250" s="13"/>
     </row>
-    <row r="251" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="251" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A251" s="12"/>
       <c r="B251" s="13"/>
       <c r="C251" s="12"/>
       <c r="D251" s="13"/>
       <c r="E251" s="13"/>
     </row>
-    <row r="252" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="252" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A252" s="12"/>
       <c r="B252" s="13"/>
       <c r="C252" s="12"/>
       <c r="D252" s="13"/>
       <c r="E252" s="13"/>
     </row>
-    <row r="253" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="253" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A253" s="12"/>
       <c r="B253" s="13"/>
       <c r="C253" s="12"/>
       <c r="D253" s="13"/>
       <c r="E253" s="13"/>
     </row>
-    <row r="254" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="254" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A254" s="12"/>
       <c r="B254" s="13"/>
       <c r="C254" s="12"/>
       <c r="D254" s="13"/>
       <c r="E254" s="13"/>
     </row>
-    <row r="255" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="255" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A255" s="12"/>
       <c r="B255" s="13"/>
       <c r="C255" s="12"/>
       <c r="D255" s="13"/>
       <c r="E255" s="13"/>
     </row>
-    <row r="256" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="256" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A256" s="12"/>
       <c r="B256" s="13"/>
       <c r="C256" s="12"/>
       <c r="D256" s="13"/>
       <c r="E256" s="13"/>
     </row>
-    <row r="257" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="257" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A257" s="12"/>
       <c r="B257" s="13"/>
       <c r="C257" s="12"/>
       <c r="D257" s="13"/>
       <c r="E257" s="13"/>
     </row>
-    <row r="258" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="258" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A258" s="12"/>
       <c r="B258" s="13"/>
       <c r="C258" s="12"/>
       <c r="D258" s="13"/>
       <c r="E258" s="13"/>
     </row>
-    <row r="259" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="259" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A259" s="12"/>
       <c r="B259" s="13"/>
       <c r="C259" s="12"/>
       <c r="D259" s="13"/>
       <c r="E259" s="13"/>
     </row>
-    <row r="260" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="260" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A260" s="12"/>
       <c r="B260" s="13"/>
       <c r="C260" s="12"/>
@@ -3162,10 +3178,11 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D37" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="D38" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="D40" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="D39" r:id="rId4" xr:uid="{722F356C-977B-46FD-B20C-ABCDA98A141D}"/>
+    <hyperlink ref="D37" r:id="rId1"/>
+    <hyperlink ref="D38" r:id="rId2"/>
+    <hyperlink ref="D40" r:id="rId3"/>
+    <hyperlink ref="D39" r:id="rId4"/>
+    <hyperlink ref="D41" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>